<commit_message>
IPD-IMGT/HLA database release 3.35.0
</commit_message>
<xml_diff>
--- a/transplanttoolbox/UNOS_antigens_to_alleles.xlsx
+++ b/transplanttoolbox/UNOS_antigens_to_alleles.xlsx
@@ -20,611 +20,611 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="364">
-  <si>
-    <t>IMGT/HLA allele</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="386">
+  <si>
+    <t>IPD-IMGT/HLA allele(s)</t>
   </si>
   <si>
     <t>UNOS Antigen</t>
   </si>
   <si>
+    <t>A*6601</t>
+  </si>
+  <si>
+    <t>A*6602</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A0203</t>
+  </si>
+  <si>
     <t>A1</t>
   </si>
   <si>
-    <t>A0</t>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A19</t>
   </si>
   <si>
     <t>A2</t>
   </si>
   <si>
-    <t>A0203</t>
+    <t>A23</t>
+  </si>
+  <si>
+    <t>A24</t>
+  </si>
+  <si>
+    <t>A2403</t>
+  </si>
+  <si>
+    <t>A25</t>
+  </si>
+  <si>
+    <t>A26</t>
+  </si>
+  <si>
+    <t>A28</t>
+  </si>
+  <si>
+    <t>A29</t>
   </si>
   <si>
     <t>A3</t>
   </si>
   <si>
-    <t>A11</t>
-  </si>
-  <si>
-    <t>A23</t>
-  </si>
-  <si>
-    <t>A24</t>
-  </si>
-  <si>
-    <t>A2403</t>
+    <t>A30</t>
+  </si>
+  <si>
+    <t>A31</t>
+  </si>
+  <si>
+    <t>A32</t>
+  </si>
+  <si>
+    <t>A33</t>
+  </si>
+  <si>
+    <t>A34</t>
+  </si>
+  <si>
+    <t>A36</t>
+  </si>
+  <si>
+    <t>A43</t>
+  </si>
+  <si>
+    <t>A66</t>
+  </si>
+  <si>
+    <t>A68</t>
+  </si>
+  <si>
+    <t>A69</t>
+  </si>
+  <si>
+    <t>A74</t>
+  </si>
+  <si>
+    <t>A80</t>
   </si>
   <si>
     <t>A9</t>
   </si>
   <si>
-    <t>A25</t>
-  </si>
-  <si>
-    <t>A26</t>
-  </si>
-  <si>
-    <t>A10</t>
-  </si>
-  <si>
-    <t>A29</t>
-  </si>
-  <si>
-    <t>A30</t>
-  </si>
-  <si>
-    <t>A31</t>
-  </si>
-  <si>
-    <t>A32</t>
-  </si>
-  <si>
-    <t>A33</t>
-  </si>
-  <si>
-    <t>A19</t>
-  </si>
-  <si>
-    <t>A34</t>
-  </si>
-  <si>
-    <t>A36</t>
-  </si>
-  <si>
-    <t>A43</t>
-  </si>
-  <si>
-    <t>A*6601</t>
-  </si>
-  <si>
-    <t>A*6602</t>
-  </si>
-  <si>
-    <t>A66</t>
-  </si>
-  <si>
-    <t>A68</t>
-  </si>
-  <si>
-    <t>A28</t>
-  </si>
-  <si>
-    <t>A69</t>
-  </si>
-  <si>
-    <t>A74</t>
-  </si>
-  <si>
-    <t>A80</t>
-  </si>
-  <si>
-    <t>A*01:01| A*01:01L| A*01:02| A*01:03| A*01:06| A*01:07| A*01:08| A*01:09| A*01:10| A*01:12| A*01:13| A*01:14| A*01:17| A*01:19| A*01:20| A*01:21| A*01:23| A*01:24| A*01:25| A*01:26| A*01:28| A*01:29| A*01:30| A*01:32| A*01:33| A*01:35| A*01:36| A*01:37| A*01:38| A*01:39| A*01:40| A*01:41| A*01:42| A*01:43| A*01:44| A*01:45| A*01:46| A*01:47| A*01:48| A*01:49| A*01:50| A*01:51| A*01:54| A*01:55| A*01:58| A*01:59| A*01:60| A*01:61| A*01:62| A*01:63| A*01:64| A*01:65| A*01:66| A*01:67| A*01:68| A*01:69| A*01:70| A*01:71| A*01:72| A*01:73| A*01:74| A*01:75| A*01:76| A*01:77| A*01:78| A*01:79| A*01:80| A*01:81| A*01:82| A*01:83| A*01:84| A*01:85| A*01:86| A*01:88| A*01:89| A*01:90| A*01:91| A*01:92| A*01:93| A*01:94| A*01:95| A*01:96| A*01:97| A*01:98| A*01:99| A*01:100| A*01:101| A*01:102| A*01:103| A*01:104| A*01:105| A*01:106| A*01:107| A*01:108| A*01:109| A*01:110| A*01:111| A*01:112| A*01:113| A*01:114| A*01:115| A*01:116| A*01:117| A*01:118| A*01:119| A*01:120| A*01:121| A*01:122| A*01:124| A*01:125| A*01:126| A*01:127| A*01:128| A*01:129| A*01:130| A*01:131| A*01:132| A*01:133| A*01:134| A*01:135| A*01:136| A*01:137| A*01:138| A*01:139| A*01:140| A*01:141| A*01:142| A*01:143| A*01:144| A*01:145| A*01:146| A*01:147Q| A*01:148| A*01:149| A*01:150| A*01:151| A*01:152| A*01:153| A*01:154| A*01:155| A*01:156| A*01:157| A*01:158| A*01:159| A*01:161| A*01:163| A*01:164| A*01:165| A*01:166| A*01:167| A*01:168| A*01:169| A*01:170| A*01:171| A*01:172| A*01:173| A*01:174| A*01:175| A*01:176| A*01:177| A*01:180| A*01:181| A*01:182| A*01:183| A*01:184| A*01:185| A*01:187| A*01:188| A*01:189| A*01:190| A*01:191| A*01:192| A*01:193| A*01:194| A*01:195| A*01:196| A*01:197| A*01:198| A*01:199| A*01:200| A*01:201| A*01:202| A*01:203| A*01:204| A*01:205| A*01:206| A*01:207| A*01:208Q| A*01:209| A*01:210| A*01:211| A*01:212| A*01:213| A*01:214| A*01:215| A*01:216| A*01:217| A*01:218| A*01:219| A*01:220| A*01:221| A*01:222| A*01:223| A*01:224| A*01:225| A*01:226| A*01:227| A*01:228Q| A*01:229| A*01:230| A*01:231| A*01:232| A*01:233| A*01:234| A*01:235| A*01:236| A*01:237| A*01:238| A*01:239| A*01:241| A*01:242| A*01:243| A*01:244</t>
-  </si>
-  <si>
-    <t>A*01:01N| A*01:04N| A*01:11N| A*01:15N| A*01:16N| A*01:18N| A*01:22N| A*01:27N| A*01:31N| A*01:52N| A*01:53N| A*01:56N| A*01:57N| A*01:87N| A*01:123N| A*01:160N| A*01:162N| A*01:178N| A*01:179N| A*01:186N| A*01:240N| A*02:15N| A*02:32N| A*02:43N| A*02:53N| A*02:82N| A*02:83N| A*02:88N| A*02:94N| A*02:113N| A*02:125N| A*02:222N| A*02:223N| A*02:225N| A*02:226N| A*02:227N| A*02:250N| A*02:284N| A*02:301N| A*02:305N| A*02:314N| A*02:321N| A*02:350N| A*02:356N| A*02:366N| A*02:373N| A*02:395N| A*02:439N| A*02:468N| A*02:476N| A*02:490N| A*02:501N| A*02:506N| A*02:514N| A*02:516N| A*02:525N| A*02:540N| A*02:608N| A*02:622N| A*02:643N| A*02:675N| A*02:691N| A*02:696N| A*03:01N| A*03:03N| A*03:11N| A*03:21N| A*03:36N| A*03:68N| A*03:69N| A*03:91N| A*03:129N| A*03:161N| A*03:162N| A*03:168N| A*03:178N| A*03:192N| A*03:197N| A*03:262N| A*03:266N| A*03:269N| A*03:275N| A*03:279N| A*03:283N| A*03:284N| A*03:286N| A*11:21N| A*11:69N| A*11:78N| A*11:99N| A*11:109N| A*11:115N| A*11:127N| A*11:137N| A*11:180N| A*11:208N| A*11:210N| A*11:215N| A*11:238N| A*11:251N| A*23:07N| A*23:08N| A*23:11N| A*23:19N| A*23:38N| A*24:09N| A*24:11N| A*24:36N| A*24:40N| A*24:45N| A*24:48N| A*24:60N| A*24:83N| A*24:84N| A*24:86N| A*24:90N| A*24:132N| A*24:155N| A*24:158N| A*24:163N| A*24:183N| A*24:185N| A*24:222N| A*24:232N| A*24:240N| A*24:252N| A*24:278N| A*24:303N| A*24:312N| A*24:323N| A*24:357N| A*24:359N| A*24:370N| A*24:388N| A*24:389N| A*25:12N| A*25:42N| A*26:01N| A*26:11N| A*26:25N| A*26:60N| A*26:71N| A*26:107N| A*26:127N| A*26:145N| A*29:01N| A*29:08N| A*29:78N| A*30:27N| A*30:59N| A*30:70N| A*30:73N| A*30:76N| A*30:78N| A*30:121N| A*30:123N| A*31:01N| A*31:14N| A*31:60N| A*31:126N| A*31:131N| A*32:19N| A*32:27N| A*32:45N| A*32:48N| A*32:56N| A*32:92N| A*33:73N| A*33:74N| A*33:80N| A*33:96N| A*33:123N| A*33:129N| A*34:10N| A*66:27N| A*66:28N| A*68:11N| A*68:18N| A*68:49N| A*68:59N| A*68:94N| A*68:120N| A*68:142N| A*68:171N| A*74:12N| A*74:14N</t>
-  </si>
-  <si>
-    <t>A*02:01| A*02:01L| A*02:01Q| A*02:02| A*02:04| A*02:05| A*02:06| A*02:07| A*02:08| A*02:09| A*02:10| A*02:11| A*02:12| A*02:13| A*02:14| A*02:16| A*02:17| A*02:18| A*02:19| A*02:20| A*02:21| A*02:22| A*02:24| A*02:25| A*02:26| A*02:27| A*02:28| A*02:29| A*02:30| A*02:31| A*02:33| A*02:34| A*02:35| A*02:36| A*02:37| A*02:38| A*02:39| A*02:40| A*02:41| A*02:42| A*02:44| A*02:45| A*02:46| A*02:47| A*02:48| A*02:49| A*02:50| A*02:51| A*02:52| A*02:54| A*02:55| A*02:56| A*02:57| A*02:58| A*02:59| A*02:60| A*02:61| A*02:62| A*02:63| A*02:64| A*02:65| A*02:66| A*02:67| A*02:68| A*02:69| A*02:70| A*02:71| A*02:72| A*02:73| A*02:74| A*02:75| A*02:76| A*02:77| A*02:78| A*02:79| A*02:80| A*02:81| A*02:84| A*02:85| A*02:86| A*02:87| A*02:89| A*02:90| A*02:91| A*02:92| A*02:93| A*02:95| A*02:96| A*02:97| A*02:99| A*02:101| A*02:102| A*02:103| A*02:104| A*02:105| A*02:106| A*02:107| A*02:108| A*02:109| A*02:110| A*02:111| A*02:112| A*02:114| A*02:115| A*02:116| A*02:117| A*02:118| A*02:119| A*02:120| A*02:121| A*02:122| A*02:123| A*02:124| A*02:126| A*02:127| A*02:128| A*02:129| A*02:130| A*02:131| A*02:132| A*02:133| A*02:134| A*02:135| A*02:136| A*02:137| A*02:138| A*02:139| A*02:140| A*02:141| A*02:142| A*02:143| A*02:144| A*02:145| A*02:146| A*02:147| A*02:148| A*02:149| A*02:150| A*02:151| A*02:152| A*02:153| A*02:154| A*02:155| A*02:156| A*02:157| A*02:158| A*02:159| A*02:160| A*02:161| A*02:162| A*02:163| A*02:164| A*02:165| A*02:166| A*02:167| A*02:168| A*02:169| A*02:170| A*02:171| A*02:172| A*02:173| A*02:174| A*02:175| A*02:176| A*02:177| A*02:178| A*02:179| A*02:180| A*02:181| A*02:182| A*02:183| A*02:184| A*02:185| A*02:186| A*02:187| A*02:188| A*02:189| A*02:190| A*02:191| A*02:192| A*02:193| A*02:194| A*02:195| A*02:196| A*02:197| A*02:198| A*02:199| A*02:200| A*02:201| A*02:202| A*02:203| A*02:204| A*02:205| A*02:206| A*02:207| A*02:208| A*02:209| A*02:210| A*02:211| A*02:212| A*02:213| A*02:214| A*02:215| A*02:216| A*02:217| A*02:218| A*02:219| A*02:220| A*02:221| A*02:224| A*02:228| A*02:229| A*02:230| A*02:231| A*02:232| A*02:233| A*02:234| A*02:235| A*02:236| A*02:237| A*02:238| A*02:239| A*02:240| A*02:241| A*02:242| A*02:243| A*02:244| A*02:245| A*02:246| A*02:247| A*02:248| A*02:249| A*02:251| A*02:252| A*02:253| A*02:254| A*02:255| A*02:256| A*02:257| A*02:258| A*02:259| A*02:260| A*02:261| A*02:262| A*02:263| A*02:264| A*02:265| A*02:266| A*02:267| A*02:268| A*02:269| A*02:270| A*02:271| A*02:272| A*02:273| A*02:274| A*02:275| A*02:276| A*02:277| A*02:278| A*02:279| A*02:280| A*02:281| A*02:282| A*02:283| A*02:285| A*02:286| A*02:287| A*02:288| A*02:289| A*02:290| A*02:291| A*02:292| A*02:293Q| A*02:294| A*02:295| A*02:296| A*02:297| A*02:298| A*02:299| A*02:300| A*02:302| A*02:303| A*02:304| A*02:306| A*02:307| A*02:308| A*02:309| A*02:310| A*02:311| A*02:312| A*02:313| A*02:315| A*02:316| A*02:317| A*02:318| A*02:319| A*02:320| A*02:322| A*02:323| A*02:324| A*02:325| A*02:326| A*02:327| A*02:328| A*02:329| A*02:330| A*02:331| A*02:332| A*02:333| A*02:334| A*02:335| A*02:336| A*02:337| A*02:338| A*02:339| A*02:340| A*02:341| A*02:342| A*02:343| A*02:344| A*02:345| A*02:346| A*02:347| A*02:348| A*02:349| A*02:351| A*02:352| A*02:353| A*02:354| A*02:355| A*02:357| A*02:358| A*02:359| A*02:360| A*02:361| A*02:362| A*02:363| A*02:364| A*02:365| A*02:367| A*02:368| A*02:369| A*02:370| A*02:371| A*02:372| A*02:374| A*02:375| A*02:376| A*02:377| A*02:378| A*02:379| A*02:380| A*02:381| A*02:382| A*02:383| A*02:384| A*02:385| A*02:386| A*02:387| A*02:388| A*02:389| A*02:390| A*02:391| A*02:392| A*02:393| A*02:394| A*02:396| A*02:397| A*02:398| A*02:399| A*02:400| A*02:401| A*02:402| A*02:403| A*02:404| A*02:405| A*02:406| A*02:407| A*02:408| A*02:409| A*02:410| A*02:411| A*02:412| A*02:413| A*02:414| A*02:415| A*02:416| A*02:417| A*02:418| A*02:419| A*02:420| A*02:421| A*02:422| A*02:423| A*02:424| A*02:425| A*02:426| A*02:427| A*02:428| A*02:429| A*02:430| A*02:431| A*02:432| A*02:433| A*02:434| A*02:435| A*02:436| A*02:437| A*02:438| A*02:440Q| A*02:441| A*02:442| A*02:443| A*02:444| A*02:445| A*02:446| A*02:447| A*02:448| A*02:449| A*02:450| A*02:451| A*02:452| A*02:453| A*02:454| A*02:455| A*02:456| A*02:457| A*02:458| A*02:459| A*02:460| A*02:461| A*02:462| A*02:463| A*02:464| A*02:465| A*02:466| A*02:467| A*02:469| A*02:470| A*02:471| A*02:472| A*02:473| A*02:474| A*02:475| A*02:477| A*02:478| A*02:479| A*02:480| A*02:481| A*02:482| A*02:483| A*02:484| A*02:485| A*02:486| A*02:487| A*02:488| A*02:489| A*02:491| A*02:492| A*02:493| A*02:494| A*02:495| A*02:496| A*02:497| A*02:498| A*02:499| A*02:500Q| A*02:502| A*02:503| A*02:504| A*02:505| A*02:507| A*02:508| A*02:509| A*02:510| A*02:511| A*02:512| A*02:513| A*02:515| A*02:517| A*02:518| A*02:519| A*02:520| A*02:521| A*02:522| A*02:523| A*02:524| A*02:526| A*02:527| A*02:528| A*02:529| A*02:530| A*02:531| A*02:532| A*02:533| A*02:534| A*02:535| A*02:536| A*02:537| A*02:538| A*02:539| A*02:541| A*02:542| A*02:543| A*02:544| A*02:545| A*02:546| A*02:547| A*02:548| A*02:549| A*02:550| A*02:551| A*02:552| A*02:553| A*02:554| A*02:555| A*02:556| A*02:557| A*02:558| A*02:559| A*02:560| A*02:561| A*02:562| A*02:563| A*02:564| A*02:565| A*02:566| A*02:567| A*02:568| A*02:569| A*02:570| A*02:571| A*02:572| A*02:573| A*02:574| A*02:575| A*02:576| A*02:577| A*02:578| A*02:579| A*02:580| A*02:581| A*02:582| A*02:583| A*02:584| A*02:585| A*02:586| A*02:587| A*02:588| A*02:589| A*02:590| A*02:591| A*02:592| A*02:593| A*02:594| A*02:595| A*02:596| A*02:597| A*02:598| A*02:599| A*02:600| A*02:601| A*02:602| A*02:603| A*02:604| A*02:605Q| A*02:606| A*02:607| A*02:609| A*02:610| A*02:611| A*02:612| A*02:613| A*02:614| A*02:615| A*02:616| A*02:617| A*02:618Q| A*02:619| A*02:620| A*02:621| A*02:623| A*02:624| A*02:625| A*02:626| A*02:627| A*02:628| A*02:629| A*02:630| A*02:631| A*02:632| A*02:633| A*02:634| A*02:635| A*02:636| A*02:637| A*02:638| A*02:639| A*02:640| A*02:641| A*02:642| A*02:644| A*02:645| A*02:646| A*02:647| A*02:648| A*02:649| A*02:650| A*02:651| A*02:652| A*02:653| A*02:654| A*02:655| A*02:656| A*02:657| A*02:658| A*02:659| A*02:660| A*02:661| A*02:662| A*02:663| A*02:664| A*02:665| A*02:666| A*02:667| A*02:668| A*02:669| A*02:670| A*02:671| A*02:672Q| A*02:673| A*02:674| A*02:676| A*02:677| A*02:678| A*02:679| A*02:680| A*02:681| A*02:682| A*02:683| A*02:684| A*02:685| A*02:686| A*02:687| A*02:688| A*02:689| A*02:690| A*02:692| A*02:693| A*02:694| A*02:695| A*02:697| A*02:698| A*02:699| A*02:700| A*02:701| A*02:702| A*02:703| A*02:704| A*02:705| A*02:706| A*02:03</t>
-  </si>
-  <si>
-    <t>A*02:03</t>
-  </si>
-  <si>
-    <t>A*03:01| A*03:02| A*03:04| A*03:05| A*03:06| A*03:07| A*03:08| A*03:09| A*03:10| A*03:12| A*03:13| A*03:14| A*03:15| A*03:16| A*03:17| A*03:18| A*03:19| A*03:20| A*03:22| A*03:23| A*03:24| A*03:25| A*03:26| A*03:27| A*03:28| A*03:29| A*03:30| A*03:31| A*03:32| A*03:33| A*03:34| A*03:35| A*03:37| A*03:38| A*03:39| A*03:40| A*03:41| A*03:42| A*03:43| A*03:44| A*03:45| A*03:46| A*03:47| A*03:48| A*03:49| A*03:50| A*03:51| A*03:52| A*03:53| A*03:54| A*03:55| A*03:56| A*03:57| A*03:58| A*03:59| A*03:60| A*03:61| A*03:62| A*03:63| A*03:64| A*03:65| A*03:66| A*03:67| A*03:70| A*03:71| A*03:72| A*03:73| A*03:74| A*03:75| A*03:76| A*03:77| A*03:78| A*03:79| A*03:80| A*03:81| A*03:82| A*03:83| A*03:84| A*03:85| A*03:86| A*03:87| A*03:88| A*03:89| A*03:90| A*03:92| A*03:93| A*03:94| A*03:95| A*03:96| A*03:97| A*03:98| A*03:99| A*03:100| A*03:101| A*03:102| A*03:103| A*03:104| A*03:105| A*03:106| A*03:107| A*03:108| A*03:109| A*03:110| A*03:111| A*03:112| A*03:113| A*03:114| A*03:115| A*03:116| A*03:117| A*03:118| A*03:119| A*03:120| A*03:121| A*03:122| A*03:123| A*03:124| A*03:125| A*03:126| A*03:127| A*03:128| A*03:130| A*03:131| A*03:132| A*03:133| A*03:134| A*03:135| A*03:136| A*03:137| A*03:138| A*03:139| A*03:140| A*03:141| A*03:142| A*03:143| A*03:144| A*03:145| A*03:146| A*03:147| A*03:148| A*03:149| A*03:150| A*03:151| A*03:152| A*03:153| A*03:154| A*03:155| A*03:156| A*03:157| A*03:158| A*03:159| A*03:160| A*03:163| A*03:164| A*03:165| A*03:166| A*03:167| A*03:169| A*03:170| A*03:171| A*03:172| A*03:173| A*03:174| A*03:175| A*03:176| A*03:177| A*03:179| A*03:180| A*03:181| A*03:182| A*03:183| A*03:184| A*03:185| A*03:186| A*03:187| A*03:188| A*03:189| A*03:190| A*03:191| A*03:193| A*03:195| A*03:196| A*03:198| A*03:199| A*03:201| A*03:202| A*03:203| A*03:204| A*03:205| A*03:206| A*03:207| A*03:208| A*03:209| A*03:210| A*03:211| A*03:212| A*03:213| A*03:214| A*03:215| A*03:216| A*03:217| A*03:218| A*03:219| A*03:220| A*03:221| A*03:222| A*03:223| A*03:224| A*03:225| A*03:226| A*03:227| A*03:228| A*03:229| A*03:230| A*03:231| A*03:232| A*03:233| A*03:234Q| A*03:235| A*03:236| A*03:237| A*03:238| A*03:239| A*03:240| A*03:241| A*03:242| A*03:243| A*03:244| A*03:245| A*03:246| A*03:247| A*03:248| A*03:249| A*03:250| A*03:251| A*03:252| A*03:253| A*03:254| A*03:255| A*03:256| A*03:257| A*03:258| A*03:259| A*03:261| A*03:263| A*03:264| A*03:265| A*03:267| A*03:268| A*03:270| A*03:271| A*03:272| A*03:273| A*03:274| A*03:276| A*03:277| A*03:278| A*03:280| A*03:281| A*03:282| A*03:285| A*03:287| A*03:288| A*03:289| A*32:04</t>
-  </si>
-  <si>
-    <t>A*11:01| A*11:02| A*11:03| A*11:04| A*11:05| A*11:06| A*11:07| A*11:08| A*11:09| A*11:10| A*11:11| A*11:12| A*11:13| A*11:14| A*11:15| A*11:16| A*11:17| A*11:18| A*11:19| A*11:20| A*11:22| A*11:23| A*11:24| A*11:25| A*11:26| A*11:27| A*11:29| A*11:30| A*11:31| A*11:32| A*11:33| A*11:34| A*11:35| A*11:36| A*11:37| A*11:38| A*11:39| A*11:40| A*11:41| A*11:42| A*11:43| A*11:44| A*11:45| A*11:46| A*11:47| A*11:48| A*11:49| A*11:50Q| A*11:51| A*11:52Q| A*11:54| A*11:55| A*11:56| A*11:57| A*11:58| A*11:59| A*11:60| A*11:61| A*11:62| A*11:63| A*11:64| A*11:65| A*11:66| A*11:67| A*11:68| A*11:70| A*11:71| A*11:72| A*11:73| A*11:74| A*11:75| A*11:76| A*11:77| A*11:79| A*11:80| A*11:81| A*11:82| A*11:83| A*11:84| A*11:85| A*11:86| A*11:87| A*11:88| A*11:89| A*11:90| A*11:91| A*11:92| A*11:93| A*11:94| A*11:95| A*11:96| A*11:97| A*11:98| A*11:100| A*11:101| A*11:102| A*11:103| A*11:104| A*11:105| A*11:106| A*11:107| A*11:108| A*11:110| A*11:111| A*11:112| A*11:113| A*11:114| A*11:116| A*11:117| A*11:118| A*11:119| A*11:120| A*11:121| A*11:122| A*11:123| A*11:124| A*11:125| A*11:126| A*11:128| A*11:129| A*11:130| A*11:131| A*11:132| A*11:133| A*11:134| A*11:135| A*11:136| A*11:138| A*11:139| A*11:140| A*11:141| A*11:142| A*11:143| A*11:144| A*11:145| A*11:146| A*11:147| A*11:148| A*11:149| A*11:150| A*11:151| A*11:152| A*11:153| A*11:154| A*11:155| A*11:156| A*11:157| A*11:158| A*11:159| A*11:160| A*11:161| A*11:162| A*11:163| A*11:164| A*11:165| A*11:166| A*11:167| A*11:168| A*11:169| A*11:170Q| A*11:171| A*11:172| A*11:173| A*11:174| A*11:175| A*11:176| A*11:177| A*11:178| A*11:179| A*11:181| A*11:182Q| A*11:183| A*11:184| A*11:185| A*11:186| A*11:187| A*11:188| A*11:189| A*11:190| A*11:191| A*11:192| A*11:193| A*11:194| A*11:195| A*11:196| A*11:197| A*11:198| A*11:199| A*11:200| A*11:201| A*11:202| A*11:203| A*11:204| A*11:205| A*11:206| A*11:207| A*11:209| A*11:211| A*11:212| A*11:213| A*11:214| A*11:216| A*11:217| A*11:218| A*11:219| A*11:220| A*11:221| A*11:222| A*11:223| A*11:224| A*11:225| A*11:226| A*11:227| A*11:228| A*11:229| A*11:230| A*11:231| A*11:232| A*11:233| A*11:234| A*11:235Q| A*11:236| A*11:237| A*11:239| A*11:240| A*11:241| A*11:242| A*11:243| A*11:244| A*11:245| A*11:246| A*11:247| A*11:248| A*11:249| A*11:250| A*11:252| A*11:253| A*11:254| A*11:255| A*11:256Q| A*11:257| A*11:258| A*11:259| A*11:260| A*11:261| A*11:262| A*11:263| A*11:264| A*11:265| A*11:266| A*11:267| A*11:268| A*11:269</t>
-  </si>
-  <si>
-    <t>A*23:01| A*23:02| A*23:03| A*23:04| A*23:05| A*23:06| A*23:09| A*23:10| A*23:12| A*23:13| A*23:14| A*23:15| A*23:16| A*23:17| A*23:18| A*23:20| A*23:21| A*23:22| A*23:23| A*23:24| A*23:25| A*23:26| A*23:27| A*23:28| A*23:29| A*23:30| A*23:31| A*23:32| A*23:33| A*23:34| A*23:35| A*23:36| A*23:37| A*23:39| A*23:40| A*23:41| A*23:42| A*23:43| A*23:44| A*23:45| A*23:46| A*23:47| A*23:48| A*23:49| A*23:50| A*23:51| A*23:52| A*23:53| A*23:54| A*23:55| A*23:56| A*23:57| A*23:58| A*23:59| A*23:60| A*23:61| A*23:62| A*23:63| A*23:64| A*23:65| A*23:66| A*23:67| A*23:68| A*23:70| A*23:71| A*23:72| A*23:73| A*23:74| A*23:75| A*23:76| A*23:77| A*23:78| A*23:79| A*23:80| A*23:81| A*23:82| A*23:83</t>
-  </si>
-  <si>
-    <t>A*24:02| A*24:02L| A*24:02Q| A*24:04| A*24:05| A*24:06| A*24:07| A*24:08| A*24:13| A*24:14| A*24:15| A*24:17| A*24:18| A*24:20| A*24:21| A*24:25| A*24:26| A*24:27| A*24:28| A*24:29| A*24:30| A*24:31| A*24:32| A*24:34| A*24:35| A*24:37| A*24:38| A*24:39| A*24:41| A*24:42| A*24:43| A*24:46| A*24:47| A*24:49| A*24:50| A*24:51| A*24:52| A*24:53| A*24:54| A*24:55| A*24:56| A*24:57| A*24:58| A*24:59| A*24:61| A*24:62| A*24:63| A*24:64| A*24:66| A*24:67| A*24:68| A*24:69| A*24:70| A*24:71| A*24:72| A*24:73| A*24:74| A*24:75| A*24:76| A*24:77| A*24:78| A*24:79| A*24:80| A*24:81| A*24:82| A*24:85| A*24:87| A*24:88| A*24:89| A*24:91| A*24:92| A*24:93| A*24:94| A*24:95| A*24:96| A*24:97| A*24:98| A*24:99| A*24:100| A*24:101| A*24:102| A*24:103| A*24:104| A*24:105| A*24:106| A*24:107| A*24:108| A*24:109| A*24:110| A*24:111| A*24:112| A*24:113| A*24:114| A*24:115| A*24:116| A*24:117| A*24:118| A*24:119| A*24:120| A*24:121| A*24:122| A*24:123| A*24:124| A*24:125| A*24:126| A*24:127| A*24:128| A*24:129| A*24:130| A*24:131| A*24:133| A*24:134| A*24:135| A*24:136| A*24:137| A*24:138| A*24:139| A*24:140| A*24:141| A*24:142| A*24:143| A*24:144| A*24:145| A*24:146| A*24:147| A*24:148| A*24:149| A*24:150| A*24:151| A*24:152| A*24:153| A*24:154| A*24:156| A*24:157| A*24:159| A*24:160| A*24:161| A*24:162| A*24:164| A*24:165| A*24:166| A*24:167| A*24:168| A*24:169| A*24:170| A*24:171| A*24:172| A*24:173| A*24:174| A*24:175| A*24:176| A*24:177| A*24:178| A*24:179| A*24:180| A*24:181| A*24:182| A*24:184| A*24:186| A*24:187| A*24:188| A*24:189| A*24:190| A*24:191| A*24:192| A*24:193| A*24:194| A*24:195| A*24:196| A*24:197| A*24:198| A*24:199| A*24:200| A*24:201| A*24:202| A*24:203| A*24:204| A*24:205| A*24:206| A*24:207| A*24:208| A*24:209| A*24:210| A*24:212| A*24:213| A*24:214| A*24:215| A*24:216| A*24:217| A*24:218| A*24:219| A*24:220| A*24:221| A*24:223| A*24:224| A*24:225| A*24:226| A*24:227| A*24:228| A*24:229| A*24:230| A*24:231| A*24:233| A*24:234| A*24:235| A*24:236| A*24:237| A*24:238| A*24:239| A*24:241| A*24:242| A*24:243| A*24:244| A*24:245| A*24:246| A*24:247| A*24:248| A*24:249| A*24:250| A*24:251| A*24:253| A*24:254| A*24:255| A*24:256| A*24:257| A*24:258| A*24:259| A*24:260| A*24:261| A*24:262| A*24:263| A*24:264| A*24:265| A*24:266| A*24:267| A*24:268| A*24:269| A*24:270| A*24:271| A*24:272| A*24:273| A*24:274| A*24:275| A*24:276| A*24:277| A*24:279| A*24:280| A*24:281| A*24:282| A*24:283| A*24:284| A*24:285| A*24:286| A*24:287| A*24:288| A*24:289| A*24:290| A*24:291| A*24:292| A*24:293| A*24:294Q| A*24:295| A*24:296| A*24:297| A*24:298| A*24:299| A*24:300| A*24:301| A*24:302| A*24:304| A*24:305| A*24:306| A*24:307| A*24:308| A*24:309| A*24:310| A*24:311| A*24:313| A*24:314| A*24:315| A*24:316| A*24:317| A*24:318| A*24:319| A*24:320| A*24:321| A*24:322| A*24:324| A*24:325| A*24:326| A*24:327| A*24:328| A*24:329| A*24:330| A*24:331| A*24:332| A*24:333| A*24:334| A*24:335| A*24:336| A*24:337| A*24:338| A*24:339| A*24:340| A*24:341| A*24:342| A*24:343| A*24:344| A*24:345| A*24:346| A*24:347| A*24:348| A*24:349| A*24:350| A*24:351| A*24:352| A*24:353| A*24:354| A*24:355| A*24:356| A*24:358| A*24:360| A*24:361| A*24:362| A*24:363| A*24:364| A*24:365| A*24:366| A*24:367| A*24:368| A*24:369| A*24:371| A*24:372| A*24:373| A*24:375| A*24:376| A*24:377| A*24:378| A*24:379| A*24:380| A*24:381| A*24:382| A*24:383| A*24:384| A*24:385| A*24:386| A*24:387| A*24:390| A*24:391| A*24:392| A*24:393| A*24:394</t>
-  </si>
-  <si>
-    <t>A*24:03| A*24:10| A*24:23| A*24:33| A*24:374</t>
-  </si>
-  <si>
-    <t>A*24:19| A*24:22| A*24:24| A*24:44| A*23:01| A*23:02| A*23:03| A*23:04| A*23:05| A*23:06| A*23:09| A*23:10| A*23:12| A*23:13| A*23:14| A*23:15| A*23:16| A*23:17| A*23:18| A*23:20| A*23:21| A*23:22| A*23:23| A*23:24| A*23:25| A*23:26| A*23:27| A*23:28| A*23:29| A*23:30| A*23:31| A*23:32| A*23:33| A*23:34| A*23:35| A*23:36| A*23:37| A*23:39| A*23:40| A*23:41| A*23:42| A*23:43| A*23:44| A*23:45| A*23:46| A*23:47| A*23:48| A*23:49| A*23:50| A*23:51| A*23:52| A*23:53| A*23:54| A*23:55| A*23:56| A*23:57| A*23:58| A*23:59| A*23:60| A*23:61| A*23:62| A*23:63| A*23:64| A*23:65| A*23:66| A*23:67| A*23:68| A*23:70| A*23:71| A*23:72| A*23:73| A*23:74| A*23:75| A*23:76| A*23:77| A*23:78| A*23:79| A*23:80| A*23:81| A*23:82| A*23:83| A*24:02| A*24:02L| A*24:02Q| A*24:04| A*24:05| A*24:06| A*24:07| A*24:08| A*24:13| A*24:14| A*24:15| A*24:17| A*24:18| A*24:20| A*24:21| A*24:25| A*24:26| A*24:27| A*24:28| A*24:29| A*24:30| A*24:31| A*24:32| A*24:34| A*24:35| A*24:37| A*24:38| A*24:39| A*24:41| A*24:42| A*24:43| A*24:46| A*24:47| A*24:49| A*24:50| A*24:51| A*24:52| A*24:53| A*24:54| A*24:55| A*24:56| A*24:57| A*24:58| A*24:59| A*24:61| A*24:62| A*24:63| A*24:64| A*24:66| A*24:67| A*24:68| A*24:69| A*24:70| A*24:71| A*24:72| A*24:73| A*24:74| A*24:75| A*24:76| A*24:77| A*24:78| A*24:79| A*24:80| A*24:81| A*24:82| A*24:85| A*24:87| A*24:88| A*24:89| A*24:91| A*24:92| A*24:93| A*24:94| A*24:95| A*24:96| A*24:97| A*24:98| A*24:99| A*24:100| A*24:101| A*24:102| A*24:103| A*24:104| A*24:105| A*24:106| A*24:107| A*24:108| A*24:109| A*24:110| A*24:111| A*24:112| A*24:113| A*24:114| A*24:115| A*24:116| A*24:117| A*24:118| A*24:119| A*24:120| A*24:121| A*24:122| A*24:123| A*24:124| A*24:125| A*24:126| A*24:127| A*24:128| A*24:129| A*24:130| A*24:131| A*24:133| A*24:134| A*24:135| A*24:136| A*24:137| A*24:138| A*24:139| A*24:140| A*24:141| A*24:142| A*24:143| A*24:144| A*24:145| A*24:146| A*24:147| A*24:148| A*24:149| A*24:150| A*24:151| A*24:152| A*24:153| A*24:154| A*24:156| A*24:157| A*24:159| A*24:160| A*24:161| A*24:162| A*24:164| A*24:165| A*24:166| A*24:167| A*24:168| A*24:169| A*24:170| A*24:171| A*24:172| A*24:173| A*24:174| A*24:175| A*24:176| A*24:177| A*24:178| A*24:179| A*24:180| A*24:181| A*24:182| A*24:184| A*24:186| A*24:187| A*24:188| A*24:189| A*24:190| A*24:191| A*24:192| A*24:193| A*24:194| A*24:195| A*24:196| A*24:197| A*24:198| A*24:199| A*24:200| A*24:201| A*24:202| A*24:203| A*24:204| A*24:205| A*24:206| A*24:207| A*24:208| A*24:209| A*24:210| A*24:212| A*24:213| A*24:214| A*24:215| A*24:216| A*24:217| A*24:218| A*24:219| A*24:220| A*24:221| A*24:223| A*24:224| A*24:225| A*24:226| A*24:227| A*24:228| A*24:229| A*24:230| A*24:231| A*24:233| A*24:234| A*24:235| A*24:236| A*24:237| A*24:238| A*24:239| A*24:241| A*24:242| A*24:243| A*24:244| A*24:245| A*24:246| A*24:247| A*24:248| A*24:249| A*24:250| A*24:251| A*24:253| A*24:254| A*24:255| A*24:256| A*24:257| A*24:258| A*24:259| A*24:260| A*24:261| A*24:262| A*24:263| A*24:264| A*24:265| A*24:266| A*24:267| A*24:268| A*24:269| A*24:270| A*24:271| A*24:272| A*24:273| A*24:274| A*24:275| A*24:276| A*24:277| A*24:279| A*24:280| A*24:281| A*24:282| A*24:283| A*24:284| A*24:285| A*24:286| A*24:287| A*24:288| A*24:289| A*24:290| A*24:291| A*24:292| A*24:293| A*24:294Q| A*24:295| A*24:296| A*24:297| A*24:298| A*24:299| A*24:300| A*24:301| A*24:302| A*24:304| A*24:305| A*24:306| A*24:307| A*24:308| A*24:309| A*24:310| A*24:311| A*24:313| A*24:314| A*24:315| A*24:316| A*24:317| A*24:318| A*24:319| A*24:320| A*24:321| A*24:322| A*24:324| A*24:325| A*24:326| A*24:327| A*24:328| A*24:329| A*24:330| A*24:331| A*24:332| A*24:333| A*24:334| A*24:335| A*24:336| A*24:337| A*24:338| A*24:339| A*24:340| A*24:341| A*24:342| A*24:343| A*24:344| A*24:345| A*24:346| A*24:347| A*24:348| A*24:349| A*24:350| A*24:351| A*24:352| A*24:353| A*24:354| A*24:355| A*24:356| A*24:358| A*24:360| A*24:361| A*24:362| A*24:363| A*24:364| A*24:365| A*24:366| A*24:367| A*24:368| A*24:369| A*24:371| A*24:372| A*24:373| A*24:375| A*24:376| A*24:377| A*24:378| A*24:379| A*24:380| A*24:381| A*24:382| A*24:383| A*24:384| A*24:385| A*24:386| A*24:387| A*24:390| A*24:391| A*24:392| A*24:393| A*24:394| A*24:03| A*24:10| A*24:23| A*24:33| A*24:374</t>
-  </si>
-  <si>
-    <t>A*25:01| A*25:02| A*25:03| A*25:04| A*25:05| A*25:06| A*25:07| A*25:08| A*25:09| A*25:10| A*25:11| A*25:13| A*25:14| A*25:15| A*25:16| A*25:17| A*25:18| A*25:19| A*25:20| A*25:21| A*25:22| A*25:23| A*25:24| A*25:25| A*25:26| A*25:27| A*25:28| A*25:29| A*25:30| A*25:31| A*25:32| A*25:33| A*25:34| A*25:35| A*25:36| A*25:37| A*25:38| A*25:39| A*25:40| A*25:41| A*25:43| A*25:44| A*25:45| A*25:46</t>
-  </si>
-  <si>
-    <t>A*26:01| A*26:02| A*26:03| A*26:04| A*26:05| A*26:06| A*26:07| A*26:08| A*26:09| A*26:12| A*26:13| A*26:14| A*26:16| A*26:17| A*26:19| A*26:20| A*26:21| A*26:22| A*26:23| A*26:24| A*26:27| A*26:28| A*26:29| A*26:30| A*26:31| A*26:32| A*26:33| A*26:34| A*26:35| A*26:36| A*26:37| A*26:38| A*26:39| A*26:40| A*26:41| A*26:42| A*26:43| A*26:45| A*26:46| A*26:47| A*26:48| A*26:49| A*26:50| A*26:51| A*26:52| A*26:53| A*26:54| A*26:55| A*26:56| A*26:57| A*26:58| A*26:59| A*26:61| A*26:62| A*26:63| A*26:64| A*26:65| A*26:66| A*26:67| A*26:68| A*26:69| A*26:70| A*26:72| A*26:73| A*26:74| A*26:75| A*26:76| A*26:77| A*26:78| A*26:79| A*26:80| A*26:81| A*26:82| A*26:83| A*26:84| A*26:85| A*26:86| A*26:87| A*26:88| A*26:89| A*26:90| A*26:91| A*26:93| A*26:94| A*26:95| A*26:96| A*26:97| A*26:98| A*26:99| A*26:100| A*26:101| A*26:102| A*26:103| A*26:104| A*26:105| A*26:106| A*26:108| A*26:109| A*26:110| A*26:111| A*26:112| A*26:113| A*26:114| A*26:115| A*26:116| A*26:117| A*26:118| A*26:119| A*26:120| A*26:121| A*26:122| A*26:123| A*26:124| A*26:125| A*26:126| A*26:128| A*26:129| A*26:130| A*26:131| A*26:132| A*26:133| A*26:134| A*26:135| A*26:136| A*26:137| A*26:138| A*26:139| A*26:140| A*26:141| A*26:142| A*26:143| A*26:144| A*26:146| A*26:147| A*26:148| A*26:149| A*66:05</t>
-  </si>
-  <si>
-    <t>A*26:10| A*26:15| A*26:18| A*26:26| A*26:92| A*34:06| A*66:03| A*66:08| A*25:01| A*25:02| A*25:03| A*25:04| A*25:05| A*25:06| A*25:07| A*25:08| A*25:09| A*25:10| A*25:11| A*25:13| A*25:14| A*25:15| A*25:16| A*25:17| A*25:18| A*25:19| A*25:20| A*25:21| A*25:22| A*25:23| A*25:24| A*25:25| A*25:26| A*25:27| A*25:28| A*25:29| A*25:30| A*25:31| A*25:32| A*25:33| A*25:34| A*25:35| A*25:36| A*25:37| A*25:38| A*25:39| A*25:40| A*25:41| A*25:43| A*25:44| A*25:45| A*25:46| A*26:01| A*26:02| A*26:03| A*26:04| A*26:05| A*26:06| A*26:07| A*26:08| A*26:09| A*26:12| A*26:13| A*26:14| A*26:16| A*26:17| A*26:19| A*26:20| A*26:21| A*26:22| A*26:23| A*26:24| A*26:27| A*26:28| A*26:29| A*26:30| A*26:31| A*26:32| A*26:33| A*26:34| A*26:35| A*26:36| A*26:37| A*26:38| A*26:39| A*26:40| A*26:41| A*26:42| A*26:43| A*26:45| A*26:46| A*26:47| A*26:48| A*26:49| A*26:50| A*26:51| A*26:52| A*26:53| A*26:54| A*26:55| A*26:56| A*26:57| A*26:58| A*26:59| A*26:61| A*26:62| A*26:63| A*26:64| A*26:65| A*26:66| A*26:67| A*26:68| A*26:69| A*26:70| A*26:72| A*26:73| A*26:74| A*26:75| A*26:76| A*26:77| A*26:78| A*26:79| A*26:80| A*26:81| A*26:82| A*26:83| A*26:84| A*26:85| A*26:86| A*26:87| A*26:88| A*26:89| A*26:90| A*26:91| A*26:93| A*26:94| A*26:95| A*26:96| A*26:97| A*26:98| A*26:99| A*26:100| A*26:101| A*26:102| A*26:103| A*26:104| A*26:105| A*26:106| A*26:108| A*26:109| A*26:110| A*26:111| A*26:112| A*26:113| A*26:114| A*26:115| A*26:116| A*26:117| A*26:118| A*26:119| A*26:120| A*26:121| A*26:122| A*26:123| A*26:124| A*26:125| A*26:126| A*26:128| A*26:129| A*26:130| A*26:131| A*26:132| A*26:133| A*26:134| A*26:135| A*26:136| A*26:137| A*26:138| A*26:139| A*26:140| A*26:141| A*26:142| A*26:143| A*26:144| A*26:146| A*26:147| A*26:148| A*26:149| A*66:05| A*34:01| A*34:02| A*34:03| A*34:04| A*34:05| A*34:07| A*34:08| A*34:09| A*34:11| A*34:12| A*34:13| A*34:14| A*34:15| A*34:16| A*34:17| A*66:04| A*66:06| A*66:07| A*66:09| A*66:10| A*66:11| A*66:12| A*66:13| A*66:14| A*66:15| A*66:16| A*66:17| A*66:18| A*66:19| A*66:20| A*66:21| A*66:22| A*66:23| A*66:24| A*66:25| A*66:26Q| A*66:29| A*66:01| A*66:02| A*43:01</t>
-  </si>
-  <si>
-    <t>A*29:01| A*29:02| A*29:03| A*29:04| A*29:05| A*29:06| A*29:07| A*29:09| A*29:10| A*29:11| A*29:12| A*29:13| A*29:14| A*29:15| A*29:16| A*29:17| A*29:18| A*29:19| A*29:20| A*29:21| A*29:22| A*29:23| A*29:24| A*29:25| A*29:26| A*29:27| A*29:28| A*29:29| A*29:30| A*29:31| A*29:32| A*29:33| A*29:34| A*29:35| A*29:36| A*29:37| A*29:38| A*29:39| A*29:40| A*29:41| A*29:42| A*29:43| A*29:44| A*29:45| A*29:46| A*29:47| A*29:48| A*29:49| A*29:50| A*29:51| A*29:52| A*29:53| A*29:54| A*29:55| A*29:56| A*29:57| A*29:58| A*29:59| A*29:60| A*29:61| A*29:62| A*29:63| A*29:64| A*29:65| A*29:66| A*29:67| A*29:68| A*29:69| A*29:70| A*29:71| A*29:72| A*29:73| A*29:74| A*29:75| A*29:76| A*29:77| A*29:79| A*29:80| A*29:81| A*29:82| A*29:83| A*29:84| A*29:85| A*29:86| A*29:87| A*29:88| A*29:89| A*29:90| A*29:91| A*29:92| A*29:93| A*29:94| A*29:95| A*29:96| A*29:97| A*29:98| A*29:99| A*29:100| A*29:101| A*29:102| A*29:103| A*29:104| A*29:105| A*29:106| A*29:107| A*29:108| A*29:109| A*29:110| A*29:111</t>
-  </si>
-  <si>
-    <t>A*30:01| A*30:02| A*30:03| A*30:04| A*30:06| A*30:07| A*30:08| A*30:09| A*30:10| A*30:11| A*30:12| A*30:13| A*30:14L| A*30:15| A*30:16| A*30:17| A*30:18| A*30:19| A*30:20| A*30:22| A*30:23| A*30:24| A*30:25| A*30:26| A*30:28| A*30:29| A*30:30| A*30:31| A*30:32| A*30:33| A*30:34| A*30:35| A*30:36| A*30:37| A*30:38| A*30:39| A*30:40| A*30:41| A*30:42| A*30:43| A*30:44| A*30:45| A*30:46| A*30:47| A*30:48| A*30:49| A*30:50| A*30:51| A*30:52| A*30:53| A*30:54| A*30:55| A*30:56| A*30:57| A*30:58| A*30:60| A*30:61| A*30:62| A*30:63| A*30:64| A*30:65| A*30:66| A*30:67| A*30:68| A*30:69| A*30:71| A*30:72| A*30:74| A*30:75| A*30:77| A*30:79| A*30:80| A*30:81| A*30:82| A*30:83| A*30:84| A*30:85| A*30:86| A*30:87| A*30:88| A*30:89| A*30:90| A*30:91| A*30:92| A*30:93| A*30:94| A*30:95| A*30:96| A*30:97| A*30:98| A*30:99| A*30:100| A*30:101Q| A*30:102| A*30:103| A*30:104| A*30:105| A*30:106| A*30:107| A*30:108| A*30:109| A*30:110| A*30:111| A*30:112| A*30:113| A*30:114| A*30:115| A*30:116| A*30:117| A*30:118| A*30:119| A*30:120| A*30:122| A*30:124| A*30:125| A*30:126| A*30:127</t>
-  </si>
-  <si>
-    <t>A*31:01| A*31:02| A*31:03| A*31:04| A*31:05| A*31:06| A*31:07| A*31:08| A*31:09| A*31:10| A*31:11| A*31:12| A*31:13| A*31:15| A*31:16| A*31:17| A*31:18| A*31:19| A*31:20| A*31:21| A*31:22| A*31:23| A*31:24| A*31:25| A*31:26| A*31:27| A*31:28| A*31:29| A*31:30| A*31:31| A*31:32| A*31:33| A*31:34| A*31:35| A*31:36| A*31:37| A*31:38| A*31:39| A*31:40| A*31:41| A*31:42| A*31:43| A*31:44| A*31:45| A*31:46| A*31:47| A*31:48| A*31:49| A*31:50| A*31:51| A*31:52| A*31:53| A*31:54| A*31:55| A*31:56| A*31:57| A*31:58| A*31:59| A*31:61| A*31:62| A*31:63| A*31:64| A*31:65| A*31:66| A*31:67| A*31:68| A*31:69| A*31:70| A*31:71| A*31:72| A*31:73| A*31:74| A*31:75| A*31:76| A*31:77| A*31:78| A*31:79| A*31:80| A*31:81| A*31:82| A*31:83| A*31:84| A*31:85| A*31:86| A*31:87| A*31:88| A*31:89| A*31:90| A*31:91| A*31:92| A*31:93| A*31:94| A*31:95| A*31:96| A*31:97| A*31:98| A*31:99| A*31:100| A*31:101| A*31:102| A*31:103| A*31:104| A*31:105| A*31:106| A*31:107| A*31:108| A*31:109| A*31:110| A*31:111| A*31:112| A*31:113| A*31:114| A*31:115| A*31:116| A*31:117| A*31:118| A*31:119| A*31:120| A*31:121| A*31:122| A*31:123| A*31:124| A*31:125| A*31:127| A*31:128| A*31:129| A*31:130| A*31:132| A*31:133</t>
-  </si>
-  <si>
-    <t>A*32:01| A*32:02| A*32:03| A*32:05| A*32:06| A*32:07| A*32:08| A*32:09| A*32:10| A*32:11Q| A*32:12| A*32:13| A*32:14| A*32:15| A*32:16| A*32:17| A*32:18| A*32:20| A*32:21| A*32:22| A*32:23| A*32:24| A*32:25| A*32:26| A*32:28| A*32:29| A*32:30| A*32:31| A*32:32| A*32:33| A*32:34| A*32:35| A*32:36| A*32:37| A*32:38| A*32:39| A*32:40| A*32:41| A*32:42| A*32:43| A*32:44| A*32:46| A*32:47| A*32:49| A*32:50| A*32:51| A*32:52| A*32:53| A*32:54| A*32:55| A*32:57| A*32:58| A*32:59| A*32:60| A*32:61| A*32:62| A*32:63| A*32:64| A*32:65| A*32:66| A*32:67| A*32:68| A*32:69| A*32:70| A*32:71| A*32:72| A*32:73| A*32:74| A*32:75| A*32:76| A*32:77| A*32:78| A*32:79| A*32:80| A*32:81| A*32:82| A*32:83| A*32:84| A*32:85| A*32:86| A*32:87| A*32:88| A*32:89| A*32:90| A*32:91| A*32:93| A*32:94| A*32:95| A*32:96| A*32:97| A*32:98| A*32:99| A*32:100| A*32:101Q| A*32:102| A*32:103| A*32:104| A*32:105| A*32:106| A*32:107</t>
-  </si>
-  <si>
-    <t>A*33:01| A*33:03| A*33:03Q| A*33:04| A*33:05| A*33:06| A*33:07| A*33:08| A*33:10| A*33:11| A*33:12| A*33:13| A*33:14| A*33:15| A*33:16| A*33:17| A*33:18| A*33:19| A*33:20| A*33:21| A*33:22| A*33:23| A*33:24| A*33:25| A*33:26| A*33:27| A*33:28| A*33:29| A*33:30| A*33:31| A*33:32| A*33:33| A*33:34| A*33:35| A*33:36| A*33:37| A*33:39| A*33:40| A*33:41| A*33:42| A*33:43| A*33:44| A*33:45| A*33:46| A*33:47| A*33:48| A*33:49| A*33:50| A*33:51| A*33:52| A*33:53| A*33:54| A*33:55| A*33:56| A*33:57| A*33:58| A*33:59| A*33:60| A*33:61| A*33:62| A*33:63| A*33:64| A*33:65| A*33:66| A*33:67| A*33:68| A*33:69| A*33:70| A*33:71| A*33:72| A*33:75| A*33:76| A*33:77| A*33:78| A*33:79| A*33:81| A*33:82| A*33:83| A*33:84| A*33:85| A*33:86| A*33:87| A*33:88| A*33:89| A*33:90| A*33:91| A*33:92| A*33:93| A*33:94| A*33:95| A*33:97| A*33:98| A*33:99| A*33:100| A*33:101| A*33:102| A*33:103| A*33:104| A*33:105| A*33:106| A*33:107| A*33:108| A*33:109| A*33:110| A*33:111| A*33:112| A*33:113| A*33:114| A*33:115| A*33:116| A*33:117| A*33:118| A*33:119| A*33:120| A*33:121| A*33:122| A*33:124| A*33:125| A*33:126| A*33:127| A*33:128| A*33:130| A*33:131| A*33:132| A*33:133| A*33:134| A*33:135| A*33:136| A*33:137</t>
-  </si>
-  <si>
-    <t>A*33:09| A*29:01| A*29:02| A*29:03| A*29:04| A*29:05| A*29:06| A*29:07| A*29:09| A*29:10| A*29:11| A*29:12| A*29:13| A*29:14| A*29:15| A*29:16| A*29:17| A*29:18| A*29:19| A*29:20| A*29:21| A*29:22| A*29:23| A*29:24| A*29:25| A*29:26| A*29:27| A*29:28| A*29:29| A*29:30| A*29:31| A*29:32| A*29:33| A*29:34| A*29:35| A*29:36| A*29:37| A*29:38| A*29:39| A*29:40| A*29:41| A*29:42| A*29:43| A*29:44| A*29:45| A*29:46| A*29:47| A*29:48| A*29:49| A*29:50| A*29:51| A*29:52| A*29:53| A*29:54| A*29:55| A*29:56| A*29:57| A*29:58| A*29:59| A*29:60| A*29:61| A*29:62| A*29:63| A*29:64| A*29:65| A*29:66| A*29:67| A*29:68| A*29:69| A*29:70| A*29:71| A*29:72| A*29:73| A*29:74| A*29:75| A*29:76| A*29:77| A*29:79| A*29:80| A*29:81| A*29:82| A*29:83| A*29:84| A*29:85| A*29:86| A*29:87| A*29:88| A*29:89| A*29:90| A*29:91| A*29:92| A*29:93| A*29:94| A*29:95| A*29:96| A*29:97| A*29:98| A*29:99| A*29:100| A*29:101| A*29:102| A*29:103| A*29:104| A*29:105| A*29:106| A*29:107| A*29:108| A*29:109| A*29:110| A*29:111| A*30:01| A*30:02| A*30:03| A*30:04| A*30:06| A*30:07| A*30:08| A*30:09| A*30:10| A*30:11| A*30:12| A*30:13| A*30:14L| A*30:15| A*30:16| A*30:17| A*30:18| A*30:19| A*30:20| A*30:22| A*30:23| A*30:24| A*30:25| A*30:26| A*30:28| A*30:29| A*30:30| A*30:31| A*30:32| A*30:33| A*30:34| A*30:35| A*30:36| A*30:37| A*30:38| A*30:39| A*30:40| A*30:41| A*30:42| A*30:43| A*30:44| A*30:45| A*30:46| A*30:47| A*30:48| A*30:49| A*30:50| A*30:51| A*30:52| A*30:53| A*30:54| A*30:55| A*30:56| A*30:57| A*30:58| A*30:60| A*30:61| A*30:62| A*30:63| A*30:64| A*30:65| A*30:66| A*30:67| A*30:68| A*30:69| A*30:71| A*30:72| A*30:74| A*30:75| A*30:77| A*30:79| A*30:80| A*30:81| A*30:82| A*30:83| A*30:84| A*30:85| A*30:86| A*30:87| A*30:88| A*30:89| A*30:90| A*30:91| A*30:92| A*30:93| A*30:94| A*30:95| A*30:96| A*30:97| A*30:98| A*30:99| A*30:100| A*30:101Q| A*30:102| A*30:103| A*30:104| A*30:105| A*30:106| A*30:107| A*30:108| A*30:109| A*30:110| A*30:111| A*30:112| A*30:113| A*30:114| A*30:115| A*30:116| A*30:117| A*30:118| A*30:119| A*30:120| A*30:122| A*30:124| A*30:125| A*30:126| A*30:127| A*31:01| A*31:02| A*31:03| A*31:04| A*31:05| A*31:06| A*31:07| A*31:08| A*31:09| A*31:10| A*31:11| A*31:12| A*31:13| A*31:15| A*31:16| A*31:17| A*31:18| A*31:19| A*31:20| A*31:21| A*31:22| A*31:23| A*31:24| A*31:25| A*31:26| A*31:27| A*31:28| A*31:29| A*31:30| A*31:31| A*31:32| A*31:33| A*31:34| A*31:35| A*31:36| A*31:37| A*31:38| A*31:39| A*31:40| A*31:41| A*31:42| A*31:43| A*31:44| A*31:45| A*31:46| A*31:47| A*31:48| A*31:49| A*31:50| A*31:51| A*31:52| A*31:53| A*31:54| A*31:55| A*31:56| A*31:57| A*31:58| A*31:59| A*31:61| A*31:62| A*31:63| A*31:64| A*31:65| A*31:66| A*31:67| A*31:68| A*31:69| A*31:70| A*31:71| A*31:72| A*31:73| A*31:74| A*31:75| A*31:76| A*31:77| A*31:78| A*31:79| A*31:80| A*31:81| A*31:82| A*31:83| A*31:84| A*31:85| A*31:86| A*31:87| A*31:88| A*31:89| A*31:90| A*31:91| A*31:92| A*31:93| A*31:94| A*31:95| A*31:96| A*31:97| A*31:98| A*31:99| A*31:100| A*31:101| A*31:102| A*31:103| A*31:104| A*31:105| A*31:106| A*31:107| A*31:108| A*31:109| A*31:110| A*31:111| A*31:112| A*31:113| A*31:114| A*31:115| A*31:116| A*31:117| A*31:118| A*31:119| A*31:120| A*31:121| A*31:122| A*31:123| A*31:124| A*31:125| A*31:127| A*31:128| A*31:129| A*31:130| A*31:132| A*31:133| A*32:01| A*32:02| A*32:03| A*32:05| A*32:06| A*32:07| A*32:08| A*32:09| A*32:10| A*32:11Q| A*32:12| A*32:13| A*32:14| A*32:15| A*32:16| A*32:17| A*32:18| A*32:20| A*32:21| A*32:22| A*32:23| A*32:24| A*32:25| A*32:26| A*32:28| A*32:29| A*32:30| A*32:31| A*32:32| A*32:33| A*32:34| A*32:35| A*32:36| A*32:37| A*32:38| A*32:39| A*32:40| A*32:41| A*32:42| A*32:43| A*32:44| A*32:46| A*32:47| A*32:49| A*32:50| A*32:51| A*32:52| A*32:53| A*32:54| A*32:55| A*32:57| A*32:58| A*32:59| A*32:60| A*32:61| A*32:62| A*32:63| A*32:64| A*32:65| A*32:66| A*32:67| A*32:68| A*32:69| A*32:70| A*32:71| A*32:72| A*32:73| A*32:74| A*32:75| A*32:76| A*32:77| A*32:78| A*32:79| A*32:80| A*32:81| A*32:82| A*32:83| A*32:84| A*32:85| A*32:86| A*32:87| A*32:88| A*32:89| A*32:90| A*32:91| A*32:93| A*32:94| A*32:95| A*32:96| A*32:97| A*32:98| A*32:99| A*32:100| A*32:101Q| A*32:102| A*32:103| A*32:104| A*32:105| A*32:106| A*32:107| A*33:01| A*33:03| A*33:03Q| A*33:04| A*33:05| A*33:06| A*33:07| A*33:08| A*33:10| A*33:11| A*33:12| A*33:13| A*33:14| A*33:15| A*33:16| A*33:17| A*33:18| A*33:19| A*33:20| A*33:21| A*33:22| A*33:23| A*33:24| A*33:25| A*33:26| A*33:27| A*33:28| A*33:29| A*33:30| A*33:31| A*33:32| A*33:33| A*33:34| A*33:35| A*33:36| A*33:37| A*33:39| A*33:40| A*33:41| A*33:42| A*33:43| A*33:44| A*33:45| A*33:46| A*33:47| A*33:48| A*33:49| A*33:50| A*33:51| A*33:52| A*33:53| A*33:54| A*33:55| A*33:56| A*33:57| A*33:58| A*33:59| A*33:60| A*33:61| A*33:62| A*33:63| A*33:64| A*33:65| A*33:66| A*33:67| A*33:68| A*33:69| A*33:70| A*33:71| A*33:72| A*33:75| A*33:76| A*33:77| A*33:78| A*33:79| A*33:81| A*33:82| A*33:83| A*33:84| A*33:85| A*33:86| A*33:87| A*33:88| A*33:89| A*33:90| A*33:91| A*33:92| A*33:93| A*33:94| A*33:95| A*33:97| A*33:98| A*33:99| A*33:100| A*33:101| A*33:102| A*33:103| A*33:104| A*33:105| A*33:106| A*33:107| A*33:108| A*33:109| A*33:110| A*33:111| A*33:112| A*33:113| A*33:114| A*33:115| A*33:116| A*33:117| A*33:118| A*33:119| A*33:120| A*33:121| A*33:122| A*33:124| A*33:125| A*33:126| A*33:127| A*33:128| A*33:130| A*33:131| A*33:132| A*33:133| A*33:134| A*33:135| A*33:136| A*33:137| A*74:01| A*74:02| A*74:03| A*74:04| A*74:05| A*74:06| A*74:07| A*74:08| A*74:09| A*74:10| A*74:11| A*74:13| A*74:15| A*74:16| A*74:17| A*74:18| A*74:19| A*74:20| A*74:21| A*74:22| A*74:23| A*74:24| A*74:25| A*74:26| A*74:27| A*74:28</t>
-  </si>
-  <si>
-    <t>A*34:01| A*34:02| A*34:03| A*34:04| A*34:05| A*34:07| A*34:08| A*34:09| A*34:11| A*34:12| A*34:13| A*34:14| A*34:15| A*34:16| A*34:17</t>
-  </si>
-  <si>
-    <t>A*36:01| A*36:02| A*36:03| A*36:04| A*36:05</t>
+    <t>A*66:01:01:01| A*66:01:01:02| A*66:01:02| A*66:01:03| A*66:01:04| A*66:01:05| A*66:04| A*66:06| A*66:07| A*66:09| A*66:10| A*66:11| A*66:12| A*66:13| A*66:14| A*66:15| A*66:16| A*66:17| A*66:18| A*66:19| A*66:20| A*66:21| A*66:22| A*66:23| A*66:24| A*66:25| A*66:26Q| A*66:29| A*66:30| A*66:31| A*66:32</t>
+  </si>
+  <si>
+    <t>A*66:02| A*66:04| A*66:06| A*66:07| A*66:09| A*66:10| A*66:11| A*66:12| A*66:13| A*66:14| A*66:15| A*66:16| A*66:17| A*66:18| A*66:19| A*66:20| A*66:21| A*66:22| A*66:23| A*66:24| A*66:25| A*66:26Q| A*66:29| A*66:30| A*66:31| A*66:32</t>
+  </si>
+  <si>
+    <t>A*01:01:01:02N| A*01:04:01:01N| A*01:04:01:02N| A*01:11N| A*01:15N| A*01:16N| A*01:18N| A*01:22N| A*01:27N| A*01:31N| A*01:52:01N| A*01:52:02N| A*01:53N| A*01:56N| A*01:57N| A*01:87N| A*01:123N| A*01:160N| A*01:162N| A*01:178N| A*01:179N| A*01:186N| A*01:240N| A*01:247N| A*01:250N| A*01:258N| A*01:269N| A*01:285N| A*01:287N| A*01:290N| A*01:293N| A*02:15N| A*02:32N| A*02:43N| A*02:53N| A*02:82N| A*02:83N| A*02:88N| A*02:94N| A*02:113:01N| A*02:113:02N| A*02:125N| A*02:222N| A*02:223N| A*02:225N| A*02:226N| A*02:227N| A*02:250N| A*02:284N| A*02:301N| A*02:305N| A*02:314N| A*02:321N| A*02:350N| A*02:356N| A*02:366N| A*02:373N| A*02:395N| A*02:439N| A*02:468:01N| A*02:468:02N| A*02:476N| A*02:490N| A*02:501N| A*02:506N| A*02:514N| A*02:516N| A*02:525N| A*02:540N| A*02:608N| A*02:622N| A*02:643N| A*02:675N| A*02:691N| A*02:696N| A*02:710N| A*02:715N| A*02:748N| A*02:760N| A*02:773N| A*02:775N| A*02:788N| A*02:789N| A*02:791N| A*02:792N| A*02:793N| A*02:796N| A*02:797N| A*02:803N| A*02:806N| A*02:807N| A*03:01:01:02N| A*03:03N| A*03:11N| A*03:21N| A*03:36N| A*03:68N| A*03:69N| A*03:91N| A*03:129N| A*03:161N| A*03:162N| A*03:168N| A*03:178N| A*03:192N| A*03:197N| A*03:262N| A*03:266N| A*03:269N| A*03:275N| A*03:279N| A*03:283N| A*03:284N| A*03:286N| A*03:297N| A*03:323N| A*03:329N| A*03:330N| A*03:334N| A*11:21N| A*11:69N| A*11:78N| A*11:99N| A*11:109N| A*11:115N| A*11:127N| A*11:137:01N| A*11:137:02N| A*11:180N| A*11:208N| A*11:210N| A*11:215N| A*11:238N| A*11:251N| A*11:287N| A*11:310N| A*23:07N| A*23:08N| A*23:11N| A*23:19N| A*23:38N| A*23:84N| A*23:91N| A*24:09N| A*24:11N| A*24:36N| A*24:40N| A*24:45N| A*24:48N| A*24:60N| A*24:83N| A*24:84N| A*24:86N| A*24:90:01N| A*24:90:02N| A*24:132N| A*24:155N| A*24:158N| A*24:163N| A*24:183N| A*24:185N| A*24:222N| A*24:232N| A*24:240N| A*24:252N| A*24:278N| A*24:303N| A*24:312N| A*24:323N| A*24:357N| A*24:359N| A*24:370N| A*24:388N| A*24:389N| A*24:396N| A*24:408N| A*24:425N| A*24:426N| A*24:427N| A*24:428N| A*24:429N| A*24:430N| A*24:433N| A*25:12N| A*25:42N| A*25:49N| A*26:01:01:03N| A*26:11N| A*26:25N| A*26:60N| A*26:71N| A*26:107N| A*26:127N| A*26:145N| A*26:161N| A*29:01:01:02N| A*29:08N| A*29:78N| A*29:112N| A*30:27N| A*30:59N| A*30:70N| A*30:73N| A*30:76N| A*30:78N| A*30:121N| A*30:123N| A*30:130N| A*30:132N| A*30:145N| A*31:01:02:03N| A*31:14N| A*31:60N| A*31:126N| A*31:131N| A*31:141N| A*31:149N| A*32:19N| A*32:27N| A*32:45N| A*32:48N| A*32:56N| A*32:92N| A*32:112N| A*32:117N| A*33:73N| A*33:74N| A*33:80N| A*33:96N| A*33:123N| A*33:129N| A*33:140N| A*33:143N| A*33:154N| A*33:156N| A*33:157N| A*34:10N| A*66:27N| A*66:28N| A*68:11N| A*68:18N| A*68:49N| A*68:59N| A*68:94N| A*68:120N| A*68:142N| A*68:171N| A*68:181N| A*68:182N| A*68:199N| A*68:203N| A*68:205N| A*74:12N| A*74:14N| A*74:32N</t>
+  </si>
+  <si>
+    <t>A*02:03:01| A*02:03:02| A*02:03:03| A*02:03:04| A*02:03:05| A*02:03:06| A*02:03:07| A*02:03:08</t>
+  </si>
+  <si>
+    <t>A*01:01:01:01| A*01:01:01:03| A*01:01:01:04| A*01:01:01:05| A*01:01:01:06| A*01:01:01:07| A*01:01:01:08| A*01:01:01:09| A*01:01:01:10| A*01:01:01:11| A*01:01:01:12| A*01:01:01:13| A*01:01:01:14| A*01:01:01:15| A*01:01:01:16| A*01:01:01:17| A*01:01:01:18| A*01:01:01:19| A*01:01:01:20| A*01:01:01:21| A*01:01:01:22| A*01:01:01:23| A*01:01:01:24| A*01:01:02| A*01:01:03| A*01:01:04| A*01:01:05| A*01:01:06| A*01:01:07| A*01:01:08| A*01:01:09| A*01:01:10| A*01:01:11| A*01:01:12| A*01:01:13| A*01:01:14| A*01:01:15| A*01:01:16| A*01:01:17| A*01:01:18| A*01:01:19| A*01:01:20| A*01:01:21| A*01:01:22| A*01:01:23| A*01:01:24| A*01:01:25| A*01:01:26| A*01:01:27| A*01:01:28| A*01:01:29| A*01:01:30| A*01:01:31| A*01:01:32| A*01:01:33| A*01:01:34| A*01:01:35| A*01:01:36| A*01:01:37| A*01:01:38L| A*01:01:39| A*01:01:40| A*01:01:41| A*01:01:42| A*01:01:43| A*01:01:44| A*01:01:45| A*01:01:46| A*01:01:47| A*01:01:48| A*01:01:49| A*01:01:50| A*01:01:51| A*01:01:52| A*01:01:53| A*01:01:54| A*01:01:55| A*01:01:56| A*01:01:57| A*01:01:58| A*01:01:59| A*01:01:60| A*01:01:61| A*01:01:62| A*01:01:63| A*01:01:64| A*01:01:65| A*01:01:66| A*01:01:67| A*01:01:68| A*01:01:69| A*01:01:70| A*01:01:71| A*01:01:72| A*01:01:73| A*01:01:74| A*01:01:75| A*01:01:76| A*01:01:77| A*01:01:78| A*01:01:79| A*01:01:80| A*01:01:81| A*01:01:82| A*01:01:83| A*01:01:84| A*01:01:85| A*01:01:86| A*01:01:87| A*01:01:88| A*01:01:89| A*01:01:90| A*01:01:91| A*01:01:92| A*01:01:93| A*01:01:94| A*01:01:95| A*01:01:96| A*01:01:97| A*01:01:98| A*01:01:99| A*01:01:100| A*01:01:101| A*01:02| A*01:03:01:01| A*01:03:01:02| A*01:06| A*01:07| A*01:08| A*01:09:01:01| A*01:09:01:02| A*01:09:02| A*01:10| A*01:12| A*01:13| A*01:14| A*01:17| A*01:19| A*01:20| A*01:21| A*01:23| A*01:24| A*01:25| A*01:26| A*01:28| A*01:29| A*01:30| A*01:32| A*01:33| A*01:35| A*01:36| A*01:37:01:01| A*01:37:01:02| A*01:38| A*01:39| A*01:40| A*01:41| A*01:42| A*01:43| A*01:44| A*01:45| A*01:46| A*01:47| A*01:48| A*01:49| A*01:50| A*01:51| A*01:54| A*01:55| A*01:58| A*01:59| A*01:60| A*01:61| A*01:62| A*01:63| A*01:64| A*01:65| A*01:66| A*01:67:01| A*01:67:02| A*01:68| A*01:69:01| A*01:69:02| A*01:70| A*01:71| A*01:72| A*01:73| A*01:74| A*01:75| A*01:76| A*01:77| A*01:78| A*01:79| A*01:80| A*01:81| A*01:82| A*01:83:01| A*01:83:02| A*01:84| A*01:85| A*01:86| A*01:88:01| A*01:88:02| A*01:88:03| A*01:89| A*01:90| A*01:91| A*01:92| A*01:93| A*01:94| A*01:95| A*01:96| A*01:97| A*01:98| A*01:99| A*01:100| A*01:101| A*01:102| A*01:103| A*01:104| A*01:105| A*01:106| A*01:107| A*01:108| A*01:109| A*01:110| A*01:111| A*01:112| A*01:113| A*01:114| A*01:115| A*01:116| A*01:117| A*01:118| A*01:119| A*01:120| A*01:121| A*01:122| A*01:124| A*01:125| A*01:126| A*01:127| A*01:128| A*01:129| A*01:130| A*01:131| A*01:132| A*01:133| A*01:134| A*01:135| A*01:136| A*01:137| A*01:138| A*01:139| A*01:140| A*01:141| A*01:142| A*01:143| A*01:144| A*01:145| A*01:146| A*01:147Q| A*01:148| A*01:149| A*01:150| A*01:151| A*01:152| A*01:153| A*01:154| A*01:155| A*01:156| A*01:157| A*01:158| A*01:159| A*01:161| A*01:163| A*01:164| A*01:165| A*01:166| A*01:167| A*01:168| A*01:169| A*01:170| A*01:171| A*01:172| A*01:173| A*01:174| A*01:175| A*01:176| A*01:177| A*01:180| A*01:181| A*01:182| A*01:183| A*01:184| A*01:185| A*01:187| A*01:188| A*01:189| A*01:190| A*01:191| A*01:192| A*01:193| A*01:194| A*01:195| A*01:196| A*01:197| A*01:198| A*01:199| A*01:200| A*01:201| A*01:202| A*01:203| A*01:204| A*01:205| A*01:206| A*01:207| A*01:208Q| A*01:209| A*01:210:01| A*01:210:02| A*01:211| A*01:212| A*01:213| A*01:214| A*01:215| A*01:216| A*01:217| A*01:218| A*01:219| A*01:220| A*01:221| A*01:222| A*01:223| A*01:224| A*01:225| A*01:226| A*01:227| A*01:228Q| A*01:229| A*01:230| A*01:231| A*01:232:01| A*01:232:02| A*01:233| A*01:234| A*01:235| A*01:236| A*01:237| A*01:238| A*01:239| A*01:241| A*01:242| A*01:243| A*01:244| A*01:245| A*01:246| A*01:248Q| A*01:249| A*01:251| A*01:252| A*01:253| A*01:254| A*01:255| A*01:256| A*01:257| A*01:259| A*01:260| A*01:261| A*01:262| A*01:263| A*01:264| A*01:265| A*01:266:01| A*01:266:02| A*01:267| A*01:268| A*01:270| A*01:271| A*01:272| A*01:273| A*01:274| A*01:275| A*01:276| A*01:277| A*01:278| A*01:279| A*01:280| A*01:281| A*01:282| A*01:283| A*01:284| A*01:286| A*01:288| A*01:289| A*01:291| A*01:292| A*01:294| A*01:295| A*01:296| A*01:297</t>
+  </si>
+  <si>
+    <t>A*26:10| A*26:15| A*26:18| A*26:26| A*26:92| A*34:06| A*66:03:01:01| A*66:03:01:02| A*66:08| A*25:01:01:01| A*25:01:01:02| A*25:01:01:03| A*25:01:01:04| A*25:01:01:05| A*25:01:02| A*25:01:03| A*25:01:04| A*25:01:05| A*25:01:06| A*25:01:07| A*25:01:08| A*25:01:09| A*25:01:10| A*25:01:11| A*25:01:12| A*25:01:13| A*25:01:14| A*25:02| A*25:03| A*25:04| A*25:05| A*25:06| A*25:07| A*25:08| A*25:09| A*25:10| A*25:11| A*25:13| A*25:14| A*25:15| A*25:16| A*25:17| A*25:18| A*25:19:01| A*25:19:02| A*25:20| A*25:21| A*25:22| A*25:23| A*25:24| A*25:25| A*25:26| A*25:27:01| A*25:27:02| A*25:28| A*25:29| A*25:30| A*25:31| A*25:32| A*25:33| A*25:34| A*25:35| A*25:36| A*25:37| A*25:38| A*25:39| A*25:40| A*25:41| A*25:43| A*25:44| A*25:45| A*25:46| A*25:47| A*25:48| A*25:50| A*25:51| A*25:52| A*25:53| A*25:54| A*25:55| A*25:56| A*25:57| A*26:01:01:01| A*26:01:01:02| A*26:01:01:04| A*26:01:01:05| A*26:01:01:06| A*26:01:01:07| A*26:01:01:08| A*26:01:01:09| A*26:01:01:10| A*26:01:01:11| A*26:01:01:12| A*26:01:01:13| A*26:01:02| A*26:01:03| A*26:01:04| A*26:01:05| A*26:01:06| A*26:01:07| A*26:01:08| A*26:01:09| A*26:01:10| A*26:01:11| A*26:01:12| A*26:01:13| A*26:01:14| A*26:01:15| A*26:01:16| A*26:01:17| A*26:01:18| A*26:01:19| A*26:01:20| A*26:01:21| A*26:01:22| A*26:01:23| A*26:01:24| A*26:01:25| A*26:01:26| A*26:01:27| A*26:01:28| A*26:01:29| A*26:01:30| A*26:01:31| A*26:01:32| A*26:01:33| A*26:01:34| A*26:01:35| A*26:01:36| A*26:01:37| A*26:01:38| A*26:01:39| A*26:01:40| A*26:01:41| A*26:01:42| A*26:01:43| A*26:01:44| A*26:01:45| A*26:01:46| A*26:01:47| A*26:01:48| A*26:01:49| A*26:01:50| A*26:01:51| A*26:01:52| A*26:01:53| A*26:01:54| A*26:02:01| A*26:02:02| A*26:03:01| A*26:04| A*26:05| A*26:06| A*26:07:01| A*26:07:02| A*26:08:01| A*26:08:02| A*26:08:03| A*26:09| A*26:12| A*26:13| A*26:14| A*26:16| A*26:17| A*26:19| A*26:20| A*26:21| A*26:22| A*26:23| A*26:24| A*26:27| A*26:28| A*26:29| A*26:30| A*26:31| A*26:32| A*26:33| A*26:34| A*26:35| A*26:36| A*26:37| A*26:38| A*26:39| A*26:40| A*26:41| A*26:42| A*26:43:01| A*26:43:02| A*26:45| A*26:46| A*26:47| A*26:48| A*26:49| A*26:50| A*26:51| A*26:52| A*26:53| A*26:54| A*26:55| A*26:56| A*26:57| A*26:58| A*26:59| A*26:61| A*26:62| A*26:63| A*26:64| A*26:65| A*26:66| A*26:67| A*26:68| A*26:69| A*26:70| A*26:72| A*26:73| A*26:74| A*26:75| A*26:76| A*26:77| A*26:78| A*26:79| A*26:80| A*26:81| A*26:82| A*26:83| A*26:84| A*26:85| A*26:86| A*26:87| A*26:88| A*26:89| A*26:90| A*26:91| A*26:93| A*26:94| A*26:95| A*26:96| A*26:97| A*26:98| A*26:99| A*26:100| A*26:101| A*26:102| A*26:103| A*26:104| A*26:105| A*26:106| A*26:108| A*26:109| A*26:110| A*26:111| A*26:112| A*26:113| A*26:114| A*26:115| A*26:116| A*26:117| A*26:118| A*26:119| A*26:120| A*26:121| A*26:122| A*26:123| A*26:124| A*26:125| A*26:126| A*26:128| A*26:129| A*26:130| A*26:131| A*26:132| A*26:133| A*26:134| A*26:135| A*26:136| A*26:137| A*26:138| A*26:139| A*26:140| A*26:141| A*26:142| A*26:143| A*26:144| A*26:146| A*26:147| A*26:148| A*26:149| A*26:150| A*26:151| A*26:152| A*26:153| A*26:154| A*26:155| A*26:156| A*26:157| A*26:158| A*26:159| A*26:160| A*26:162| A*26:163| A*26:164| A*26:165| A*26:166Q| A*26:167| A*26:168| A*26:169| A*26:170| A*26:171| A*26:172| A*26:173| A*26:174| A*26:175| A*26:176| A*26:177| A*26:178| A*66:05| A*34:01:01:01| A*34:01:01:02| A*34:01:02| A*34:02:01:01| A*34:02:01:02| A*34:02:02| A*34:02:03| A*34:02:04| A*34:03| A*34:04| A*34:05| A*34:07| A*34:08| A*34:09| A*34:11| A*34:12| A*34:13| A*34:14| A*34:15| A*34:16| A*34:17| A*34:18| A*34:19| A*34:20| A*34:21| A*66:04| A*66:06| A*66:07| A*66:09| A*66:10| A*66:11| A*66:12| A*66:13| A*66:14| A*66:15| A*66:16| A*66:17| A*66:18| A*66:19| A*66:20| A*66:21| A*66:22| A*66:23| A*66:24| A*66:25| A*66:26Q| A*66:29| A*66:30| A*66:31| A*66:32| A*66:01:01:01| A*66:01:01:02| A*66:01:02| A*66:01:03| A*66:01:04| A*66:01:05| A*66:02| A*43:01</t>
+  </si>
+  <si>
+    <t>A*11:01:01:01| A*11:01:01:02| A*11:01:01:03| A*11:01:01:04| A*11:01:01:05| A*11:01:01:06| A*11:01:01:07| A*11:01:01:08| A*11:01:01:09| A*11:01:01:10| A*11:01:01:11| A*11:01:01:12| A*11:01:01:13| A*11:01:01:14| A*11:01:01:15| A*11:01:02| A*11:01:03| A*11:01:04| A*11:01:05| A*11:01:06| A*11:01:07| A*11:01:08| A*11:01:09| A*11:01:10| A*11:01:11| A*11:01:12| A*11:01:13| A*11:01:14| A*11:01:15| A*11:01:16| A*11:01:17| A*11:01:18| A*11:01:19| A*11:01:20| A*11:01:21| A*11:01:22| A*11:01:23| A*11:01:24| A*11:01:25| A*11:01:26| A*11:01:27| A*11:01:28| A*11:01:29| A*11:01:30| A*11:01:31| A*11:01:32| A*11:01:33| A*11:01:34| A*11:01:35| A*11:01:36| A*11:01:37| A*11:01:38| A*11:01:39| A*11:01:40| A*11:01:41| A*11:01:42| A*11:01:43| A*11:01:44| A*11:01:45| A*11:01:46| A*11:01:47| A*11:01:48| A*11:01:49| A*11:01:50| A*11:01:51| A*11:01:52| A*11:01:53| A*11:01:54| A*11:01:55| A*11:01:56| A*11:01:57| A*11:01:58| A*11:01:59| A*11:01:60| A*11:01:61| A*11:01:62| A*11:01:63| A*11:01:64| A*11:01:65| A*11:01:66| A*11:01:67| A*11:01:68| A*11:01:69| A*11:01:70| A*11:01:71| A*11:01:72| A*11:01:73| A*11:01:74| A*11:01:75| A*11:01:76| A*11:01:77| A*11:01:78| A*11:01:79| A*11:01:80| A*11:01:81| A*11:01:82| A*11:01:83| A*11:01:84| A*11:01:85| A*11:01:86| A*11:02:01| A*11:02:02| A*11:02:03| A*11:02:04| A*11:02:05| A*11:02:06| A*11:03| A*11:04| A*11:05| A*11:06| A*11:07| A*11:08| A*11:09| A*11:10| A*11:11| A*11:12| A*11:13| A*11:14| A*11:15:01| A*11:15:02| A*11:16| A*11:17| A*11:18| A*11:19| A*11:20| A*11:22| A*11:23| A*11:24:01| A*11:24:02| A*11:25:01| A*11:25:02| A*11:26| A*11:27| A*11:29| A*11:30| A*11:31| A*11:32:01| A*11:32:02| A*11:33:01| A*11:33:02| A*11:34| A*11:35| A*11:36| A*11:37| A*11:38| A*11:39| A*11:40| A*11:41| A*11:42| A*11:43| A*11:44| A*11:45| A*11:46| A*11:47| A*11:48| A*11:49| A*11:50Q| A*11:51| A*11:52Q| A*11:54:01| A*11:54:02| A*11:55| A*11:56| A*11:57| A*11:58| A*11:59| A*11:60| A*11:61| A*11:62| A*11:63| A*11:64| A*11:65| A*11:66| A*11:67| A*11:68| A*11:70:01| A*11:70:02| A*11:71| A*11:72| A*11:73| A*11:74| A*11:75| A*11:76| A*11:77| A*11:79| A*11:80| A*11:81| A*11:82| A*11:83| A*11:84| A*11:85| A*11:86| A*11:87| A*11:88| A*11:89| A*11:90| A*11:91:01| A*11:91:02| A*11:92| A*11:93| A*11:94| A*11:95| A*11:96| A*11:97| A*11:98| A*11:100| A*11:101| A*11:102| A*11:103| A*11:104| A*11:105| A*11:106| A*11:107| A*11:108| A*11:110| A*11:111| A*11:112| A*11:113| A*11:114| A*11:116| A*11:117| A*11:118| A*11:119:01| A*11:119:02| A*11:120| A*11:121| A*11:122| A*11:123| A*11:124| A*11:125| A*11:126| A*11:128| A*11:129| A*11:130| A*11:131| A*11:132| A*11:133| A*11:134| A*11:135| A*11:136| A*11:138| A*11:139| A*11:140| A*11:141| A*11:142| A*11:143| A*11:144| A*11:145| A*11:146| A*11:147| A*11:148| A*11:149| A*11:150| A*11:151| A*11:152| A*11:153:01| A*11:153:02| A*11:154| A*11:155| A*11:156| A*11:157| A*11:158| A*11:159| A*11:160| A*11:161| A*11:162| A*11:163| A*11:164| A*11:165| A*11:166| A*11:167| A*11:168| A*11:169| A*11:170Q| A*11:171| A*11:172| A*11:173| A*11:174| A*11:175| A*11:176| A*11:177| A*11:178| A*11:179| A*11:181| A*11:182Q| A*11:183| A*11:184| A*11:185| A*11:186| A*11:187| A*11:188| A*11:189| A*11:190| A*11:191| A*11:192| A*11:193| A*11:194| A*11:195| A*11:196| A*11:197| A*11:198| A*11:199:01| A*11:199:02| A*11:200| A*11:201| A*11:202| A*11:203| A*11:204| A*11:205| A*11:206| A*11:207| A*11:209| A*11:211| A*11:212| A*11:213| A*11:214| A*11:216| A*11:217| A*11:218| A*11:219| A*11:220| A*11:221| A*11:222| A*11:223| A*11:224| A*11:225| A*11:226| A*11:227| A*11:228| A*11:229| A*11:230| A*11:231| A*11:232| A*11:233| A*11:234| A*11:235Q| A*11:236| A*11:237| A*11:239| A*11:240| A*11:241| A*11:242| A*11:243| A*11:244| A*11:245| A*11:246| A*11:247| A*11:248| A*11:249| A*11:250| A*11:252| A*11:253| A*11:254| A*11:255| A*11:256Q| A*11:257| A*11:258| A*11:259| A*11:260| A*11:261| A*11:262| A*11:263| A*11:264| A*11:265| A*11:266| A*11:267| A*11:268| A*11:269| A*11:270| A*11:271| A*11:272Q| A*11:273| A*11:274| A*11:275| A*11:276| A*11:277| A*11:278| A*11:279| A*11:280| A*11:281| A*11:282| A*11:283| A*11:284| A*11:285| A*11:286| A*11:288| A*11:289| A*11:290| A*11:291| A*11:292| A*11:293| A*11:294| A*11:295| A*11:296| A*11:297| A*11:298| A*11:299| A*11:300| A*11:301| A*11:302| A*11:303| A*11:304| A*11:305| A*11:306| A*11:307| A*11:308| A*11:309| A*11:311| A*11:312</t>
+  </si>
+  <si>
+    <t>A*33:09| A*29:01:01:01| A*29:01:01:03| A*29:01:02| A*29:01:03| A*29:01:04| A*29:01:05| A*29:01:06| A*29:01:07| A*29:01:08| A*29:01:09| A*29:01:10| A*29:01:11| A*29:02:01:01| A*29:02:01:02| A*29:02:01:03| A*29:02:01:04| A*29:02:01:05| A*29:02:01:06| A*29:02:02| A*29:02:03| A*29:02:04| A*29:02:05| A*29:02:06| A*29:02:07| A*29:02:08| A*29:02:09| A*29:02:10| A*29:02:11| A*29:02:12| A*29:02:13| A*29:02:14| A*29:02:15| A*29:02:16| A*29:02:17:01| A*29:02:17:02| A*29:02:18| A*29:02:19| A*29:02:20| A*29:02:21| A*29:02:22| A*29:02:23| A*29:02:24| A*29:02:25| A*29:02:26| A*29:03| A*29:04| A*29:05| A*29:06| A*29:07| A*29:09| A*29:10:01| A*29:10:02| A*29:11| A*29:12| A*29:13| A*29:14| A*29:15| A*29:16| A*29:17| A*29:18| A*29:19| A*29:20| A*29:21| A*29:22| A*29:23| A*29:24| A*29:25| A*29:26| A*29:27| A*29:28| A*29:29| A*29:30| A*29:31| A*29:32| A*29:33| A*29:34| A*29:35| A*29:36| A*29:37| A*29:38| A*29:39| A*29:40| A*29:41| A*29:42| A*29:43| A*29:44| A*29:45| A*29:46| A*29:47| A*29:48| A*29:49| A*29:50| A*29:51| A*29:52| A*29:53| A*29:54| A*29:55| A*29:56| A*29:57| A*29:58| A*29:59| A*29:60| A*29:61| A*29:62| A*29:63| A*29:64| A*29:65| A*29:66| A*29:67| A*29:68| A*29:69| A*29:70| A*29:71| A*29:72| A*29:73| A*29:74| A*29:75| A*29:76| A*29:77| A*29:79| A*29:80| A*29:81| A*29:82| A*29:83| A*29:84| A*29:85| A*29:86| A*29:87| A*29:88| A*29:89| A*29:90| A*29:91| A*29:92| A*29:93| A*29:94| A*29:95| A*29:96| A*29:97| A*29:98| A*29:99| A*29:100| A*29:101| A*29:102| A*29:103| A*29:104| A*29:105| A*29:106| A*29:107| A*29:108| A*29:109| A*29:110| A*29:111| A*29:113| A*29:114| A*29:115| A*29:116| A*29:117| A*29:118| A*29:119| A*29:120| A*29:121| A*29:122| A*29:123| A*29:124| A*29:125| A*29:126Q| A*29:127| A*29:128| A*30:01:01:01| A*30:01:01:02| A*30:01:02| A*30:01:03| A*30:01:04| A*30:01:05| A*30:01:06| A*30:01:07| A*30:01:08| A*30:01:09| A*30:01:10| A*30:01:11| A*30:01:12| A*30:02:01:01| A*30:02:01:02| A*30:02:01:03| A*30:02:01:04| A*30:02:02| A*30:02:03| A*30:02:04| A*30:02:05| A*30:02:06| A*30:02:07| A*30:02:08| A*30:02:09| A*30:02:10| A*30:02:11| A*30:02:12| A*30:02:13| A*30:02:14| A*30:02:15| A*30:02:16| A*30:02:17| A*30:02:18| A*30:02:19| A*30:02:20| A*30:02:21| A*30:03| A*30:04:01| A*30:04:02| A*30:06| A*30:07| A*30:08:01| A*30:08:02| A*30:09| A*30:10| A*30:11:01| A*30:11:02| A*30:12:01| A*30:12:02| A*30:13| A*30:14L| A*30:15| A*30:16| A*30:17| A*30:18| A*30:19| A*30:20| A*30:22| A*30:23| A*30:24| A*30:25| A*30:26| A*30:28| A*30:29| A*30:30| A*30:31| A*30:32| A*30:33| A*30:34| A*30:35| A*30:36| A*30:37| A*30:38| A*30:39| A*30:40| A*30:41| A*30:42| A*30:43| A*30:44| A*30:45| A*30:46| A*30:47| A*30:48| A*30:49| A*30:50| A*30:51| A*30:52| A*30:53| A*30:54| A*30:55| A*30:56| A*30:57| A*30:58| A*30:60| A*30:61| A*30:62| A*30:63| A*30:64| A*30:65| A*30:66| A*30:67| A*30:68| A*30:69| A*30:71| A*30:72| A*30:74| A*30:75| A*30:77| A*30:79| A*30:80| A*30:81| A*30:82| A*30:83| A*30:84| A*30:85| A*30:86| A*30:87| A*30:88| A*30:89| A*30:90| A*30:91| A*30:92| A*30:93| A*30:94| A*30:95| A*30:96| A*30:97| A*30:98| A*30:99| A*30:100| A*30:101Q| A*30:102| A*30:103| A*30:104| A*30:105| A*30:106| A*30:107| A*30:108| A*30:109| A*30:110| A*30:111| A*30:112| A*30:113| A*30:114| A*30:115| A*30:116| A*30:117| A*30:118| A*30:119| A*30:120| A*30:122| A*30:124| A*30:125| A*30:126| A*30:127| A*30:128| A*30:129| A*30:131| A*30:133| A*30:134| A*30:135| A*30:136| A*30:137| A*30:138| A*30:139| A*30:140| A*30:141| A*30:142| A*30:143| A*30:144| A*31:01:02:01| A*31:01:02:02| A*31:01:02:04| A*31:01:02:05| A*31:01:02:06| A*31:01:02:07| A*31:01:02:08| A*31:01:02:09| A*31:01:02:10| A*31:01:03| A*31:01:04| A*31:01:05| A*31:01:06| A*31:01:07| A*31:01:08| A*31:01:09| A*31:01:10| A*31:01:11| A*31:01:12| A*31:01:13| A*31:01:14| A*31:01:15| A*31:01:16| A*31:01:17| A*31:01:18| A*31:01:19| A*31:01:20| A*31:01:21| A*31:01:22| A*31:01:23| A*31:01:24| A*31:01:25| A*31:01:26| A*31:01:27| A*31:01:28| A*31:01:29| A*31:01:30| A*31:01:31| A*31:01:32| A*31:01:33| A*31:02| A*31:03| A*31:04| A*31:05| A*31:06| A*31:07| A*31:08| A*31:09| A*31:10| A*31:11| A*31:12| A*31:13| A*31:15| A*31:16| A*31:17| A*31:18| A*31:19| A*31:20| A*31:21| A*31:22| A*31:23| A*31:24| A*31:25| A*31:26| A*31:27| A*31:28| A*31:29| A*31:30| A*31:31| A*31:32| A*31:33| A*31:34| A*31:35| A*31:36| A*31:37| A*31:38| A*31:39| A*31:40| A*31:41| A*31:42| A*31:43| A*31:44| A*31:45| A*31:46| A*31:47| A*31:48| A*31:49| A*31:50| A*31:51| A*31:52| A*31:53| A*31:54| A*31:55| A*31:56| A*31:57| A*31:58| A*31:59| A*31:61| A*31:62| A*31:63| A*31:64| A*31:65| A*31:66| A*31:67| A*31:68| A*31:69| A*31:70| A*31:71| A*31:72| A*31:73| A*31:74| A*31:75| A*31:76| A*31:77| A*31:78| A*31:79| A*31:80| A*31:81| A*31:82| A*31:83| A*31:84| A*31:85| A*31:86| A*31:87| A*31:88| A*31:89| A*31:90| A*31:91| A*31:92| A*31:93| A*31:94| A*31:95| A*31:96| A*31:97| A*31:98| A*31:99| A*31:100| A*31:101| A*31:102| A*31:103| A*31:104| A*31:105| A*31:106| A*31:107| A*31:108| A*31:109| A*31:110| A*31:111| A*31:112| A*31:113| A*31:114| A*31:115| A*31:116| A*31:117| A*31:118| A*31:119| A*31:120| A*31:121| A*31:122| A*31:123| A*31:124| A*31:125| A*31:127| A*31:128| A*31:129| A*31:130| A*31:132| A*31:133| A*31:134| A*31:135| A*31:136| A*31:137| A*31:138| A*31:139| A*31:140| A*31:142| A*31:143| A*31:144| A*31:145| A*31:146| A*31:147| A*31:148| A*32:01:01:01| A*32:01:01:02| A*32:01:01:03| A*32:01:01:04| A*32:01:01:05| A*32:01:01:06| A*32:01:01:07| A*32:01:01:08| A*32:01:01:09| A*32:01:01:10| A*32:01:02| A*32:01:03| A*32:01:04| A*32:01:05| A*32:01:06| A*32:01:07| A*32:01:08| A*32:01:09| A*32:01:10| A*32:01:11| A*32:01:12| A*32:01:13| A*32:01:14| A*32:01:15| A*32:01:16| A*32:01:17| A*32:01:18| A*32:01:19| A*32:01:20| A*32:01:21| A*32:01:22| A*32:01:23| A*32:01:24| A*32:01:25| A*32:01:26| A*32:01:27| A*32:01:28| A*32:01:29| A*32:01:30| A*32:01:31| A*32:01:32| A*32:01:33| A*32:02| A*32:03| A*32:05| A*32:06| A*32:07| A*32:08| A*32:09| A*32:10| A*32:11Q| A*32:12| A*32:13| A*32:14| A*32:15| A*32:16| A*32:17| A*32:18| A*32:20| A*32:21| A*32:22| A*32:23| A*32:24| A*32:25| A*32:26:01| A*32:26:02| A*32:28| A*32:29| A*32:30:01| A*32:30:02| A*32:31| A*32:32| A*32:33:01| A*32:33:02| A*32:34| A*32:35| A*32:36| A*32:37| A*32:38| A*32:39| A*32:40| A*32:41| A*32:42| A*32:43| A*32:44| A*32:46| A*32:47| A*32:49| A*32:50| A*32:51| A*32:52| A*32:53| A*32:54| A*32:55:01| A*32:55:02| A*32:57| A*32:58| A*32:59| A*32:60| A*32:61| A*32:62| A*32:63| A*32:64| A*32:65| A*32:66| A*32:67| A*32:68| A*32:69| A*32:70| A*32:71| A*32:72| A*32:73| A*32:74| A*32:75| A*32:76| A*32:77| A*32:78| A*32:79| A*32:80| A*32:81| A*32:82| A*32:83| A*32:84| A*32:85| A*32:86| A*32:87| A*32:88| A*32:89| A*32:90| A*32:91| A*32:93| A*32:94| A*32:95| A*32:96| A*32:97| A*32:98| A*32:99| A*32:100| A*32:101Q| A*32:102| A*32:103| A*32:104| A*32:105| A*32:106| A*32:107| A*32:108| A*32:109| A*32:110| A*32:111| A*32:113| A*32:114| A*32:115| A*32:116| A*32:118| A*32:119| A*32:120| A*32:121| A*33:01:01:01| A*33:01:01:02| A*33:01:02| A*33:01:03| A*33:01:04| A*33:01:05| A*33:01:06| A*33:01:07| A*33:01:08| A*33:01:09| A*33:01:10| A*33:01:11| A*33:01:12| A*33:03:01:01| A*33:03:01:02| A*33:03:01:03| A*33:03:01:04| A*33:03:01:05| A*33:03:02| A*33:03:03Q| A*33:03:04| A*33:03:05| A*33:03:06| A*33:03:07| A*33:03:08| A*33:03:09| A*33:03:10| A*33:03:11| A*33:03:12| A*33:03:13| A*33:03:14| A*33:03:15| A*33:03:16| A*33:03:17| A*33:03:18| A*33:03:19| A*33:03:20| A*33:03:21| A*33:03:22| A*33:03:23| A*33:03:24| A*33:03:25| A*33:03:26| A*33:03:27| A*33:03:28| A*33:03:29| A*33:03:30| A*33:03:31| A*33:03:32| A*33:03:33| A*33:03:34| A*33:03:35| A*33:03:36| A*33:03:37| A*33:03:38| A*33:04| A*33:05| A*33:06| A*33:07| A*33:08| A*33:10| A*33:11| A*33:12| A*33:13| A*33:14| A*33:15| A*33:16| A*33:17| A*33:18:01| A*33:18:02| A*33:19| A*33:20| A*33:21| A*33:22| A*33:23| A*33:24| A*33:25| A*33:26| A*33:27| A*33:28| A*33:29| A*33:30| A*33:31| A*33:32:01| A*33:32:02| A*33:33| A*33:34| A*33:35| A*33:36| A*33:37| A*33:39| A*33:40| A*33:41| A*33:42| A*33:43| A*33:44| A*33:45| A*33:46| A*33:47| A*33:48| A*33:49| A*33:50| A*33:51| A*33:52| A*33:53| A*33:54| A*33:55| A*33:56| A*33:57| A*33:58| A*33:59| A*33:60| A*33:61| A*33:62| A*33:63| A*33:64| A*33:65| A*33:66| A*33:67| A*33:68| A*33:69| A*33:70| A*33:71| A*33:72| A*33:75| A*33:76| A*33:77| A*33:78| A*33:79| A*33:81| A*33:82| A*33:83| A*33:84| A*33:85| A*33:86| A*33:87| A*33:88| A*33:89| A*33:90| A*33:91| A*33:92| A*33:93| A*33:94| A*33:95| A*33:97| A*33:98| A*33:99| A*33:100| A*33:101| A*33:102| A*33:103| A*33:104| A*33:105| A*33:106| A*33:107| A*33:108| A*33:109| A*33:110| A*33:111| A*33:112| A*33:113| A*33:114| A*33:115| A*33:116| A*33:117| A*33:118| A*33:119| A*33:120| A*33:121| A*33:122| A*33:124| A*33:125| A*33:126| A*33:127| A*33:128| A*33:130| A*33:131| A*33:132| A*33:133| A*33:134| A*33:135| A*33:136| A*33:137| A*33:138| A*33:139| A*33:141| A*33:142| A*33:144| A*33:145| A*33:146| A*33:147| A*33:148| A*33:149| A*33:150| A*33:151| A*33:152| A*33:153| A*33:155| A*33:158| A*33:159| A*33:160| A*33:161| A*33:162| A*33:163| A*33:164| A*33:165| A*33:166| A*33:167| A*33:168| A*33:169| A*33:170| A*74:01:01:01| A*74:01:01:02| A*74:01:01:03| A*74:01:01:04| A*74:01:02| A*74:01:03| A*74:01:04| A*74:01:05| A*74:01:06| A*74:01:07| A*74:01:08| A*74:02:01:01| A*74:02:01:02| A*74:03| A*74:04| A*74:05| A*74:06| A*74:07| A*74:08| A*74:09| A*74:10| A*74:11| A*74:13| A*74:15| A*74:16:01| A*74:16:02| A*74:17| A*74:18| A*74:19| A*74:20| A*74:21| A*74:22| A*74:23| A*74:24| A*74:25| A*74:26| A*74:27| A*74:28| A*74:29| A*74:30| A*74:31| A*74:33| A*74:34</t>
+  </si>
+  <si>
+    <t>A*02:01:01:01| A*02:01:01:02L| A*02:01:01:03| A*02:01:01:04| A*02:01:01:05| A*02:01:01:06| A*02:01:01:07| A*02:01:01:08| A*02:01:01:09| A*02:01:01:10| A*02:01:01:11| A*02:01:01:12| A*02:01:01:13| A*02:01:01:14| A*02:01:01:15| A*02:01:01:16| A*02:01:01:17| A*02:01:01:18| A*02:01:01:19| A*02:01:01:20| A*02:01:01:21| A*02:01:01:22| A*02:01:01:23| A*02:01:01:24| A*02:01:01:25| A*02:01:01:26| A*02:01:01:27| A*02:01:01:28| A*02:01:01:29| A*02:01:01:30| A*02:01:01:31| A*02:01:01:32| A*02:01:01:33| A*02:01:01:34| A*02:01:01:35| A*02:01:01:36| A*02:01:01:37| A*02:01:01:38| A*02:01:01:39| A*02:01:01:40| A*02:01:01:41| A*02:01:01:42| A*02:01:01:43| A*02:01:01:44| A*02:01:01:45| A*02:01:01:46| A*02:01:01:47| A*02:01:01:48| A*02:01:01:49| A*02:01:01:50| A*02:01:01:51| A*02:01:01:52| A*02:01:01:53| A*02:01:01:54| A*02:01:01:55| A*02:01:02| A*02:01:03| A*02:01:04| A*02:01:05| A*02:01:06| A*02:01:07| A*02:01:08| A*02:01:09| A*02:01:10| A*02:01:11| A*02:01:12| A*02:01:13| A*02:01:14Q| A*02:01:15| A*02:01:17| A*02:01:18| A*02:01:19| A*02:01:21| A*02:01:22| A*02:01:23| A*02:01:24| A*02:01:25| A*02:01:26| A*02:01:27| A*02:01:28| A*02:01:29| A*02:01:30| A*02:01:31| A*02:01:32| A*02:01:33| A*02:01:34| A*02:01:35| A*02:01:36| A*02:01:37| A*02:01:38| A*02:01:39| A*02:01:40| A*02:01:41| A*02:01:42| A*02:01:43| A*02:01:44| A*02:01:45| A*02:01:46| A*02:01:47| A*02:01:48| A*02:01:49| A*02:01:50| A*02:01:51| A*02:01:52| A*02:01:53| A*02:01:54| A*02:01:55| A*02:01:56| A*02:01:57| A*02:01:58| A*02:01:59| A*02:01:60| A*02:01:61| A*02:01:62| A*02:01:63| A*02:01:64| A*02:01:65| A*02:01:66| A*02:01:67| A*02:01:68| A*02:01:69| A*02:01:70| A*02:01:71| A*02:01:72| A*02:01:73| A*02:01:74| A*02:01:75| A*02:01:76| A*02:01:77| A*02:01:78| A*02:01:79| A*02:01:80| A*02:01:81| A*02:01:83| A*02:01:84| A*02:01:85| A*02:01:86| A*02:01:87| A*02:01:88| A*02:01:89| A*02:01:90| A*02:01:91| A*02:01:92| A*02:01:93| A*02:01:94| A*02:01:95| A*02:01:96| A*02:01:97| A*02:01:98| A*02:01:99| A*02:01:100| A*02:01:101| A*02:01:102| A*02:01:103| A*02:01:104| A*02:01:105| A*02:01:106| A*02:01:107| A*02:01:108| A*02:01:109| A*02:01:110| A*02:01:111| A*02:01:112| A*02:01:113| A*02:01:114| A*02:01:115| A*02:01:116| A*02:01:117| A*02:01:118| A*02:01:119| A*02:01:120| A*02:01:121| A*02:01:122| A*02:01:123| A*02:01:124| A*02:01:125| A*02:01:126| A*02:01:127| A*02:01:128| A*02:01:129| A*02:01:130| A*02:01:131| A*02:01:132| A*02:01:133| A*02:01:134| A*02:01:135| A*02:01:136| A*02:01:137| A*02:01:138| A*02:01:139| A*02:01:140| A*02:01:141| A*02:01:142| A*02:01:143| A*02:01:144| A*02:01:145| A*02:01:146| A*02:01:147| A*02:01:148| A*02:01:149| A*02:01:150| A*02:01:151| A*02:01:152| A*02:01:153| A*02:01:154| A*02:01:155| A*02:01:156| A*02:01:157| A*02:01:158| A*02:01:159| A*02:01:160| A*02:01:161| A*02:02:01:01| A*02:02:01:02| A*02:02:01:03| A*02:02:01:04| A*02:02:02| A*02:02:03| A*02:02:04| A*02:04| A*02:05:01:01| A*02:05:01:02| A*02:05:02| A*02:05:03| A*02:05:04| A*02:05:05| A*02:05:06| A*02:05:07| A*02:05:08| A*02:05:09| A*02:06:01:01| A*02:06:01:02| A*02:06:01:03| A*02:06:01:04| A*02:06:01:05| A*02:06:01:06| A*02:06:02| A*02:06:03| A*02:06:04| A*02:06:05| A*02:06:06| A*02:06:07| A*02:06:08| A*02:06:09| A*02:06:10| A*02:06:11| A*02:06:12| A*02:06:13| A*02:06:14| A*02:06:15| A*02:06:16| A*02:06:17| A*02:06:18| A*02:06:19| A*02:06:20| A*02:06:21| A*02:06:22| A*02:06:23| A*02:06:24| A*02:06:25| A*02:06:26| A*02:06:27| A*02:07:01| A*02:07:02| A*02:07:03| A*02:07:04| A*02:07:05| A*02:07:06| A*02:07:07| A*02:07:08| A*02:07:09| A*02:07:10| A*02:07:11| A*02:07:12| A*02:08| A*02:09:01:01| A*02:09:01:02| A*02:10| A*02:11:01:01| A*02:11:01:02| A*02:11:02| A*02:11:03| A*02:11:04| A*02:11:05| A*02:11:06| A*02:11:07| A*02:11:08| A*02:11:09| A*02:12| A*02:13| A*02:14| A*02:16| A*02:17:02| A*02:17:03| A*02:17:04| A*02:18| A*02:19| A*02:20:01| A*02:20:02| A*02:21| A*02:22:01:01| A*02:22:01:02| A*02:22:02| A*02:24:01| A*02:24:02| A*02:25| A*02:26| A*02:27| A*02:28| A*02:29| A*02:30:01| A*02:30:02| A*02:31| A*02:33| A*02:34| A*02:35:01| A*02:35:02| A*02:35:03| A*02:36| A*02:37| A*02:38| A*02:39| A*02:40:01| A*02:40:02| A*02:41| A*02:42| A*02:44| A*02:45| A*02:46| A*02:47| A*02:48| A*02:49| A*02:50| A*02:51| A*02:52| A*02:54| A*02:55| A*02:56:01| A*02:56:02| A*02:57| A*02:58| A*02:59| A*02:60:01| A*02:60:02| A*02:61| A*02:62| A*02:63| A*02:64:01| A*02:64:02| A*02:65| A*02:66| A*02:67| A*02:68| A*02:69| A*02:70| A*02:71| A*02:72| A*02:73| A*02:74:01| A*02:74:02| A*02:75| A*02:76:01| A*02:76:02| A*02:77| A*02:78| A*02:79:01| A*02:79:02| A*02:80| A*02:81| A*02:84| A*02:85| A*02:86:01| A*02:86:02| A*02:87| A*02:89:01| A*02:89:02| A*02:90| A*02:91| A*02:92| A*02:93:01| A*02:93:02| A*02:95| A*02:96| A*02:97:01| A*02:97:02| A*02:99| A*02:101:01| A*02:101:02| A*02:102| A*02:103| A*02:104| A*02:105| A*02:106| A*02:107| A*02:108| A*02:109| A*02:110| A*02:111| A*02:112| A*02:114| A*02:115| A*02:116| A*02:117| A*02:118| A*02:119| A*02:120| A*02:121| A*02:122| A*02:123| A*02:124| A*02:126| A*02:127| A*02:128| A*02:129| A*02:130| A*02:131:01| A*02:131:02| A*02:132| A*02:133| A*02:134| A*02:135| A*02:136| A*02:137| A*02:138| A*02:139| A*02:140| A*02:141| A*02:142| A*02:143| A*02:144| A*02:145| A*02:146| A*02:147| A*02:148| A*02:149| A*02:150:01| A*02:150:02| A*02:151| A*02:152| A*02:153:01| A*02:153:02| A*02:154| A*02:155| A*02:156| A*02:157:01| A*02:157:02| A*02:158| A*02:159| A*02:160| A*02:161| A*02:162| A*02:163| A*02:164:01| A*02:164:02| A*02:165| A*02:166| A*02:167| A*02:168| A*02:169| A*02:170| A*02:171:01| A*02:171:02| A*02:172| A*02:173| A*02:174| A*02:175| A*02:176| A*02:177| A*02:178| A*02:179| A*02:180| A*02:181| A*02:182| A*02:183| A*02:184| A*02:185| A*02:186| A*02:187| A*02:188| A*02:189| A*02:190| A*02:191| A*02:192| A*02:193| A*02:194| A*02:195| A*02:196| A*02:197:01| A*02:197:02| A*02:198| A*02:199| A*02:200| A*02:201| A*02:202| A*02:203| A*02:204| A*02:205| A*02:206| A*02:207| A*02:208| A*02:209| A*02:210| A*02:211:01| A*02:211:02| A*02:212| A*02:213| A*02:214| A*02:215| A*02:216| A*02:217:01| A*02:217:02| A*02:218| A*02:219| A*02:220| A*02:221| A*02:224| A*02:228| A*02:229| A*02:230| A*02:231| A*02:232| A*02:233| A*02:234| A*02:235| A*02:236| A*02:237| A*02:238| A*02:239| A*02:240| A*02:241| A*02:242| A*02:243:01| A*02:243:02| A*02:243:03| A*02:244| A*02:245| A*02:246| A*02:247| A*02:248| A*02:249| A*02:251| A*02:252| A*02:253| A*02:254| A*02:255| A*02:256| A*02:257| A*02:258| A*02:259| A*02:260| A*02:261| A*02:262| A*02:263| A*02:264| A*02:265| A*02:266| A*02:267| A*02:268| A*02:269| A*02:270| A*02:271| A*02:272| A*02:273| A*02:274| A*02:275| A*02:276| A*02:277| A*02:278| A*02:279| A*02:280| A*02:281| A*02:282| A*02:283| A*02:285| A*02:286| A*02:287| A*02:288| A*02:289:01| A*02:289:02| A*02:290| A*02:291| A*02:292| A*02:293Q| A*02:294| A*02:295| A*02:296| A*02:297| A*02:298| A*02:299| A*02:300| A*02:302| A*02:303| A*02:304| A*02:306| A*02:307| A*02:308| A*02:309| A*02:310| A*02:311| A*02:312| A*02:313| A*02:315| A*02:316| A*02:317| A*02:318| A*02:319| A*02:320| A*02:322| A*02:323| A*02:324| A*02:325| A*02:326| A*02:327| A*02:328| A*02:329| A*02:330| A*02:331| A*02:332| A*02:333| A*02:334| A*02:335| A*02:336| A*02:337| A*02:338| A*02:339| A*02:340| A*02:341| A*02:342| A*02:343| A*02:344| A*02:345| A*02:346| A*02:347| A*02:348| A*02:349| A*02:351| A*02:352| A*02:353| A*02:354| A*02:355| A*02:357| A*02:358| A*02:359| A*02:360| A*02:361| A*02:362| A*02:363| A*02:364| A*02:365| A*02:367| A*02:368| A*02:369| A*02:370| A*02:371| A*02:372| A*02:374| A*02:375| A*02:376| A*02:377| A*02:378| A*02:379| A*02:380| A*02:381| A*02:382| A*02:383| A*02:384| A*02:385| A*02:386| A*02:387| A*02:388| A*02:389| A*02:390| A*02:391| A*02:392| A*02:393| A*02:394| A*02:396| A*02:397| A*02:398| A*02:399| A*02:400| A*02:401| A*02:402| A*02:403| A*02:404| A*02:405| A*02:406| A*02:407| A*02:408| A*02:409| A*02:410| A*02:411| A*02:412| A*02:413| A*02:414| A*02:415| A*02:416| A*02:417| A*02:418| A*02:419:01| A*02:419:02| A*02:420| A*02:421| A*02:422| A*02:423| A*02:424| A*02:425| A*02:426| A*02:427| A*02:428| A*02:429| A*02:430| A*02:431| A*02:432| A*02:433| A*02:434| A*02:435| A*02:436| A*02:437| A*02:438| A*02:440Q| A*02:441| A*02:442| A*02:443| A*02:444| A*02:445| A*02:446| A*02:447| A*02:448| A*02:449| A*02:450| A*02:451| A*02:452| A*02:453| A*02:454| A*02:455| A*02:456| A*02:457| A*02:458| A*02:459| A*02:460| A*02:461| A*02:462| A*02:463| A*02:464| A*02:465| A*02:466| A*02:467| A*02:469| A*02:470| A*02:471| A*02:472| A*02:473| A*02:474| A*02:475| A*02:477| A*02:478| A*02:479| A*02:480| A*02:481| A*02:482| A*02:483| A*02:484| A*02:485| A*02:486| A*02:487| A*02:488| A*02:489| A*02:491| A*02:492| A*02:493| A*02:494| A*02:495| A*02:496| A*02:497| A*02:498| A*02:499| A*02:500Q| A*02:502| A*02:503| A*02:504| A*02:505| A*02:507| A*02:508| A*02:509| A*02:510| A*02:511| A*02:512| A*02:513| A*02:515| A*02:517| A*02:518| A*02:519| A*02:520| A*02:521| A*02:522| A*02:523| A*02:524:01| A*02:524:02| A*02:526| A*02:527| A*02:528:01| A*02:528:02| A*02:529| A*02:530| A*02:531| A*02:532| A*02:533| A*02:534| A*02:535| A*02:536| A*02:537| A*02:538| A*02:539| A*02:541| A*02:542| A*02:543| A*02:544| A*02:545| A*02:546| A*02:547| A*02:548| A*02:549| A*02:550| A*02:551| A*02:552| A*02:553| A*02:554| A*02:555| A*02:556| A*02:557| A*02:558| A*02:559| A*02:560| A*02:561| A*02:562| A*02:563| A*02:564| A*02:565| A*02:566| A*02:567| A*02:568| A*02:569| A*02:570:01| A*02:570:02| A*02:571| A*02:572| A*02:573| A*02:574| A*02:575| A*02:576| A*02:577| A*02:578| A*02:579| A*02:580| A*02:581| A*02:582| A*02:583| A*02:584| A*02:585| A*02:586| A*02:587| A*02:588| A*02:589| A*02:590| A*02:591:01| A*02:591:02| A*02:592| A*02:593| A*02:594| A*02:595| A*02:596| A*02:597| A*02:598| A*02:599| A*02:600| A*02:601| A*02:602| A*02:603| A*02:604| A*02:605Q| A*02:606| A*02:607| A*02:609| A*02:610:01| A*02:610:02| A*02:611| A*02:612| A*02:613| A*02:614| A*02:615| A*02:616| A*02:617| A*02:618Q| A*02:619| A*02:620| A*02:621| A*02:623| A*02:624| A*02:625| A*02:626| A*02:627| A*02:628| A*02:629| A*02:630| A*02:631| A*02:632| A*02:633| A*02:634| A*02:635| A*02:636| A*02:637| A*02:638| A*02:639| A*02:640| A*02:641| A*02:642| A*02:644| A*02:645| A*02:646| A*02:647| A*02:648| A*02:649| A*02:650| A*02:651| A*02:652| A*02:653| A*02:654| A*02:655| A*02:656| A*02:657| A*02:658| A*02:659| A*02:660| A*02:661| A*02:662| A*02:663| A*02:664| A*02:665| A*02:666| A*02:667| A*02:668| A*02:669| A*02:670| A*02:671| A*02:672Q| A*02:673| A*02:674| A*02:676| A*02:677| A*02:678| A*02:679| A*02:680| A*02:681| A*02:682| A*02:683| A*02:684| A*02:685| A*02:686| A*02:687| A*02:688| A*02:689| A*02:690| A*02:692| A*02:693| A*02:694| A*02:695| A*02:697| A*02:698| A*02:699| A*02:700| A*02:701| A*02:702| A*02:703| A*02:704| A*02:705| A*02:706| A*02:707| A*02:708| A*02:709| A*02:711| A*02:712| A*02:713| A*02:714| A*02:716| A*02:717| A*02:718| A*02:719| A*02:720| A*02:721| A*02:722| A*02:723| A*02:724| A*02:725| A*02:726| A*02:727| A*02:728| A*02:729| A*02:730| A*02:731| A*02:732| A*02:733| A*02:734| A*02:735| A*02:736| A*02:737| A*02:738| A*02:739| A*02:740| A*02:741| A*02:742| A*02:743| A*02:744| A*02:745| A*02:746| A*02:747| A*02:749| A*02:750| A*02:751| A*02:752| A*02:753| A*02:754| A*02:755| A*02:756| A*02:757| A*02:758| A*02:759| A*02:761| A*02:762| A*02:763| A*02:764| A*02:765| A*02:766| A*02:767| A*02:768| A*02:769| A*02:770| A*02:771| A*02:772| A*02:774| A*02:776| A*02:777| A*02:778| A*02:779| A*02:780| A*02:781| A*02:782| A*02:783| A*02:784| A*02:785| A*02:786| A*02:787| A*02:790| A*02:794| A*02:795| A*02:798| A*02:799| A*02:800| A*02:801| A*02:802| A*02:804| A*02:805Q| A*02:808| A*02:809| A*02:810| A*02:811| A*02:812| A*02:813| A*02:814| A*02:815| A*02:816| A*02:817| A*02:818| A*02:819| A*02:820| A*02:821| A*02:822| A*02:823| A*02:824| A*02:825| A*02:03:01| A*02:03:02| A*02:03:03| A*02:03:04| A*02:03:05| A*02:03:06| A*02:03:07| A*02:03:08</t>
+  </si>
+  <si>
+    <t>A*23:01:01:01| A*23:01:01:02| A*23:01:01:03| A*23:01:01:04| A*23:01:02| A*23:01:03| A*23:01:04| A*23:01:05| A*23:01:06| A*23:01:07| A*23:01:08| A*23:01:09| A*23:01:10| A*23:01:11| A*23:01:12| A*23:01:13| A*23:01:14| A*23:01:15| A*23:01:16| A*23:01:17| A*23:01:18| A*23:01:19| A*23:01:20| A*23:01:21| A*23:01:22| A*23:01:23| A*23:01:24| A*23:01:25| A*23:01:26| A*23:02| A*23:03:01| A*23:03:02| A*23:04| A*23:05| A*23:06| A*23:09| A*23:10| A*23:12| A*23:13| A*23:14:01| A*23:14:02| A*23:15| A*23:16| A*23:17:01:01| A*23:17:01:02| A*23:17:01:03| A*23:18| A*23:20| A*23:21| A*23:22| A*23:23| A*23:24| A*23:25| A*23:26| A*23:27| A*23:28| A*23:29| A*23:30| A*23:31| A*23:32| A*23:33| A*23:34| A*23:35| A*23:36| A*23:37:01| A*23:37:02| A*23:39| A*23:40| A*23:41| A*23:42| A*23:43| A*23:44| A*23:45| A*23:46| A*23:47| A*23:48| A*23:49| A*23:50| A*23:51| A*23:52| A*23:53| A*23:54| A*23:55| A*23:56| A*23:57| A*23:58| A*23:59| A*23:60| A*23:61| A*23:62| A*23:63| A*23:64| A*23:65| A*23:66| A*23:67| A*23:68| A*23:70| A*23:71| A*23:72| A*23:73| A*23:74| A*23:75| A*23:76| A*23:77| A*23:78| A*23:79| A*23:80| A*23:81| A*23:82| A*23:83| A*23:85| A*23:86| A*23:87| A*23:88| A*23:89| A*23:90| A*23:92</t>
+  </si>
+  <si>
+    <t>A*24:02:01:01| A*24:02:01:02L| A*24:02:01:03| A*24:02:01:04| A*24:02:01:05| A*24:02:01:06| A*24:02:01:07| A*24:02:01:08| A*24:02:01:09| A*24:02:01:10| A*24:02:01:11| A*24:02:01:12| A*24:02:01:13| A*24:02:01:14| A*24:02:01:15| A*24:02:01:16| A*24:02:01:17| A*24:02:01:18| A*24:02:01:19| A*24:02:01:20| A*24:02:02| A*24:02:03Q| A*24:02:04| A*24:02:05| A*24:02:06| A*24:02:07| A*24:02:08| A*24:02:09| A*24:02:10| A*24:02:11| A*24:02:12| A*24:02:13| A*24:02:14| A*24:02:15| A*24:02:16| A*24:02:17| A*24:02:18| A*24:02:19| A*24:02:20| A*24:02:21| A*24:02:22| A*24:02:23| A*24:02:24| A*24:02:25| A*24:02:26| A*24:02:27| A*24:02:28| A*24:02:29| A*24:02:30| A*24:02:31| A*24:02:32| A*24:02:33| A*24:02:34| A*24:02:35| A*24:02:36| A*24:02:37| A*24:02:38| A*24:02:39| A*24:02:40| A*24:02:41| A*24:02:42| A*24:02:43| A*24:02:44| A*24:02:45| A*24:02:46| A*24:02:47| A*24:02:48| A*24:02:49| A*24:02:50| A*24:02:51| A*24:02:52| A*24:02:53| A*24:02:54| A*24:02:55| A*24:02:56| A*24:02:57| A*24:02:58| A*24:02:59| A*24:02:60| A*24:02:61| A*24:02:62| A*24:02:63| A*24:02:64| A*24:02:65| A*24:02:66| A*24:02:67| A*24:02:68| A*24:02:69| A*24:02:70| A*24:02:71| A*24:02:72| A*24:02:73| A*24:02:74| A*24:02:75| A*24:02:76| A*24:02:77| A*24:02:78| A*24:02:79| A*24:02:80| A*24:02:81| A*24:02:82| A*24:02:83| A*24:02:84| A*24:02:85| A*24:02:86| A*24:02:87| A*24:02:88| A*24:02:89| A*24:02:90| A*24:02:91| A*24:02:92| A*24:02:93| A*24:02:94| A*24:02:95| A*24:02:96| A*24:02:97| A*24:02:98| A*24:02:99| A*24:02:100| A*24:02:101| A*24:02:102| A*24:02:103| A*24:02:104| A*24:02:105| A*24:02:106| A*24:02:107| A*24:02:108| A*24:02:109| A*24:02:110| A*24:02:111| A*24:02:112| A*24:02:113| A*24:02:114| A*24:02:115| A*24:04| A*24:05:01| A*24:05:02| A*24:06| A*24:07:01| A*24:07:02| A*24:08| A*24:13:01| A*24:13:02| A*24:14:01:01| A*24:14:01:02| A*24:14:01:03| A*24:15| A*24:17| A*24:18| A*24:20:01:01| A*24:20:01:02| A*24:21:01| A*24:21:02| A*24:21:03| A*24:25| A*24:26| A*24:27| A*24:28| A*24:29| A*24:30| A*24:31| A*24:32| A*24:34| A*24:35| A*24:37| A*24:38| A*24:39| A*24:41| A*24:42| A*24:43| A*24:46| A*24:47| A*24:49| A*24:50| A*24:51| A*24:52| A*24:53| A*24:54| A*24:55| A*24:56| A*24:57| A*24:58| A*24:59| A*24:61| A*24:62| A*24:63| A*24:64| A*24:66| A*24:67| A*24:68| A*24:69| A*24:70| A*24:71| A*24:72| A*24:73| A*24:74:01| A*24:74:02| A*24:75| A*24:76| A*24:77| A*24:78| A*24:79| A*24:80| A*24:81| A*24:82| A*24:85| A*24:87| A*24:88| A*24:89| A*24:91| A*24:92| A*24:93| A*24:94| A*24:95| A*24:96| A*24:97| A*24:98| A*24:99| A*24:100| A*24:101| A*24:102| A*24:103| A*24:104| A*24:105| A*24:106| A*24:107| A*24:108| A*24:109| A*24:110| A*24:111| A*24:112| A*24:113| A*24:114| A*24:115| A*24:116| A*24:117| A*24:118| A*24:119| A*24:120| A*24:121| A*24:122| A*24:123| A*24:124| A*24:125| A*24:126| A*24:127| A*24:128| A*24:129| A*24:130| A*24:131| A*24:133| A*24:134| A*24:135:01| A*24:135:02| A*24:136| A*24:137| A*24:138| A*24:139| A*24:140| A*24:141| A*24:142:01| A*24:142:02| A*24:143| A*24:144| A*24:145| A*24:146| A*24:147| A*24:148| A*24:149| A*24:150| A*24:151| A*24:152| A*24:153| A*24:154| A*24:156| A*24:157| A*24:159| A*24:160| A*24:161| A*24:162| A*24:164| A*24:165| A*24:166| A*24:167| A*24:168| A*24:169| A*24:170| A*24:171| A*24:172:01| A*24:172:02| A*24:173| A*24:174| A*24:175| A*24:176| A*24:177| A*24:178| A*24:179| A*24:180| A*24:181| A*24:182| A*24:184| A*24:186| A*24:187| A*24:188| A*24:189| A*24:190| A*24:191| A*24:192| A*24:193| A*24:194| A*24:195| A*24:196| A*24:197| A*24:198| A*24:199| A*24:200| A*24:201| A*24:202| A*24:203| A*24:204| A*24:205| A*24:206| A*24:207:01| A*24:207:02| A*24:208:01| A*24:208:02| A*24:209| A*24:210| A*24:212| A*24:213| A*24:214| A*24:215| A*24:216| A*24:217| A*24:218| A*24:219| A*24:220| A*24:221| A*24:223| A*24:224| A*24:225:01| A*24:225:02| A*24:226:01| A*24:226:02| A*24:227| A*24:228| A*24:229| A*24:230| A*24:231| A*24:233| A*24:234| A*24:235| A*24:236| A*24:237| A*24:238| A*24:239| A*24:241| A*24:242| A*24:243| A*24:244| A*24:245| A*24:246| A*24:247| A*24:248| A*24:249| A*24:250| A*24:251| A*24:253| A*24:254| A*24:255| A*24:256| A*24:257| A*24:258| A*24:259| A*24:260| A*24:261| A*24:262| A*24:263| A*24:264| A*24:265| A*24:266| A*24:267| A*24:268| A*24:269| A*24:270| A*24:271| A*24:272| A*24:273| A*24:274| A*24:275| A*24:276| A*24:277| A*24:279| A*24:280| A*24:281| A*24:282| A*24:283| A*24:284| A*24:285| A*24:286| A*24:287| A*24:288| A*24:289| A*24:290| A*24:291| A*24:292| A*24:293| A*24:294Q| A*24:295| A*24:296| A*24:297| A*24:298| A*24:299| A*24:300| A*24:301| A*24:302| A*24:304| A*24:305| A*24:306| A*24:307| A*24:308| A*24:309| A*24:310:01| A*24:310:02| A*24:311| A*24:313:01| A*24:313:02| A*24:314| A*24:315| A*24:316| A*24:317| A*24:318| A*24:319| A*24:320| A*24:321| A*24:322| A*24:324| A*24:325| A*24:326| A*24:327| A*24:328| A*24:329| A*24:330| A*24:331| A*24:332| A*24:333| A*24:334| A*24:335| A*24:336| A*24:337| A*24:338| A*24:339| A*24:340| A*24:341| A*24:342| A*24:343| A*24:344| A*24:345| A*24:346| A*24:347:01| A*24:347:02| A*24:348| A*24:349| A*24:350| A*24:351| A*24:352| A*24:353| A*24:354| A*24:355| A*24:356| A*24:358| A*24:360| A*24:361| A*24:362| A*24:363| A*24:364| A*24:365| A*24:366| A*24:367| A*24:368| A*24:369| A*24:371| A*24:372| A*24:373| A*24:375| A*24:376| A*24:377| A*24:378| A*24:379| A*24:380| A*24:381| A*24:382| A*24:383| A*24:384| A*24:385| A*24:386| A*24:387| A*24:390| A*24:391| A*24:392| A*24:393| A*24:394| A*24:395| A*24:397| A*24:398| A*24:399| A*24:400| A*24:401| A*24:402| A*24:403| A*24:404| A*24:405| A*24:406| A*24:407| A*24:409| A*24:410| A*24:411| A*24:412| A*24:413| A*24:414| A*24:415| A*24:416| A*24:417| A*24:418| A*24:419| A*24:420| A*24:421| A*24:422| A*24:423| A*24:424| A*24:431| A*24:432</t>
+  </si>
+  <si>
+    <t>A*24:03:01:01| A*24:03:01:02| A*24:03:02| A*24:03:03| A*24:03:04| A*24:10:01| A*24:10:02| A*24:23| A*24:33| A*24:374</t>
+  </si>
+  <si>
+    <t>A*25:01:01:01| A*25:01:01:02| A*25:01:01:03| A*25:01:01:04| A*25:01:01:05| A*25:01:02| A*25:01:03| A*25:01:04| A*25:01:05| A*25:01:06| A*25:01:07| A*25:01:08| A*25:01:09| A*25:01:10| A*25:01:11| A*25:01:12| A*25:01:13| A*25:01:14| A*25:02| A*25:03| A*25:04| A*25:05| A*25:06| A*25:07| A*25:08| A*25:09| A*25:10| A*25:11| A*25:13| A*25:14| A*25:15| A*25:16| A*25:17| A*25:18| A*25:19:01| A*25:19:02| A*25:20| A*25:21| A*25:22| A*25:23| A*25:24| A*25:25| A*25:26| A*25:27:01| A*25:27:02| A*25:28| A*25:29| A*25:30| A*25:31| A*25:32| A*25:33| A*25:34| A*25:35| A*25:36| A*25:37| A*25:38| A*25:39| A*25:40| A*25:41| A*25:43| A*25:44| A*25:45| A*25:46| A*25:47| A*25:48| A*25:50| A*25:51| A*25:52| A*25:53| A*25:54| A*25:55| A*25:56| A*25:57</t>
+  </si>
+  <si>
+    <t>A*26:01:01:01| A*26:01:01:02| A*26:01:01:04| A*26:01:01:05| A*26:01:01:06| A*26:01:01:07| A*26:01:01:08| A*26:01:01:09| A*26:01:01:10| A*26:01:01:11| A*26:01:01:12| A*26:01:01:13| A*26:01:02| A*26:01:03| A*26:01:04| A*26:01:05| A*26:01:06| A*26:01:07| A*26:01:08| A*26:01:09| A*26:01:10| A*26:01:11| A*26:01:12| A*26:01:13| A*26:01:14| A*26:01:15| A*26:01:16| A*26:01:17| A*26:01:18| A*26:01:19| A*26:01:20| A*26:01:21| A*26:01:22| A*26:01:23| A*26:01:24| A*26:01:25| A*26:01:26| A*26:01:27| A*26:01:28| A*26:01:29| A*26:01:30| A*26:01:31| A*26:01:32| A*26:01:33| A*26:01:34| A*26:01:35| A*26:01:36| A*26:01:37| A*26:01:38| A*26:01:39| A*26:01:40| A*26:01:41| A*26:01:42| A*26:01:43| A*26:01:44| A*26:01:45| A*26:01:46| A*26:01:47| A*26:01:48| A*26:01:49| A*26:01:50| A*26:01:51| A*26:01:52| A*26:01:53| A*26:01:54| A*26:02:01| A*26:02:02| A*26:03:01| A*26:04| A*26:05| A*26:06| A*26:07:01| A*26:07:02| A*26:08:01| A*26:08:02| A*26:08:03| A*26:09| A*26:12| A*26:13| A*26:14| A*26:16| A*26:17| A*26:19| A*26:20| A*26:21| A*26:22| A*26:23| A*26:24| A*26:27| A*26:28| A*26:29| A*26:30| A*26:31| A*26:32| A*26:33| A*26:34| A*26:35| A*26:36| A*26:37| A*26:38| A*26:39| A*26:40| A*26:41| A*26:42| A*26:43:01| A*26:43:02| A*26:45| A*26:46| A*26:47| A*26:48| A*26:49| A*26:50| A*26:51| A*26:52| A*26:53| A*26:54| A*26:55| A*26:56| A*26:57| A*26:58| A*26:59| A*26:61| A*26:62| A*26:63| A*26:64| A*26:65| A*26:66| A*26:67| A*26:68| A*26:69| A*26:70| A*26:72| A*26:73| A*26:74| A*26:75| A*26:76| A*26:77| A*26:78| A*26:79| A*26:80| A*26:81| A*26:82| A*26:83| A*26:84| A*26:85| A*26:86| A*26:87| A*26:88| A*26:89| A*26:90| A*26:91| A*26:93| A*26:94| A*26:95| A*26:96| A*26:97| A*26:98| A*26:99| A*26:100| A*26:101| A*26:102| A*26:103| A*26:104| A*26:105| A*26:106| A*26:108| A*26:109| A*26:110| A*26:111| A*26:112| A*26:113| A*26:114| A*26:115| A*26:116| A*26:117| A*26:118| A*26:119| A*26:120| A*26:121| A*26:122| A*26:123| A*26:124| A*26:125| A*26:126| A*26:128| A*26:129| A*26:130| A*26:131| A*26:132| A*26:133| A*26:134| A*26:135| A*26:136| A*26:137| A*26:138| A*26:139| A*26:140| A*26:141| A*26:142| A*26:143| A*26:144| A*26:146| A*26:147| A*26:148| A*26:149| A*26:150| A*26:151| A*26:152| A*26:153| A*26:154| A*26:155| A*26:156| A*26:157| A*26:158| A*26:159| A*26:160| A*26:162| A*26:163| A*26:164| A*26:165| A*26:166Q| A*26:167| A*26:168| A*26:169| A*26:170| A*26:171| A*26:172| A*26:173| A*26:174| A*26:175| A*26:176| A*26:177| A*26:178| A*66:05</t>
+  </si>
+  <si>
+    <t>A*68:10| A*68:12| A*68:17| A*68:26| A*68:01:01:01| A*68:01:01:02| A*68:01:01:03| A*68:01:02:01| A*68:01:02:02| A*68:01:02:03| A*68:01:02:04| A*68:01:02:05| A*68:01:02:06| A*68:01:02:07| A*68:01:03| A*68:01:04| A*68:01:05| A*68:01:06| A*68:01:07| A*68:01:08| A*68:01:09| A*68:01:10| A*68:01:11| A*68:01:12| A*68:01:13| A*68:01:14| A*68:01:15| A*68:01:16| A*68:01:17| A*68:01:18| A*68:01:19| A*68:01:20| A*68:01:21| A*68:01:22| A*68:01:23| A*68:01:24| A*68:01:25| A*68:01:26| A*68:01:27| A*68:01:28| A*68:01:29| A*68:01:30| A*68:01:31| A*68:01:32| A*68:01:33| A*68:01:34| A*68:01:35| A*68:01:36| A*68:01:37| A*68:01:38| A*68:01:39| A*68:01:40| A*68:01:41| A*68:01:42| A*68:01:43| A*68:02:01:01| A*68:02:01:02| A*68:02:01:03| A*68:02:01:04| A*68:02:01:05| A*68:02:02| A*68:02:03| A*68:02:04| A*68:02:05| A*68:02:06| A*68:02:07| A*68:02:08| A*68:02:09| A*68:02:10| A*68:02:11| A*68:02:12| A*68:02:13| A*68:03:01| A*68:03:02| A*68:03:03| A*68:04:01| A*68:04:02| A*68:05| A*68:06| A*68:07| A*68:08:01| A*68:08:02| A*68:09| A*68:13:01| A*68:13:02| A*68:14| A*68:15| A*68:16| A*68:19| A*68:20| A*68:21:01| A*68:21:02| A*68:22| A*68:23| A*68:24| A*68:25| A*68:27:01| A*68:27:02| A*68:28| A*68:29| A*68:30| A*68:31| A*68:32| A*68:33| A*68:34| A*68:35| A*68:36| A*68:37| A*68:38| A*68:39| A*68:40| A*68:41| A*68:42| A*68:43:01| A*68:43:02| A*68:44| A*68:45| A*68:46| A*68:47| A*68:48| A*68:50| A*68:51| A*68:52| A*68:53| A*68:54| A*68:55:01| A*68:55:02| A*68:56| A*68:57| A*68:58:01| A*68:58:02| A*68:60| A*68:61| A*68:62| A*68:63| A*68:64| A*68:65| A*68:66:01| A*68:66:02| A*68:67| A*68:68| A*68:69| A*68:70| A*68:71| A*68:72| A*68:73| A*68:74| A*68:75:01| A*68:75:02| A*68:76:01| A*68:76:02| A*68:77| A*68:78| A*68:79| A*68:80| A*68:81| A*68:82| A*68:83| A*68:84| A*68:85| A*68:86| A*68:87| A*68:88| A*68:89| A*68:90| A*68:91| A*68:92| A*68:93| A*68:95| A*68:96| A*68:97| A*68:98| A*68:99| A*68:100| A*68:101:01| A*68:101:02| A*68:102| A*68:103:01| A*68:103:02| A*68:104:01| A*68:104:02| A*68:105| A*68:106| A*68:107| A*68:108| A*68:109| A*68:110| A*68:111| A*68:112:01| A*68:112:02| A*68:113| A*68:114| A*68:115| A*68:116| A*68:117| A*68:118| A*68:119:01| A*68:119:02| A*68:121:01| A*68:121:02| A*68:122| A*68:123| A*68:124| A*68:125| A*68:126| A*68:127| A*68:128| A*68:129| A*68:130:01| A*68:130:02| A*68:131| A*68:132| A*68:133| A*68:134| A*68:135| A*68:136| A*68:137| A*68:138| A*68:139| A*68:140| A*68:141| A*68:143| A*68:144| A*68:145| A*68:146| A*68:147| A*68:148Q| A*68:149| A*68:150| A*68:151| A*68:152| A*68:153| A*68:154| A*68:155| A*68:156| A*68:157| A*68:158| A*68:159Q| A*68:160| A*68:161| A*68:162| A*68:163| A*68:164| A*68:165| A*68:166| A*68:167| A*68:168| A*68:169| A*68:170| A*68:172| A*68:173| A*68:174| A*68:175| A*68:176| A*68:177| A*68:178| A*68:179| A*68:180| A*68:183| A*68:184| A*68:185| A*68:186| A*68:187| A*68:188| A*68:189| A*68:190| A*68:191| A*68:192| A*68:193| A*68:194| A*68:195| A*68:196| A*68:197| A*68:198| A*68:200| A*68:201| A*68:202| A*68:204| A*69:01:01:01| A*69:01:01:02| A*69:01:02| A*69:01:03| A*69:02| A*69:03| A*69:04| A*69:05</t>
+  </si>
+  <si>
+    <t>A*29:01:01:01| A*29:01:01:03| A*29:01:02| A*29:01:03| A*29:01:04| A*29:01:05| A*29:01:06| A*29:01:07| A*29:01:08| A*29:01:09| A*29:01:10| A*29:01:11| A*29:02:01:01| A*29:02:01:02| A*29:02:01:03| A*29:02:01:04| A*29:02:01:05| A*29:02:01:06| A*29:02:02| A*29:02:03| A*29:02:04| A*29:02:05| A*29:02:06| A*29:02:07| A*29:02:08| A*29:02:09| A*29:02:10| A*29:02:11| A*29:02:12| A*29:02:13| A*29:02:14| A*29:02:15| A*29:02:16| A*29:02:17:01| A*29:02:17:02| A*29:02:18| A*29:02:19| A*29:02:20| A*29:02:21| A*29:02:22| A*29:02:23| A*29:02:24| A*29:02:25| A*29:02:26| A*29:03| A*29:04| A*29:05| A*29:06| A*29:07| A*29:09| A*29:10:01| A*29:10:02| A*29:11| A*29:12| A*29:13| A*29:14| A*29:15| A*29:16| A*29:17| A*29:18| A*29:19| A*29:20| A*29:21| A*29:22| A*29:23| A*29:24| A*29:25| A*29:26| A*29:27| A*29:28| A*29:29| A*29:30| A*29:31| A*29:32| A*29:33| A*29:34| A*29:35| A*29:36| A*29:37| A*29:38| A*29:39| A*29:40| A*29:41| A*29:42| A*29:43| A*29:44| A*29:45| A*29:46| A*29:47| A*29:48| A*29:49| A*29:50| A*29:51| A*29:52| A*29:53| A*29:54| A*29:55| A*29:56| A*29:57| A*29:58| A*29:59| A*29:60| A*29:61| A*29:62| A*29:63| A*29:64| A*29:65| A*29:66| A*29:67| A*29:68| A*29:69| A*29:70| A*29:71| A*29:72| A*29:73| A*29:74| A*29:75| A*29:76| A*29:77| A*29:79| A*29:80| A*29:81| A*29:82| A*29:83| A*29:84| A*29:85| A*29:86| A*29:87| A*29:88| A*29:89| A*29:90| A*29:91| A*29:92| A*29:93| A*29:94| A*29:95| A*29:96| A*29:97| A*29:98| A*29:99| A*29:100| A*29:101| A*29:102| A*29:103| A*29:104| A*29:105| A*29:106| A*29:107| A*29:108| A*29:109| A*29:110| A*29:111| A*29:113| A*29:114| A*29:115| A*29:116| A*29:117| A*29:118| A*29:119| A*29:120| A*29:121| A*29:122| A*29:123| A*29:124| A*29:125| A*29:126Q| A*29:127| A*29:128</t>
+  </si>
+  <si>
+    <t>A*03:01:01:01| A*03:01:01:03| A*03:01:01:04| A*03:01:01:05| A*03:01:01:06| A*03:01:01:07| A*03:01:01:08| A*03:01:01:09| A*03:01:01:10| A*03:01:01:11| A*03:01:01:12| A*03:01:01:13| A*03:01:01:14| A*03:01:01:15| A*03:01:01:16| A*03:01:01:17| A*03:01:01:18| A*03:01:01:19| A*03:01:01:20| A*03:01:01:21| A*03:01:01:22| A*03:01:01:23| A*03:01:01:24| A*03:01:02| A*03:01:03| A*03:01:04| A*03:01:05| A*03:01:06| A*03:01:07| A*03:01:08| A*03:01:09| A*03:01:10| A*03:01:11| A*03:01:12| A*03:01:13| A*03:01:14| A*03:01:15| A*03:01:16| A*03:01:17| A*03:01:18| A*03:01:19| A*03:01:20| A*03:01:21| A*03:01:22| A*03:01:23| A*03:01:24| A*03:01:25| A*03:01:26| A*03:01:27| A*03:01:28| A*03:01:29| A*03:01:30| A*03:01:31| A*03:01:32| A*03:01:33| A*03:01:34| A*03:01:35| A*03:01:36| A*03:01:37| A*03:01:38| A*03:01:39| A*03:01:40| A*03:01:41| A*03:01:42| A*03:01:43| A*03:01:44| A*03:01:45| A*03:01:46| A*03:01:47| A*03:01:48| A*03:01:49| A*03:01:50| A*03:01:51| A*03:01:52| A*03:01:53| A*03:01:54| A*03:01:55| A*03:01:56| A*03:01:57| A*03:01:58| A*03:01:59| A*03:01:60| A*03:01:61| A*03:01:62| A*03:01:63| A*03:01:64| A*03:01:65| A*03:01:66| A*03:01:67| A*03:01:68| A*03:01:69| A*03:01:70| A*03:01:71| A*03:01:72| A*03:01:73| A*03:01:74| A*03:01:75| A*03:01:76| A*03:01:77| A*03:01:78| A*03:02:01| A*03:02:02| A*03:02:03| A*03:02:04| A*03:04:01| A*03:04:02| A*03:04:03| A*03:05:01| A*03:05:02| A*03:06| A*03:07:01| A*03:07:02| A*03:08| A*03:09| A*03:10| A*03:12| A*03:13| A*03:14| A*03:15| A*03:16| A*03:17:01| A*03:17:02| A*03:18| A*03:19| A*03:20| A*03:22:01| A*03:22:02| A*03:23:01| A*03:23:02| A*03:24| A*03:25| A*03:26| A*03:27| A*03:28| A*03:29| A*03:30| A*03:31| A*03:32| A*03:33| A*03:34| A*03:35| A*03:37| A*03:38| A*03:39| A*03:40| A*03:41| A*03:42| A*03:43| A*03:44:01| A*03:44:02| A*03:45| A*03:46| A*03:47| A*03:48| A*03:49| A*03:50| A*03:51:01| A*03:51:02| A*03:52| A*03:53| A*03:54| A*03:55| A*03:56| A*03:57| A*03:58| A*03:59| A*03:60| A*03:61| A*03:62| A*03:63| A*03:64| A*03:65| A*03:66| A*03:67| A*03:70| A*03:71| A*03:72| A*03:73| A*03:74| A*03:75| A*03:76| A*03:77| A*03:78| A*03:79| A*03:80| A*03:81| A*03:82| A*03:83| A*03:84| A*03:85| A*03:86| A*03:87| A*03:88| A*03:89:01| A*03:89:02| A*03:90| A*03:92| A*03:93| A*03:94| A*03:95| A*03:96| A*03:97| A*03:98| A*03:99| A*03:100| A*03:101| A*03:102| A*03:103:01| A*03:103:02| A*03:104| A*03:105| A*03:106| A*03:107| A*03:108| A*03:109| A*03:110| A*03:111| A*03:112| A*03:113| A*03:114| A*03:115| A*03:116| A*03:117| A*03:118| A*03:119| A*03:120| A*03:121| A*03:122| A*03:123:01| A*03:123:02| A*03:124| A*03:125| A*03:126| A*03:127| A*03:128| A*03:130| A*03:131| A*03:132| A*03:133| A*03:134| A*03:135| A*03:136| A*03:137| A*03:138| A*03:139| A*03:140| A*03:141| A*03:142| A*03:143| A*03:144| A*03:145:01| A*03:145:02| A*03:146| A*03:147| A*03:148| A*03:149| A*03:150| A*03:151| A*03:152| A*03:153| A*03:154:01| A*03:154:02| A*03:155| A*03:156| A*03:157:01| A*03:157:02| A*03:158| A*03:159| A*03:160| A*03:163| A*03:164| A*03:165| A*03:166| A*03:167| A*03:169| A*03:170| A*03:171| A*03:172| A*03:173| A*03:174| A*03:175| A*03:176| A*03:177| A*03:179| A*03:180| A*03:181| A*03:182| A*03:183| A*03:184| A*03:185| A*03:186| A*03:187| A*03:188| A*03:189| A*03:190| A*03:191| A*03:193| A*03:195| A*03:196| A*03:198| A*03:199| A*03:201| A*03:202| A*03:203| A*03:204| A*03:205| A*03:206| A*03:207| A*03:208| A*03:209| A*03:210| A*03:211| A*03:212| A*03:213| A*03:214| A*03:215| A*03:216| A*03:217| A*03:218| A*03:219| A*03:220| A*03:221| A*03:222| A*03:223| A*03:224| A*03:225| A*03:226| A*03:227| A*03:228| A*03:229| A*03:230| A*03:231:01| A*03:231:02| A*03:232| A*03:233| A*03:234Q| A*03:235| A*03:236| A*03:237| A*03:238| A*03:239| A*03:240| A*03:241| A*03:242| A*03:243| A*03:244| A*03:245| A*03:246| A*03:247| A*03:248| A*03:249| A*03:250| A*03:251| A*03:252| A*03:253| A*03:254| A*03:255| A*03:256| A*03:257| A*03:258| A*03:259| A*03:261| A*03:263| A*03:264| A*03:265| A*03:267| A*03:268| A*03:270| A*03:271| A*03:272| A*03:273| A*03:274| A*03:276| A*03:277| A*03:278| A*03:280:01| A*03:280:02| A*03:281| A*03:282| A*03:285| A*03:287| A*03:288| A*03:289| A*03:290| A*03:291| A*03:292| A*03:293| A*03:294| A*03:295| A*03:296| A*03:298| A*03:299| A*03:300| A*03:301| A*03:302| A*03:303| A*03:304| A*03:305| A*03:306| A*03:307| A*03:308| A*03:309| A*03:310| A*03:311| A*03:312| A*03:313| A*03:314| A*03:315| A*03:316| A*03:317| A*03:318| A*03:319| A*03:320| A*03:321| A*03:322| A*03:324| A*03:325| A*03:326| A*03:327| A*03:328| A*03:331| A*03:332| A*03:333| A*32:04</t>
+  </si>
+  <si>
+    <t>A*30:01:01:01| A*30:01:01:02| A*30:01:02| A*30:01:03| A*30:01:04| A*30:01:05| A*30:01:06| A*30:01:07| A*30:01:08| A*30:01:09| A*30:01:10| A*30:01:11| A*30:01:12| A*30:02:01:01| A*30:02:01:02| A*30:02:01:03| A*30:02:01:04| A*30:02:02| A*30:02:03| A*30:02:04| A*30:02:05| A*30:02:06| A*30:02:07| A*30:02:08| A*30:02:09| A*30:02:10| A*30:02:11| A*30:02:12| A*30:02:13| A*30:02:14| A*30:02:15| A*30:02:16| A*30:02:17| A*30:02:18| A*30:02:19| A*30:02:20| A*30:02:21| A*30:03| A*30:04:01| A*30:04:02| A*30:06| A*30:07| A*30:08:01| A*30:08:02| A*30:09| A*30:10| A*30:11:01| A*30:11:02| A*30:12:01| A*30:12:02| A*30:13| A*30:14L| A*30:15| A*30:16| A*30:17| A*30:18| A*30:19| A*30:20| A*30:22| A*30:23| A*30:24| A*30:25| A*30:26| A*30:28| A*30:29| A*30:30| A*30:31| A*30:32| A*30:33| A*30:34| A*30:35| A*30:36| A*30:37| A*30:38| A*30:39| A*30:40| A*30:41| A*30:42| A*30:43| A*30:44| A*30:45| A*30:46| A*30:47| A*30:48| A*30:49| A*30:50| A*30:51| A*30:52| A*30:53| A*30:54| A*30:55| A*30:56| A*30:57| A*30:58| A*30:60| A*30:61| A*30:62| A*30:63| A*30:64| A*30:65| A*30:66| A*30:67| A*30:68| A*30:69| A*30:71| A*30:72| A*30:74| A*30:75| A*30:77| A*30:79| A*30:80| A*30:81| A*30:82| A*30:83| A*30:84| A*30:85| A*30:86| A*30:87| A*30:88| A*30:89| A*30:90| A*30:91| A*30:92| A*30:93| A*30:94| A*30:95| A*30:96| A*30:97| A*30:98| A*30:99| A*30:100| A*30:101Q| A*30:102| A*30:103| A*30:104| A*30:105| A*30:106| A*30:107| A*30:108| A*30:109| A*30:110| A*30:111| A*30:112| A*30:113| A*30:114| A*30:115| A*30:116| A*30:117| A*30:118| A*30:119| A*30:120| A*30:122| A*30:124| A*30:125| A*30:126| A*30:127| A*30:128| A*30:129| A*30:131| A*30:133| A*30:134| A*30:135| A*30:136| A*30:137| A*30:138| A*30:139| A*30:140| A*30:141| A*30:142| A*30:143| A*30:144</t>
+  </si>
+  <si>
+    <t>A*31:01:02:01| A*31:01:02:02| A*31:01:02:04| A*31:01:02:05| A*31:01:02:06| A*31:01:02:07| A*31:01:02:08| A*31:01:02:09| A*31:01:02:10| A*31:01:03| A*31:01:04| A*31:01:05| A*31:01:06| A*31:01:07| A*31:01:08| A*31:01:09| A*31:01:10| A*31:01:11| A*31:01:12| A*31:01:13| A*31:01:14| A*31:01:15| A*31:01:16| A*31:01:17| A*31:01:18| A*31:01:19| A*31:01:20| A*31:01:21| A*31:01:22| A*31:01:23| A*31:01:24| A*31:01:25| A*31:01:26| A*31:01:27| A*31:01:28| A*31:01:29| A*31:01:30| A*31:01:31| A*31:01:32| A*31:01:33| A*31:02| A*31:03| A*31:04| A*31:05| A*31:06| A*31:07| A*31:08| A*31:09| A*31:10| A*31:11| A*31:12| A*31:13| A*31:15| A*31:16| A*31:17| A*31:18| A*31:19| A*31:20| A*31:21| A*31:22| A*31:23| A*31:24| A*31:25| A*31:26| A*31:27| A*31:28| A*31:29| A*31:30| A*31:31| A*31:32| A*31:33| A*31:34| A*31:35| A*31:36| A*31:37| A*31:38| A*31:39| A*31:40| A*31:41| A*31:42| A*31:43| A*31:44| A*31:45| A*31:46| A*31:47| A*31:48| A*31:49| A*31:50| A*31:51| A*31:52| A*31:53| A*31:54| A*31:55| A*31:56| A*31:57| A*31:58| A*31:59| A*31:61| A*31:62| A*31:63| A*31:64| A*31:65| A*31:66| A*31:67| A*31:68| A*31:69| A*31:70| A*31:71| A*31:72| A*31:73| A*31:74| A*31:75| A*31:76| A*31:77| A*31:78| A*31:79| A*31:80| A*31:81| A*31:82| A*31:83| A*31:84| A*31:85| A*31:86| A*31:87| A*31:88| A*31:89| A*31:90| A*31:91| A*31:92| A*31:93| A*31:94| A*31:95| A*31:96| A*31:97| A*31:98| A*31:99| A*31:100| A*31:101| A*31:102| A*31:103| A*31:104| A*31:105| A*31:106| A*31:107| A*31:108| A*31:109| A*31:110| A*31:111| A*31:112| A*31:113| A*31:114| A*31:115| A*31:116| A*31:117| A*31:118| A*31:119| A*31:120| A*31:121| A*31:122| A*31:123| A*31:124| A*31:125| A*31:127| A*31:128| A*31:129| A*31:130| A*31:132| A*31:133| A*31:134| A*31:135| A*31:136| A*31:137| A*31:138| A*31:139| A*31:140| A*31:142| A*31:143| A*31:144| A*31:145| A*31:146| A*31:147| A*31:148</t>
+  </si>
+  <si>
+    <t>A*32:01:01:01| A*32:01:01:02| A*32:01:01:03| A*32:01:01:04| A*32:01:01:05| A*32:01:01:06| A*32:01:01:07| A*32:01:01:08| A*32:01:01:09| A*32:01:01:10| A*32:01:02| A*32:01:03| A*32:01:04| A*32:01:05| A*32:01:06| A*32:01:07| A*32:01:08| A*32:01:09| A*32:01:10| A*32:01:11| A*32:01:12| A*32:01:13| A*32:01:14| A*32:01:15| A*32:01:16| A*32:01:17| A*32:01:18| A*32:01:19| A*32:01:20| A*32:01:21| A*32:01:22| A*32:01:23| A*32:01:24| A*32:01:25| A*32:01:26| A*32:01:27| A*32:01:28| A*32:01:29| A*32:01:30| A*32:01:31| A*32:01:32| A*32:01:33| A*32:02| A*32:03| A*32:05| A*32:06| A*32:07| A*32:08| A*32:09| A*32:10| A*32:11Q| A*32:12| A*32:13| A*32:14| A*32:15| A*32:16| A*32:17| A*32:18| A*32:20| A*32:21| A*32:22| A*32:23| A*32:24| A*32:25| A*32:26:01| A*32:26:02| A*32:28| A*32:29| A*32:30:01| A*32:30:02| A*32:31| A*32:32| A*32:33:01| A*32:33:02| A*32:34| A*32:35| A*32:36| A*32:37| A*32:38| A*32:39| A*32:40| A*32:41| A*32:42| A*32:43| A*32:44| A*32:46| A*32:47| A*32:49| A*32:50| A*32:51| A*32:52| A*32:53| A*32:54| A*32:55:01| A*32:55:02| A*32:57| A*32:58| A*32:59| A*32:60| A*32:61| A*32:62| A*32:63| A*32:64| A*32:65| A*32:66| A*32:67| A*32:68| A*32:69| A*32:70| A*32:71| A*32:72| A*32:73| A*32:74| A*32:75| A*32:76| A*32:77| A*32:78| A*32:79| A*32:80| A*32:81| A*32:82| A*32:83| A*32:84| A*32:85| A*32:86| A*32:87| A*32:88| A*32:89| A*32:90| A*32:91| A*32:93| A*32:94| A*32:95| A*32:96| A*32:97| A*32:98| A*32:99| A*32:100| A*32:101Q| A*32:102| A*32:103| A*32:104| A*32:105| A*32:106| A*32:107| A*32:108| A*32:109| A*32:110| A*32:111| A*32:113| A*32:114| A*32:115| A*32:116| A*32:118| A*32:119| A*32:120| A*32:121</t>
+  </si>
+  <si>
+    <t>A*33:01:01:01| A*33:01:01:02| A*33:01:02| A*33:01:03| A*33:01:04| A*33:01:05| A*33:01:06| A*33:01:07| A*33:01:08| A*33:01:09| A*33:01:10| A*33:01:11| A*33:01:12| A*33:03:01:01| A*33:03:01:02| A*33:03:01:03| A*33:03:01:04| A*33:03:01:05| A*33:03:02| A*33:03:03Q| A*33:03:04| A*33:03:05| A*33:03:06| A*33:03:07| A*33:03:08| A*33:03:09| A*33:03:10| A*33:03:11| A*33:03:12| A*33:03:13| A*33:03:14| A*33:03:15| A*33:03:16| A*33:03:17| A*33:03:18| A*33:03:19| A*33:03:20| A*33:03:21| A*33:03:22| A*33:03:23| A*33:03:24| A*33:03:25| A*33:03:26| A*33:03:27| A*33:03:28| A*33:03:29| A*33:03:30| A*33:03:31| A*33:03:32| A*33:03:33| A*33:03:34| A*33:03:35| A*33:03:36| A*33:03:37| A*33:03:38| A*33:04| A*33:05| A*33:06| A*33:07| A*33:08| A*33:10| A*33:11| A*33:12| A*33:13| A*33:14| A*33:15| A*33:16| A*33:17| A*33:18:01| A*33:18:02| A*33:19| A*33:20| A*33:21| A*33:22| A*33:23| A*33:24| A*33:25| A*33:26| A*33:27| A*33:28| A*33:29| A*33:30| A*33:31| A*33:32:01| A*33:32:02| A*33:33| A*33:34| A*33:35| A*33:36| A*33:37| A*33:39| A*33:40| A*33:41| A*33:42| A*33:43| A*33:44| A*33:45| A*33:46| A*33:47| A*33:48| A*33:49| A*33:50| A*33:51| A*33:52| A*33:53| A*33:54| A*33:55| A*33:56| A*33:57| A*33:58| A*33:59| A*33:60| A*33:61| A*33:62| A*33:63| A*33:64| A*33:65| A*33:66| A*33:67| A*33:68| A*33:69| A*33:70| A*33:71| A*33:72| A*33:75| A*33:76| A*33:77| A*33:78| A*33:79| A*33:81| A*33:82| A*33:83| A*33:84| A*33:85| A*33:86| A*33:87| A*33:88| A*33:89| A*33:90| A*33:91| A*33:92| A*33:93| A*33:94| A*33:95| A*33:97| A*33:98| A*33:99| A*33:100| A*33:101| A*33:102| A*33:103| A*33:104| A*33:105| A*33:106| A*33:107| A*33:108| A*33:109| A*33:110| A*33:111| A*33:112| A*33:113| A*33:114| A*33:115| A*33:116| A*33:117| A*33:118| A*33:119| A*33:120| A*33:121| A*33:122| A*33:124| A*33:125| A*33:126| A*33:127| A*33:128| A*33:130| A*33:131| A*33:132| A*33:133| A*33:134| A*33:135| A*33:136| A*33:137| A*33:138| A*33:139| A*33:141| A*33:142| A*33:144| A*33:145| A*33:146| A*33:147| A*33:148| A*33:149| A*33:150| A*33:151| A*33:152| A*33:153| A*33:155| A*33:158| A*33:159| A*33:160| A*33:161| A*33:162| A*33:163| A*33:164| A*33:165| A*33:166| A*33:167| A*33:168| A*33:169| A*33:170</t>
+  </si>
+  <si>
+    <t>A*34:01:01:01| A*34:01:01:02| A*34:01:02| A*34:02:01:01| A*34:02:01:02| A*34:02:02| A*34:02:03| A*34:02:04| A*34:03| A*34:04| A*34:05| A*34:07| A*34:08| A*34:09| A*34:11| A*34:12| A*34:13| A*34:14| A*34:15| A*34:16| A*34:17| A*34:18| A*34:19| A*34:20| A*34:21</t>
+  </si>
+  <si>
+    <t>A*36:01| A*36:02| A*36:03| A*36:04| A*36:05| A*36:06| A*36:07| A*36:08</t>
   </si>
   <si>
     <t>A*43:01</t>
   </si>
   <si>
-    <t>A*66:01| A*66:04| A*66:06| A*66:07| A*66:09| A*66:10| A*66:11| A*66:12| A*66:13| A*66:14| A*66:15| A*66:16| A*66:17| A*66:18| A*66:19| A*66:20| A*66:21| A*66:22| A*66:23| A*66:24| A*66:25| A*66:26Q| A*66:29</t>
-  </si>
-  <si>
-    <t>A*66:02| A*66:04| A*66:06| A*66:07| A*66:09| A*66:10| A*66:11| A*66:12| A*66:13| A*66:14| A*66:15| A*66:16| A*66:17| A*66:18| A*66:19| A*66:20| A*66:21| A*66:22| A*66:23| A*66:24| A*66:25| A*66:26Q| A*66:29</t>
-  </si>
-  <si>
-    <t>A*66:04| A*66:06| A*66:07| A*66:09| A*66:10| A*66:11| A*66:12| A*66:13| A*66:14| A*66:15| A*66:16| A*66:17| A*66:18| A*66:19| A*66:20| A*66:21| A*66:22| A*66:23| A*66:24| A*66:25| A*66:26Q| A*66:29| A*66:01| A*66:02</t>
-  </si>
-  <si>
-    <t>A*68:01| A*68:02| A*68:03| A*68:04| A*68:05| A*68:06| A*68:07| A*68:08| A*68:09| A*68:13| A*68:14| A*68:15| A*68:16| A*68:19| A*68:20| A*68:21| A*68:22| A*68:23| A*68:24| A*68:25| A*68:27| A*68:28| A*68:29| A*68:30| A*68:31| A*68:32| A*68:33| A*68:34| A*68:35| A*68:36| A*68:37| A*68:38| A*68:39| A*68:40| A*68:41| A*68:42| A*68:43| A*68:44| A*68:45| A*68:46| A*68:47| A*68:48| A*68:50| A*68:51| A*68:52| A*68:53| A*68:54| A*68:55| A*68:56| A*68:57| A*68:58| A*68:60| A*68:61| A*68:62| A*68:63| A*68:64| A*68:65| A*68:66| A*68:67| A*68:68| A*68:69| A*68:70| A*68:71| A*68:72| A*68:73| A*68:74| A*68:75| A*68:76| A*68:77| A*68:78| A*68:79| A*68:80| A*68:81| A*68:82| A*68:83| A*68:84| A*68:85| A*68:86| A*68:87| A*68:88| A*68:89| A*68:90| A*68:91| A*68:92| A*68:93| A*68:95| A*68:96| A*68:97| A*68:98| A*68:99| A*68:100| A*68:101| A*68:102| A*68:103| A*68:104| A*68:105| A*68:106| A*68:107| A*68:108| A*68:109| A*68:110| A*68:111| A*68:112| A*68:113| A*68:114| A*68:115| A*68:116| A*68:117| A*68:118| A*68:119| A*68:121| A*68:122| A*68:123| A*68:124| A*68:125| A*68:126| A*68:127| A*68:128| A*68:129| A*68:130| A*68:131| A*68:132| A*68:133| A*68:134| A*68:135| A*68:136| A*68:137| A*68:138| A*68:139| A*68:140| A*68:141| A*68:143| A*68:144| A*68:145| A*68:146| A*68:147| A*68:148Q| A*68:149| A*68:150| A*68:151| A*68:152| A*68:153| A*68:154| A*68:155| A*68:156| A*68:157| A*68:158| A*68:159Q| A*68:160| A*68:161| A*68:162| A*68:163| A*68:164| A*68:165| A*68:166| A*68:167| A*68:168| A*68:169| A*68:170| A*68:172| A*68:173| A*68:174</t>
-  </si>
-  <si>
-    <t>A*68:10| A*68:12| A*68:17| A*68:26| A*68:01| A*68:02| A*68:03| A*68:04| A*68:05| A*68:06| A*68:07| A*68:08| A*68:09| A*68:13| A*68:14| A*68:15| A*68:16| A*68:19| A*68:20| A*68:21| A*68:22| A*68:23| A*68:24| A*68:25| A*68:27| A*68:28| A*68:29| A*68:30| A*68:31| A*68:32| A*68:33| A*68:34| A*68:35| A*68:36| A*68:37| A*68:38| A*68:39| A*68:40| A*68:41| A*68:42| A*68:43| A*68:44| A*68:45| A*68:46| A*68:47| A*68:48| A*68:50| A*68:51| A*68:52| A*68:53| A*68:54| A*68:55| A*68:56| A*68:57| A*68:58| A*68:60| A*68:61| A*68:62| A*68:63| A*68:64| A*68:65| A*68:66| A*68:67| A*68:68| A*68:69| A*68:70| A*68:71| A*68:72| A*68:73| A*68:74| A*68:75| A*68:76| A*68:77| A*68:78| A*68:79| A*68:80| A*68:81| A*68:82| A*68:83| A*68:84| A*68:85| A*68:86| A*68:87| A*68:88| A*68:89| A*68:90| A*68:91| A*68:92| A*68:93| A*68:95| A*68:96| A*68:97| A*68:98| A*68:99| A*68:100| A*68:101| A*68:102| A*68:103| A*68:104| A*68:105| A*68:106| A*68:107| A*68:108| A*68:109| A*68:110| A*68:111| A*68:112| A*68:113| A*68:114| A*68:115| A*68:116| A*68:117| A*68:118| A*68:119| A*68:121| A*68:122| A*68:123| A*68:124| A*68:125| A*68:126| A*68:127| A*68:128| A*68:129| A*68:130| A*68:131| A*68:132| A*68:133| A*68:134| A*68:135| A*68:136| A*68:137| A*68:138| A*68:139| A*68:140| A*68:141| A*68:143| A*68:144| A*68:145| A*68:146| A*68:147| A*68:148Q| A*68:149| A*68:150| A*68:151| A*68:152| A*68:153| A*68:154| A*68:155| A*68:156| A*68:157| A*68:158| A*68:159Q| A*68:160| A*68:161| A*68:162| A*68:163| A*68:164| A*68:165| A*68:166| A*68:167| A*68:168| A*68:169| A*68:170| A*68:172| A*68:173| A*68:174| A*69:01| A*69:02| A*69:03</t>
-  </si>
-  <si>
-    <t>A*69:01| A*69:02| A*69:03</t>
-  </si>
-  <si>
-    <t>A*74:01| A*74:02| A*74:03| A*74:04| A*74:05| A*74:06| A*74:07| A*74:08| A*74:09| A*74:10| A*74:11| A*74:13| A*74:15| A*74:16| A*74:17| A*74:18| A*74:19| A*74:20| A*74:21| A*74:22| A*74:23| A*74:24| A*74:25| A*74:26| A*74:27| A*74:28</t>
-  </si>
-  <si>
-    <t>A*80:01| A*80:02| A*80:03</t>
+    <t>A*66:04| A*66:06| A*66:07| A*66:09| A*66:10| A*66:11| A*66:12| A*66:13| A*66:14| A*66:15| A*66:16| A*66:17| A*66:18| A*66:19| A*66:20| A*66:21| A*66:22| A*66:23| A*66:24| A*66:25| A*66:26Q| A*66:29| A*66:30| A*66:31| A*66:32| A*66:01:01:01| A*66:01:01:02| A*66:01:02| A*66:01:03| A*66:01:04| A*66:01:05| A*66:02</t>
+  </si>
+  <si>
+    <t>A*68:01:01:01| A*68:01:01:02| A*68:01:01:03| A*68:01:02:01| A*68:01:02:02| A*68:01:02:03| A*68:01:02:04| A*68:01:02:05| A*68:01:02:06| A*68:01:02:07| A*68:01:03| A*68:01:04| A*68:01:05| A*68:01:06| A*68:01:07| A*68:01:08| A*68:01:09| A*68:01:10| A*68:01:11| A*68:01:12| A*68:01:13| A*68:01:14| A*68:01:15| A*68:01:16| A*68:01:17| A*68:01:18| A*68:01:19| A*68:01:20| A*68:01:21| A*68:01:22| A*68:01:23| A*68:01:24| A*68:01:25| A*68:01:26| A*68:01:27| A*68:01:28| A*68:01:29| A*68:01:30| A*68:01:31| A*68:01:32| A*68:01:33| A*68:01:34| A*68:01:35| A*68:01:36| A*68:01:37| A*68:01:38| A*68:01:39| A*68:01:40| A*68:01:41| A*68:01:42| A*68:01:43| A*68:02:01:01| A*68:02:01:02| A*68:02:01:03| A*68:02:01:04| A*68:02:01:05| A*68:02:02| A*68:02:03| A*68:02:04| A*68:02:05| A*68:02:06| A*68:02:07| A*68:02:08| A*68:02:09| A*68:02:10| A*68:02:11| A*68:02:12| A*68:02:13| A*68:03:01| A*68:03:02| A*68:03:03| A*68:04:01| A*68:04:02| A*68:05| A*68:06| A*68:07| A*68:08:01| A*68:08:02| A*68:09| A*68:13:01| A*68:13:02| A*68:14| A*68:15| A*68:16| A*68:19| A*68:20| A*68:21:01| A*68:21:02| A*68:22| A*68:23| A*68:24| A*68:25| A*68:27:01| A*68:27:02| A*68:28| A*68:29| A*68:30| A*68:31| A*68:32| A*68:33| A*68:34| A*68:35| A*68:36| A*68:37| A*68:38| A*68:39| A*68:40| A*68:41| A*68:42| A*68:43:01| A*68:43:02| A*68:44| A*68:45| A*68:46| A*68:47| A*68:48| A*68:50| A*68:51| A*68:52| A*68:53| A*68:54| A*68:55:01| A*68:55:02| A*68:56| A*68:57| A*68:58:01| A*68:58:02| A*68:60| A*68:61| A*68:62| A*68:63| A*68:64| A*68:65| A*68:66:01| A*68:66:02| A*68:67| A*68:68| A*68:69| A*68:70| A*68:71| A*68:72| A*68:73| A*68:74| A*68:75:01| A*68:75:02| A*68:76:01| A*68:76:02| A*68:77| A*68:78| A*68:79| A*68:80| A*68:81| A*68:82| A*68:83| A*68:84| A*68:85| A*68:86| A*68:87| A*68:88| A*68:89| A*68:90| A*68:91| A*68:92| A*68:93| A*68:95| A*68:96| A*68:97| A*68:98| A*68:99| A*68:100| A*68:101:01| A*68:101:02| A*68:102| A*68:103:01| A*68:103:02| A*68:104:01| A*68:104:02| A*68:105| A*68:106| A*68:107| A*68:108| A*68:109| A*68:110| A*68:111| A*68:112:01| A*68:112:02| A*68:113| A*68:114| A*68:115| A*68:116| A*68:117| A*68:118| A*68:119:01| A*68:119:02| A*68:121:01| A*68:121:02| A*68:122| A*68:123| A*68:124| A*68:125| A*68:126| A*68:127| A*68:128| A*68:129| A*68:130:01| A*68:130:02| A*68:131| A*68:132| A*68:133| A*68:134| A*68:135| A*68:136| A*68:137| A*68:138| A*68:139| A*68:140| A*68:141| A*68:143| A*68:144| A*68:145| A*68:146| A*68:147| A*68:148Q| A*68:149| A*68:150| A*68:151| A*68:152| A*68:153| A*68:154| A*68:155| A*68:156| A*68:157| A*68:158| A*68:159Q| A*68:160| A*68:161| A*68:162| A*68:163| A*68:164| A*68:165| A*68:166| A*68:167| A*68:168| A*68:169| A*68:170| A*68:172| A*68:173| A*68:174| A*68:175| A*68:176| A*68:177| A*68:178| A*68:179| A*68:180| A*68:183| A*68:184| A*68:185| A*68:186| A*68:187| A*68:188| A*68:189| A*68:190| A*68:191| A*68:192| A*68:193| A*68:194| A*68:195| A*68:196| A*68:197| A*68:198| A*68:200| A*68:201| A*68:202| A*68:204</t>
+  </si>
+  <si>
+    <t>A*69:01:01:01| A*69:01:01:02| A*69:01:02| A*69:01:03| A*69:02| A*69:03| A*69:04| A*69:05</t>
+  </si>
+  <si>
+    <t>A*74:01:01:01| A*74:01:01:02| A*74:01:01:03| A*74:01:01:04| A*74:01:02| A*74:01:03| A*74:01:04| A*74:01:05| A*74:01:06| A*74:01:07| A*74:01:08| A*74:02:01:01| A*74:02:01:02| A*74:03| A*74:04| A*74:05| A*74:06| A*74:07| A*74:08| A*74:09| A*74:10| A*74:11| A*74:13| A*74:15| A*74:16:01| A*74:16:02| A*74:17| A*74:18| A*74:19| A*74:20| A*74:21| A*74:22| A*74:23| A*74:24| A*74:25| A*74:26| A*74:27| A*74:28| A*74:29| A*74:30| A*74:31| A*74:33| A*74:34</t>
+  </si>
+  <si>
+    <t>A*80:01:01:01| A*80:01:01:02| A*80:02| A*80:03| A*80:04</t>
+  </si>
+  <si>
+    <t>A*24:19| A*24:22| A*24:24| A*24:44| A*23:01:01:01| A*23:01:01:02| A*23:01:01:03| A*23:01:01:04| A*23:01:02| A*23:01:03| A*23:01:04| A*23:01:05| A*23:01:06| A*23:01:07| A*23:01:08| A*23:01:09| A*23:01:10| A*23:01:11| A*23:01:12| A*23:01:13| A*23:01:14| A*23:01:15| A*23:01:16| A*23:01:17| A*23:01:18| A*23:01:19| A*23:01:20| A*23:01:21| A*23:01:22| A*23:01:23| A*23:01:24| A*23:01:25| A*23:01:26| A*23:02| A*23:03:01| A*23:03:02| A*23:04| A*23:05| A*23:06| A*23:09| A*23:10| A*23:12| A*23:13| A*23:14:01| A*23:14:02| A*23:15| A*23:16| A*23:17:01:01| A*23:17:01:02| A*23:17:01:03| A*23:18| A*23:20| A*23:21| A*23:22| A*23:23| A*23:24| A*23:25| A*23:26| A*23:27| A*23:28| A*23:29| A*23:30| A*23:31| A*23:32| A*23:33| A*23:34| A*23:35| A*23:36| A*23:37:01| A*23:37:02| A*23:39| A*23:40| A*23:41| A*23:42| A*23:43| A*23:44| A*23:45| A*23:46| A*23:47| A*23:48| A*23:49| A*23:50| A*23:51| A*23:52| A*23:53| A*23:54| A*23:55| A*23:56| A*23:57| A*23:58| A*23:59| A*23:60| A*23:61| A*23:62| A*23:63| A*23:64| A*23:65| A*23:66| A*23:67| A*23:68| A*23:70| A*23:71| A*23:72| A*23:73| A*23:74| A*23:75| A*23:76| A*23:77| A*23:78| A*23:79| A*23:80| A*23:81| A*23:82| A*23:83| A*23:85| A*23:86| A*23:87| A*23:88| A*23:89| A*23:90| A*23:92| A*24:02:01:01| A*24:02:01:02L| A*24:02:01:03| A*24:02:01:04| A*24:02:01:05| A*24:02:01:06| A*24:02:01:07| A*24:02:01:08| A*24:02:01:09| A*24:02:01:10| A*24:02:01:11| A*24:02:01:12| A*24:02:01:13| A*24:02:01:14| A*24:02:01:15| A*24:02:01:16| A*24:02:01:17| A*24:02:01:18| A*24:02:01:19| A*24:02:01:20| A*24:02:02| A*24:02:03Q| A*24:02:04| A*24:02:05| A*24:02:06| A*24:02:07| A*24:02:08| A*24:02:09| A*24:02:10| A*24:02:11| A*24:02:12| A*24:02:13| A*24:02:14| A*24:02:15| A*24:02:16| A*24:02:17| A*24:02:18| A*24:02:19| A*24:02:20| A*24:02:21| A*24:02:22| A*24:02:23| A*24:02:24| A*24:02:25| A*24:02:26| A*24:02:27| A*24:02:28| A*24:02:29| A*24:02:30| A*24:02:31| A*24:02:32| A*24:02:33| A*24:02:34| A*24:02:35| A*24:02:36| A*24:02:37| A*24:02:38| A*24:02:39| A*24:02:40| A*24:02:41| A*24:02:42| A*24:02:43| A*24:02:44| A*24:02:45| A*24:02:46| A*24:02:47| A*24:02:48| A*24:02:49| A*24:02:50| A*24:02:51| A*24:02:52| A*24:02:53| A*24:02:54| A*24:02:55| A*24:02:56| A*24:02:57| A*24:02:58| A*24:02:59| A*24:02:60| A*24:02:61| A*24:02:62| A*24:02:63| A*24:02:64| A*24:02:65| A*24:02:66| A*24:02:67| A*24:02:68| A*24:02:69| A*24:02:70| A*24:02:71| A*24:02:72| A*24:02:73| A*24:02:74| A*24:02:75| A*24:02:76| A*24:02:77| A*24:02:78| A*24:02:79| A*24:02:80| A*24:02:81| A*24:02:82| A*24:02:83| A*24:02:84| A*24:02:85| A*24:02:86| A*24:02:87| A*24:02:88| A*24:02:89| A*24:02:90| A*24:02:91| A*24:02:92| A*24:02:93| A*24:02:94| A*24:02:95| A*24:02:96| A*24:02:97| A*24:02:98| A*24:02:99| A*24:02:100| A*24:02:101| A*24:02:102| A*24:02:103| A*24:02:104| A*24:02:105| A*24:02:106| A*24:02:107| A*24:02:108| A*24:02:109| A*24:02:110| A*24:02:111| A*24:02:112| A*24:02:113| A*24:02:114| A*24:02:115| A*24:04| A*24:05:01| A*24:05:02| A*24:06| A*24:07:01| A*24:07:02| A*24:08| A*24:13:01| A*24:13:02| A*24:14:01:01| A*24:14:01:02| A*24:14:01:03| A*24:15| A*24:17| A*24:18| A*24:20:01:01| A*24:20:01:02| A*24:21:01| A*24:21:02| A*24:21:03| A*24:25| A*24:26| A*24:27| A*24:28| A*24:29| A*24:30| A*24:31| A*24:32| A*24:34| A*24:35| A*24:37| A*24:38| A*24:39| A*24:41| A*24:42| A*24:43| A*24:46| A*24:47| A*24:49| A*24:50| A*24:51| A*24:52| A*24:53| A*24:54| A*24:55| A*24:56| A*24:57| A*24:58| A*24:59| A*24:61| A*24:62| A*24:63| A*24:64| A*24:66| A*24:67| A*24:68| A*24:69| A*24:70| A*24:71| A*24:72| A*24:73| A*24:74:01| A*24:74:02| A*24:75| A*24:76| A*24:77| A*24:78| A*24:79| A*24:80| A*24:81| A*24:82| A*24:85| A*24:87| A*24:88| A*24:89| A*24:91| A*24:92| A*24:93| A*24:94| A*24:95| A*24:96| A*24:97| A*24:98| A*24:99| A*24:100| A*24:101| A*24:102| A*24:103| A*24:104| A*24:105| A*24:106| A*24:107| A*24:108| A*24:109| A*24:110| A*24:111| A*24:112| A*24:113| A*24:114| A*24:115| A*24:116| A*24:117| A*24:118| A*24:119| A*24:120| A*24:121| A*24:122| A*24:123| A*24:124| A*24:125| A*24:126| A*24:127| A*24:128| A*24:129| A*24:130| A*24:131| A*24:133| A*24:134| A*24:135:01| A*24:135:02| A*24:136| A*24:137| A*24:138| A*24:139| A*24:140| A*24:141| A*24:142:01| A*24:142:02| A*24:143| A*24:144| A*24:145| A*24:146| A*24:147| A*24:148| A*24:149| A*24:150| A*24:151| A*24:152| A*24:153| A*24:154| A*24:156| A*24:157| A*24:159| A*24:160| A*24:161| A*24:162| A*24:164| A*24:165| A*24:166| A*24:167| A*24:168| A*24:169| A*24:170| A*24:171| A*24:172:01| A*24:172:02| A*24:173| A*24:174| A*24:175| A*24:176| A*24:177| A*24:178| A*24:179| A*24:180| A*24:181| A*24:182| A*24:184| A*24:186| A*24:187| A*24:188| A*24:189| A*24:190| A*24:191| A*24:192| A*24:193| A*24:194| A*24:195| A*24:196| A*24:197| A*24:198| A*24:199| A*24:200| A*24:201| A*24:202| A*24:203| A*24:204| A*24:205| A*24:206| A*24:207:01| A*24:207:02| A*24:208:01| A*24:208:02| A*24:209| A*24:210| A*24:212| A*24:213| A*24:214| A*24:215| A*24:216| A*24:217| A*24:218| A*24:219| A*24:220| A*24:221| A*24:223| A*24:224| A*24:225:01| A*24:225:02| A*24:226:01| A*24:226:02| A*24:227| A*24:228| A*24:229| A*24:230| A*24:231| A*24:233| A*24:234| A*24:235| A*24:236| A*24:237| A*24:238| A*24:239| A*24:241| A*24:242| A*24:243| A*24:244| A*24:245| A*24:246| A*24:247| A*24:248| A*24:249| A*24:250| A*24:251| A*24:253| A*24:254| A*24:255| A*24:256| A*24:257| A*24:258| A*24:259| A*24:260| A*24:261| A*24:262| A*24:263| A*24:264| A*24:265| A*24:266| A*24:267| A*24:268| A*24:269| A*24:270| A*24:271| A*24:272| A*24:273| A*24:274| A*24:275| A*24:276| A*24:277| A*24:279| A*24:280| A*24:281| A*24:282| A*24:283| A*24:284| A*24:285| A*24:286| A*24:287| A*24:288| A*24:289| A*24:290| A*24:291| A*24:292| A*24:293| A*24:294Q| A*24:295| A*24:296| A*24:297| A*24:298| A*24:299| A*24:300| A*24:301| A*24:302| A*24:304| A*24:305| A*24:306| A*24:307| A*24:308| A*24:309| A*24:310:01| A*24:310:02| A*24:311| A*24:313:01| A*24:313:02| A*24:314| A*24:315| A*24:316| A*24:317| A*24:318| A*24:319| A*24:320| A*24:321| A*24:322| A*24:324| A*24:325| A*24:326| A*24:327| A*24:328| A*24:329| A*24:330| A*24:331| A*24:332| A*24:333| A*24:334| A*24:335| A*24:336| A*24:337| A*24:338| A*24:339| A*24:340| A*24:341| A*24:342| A*24:343| A*24:344| A*24:345| A*24:346| A*24:347:01| A*24:347:02| A*24:348| A*24:349| A*24:350| A*24:351| A*24:352| A*24:353| A*24:354| A*24:355| A*24:356| A*24:358| A*24:360| A*24:361| A*24:362| A*24:363| A*24:364| A*24:365| A*24:366| A*24:367| A*24:368| A*24:369| A*24:371| A*24:372| A*24:373| A*24:375| A*24:376| A*24:377| A*24:378| A*24:379| A*24:380| A*24:381| A*24:382| A*24:383| A*24:384| A*24:385| A*24:386| A*24:387| A*24:390| A*24:391| A*24:392| A*24:393| A*24:394| A*24:395| A*24:397| A*24:398| A*24:399| A*24:400| A*24:401| A*24:402| A*24:403| A*24:404| A*24:405| A*24:406| A*24:407| A*24:409| A*24:410| A*24:411| A*24:412| A*24:413| A*24:414| A*24:415| A*24:416| A*24:417| A*24:418| A*24:419| A*24:420| A*24:421| A*24:422| A*24:423| A*24:424| A*24:431| A*24:432| A*24:03:01:01| A*24:03:01:02| A*24:03:02| A*24:03:03| A*24:03:04| A*24:10:01| A*24:10:02| A*24:23| A*24:33| A*24:374</t>
+  </si>
+  <si>
+    <t>B*0804</t>
+  </si>
+  <si>
+    <t>B*1304</t>
+  </si>
+  <si>
+    <t>B*3905</t>
+  </si>
+  <si>
+    <t>B*8201</t>
+  </si>
+  <si>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>B13</t>
+  </si>
+  <si>
+    <t>B14</t>
+  </si>
+  <si>
+    <t>B15</t>
+  </si>
+  <si>
+    <t>B16</t>
+  </si>
+  <si>
+    <t>B17</t>
+  </si>
+  <si>
+    <t>B18</t>
+  </si>
+  <si>
+    <t>B21</t>
+  </si>
+  <si>
+    <t>B22</t>
+  </si>
+  <si>
+    <t>B27</t>
+  </si>
+  <si>
+    <t>B2708</t>
+  </si>
+  <si>
+    <t>B35</t>
+  </si>
+  <si>
+    <t>B37</t>
+  </si>
+  <si>
+    <t>B38</t>
+  </si>
+  <si>
+    <t>B39</t>
+  </si>
+  <si>
+    <t>B3901</t>
+  </si>
+  <si>
+    <t>B3902</t>
+  </si>
+  <si>
+    <t>B40</t>
+  </si>
+  <si>
+    <t>B4005</t>
+  </si>
+  <si>
+    <t>B41</t>
+  </si>
+  <si>
+    <t>B42</t>
+  </si>
+  <si>
+    <t>B44</t>
+  </si>
+  <si>
+    <t>B45</t>
+  </si>
+  <si>
+    <t>B46</t>
+  </si>
+  <si>
+    <t>B47</t>
+  </si>
+  <si>
+    <t>B48</t>
+  </si>
+  <si>
+    <t>B49</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B50</t>
+  </si>
+  <si>
+    <t>B51</t>
+  </si>
+  <si>
+    <t>B5102</t>
+  </si>
+  <si>
+    <t>B52</t>
+  </si>
+  <si>
+    <t>B53</t>
+  </si>
+  <si>
+    <t>B54</t>
+  </si>
+  <si>
+    <t>B55</t>
+  </si>
+  <si>
+    <t>B56</t>
+  </si>
+  <si>
+    <t>B57</t>
+  </si>
+  <si>
+    <t>B58</t>
+  </si>
+  <si>
+    <t>B59</t>
+  </si>
+  <si>
+    <t>B60</t>
+  </si>
+  <si>
+    <t>B61</t>
+  </si>
+  <si>
+    <t>B62</t>
+  </si>
+  <si>
+    <t>B63</t>
+  </si>
+  <si>
+    <t>B64</t>
+  </si>
+  <si>
+    <t>B65</t>
+  </si>
+  <si>
+    <t>B67</t>
   </si>
   <si>
     <t>B7</t>
   </si>
   <si>
-    <t>B0</t>
+    <t>B70</t>
+  </si>
+  <si>
+    <t>B71</t>
+  </si>
+  <si>
+    <t>B72</t>
+  </si>
+  <si>
+    <t>B73</t>
+  </si>
+  <si>
+    <t>B75</t>
+  </si>
+  <si>
+    <t>B76</t>
+  </si>
+  <si>
+    <t>B77</t>
+  </si>
+  <si>
+    <t>B78</t>
   </si>
   <si>
     <t>B8</t>
   </si>
   <si>
-    <t>B*0804</t>
-  </si>
-  <si>
-    <t>B13</t>
-  </si>
-  <si>
-    <t>B*1304</t>
-  </si>
-  <si>
-    <t>B64</t>
-  </si>
-  <si>
-    <t>B65</t>
-  </si>
-  <si>
-    <t>B14</t>
-  </si>
-  <si>
-    <t>B62</t>
-  </si>
-  <si>
-    <t>B75</t>
-  </si>
-  <si>
-    <t>B72</t>
-  </si>
-  <si>
-    <t>B70</t>
-  </si>
-  <si>
-    <t>B71</t>
-  </si>
-  <si>
-    <t>B76</t>
-  </si>
-  <si>
-    <t>B77</t>
-  </si>
-  <si>
-    <t>B63</t>
-  </si>
-  <si>
-    <t>B51</t>
-  </si>
-  <si>
-    <t>B15</t>
-  </si>
-  <si>
-    <t>B50</t>
-  </si>
-  <si>
-    <t>B35</t>
-  </si>
-  <si>
-    <t>B18</t>
-  </si>
-  <si>
-    <t>B27</t>
-  </si>
-  <si>
-    <t>B2708</t>
-  </si>
-  <si>
-    <t>B37</t>
-  </si>
-  <si>
-    <t>B38</t>
-  </si>
-  <si>
-    <t>B16</t>
-  </si>
-  <si>
-    <t>B3901</t>
-  </si>
-  <si>
-    <t>B3902</t>
-  </si>
-  <si>
-    <t>B39</t>
-  </si>
-  <si>
-    <t>B*3905</t>
-  </si>
-  <si>
-    <t>B60</t>
-  </si>
-  <si>
-    <t>B61</t>
-  </si>
-  <si>
-    <t>B4005</t>
-  </si>
-  <si>
-    <t>B48</t>
-  </si>
-  <si>
-    <t>B40</t>
-  </si>
-  <si>
-    <t>B47</t>
-  </si>
-  <si>
-    <t>B21</t>
-  </si>
-  <si>
-    <t>B41</t>
-  </si>
-  <si>
-    <t>B42</t>
-  </si>
-  <si>
-    <t>B44</t>
-  </si>
-  <si>
-    <t>B45</t>
-  </si>
-  <si>
-    <t>B12</t>
-  </si>
-  <si>
-    <t>B46</t>
-  </si>
-  <si>
-    <t>B22</t>
-  </si>
-  <si>
-    <t>B17</t>
-  </si>
-  <si>
-    <t>B49</t>
-  </si>
-  <si>
-    <t>B5102</t>
-  </si>
-  <si>
-    <t>B5</t>
-  </si>
-  <si>
-    <t>B52</t>
-  </si>
-  <si>
-    <t>B53</t>
-  </si>
-  <si>
-    <t>B54</t>
-  </si>
-  <si>
-    <t>B55</t>
-  </si>
-  <si>
-    <t>B56</t>
-  </si>
-  <si>
-    <t>B78</t>
-  </si>
-  <si>
-    <t>B57</t>
-  </si>
-  <si>
-    <t>B58</t>
-  </si>
-  <si>
-    <t>B59</t>
-  </si>
-  <si>
-    <t>B67</t>
-  </si>
-  <si>
-    <t>B73</t>
-  </si>
-  <si>
     <t>B81</t>
   </si>
   <si>
-    <t>B*8201</t>
-  </si>
-  <si>
     <t>B82</t>
   </si>
   <si>
     <t>B83</t>
   </si>
   <si>
-    <t>B*07:02| B*07:03| B*07:04| B*07:05| B*07:06| B*07:07| B*07:08| B*07:09| B*07:10| B*07:11| B*07:12| B*07:13| B*07:14| B*07:15| B*07:16| B*07:17| B*07:18| B*07:19| B*07:20| B*07:21| B*07:22| B*07:23| B*07:24| B*07:25| B*07:26| B*07:27| B*07:28| B*07:29| B*07:30| B*07:31| B*07:32| B*07:33| B*07:34| B*07:35| B*07:36| B*07:37| B*07:38| B*07:39| B*07:40| B*07:41| B*07:42| B*07:43| B*07:45| B*07:46| B*07:47| B*07:48| B*07:50| B*07:51| B*07:52| B*07:53| B*07:54| B*07:55| B*07:56| B*07:57| B*07:58| B*07:59| B*07:60| B*07:61| B*07:62| B*07:63| B*07:64| B*07:65| B*07:66| B*07:68| B*07:69| B*07:70| B*07:71| B*07:72| B*07:73| B*07:74| B*07:75| B*07:76| B*07:77| B*07:78| B*07:79| B*07:80| B*07:81| B*07:82| B*07:83| B*07:84| B*07:85| B*07:86| B*07:87| B*07:88| B*07:89| B*07:90| B*07:91| B*07:92| B*07:93| B*07:94| B*07:95| B*07:96| B*07:97| B*07:98| B*07:99| B*07:100| B*07:101| B*07:102| B*07:103| B*07:104| B*07:105| B*07:106| B*07:107| B*07:108| B*07:109| B*07:110| B*07:112| B*07:113| B*07:114| B*07:115| B*07:116| B*07:117| B*07:118| B*07:119| B*07:120| B*07:121| B*07:122| B*07:123| B*07:124| B*07:125| B*07:126| B*07:127| B*07:128| B*07:129| B*07:130| B*07:131| B*07:132| B*07:133| B*07:134| B*07:136| B*07:137| B*07:138| B*07:139| B*07:140| B*07:141| B*07:142| B*07:143| B*07:144| B*07:145| B*07:146| B*07:147| B*07:148| B*07:149| B*07:150| B*07:151| B*07:152| B*07:153| B*07:154| B*07:155| B*07:156| B*07:157| B*07:158| B*07:159| B*07:160| B*07:162| B*07:163| B*07:164| B*07:165| B*07:166| B*07:168| B*07:169| B*07:170| B*07:171| B*07:172| B*07:173| B*07:174| B*07:175| B*07:176| B*07:177| B*07:178| B*07:179| B*07:180| B*07:183| B*07:184| B*07:185| B*07:186| B*07:187| B*07:188| B*07:189| B*07:190| B*07:191| B*07:192| B*07:193| B*07:194| B*07:195| B*07:196| B*07:197| B*07:198| B*07:199| B*07:200| B*07:202| B*07:203| B*07:204| B*07:205| B*07:206| B*07:207| B*07:208| B*07:209| B*07:210| B*07:211| B*07:212| B*07:213| B*07:214| B*07:215| B*07:216| B*07:217| B*07:218| B*07:219| B*07:220| B*07:221| B*07:222| B*07:223| B*07:224| B*07:225| B*07:226| B*07:227| B*07:228| B*07:229| B*07:230| B*07:232| B*07:233| B*07:234| B*07:235| B*07:236| B*07:237| B*07:238| B*07:239| B*07:240| B*07:241| B*07:242| B*07:243| B*07:244| B*07:245| B*07:246| B*07:247| B*07:248| B*07:249| B*07:250| B*07:252| B*07:253| B*07:254| B*07:255| B*07:256| B*07:257| B*07:258| B*07:259| B*07:260| B*07:261| B*07:262| B*07:263| B*07:264| B*07:265| B*07:266| B*07:267| B*07:268| B*07:269| B*07:270| B*07:271| B*07:273| B*07:274| B*07:275| B*07:276| B*07:277| B*07:278| B*07:279| B*07:280| B*07:281| B*07:282| B*07:283| B*07:284| B*07:286| B*07:287| B*07:288| B*07:289| B*07:290| B*07:291| B*07:292| B*07:293| B*07:294| B*07:295| B*07:296| B*07:297| B*07:298| B*07:299| B*07:300| B*07:301| B*07:302| B*07:303| B*07:304| B*07:305| B*56:05</t>
-  </si>
-  <si>
-    <t>B*07:44N| B*07:49N| B*07:67N| B*07:111N| B*07:135N| B*07:161N| B*07:167N| B*07:181N| B*07:182N| B*07:201N| B*07:231N| B*07:251N| B*07:272N| B*07:285N| B*08:08N| B*08:19N| B*08:30N| B*08:67N| B*08:72N| B*08:82N| B*08:86N| B*08:148N| B*13:07N| B*13:49N| B*13:56N| B*13:63N| B*13:76N| B*13:103N| B*14:07N| B*14:41N| B*15:01N| B*15:26N| B*15:79N| B*15:94N| B*15:111N| B*15:149N| B*15:181N| B*15:182N| B*15:190N| B*15:209N| B*15:226N| B*15:246N| B*15:258N| B*15:262N| B*15:272N| B*15:294N| B*15:302N| B*15:304N| B*15:375N| B*15:380N| B*15:400N| B*18:17N| B*18:23N| B*18:74N| B*18:94N| B*18:138N| B*27:59N| B*27:64N| B*27:65N| B*27:66N| B*27:94N| B*35:40N| B*35:53N| B*35:129N| B*35:130N| B*35:134N| B*35:145N| B*35:165N| B*35:173N| B*35:216N| B*37:03N| B*37:30N| B*37:33N| B*37:42N| B*38:34N| B*39:25N| B*39:40N| B*39:87N| B*39:95N| B*39:97N| B*39:116N| B*40:22N| B*40:118N| B*40:142N| B*40:144N| B*40:155N| B*40:216N| B*40:256N| B*40:263N| B*40:265N| B*40:286N| B*40:291N| B*40:337N| B*40:338N| B*40:345N| B*40:361N| B*41:45N| B*44:02S| B*44:19N| B*44:23N| B*44:52N| B*44:56N| B*44:58N| B*44:61N| B*44:108N| B*44:149N| B*44:171N| B*44:195N| B*44:198N| B*44:217N| B*44:237N| B*44:267N| B*46:07N| B*46:15N| B*46:41N| B*46:55N| B*49:19N| B*51:11N| B*51:27N| B*51:41N| B*51:44N| B*51:98N| B*51:110N| B*51:118N| B*51:149N| B*51:178N| B*51:184N| B*52:49N| B*53:48N| B*54:05N| B*54:08N| B*55:55N| B*55:83N| B*56:19N| B*56:28N| B*56:38N| B*57:28N| B*57:79N| B*58:10N| B*58:17N| B*58:31N| B*58:39N| B*58:72N| B*59:10N| B*81:04N</t>
-  </si>
-  <si>
-    <t>B*08:01| B*08:02| B*08:03| B*08:05| B*08:07| B*08:09| B*08:10| B*08:11| B*08:12| B*08:13| B*08:14| B*08:15| B*08:16| B*08:17| B*08:18| B*08:20| B*08:21| B*08:22| B*08:23| B*08:24| B*08:25| B*08:26| B*08:27| B*08:28| B*08:29| B*08:31| B*08:32| B*08:33| B*08:34| B*08:35| B*08:36| B*08:37| B*08:38| B*08:39| B*08:40| B*08:41| B*08:42| B*08:43| B*08:44| B*08:45| B*08:46| B*08:47| B*08:48| B*08:49| B*08:50| B*08:51| B*08:52| B*08:53| B*08:54| B*08:55| B*08:56| B*08:57| B*08:58| B*08:59| B*08:60| B*08:61| B*08:62| B*08:63| B*08:64| B*08:65| B*08:66| B*08:68| B*08:69| B*08:70| B*08:71| B*08:73| B*08:74| B*08:75| B*08:76| B*08:77| B*08:78| B*08:79| B*08:80| B*08:81| B*08:83| B*08:84| B*08:85| B*08:87| B*08:88| B*08:89| B*08:90| B*08:91| B*08:92| B*08:93| B*08:94| B*08:95| B*08:96| B*08:97| B*08:98| B*08:99| B*08:100| B*08:101| B*08:102| B*08:103| B*08:104| B*08:105| B*08:106| B*08:107| B*08:108| B*08:109| B*08:110| B*08:111| B*08:112| B*08:113| B*08:114| B*08:115| B*08:116| B*08:117| B*08:118| B*08:119| B*08:120| B*08:121| B*08:122| B*08:123| B*08:124| B*08:125| B*08:126| B*08:127| B*08:128| B*08:129| B*08:130| B*08:131| B*08:132| B*08:133| B*08:134| B*08:135| B*08:136| B*08:137| B*08:138| B*08:139| B*08:140| B*08:141| B*08:142| B*08:143| B*08:144| B*08:145| B*08:146| B*08:147| B*08:149| B*08:150| B*08:151| B*08:152| B*08:153| B*08:154| B*08:155| B*08:156| B*08:157| B*08:158| B*08:159| B*08:160| B*08:161| B*08:162| B*08:163| B*08:164| B*08:165| B*08:166| B*08:167| B*08:168| B*08:169| B*08:170| B*08:171| B*08:172| B*08:173| B*08:174| B*08:175| B*08:176| B*08:177| B*08:178| B*08:179| B*08:180| B*08:181| B*08:182| B*08:183| B*08:184| B*08:185| B*08:186| B*08:187| B*08:188| B*08:189| B*08:190</t>
-  </si>
-  <si>
-    <t>B*08:04</t>
-  </si>
-  <si>
-    <t>B*13:01| B*13:02| B*13:03| B*13:06| B*13:08| B*13:09| B*13:10| B*13:11| B*13:12| B*13:13| B*13:14| B*13:15| B*13:16| B*13:17| B*13:18| B*13:19| B*13:20| B*13:21| B*13:22| B*13:23| B*13:25| B*13:26| B*13:27| B*13:28| B*13:29| B*13:30| B*13:31| B*13:32| B*13:33| B*13:34| B*13:35| B*13:36| B*13:37| B*13:38| B*13:39| B*13:40| B*13:41| B*13:42| B*13:43| B*13:44| B*13:45| B*13:46| B*13:47| B*13:48| B*13:50| B*13:51| B*13:52| B*13:53| B*13:54| B*13:55| B*13:57| B*13:58| B*13:59| B*13:60| B*13:61| B*13:62| B*13:64| B*13:65| B*13:66| B*13:67| B*13:68| B*13:69| B*13:70| B*13:71| B*13:72| B*13:73| B*13:74| B*13:75| B*13:77| B*13:78| B*13:79| B*13:80| B*13:81| B*13:82| B*13:83| B*13:84| B*13:85| B*13:86| B*13:87| B*13:88| B*13:89| B*13:90| B*13:91| B*13:92| B*13:93| B*13:94| B*13:95| B*13:96| B*13:97| B*13:98| B*13:99| B*13:100| B*13:101| B*13:102| B*13:104| B*13:105| B*13:106| B*13:107| B*13:108| B*15:36</t>
+    <t>B*08:04:01| B*08:04:02</t>
   </si>
   <si>
     <t>B*13:04</t>
   </si>
   <si>
-    <t>B*14:01</t>
-  </si>
-  <si>
-    <t>B*14:02</t>
-  </si>
-  <si>
-    <t>B*14:03| B*14:04| B*14:05| B*14:06| B*14:08| B*14:09| B*14:10| B*14:11| B*14:12| B*14:13| B*14:14| B*14:15| B*14:16| B*14:17| B*14:18| B*14:19| B*14:20| B*14:21| B*14:22| B*14:23| B*14:24| B*14:25| B*14:26| B*14:27| B*14:28| B*14:29| B*14:30| B*14:31| B*14:32| B*14:33| B*14:34| B*14:35| B*14:36| B*14:37| B*14:38| B*14:39| B*14:40| B*14:42| B*14:43| B*14:44| B*14:45| B*14:46| B*14:47| B*14:48| B*14:49| B*14:50| B*14:51| B*14:52| B*14:53| B*14:54| B*14:55| B*14:56| B*14:57| B*14:58| B*14:59| B*14:01| B*14:02</t>
-  </si>
-  <si>
-    <t>B*15:01| B*15:04| B*15:05| B*15:06| B*15:07| B*15:15| B*15:20| B*15:24| B*15:25| B*15:27| B*15:28| B*15:30| B*15:32| B*15:34| B*15:35| B*15:38| B*15:39| B*15:40| B*15:45| B*15:48| B*15:50| B*15:56| B*15:57| B*15:58| B*15:60| B*15:63| B*15:65| B*15:66| B*15:70| B*15:71| B*15:73| B*15:75| B*15:77| B*15:81| B*15:82| B*15:83| B*15:84| B*15:85| B*15:92| B*15:96| B*15:97| B*15:102| B*15:107| B*15:146</t>
-  </si>
-  <si>
-    <t>B*15:02| B*15:08| B*15:11| B*15:21| B*15:31| B*15:44| B*15:88</t>
-  </si>
-  <si>
-    <t>B*15:03| B*15:49| B*15:54| B*15:61| B*15:69| B*15:74| B*15:98</t>
-  </si>
-  <si>
-    <t>B*15:09| B*15:29| B*15:37| B*15:47| B*15:51| B*15:80| B*15:103| B*15:114| B*15:220| B*15:10| B*15:18| B*15:64| B*15:72| B*15:90| B*15:93| B*15:99| B*15:108| B*15:03| B*15:49| B*15:54| B*15:61| B*15:69| B*15:74| B*15:98</t>
-  </si>
-  <si>
-    <t>B*15:10| B*15:18| B*15:64| B*15:72| B*15:90| B*15:93| B*15:99| B*15:108</t>
-  </si>
-  <si>
-    <t>B*15:12| B*15:14| B*15:19</t>
-  </si>
-  <si>
-    <t>B*15:13| B*15:89</t>
-  </si>
-  <si>
-    <t>B*15:16| B*15:17| B*15:67| B*15:95</t>
-  </si>
-  <si>
-    <t>B*15:23| B*51:01| B*51:03| B*51:04| B*51:05| B*51:06| B*51:07| B*51:08| B*51:09| B*51:10| B*51:12| B*51:13| B*51:14| B*51:15| B*51:17| B*51:18| B*51:19| B*51:20| B*51:21| B*51:22| B*51:23| B*51:24| B*51:26| B*51:28| B*51:29| B*51:30| B*51:31| B*51:32| B*51:33| B*51:34| B*51:35| B*51:36| B*51:37| B*51:38| B*51:39| B*51:40| B*51:43| B*51:45| B*51:46| B*51:48| B*51:49| B*51:50| B*51:51| B*51:52| B*51:53| B*51:54| B*51:55| B*51:56| B*51:57| B*51:58| B*51:59| B*51:60| B*51:61| B*51:62| B*51:63| B*51:64| B*51:65| B*51:66| B*51:67| B*51:68| B*51:69| B*51:70| B*51:71| B*51:72| B*51:73| B*51:74| B*51:75| B*51:76| B*51:77| B*51:78| B*51:79| B*51:80| B*51:81| B*51:82| B*51:83| B*51:84| B*51:85| B*51:86| B*51:87| B*51:88| B*51:89| B*51:90| B*51:91| B*51:92| B*51:93| B*51:94| B*51:95| B*51:96| B*51:97| B*51:99| B*51:100| B*51:101| B*51:102| B*51:103| B*51:104| B*51:105| B*51:106| B*51:107| B*51:108| B*51:109| B*51:111| B*51:112| B*51:113| B*51:114| B*51:115| B*51:116| B*51:117| B*51:119| B*51:120| B*51:121| B*51:122| B*51:123| B*51:124| B*51:125| B*51:126| B*51:127| B*51:128| B*51:129| B*51:130| B*51:131| B*51:132| B*51:133| B*51:134| B*51:135| B*51:136| B*51:137| B*51:138| B*51:139| B*51:140| B*51:141| B*51:142| B*51:143| B*51:144| B*51:145| B*51:146| B*51:147| B*51:148| B*51:150| B*51:151| B*51:152| B*51:153| B*51:154| B*51:155| B*51:156| B*51:157| B*51:158| B*51:159| B*51:160| B*51:161| B*51:162| B*51:163| B*51:164| B*51:165| B*51:166| B*51:167| B*51:168| B*51:169| B*51:170| B*51:171| B*51:172| B*51:173Q| B*51:174| B*51:175| B*51:176| B*51:177| B*51:179| B*51:180| B*51:181| B*51:182| B*51:183| B*51:185| B*51:186| B*51:187| B*51:188| B*51:189| B*51:190| B*51:191| B*51:192| B*51:193| B*51:194| B*51:195| B*51:196| B*51:197| B*51:198| B*51:199| B*51:200| B*51:201| B*51:202| B*51:203| B*51:204| B*51:205| B*51:206| B*51:207| B*51:208| B*51:209| B*51:210| B*51:211| B*51:212| B*51:213| B*51:214| B*51:215| B*51:216| B*51:217| B*51:218| B*51:219| B*51:220| B*51:221| B*51:222| B*51:223| B*51:224| B*51:225| B*51:226| B*51:227| B*51:228| B*51:229</t>
-  </si>
-  <si>
-    <t>B*15:33| B*15:42| B*15:43| B*15:52| B*15:53| B*15:55| B*15:62| B*15:76| B*15:78| B*15:86| B*15:87| B*15:91| B*15:101| B*15:104| B*15:105| B*15:106| B*15:109| B*15:110| B*15:112| B*15:113| B*15:115| B*15:116| B*15:117| B*15:118| B*15:119| B*15:120| B*15:121| B*15:122| B*15:123| B*15:124| B*15:125| B*15:126| B*15:127| B*15:128| B*15:129| B*15:131| B*15:132| B*15:133| B*15:134| B*15:135| B*15:136| B*15:137| B*15:138| B*15:139| B*15:140| B*15:141| B*15:142| B*15:143| B*15:144| B*15:145| B*15:147| B*15:148| B*15:150| B*15:151| B*15:152| B*15:153| B*15:154| B*15:155| B*15:156| B*15:157| B*15:158| B*15:159| B*15:160| B*15:161| B*15:162| B*15:163| B*15:164| B*15:165| B*15:166| B*15:167| B*15:168| B*15:169| B*15:170| B*15:171| B*15:172| B*15:173| B*15:174| B*15:175| B*15:176| B*15:177| B*15:178| B*15:179| B*15:180| B*15:183| B*15:184| B*15:185| B*15:186| B*15:187| B*15:188| B*15:189| B*15:191| B*15:192| B*15:193| B*15:194| B*15:195| B*15:196| B*15:197| B*15:198| B*15:199| B*15:200| B*15:201| B*15:202| B*15:203| B*15:204| B*15:205| B*15:206| B*15:207| B*15:208| B*15:210| B*15:211| B*15:212| B*15:213| B*15:214| B*15:215| B*15:216| B*15:217| B*15:218Q| B*15:219| B*15:221| B*15:222| B*15:223| B*15:224| B*15:225| B*15:227| B*15:228| B*15:229| B*15:230| B*15:231| B*15:232| B*15:233| B*15:234| B*15:235| B*15:236| B*15:237| B*15:238| B*15:239| B*15:240| B*15:241| B*15:242| B*15:243| B*15:244| B*15:245Q| B*15:247| B*15:248| B*15:249| B*15:250| B*15:251| B*15:252| B*15:253| B*15:254| B*15:255| B*15:256| B*15:257| B*15:259| B*15:260| B*15:261| B*15:263| B*15:264| B*15:265| B*15:266| B*15:267| B*15:268| B*15:269| B*15:270| B*15:271| B*15:273| B*15:274| B*15:275| B*15:276| B*15:277| B*15:278| B*15:279| B*15:280| B*15:281| B*15:282| B*15:283| B*15:284| B*15:285| B*15:286| B*15:287| B*15:288| B*15:289| B*15:290| B*15:291| B*15:292| B*15:293| B*15:295| B*15:296| B*15:297| B*15:298| B*15:299| B*15:300| B*15:301| B*15:303| B*15:305| B*15:306| B*15:307| B*15:308| B*15:309| B*15:310| B*15:311| B*15:312| B*15:313| B*15:314| B*15:315| B*15:316| B*15:317| B*15:318| B*15:319| B*15:320| B*15:321Q| B*15:322| B*15:323| B*15:324| B*15:325| B*15:326| B*15:327| B*15:328| B*15:329| B*15:330| B*15:331| B*15:332| B*15:333| B*15:334| B*15:335| B*15:336| B*15:337| B*15:338| B*15:339| B*15:340| B*15:341| B*15:342| B*15:343| B*15:344| B*15:345| B*15:346| B*15:347| B*15:348| B*15:349| B*15:350| B*15:351| B*15:352| B*15:353| B*15:354| B*15:355| B*15:356| B*15:357| B*15:358| B*15:359| B*15:360| B*15:361| B*15:362| B*15:363| B*15:364| B*15:365| B*15:366| B*15:367| B*15:368| B*15:369| B*15:370| B*15:371| B*15:372| B*15:373| B*15:374| B*15:376| B*15:377Q| B*15:378| B*15:379| B*15:381| B*15:382| B*15:383| B*15:384| B*15:385| B*15:386| B*15:387| B*15:388| B*15:389| B*15:390| B*15:391| B*15:392| B*15:393| B*15:394| B*15:395| B*15:396| B*15:397| B*15:398| B*15:399| B*15:401| B*15:402| B*15:403| B*15:404| B*15:405| B*15:406| B*15:407| B*15:408| B*15:409| B*15:410| B*15:411| B*15:412| B*15:413| B*15:414| B*15:415| B*15:416| B*15:417| B*15:418| B*15:419| B*15:420| B*15:421| B*15:422| B*15:423| B*15:424| B*15:425| B*15:426| B*15:427| B*15:428| B*15:429| B*15:430| B*15:431| B*15:432| B*15:433| B*15:434| B*15:435| B*15:01| B*15:04| B*15:05| B*15:06| B*15:07| B*15:15| B*15:20| B*15:24| B*15:25| B*15:27| B*15:28| B*15:30| B*15:32| B*15:34| B*15:35| B*15:38| B*15:39| B*15:40| B*15:45| B*15:48| B*15:50| B*15:56| B*15:57| B*15:58| B*15:60| B*15:63| B*15:65| B*15:66| B*15:70| B*15:71| B*15:73| B*15:75| B*15:77| B*15:81| B*15:82| B*15:83| B*15:84| B*15:85| B*15:92| B*15:96| B*15:97| B*15:102| B*15:107| B*15:146| B*15:16| B*15:17| B*15:67| B*15:95| B*15:02| B*15:08| B*15:11| B*15:21| B*15:31| B*15:44| B*15:88| B*15:12| B*15:14| B*15:19| B*15:13| B*15:89</t>
-  </si>
-  <si>
-    <t>B*15:46| B*50:01| B*50:04| B*50:05| B*50:06| B*50:07| B*50:08| B*50:09| B*50:10| B*50:11| B*50:12| B*50:13| B*50:14| B*50:15| B*50:16| B*50:17| B*50:18| B*50:19| B*50:20| B*50:31| B*50:32| B*50:33| B*50:34| B*50:35| B*50:36| B*50:37| B*50:38| B*50:39| B*50:40| B*50:41| B*50:42| B*50:43| B*50:44| B*50:45| B*50:46| B*50:47| B*50:48| B*50:49| B*50:50| B*50:51| B*50:52| B*50:53| B*50:54| B*40:05</t>
-  </si>
-  <si>
-    <t>B*15:68| B*35:01| B*35:02| B*35:03| B*35:04| B*35:05| B*35:06| B*35:07| B*35:08| B*35:09| B*35:10| B*35:11| B*35:12| B*35:13| B*35:14| B*35:15| B*35:16| B*35:17| B*35:18| B*35:19| B*35:20| B*35:21| B*35:22| B*35:23| B*35:24| B*35:25| B*35:26| B*35:27| B*35:28| B*35:29| B*35:30| B*35:31| B*35:32| B*35:33| B*35:34| B*35:35| B*35:36| B*35:37| B*35:38| B*35:39| B*35:41| B*35:42| B*35:43| B*35:44| B*35:45| B*35:46| B*35:47| B*35:48| B*35:49| B*35:50| B*35:51| B*35:52| B*35:54| B*35:55| B*35:56| B*35:57| B*35:58| B*35:59| B*35:60| B*35:61| B*35:62| B*35:63| B*35:64| B*35:65Q| B*35:66| B*35:67| B*35:68| B*35:69| B*35:70| B*35:71| B*35:72| B*35:74| B*35:75| B*35:76| B*35:77| B*35:78| B*35:79| B*35:80| B*35:81| B*35:82| B*35:83| B*35:84| B*35:85| B*35:86| B*35:87| B*35:88| B*35:89| B*35:90| B*35:91| B*35:92| B*35:93| B*35:94| B*35:95| B*35:96| B*35:97| B*35:98| B*35:99| B*35:100| B*35:101| B*35:102| B*35:103| B*35:104| B*35:105| B*35:106| B*35:107| B*35:108| B*35:109| B*35:110| B*35:111| B*35:112| B*35:113| B*35:114| B*35:115| B*35:116| B*35:117| B*35:118| B*35:119| B*35:120| B*35:121| B*35:122| B*35:123| B*35:124| B*35:125| B*35:126| B*35:127| B*35:128| B*35:131| B*35:132| B*35:133| B*35:135| B*35:136| B*35:137| B*35:138| B*35:139| B*35:140| B*35:141| B*35:142| B*35:143| B*35:144| B*35:146| B*35:147| B*35:148| B*35:149| B*35:150| B*35:151| B*35:152| B*35:153| B*35:154| B*35:155| B*35:156| B*35:157| B*35:158| B*35:159| B*35:160| B*35:161| B*35:162| B*35:163| B*35:164| B*35:166| B*35:167| B*35:168| B*35:169| B*35:170| B*35:171| B*35:172| B*35:174| B*35:175| B*35:176| B*35:177| B*35:178| B*35:179| B*35:180| B*35:181| B*35:182| B*35:183| B*35:184| B*35:185| B*35:186| B*35:187| B*35:188| B*35:189| B*35:190| B*35:191| B*35:192| B*35:193| B*35:194| B*35:195| B*35:196| B*35:197| B*35:198| B*35:199| B*35:200| B*35:201| B*35:202| B*35:203| B*35:204| B*35:205| B*35:206| B*35:207| B*35:208| B*35:209| B*35:210| B*35:211| B*35:212| B*35:213| B*35:214| B*35:215| B*35:217| B*35:218| B*35:219| B*35:220| B*35:221| B*35:222| B*35:223| B*35:224| B*35:225| B*35:226| B*35:227| B*35:228| B*35:229| B*35:230| B*35:231| B*35:232| B*35:233| B*35:234| B*35:235| B*35:236| B*35:237| B*35:238| B*35:239| B*35:240| B*35:241| B*35:242| B*35:243| B*35:244| B*35:245| B*35:246| B*35:247| B*35:248| B*35:249| B*35:250| B*35:251| B*35:252| B*35:253| B*35:254| B*35:255| B*35:256| B*35:257| B*35:258| B*35:259| B*35:260| B*35:261| B*35:262| B*35:263| B*35:264| B*35:265| B*35:266| B*35:267| B*35:268| B*35:269| B*35:270| B*35:271| B*35:272| B*35:273| B*35:274| B*35:275| B*35:276| B*35:277| B*35:278| B*35:279| B*35:280| B*35:281| B*35:282| B*35:283| B*35:284| B*35:285| B*35:286| B*35:287| B*35:288| B*35:289| B*35:290| B*35:291| B*35:292| B*35:293| B*35:294| B*35:295| B*35:296| B*35:297| B*35:298| B*35:299| B*35:300| B*35:301| B*35:302| B*35:303| B*35:304| B*35:305| B*35:306| B*35:307| B*35:308| B*35:309| B*35:310| B*35:311| B*35:312| B*35:313| B*35:314| B*35:315| B*35:316| B*35:317| B*35:318| B*35:319| B*35:320| B*35:321| B*35:322| B*35:323| B*35:324| B*35:325| B*35:326| B*35:327| B*35:328| B*35:329| B*35:330| B*35:331| B*35:332| B*35:333Q| B*35:334| B*35:335| B*35:336| B*35:337| B*35:338| B*35:339| B*35:340| B*35:341| B*35:342| B*35:343| B*35:344| B*35:345| B*35:346| B*35:347| B*35:348| B*35:349| B*35:350| B*35:351| B*35:352| B*35:353| B*35:354| B*35:355| B*35:356| B*35:357| B*35:358| B*35:359| B*35:360| B*78:04</t>
-  </si>
-  <si>
-    <t>B*18:01| B*18:02| B*18:03| B*18:04| B*18:05| B*18:06| B*18:07| B*18:08| B*18:09| B*18:10| B*18:11| B*18:12| B*18:13| B*18:14| B*18:15| B*18:18| B*18:19| B*18:20| B*18:21| B*18:22| B*18:24| B*18:25| B*18:26| B*18:27| B*18:28| B*18:29| B*18:30| B*18:31| B*18:32| B*18:33| B*18:34| B*18:35| B*18:36| B*18:37| B*18:38| B*18:39| B*18:40| B*18:41| B*18:42| B*18:43| B*18:44| B*18:45| B*18:46| B*18:47| B*18:48| B*18:49| B*18:50| B*18:51| B*18:52| B*18:53| B*18:54| B*18:55| B*18:56| B*18:57| B*18:58| B*18:59| B*18:60| B*18:61| B*18:62| B*18:63| B*18:64| B*18:65| B*18:66| B*18:67| B*18:68| B*18:69| B*18:70| B*18:71| B*18:72| B*18:73| B*18:75| B*18:76| B*18:77| B*18:78| B*18:79| B*18:80| B*18:81| B*18:82| B*18:83| B*18:84| B*18:85| B*18:86| B*18:87| B*18:88| B*18:89| B*18:90| B*18:91| B*18:92| B*18:93| B*18:95| B*18:96| B*18:97| B*18:98| B*18:99| B*18:100| B*18:101| B*18:102| B*18:103| B*18:104| B*18:105| B*18:106| B*18:107| B*18:108| B*18:109| B*18:110| B*18:111| B*18:112| B*18:113| B*18:114| B*18:115| B*18:116| B*18:117| B*18:118| B*18:119| B*18:120| B*18:121| B*18:122| B*18:123| B*18:124| B*18:125| B*18:126| B*18:127| B*18:128| B*18:129| B*18:130| B*18:131| B*18:132| B*18:133| B*18:134| B*18:135| B*18:136| B*18:137| B*18:139| B*18:140| B*18:141| B*18:142| B*18:143</t>
-  </si>
-  <si>
-    <t>B*27:01| B*27:02| B*27:03| B*27:04| B*27:05| B*27:05Q| B*27:06| B*27:07| B*27:09| B*27:10| B*27:11| B*27:12| B*27:13| B*27:14| B*27:15| B*27:16| B*27:17| B*27:18| B*27:19| B*27:20| B*27:21| B*27:23| B*27:24| B*27:25| B*27:26| B*27:27| B*27:28| B*27:29| B*27:30| B*27:31| B*27:32| B*27:33| B*27:34| B*27:35| B*27:36| B*27:37| B*27:38| B*27:39| B*27:40| B*27:41| B*27:42| B*27:43| B*27:44| B*27:45| B*27:46| B*27:47| B*27:48| B*27:49| B*27:50| B*27:51| B*27:52| B*27:53| B*27:54| B*27:55| B*27:56| B*27:57| B*27:58| B*27:60| B*27:61| B*27:62| B*27:63| B*27:67| B*27:68| B*27:69| B*27:70| B*27:71| B*27:72| B*27:73| B*27:74| B*27:75| B*27:76| B*27:77| B*27:78| B*27:79| B*27:80| B*27:81| B*27:82| B*27:83| B*27:84| B*27:85| B*27:86| B*27:87| B*27:88| B*27:89| B*27:90| B*27:91| B*27:92| B*27:93| B*27:95| B*27:96| B*27:97| B*27:98| B*27:99| B*27:100| B*27:101| B*27:102| B*27:103| B*27:104| B*27:105| B*27:106| B*27:107| B*27:108| B*27:109| B*27:110| B*27:111| B*27:112| B*27:113| B*27:114| B*27:115| B*27:116| B*27:117| B*27:118| B*27:119| B*27:120| B*27:121| B*27:122| B*27:123| B*27:124| B*27:125| B*27:126| B*27:127| B*27:128| B*27:129| B*27:130| B*27:131| B*27:132| B*27:133| B*27:134| B*27:135| B*27:136| B*27:137| B*27:138| B*27:139| B*27:140| B*27:141| B*27:142| B*27:143| B*27:144| B*27:145| B*27:146| B*27:147| B*27:148| B*27:149| B*27:150| B*27:151| B*27:152| B*27:153| B*27:154| B*27:155| B*27:156| B*27:157| B*27:158| B*27:159| B*27:160| B*27:161| B*27:162| B*27:163| B*27:164| B*27:165| B*27:166| B*27:167</t>
+    <t>B*39:05:01:01| B*39:05:01:02| B*39:05:02| B*39:05:03</t>
+  </si>
+  <si>
+    <t>B*82:01:01:01| B*82:01:01:02| B*82:01:02| B*82:02:01:01| B*82:02:01:02| B*82:02:02| B*82:03</t>
+  </si>
+  <si>
+    <t>B*07:44N| B*07:49N| B*07:67N| B*07:111N| B*07:135N| B*07:161N| B*07:167N| B*07:181N| B*07:182N| B*07:201N| B*07:231N| B*07:251N| B*07:272N| B*07:285N| B*07:315N| B*07:316N| B*07:318N| B*07:325N| B*07:330N| B*07:343N| B*07:351N| B*08:08N| B*08:19N| B*08:30N| B*08:67N| B*08:72N| B*08:82N| B*08:86N| B*08:148N| B*08:214N| B*08:215N| B*08:220N| B*13:07N| B*13:49N| B*13:56:01N| B*13:56:02N| B*13:63N| B*13:76N| B*13:103N| B*13:116N| B*14:07N| B*14:41N| B*15:01:01:02N| B*15:26N| B*15:79N| B*15:94N| B*15:111N| B*15:149N| B*15:181N| B*15:182N| B*15:190N| B*15:209N| B*15:226N| B*15:246N| B*15:258N| B*15:262N| B*15:272N| B*15:294N| B*15:302N| B*15:304N| B*15:375N| B*15:380N| B*15:400N| B*15:454N| B*15:463N| B*15:483N| B*15:487N| B*15:496N| B*18:17N| B*18:23N| B*18:74N| B*18:94N| B*18:138N| B*18:154N| B*27:59N| B*27:64N| B*27:65N| B*27:66N| B*27:94N| B*27:176N| B*35:40N| B*35:53N| B*35:129N| B*35:130N| B*35:134N| B*35:145N| B*35:165N| B*35:173:01N| B*35:173:02N| B*35:216N| B*35:381N| B*35:390N| B*37:03N| B*37:30N| B*37:33N| B*37:42N| B*37:79N| B*38:34N| B*38:80N| B*39:25N| B*39:40:01N| B*39:40:02N| B*39:87N| B*39:95N| B*39:97N| B*39:116N| B*39:133N| B*39:139N| B*39:142N| B*40:22N| B*40:118N| B*40:142N| B*40:144N| B*40:155:01N| B*40:155:02N| B*40:216N| B*40:256N| B*40:263N| B*40:265N| B*40:286N| B*40:291N| B*40:337N| B*40:338N| B*40:345N| B*40:361N| B*40:372N| B*40:399N| B*41:45N| B*44:02:01:02S| B*44:19N| B*44:23N| B*44:52N| B*44:56N| B*44:58N| B*44:61N| B*44:108N| B*44:149N| B*44:171N| B*44:195N| B*44:198N| B*44:217N| B*44:237N| B*44:267N| B*44:303N| B*44:306N| B*44:309N| B*44:310N| B*44:314N| B*44:328N| B*44:333N| B*46:07N| B*46:15N| B*46:41N| B*46:55N| B*49:19N| B*51:11N| B*51:27N| B*51:41N| B*51:44N| B*51:98N| B*51:110N| B*51:118N| B*51:149N| B*51:178N| B*51:184N| B*51:235N| B*51:245N| B*51:256N| B*51:264N| B*52:49N| B*53:48N| B*54:05N| B*54:08N| B*55:55N| B*55:83N| B*55:89N| B*55:97N| B*56:01:01:05S| B*56:19N| B*56:28N| B*56:38N| B*57:28N| B*57:79N| B*58:10N| B*58:17N| B*58:31N| B*58:39N| B*58:72N| B*58:93N| B*58:94N| B*59:10N| B*81:04N</t>
+  </si>
+  <si>
+    <t>B*44:15:01:01| B*44:15:01:02| B*44:46| B*44:02:01:01| B*44:02:01:03| B*44:02:01:04| B*44:02:01:05| B*44:02:01:06| B*44:02:01:07| B*44:02:01:08| B*44:02:01:09| B*44:02:01:10| B*44:02:01:11| B*44:02:01:12| B*44:02:01:13| B*44:02:01:14| B*44:02:01:15| B*44:02:01:16| B*44:02:01:17| B*44:02:01:18| B*44:02:01:19| B*44:02:01:20| B*44:02:02| B*44:02:03| B*44:02:04| B*44:02:05| B*44:02:06| B*44:02:07| B*44:02:08| B*44:02:09| B*44:02:10| B*44:02:11| B*44:02:12| B*44:02:13| B*44:02:14| B*44:02:15| B*44:02:16| B*44:02:17| B*44:02:18| B*44:02:19| B*44:02:20| B*44:02:21| B*44:02:22| B*44:02:23| B*44:02:24| B*44:02:25| B*44:02:26| B*44:02:27| B*44:02:28| B*44:02:29| B*44:02:30| B*44:02:31| B*44:02:32| B*44:02:33| B*44:02:34| B*44:02:35| B*44:02:36| B*44:02:37| B*44:02:38| B*44:02:39| B*44:02:40| B*44:02:41| B*44:02:42| B*44:02:43| B*44:02:44| B*44:02:45| B*44:02:46| B*44:02:47| B*44:02:48| B*44:02:49| B*44:02:50| B*44:02:51| B*44:02:52| B*44:02:53| B*44:02:54| B*44:02:55| B*44:02:56| B*44:02:57| B*44:02:58| B*44:03:01:01| B*44:03:01:02| B*44:03:01:03| B*44:03:01:04| B*44:03:01:05| B*44:03:01:06| B*44:03:01:07| B*44:03:01:08| B*44:03:01:09| B*44:03:01:10| B*44:03:01:11| B*44:03:01:12| B*44:03:01:13| B*44:03:01:14| B*44:03:01:15| B*44:03:01:16| B*44:03:02| B*44:03:03| B*44:03:04| B*44:03:05| B*44:03:06| B*44:03:07| B*44:03:08| B*44:03:09| B*44:03:10| B*44:03:11| B*44:03:12| B*44:03:13| B*44:03:14| B*44:03:15| B*44:03:16| B*44:03:17| B*44:03:18| B*44:03:19| B*44:03:20| B*44:03:21| B*44:03:22| B*44:03:23| B*44:03:24| B*44:03:25| B*44:03:26| B*44:03:27| B*44:03:28| B*44:03:29| B*44:03:30| B*44:03:31| B*44:03:32| B*44:03:33| B*44:03:34| B*44:03:35| B*44:03:36| B*44:03:37| B*44:03:38| B*44:03:39| B*44:03:40| B*44:03:41| B*44:03:42| B*44:03:43| B*44:03:44| B*44:03:45| B*44:03:46| B*44:03:47| B*44:03:48| B*44:04| B*44:05:01| B*44:05:02| B*44:05:03| B*44:05:04| B*44:06| B*44:07| B*44:08| B*44:10| B*44:11| B*44:12| B*44:13| B*44:14| B*44:17| B*44:18| B*44:20| B*44:21| B*44:22| B*44:24| B*44:25| B*44:26| B*44:27:01:01| B*44:27:01:02| B*44:27:02| B*44:27:03| B*44:28:01| B*44:28:02| B*44:29| B*44:30| B*44:31| B*44:32| B*44:33| B*44:34:01| B*44:34:02| B*44:35| B*44:36| B*44:37:01| B*44:37:02| B*44:38| B*44:39| B*44:40| B*44:41:01| B*44:41:02| B*44:43:01| B*44:43:02| B*44:44| B*44:45| B*44:47| B*44:48| B*44:49| B*44:50:01| B*44:50:02| B*44:51| B*44:53:01| B*44:53:02| B*44:54| B*44:55| B*44:57| B*44:59:01| B*44:59:02| B*44:60| B*44:62| B*44:63| B*44:64:01| B*44:64:02| B*44:65| B*44:66| B*44:67| B*44:68| B*44:69:01| B*44:69:02| B*44:70| B*44:71| B*44:72| B*44:73| B*44:74| B*44:75| B*44:76| B*44:77| B*44:78| B*44:79:01| B*44:79:02| B*44:80| B*44:81| B*44:82| B*44:83| B*44:84:01| B*44:84:02| B*44:85| B*44:86| B*44:87| B*44:88| B*44:89| B*44:90| B*44:91| B*44:92| B*44:93| B*44:94| B*44:95| B*44:96| B*44:97| B*44:98| B*44:99| B*44:100| B*44:101| B*44:102| B*44:103| B*44:104| B*44:105| B*44:106| B*44:107| B*44:109| B*44:110| B*44:111| B*44:112| B*44:113| B*44:114| B*44:115| B*44:116| B*44:117| B*44:118| B*44:119| B*44:120| B*44:121| B*44:122| B*44:123| B*44:124| B*44:125| B*44:126:01| B*44:126:02| B*44:127| B*44:128:01| B*44:128:02| B*44:129| B*44:130| B*44:131| B*44:132| B*44:133| B*44:134| B*44:135| B*44:136| B*44:137| B*44:138Q| B*44:139| B*44:140| B*44:141| B*44:142| B*44:143| B*44:144| B*44:145| B*44:146| B*44:147| B*44:148| B*44:150| B*44:151| B*44:152| B*44:153| B*44:154| B*44:155| B*44:156| B*44:157| B*44:158| B*44:159| B*44:160Q| B*44:161| B*44:162| B*44:163:01| B*44:163:02| B*44:164| B*44:165| B*44:166| B*44:167| B*44:168| B*44:169| B*44:170| B*44:172| B*44:173| B*44:174| B*44:175| B*44:176| B*44:177| B*44:178| B*44:179| B*44:180| B*44:181| B*44:182| B*44:183| B*44:184| B*44:185| B*44:186:01| B*44:186:02| B*44:187| B*44:188| B*44:189| B*44:190| B*44:191| B*44:192:01| B*44:192:02| B*44:192:03| B*44:193| B*44:194| B*44:196| B*44:197| B*44:199| B*44:200| B*44:201| B*44:202| B*44:203:01| B*44:203:02| B*44:204| B*44:205:01| B*44:205:02| B*44:206| B*44:207| B*44:208| B*44:209| B*44:210:01| B*44:210:02| B*44:211| B*44:212| B*44:213| B*44:214| B*44:215| B*44:216| B*44:218| B*44:219| B*44:220| B*44:221| B*44:222| B*44:223| B*44:224| B*44:225| B*44:226| B*44:227| B*44:228| B*44:229| B*44:230| B*44:231| B*44:232| B*44:233| B*44:234| B*44:235| B*44:236| B*44:238| B*44:239| B*44:240| B*44:241| B*44:242| B*44:243| B*44:244| B*44:245| B*44:247| B*44:248| B*44:249| B*44:250| B*44:251| B*44:252| B*44:253| B*44:254| B*44:255| B*44:256| B*44:257| B*44:258| B*44:259| B*44:260| B*44:261| B*44:262| B*44:263| B*44:264| B*44:265| B*44:266| B*44:268| B*44:269| B*44:270:01| B*44:270:02| B*44:271| B*44:272| B*44:273| B*44:274| B*44:275| B*44:276| B*44:277| B*44:278| B*44:279| B*44:280| B*44:281| B*44:282| B*44:283| B*44:284| B*44:285| B*44:286| B*44:287| B*44:288| B*44:289| B*44:290| B*44:291| B*44:292| B*44:293| B*44:294| B*44:295| B*44:296| B*44:297| B*44:298| B*44:299| B*44:300| B*44:301| B*44:302| B*44:304| B*44:305| B*44:307| B*44:308| B*44:311| B*44:312| B*44:313| B*44:315| B*44:316| B*44:317| B*44:318| B*44:319| B*44:320| B*44:321| B*44:322| B*44:323| B*44:324| B*44:325| B*44:326| B*44:327| B*44:329| B*44:330| B*44:331| B*44:332| B*51:42| B*44:09| B*45:01:01:01| B*45:01:01:02| B*45:01:02| B*45:01:03| B*45:01:04| B*45:01:05| B*45:02| B*45:03| B*45:05| B*45:06| B*45:07| B*45:08| B*45:09| B*45:10| B*45:11| B*45:12| B*45:13| B*45:14| B*45:15| B*45:16| B*45:17| B*45:18| B*45:19| B*45:20| B*45:21| B*45:22| B*45:23| B*45:24| B*50:02</t>
+  </si>
+  <si>
+    <t>B*13:01:01:01| B*13:01:01:02| B*13:01:02| B*13:01:03| B*13:01:04| B*13:01:05| B*13:01:06| B*13:01:07| B*13:01:08| B*13:01:09| B*13:01:10| B*13:01:11| B*13:01:12| B*13:01:13| B*13:01:14| B*13:02:01:01| B*13:02:01:02| B*13:02:01:03| B*13:02:01:04| B*13:02:01:05| B*13:02:01:06| B*13:02:02| B*13:02:03| B*13:02:04| B*13:02:05| B*13:02:06| B*13:02:07| B*13:02:08| B*13:02:09| B*13:02:10| B*13:02:11| B*13:02:12| B*13:02:13| B*13:02:14| B*13:02:15| B*13:02:16| B*13:02:17| B*13:02:18| B*13:02:19| B*13:02:20| B*13:02:21| B*13:02:22| B*13:02:23| B*13:02:24| B*13:02:25| B*13:02:26| B*13:02:27| B*13:02:28| B*13:03| B*13:06| B*13:08| B*13:09| B*13:10| B*13:11| B*13:12:01| B*13:12:02| B*13:13:01| B*13:13:02| B*13:14| B*13:15| B*13:16| B*13:17| B*13:18| B*13:19| B*13:20| B*13:21| B*13:22:01| B*13:22:02| B*13:23| B*13:25| B*13:26:01| B*13:26:02| B*13:27| B*13:28| B*13:29| B*13:30| B*13:31| B*13:32| B*13:33| B*13:34| B*13:35| B*13:36| B*13:37| B*13:38| B*13:39| B*13:40| B*13:41| B*13:42| B*13:43| B*13:44| B*13:45| B*13:46| B*13:47| B*13:48| B*13:50| B*13:51| B*13:52| B*13:53| B*13:54| B*13:55| B*13:57| B*13:58| B*13:59| B*13:60| B*13:61| B*13:62| B*13:64| B*13:65| B*13:66| B*13:67| B*13:68| B*13:69| B*13:70| B*13:71| B*13:72| B*13:73| B*13:74| B*13:75| B*13:77| B*13:78| B*13:79| B*13:80| B*13:81| B*13:82| B*13:83| B*13:84| B*13:85| B*13:86| B*13:87| B*13:88| B*13:89| B*13:90| B*13:91| B*13:92| B*13:93| B*13:94| B*13:95| B*13:96| B*13:97| B*13:98| B*13:99| B*13:100| B*13:101| B*13:102| B*13:104| B*13:105| B*13:106| B*13:107| B*13:108| B*13:109| B*13:110| B*13:111| B*13:112| B*13:113| B*13:114| B*13:115| B*13:117| B*13:118| B*13:119| B*13:120| B*13:121| B*13:122| B*13:123Q| B*13:124| B*13:125| B*13:126| B*13:127| B*13:128| B*13:129| B*13:130| B*15:36</t>
+  </si>
+  <si>
+    <t>B*14:03| B*14:04| B*14:05| B*14:06:01| B*14:06:02| B*14:08:01| B*14:08:02| B*14:09| B*14:10| B*14:11| B*14:12| B*14:13| B*14:14| B*14:15| B*14:16| B*14:17| B*14:18| B*14:19| B*14:20| B*14:21| B*14:22| B*14:23| B*14:24| B*14:25| B*14:26| B*14:27| B*14:28| B*14:29| B*14:30| B*14:31| B*14:32| B*14:33| B*14:34| B*14:35| B*14:36| B*14:37| B*14:38| B*14:39| B*14:40| B*14:42| B*14:43| B*14:44| B*14:45| B*14:46| B*14:47| B*14:48| B*14:49| B*14:50| B*14:51| B*14:52| B*14:53| B*14:54| B*14:55| B*14:56| B*14:57| B*14:58| B*14:59| B*14:60| B*14:61| B*14:62| B*14:63| B*14:64| B*14:65| B*14:66| B*14:67| B*14:68| B*14:01:01:01| B*14:01:01:02| B*14:01:01:03| B*14:01:02| B*14:01:03| B*14:01:04| B*14:01:05| B*14:01:06| B*14:01:07| B*14:01:08| B*14:01:09| B*14:02:01:01| B*14:02:01:02| B*14:02:01:03| B*14:02:01:04| B*14:02:01:05| B*14:02:01:06| B*14:02:02| B*14:02:03| B*14:02:04| B*14:02:05| B*14:02:06| B*14:02:07| B*14:02:08| B*14:02:09| B*14:02:10| B*14:02:11| B*14:02:12| B*14:02:13| B*14:02:14| B*14:02:15| B*14:02:16| B*14:02:17| B*14:02:18| B*14:02:19| B*14:02:20| B*14:02:21</t>
+  </si>
+  <si>
+    <t>B*15:33| B*15:42| B*15:43| B*15:52| B*15:53| B*15:55| B*15:62| B*15:76| B*15:78:01| B*15:78:02| B*15:78:03| B*15:78:04| B*15:86| B*15:87| B*15:91| B*15:101| B*15:104| B*15:105| B*15:106| B*15:109| B*15:110| B*15:112| B*15:113| B*15:115| B*15:116| B*15:117| B*15:118| B*15:119| B*15:120| B*15:121| B*15:122| B*15:123| B*15:124| B*15:125| B*15:126| B*15:127| B*15:128| B*15:129| B*15:131| B*15:132| B*15:133| B*15:134| B*15:135| B*15:136| B*15:137| B*15:138| B*15:139| B*15:140| B*15:141| B*15:142| B*15:143| B*15:144| B*15:145| B*15:147| B*15:148| B*15:150| B*15:151| B*15:152| B*15:153| B*15:154| B*15:155| B*15:156| B*15:157| B*15:158| B*15:159| B*15:160:01:01| B*15:160:01:02| B*15:161| B*15:162| B*15:163| B*15:164| B*15:165| B*15:166| B*15:167| B*15:168| B*15:169| B*15:170| B*15:171| B*15:172| B*15:173| B*15:174| B*15:175| B*15:176| B*15:177| B*15:178| B*15:179:01| B*15:179:02| B*15:180| B*15:183| B*15:184| B*15:185| B*15:186| B*15:187| B*15:188| B*15:189| B*15:191| B*15:192| B*15:193| B*15:194| B*15:195| B*15:196| B*15:197:01| B*15:197:02| B*15:198| B*15:199| B*15:200| B*15:201| B*15:202| B*15:203| B*15:204| B*15:205| B*15:206| B*15:207| B*15:208| B*15:210| B*15:211| B*15:212| B*15:213| B*15:214| B*15:215| B*15:216| B*15:217| B*15:218Q| B*15:219| B*15:221| B*15:222| B*15:223| B*15:224| B*15:225| B*15:227| B*15:228| B*15:229| B*15:230| B*15:231| B*15:232| B*15:233| B*15:234| B*15:235| B*15:236| B*15:237| B*15:238| B*15:239| B*15:240| B*15:241| B*15:242:01| B*15:242:02| B*15:243| B*15:244| B*15:245Q| B*15:247| B*15:248| B*15:249| B*15:250| B*15:251:01| B*15:251:02| B*15:251:03| B*15:252| B*15:253| B*15:254| B*15:255| B*15:256| B*15:257| B*15:259| B*15:260| B*15:261| B*15:263| B*15:264| B*15:265| B*15:266| B*15:267| B*15:268| B*15:269| B*15:270| B*15:271| B*15:273| B*15:274| B*15:275:01| B*15:275:02| B*15:276| B*15:277| B*15:278| B*15:279| B*15:280| B*15:281| B*15:282| B*15:283| B*15:284| B*15:285| B*15:286| B*15:287| B*15:288| B*15:289| B*15:290| B*15:291| B*15:292| B*15:293| B*15:295| B*15:296| B*15:297| B*15:298| B*15:299| B*15:300| B*15:301| B*15:303| B*15:305| B*15:306| B*15:307| B*15:308| B*15:309| B*15:310| B*15:311| B*15:312| B*15:313| B*15:314| B*15:315| B*15:316| B*15:317| B*15:318| B*15:319| B*15:320| B*15:321Q| B*15:322| B*15:323| B*15:324| B*15:325| B*15:326| B*15:327| B*15:328| B*15:329| B*15:330| B*15:331| B*15:332| B*15:333| B*15:334| B*15:335| B*15:336| B*15:337| B*15:338| B*15:339| B*15:340| B*15:341| B*15:342| B*15:343| B*15:344| B*15:345| B*15:346| B*15:347| B*15:348| B*15:349:01| B*15:349:02| B*15:350| B*15:351| B*15:352| B*15:353| B*15:354| B*15:355| B*15:356| B*15:357| B*15:358| B*15:359| B*15:360| B*15:361| B*15:362| B*15:363:01| B*15:363:02| B*15:364| B*15:365| B*15:366| B*15:367| B*15:368| B*15:369| B*15:370| B*15:371| B*15:372| B*15:373| B*15:374| B*15:376| B*15:377Q| B*15:378| B*15:379| B*15:381| B*15:382| B*15:383| B*15:384| B*15:385| B*15:386| B*15:387| B*15:388| B*15:389| B*15:390| B*15:391| B*15:392| B*15:393| B*15:394| B*15:395| B*15:396| B*15:397| B*15:398| B*15:399| B*15:401| B*15:402| B*15:403| B*15:404| B*15:405| B*15:406| B*15:407| B*15:408| B*15:409| B*15:410| B*15:411| B*15:412| B*15:413| B*15:414| B*15:415| B*15:416| B*15:417| B*15:418| B*15:419| B*15:420| B*15:421| B*15:422| B*15:423| B*15:424| B*15:425| B*15:426| B*15:427| B*15:428| B*15:429| B*15:430| B*15:431| B*15:432| B*15:433| B*15:434| B*15:435| B*15:436| B*15:437| B*15:438| B*15:439| B*15:440| B*15:441| B*15:442| B*15:443| B*15:444| B*15:445| B*15:446| B*15:447| B*15:448| B*15:449| B*15:450| B*15:451| B*15:452| B*15:453| B*15:455| B*15:456| B*15:457| B*15:458| B*15:459| B*15:460| B*15:461| B*15:462| B*15:464| B*15:465| B*15:466| B*15:467| B*15:468| B*15:469| B*15:470| B*15:471| B*15:472| B*15:473| B*15:474| B*15:475| B*15:476| B*15:477| B*15:478| B*15:479| B*15:480| B*15:481| B*15:482| B*15:484| B*15:485| B*15:486| B*15:488| B*15:489| B*15:490| B*15:491| B*15:492| B*15:493| B*15:494| B*15:495| B*15:497| B*15:498| B*15:01:01:01| B*15:01:01:03| B*15:01:01:04| B*15:01:01:05| B*15:01:01:06| B*15:01:01:07| B*15:01:01:08| B*15:01:01:09| B*15:01:01:10| B*15:01:01:11| B*15:01:01:12| B*15:01:01:13| B*15:01:01:14| B*15:01:01:15| B*15:01:01:16| B*15:01:01:17| B*15:01:01:18| B*15:01:01:19| B*15:01:01:20| B*15:01:02| B*15:01:03| B*15:01:04| B*15:01:06| B*15:01:07| B*15:01:08| B*15:01:09| B*15:01:10| B*15:01:11| B*15:01:12| B*15:01:13| B*15:01:14| B*15:01:15| B*15:01:16| B*15:01:17| B*15:01:18| B*15:01:19| B*15:01:20| B*15:01:21| B*15:01:22| B*15:01:23| B*15:01:24| B*15:01:25| B*15:01:26| B*15:01:27| B*15:01:28| B*15:01:29| B*15:01:30| B*15:01:31| B*15:01:32| B*15:01:33| B*15:01:34| B*15:01:35| B*15:01:36| B*15:01:37| B*15:01:38| B*15:01:39| B*15:01:40| B*15:01:41| B*15:01:42| B*15:01:43| B*15:01:44| B*15:01:45| B*15:01:46| B*15:01:47| B*15:01:48| B*15:01:49| B*15:01:50| B*15:01:51| B*15:01:52| B*15:01:53| B*15:01:54| B*15:01:55| B*15:04:01:01| B*15:04:01:02| B*15:04:02| B*15:04:03| B*15:04:04| B*15:05:01| B*15:05:02| B*15:05:03| B*15:06| B*15:07:01:01| B*15:07:01:02| B*15:07:02| B*15:07:03| B*15:15| B*15:20| B*15:24:01| B*15:24:02| B*15:25:01| B*15:25:02| B*15:25:03| B*15:25:04| B*15:27:01| B*15:27:02| B*15:27:03| B*15:27:04| B*15:28| B*15:30:01:01| B*15:30:01:02| B*15:32:01| B*15:32:02| B*15:34| B*15:35| B*15:38:01| B*15:38:02| B*15:39:01| B*15:39:02| B*15:40:01| B*15:40:02| B*15:45| B*15:48| B*15:50| B*15:56| B*15:57| B*15:58| B*15:60| B*15:63| B*15:65| B*15:66| B*15:70| B*15:71| B*15:73| B*15:75| B*15:77| B*15:81| B*15:82| B*15:83| B*15:84| B*15:85| B*15:92| B*15:96| B*15:97| B*15:102| B*15:107| B*15:146| B*15:16:01:01| B*15:16:01:02| B*15:16:01:03| B*15:16:02| B*15:16:03| B*15:17:01:01| B*15:17:01:02| B*15:17:02| B*15:17:03| B*15:17:04| B*15:17:05| B*15:17:06| B*15:17:07| B*15:67| B*15:95| B*15:02:01:01| B*15:02:01:02| B*15:02:01:03| B*15:02:02| B*15:02:03| B*15:02:04| B*15:02:05| B*15:02:06| B*15:02:07| B*15:02:08| B*15:02:09| B*15:02:10| B*15:02:11| B*15:02:12| B*15:08:01| B*15:08:02| B*15:11:01| B*15:11:02| B*15:11:03| B*15:11:04| B*15:11:05| B*15:11:06| B*15:11:07| B*15:21:01:01| B*15:21:01:02| B*15:31| B*15:44| B*15:88| B*15:12:01| B*15:12:02| B*15:12:03| B*15:14| B*15:19| B*15:13:01| B*15:13:02| B*15:89</t>
+  </si>
+  <si>
+    <t>B*38:03| B*38:09| B*39:07| B*39:32| B*38:01:01:01| B*38:01:01:02| B*38:01:02| B*38:01:03| B*38:01:04| B*38:01:05| B*38:01:06| B*38:01:07| B*38:01:08| B*38:01:09| B*38:01:10| B*38:01:11| B*38:01:12| B*38:01:13| B*38:01:14| B*38:01:15| B*38:02:01| B*38:02:02| B*38:02:03| B*38:02:04| B*38:02:05| B*38:02:06| B*38:02:07| B*38:02:08| B*38:04| B*38:05| B*38:06| B*38:07| B*38:08| B*38:10| B*38:11| B*38:12| B*38:13| B*38:14| B*38:15| B*38:16| B*38:17| B*38:18| B*38:19| B*38:20:01| B*38:20:02| B*38:21| B*38:22| B*38:23| B*38:24| B*38:25| B*38:26| B*38:27| B*38:28| B*38:29| B*38:30| B*38:31| B*38:32| B*38:33| B*38:35| B*38:36| B*38:37| B*38:38| B*38:39| B*38:40| B*38:41| B*38:42| B*38:43| B*38:44| B*38:45| B*38:46| B*38:47| B*38:48| B*38:49| B*38:50| B*38:51| B*38:52| B*38:53| B*38:54| B*38:55Q| B*38:56| B*38:57| B*38:58| B*38:59| B*38:60| B*38:61| B*38:62| B*38:63| B*38:64| B*38:65| B*38:66| B*38:67| B*38:68Q| B*38:69| B*38:70| B*38:71| B*38:72| B*38:73| B*38:74| B*38:75| B*38:76| B*38:77| B*38:78| B*38:79| B*38:81| B*38:82| B*39:03:01:01| B*39:03:01:02| B*39:04| B*39:06:01| B*39:06:02:01| B*39:06:02:02| B*39:06:02:03| B*39:06:02:04| B*39:06:03| B*39:06:04| B*39:06:05| B*39:06:06| B*39:08| B*39:09:01:01| B*39:09:01:02| B*39:09:01:03| B*39:09:02| B*39:09:03| B*39:10:01| B*39:10:02| B*39:11| B*39:12:01:01| B*39:12:01:02| B*39:13:01| B*39:13:02| B*39:14:01:01| B*39:14:01:02| B*39:15| B*39:16| B*39:17| B*39:18| B*39:19:01| B*39:19:02| B*39:20| B*39:22| B*39:23| B*39:24:01| B*39:24:02| B*39:26| B*39:27| B*39:28| B*39:29| B*39:30| B*39:31:01:01| B*39:31:01:02| B*39:33| B*39:34| B*39:35| B*39:36| B*39:37| B*39:38Q| B*39:39:01| B*39:39:02| B*39:41| B*39:42| B*39:43| B*39:44| B*39:45| B*39:46| B*39:47| B*39:48| B*39:49| B*39:50| B*39:51| B*39:52| B*39:53| B*39:54| B*39:55| B*39:56| B*39:57| B*39:58| B*39:59| B*39:60| B*39:61| B*39:62| B*39:63| B*39:64| B*39:65| B*39:66| B*39:67| B*39:68| B*39:69| B*39:70| B*39:71| B*39:72| B*39:73| B*39:74| B*39:75| B*39:76| B*39:77| B*39:78| B*39:79| B*39:80| B*39:81| B*39:82| B*39:83| B*39:84| B*39:85| B*39:86| B*39:88| B*39:89| B*39:90| B*39:91| B*39:92| B*39:93| B*39:94| B*39:96| B*39:98| B*39:99| B*39:100| B*39:101| B*39:102| B*39:103| B*39:104| B*39:105| B*39:106| B*39:107| B*39:108| B*39:109| B*39:110| B*39:111| B*39:112| B*39:113| B*39:114| B*39:115| B*39:117| B*39:118| B*39:119| B*39:120| B*39:121| B*39:122| B*39:123| B*39:124| B*39:125| B*39:126| B*39:127| B*39:128| B*39:129| B*39:130| B*39:131| B*39:132| B*39:134| B*39:135| B*39:136| B*39:137| B*39:138| B*39:140| B*39:141| B*39:143</t>
+  </si>
+  <si>
+    <t>B*47:05| B*58:08:01| B*58:08:02| B*58:09| B*57:01:01:01| B*57:01:01:02| B*57:01:01:03| B*57:01:01:04| B*57:01:02| B*57:01:03| B*57:01:04| B*57:01:05| B*57:01:06| B*57:01:07| B*57:01:08| B*57:01:09| B*57:01:10| B*57:01:11| B*57:01:12| B*57:01:13| B*57:01:14| B*57:01:15| B*57:01:16| B*57:01:17| B*57:01:18| B*57:01:19| B*57:01:20| B*57:01:21| B*57:01:22| B*57:01:23| B*57:01:24| B*57:01:25| B*57:01:26| B*57:01:27| B*57:01:28| B*57:01:29| B*57:01:30| B*57:01:31| B*57:01:32| B*57:01:33| B*57:01:34| B*57:01:35| B*57:01:36| B*57:02:01| B*57:02:02| B*57:03:01:01| B*57:03:01:02| B*57:03:01:03| B*57:03:02| B*57:03:03| B*57:03:04| B*57:04:01| B*57:04:02| B*57:04:03| B*57:05| B*57:06| B*57:07| B*57:08| B*57:09| B*57:10| B*57:11| B*57:12| B*57:13| B*57:14:01| B*57:14:02| B*57:15| B*57:16| B*57:17| B*57:18| B*57:19| B*57:20| B*57:21| B*57:22| B*57:23| B*57:24| B*57:25| B*57:26| B*57:27| B*57:29| B*57:30| B*57:31| B*57:32| B*57:33| B*57:34| B*57:35| B*57:36| B*57:37| B*57:38| B*57:39| B*57:40| B*57:41| B*57:42| B*57:43| B*57:44| B*57:45| B*57:46| B*57:47| B*57:48| B*57:49| B*57:50| B*57:51| B*57:52| B*57:53| B*57:54| B*57:55| B*57:56| B*57:57| B*57:58| B*57:59| B*57:60| B*57:61| B*57:62| B*57:63| B*57:64| B*57:65| B*57:66| B*57:67:01| B*57:67:02| B*57:68| B*57:69| B*57:70| B*57:71| B*57:72| B*57:73| B*57:74| B*57:75| B*57:76| B*57:77| B*57:78| B*57:80| B*57:81| B*57:82| B*57:83| B*57:84| B*57:85| B*57:86| B*57:87| B*57:88| B*57:89| B*57:90| B*57:91| B*57:92| B*57:93| B*57:94| B*57:95| B*57:96| B*57:97| B*57:98Q| B*57:99| B*57:100| B*57:101| B*57:102| B*57:103| B*57:104| B*57:105| B*57:106| B*57:107| B*57:108| B*57:109| B*57:110| B*57:111| B*57:112| B*57:113| B*57:114| B*58:01:01:01| B*58:01:01:02| B*58:01:01:03| B*58:01:01:04| B*58:01:01:05| B*58:01:02| B*58:01:03| B*58:01:04| B*58:01:05| B*58:01:06| B*58:01:07| B*58:01:08| B*58:01:09| B*58:01:10| B*58:01:11| B*58:01:12| B*58:01:13| B*58:01:14| B*58:01:15| B*58:01:16| B*58:01:17| B*58:01:18| B*58:01:19| B*58:01:20| B*58:01:21| B*58:01:22| B*58:01:23| B*58:01:24| B*58:01:25| B*58:01:26| B*58:01:27| B*58:01:28| B*58:01:29| B*58:01:30| B*58:01:31| B*58:02:01| B*58:02:02| B*58:04| B*58:05| B*58:06| B*58:07| B*58:11| B*58:12| B*58:13| B*58:14| B*58:15| B*58:16:01| B*58:16:02| B*58:18| B*58:19| B*58:20| B*58:21| B*58:22| B*58:23| B*58:24| B*58:25| B*58:26| B*58:27| B*58:28:01| B*58:28:02| B*58:29| B*58:32| B*58:33| B*58:34| B*58:35| B*58:36| B*58:37| B*58:38| B*58:40| B*58:41| B*58:42| B*58:43| B*58:44| B*58:45:01| B*58:45:02| B*58:46| B*58:47| B*58:48| B*58:49| B*58:50| B*58:51| B*58:52| B*58:53| B*58:54| B*58:55| B*58:56| B*58:57| B*58:58| B*58:59:01| B*58:59:02| B*58:60| B*58:61| B*58:62| B*58:63| B*58:64| B*58:65| B*58:66| B*58:67| B*58:68| B*58:69| B*58:70| B*58:71| B*58:73| B*58:74| B*58:75| B*58:76| B*58:77| B*58:78| B*58:79| B*58:80| B*58:81| B*58:82| B*58:83| B*58:84| B*58:85| B*58:86| B*58:87| B*58:88| B*58:89| B*58:90| B*58:91| B*58:92| B*58:95| B*58:96| B*58:97| B*58:98| B*58:99| B*58:100</t>
+  </si>
+  <si>
+    <t>B*18:01:01:01| B*18:01:01:02| B*18:01:01:03| B*18:01:01:04| B*18:01:01:05| B*18:01:01:06| B*18:01:01:07| B*18:01:01:08| B*18:01:01:09| B*18:01:01:10| B*18:01:01:11| B*18:01:01:12| B*18:01:01:13| B*18:01:01:14| B*18:01:01:15| B*18:01:01:16| B*18:01:01:17| B*18:01:01:18| B*18:01:01:19| B*18:01:02| B*18:01:03| B*18:01:04| B*18:01:05| B*18:01:06| B*18:01:07| B*18:01:08| B*18:01:09| B*18:01:10| B*18:01:11| B*18:01:12| B*18:01:13| B*18:01:14| B*18:01:15| B*18:01:16| B*18:01:17| B*18:01:18| B*18:01:19| B*18:01:20| B*18:01:21| B*18:01:22| B*18:01:23| B*18:01:24| B*18:01:25| B*18:01:26| B*18:01:27| B*18:01:28| B*18:01:29| B*18:01:30| B*18:01:31| B*18:01:32| B*18:02| B*18:03:01| B*18:03:02| B*18:04:01| B*18:04:02| B*18:05:01:01| B*18:05:01:02| B*18:06| B*18:07:01| B*18:07:02| B*18:08| B*18:09| B*18:10| B*18:11| B*18:12:01| B*18:12:02| B*18:13| B*18:14| B*18:15| B*18:18:01:01| B*18:18:01:02| B*18:19| B*18:20| B*18:21| B*18:22| B*18:24| B*18:25| B*18:26| B*18:27| B*18:28| B*18:29| B*18:30| B*18:31| B*18:32| B*18:33| B*18:34| B*18:35| B*18:36| B*18:37:01| B*18:37:02| B*18:38| B*18:39| B*18:40| B*18:41| B*18:42| B*18:43| B*18:44:01| B*18:44:02| B*18:45| B*18:46| B*18:47| B*18:48| B*18:49| B*18:50| B*18:51| B*18:52| B*18:53| B*18:54| B*18:55| B*18:56| B*18:57:01| B*18:57:02| B*18:58| B*18:59| B*18:60| B*18:61| B*18:62| B*18:63| B*18:64| B*18:65| B*18:66| B*18:67| B*18:68| B*18:69| B*18:70| B*18:71| B*18:72:01| B*18:72:02| B*18:72:03| B*18:73| B*18:75| B*18:76| B*18:77| B*18:78| B*18:79| B*18:80| B*18:81| B*18:82| B*18:83| B*18:84| B*18:85| B*18:86| B*18:87| B*18:88| B*18:89| B*18:90| B*18:91| B*18:92| B*18:93| B*18:95| B*18:96| B*18:97| B*18:98| B*18:99| B*18:100| B*18:101| B*18:102| B*18:103| B*18:104| B*18:105| B*18:106| B*18:107| B*18:108| B*18:109| B*18:110| B*18:111| B*18:112| B*18:113| B*18:114| B*18:115| B*18:116| B*18:117| B*18:118| B*18:119| B*18:120| B*18:121| B*18:122| B*18:123| B*18:124| B*18:125| B*18:126| B*18:127| B*18:128| B*18:129| B*18:130| B*18:131:01:01| B*18:131:01:02| B*18:132| B*18:133| B*18:134| B*18:135| B*18:136| B*18:137| B*18:139| B*18:140| B*18:141| B*18:142| B*18:143| B*18:144| B*18:145| B*18:146| B*18:147| B*18:148| B*18:149| B*18:150| B*18:151| B*18:152| B*18:153| B*18:155| B*18:156:01:01| B*18:156:01:02| B*18:157:01:01| B*18:157:01:02| B*18:158| B*18:159| B*18:160| B*18:161</t>
+  </si>
+  <si>
+    <t>B*40:26| B*44:42| B*45:04| B*49:01:01:01| B*49:01:01:02| B*49:01:01:03| B*49:01:01:04| B*49:01:02| B*49:01:03| B*49:01:04| B*49:01:05| B*49:01:06| B*49:01:07| B*49:01:08| B*49:01:09| B*49:01:10| B*49:01:11| B*49:01:12| B*49:01:13| B*49:02| B*49:03| B*49:04:01| B*49:04:02| B*49:05| B*49:06| B*49:08| B*49:09| B*49:10| B*49:11| B*49:12| B*49:13| B*49:14| B*49:16| B*49:17| B*49:18:01| B*49:18:02| B*49:20| B*49:21| B*49:22| B*49:23| B*49:24| B*49:25| B*49:26| B*49:27| B*49:28| B*49:29| B*49:30| B*49:31| B*49:32| B*49:33| B*49:34| B*49:35| B*49:36| B*49:37| B*49:38| B*49:39| B*49:40| B*49:41| B*49:42| B*49:43| B*49:44| B*49:45| B*49:46| B*49:47| B*49:48| B*49:49| B*49:50| B*49:51| B*49:52| B*49:53| B*49:54| B*49:55| B*49:56| B*49:57| B*49:58| B*49:59| B*15:46| B*50:01:01:01| B*50:01:01:02| B*50:01:02| B*50:01:03| B*50:01:04| B*50:01:05| B*50:01:06| B*50:01:07| B*50:01:08| B*50:01:09| B*50:01:10| B*50:04| B*50:05| B*50:06| B*50:07| B*50:08| B*50:09| B*50:10| B*50:11| B*50:12| B*50:13| B*50:14| B*50:15| B*50:16| B*50:17| B*50:18| B*50:19| B*50:20| B*50:31| B*50:32| B*50:33| B*50:34| B*50:35| B*50:36| B*50:37| B*50:38| B*50:39| B*50:40| B*50:41| B*50:42| B*50:43| B*50:44| B*50:45| B*50:46| B*50:47| B*50:48| B*50:49| B*50:50| B*50:51| B*50:52| B*50:53| B*50:54| B*50:55| B*50:56| B*50:57| B*50:58| B*50:59| B*50:60| B*50:61| B*40:05:01:01| B*40:05:01:02</t>
+  </si>
+  <si>
+    <t>B*46:11| B*54:03| B*55:05| B*55:09| B*55:12| B*55:16| B*55:20| B*56:03| B*54:01:01| B*54:01:02| B*54:01:03| B*54:01:04| B*54:01:05| B*54:01:06| B*54:01:07| B*54:02| B*54:04| B*54:06| B*54:07| B*54:09| B*54:10| B*54:11| B*54:12| B*54:13| B*54:14| B*54:15| B*54:16| B*54:17| B*54:18| B*54:19| B*54:20| B*54:21| B*54:22| B*54:23| B*54:24| B*54:25| B*54:26| B*54:27| B*54:28| B*54:29| B*54:30| B*54:31| B*54:32| B*54:33| B*54:34| B*54:35| B*54:36| B*54:37| B*54:38| B*55:07| B*55:01:01:01| B*55:01:01:02| B*55:01:02| B*55:01:03| B*55:01:04| B*55:01:05| B*55:01:06| B*55:01:07| B*55:01:08| B*55:01:09| B*55:01:10| B*55:01:11| B*55:01:12| B*55:01:13| B*55:01:14| B*55:01:15| B*55:01:16| B*55:02:01:01| B*55:02:01:02| B*55:02:01:03| B*55:02:02| B*55:02:03| B*55:02:04| B*55:02:05| B*55:02:06| B*55:02:07| B*55:02:08| B*55:02:09| B*55:02:10| B*55:03| B*55:04| B*55:10| B*55:11| B*55:13| B*55:14| B*55:15| B*55:17| B*55:18| B*55:19| B*55:21| B*55:22| B*55:23| B*55:24| B*55:25| B*55:26| B*55:27| B*55:28| B*55:29| B*55:30| B*55:31| B*55:32| B*55:33| B*55:34| B*55:35| B*55:36| B*55:37| B*55:38| B*55:39| B*55:40| B*55:41| B*55:42| B*55:43| B*55:44| B*55:45| B*55:46| B*55:47| B*55:48| B*55:49| B*55:50| B*55:51| B*55:52| B*55:53| B*55:54| B*55:56| B*55:57| B*55:58| B*55:59| B*55:60| B*55:61| B*55:62| B*55:63| B*55:64| B*55:65| B*55:66| B*55:67| B*55:68| B*55:69| B*55:70| B*55:71| B*55:72| B*55:73| B*55:74| B*55:75| B*55:76| B*55:77| B*55:78| B*55:79| B*55:80| B*55:81| B*55:82| B*55:84| B*55:85| B*55:86| B*55:87| B*55:88| B*55:90| B*55:91| B*55:92| B*55:93| B*55:94| B*55:95| B*55:96| B*56:10| B*56:12| B*55:08| B*56:01:01:01| B*56:01:01:02| B*56:01:01:03| B*56:01:01:04| B*56:01:01:06| B*56:01:01:07| B*56:01:02| B*56:01:03| B*56:01:04| B*56:01:05| B*56:01:06| B*56:01:07| B*56:01:08| B*56:01:09| B*56:01:10| B*56:01:11| B*56:01:12| B*56:01:13| B*56:01:14| B*56:01:15| B*56:02:01| B*56:02:02| B*56:04:01| B*56:04:02| B*56:07| B*56:08| B*56:09| B*56:11| B*56:13| B*56:14| B*56:15| B*56:16| B*56:17| B*56:18| B*56:20:01| B*56:20:02| B*56:21| B*56:22| B*56:23| B*56:24| B*56:25| B*56:26| B*56:27| B*56:29| B*56:30| B*56:31| B*56:32| B*56:33| B*56:34| B*56:35| B*56:36| B*56:37| B*56:39| B*56:40| B*56:41| B*56:42| B*56:43| B*56:44| B*56:45| B*56:46| B*56:47| B*56:48| B*56:49| B*56:50| B*56:51| B*56:52| B*56:53| B*56:54| B*56:55:01:02| B*56:56| B*56:57| B*56:58| B*56:59| B*56:60| B*56:61| B*56:62| B*56:63| B*56:64</t>
+  </si>
+  <si>
+    <t>B*27:01| B*27:02:01:01| B*27:02:01:02| B*27:02:01:03| B*27:02:01:04| B*27:02:01:05| B*27:02:02| B*27:02:03| B*27:02:04| B*27:02:05| B*27:03| B*27:04:01| B*27:04:02| B*27:04:03| B*27:04:04| B*27:04:05| B*27:04:06| B*27:05:02:01| B*27:05:02:02| B*27:05:02:03| B*27:05:02:04Q| B*27:05:02:05| B*27:05:02:06| B*27:05:02:07| B*27:05:02:08| B*27:05:02:09| B*27:05:02:10| B*27:05:03| B*27:05:04| B*27:05:05| B*27:05:06| B*27:05:07| B*27:05:08| B*27:05:09| B*27:05:10| B*27:05:11| B*27:05:12| B*27:05:13| B*27:05:14| B*27:05:15| B*27:05:16| B*27:05:17| B*27:05:18| B*27:05:19| B*27:05:20| B*27:05:21| B*27:05:22| B*27:05:23| B*27:05:24| B*27:05:25| B*27:05:26| B*27:05:27| B*27:05:28| B*27:05:29| B*27:05:30| B*27:05:31| B*27:05:32| B*27:05:33| B*27:05:34| B*27:05:35| B*27:05:36| B*27:05:37| B*27:06| B*27:07:01| B*27:07:02| B*27:07:03| B*27:07:04| B*27:07:05| B*27:07:06| B*27:09| B*27:10| B*27:11| B*27:12:01:01| B*27:12:01:02| B*27:13| B*27:14| B*27:15| B*27:16| B*27:17| B*27:18| B*27:19| B*27:20| B*27:21| B*27:23| B*27:24| B*27:25| B*27:26| B*27:27| B*27:28| B*27:29| B*27:30| B*27:31| B*27:32| B*27:33| B*27:34| B*27:35| B*27:36| B*27:37| B*27:38| B*27:39| B*27:40| B*27:41| B*27:42| B*27:43| B*27:44| B*27:45| B*27:46| B*27:47| B*27:48| B*27:49| B*27:50:01| B*27:50:02| B*27:51| B*27:52| B*27:53| B*27:54| B*27:55| B*27:56| B*27:57| B*27:58| B*27:60| B*27:61| B*27:62| B*27:63| B*27:67| B*27:68| B*27:69| B*27:70| B*27:71| B*27:72| B*27:73| B*27:74| B*27:75| B*27:76| B*27:77| B*27:78| B*27:79| B*27:80| B*27:81| B*27:82| B*27:83| B*27:84| B*27:85| B*27:86| B*27:87| B*27:88| B*27:89| B*27:90:01| B*27:90:02| B*27:90:03| B*27:90:04| B*27:91| B*27:92| B*27:93| B*27:95| B*27:96:01| B*27:96:02| B*27:97| B*27:98| B*27:99| B*27:100| B*27:101| B*27:102| B*27:103| B*27:104| B*27:105| B*27:106| B*27:107| B*27:108| B*27:109| B*27:110| B*27:111| B*27:112| B*27:113| B*27:114| B*27:115| B*27:116| B*27:117| B*27:118| B*27:119| B*27:120| B*27:121| B*27:122| B*27:123| B*27:124| B*27:125| B*27:126| B*27:127| B*27:128| B*27:129| B*27:130| B*27:131| B*27:132| B*27:133| B*27:134| B*27:135| B*27:136| B*27:137| B*27:138| B*27:139| B*27:140| B*27:141| B*27:142| B*27:143| B*27:144| B*27:145| B*27:146| B*27:147| B*27:148| B*27:149| B*27:150| B*27:151| B*27:152| B*27:153| B*27:154| B*27:155| B*27:156| B*27:157| B*27:158| B*27:159| B*27:160| B*27:161| B*27:162| B*27:163| B*27:164| B*27:165| B*27:166| B*27:167| B*27:168| B*27:169| B*27:170| B*27:171| B*27:172| B*27:173| B*27:174| B*27:175| B*27:177| B*27:178| B*27:179| B*27:180| B*27:181| B*27:182| B*27:183| B*27:184| B*27:185| B*27:186| B*27:187| B*27:188</t>
   </si>
   <si>
     <t>B*27:08</t>
   </si>
   <si>
-    <t>B*37:01| B*37:02| B*37:04| B*37:05| B*37:06| B*37:07| B*37:08| B*37:09| B*37:10| B*37:11| B*37:12| B*37:13| B*37:14| B*37:15| B*37:16Q| B*37:17| B*37:18| B*37:19| B*37:20| B*37:21| B*37:22| B*37:23| B*37:24| B*37:25| B*37:26| B*37:27| B*37:28| B*37:29| B*37:31| B*37:32| B*37:34| B*37:35| B*37:36| B*37:37| B*37:38| B*37:39| B*37:40| B*37:41| B*37:43| B*37:44| B*37:45| B*37:46| B*37:47| B*37:48| B*37:49| B*37:50| B*37:51| B*37:52| B*37:53| B*37:54| B*37:55| B*37:56| B*37:57| B*37:58| B*37:59| B*37:60| B*37:61| B*37:62| B*37:63| B*37:64| B*37:65| B*37:66| B*37:67| B*37:68| B*37:69| B*37:70</t>
-  </si>
-  <si>
-    <t>B*38:01| B*38:02| B*38:04| B*38:05| B*38:06| B*38:07| B*38:08| B*38:10| B*38:11| B*38:12| B*38:13| B*38:14| B*38:15| B*38:16| B*38:17| B*38:18| B*38:19| B*38:20| B*38:21| B*38:22| B*38:23| B*38:24| B*38:25| B*38:26| B*38:27| B*38:28| B*38:29| B*38:30| B*38:31| B*38:32| B*38:33| B*38:35| B*38:36| B*38:37| B*38:38| B*38:39| B*38:40| B*38:41| B*38:42| B*38:43| B*38:44| B*38:45| B*38:46| B*38:47| B*38:48| B*38:49| B*38:50| B*38:51| B*38:52| B*38:53| B*38:54| B*38:55Q| B*38:56| B*38:57| B*38:58| B*38:59| B*38:60| B*38:61| B*38:62| B*38:63| B*38:64| B*38:65| B*38:66| B*38:67| B*38:68Q</t>
-  </si>
-  <si>
-    <t>B*38:03| B*38:09| B*39:07| B*39:32| B*38:01| B*38:02| B*38:04| B*38:05| B*38:06| B*38:07| B*38:08| B*38:10| B*38:11| B*38:12| B*38:13| B*38:14| B*38:15| B*38:16| B*38:17| B*38:18| B*38:19| B*38:20| B*38:21| B*38:22| B*38:23| B*38:24| B*38:25| B*38:26| B*38:27| B*38:28| B*38:29| B*38:30| B*38:31| B*38:32| B*38:33| B*38:35| B*38:36| B*38:37| B*38:38| B*38:39| B*38:40| B*38:41| B*38:42| B*38:43| B*38:44| B*38:45| B*38:46| B*38:47| B*38:48| B*38:49| B*38:50| B*38:51| B*38:52| B*38:53| B*38:54| B*38:55Q| B*38:56| B*38:57| B*38:58| B*38:59| B*38:60| B*38:61| B*38:62| B*38:63| B*38:64| B*38:65| B*38:66| B*38:67| B*38:68Q| B*39:03| B*39:04| B*39:05| B*39:06| B*39:08| B*39:09| B*39:10| B*39:11| B*39:12| B*39:13| B*39:14| B*39:15| B*39:16| B*39:17| B*39:18| B*39:19| B*39:20| B*39:22| B*39:23| B*39:24| B*39:26| B*39:27| B*39:28| B*39:29| B*39:30| B*39:31| B*39:33| B*39:34| B*39:35| B*39:36| B*39:37| B*39:38Q| B*39:39| B*39:41| B*39:42| B*39:43| B*39:44| B*39:45| B*39:46| B*39:47| B*39:48| B*39:49| B*39:50| B*39:51| B*39:52| B*39:53| B*39:54| B*39:55| B*39:56| B*39:57| B*39:58| B*39:59| B*39:60| B*39:61| B*39:62| B*39:63| B*39:64| B*39:65| B*39:66| B*39:67| B*39:68| B*39:69| B*39:70| B*39:71| B*39:72| B*39:73| B*39:74| B*39:75| B*39:76| B*39:77| B*39:78| B*39:79| B*39:80| B*39:81| B*39:82| B*39:83| B*39:84| B*39:85| B*39:86| B*39:88| B*39:89| B*39:90| B*39:91| B*39:92| B*39:93| B*39:94| B*39:96| B*39:98| B*39:99| B*39:100| B*39:101| B*39:102| B*39:103| B*39:104| B*39:105| B*39:106| B*39:107| B*39:108| B*39:109| B*39:110| B*39:111| B*39:112| B*39:113| B*39:114| B*39:115| B*39:117| B*39:118| B*39:119| B*39:120| B*39:121| B*39:122| B*39:123| B*39:124| B*39:125| B*39:126| B*39:127| B*39:128| B*39:129| B*39:130| B*39:131</t>
-  </si>
-  <si>
-    <t>B*39:01| B*39:01L</t>
-  </si>
-  <si>
-    <t>B*39:02</t>
-  </si>
-  <si>
-    <t>B*39:03| B*39:04| B*39:05| B*39:06| B*39:08| B*39:09| B*39:10| B*39:11| B*39:12| B*39:13| B*39:14| B*39:15| B*39:16| B*39:17| B*39:18| B*39:19| B*39:20| B*39:22| B*39:23| B*39:24| B*39:26| B*39:27| B*39:28| B*39:29| B*39:30| B*39:31| B*39:33| B*39:34| B*39:35| B*39:36| B*39:37| B*39:38Q| B*39:39| B*39:41| B*39:42| B*39:43| B*39:44| B*39:45| B*39:46| B*39:47| B*39:48| B*39:49| B*39:50| B*39:51| B*39:52| B*39:53| B*39:54| B*39:55| B*39:56| B*39:57| B*39:58| B*39:59| B*39:60| B*39:61| B*39:62| B*39:63| B*39:64| B*39:65| B*39:66| B*39:67| B*39:68| B*39:69| B*39:70| B*39:71| B*39:72| B*39:73| B*39:74| B*39:75| B*39:76| B*39:77| B*39:78| B*39:79| B*39:80| B*39:81| B*39:82| B*39:83| B*39:84| B*39:85| B*39:86| B*39:88| B*39:89| B*39:90| B*39:91| B*39:92| B*39:93| B*39:94| B*39:96| B*39:98| B*39:99| B*39:100| B*39:101| B*39:102| B*39:103| B*39:104| B*39:105| B*39:106| B*39:107| B*39:108| B*39:109| B*39:110| B*39:111| B*39:112| B*39:113| B*39:114| B*39:115| B*39:117| B*39:118| B*39:119| B*39:120| B*39:121| B*39:122| B*39:123| B*39:124| B*39:125| B*39:126| B*39:127| B*39:128| B*39:129| B*39:130| B*39:131| B*39:01| B*39:01L| B*39:02| B*39:05</t>
-  </si>
-  <si>
-    <t>B*39:05</t>
-  </si>
-  <si>
-    <t>B*40:01| B*40:07| B*40:10| B*40:14| B*40:30| B*40:31| B*40:33| B*40:34| B*40:36| B*40:38| B*40:42| B*40:43| B*40:45| B*40:46| B*40:48| B*40:49| B*40:52| B*40:54| B*40:55| B*40:61| B*40:62| B*40:63| B*40:65| B*40:66| B*40:67| B*40:69| B*40:72| B*40:73| B*40:74| B*40:76| B*40:77| B*47:02</t>
-  </si>
-  <si>
-    <t>B*40:02| B*40:03| B*40:04| B*40:06| B*40:08| B*40:09| B*40:11| B*40:16| B*40:18| B*40:20| B*40:24| B*40:27| B*40:29| B*40:35| B*40:37| B*40:40| B*40:44| B*40:50| B*40:53| B*40:56| B*40:57| B*40:70| B*40:71| B*40:75</t>
-  </si>
-  <si>
-    <t>B*40:05| B*15:46| B*50:01| B*50:04| B*50:05| B*50:06| B*50:07| B*50:08| B*50:09| B*50:10| B*50:11| B*50:12| B*50:13| B*50:14| B*50:15| B*50:16| B*50:17| B*50:18| B*50:19| B*50:20| B*50:31| B*50:32| B*50:33| B*50:34| B*50:35| B*50:36| B*50:37| B*50:38| B*50:39| B*50:40| B*50:41| B*50:42| B*50:43| B*50:44| B*50:45| B*50:46| B*50:47| B*50:48| B*50:49| B*50:50| B*50:51| B*50:52| B*50:53| B*50:54</t>
-  </si>
-  <si>
-    <t>B*40:12| B*48:01| B*48:02| B*48:03| B*48:04| B*48:05| B*48:06| B*48:07| B*48:08| B*48:09| B*48:10| B*48:11| B*48:12| B*48:13| B*48:14| B*48:15| B*48:16| B*48:17| B*48:18| B*48:19| B*48:20| B*48:21| B*48:22| B*48:23| B*48:24| B*48:25| B*48:26| B*48:27| B*48:28| B*48:29| B*48:30| B*48:31| B*48:32| B*48:33| B*48:34| B*48:35| B*48:36| B*48:37| B*48:38| B*48:39| B*48:40| B*48:41| B*48:42| B*48:43</t>
-  </si>
-  <si>
-    <t>B*40:13| B*40:15| B*40:21| B*40:23| B*40:25| B*40:28| B*40:32| B*40:47| B*40:51| B*40:58| B*40:59| B*40:60| B*40:64| B*40:68| B*40:78| B*40:79| B*40:80| B*40:81| B*40:82| B*40:83| B*40:84| B*40:85| B*40:86| B*40:87| B*40:88| B*40:89| B*40:90| B*40:91| B*40:92| B*40:93| B*40:94| B*40:95| B*40:96| B*40:97| B*40:98| B*40:99| B*40:100| B*40:101| B*40:102| B*40:103| B*40:104| B*40:105| B*40:106| B*40:107| B*40:108| B*40:109| B*40:110| B*40:111| B*40:112| B*40:113| B*40:114| B*40:115| B*40:116| B*40:117| B*40:119| B*40:120| B*40:121| B*40:122| B*40:123| B*40:124| B*40:125| B*40:126| B*40:127| B*40:128| B*40:129| B*40:130| B*40:131| B*40:132| B*40:133Q| B*40:134| B*40:135| B*40:136| B*40:137| B*40:138| B*40:139| B*40:140| B*40:141| B*40:143| B*40:145| B*40:146| B*40:147| B*40:148| B*40:149| B*40:150| B*40:151| B*40:152| B*40:153| B*40:154| B*40:156| B*40:157| B*40:158| B*40:159| B*40:160| B*40:161| B*40:162| B*40:163| B*40:164| B*40:165| B*40:166| B*40:167| B*40:168| B*40:169| B*40:170| B*40:171| B*40:172| B*40:173| B*40:174| B*40:175| B*40:176| B*40:177| B*40:178| B*40:179| B*40:180| B*40:181| B*40:182| B*40:183| B*40:184| B*40:185| B*40:186| B*40:187| B*40:188| B*40:189| B*40:190| B*40:191| B*40:192| B*40:193| B*40:194| B*40:195| B*40:196| B*40:197| B*40:198| B*40:199| B*40:200| B*40:201| B*40:202| B*40:203| B*40:204| B*40:205| B*40:206| B*40:207| B*40:208| B*40:209| B*40:210| B*40:211| B*40:212| B*40:213| B*40:214| B*40:215| B*40:217| B*40:218| B*40:219| B*40:220| B*40:221| B*40:222| B*40:223| B*40:224| B*40:225| B*40:226| B*40:227| B*40:228| B*40:229| B*40:230| B*40:231| B*40:232| B*40:233| B*40:234| B*40:235| B*40:236| B*40:237| B*40:238| B*40:239| B*40:240| B*40:241| B*40:242| B*40:243| B*40:244| B*40:245| B*40:246| B*40:247| B*40:248| B*40:249| B*40:250| B*40:251| B*40:252| B*40:253| B*40:254| B*40:255| B*40:257| B*40:258| B*40:259| B*40:260| B*40:261| B*40:262| B*40:264| B*40:266| B*40:267| B*40:268| B*40:269| B*40:270| B*40:271| B*40:272| B*40:273| B*40:274| B*40:275| B*40:276| B*40:277| B*40:278| B*40:279| B*40:280| B*40:281| B*40:282| B*40:283| B*40:284| B*40:285| B*40:287| B*40:288| B*40:289| B*40:290| B*40:292| B*40:293| B*40:294| B*40:295| B*40:296| B*40:297| B*40:298| B*40:299| B*40:300| B*40:301| B*40:302| B*40:303| B*40:304| B*40:305| B*40:306| B*40:307| B*40:308| B*40:309| B*40:310| B*40:311| B*40:312| B*40:313| B*40:314| B*40:315| B*40:316| B*40:317| B*40:318| B*40:319| B*40:320| B*40:321| B*40:322| B*40:323| B*40:324| B*40:325| B*40:326| B*40:327| B*40:328| B*40:329| B*40:330| B*40:331| B*40:332| B*40:333| B*40:334| B*40:335| B*40:336| B*40:339| B*40:340| B*40:341| B*40:342| B*40:343| B*40:344| B*40:346| B*40:347| B*40:348| B*40:349| B*40:350| B*40:351| B*40:352| B*40:353| B*40:354| B*40:355| B*40:356| B*40:357| B*40:358| B*40:359| B*40:360| B*40:362| B*40:363| B*40:364| B*40:365| B*40:01| B*40:07| B*40:10| B*40:14| B*40:30| B*40:31| B*40:33| B*40:34| B*40:36| B*40:38| B*40:42| B*40:43| B*40:45| B*40:46| B*40:48| B*40:49| B*40:52| B*40:54| B*40:55| B*40:61| B*40:62| B*40:63| B*40:65| B*40:66| B*40:67| B*40:69| B*40:72| B*40:73| B*40:74| B*40:76| B*40:77| B*47:02| B*40:02| B*40:03| B*40:04| B*40:06| B*40:08| B*40:09| B*40:11| B*40:16| B*40:18| B*40:20| B*40:24| B*40:27| B*40:29| B*40:35| B*40:37| B*40:40| B*40:44| B*40:50| B*40:53| B*40:56| B*40:57| B*40:70| B*40:71| B*40:75</t>
-  </si>
-  <si>
-    <t>B*40:19| B*44:16| B*47:01| B*47:03| B*47:04| B*47:06| B*47:07| B*47:08| B*47:09| B*47:10| B*49:07</t>
-  </si>
-  <si>
-    <t>B*40:26| B*44:42| B*45:04| B*49:01| B*49:02| B*49:03| B*49:04| B*49:05| B*49:06| B*49:08| B*49:09| B*49:10| B*49:11| B*49:12| B*49:13| B*49:14| B*49:16| B*49:17| B*49:18| B*49:20| B*49:21| B*49:22| B*49:23| B*49:24| B*49:25| B*49:26| B*49:27| B*49:28| B*49:29| B*49:30| B*49:31| B*49:32| B*49:33| B*49:34| B*49:35| B*49:36| B*49:37| B*49:38| B*49:39| B*49:40| B*49:41| B*49:42| B*49:43| B*49:44| B*49:45| B*49:46| B*49:47| B*49:48| B*15:46| B*50:01| B*50:04| B*50:05| B*50:06| B*50:07| B*50:08| B*50:09| B*50:10| B*50:11| B*50:12| B*50:13| B*50:14| B*50:15| B*50:16| B*50:17| B*50:18| B*50:19| B*50:20| B*50:31| B*50:32| B*50:33| B*50:34| B*50:35| B*50:36| B*50:37| B*50:38| B*50:39| B*50:40| B*50:41| B*50:42| B*50:43| B*50:44| B*50:45| B*50:46| B*50:47| B*50:48| B*50:49| B*50:50| B*50:51| B*50:52| B*50:53| B*50:54| B*40:05</t>
-  </si>
-  <si>
-    <t>B*40:39| B*41:01| B*41:02| B*41:03| B*41:04| B*41:05| B*41:06| B*41:07| B*41:08| B*41:09| B*41:10| B*41:11| B*41:12| B*41:13| B*41:14| B*41:15| B*41:16| B*41:17| B*41:18| B*41:19| B*41:20| B*41:21| B*41:22| B*41:23| B*41:24| B*41:25| B*41:26| B*41:27| B*41:28| B*41:29| B*41:30| B*41:31| B*41:32| B*41:33| B*41:34| B*41:35| B*41:36| B*41:37| B*41:38| B*41:39| B*41:40| B*41:41| B*41:42| B*41:43| B*41:44| B*41:46| B*41:47| B*41:48| B*41:49| B*41:50| B*41:51| B*41:52| B*41:53| B*41:54</t>
-  </si>
-  <si>
-    <t>B*42:01| B*42:02| B*42:04| B*42:05| B*42:06| B*42:07| B*42:08| B*42:09| B*42:10| B*42:11| B*42:12| B*42:13| B*42:14| B*42:15| B*42:16| B*42:17| B*42:18| B*42:19| B*42:20| B*42:21| B*42:22| B*42:23| B*42:24</t>
-  </si>
-  <si>
-    <t>B*44:02| B*44:03| B*44:04| B*44:05| B*44:06| B*44:07| B*44:08| B*44:10| B*44:11| B*44:12| B*44:13| B*44:14| B*44:17| B*44:18| B*44:20| B*44:21| B*44:22| B*44:24| B*44:25| B*44:26| B*44:27| B*44:28| B*44:29| B*44:30| B*44:31| B*44:32| B*44:33| B*44:34| B*44:35| B*44:36| B*44:37| B*44:38| B*44:39| B*44:40| B*44:41| B*44:43| B*44:44| B*44:45| B*44:47| B*44:48| B*44:49| B*44:50| B*44:51| B*44:53| B*44:54| B*44:55| B*44:57| B*44:59| B*44:60| B*44:62| B*44:63| B*44:64| B*44:65| B*44:66| B*44:67| B*44:68| B*44:69| B*44:70| B*44:71| B*44:72| B*44:73| B*44:74| B*44:75| B*44:76| B*44:77| B*44:78| B*44:79| B*44:80| B*44:81| B*44:82| B*44:83| B*44:84| B*44:85| B*44:86| B*44:87| B*44:88| B*44:89| B*44:90| B*44:91| B*44:92| B*44:93| B*44:94| B*44:95| B*44:96| B*44:97| B*44:98| B*44:99| B*44:100| B*44:101| B*44:102| B*44:103| B*44:104| B*44:105| B*44:106| B*44:107| B*44:109| B*44:110| B*44:111| B*44:112| B*44:113| B*44:114| B*44:115| B*44:116| B*44:117| B*44:118| B*44:119| B*44:120| B*44:121| B*44:122| B*44:123| B*44:124| B*44:125| B*44:126| B*44:127| B*44:128| B*44:129| B*44:130| B*44:131| B*44:132| B*44:133| B*44:134| B*44:135| B*44:136| B*44:137| B*44:138Q| B*44:139| B*44:140| B*44:141| B*44:142| B*44:143| B*44:144| B*44:145| B*44:146| B*44:147| B*44:148| B*44:150| B*44:151| B*44:152| B*44:153| B*44:154| B*44:155| B*44:156| B*44:157| B*44:158| B*44:159| B*44:160Q| B*44:161| B*44:162| B*44:163| B*44:164| B*44:165| B*44:166| B*44:167| B*44:168| B*44:169| B*44:170| B*44:172| B*44:173| B*44:174| B*44:175| B*44:176| B*44:177| B*44:178| B*44:179| B*44:180| B*44:181| B*44:182| B*44:183| B*44:184| B*44:185| B*44:186| B*44:187| B*44:188| B*44:189| B*44:190| B*44:191| B*44:192| B*44:193| B*44:194| B*44:196| B*44:197| B*44:199| B*44:200| B*44:201| B*44:202| B*44:203| B*44:204| B*44:205| B*44:206| B*44:207| B*44:208| B*44:209| B*44:210| B*44:211| B*44:212| B*44:213| B*44:214| B*44:215| B*44:216| B*44:218| B*44:219| B*44:220| B*44:221| B*44:222| B*44:223| B*44:224| B*44:225| B*44:226| B*44:227| B*44:228| B*44:229| B*44:230| B*44:231| B*44:232| B*44:233| B*44:234| B*44:235| B*44:236| B*44:238| B*44:239| B*44:240| B*44:241| B*44:242| B*44:243| B*44:244| B*44:245| B*44:247| B*44:248| B*44:249| B*44:250| B*44:251| B*44:252| B*44:253| B*44:254| B*44:255| B*44:256| B*44:257| B*44:258| B*44:259| B*44:260| B*44:261| B*44:262| B*44:263| B*44:264| B*44:265| B*44:266| B*44:268| B*44:269| B*44:270| B*44:271| B*44:272| B*44:273| B*44:274| B*44:275| B*44:276| B*44:277| B*51:42</t>
-  </si>
-  <si>
-    <t>B*44:09| B*45:01| B*45:02| B*45:03| B*45:05| B*45:06| B*45:07| B*45:08| B*45:09| B*45:10| B*45:11| B*45:12| B*45:13| B*45:14| B*45:15| B*45:16| B*45:17| B*45:18| B*45:19| B*45:20| B*45:21| B*50:02</t>
-  </si>
-  <si>
-    <t>B*44:15| B*44:46| B*44:02| B*44:03| B*44:04| B*44:05| B*44:06| B*44:07| B*44:08| B*44:10| B*44:11| B*44:12| B*44:13| B*44:14| B*44:17| B*44:18| B*44:20| B*44:21| B*44:22| B*44:24| B*44:25| B*44:26| B*44:27| B*44:28| B*44:29| B*44:30| B*44:31| B*44:32| B*44:33| B*44:34| B*44:35| B*44:36| B*44:37| B*44:38| B*44:39| B*44:40| B*44:41| B*44:43| B*44:44| B*44:45| B*44:47| B*44:48| B*44:49| B*44:50| B*44:51| B*44:53| B*44:54| B*44:55| B*44:57| B*44:59| B*44:60| B*44:62| B*44:63| B*44:64| B*44:65| B*44:66| B*44:67| B*44:68| B*44:69| B*44:70| B*44:71| B*44:72| B*44:73| B*44:74| B*44:75| B*44:76| B*44:77| B*44:78| B*44:79| B*44:80| B*44:81| B*44:82| B*44:83| B*44:84| B*44:85| B*44:86| B*44:87| B*44:88| B*44:89| B*44:90| B*44:91| B*44:92| B*44:93| B*44:94| B*44:95| B*44:96| B*44:97| B*44:98| B*44:99| B*44:100| B*44:101| B*44:102| B*44:103| B*44:104| B*44:105| B*44:106| B*44:107| B*44:109| B*44:110| B*44:111| B*44:112| B*44:113| B*44:114| B*44:115| B*44:116| B*44:117| B*44:118| B*44:119| B*44:120| B*44:121| B*44:122| B*44:123| B*44:124| B*44:125| B*44:126| B*44:127| B*44:128| B*44:129| B*44:130| B*44:131| B*44:132| B*44:133| B*44:134| B*44:135| B*44:136| B*44:137| B*44:138Q| B*44:139| B*44:140| B*44:141| B*44:142| B*44:143| B*44:144| B*44:145| B*44:146| B*44:147| B*44:148| B*44:150| B*44:151| B*44:152| B*44:153| B*44:154| B*44:155| B*44:156| B*44:157| B*44:158| B*44:159| B*44:160Q| B*44:161| B*44:162| B*44:163| B*44:164| B*44:165| B*44:166| B*44:167| B*44:168| B*44:169| B*44:170| B*44:172| B*44:173| B*44:174| B*44:175| B*44:176| B*44:177| B*44:178| B*44:179| B*44:180| B*44:181| B*44:182| B*44:183| B*44:184| B*44:185| B*44:186| B*44:187| B*44:188| B*44:189| B*44:190| B*44:191| B*44:192| B*44:193| B*44:194| B*44:196| B*44:197| B*44:199| B*44:200| B*44:201| B*44:202| B*44:203| B*44:204| B*44:205| B*44:206| B*44:207| B*44:208| B*44:209| B*44:210| B*44:211| B*44:212| B*44:213| B*44:214| B*44:215| B*44:216| B*44:218| B*44:219| B*44:220| B*44:221| B*44:222| B*44:223| B*44:224| B*44:225| B*44:226| B*44:227| B*44:228| B*44:229| B*44:230| B*44:231| B*44:232| B*44:233| B*44:234| B*44:235| B*44:236| B*44:238| B*44:239| B*44:240| B*44:241| B*44:242| B*44:243| B*44:244| B*44:245| B*44:247| B*44:248| B*44:249| B*44:250| B*44:251| B*44:252| B*44:253| B*44:254| B*44:255| B*44:256| B*44:257| B*44:258| B*44:259| B*44:260| B*44:261| B*44:262| B*44:263| B*44:264| B*44:265| B*44:266| B*44:268| B*44:269| B*44:270| B*44:271| B*44:272| B*44:273| B*44:274| B*44:275| B*44:276| B*44:277| B*51:42| B*44:09| B*45:01| B*45:02| B*45:03| B*45:05| B*45:06| B*45:07| B*45:08| B*45:09| B*45:10| B*45:11| B*45:12| B*45:13| B*45:14| B*45:15| B*45:16| B*45:17| B*45:18| B*45:19| B*45:20| B*45:21| B*50:02</t>
-  </si>
-  <si>
-    <t>B*46:01| B*46:02| B*46:03| B*46:04| B*46:05| B*46:06| B*46:08| B*46:09| B*46:10| B*46:12| B*46:13| B*46:14| B*46:16| B*46:17| B*46:18| B*46:19| B*46:20| B*46:21| B*46:22| B*46:23| B*46:24| B*46:25| B*46:26| B*46:27| B*46:28| B*46:29| B*46:30| B*46:31| B*46:32| B*46:33| B*46:34| B*46:35| B*46:36| B*46:37| B*46:38| B*46:39| B*46:40| B*46:42| B*46:43| B*46:44| B*46:45| B*46:46| B*46:47| B*46:48| B*46:49| B*46:50| B*46:51Q| B*46:52| B*46:53| B*46:54| B*46:56| B*46:57| B*46:58| B*46:59| B*46:60| B*46:61| B*46:62| B*46:63| B*46:64| B*46:65| B*46:66| B*46:67| B*46:68| B*46:69| B*46:70| B*46:71| B*46:72| B*46:73</t>
-  </si>
-  <si>
-    <t>B*46:11| B*54:03| B*55:05| B*55:09| B*55:12| B*55:16| B*55:20| B*56:03| B*54:01| B*54:02| B*54:04| B*54:06| B*54:07| B*54:09| B*54:10| B*54:11| B*54:12| B*54:13| B*54:14| B*54:15| B*54:16| B*54:17| B*54:18| B*54:19| B*54:20| B*54:21| B*54:22| B*54:23| B*54:24| B*54:25| B*54:26| B*54:27| B*54:28| B*54:29| B*54:30| B*54:31| B*54:32| B*54:33| B*54:34| B*54:35| B*54:36| B*54:37| B*54:38| B*55:07| B*55:01| B*55:02| B*55:03| B*55:04| B*55:10| B*55:11| B*55:13| B*55:14| B*55:15| B*55:17| B*55:18| B*55:19| B*55:21| B*55:22| B*55:23| B*55:24| B*55:25| B*55:26| B*55:27| B*55:28| B*55:29| B*55:30| B*55:31| B*55:32| B*55:33| B*55:34| B*55:35| B*55:36| B*55:37| B*55:38| B*55:39| B*55:40| B*55:41| B*55:42| B*55:43| B*55:44| B*55:45| B*55:46| B*55:47| B*55:48| B*55:49| B*55:50| B*55:51| B*55:52| B*55:53| B*55:54| B*55:56| B*55:57| B*55:58| B*55:59| B*55:60| B*55:61| B*55:62| B*55:63| B*55:64| B*55:65| B*55:66| B*55:67| B*55:68| B*55:69| B*55:70| B*55:71| B*55:72| B*55:73| B*55:74| B*55:75| B*55:76| B*55:77| B*55:78| B*55:79| B*55:80| B*55:81| B*55:82| B*55:84| B*55:85| B*55:86| B*55:87| B*56:10| B*56:12| B*55:08| B*56:01| B*56:02| B*56:04| B*56:07| B*56:08| B*56:09| B*56:11| B*56:13| B*56:14| B*56:15| B*56:16| B*56:17| B*56:18| B*56:20| B*56:21| B*56:22| B*56:23| B*56:24| B*56:25| B*56:26| B*56:27| B*56:29| B*56:30| B*56:31| B*56:32| B*56:33| B*56:34| B*56:35| B*56:36| B*56:37| B*56:39| B*56:40| B*56:41| B*56:42| B*56:43| B*56:44| B*56:45| B*56:46| B*56:47| B*56:48| B*56:49| B*56:50| B*56:51| B*56:52| B*56:53| B*56:54| B*56:55</t>
-  </si>
-  <si>
-    <t>B*47:05| B*58:08| B*58:09| B*57:01| B*57:02| B*57:03| B*57:04| B*57:05| B*57:06| B*57:07| B*57:08| B*57:09| B*57:10| B*57:11| B*57:12| B*57:13| B*57:14| B*57:15| B*57:16| B*57:17| B*57:18| B*57:19| B*57:20| B*57:21| B*57:22| B*57:23| B*57:24| B*57:25| B*57:26| B*57:27| B*57:29| B*57:30| B*57:31| B*57:32| B*57:33| B*57:34| B*57:35| B*57:36| B*57:37| B*57:38| B*57:39| B*57:40| B*57:41| B*57:42| B*57:43| B*57:44| B*57:45| B*57:46| B*57:47| B*57:48| B*57:49| B*57:50| B*57:51| B*57:52| B*57:53| B*57:54| B*57:55| B*57:56| B*57:57| B*57:58| B*57:59| B*57:60| B*57:61| B*57:62| B*57:63| B*57:64| B*57:65| B*57:66| B*57:67| B*57:68| B*57:69| B*57:70| B*57:71| B*57:72| B*57:73| B*57:74| B*57:75| B*57:76| B*57:77| B*57:78| B*57:80| B*57:81| B*57:82| B*57:83| B*57:84| B*57:85| B*57:86| B*57:87| B*57:88| B*57:89| B*57:90| B*57:91| B*57:92| B*57:93| B*58:01| B*58:02| B*58:04| B*58:05| B*58:06| B*58:07| B*58:11| B*58:12| B*58:13| B*58:14| B*58:15| B*58:16| B*58:18| B*58:19| B*58:20| B*58:21| B*58:22| B*58:23| B*58:24| B*58:25| B*58:26| B*58:27| B*58:28| B*58:29| B*58:32| B*58:33| B*58:34| B*58:35| B*58:36| B*58:37| B*58:38| B*58:40| B*58:41| B*58:42| B*58:43| B*58:44| B*58:45| B*58:46| B*58:47| B*58:48| B*58:49| B*58:50| B*58:51| B*58:52| B*58:53| B*58:54| B*58:55| B*58:56| B*58:57| B*58:58| B*58:59| B*58:60| B*58:61| B*58:62| B*58:63| B*58:64| B*58:65| B*58:66| B*58:67| B*58:68| B*58:69| B*58:70| B*58:71| B*58:73| B*58:74| B*58:75| B*58:76| B*58:77| B*58:78| B*58:79| B*58:80| B*58:81| B*58:82| B*58:83| B*58:84| B*58:85| B*58:86| B*58:87| B*58:88| B*58:89| B*58:90| B*58:91</t>
-  </si>
-  <si>
-    <t>B*49:01| B*49:02| B*49:03| B*49:04| B*49:05| B*49:06| B*49:08| B*49:09| B*49:10| B*49:11| B*49:12| B*49:13| B*49:14| B*49:16| B*49:17| B*49:18| B*49:20| B*49:21| B*49:22| B*49:23| B*49:24| B*49:25| B*49:26| B*49:27| B*49:28| B*49:29| B*49:30| B*49:31| B*49:32| B*49:33| B*49:34| B*49:35| B*49:36| B*49:37| B*49:38| B*49:39| B*49:40| B*49:41| B*49:42| B*49:43| B*49:44| B*49:45| B*49:46| B*49:47| B*49:48</t>
-  </si>
-  <si>
-    <t>B*51:02</t>
-  </si>
-  <si>
-    <t>B*51:16| B*15:23| B*51:01| B*51:03| B*51:04| B*51:05| B*51:06| B*51:07| B*51:08| B*51:09| B*51:10| B*51:12| B*51:13| B*51:14| B*51:15| B*51:17| B*51:18| B*51:19| B*51:20| B*51:21| B*51:22| B*51:23| B*51:24| B*51:26| B*51:28| B*51:29| B*51:30| B*51:31| B*51:32| B*51:33| B*51:34| B*51:35| B*51:36| B*51:37| B*51:38| B*51:39| B*51:40| B*51:43| B*51:45| B*51:46| B*51:48| B*51:49| B*51:50| B*51:51| B*51:52| B*51:53| B*51:54| B*51:55| B*51:56| B*51:57| B*51:58| B*51:59| B*51:60| B*51:61| B*51:62| B*51:63| B*51:64| B*51:65| B*51:66| B*51:67| B*51:68| B*51:69| B*51:70| B*51:71| B*51:72| B*51:73| B*51:74| B*51:75| B*51:76| B*51:77| B*51:78| B*51:79| B*51:80| B*51:81| B*51:82| B*51:83| B*51:84| B*51:85| B*51:86| B*51:87| B*51:88| B*51:89| B*51:90| B*51:91| B*51:92| B*51:93| B*51:94| B*51:95| B*51:96| B*51:97| B*51:99| B*51:100| B*51:101| B*51:102| B*51:103| B*51:104| B*51:105| B*51:106| B*51:107| B*51:108| B*51:109| B*51:111| B*51:112| B*51:113| B*51:114| B*51:115| B*51:116| B*51:117| B*51:119| B*51:120| B*51:121| B*51:122| B*51:123| B*51:124| B*51:125| B*51:126| B*51:127| B*51:128| B*51:129| B*51:130| B*51:131| B*51:132| B*51:133| B*51:134| B*51:135| B*51:136| B*51:137| B*51:138| B*51:139| B*51:140| B*51:141| B*51:142| B*51:143| B*51:144| B*51:145| B*51:146| B*51:147| B*51:148| B*51:150| B*51:151| B*51:152| B*51:153| B*51:154| B*51:155| B*51:156| B*51:157| B*51:158| B*51:159| B*51:160| B*51:161| B*51:162| B*51:163| B*51:164| B*51:165| B*51:166| B*51:167| B*51:168| B*51:169| B*51:170| B*51:171| B*51:172| B*51:173Q| B*51:174| B*51:175| B*51:176| B*51:177| B*51:179| B*51:180| B*51:181| B*51:182| B*51:183| B*51:185| B*51:186| B*51:187| B*51:188| B*51:189| B*51:190| B*51:191| B*51:192| B*51:193| B*51:194| B*51:195| B*51:196| B*51:197| B*51:198| B*51:199| B*51:200| B*51:201| B*51:202| B*51:203| B*51:204| B*51:205| B*51:206| B*51:207| B*51:208| B*51:209| B*51:210| B*51:211| B*51:212| B*51:213| B*51:214| B*51:215| B*51:216| B*51:217| B*51:218| B*51:219| B*51:220| B*51:221| B*51:222| B*51:223| B*51:224| B*51:225| B*51:226| B*51:227| B*51:228| B*51:229| B*52:01| B*52:02| B*52:03| B*52:04| B*52:05| B*52:06| B*52:07| B*52:08| B*52:09| B*52:10| B*52:11| B*52:12| B*52:13| B*52:14| B*52:15| B*52:16| B*52:17| B*52:18| B*52:19| B*52:20| B*52:21| B*52:22| B*52:23| B*52:24| B*52:25| B*52:26| B*52:27| B*52:28| B*52:29| B*52:30| B*52:31| B*52:32| B*52:33| B*52:34| B*52:35| B*52:36| B*52:37| B*52:38| B*52:39| B*52:40| B*52:41| B*52:42| B*52:43| B*52:44| B*52:45| B*52:46| B*52:47| B*52:48| B*52:50| B*52:51| B*52:52| B*52:53| B*52:54| B*52:55| B*52:56| B*52:57| B*52:58| B*52:59| B*52:60| B*52:61| B*52:62| B*52:63| B*52:64| B*52:65| B*52:66| B*52:67| B*52:68| B*52:69| B*52:70| B*52:71| B*52:72| B*52:73| B*56:06| B*78:01| B*78:02| B*78:03| B*78:05| B*78:06| B*78:07| B*78:08| B*78:09</t>
-  </si>
-  <si>
-    <t>B*52:01| B*52:02| B*52:03| B*52:04| B*52:05| B*52:06| B*52:07| B*52:08| B*52:09| B*52:10| B*52:11| B*52:12| B*52:13| B*52:14| B*52:15| B*52:16| B*52:17| B*52:18| B*52:19| B*52:20| B*52:21| B*52:22| B*52:23| B*52:24| B*52:25| B*52:26| B*52:27| B*52:28| B*52:29| B*52:30| B*52:31| B*52:32| B*52:33| B*52:34| B*52:35| B*52:36| B*52:37| B*52:38| B*52:39| B*52:40| B*52:41| B*52:42| B*52:43| B*52:44| B*52:45| B*52:46| B*52:47| B*52:48| B*52:50| B*52:51| B*52:52| B*52:53| B*52:54| B*52:55| B*52:56| B*52:57| B*52:58| B*52:59| B*52:60| B*52:61| B*52:62| B*52:63| B*52:64| B*52:65| B*52:66| B*52:67| B*52:68| B*52:69| B*52:70| B*52:71| B*52:72| B*52:73</t>
-  </si>
-  <si>
-    <t>B*53:01| B*53:02| B*53:03| B*53:04| B*53:05| B*53:06| B*53:07| B*53:08| B*53:09| B*53:10| B*53:11| B*53:12| B*53:13| B*53:14| B*53:15| B*53:16| B*53:17| B*53:18| B*53:19| B*53:20| B*53:21| B*53:22| B*53:23| B*53:24| B*53:25| B*53:26| B*53:27| B*53:28| B*53:29| B*53:30| B*53:31| B*53:32| B*53:33| B*53:34| B*53:35| B*53:36| B*53:37| B*53:38| B*53:39| B*53:40| B*53:41| B*53:42| B*53:43| B*53:44| B*53:45| B*53:46| B*53:47| B*53:49</t>
-  </si>
-  <si>
-    <t>B*54:01| B*54:02| B*54:04| B*54:06| B*54:07| B*54:09| B*54:10| B*54:11| B*54:12| B*54:13| B*54:14| B*54:15| B*54:16| B*54:17| B*54:18| B*54:19| B*54:20| B*54:21| B*54:22| B*54:23| B*54:24| B*54:25| B*54:26| B*54:27| B*54:28| B*54:29| B*54:30| B*54:31| B*54:32| B*54:33| B*54:34| B*54:35| B*54:36| B*54:37| B*54:38| B*55:07</t>
-  </si>
-  <si>
-    <t>B*55:01| B*55:02| B*55:03| B*55:04| B*55:10| B*55:11| B*55:13| B*55:14| B*55:15| B*55:17| B*55:18| B*55:19| B*55:21| B*55:22| B*55:23| B*55:24| B*55:25| B*55:26| B*55:27| B*55:28| B*55:29| B*55:30| B*55:31| B*55:32| B*55:33| B*55:34| B*55:35| B*55:36| B*55:37| B*55:38| B*55:39| B*55:40| B*55:41| B*55:42| B*55:43| B*55:44| B*55:45| B*55:46| B*55:47| B*55:48| B*55:49| B*55:50| B*55:51| B*55:52| B*55:53| B*55:54| B*55:56| B*55:57| B*55:58| B*55:59| B*55:60| B*55:61| B*55:62| B*55:63| B*55:64| B*55:65| B*55:66| B*55:67| B*55:68| B*55:69| B*55:70| B*55:71| B*55:72| B*55:73| B*55:74| B*55:75| B*55:76| B*55:77| B*55:78| B*55:79| B*55:80| B*55:81| B*55:82| B*55:84| B*55:85| B*55:86| B*55:87| B*56:10| B*56:12</t>
-  </si>
-  <si>
-    <t>B*55:08| B*56:01| B*56:02| B*56:04| B*56:07| B*56:08| B*56:09| B*56:11| B*56:13| B*56:14| B*56:15| B*56:16| B*56:17| B*56:18| B*56:20| B*56:21| B*56:22| B*56:23| B*56:24| B*56:25| B*56:26| B*56:27| B*56:29| B*56:30| B*56:31| B*56:32| B*56:33| B*56:34| B*56:35| B*56:36| B*56:37| B*56:39| B*56:40| B*56:41| B*56:42| B*56:43| B*56:44| B*56:45| B*56:46| B*56:47| B*56:48| B*56:49| B*56:50| B*56:51| B*56:52| B*56:53| B*56:54| B*56:55</t>
-  </si>
-  <si>
-    <t>B*56:06| B*78:01| B*78:02| B*78:03| B*78:05| B*78:06| B*78:07| B*78:08| B*78:09</t>
-  </si>
-  <si>
-    <t>B*57:01| B*57:02| B*57:03| B*57:04| B*57:05| B*57:06| B*57:07| B*57:08| B*57:09| B*57:10| B*57:11| B*57:12| B*57:13| B*57:14| B*57:15| B*57:16| B*57:17| B*57:18| B*57:19| B*57:20| B*57:21| B*57:22| B*57:23| B*57:24| B*57:25| B*57:26| B*57:27| B*57:29| B*57:30| B*57:31| B*57:32| B*57:33| B*57:34| B*57:35| B*57:36| B*57:37| B*57:38| B*57:39| B*57:40| B*57:41| B*57:42| B*57:43| B*57:44| B*57:45| B*57:46| B*57:47| B*57:48| B*57:49| B*57:50| B*57:51| B*57:52| B*57:53| B*57:54| B*57:55| B*57:56| B*57:57| B*57:58| B*57:59| B*57:60| B*57:61| B*57:62| B*57:63| B*57:64| B*57:65| B*57:66| B*57:67| B*57:68| B*57:69| B*57:70| B*57:71| B*57:72| B*57:73| B*57:74| B*57:75| B*57:76| B*57:77| B*57:78| B*57:80| B*57:81| B*57:82| B*57:83| B*57:84| B*57:85| B*57:86| B*57:87| B*57:88| B*57:89| B*57:90| B*57:91| B*57:92| B*57:93</t>
-  </si>
-  <si>
-    <t>B*58:01| B*58:02| B*58:04| B*58:05| B*58:06| B*58:07| B*58:11| B*58:12| B*58:13| B*58:14| B*58:15| B*58:16| B*58:18| B*58:19| B*58:20| B*58:21| B*58:22| B*58:23| B*58:24| B*58:25| B*58:26| B*58:27| B*58:28| B*58:29| B*58:32| B*58:33| B*58:34| B*58:35| B*58:36| B*58:37| B*58:38| B*58:40| B*58:41| B*58:42| B*58:43| B*58:44| B*58:45| B*58:46| B*58:47| B*58:48| B*58:49| B*58:50| B*58:51| B*58:52| B*58:53| B*58:54| B*58:55| B*58:56| B*58:57| B*58:58| B*58:59| B*58:60| B*58:61| B*58:62| B*58:63| B*58:64| B*58:65| B*58:66| B*58:67| B*58:68| B*58:69| B*58:70| B*58:71| B*58:73| B*58:74| B*58:75| B*58:76| B*58:77| B*58:78| B*58:79| B*58:80| B*58:81| B*58:82| B*58:83| B*58:84| B*58:85| B*58:86| B*58:87| B*58:88| B*58:89| B*58:90| B*58:91</t>
-  </si>
-  <si>
-    <t>B*59:01| B*59:02| B*59:03| B*59:04| B*59:05| B*59:06| B*59:07| B*59:08| B*59:09</t>
-  </si>
-  <si>
-    <t>B*67:01| B*67:02| B*67:03| B*67:04| B*67:05| B*67:06| B*67:07</t>
+    <t>B*15:68| B*35:01:01:01| B*35:01:01:02| B*35:01:01:03| B*35:01:01:04| B*35:01:01:05| B*35:01:01:06| B*35:01:01:07| B*35:01:01:08| B*35:01:01:09| B*35:01:01:10| B*35:01:01:11| B*35:01:01:12| B*35:01:01:13| B*35:01:01:14| B*35:01:01:15| B*35:01:01:16| B*35:01:01:17| B*35:01:01:18| B*35:01:02| B*35:01:03| B*35:01:04| B*35:01:05| B*35:01:06| B*35:01:07| B*35:01:08| B*35:01:09| B*35:01:10| B*35:01:11| B*35:01:12| B*35:01:13| B*35:01:14| B*35:01:15| B*35:01:16| B*35:01:17| B*35:01:18| B*35:01:19| B*35:01:20| B*35:01:21| B*35:01:22| B*35:01:23| B*35:01:24| B*35:01:25| B*35:01:26| B*35:01:27| B*35:01:28| B*35:01:29| B*35:01:30| B*35:01:31| B*35:01:32| B*35:01:33| B*35:01:34| B*35:01:35| B*35:01:36| B*35:01:37| B*35:01:38| B*35:01:39| B*35:01:40| B*35:01:41| B*35:01:42| B*35:01:43| B*35:01:44| B*35:01:45| B*35:01:46| B*35:01:47| B*35:01:48| B*35:01:49| B*35:01:50| B*35:01:51| B*35:01:52| B*35:01:53| B*35:01:54| B*35:01:55| B*35:02:01:01| B*35:02:01:02| B*35:02:01:03| B*35:02:02| B*35:02:03| B*35:02:04| B*35:02:05| B*35:02:06| B*35:02:07| B*35:02:08| B*35:02:09| B*35:02:10| B*35:02:11| B*35:02:12| B*35:03:01:01| B*35:03:01:02| B*35:03:01:03| B*35:03:01:04| B*35:03:01:05| B*35:03:01:06| B*35:03:01:07| B*35:03:01:08| B*35:03:01:09| B*35:03:01:10| B*35:03:02| B*35:03:03| B*35:03:04| B*35:03:05| B*35:03:06| B*35:03:07| B*35:03:08| B*35:03:09| B*35:03:10| B*35:03:11| B*35:03:12| B*35:03:13| B*35:03:14| B*35:03:15| B*35:03:16| B*35:03:17| B*35:03:18| B*35:03:19| B*35:03:20| B*35:03:21| B*35:03:22| B*35:03:23| B*35:03:24| B*35:03:25| B*35:04:01| B*35:04:02| B*35:04:03| B*35:05:01:01| B*35:05:01:02| B*35:05:01:03| B*35:05:02| B*35:05:03| B*35:06| B*35:07| B*35:08:01:01| B*35:08:01:02| B*35:08:02| B*35:08:03| B*35:08:04| B*35:08:05| B*35:08:06| B*35:08:07| B*35:08:08| B*35:08:09| B*35:08:10| B*35:09:01| B*35:09:02| B*35:09:03| B*35:10| B*35:11:01| B*35:11:02| B*35:11:03| B*35:12:01| B*35:12:02| B*35:12:03| B*35:12:04| B*35:13| B*35:14:01| B*35:14:02| B*35:14:03| B*35:15:01| B*35:15:02| B*35:16| B*35:17:01| B*35:17:02| B*35:18| B*35:19| B*35:20:01| B*35:20:02| B*35:21| B*35:22:01:01| B*35:22:01:02| B*35:23| B*35:24:01| B*35:24:02| B*35:25| B*35:26| B*35:27| B*35:28| B*35:29:01| B*35:29:02| B*35:30| B*35:31| B*35:32:01| B*35:32:02| B*35:33| B*35:34| B*35:35| B*35:36| B*35:37| B*35:38| B*35:39| B*35:41| B*35:42:01| B*35:42:02| B*35:43:01| B*35:43:03| B*35:44| B*35:45| B*35:46| B*35:47| B*35:48| B*35:49| B*35:50| B*35:51| B*35:52| B*35:54| B*35:55| B*35:56| B*35:57| B*35:58| B*35:59:01| B*35:59:02| B*35:60| B*35:61:01| B*35:61:02| B*35:62| B*35:63| B*35:64:01| B*35:64:02| B*35:65Q| B*35:66| B*35:67| B*35:68:01| B*35:68:02| B*35:69| B*35:70| B*35:71| B*35:72| B*35:74| B*35:75| B*35:76| B*35:77| B*35:78| B*35:79| B*35:80| B*35:81| B*35:82| B*35:83| B*35:84| B*35:85| B*35:86| B*35:87| B*35:88| B*35:89| B*35:90| B*35:91| B*35:92| B*35:93| B*35:94| B*35:95| B*35:96| B*35:97| B*35:98| B*35:99| B*35:100| B*35:101:01| B*35:101:02| B*35:102| B*35:103| B*35:104| B*35:105| B*35:106| B*35:107| B*35:108:01| B*35:108:02| B*35:109| B*35:110| B*35:111| B*35:112| B*35:113| B*35:114| B*35:115| B*35:116| B*35:117| B*35:118| B*35:119| B*35:120| B*35:121| B*35:122| B*35:123| B*35:124| B*35:125| B*35:126| B*35:127| B*35:128| B*35:131:01| B*35:131:02| B*35:132| B*35:133| B*35:135| B*35:136| B*35:137| B*35:138| B*35:139| B*35:140| B*35:141| B*35:142| B*35:143| B*35:144| B*35:146| B*35:147| B*35:148| B*35:149| B*35:150:01| B*35:150:02| B*35:151:01| B*35:151:02| B*35:152| B*35:153| B*35:154| B*35:155| B*35:156| B*35:157| B*35:158| B*35:159| B*35:160| B*35:161| B*35:162| B*35:163| B*35:164| B*35:166| B*35:167| B*35:168| B*35:169| B*35:170| B*35:171| B*35:172| B*35:174| B*35:175| B*35:176| B*35:177| B*35:178| B*35:179| B*35:180| B*35:181| B*35:182| B*35:183| B*35:184| B*35:185| B*35:186| B*35:187| B*35:188| B*35:189| B*35:190| B*35:191| B*35:192| B*35:193| B*35:194| B*35:195| B*35:196| B*35:197| B*35:198| B*35:199| B*35:200| B*35:201| B*35:202| B*35:203| B*35:204| B*35:205| B*35:206| B*35:207| B*35:208:01| B*35:208:02| B*35:209| B*35:210| B*35:211| B*35:212| B*35:213| B*35:214| B*35:215| B*35:217| B*35:218| B*35:219| B*35:220| B*35:221| B*35:222| B*35:223| B*35:224| B*35:225| B*35:226| B*35:227| B*35:228| B*35:229| B*35:230| B*35:231| B*35:232| B*35:233| B*35:234| B*35:235| B*35:236| B*35:237| B*35:238| B*35:239| B*35:240| B*35:241| B*35:242| B*35:243| B*35:244| B*35:245| B*35:246| B*35:247| B*35:248| B*35:249| B*35:250| B*35:251| B*35:252| B*35:253| B*35:254| B*35:255| B*35:256| B*35:257| B*35:258| B*35:259| B*35:260| B*35:261| B*35:262| B*35:263| B*35:264| B*35:265| B*35:266| B*35:267| B*35:268| B*35:269| B*35:270| B*35:271| B*35:272| B*35:273| B*35:274| B*35:275| B*35:276| B*35:277| B*35:278| B*35:279| B*35:280| B*35:281| B*35:282| B*35:283| B*35:284| B*35:285| B*35:286| B*35:287| B*35:288| B*35:289| B*35:290| B*35:291| B*35:292| B*35:293| B*35:294| B*35:295| B*35:296| B*35:297| B*35:298| B*35:299| B*35:300| B*35:301| B*35:302| B*35:303| B*35:304| B*35:305| B*35:306| B*35:307| B*35:308| B*35:309| B*35:310| B*35:311| B*35:312| B*35:313| B*35:314| B*35:315| B*35:316| B*35:317| B*35:318| B*35:319| B*35:320| B*35:321| B*35:322| B*35:323| B*35:324| B*35:325| B*35:326| B*35:327| B*35:328| B*35:329| B*35:330| B*35:331| B*35:332| B*35:333Q| B*35:334| B*35:335| B*35:336| B*35:337:01| B*35:337:02| B*35:338| B*35:339| B*35:340| B*35:341| B*35:342| B*35:343| B*35:344| B*35:345| B*35:346| B*35:347| B*35:348| B*35:349| B*35:350| B*35:351| B*35:352| B*35:353| B*35:354| B*35:355| B*35:356| B*35:357| B*35:358| B*35:359| B*35:360| B*35:361| B*35:362| B*35:363| B*35:364| B*35:365| B*35:366| B*35:367| B*35:368| B*35:369| B*35:370| B*35:371| B*35:372| B*35:373| B*35:374| B*35:375| B*35:376| B*35:377| B*35:378| B*35:379| B*35:380| B*35:382| B*35:383| B*35:384| B*35:385| B*35:386| B*35:387| B*35:388| B*35:389| B*35:391| B*35:392| B*35:393| B*35:394| B*35:395| B*35:396| B*35:397| B*35:398| B*35:399| B*35:400| B*35:401| B*35:402| B*35:403| B*35:404| B*35:405| B*35:406| B*35:407| B*35:408| B*35:409| B*35:410| B*35:411| B*35:412| B*35:413| B*78:04</t>
+  </si>
+  <si>
+    <t>B*37:01:01:01| B*37:01:01:02| B*37:01:01:03| B*37:01:01:04| B*37:01:02| B*37:01:03| B*37:01:04| B*37:01:05| B*37:01:06| B*37:01:07| B*37:01:08| B*37:01:09| B*37:01:10| B*37:01:11| B*37:01:12| B*37:01:13| B*37:01:14| B*37:01:15| B*37:02| B*37:04:01| B*37:04:02| B*37:05| B*37:06:01| B*37:06:02| B*37:07| B*37:08| B*37:09| B*37:10| B*37:11| B*37:12| B*37:13| B*37:14| B*37:15| B*37:16Q| B*37:17| B*37:18| B*37:19:01| B*37:19:02| B*37:20| B*37:21| B*37:22| B*37:23| B*37:24| B*37:25| B*37:26| B*37:27| B*37:28| B*37:29| B*37:31| B*37:32| B*37:34| B*37:35| B*37:36| B*37:37| B*37:38| B*37:39| B*37:40| B*37:41| B*37:43| B*37:44| B*37:45| B*37:46| B*37:47| B*37:48| B*37:49| B*37:50| B*37:51| B*37:52| B*37:53| B*37:54| B*37:55| B*37:56| B*37:57| B*37:58| B*37:59| B*37:60| B*37:61| B*37:62| B*37:63| B*37:64| B*37:65| B*37:66| B*37:67| B*37:68| B*37:69| B*37:70| B*37:71| B*37:72| B*37:73| B*37:74| B*37:75| B*37:76| B*37:77| B*37:78| B*37:80</t>
+  </si>
+  <si>
+    <t>B*38:01:01:01| B*38:01:01:02| B*38:01:02| B*38:01:03| B*38:01:04| B*38:01:05| B*38:01:06| B*38:01:07| B*38:01:08| B*38:01:09| B*38:01:10| B*38:01:11| B*38:01:12| B*38:01:13| B*38:01:14| B*38:01:15| B*38:02:01| B*38:02:02| B*38:02:03| B*38:02:04| B*38:02:05| B*38:02:06| B*38:02:07| B*38:02:08| B*38:04| B*38:05| B*38:06| B*38:07| B*38:08| B*38:10| B*38:11| B*38:12| B*38:13| B*38:14| B*38:15| B*38:16| B*38:17| B*38:18| B*38:19| B*38:20:01| B*38:20:02| B*38:21| B*38:22| B*38:23| B*38:24| B*38:25| B*38:26| B*38:27| B*38:28| B*38:29| B*38:30| B*38:31| B*38:32| B*38:33| B*38:35| B*38:36| B*38:37| B*38:38| B*38:39| B*38:40| B*38:41| B*38:42| B*38:43| B*38:44| B*38:45| B*38:46| B*38:47| B*38:48| B*38:49| B*38:50| B*38:51| B*38:52| B*38:53| B*38:54| B*38:55Q| B*38:56| B*38:57| B*38:58| B*38:59| B*38:60| B*38:61| B*38:62| B*38:63| B*38:64| B*38:65| B*38:66| B*38:67| B*38:68Q| B*38:69| B*38:70| B*38:71| B*38:72| B*38:73| B*38:74| B*38:75| B*38:76| B*38:77| B*38:78| B*38:79| B*38:81| B*38:82</t>
+  </si>
+  <si>
+    <t>B*39:03:01:01| B*39:03:01:02| B*39:04| B*39:06:01| B*39:06:02:01| B*39:06:02:02| B*39:06:02:03| B*39:06:02:04| B*39:06:03| B*39:06:04| B*39:06:05| B*39:06:06| B*39:08| B*39:09:01:01| B*39:09:01:02| B*39:09:01:03| B*39:09:02| B*39:09:03| B*39:10:01| B*39:10:02| B*39:11| B*39:12:01:01| B*39:12:01:02| B*39:13:01| B*39:13:02| B*39:14:01:01| B*39:14:01:02| B*39:15| B*39:16| B*39:17| B*39:18| B*39:19:01| B*39:19:02| B*39:20| B*39:22| B*39:23| B*39:24:01| B*39:24:02| B*39:26| B*39:27| B*39:28| B*39:29| B*39:30| B*39:31:01:01| B*39:31:01:02| B*39:33| B*39:34| B*39:35| B*39:36| B*39:37| B*39:38Q| B*39:39:01| B*39:39:02| B*39:41| B*39:42| B*39:43| B*39:44| B*39:45| B*39:46| B*39:47| B*39:48| B*39:49| B*39:50| B*39:51| B*39:52| B*39:53| B*39:54| B*39:55| B*39:56| B*39:57| B*39:58| B*39:59| B*39:60| B*39:61| B*39:62| B*39:63| B*39:64| B*39:65| B*39:66| B*39:67| B*39:68| B*39:69| B*39:70| B*39:71| B*39:72| B*39:73| B*39:74| B*39:75| B*39:76| B*39:77| B*39:78| B*39:79| B*39:80| B*39:81| B*39:82| B*39:83| B*39:84| B*39:85| B*39:86| B*39:88| B*39:89| B*39:90| B*39:91| B*39:92| B*39:93| B*39:94| B*39:96| B*39:98| B*39:99| B*39:100| B*39:101| B*39:102| B*39:103| B*39:104| B*39:105| B*39:106| B*39:107| B*39:108| B*39:109| B*39:110| B*39:111| B*39:112| B*39:113| B*39:114| B*39:115| B*39:117| B*39:118| B*39:119| B*39:120| B*39:121| B*39:122| B*39:123| B*39:124| B*39:125| B*39:126| B*39:127| B*39:128| B*39:129| B*39:130| B*39:131| B*39:132| B*39:134| B*39:135| B*39:136| B*39:137| B*39:138| B*39:140| B*39:141| B*39:143| B*39:01:01:01| B*39:01:01:02L| B*39:01:01:03| B*39:01:01:04| B*39:01:01:05| B*39:01:01:06| B*39:01:01:07| B*39:01:01:08| B*39:01:01:09| B*39:01:03:01| B*39:01:03:02| B*39:01:04| B*39:01:05| B*39:01:06| B*39:01:07| B*39:01:08| B*39:01:09| B*39:01:10| B*39:01:11| B*39:01:12| B*39:01:13| B*39:01:14| B*39:01:15| B*39:01:16| B*39:01:17| B*39:01:18| B*39:01:19| B*39:01:20| B*39:01:21| B*39:01:22| B*39:01:23| B*39:01:24| B*39:01:25| B*39:01:26| B*39:02:01| B*39:02:02:01| B*39:02:02:02| B*39:02:02:03| B*39:02:03| B*39:05:01:01| B*39:05:01:02| B*39:05:02| B*39:05:03</t>
+  </si>
+  <si>
+    <t>B*39:01:01:01| B*39:01:01:02L| B*39:01:01:03| B*39:01:01:04| B*39:01:01:05| B*39:01:01:06| B*39:01:01:07| B*39:01:01:08| B*39:01:01:09| B*39:01:03:01| B*39:01:03:02| B*39:01:04| B*39:01:05| B*39:01:06| B*39:01:07| B*39:01:08| B*39:01:09| B*39:01:10| B*39:01:11| B*39:01:12| B*39:01:13| B*39:01:14| B*39:01:15| B*39:01:16| B*39:01:17| B*39:01:18| B*39:01:19| B*39:01:20| B*39:01:21| B*39:01:22| B*39:01:23| B*39:01:24| B*39:01:25| B*39:01:26</t>
+  </si>
+  <si>
+    <t>B*39:02:01| B*39:02:02:01| B*39:02:02:02| B*39:02:02:03| B*39:02:03</t>
+  </si>
+  <si>
+    <t>B*40:13| B*40:15| B*40:21| B*40:23| B*40:25| B*40:28| B*40:32| B*40:47| B*40:51| B*40:58| B*40:59| B*40:60| B*40:64:01:01| B*40:64:01:02| B*40:68| B*40:78| B*40:79| B*40:80| B*40:81| B*40:82| B*40:83| B*40:84| B*40:85| B*40:86| B*40:87:01| B*40:87:02| B*40:88| B*40:89| B*40:90| B*40:91| B*40:92| B*40:93| B*40:94| B*40:95| B*40:96| B*40:97| B*40:98| B*40:99| B*40:100| B*40:101| B*40:102| B*40:103| B*40:104| B*40:105| B*40:106| B*40:107| B*40:108| B*40:109| B*40:110| B*40:111| B*40:112| B*40:113| B*40:114:01| B*40:114:02| B*40:115| B*40:116| B*40:117| B*40:119| B*40:120| B*40:121| B*40:122| B*40:123| B*40:124:01| B*40:124:02| B*40:125:01| B*40:125:02| B*40:126| B*40:127| B*40:128| B*40:129| B*40:130:01| B*40:130:02| B*40:131| B*40:132| B*40:133Q| B*40:134| B*40:135| B*40:136| B*40:137| B*40:138| B*40:139| B*40:140| B*40:141| B*40:143| B*40:145| B*40:146| B*40:147| B*40:148| B*40:149| B*40:150| B*40:151| B*40:152| B*40:153| B*40:154| B*40:156| B*40:157| B*40:158| B*40:159| B*40:160:01| B*40:160:02| B*40:161| B*40:162| B*40:163| B*40:164| B*40:165| B*40:166| B*40:167| B*40:168| B*40:169| B*40:170| B*40:171| B*40:172| B*40:173| B*40:174| B*40:175| B*40:176| B*40:177| B*40:178| B*40:179| B*40:180| B*40:181| B*40:182| B*40:183| B*40:184| B*40:185| B*40:186:01| B*40:186:02| B*40:187| B*40:188| B*40:189| B*40:190| B*40:191| B*40:192| B*40:193| B*40:194| B*40:195| B*40:196| B*40:197| B*40:198| B*40:199| B*40:200| B*40:201| B*40:202| B*40:203| B*40:204| B*40:205| B*40:206| B*40:207| B*40:208| B*40:209| B*40:210| B*40:211| B*40:212| B*40:213| B*40:214| B*40:215| B*40:217| B*40:218| B*40:219| B*40:220| B*40:221| B*40:222| B*40:223| B*40:224| B*40:225| B*40:226| B*40:227| B*40:228| B*40:229| B*40:230| B*40:231| B*40:232| B*40:233| B*40:234| B*40:235| B*40:236| B*40:237| B*40:238| B*40:239| B*40:240| B*40:241| B*40:242| B*40:243| B*40:244| B*40:245| B*40:246| B*40:247| B*40:248| B*40:249| B*40:250| B*40:251| B*40:252| B*40:253| B*40:254| B*40:255| B*40:257| B*40:258| B*40:259| B*40:260| B*40:261| B*40:262| B*40:264| B*40:266| B*40:267| B*40:268| B*40:269| B*40:270| B*40:271| B*40:272| B*40:273| B*40:274| B*40:275| B*40:276| B*40:277| B*40:278| B*40:279| B*40:280| B*40:281| B*40:282| B*40:283| B*40:284| B*40:285| B*40:287| B*40:288| B*40:289| B*40:290| B*40:292| B*40:293| B*40:294| B*40:295| B*40:296| B*40:297| B*40:298:01| B*40:298:02| B*40:299| B*40:300| B*40:301| B*40:302| B*40:303| B*40:304| B*40:305| B*40:306| B*40:307| B*40:308| B*40:309| B*40:310| B*40:311| B*40:312| B*40:313| B*40:314| B*40:315| B*40:316| B*40:317| B*40:318| B*40:319| B*40:320| B*40:321| B*40:322| B*40:323| B*40:324| B*40:325| B*40:326| B*40:327| B*40:328| B*40:329| B*40:330| B*40:331| B*40:332| B*40:333| B*40:334| B*40:335| B*40:336| B*40:339| B*40:340| B*40:341| B*40:342| B*40:343| B*40:344| B*40:346| B*40:347| B*40:348| B*40:349| B*40:350| B*40:351| B*40:352| B*40:353| B*40:354| B*40:355| B*40:356| B*40:357| B*40:358| B*40:359| B*40:360| B*40:362| B*40:363| B*40:364| B*40:365| B*40:366| B*40:367| B*40:368| B*40:369| B*40:370| B*40:371| B*40:373| B*40:374| B*40:375| B*40:376| B*40:377| B*40:378| B*40:379| B*40:380| B*40:381| B*40:382| B*40:383| B*40:384| B*40:385| B*40:386| B*40:387| B*40:388| B*40:389| B*40:390| B*40:391| B*40:392| B*40:393| B*40:394| B*40:395| B*40:396| B*40:397| B*40:398| B*40:400| B*40:401| B*40:402| B*40:403| B*40:404| B*40:405| B*40:406| B*40:407| B*40:408| B*40:409| B*40:410| B*40:411| B*40:412| B*40:413| B*40:414| B*40:01:01| B*40:01:02:01| B*40:01:02:02| B*40:01:02:03| B*40:01:02:04| B*40:01:02:05| B*40:01:02:06| B*40:01:02:07| B*40:01:02:08| B*40:01:02:09| B*40:01:03| B*40:01:04| B*40:01:05| B*40:01:06| B*40:01:07| B*40:01:08| B*40:01:09| B*40:01:10| B*40:01:11| B*40:01:12| B*40:01:13| B*40:01:14| B*40:01:15| B*40:01:16| B*40:01:17| B*40:01:18| B*40:01:19| B*40:01:20| B*40:01:21| B*40:01:22| B*40:01:23| B*40:01:24| B*40:01:25| B*40:01:26| B*40:01:27| B*40:01:28| B*40:01:29| B*40:01:30| B*40:01:31| B*40:01:32| B*40:01:33| B*40:01:34| B*40:01:35| B*40:01:36| B*40:01:37| B*40:01:38| B*40:01:39| B*40:01:40| B*40:01:41| B*40:01:42| B*40:01:43| B*40:01:44| B*40:01:45| B*40:01:46| B*40:01:47| B*40:01:48| B*40:01:49| B*40:01:50| B*40:01:51| B*40:01:52| B*40:01:53| B*40:01:54| B*40:01:55| B*40:01:56| B*40:01:57| B*40:01:58| B*40:01:59| B*40:01:60| B*40:07| B*40:10:01:01| B*40:10:01:02| B*40:10:02| B*40:14:01| B*40:14:02| B*40:14:03| B*40:30| B*40:31| B*40:33| B*40:34| B*40:36| B*40:38| B*40:42| B*40:43| B*40:45| B*40:46| B*40:48| B*40:49| B*40:52| B*40:54| B*40:55| B*40:61| B*40:62| B*40:63| B*40:65| B*40:66| B*40:67| B*40:69| B*40:72:01| B*40:72:02| B*40:73| B*40:74| B*40:76| B*40:77| B*47:02| B*40:02:01:01| B*40:02:01:02| B*40:02:01:03| B*40:02:01:04| B*40:02:01:05| B*40:02:01:06| B*40:02:01:07| B*40:02:01:08| B*40:02:02| B*40:02:03| B*40:02:04| B*40:02:05| B*40:02:06| B*40:02:07| B*40:02:08| B*40:02:09| B*40:02:10| B*40:02:11| B*40:02:12| B*40:02:13| B*40:02:14| B*40:02:15| B*40:02:16| B*40:02:17| B*40:02:18| B*40:02:19| B*40:02:20| B*40:02:21| B*40:02:22| B*40:02:23| B*40:02:24| B*40:02:25| B*40:02:26| B*40:03:01:01| B*40:03:01:02| B*40:04:01| B*40:04:02| B*40:06:01:01| B*40:06:01:02| B*40:06:02| B*40:06:03| B*40:06:04:01| B*40:06:04:02| B*40:06:05| B*40:06:06| B*40:06:07| B*40:06:08| B*40:06:09| B*40:06:10| B*40:06:11| B*40:06:12| B*40:06:13| B*40:06:14| B*40:06:15| B*40:06:16| B*40:06:17| B*40:06:18| B*40:08| B*40:09| B*40:11:01| B*40:11:02| B*40:16| B*40:18| B*40:20:01:01| B*40:20:01:02| B*40:24| B*40:27:01| B*40:27:02| B*40:29| B*40:35:01| B*40:35:02| B*40:37| B*40:40| B*40:44| B*40:50| B*40:53| B*40:56| B*40:57| B*40:70:01| B*40:70:02| B*40:71| B*40:75</t>
+  </si>
+  <si>
+    <t>B*40:05:01:01| B*40:05:01:02| B*15:46| B*50:01:01:01| B*50:01:01:02| B*50:01:02| B*50:01:03| B*50:01:04| B*50:01:05| B*50:01:06| B*50:01:07| B*50:01:08| B*50:01:09| B*50:01:10| B*50:04| B*50:05| B*50:06| B*50:07| B*50:08| B*50:09| B*50:10| B*50:11| B*50:12| B*50:13| B*50:14| B*50:15| B*50:16| B*50:17| B*50:18| B*50:19| B*50:20| B*50:31| B*50:32| B*50:33| B*50:34| B*50:35| B*50:36| B*50:37| B*50:38| B*50:39| B*50:40| B*50:41| B*50:42| B*50:43| B*50:44| B*50:45| B*50:46| B*50:47| B*50:48| B*50:49| B*50:50| B*50:51| B*50:52| B*50:53| B*50:54| B*50:55| B*50:56| B*50:57| B*50:58| B*50:59| B*50:60| B*50:61</t>
+  </si>
+  <si>
+    <t>B*40:39| B*41:01:01:01| B*41:01:01:02| B*41:01:02| B*41:01:03| B*41:01:04| B*41:01:05| B*41:02:01:01| B*41:02:01:02| B*41:02:01:03| B*41:02:02| B*41:02:03| B*41:02:04| B*41:02:05| B*41:02:06| B*41:02:07| B*41:02:08| B*41:03:01| B*41:03:02| B*41:04| B*41:05| B*41:06| B*41:07| B*41:08| B*41:09| B*41:10| B*41:11| B*41:12| B*41:13| B*41:14| B*41:15| B*41:16| B*41:17| B*41:18| B*41:19| B*41:20| B*41:21| B*41:22| B*41:23| B*41:24| B*41:25| B*41:26| B*41:27| B*41:28| B*41:29| B*41:30| B*41:31| B*41:32| B*41:33| B*41:34| B*41:35| B*41:36| B*41:37| B*41:38| B*41:39| B*41:40| B*41:41| B*41:42| B*41:43| B*41:44| B*41:46| B*41:47| B*41:48| B*41:49| B*41:50| B*41:51| B*41:52| B*41:53| B*41:54| B*41:55| B*41:56</t>
+  </si>
+  <si>
+    <t>B*42:01:01| B*42:01:02| B*42:01:03| B*42:02:01:01| B*42:02:01:02| B*42:04| B*42:05:01| B*42:05:02| B*42:06| B*42:07| B*42:08| B*42:09| B*42:10| B*42:11| B*42:12| B*42:13| B*42:14| B*42:15| B*42:16| B*42:17| B*42:18| B*42:19| B*42:20| B*42:21| B*42:22| B*42:23| B*42:24| B*42:25</t>
+  </si>
+  <si>
+    <t>B*44:02:01:01| B*44:02:01:03| B*44:02:01:04| B*44:02:01:05| B*44:02:01:06| B*44:02:01:07| B*44:02:01:08| B*44:02:01:09| B*44:02:01:10| B*44:02:01:11| B*44:02:01:12| B*44:02:01:13| B*44:02:01:14| B*44:02:01:15| B*44:02:01:16| B*44:02:01:17| B*44:02:01:18| B*44:02:01:19| B*44:02:01:20| B*44:02:02| B*44:02:03| B*44:02:04| B*44:02:05| B*44:02:06| B*44:02:07| B*44:02:08| B*44:02:09| B*44:02:10| B*44:02:11| B*44:02:12| B*44:02:13| B*44:02:14| B*44:02:15| B*44:02:16| B*44:02:17| B*44:02:18| B*44:02:19| B*44:02:20| B*44:02:21| B*44:02:22| B*44:02:23| B*44:02:24| B*44:02:25| B*44:02:26| B*44:02:27| B*44:02:28| B*44:02:29| B*44:02:30| B*44:02:31| B*44:02:32| B*44:02:33| B*44:02:34| B*44:02:35| B*44:02:36| B*44:02:37| B*44:02:38| B*44:02:39| B*44:02:40| B*44:02:41| B*44:02:42| B*44:02:43| B*44:02:44| B*44:02:45| B*44:02:46| B*44:02:47| B*44:02:48| B*44:02:49| B*44:02:50| B*44:02:51| B*44:02:52| B*44:02:53| B*44:02:54| B*44:02:55| B*44:02:56| B*44:02:57| B*44:02:58| B*44:03:01:01| B*44:03:01:02| B*44:03:01:03| B*44:03:01:04| B*44:03:01:05| B*44:03:01:06| B*44:03:01:07| B*44:03:01:08| B*44:03:01:09| B*44:03:01:10| B*44:03:01:11| B*44:03:01:12| B*44:03:01:13| B*44:03:01:14| B*44:03:01:15| B*44:03:01:16| B*44:03:02| B*44:03:03| B*44:03:04| B*44:03:05| B*44:03:06| B*44:03:07| B*44:03:08| B*44:03:09| B*44:03:10| B*44:03:11| B*44:03:12| B*44:03:13| B*44:03:14| B*44:03:15| B*44:03:16| B*44:03:17| B*44:03:18| B*44:03:19| B*44:03:20| B*44:03:21| B*44:03:22| B*44:03:23| B*44:03:24| B*44:03:25| B*44:03:26| B*44:03:27| B*44:03:28| B*44:03:29| B*44:03:30| B*44:03:31| B*44:03:32| B*44:03:33| B*44:03:34| B*44:03:35| B*44:03:36| B*44:03:37| B*44:03:38| B*44:03:39| B*44:03:40| B*44:03:41| B*44:03:42| B*44:03:43| B*44:03:44| B*44:03:45| B*44:03:46| B*44:03:47| B*44:03:48| B*44:04| B*44:05:01| B*44:05:02| B*44:05:03| B*44:05:04| B*44:06| B*44:07| B*44:08| B*44:10| B*44:11| B*44:12| B*44:13| B*44:14| B*44:17| B*44:18| B*44:20| B*44:21| B*44:22| B*44:24| B*44:25| B*44:26| B*44:27:01:01| B*44:27:01:02| B*44:27:02| B*44:27:03| B*44:28:01| B*44:28:02| B*44:29| B*44:30| B*44:31| B*44:32| B*44:33| B*44:34:01| B*44:34:02| B*44:35| B*44:36| B*44:37:01| B*44:37:02| B*44:38| B*44:39| B*44:40| B*44:41:01| B*44:41:02| B*44:43:01| B*44:43:02| B*44:44| B*44:45| B*44:47| B*44:48| B*44:49| B*44:50:01| B*44:50:02| B*44:51| B*44:53:01| B*44:53:02| B*44:54| B*44:55| B*44:57| B*44:59:01| B*44:59:02| B*44:60| B*44:62| B*44:63| B*44:64:01| B*44:64:02| B*44:65| B*44:66| B*44:67| B*44:68| B*44:69:01| B*44:69:02| B*44:70| B*44:71| B*44:72| B*44:73| B*44:74| B*44:75| B*44:76| B*44:77| B*44:78| B*44:79:01| B*44:79:02| B*44:80| B*44:81| B*44:82| B*44:83| B*44:84:01| B*44:84:02| B*44:85| B*44:86| B*44:87| B*44:88| B*44:89| B*44:90| B*44:91| B*44:92| B*44:93| B*44:94| B*44:95| B*44:96| B*44:97| B*44:98| B*44:99| B*44:100| B*44:101| B*44:102| B*44:103| B*44:104| B*44:105| B*44:106| B*44:107| B*44:109| B*44:110| B*44:111| B*44:112| B*44:113| B*44:114| B*44:115| B*44:116| B*44:117| B*44:118| B*44:119| B*44:120| B*44:121| B*44:122| B*44:123| B*44:124| B*44:125| B*44:126:01| B*44:126:02| B*44:127| B*44:128:01| B*44:128:02| B*44:129| B*44:130| B*44:131| B*44:132| B*44:133| B*44:134| B*44:135| B*44:136| B*44:137| B*44:138Q| B*44:139| B*44:140| B*44:141| B*44:142| B*44:143| B*44:144| B*44:145| B*44:146| B*44:147| B*44:148| B*44:150| B*44:151| B*44:152| B*44:153| B*44:154| B*44:155| B*44:156| B*44:157| B*44:158| B*44:159| B*44:160Q| B*44:161| B*44:162| B*44:163:01| B*44:163:02| B*44:164| B*44:165| B*44:166| B*44:167| B*44:168| B*44:169| B*44:170| B*44:172| B*44:173| B*44:174| B*44:175| B*44:176| B*44:177| B*44:178| B*44:179| B*44:180| B*44:181| B*44:182| B*44:183| B*44:184| B*44:185| B*44:186:01| B*44:186:02| B*44:187| B*44:188| B*44:189| B*44:190| B*44:191| B*44:192:01| B*44:192:02| B*44:192:03| B*44:193| B*44:194| B*44:196| B*44:197| B*44:199| B*44:200| B*44:201| B*44:202| B*44:203:01| B*44:203:02| B*44:204| B*44:205:01| B*44:205:02| B*44:206| B*44:207| B*44:208| B*44:209| B*44:210:01| B*44:210:02| B*44:211| B*44:212| B*44:213| B*44:214| B*44:215| B*44:216| B*44:218| B*44:219| B*44:220| B*44:221| B*44:222| B*44:223| B*44:224| B*44:225| B*44:226| B*44:227| B*44:228| B*44:229| B*44:230| B*44:231| B*44:232| B*44:233| B*44:234| B*44:235| B*44:236| B*44:238| B*44:239| B*44:240| B*44:241| B*44:242| B*44:243| B*44:244| B*44:245| B*44:247| B*44:248| B*44:249| B*44:250| B*44:251| B*44:252| B*44:253| B*44:254| B*44:255| B*44:256| B*44:257| B*44:258| B*44:259| B*44:260| B*44:261| B*44:262| B*44:263| B*44:264| B*44:265| B*44:266| B*44:268| B*44:269| B*44:270:01| B*44:270:02| B*44:271| B*44:272| B*44:273| B*44:274| B*44:275| B*44:276| B*44:277| B*44:278| B*44:279| B*44:280| B*44:281| B*44:282| B*44:283| B*44:284| B*44:285| B*44:286| B*44:287| B*44:288| B*44:289| B*44:290| B*44:291| B*44:292| B*44:293| B*44:294| B*44:295| B*44:296| B*44:297| B*44:298| B*44:299| B*44:300| B*44:301| B*44:302| B*44:304| B*44:305| B*44:307| B*44:308| B*44:311| B*44:312| B*44:313| B*44:315| B*44:316| B*44:317| B*44:318| B*44:319| B*44:320| B*44:321| B*44:322| B*44:323| B*44:324| B*44:325| B*44:326| B*44:327| B*44:329| B*44:330| B*44:331| B*44:332| B*51:42</t>
+  </si>
+  <si>
+    <t>B*44:09| B*45:01:01:01| B*45:01:01:02| B*45:01:02| B*45:01:03| B*45:01:04| B*45:01:05| B*45:02| B*45:03| B*45:05| B*45:06| B*45:07| B*45:08| B*45:09| B*45:10| B*45:11| B*45:12| B*45:13| B*45:14| B*45:15| B*45:16| B*45:17| B*45:18| B*45:19| B*45:20| B*45:21| B*45:22| B*45:23| B*45:24| B*50:02</t>
+  </si>
+  <si>
+    <t>B*46:01:01| B*46:01:02| B*46:01:03| B*46:01:04| B*46:01:05| B*46:01:06| B*46:01:07| B*46:01:08| B*46:01:09| B*46:01:10| B*46:01:11| B*46:01:12| B*46:01:13| B*46:01:14| B*46:01:15| B*46:01:16| B*46:01:17| B*46:01:18| B*46:01:19| B*46:01:20| B*46:01:21| B*46:01:22| B*46:01:23| B*46:01:24| B*46:01:25| B*46:02| B*46:03| B*46:04| B*46:05| B*46:06| B*46:08| B*46:09| B*46:10| B*46:12| B*46:13:01| B*46:13:02| B*46:13:03| B*46:14| B*46:16| B*46:17| B*46:18| B*46:19| B*46:20| B*46:21:01| B*46:21:02| B*46:22| B*46:23| B*46:24| B*46:25| B*46:26| B*46:27| B*46:28| B*46:29| B*46:30| B*46:31| B*46:32| B*46:33| B*46:34| B*46:35| B*46:36| B*46:37| B*46:38| B*46:39| B*46:40:01| B*46:40:02| B*46:42| B*46:43| B*46:44| B*46:45| B*46:46| B*46:47| B*46:48| B*46:49| B*46:50| B*46:51Q| B*46:52| B*46:53| B*46:54| B*46:56| B*46:57| B*46:58| B*46:59| B*46:60| B*46:61| B*46:62| B*46:63| B*46:64| B*46:65| B*46:66| B*46:67| B*46:68| B*46:69| B*46:70| B*46:71| B*46:72| B*46:73| B*46:74| B*46:75</t>
+  </si>
+  <si>
+    <t>B*40:19| B*44:16| B*47:01:01:02| B*47:01:01:03| B*47:01:02| B*47:01:03| B*47:03| B*47:04| B*47:06| B*47:07| B*47:08| B*47:09| B*47:10| B*49:07</t>
+  </si>
+  <si>
+    <t>B*40:12| B*48:01:01:01| B*48:01:01:02| B*48:01:02| B*48:01:03| B*48:01:04| B*48:01:05| B*48:01:06| B*48:01:07| B*48:02:01| B*48:02:02| B*48:02:03| B*48:03:01| B*48:03:02| B*48:04:01| B*48:04:02| B*48:05| B*48:06| B*48:07| B*48:08| B*48:09| B*48:10| B*48:11| B*48:12| B*48:13| B*48:14| B*48:15| B*48:16| B*48:17| B*48:18| B*48:19| B*48:20| B*48:21| B*48:22| B*48:23| B*48:24| B*48:25| B*48:26| B*48:27| B*48:28| B*48:29| B*48:30| B*48:31| B*48:32| B*48:33| B*48:34| B*48:35| B*48:36| B*48:37| B*48:38| B*48:39| B*48:40| B*48:41| B*48:42| B*48:43| B*48:44| B*48:45| B*48:46| B*48:47| B*48:48</t>
+  </si>
+  <si>
+    <t>B*49:01:01:01| B*49:01:01:02| B*49:01:01:03| B*49:01:01:04| B*49:01:02| B*49:01:03| B*49:01:04| B*49:01:05| B*49:01:06| B*49:01:07| B*49:01:08| B*49:01:09| B*49:01:10| B*49:01:11| B*49:01:12| B*49:01:13| B*49:02| B*49:03| B*49:04:01| B*49:04:02| B*49:05| B*49:06| B*49:08| B*49:09| B*49:10| B*49:11| B*49:12| B*49:13| B*49:14| B*49:16| B*49:17| B*49:18:01| B*49:18:02| B*49:20| B*49:21| B*49:22| B*49:23| B*49:24| B*49:25| B*49:26| B*49:27| B*49:28| B*49:29| B*49:30| B*49:31| B*49:32| B*49:33| B*49:34| B*49:35| B*49:36| B*49:37| B*49:38| B*49:39| B*49:40| B*49:41| B*49:42| B*49:43| B*49:44| B*49:45| B*49:46| B*49:47| B*49:48| B*49:49| B*49:50| B*49:51| B*49:52| B*49:53| B*49:54| B*49:55| B*49:56| B*49:57| B*49:58| B*49:59</t>
+  </si>
+  <si>
+    <t>B*51:16| B*15:23| B*51:01:01:01| B*51:01:01:02| B*51:01:01:03| B*51:01:01:04| B*51:01:01:05| B*51:01:01:06| B*51:01:01:07| B*51:01:01:08| B*51:01:01:09| B*51:01:01:10| B*51:01:01:11| B*51:01:01:12| B*51:01:01:13| B*51:01:01:14| B*51:01:01:15| B*51:01:01:16| B*51:01:01:17| B*51:01:01:18| B*51:01:01:19| B*51:01:01:20| B*51:01:01:21| B*51:01:01:22| B*51:01:01:23| B*51:01:01:24| B*51:01:01:25| B*51:01:01:26| B*51:01:01:27| B*51:01:01:28| B*51:01:01:29| B*51:01:01:30| B*51:01:01:31| B*51:01:01:32| B*51:01:02| B*51:01:03| B*51:01:04| B*51:01:05| B*51:01:06| B*51:01:07| B*51:01:08| B*51:01:09| B*51:01:10| B*51:01:11| B*51:01:12| B*51:01:13| B*51:01:14| B*51:01:15| B*51:01:16| B*51:01:17| B*51:01:18| B*51:01:19| B*51:01:20| B*51:01:21| B*51:01:22| B*51:01:23| B*51:01:24| B*51:01:25| B*51:01:26| B*51:01:27| B*51:01:28| B*51:01:29| B*51:01:30| B*51:01:31| B*51:01:32| B*51:01:33| B*51:01:34| B*51:01:35| B*51:01:36| B*51:01:37| B*51:01:38| B*51:01:39| B*51:01:40| B*51:01:41| B*51:01:42| B*51:01:43| B*51:01:44| B*51:01:45| B*51:01:46| B*51:01:47| B*51:01:48| B*51:01:49| B*51:01:50| B*51:01:51| B*51:01:52| B*51:01:53| B*51:01:54| B*51:01:55| B*51:01:56| B*51:01:57| B*51:01:58| B*51:01:59| B*51:01:60| B*51:01:61| B*51:01:62| B*51:01:63| B*51:01:64| B*51:01:65| B*51:01:66| B*51:01:67| B*51:01:68| B*51:01:69| B*51:01:70| B*51:03| B*51:04:01| B*51:04:02| B*51:05| B*51:06:01| B*51:06:02| B*51:06:03| B*51:06:04| B*51:07:01| B*51:07:02| B*51:08:01:01| B*51:08:01:02| B*51:08:02| B*51:08:03| B*51:09:01| B*51:09:02| B*51:09:03| B*51:10| B*51:12| B*51:13:01| B*51:13:02| B*51:14| B*51:15| B*51:17| B*51:18| B*51:19| B*51:20| B*51:21| B*51:22| B*51:23| B*51:24:01| B*51:24:02| B*51:24:03| B*51:24:04| B*51:24:05| B*51:26| B*51:28| B*51:29| B*51:30| B*51:31| B*51:32| B*51:33| B*51:34| B*51:35| B*51:36| B*51:37| B*51:38| B*51:39| B*51:40| B*51:43| B*51:45| B*51:46| B*51:48| B*51:49| B*51:50| B*51:51| B*51:52| B*51:53| B*51:54| B*51:55| B*51:56:01| B*51:56:02| B*51:56:03| B*51:57| B*51:58| B*51:59| B*51:60| B*51:61:01| B*51:61:02| B*51:62| B*51:63:01| B*51:63:02| B*51:64| B*51:65| B*51:66| B*51:67| B*51:68| B*51:69| B*51:70| B*51:71| B*51:72| B*51:73| B*51:74| B*51:75| B*51:76| B*51:77| B*51:78:01| B*51:78:02| B*51:79| B*51:80| B*51:81| B*51:82| B*51:83| B*51:84| B*51:85| B*51:86| B*51:87| B*51:88| B*51:89| B*51:90| B*51:91| B*51:92:01| B*51:92:02| B*51:93| B*51:94| B*51:95| B*51:96| B*51:97| B*51:99| B*51:100| B*51:101| B*51:102| B*51:103| B*51:104| B*51:105| B*51:106:01| B*51:106:02| B*51:107| B*51:108| B*51:109| B*51:111| B*51:112| B*51:113| B*51:114| B*51:115| B*51:116| B*51:117| B*51:119| B*51:120| B*51:121| B*51:122| B*51:123| B*51:124| B*51:125| B*51:126| B*51:127| B*51:128| B*51:129| B*51:130| B*51:131| B*51:132| B*51:133| B*51:134| B*51:135| B*51:136| B*51:137| B*51:138| B*51:139| B*51:140| B*51:141| B*51:142| B*51:143| B*51:144| B*51:145| B*51:146| B*51:147| B*51:148| B*51:150| B*51:151| B*51:152| B*51:153| B*51:154| B*51:155| B*51:156| B*51:157| B*51:158:01| B*51:158:02| B*51:159| B*51:160| B*51:161| B*51:162| B*51:163| B*51:164| B*51:165| B*51:166| B*51:167| B*51:168| B*51:169| B*51:170| B*51:171| B*51:172| B*51:173Q| B*51:174:01| B*51:174:02| B*51:175| B*51:176| B*51:177| B*51:179| B*51:180| B*51:181| B*51:182| B*51:183| B*51:185| B*51:186| B*51:187| B*51:188| B*51:189| B*51:190| B*51:191| B*51:192| B*51:193| B*51:194| B*51:195| B*51:196| B*51:197| B*51:198| B*51:199| B*51:200| B*51:201| B*51:202| B*51:203| B*51:204:01| B*51:204:02| B*51:205| B*51:206| B*51:207| B*51:208| B*51:209| B*51:210| B*51:211| B*51:212| B*51:213| B*51:214| B*51:215| B*51:216| B*51:217| B*51:218| B*51:219| B*51:220| B*51:221| B*51:222| B*51:223| B*51:224| B*51:225| B*51:226| B*51:227| B*51:228| B*51:229| B*51:230:01:01| B*51:230:01:02| B*51:231| B*51:232| B*51:233| B*51:234| B*51:236| B*51:237| B*51:238| B*51:239| B*51:240| B*51:241| B*51:242| B*51:243| B*51:244| B*51:246| B*51:247| B*51:248| B*51:249| B*51:250| B*51:251| B*51:252| B*51:253| B*51:254| B*51:255| B*51:257| B*51:258| B*51:259| B*51:260| B*51:261| B*51:262| B*51:263| B*51:265| B*51:266| B*51:267| B*52:01:01:01| B*52:01:01:02| B*52:01:01:03| B*52:01:01:04| B*52:01:01:05| B*52:01:01:06| B*52:01:02:01| B*52:01:02:02| B*52:01:02:03| B*52:01:03| B*52:01:04| B*52:01:05| B*52:01:06| B*52:01:07| B*52:01:08| B*52:01:09| B*52:01:10| B*52:01:11| B*52:01:12| B*52:01:13| B*52:01:14| B*52:01:15| B*52:01:16| B*52:01:17| B*52:01:18| B*52:01:19| B*52:01:20| B*52:01:21| B*52:01:22| B*52:01:23| B*52:01:24| B*52:01:25| B*52:01:26| B*52:01:27| B*52:01:28| B*52:01:29| B*52:01:30| B*52:01:31| B*52:01:32| B*52:01:33| B*52:01:34| B*52:01:35| B*52:01:36| B*52:02:01| B*52:02:02| B*52:03| B*52:04| B*52:05| B*52:06:01| B*52:06:02| B*52:06:03| B*52:07| B*52:08| B*52:09:01| B*52:09:02| B*52:10:01| B*52:10:02| B*52:10:03| B*52:11| B*52:12| B*52:13| B*52:14:01| B*52:14:02| B*52:15| B*52:16| B*52:17| B*52:18| B*52:19| B*52:20| B*52:21:01| B*52:21:02| B*52:22| B*52:23| B*52:24| B*52:25:01| B*52:25:02| B*52:26| B*52:27| B*52:28| B*52:29| B*52:30| B*52:31:01| B*52:31:02| B*52:32| B*52:33| B*52:34| B*52:35| B*52:36| B*52:37| B*52:38| B*52:39| B*52:40| B*52:41| B*52:42| B*52:43| B*52:44| B*52:45| B*52:46| B*52:47| B*52:48| B*52:50| B*52:51| B*52:52| B*52:53| B*52:54| B*52:55| B*52:56| B*52:57| B*52:58| B*52:59| B*52:60| B*52:61| B*52:62| B*52:63| B*52:64| B*52:65| B*52:66| B*52:67| B*52:68| B*52:69| B*52:70| B*52:71| B*52:72| B*52:73| B*52:74| B*52:75| B*52:76| B*52:77| B*52:78| B*52:79| B*52:80| B*52:81| B*52:82| B*52:83| B*52:84| B*56:06| B*78:01:01:01| B*78:01:01:02| B*78:01:02| B*78:02:01| B*78:02:02| B*78:03| B*78:05| B*78:06| B*78:07| B*78:08| B*78:09| B*78:10</t>
+  </si>
+  <si>
+    <t>B*15:46| B*50:01:01:01| B*50:01:01:02| B*50:01:02| B*50:01:03| B*50:01:04| B*50:01:05| B*50:01:06| B*50:01:07| B*50:01:08| B*50:01:09| B*50:01:10| B*50:04| B*50:05| B*50:06| B*50:07| B*50:08| B*50:09| B*50:10| B*50:11| B*50:12| B*50:13| B*50:14| B*50:15| B*50:16| B*50:17| B*50:18| B*50:19| B*50:20| B*50:31| B*50:32| B*50:33| B*50:34| B*50:35| B*50:36| B*50:37| B*50:38| B*50:39| B*50:40| B*50:41| B*50:42| B*50:43| B*50:44| B*50:45| B*50:46| B*50:47| B*50:48| B*50:49| B*50:50| B*50:51| B*50:52| B*50:53| B*50:54| B*50:55| B*50:56| B*50:57| B*50:58| B*50:59| B*50:60| B*50:61| B*40:05:01:01| B*40:05:01:02</t>
+  </si>
+  <si>
+    <t>B*15:23| B*51:01:01:01| B*51:01:01:02| B*51:01:01:03| B*51:01:01:04| B*51:01:01:05| B*51:01:01:06| B*51:01:01:07| B*51:01:01:08| B*51:01:01:09| B*51:01:01:10| B*51:01:01:11| B*51:01:01:12| B*51:01:01:13| B*51:01:01:14| B*51:01:01:15| B*51:01:01:16| B*51:01:01:17| B*51:01:01:18| B*51:01:01:19| B*51:01:01:20| B*51:01:01:21| B*51:01:01:22| B*51:01:01:23| B*51:01:01:24| B*51:01:01:25| B*51:01:01:26| B*51:01:01:27| B*51:01:01:28| B*51:01:01:29| B*51:01:01:30| B*51:01:01:31| B*51:01:01:32| B*51:01:02| B*51:01:03| B*51:01:04| B*51:01:05| B*51:01:06| B*51:01:07| B*51:01:08| B*51:01:09| B*51:01:10| B*51:01:11| B*51:01:12| B*51:01:13| B*51:01:14| B*51:01:15| B*51:01:16| B*51:01:17| B*51:01:18| B*51:01:19| B*51:01:20| B*51:01:21| B*51:01:22| B*51:01:23| B*51:01:24| B*51:01:25| B*51:01:26| B*51:01:27| B*51:01:28| B*51:01:29| B*51:01:30| B*51:01:31| B*51:01:32| B*51:01:33| B*51:01:34| B*51:01:35| B*51:01:36| B*51:01:37| B*51:01:38| B*51:01:39| B*51:01:40| B*51:01:41| B*51:01:42| B*51:01:43| B*51:01:44| B*51:01:45| B*51:01:46| B*51:01:47| B*51:01:48| B*51:01:49| B*51:01:50| B*51:01:51| B*51:01:52| B*51:01:53| B*51:01:54| B*51:01:55| B*51:01:56| B*51:01:57| B*51:01:58| B*51:01:59| B*51:01:60| B*51:01:61| B*51:01:62| B*51:01:63| B*51:01:64| B*51:01:65| B*51:01:66| B*51:01:67| B*51:01:68| B*51:01:69| B*51:01:70| B*51:03| B*51:04:01| B*51:04:02| B*51:05| B*51:06:01| B*51:06:02| B*51:06:03| B*51:06:04| B*51:07:01| B*51:07:02| B*51:08:01:01| B*51:08:01:02| B*51:08:02| B*51:08:03| B*51:09:01| B*51:09:02| B*51:09:03| B*51:10| B*51:12| B*51:13:01| B*51:13:02| B*51:14| B*51:15| B*51:17| B*51:18| B*51:19| B*51:20| B*51:21| B*51:22| B*51:23| B*51:24:01| B*51:24:02| B*51:24:03| B*51:24:04| B*51:24:05| B*51:26| B*51:28| B*51:29| B*51:30| B*51:31| B*51:32| B*51:33| B*51:34| B*51:35| B*51:36| B*51:37| B*51:38| B*51:39| B*51:40| B*51:43| B*51:45| B*51:46| B*51:48| B*51:49| B*51:50| B*51:51| B*51:52| B*51:53| B*51:54| B*51:55| B*51:56:01| B*51:56:02| B*51:56:03| B*51:57| B*51:58| B*51:59| B*51:60| B*51:61:01| B*51:61:02| B*51:62| B*51:63:01| B*51:63:02| B*51:64| B*51:65| B*51:66| B*51:67| B*51:68| B*51:69| B*51:70| B*51:71| B*51:72| B*51:73| B*51:74| B*51:75| B*51:76| B*51:77| B*51:78:01| B*51:78:02| B*51:79| B*51:80| B*51:81| B*51:82| B*51:83| B*51:84| B*51:85| B*51:86| B*51:87| B*51:88| B*51:89| B*51:90| B*51:91| B*51:92:01| B*51:92:02| B*51:93| B*51:94| B*51:95| B*51:96| B*51:97| B*51:99| B*51:100| B*51:101| B*51:102| B*51:103| B*51:104| B*51:105| B*51:106:01| B*51:106:02| B*51:107| B*51:108| B*51:109| B*51:111| B*51:112| B*51:113| B*51:114| B*51:115| B*51:116| B*51:117| B*51:119| B*51:120| B*51:121| B*51:122| B*51:123| B*51:124| B*51:125| B*51:126| B*51:127| B*51:128| B*51:129| B*51:130| B*51:131| B*51:132| B*51:133| B*51:134| B*51:135| B*51:136| B*51:137| B*51:138| B*51:139| B*51:140| B*51:141| B*51:142| B*51:143| B*51:144| B*51:145| B*51:146| B*51:147| B*51:148| B*51:150| B*51:151| B*51:152| B*51:153| B*51:154| B*51:155| B*51:156| B*51:157| B*51:158:01| B*51:158:02| B*51:159| B*51:160| B*51:161| B*51:162| B*51:163| B*51:164| B*51:165| B*51:166| B*51:167| B*51:168| B*51:169| B*51:170| B*51:171| B*51:172| B*51:173Q| B*51:174:01| B*51:174:02| B*51:175| B*51:176| B*51:177| B*51:179| B*51:180| B*51:181| B*51:182| B*51:183| B*51:185| B*51:186| B*51:187| B*51:188| B*51:189| B*51:190| B*51:191| B*51:192| B*51:193| B*51:194| B*51:195| B*51:196| B*51:197| B*51:198| B*51:199| B*51:200| B*51:201| B*51:202| B*51:203| B*51:204:01| B*51:204:02| B*51:205| B*51:206| B*51:207| B*51:208| B*51:209| B*51:210| B*51:211| B*51:212| B*51:213| B*51:214| B*51:215| B*51:216| B*51:217| B*51:218| B*51:219| B*51:220| B*51:221| B*51:222| B*51:223| B*51:224| B*51:225| B*51:226| B*51:227| B*51:228| B*51:229| B*51:230:01:01| B*51:230:01:02| B*51:231| B*51:232| B*51:233| B*51:234| B*51:236| B*51:237| B*51:238| B*51:239| B*51:240| B*51:241| B*51:242| B*51:243| B*51:244| B*51:246| B*51:247| B*51:248| B*51:249| B*51:250| B*51:251| B*51:252| B*51:253| B*51:254| B*51:255| B*51:257| B*51:258| B*51:259| B*51:260| B*51:261| B*51:262| B*51:263| B*51:265| B*51:266| B*51:267</t>
+  </si>
+  <si>
+    <t>B*51:02:01:01| B*51:02:01:02| B*51:02:02| B*51:02:03| B*51:02:04| B*51:02:05| B*51:02:06</t>
+  </si>
+  <si>
+    <t>B*52:01:01:01| B*52:01:01:02| B*52:01:01:03| B*52:01:01:04| B*52:01:01:05| B*52:01:01:06| B*52:01:02:01| B*52:01:02:02| B*52:01:02:03| B*52:01:03| B*52:01:04| B*52:01:05| B*52:01:06| B*52:01:07| B*52:01:08| B*52:01:09| B*52:01:10| B*52:01:11| B*52:01:12| B*52:01:13| B*52:01:14| B*52:01:15| B*52:01:16| B*52:01:17| B*52:01:18| B*52:01:19| B*52:01:20| B*52:01:21| B*52:01:22| B*52:01:23| B*52:01:24| B*52:01:25| B*52:01:26| B*52:01:27| B*52:01:28| B*52:01:29| B*52:01:30| B*52:01:31| B*52:01:32| B*52:01:33| B*52:01:34| B*52:01:35| B*52:01:36| B*52:02:01| B*52:02:02| B*52:03| B*52:04| B*52:05| B*52:06:01| B*52:06:02| B*52:06:03| B*52:07| B*52:08| B*52:09:01| B*52:09:02| B*52:10:01| B*52:10:02| B*52:10:03| B*52:11| B*52:12| B*52:13| B*52:14:01| B*52:14:02| B*52:15| B*52:16| B*52:17| B*52:18| B*52:19| B*52:20| B*52:21:01| B*52:21:02| B*52:22| B*52:23| B*52:24| B*52:25:01| B*52:25:02| B*52:26| B*52:27| B*52:28| B*52:29| B*52:30| B*52:31:01| B*52:31:02| B*52:32| B*52:33| B*52:34| B*52:35| B*52:36| B*52:37| B*52:38| B*52:39| B*52:40| B*52:41| B*52:42| B*52:43| B*52:44| B*52:45| B*52:46| B*52:47| B*52:48| B*52:50| B*52:51| B*52:52| B*52:53| B*52:54| B*52:55| B*52:56| B*52:57| B*52:58| B*52:59| B*52:60| B*52:61| B*52:62| B*52:63| B*52:64| B*52:65| B*52:66| B*52:67| B*52:68| B*52:69| B*52:70| B*52:71| B*52:72| B*52:73| B*52:74| B*52:75| B*52:76| B*52:77| B*52:78| B*52:79| B*52:80| B*52:81| B*52:82| B*52:83| B*52:84</t>
+  </si>
+  <si>
+    <t>B*53:01:01:01| B*53:01:01:02| B*53:01:02| B*53:01:03| B*53:01:04| B*53:01:05| B*53:01:06| B*53:01:07| B*53:01:08| B*53:01:09| B*53:01:10| B*53:01:11| B*53:01:12| B*53:01:13| B*53:01:14| B*53:01:15| B*53:01:16| B*53:01:17| B*53:01:18| B*53:01:19| B*53:01:20| B*53:02| B*53:03| B*53:04| B*53:05:01| B*53:05:02| B*53:06| B*53:07| B*53:08:01| B*53:08:02| B*53:09| B*53:10| B*53:11| B*53:12| B*53:13| B*53:14| B*53:15| B*53:16| B*53:17:01| B*53:17:02| B*53:18| B*53:19| B*53:20| B*53:21| B*53:22| B*53:23| B*53:24| B*53:25| B*53:26| B*53:27| B*53:28| B*53:29| B*53:30| B*53:31| B*53:32| B*53:33| B*53:34| B*53:35| B*53:36| B*53:37| B*53:38| B*53:39| B*53:40| B*53:41| B*53:42| B*53:43| B*53:44| B*53:45| B*53:46| B*53:47| B*53:49| B*53:50| B*53:51| B*53:52| B*53:53</t>
+  </si>
+  <si>
+    <t>B*54:01:01| B*54:01:02| B*54:01:03| B*54:01:04| B*54:01:05| B*54:01:06| B*54:01:07| B*54:02| B*54:04| B*54:06| B*54:07| B*54:09| B*54:10| B*54:11| B*54:12| B*54:13| B*54:14| B*54:15| B*54:16| B*54:17| B*54:18| B*54:19| B*54:20| B*54:21| B*54:22| B*54:23| B*54:24| B*54:25| B*54:26| B*54:27| B*54:28| B*54:29| B*54:30| B*54:31| B*54:32| B*54:33| B*54:34| B*54:35| B*54:36| B*54:37| B*54:38| B*55:07</t>
+  </si>
+  <si>
+    <t>B*55:01:01:01| B*55:01:01:02| B*55:01:02| B*55:01:03| B*55:01:04| B*55:01:05| B*55:01:06| B*55:01:07| B*55:01:08| B*55:01:09| B*55:01:10| B*55:01:11| B*55:01:12| B*55:01:13| B*55:01:14| B*55:01:15| B*55:01:16| B*55:02:01:01| B*55:02:01:02| B*55:02:01:03| B*55:02:02| B*55:02:03| B*55:02:04| B*55:02:05| B*55:02:06| B*55:02:07| B*55:02:08| B*55:02:09| B*55:02:10| B*55:03| B*55:04| B*55:10| B*55:11| B*55:13| B*55:14| B*55:15| B*55:17| B*55:18| B*55:19| B*55:21| B*55:22| B*55:23| B*55:24| B*55:25| B*55:26| B*55:27| B*55:28| B*55:29| B*55:30| B*55:31| B*55:32| B*55:33| B*55:34| B*55:35| B*55:36| B*55:37| B*55:38| B*55:39| B*55:40| B*55:41| B*55:42| B*55:43| B*55:44| B*55:45| B*55:46| B*55:47| B*55:48| B*55:49| B*55:50| B*55:51| B*55:52| B*55:53| B*55:54| B*55:56| B*55:57| B*55:58| B*55:59| B*55:60| B*55:61| B*55:62| B*55:63| B*55:64| B*55:65| B*55:66| B*55:67| B*55:68| B*55:69| B*55:70| B*55:71| B*55:72| B*55:73| B*55:74| B*55:75| B*55:76| B*55:77| B*55:78| B*55:79| B*55:80| B*55:81| B*55:82| B*55:84| B*55:85| B*55:86| B*55:87| B*55:88| B*55:90| B*55:91| B*55:92| B*55:93| B*55:94| B*55:95| B*55:96| B*56:10| B*56:12</t>
+  </si>
+  <si>
+    <t>B*55:08| B*56:01:01:01| B*56:01:01:02| B*56:01:01:03| B*56:01:01:04| B*56:01:01:06| B*56:01:01:07| B*56:01:02| B*56:01:03| B*56:01:04| B*56:01:05| B*56:01:06| B*56:01:07| B*56:01:08| B*56:01:09| B*56:01:10| B*56:01:11| B*56:01:12| B*56:01:13| B*56:01:14| B*56:01:15| B*56:02:01| B*56:02:02| B*56:04:01| B*56:04:02| B*56:07| B*56:08| B*56:09| B*56:11| B*56:13| B*56:14| B*56:15| B*56:16| B*56:17| B*56:18| B*56:20:01| B*56:20:02| B*56:21| B*56:22| B*56:23| B*56:24| B*56:25| B*56:26| B*56:27| B*56:29| B*56:30| B*56:31| B*56:32| B*56:33| B*56:34| B*56:35| B*56:36| B*56:37| B*56:39| B*56:40| B*56:41| B*56:42| B*56:43| B*56:44| B*56:45| B*56:46| B*56:47| B*56:48| B*56:49| B*56:50| B*56:51| B*56:52| B*56:53| B*56:54| B*56:55:01:02| B*56:56| B*56:57| B*56:58| B*56:59| B*56:60| B*56:61| B*56:62| B*56:63| B*56:64</t>
+  </si>
+  <si>
+    <t>B*57:01:01:01| B*57:01:01:02| B*57:01:01:03| B*57:01:01:04| B*57:01:02| B*57:01:03| B*57:01:04| B*57:01:05| B*57:01:06| B*57:01:07| B*57:01:08| B*57:01:09| B*57:01:10| B*57:01:11| B*57:01:12| B*57:01:13| B*57:01:14| B*57:01:15| B*57:01:16| B*57:01:17| B*57:01:18| B*57:01:19| B*57:01:20| B*57:01:21| B*57:01:22| B*57:01:23| B*57:01:24| B*57:01:25| B*57:01:26| B*57:01:27| B*57:01:28| B*57:01:29| B*57:01:30| B*57:01:31| B*57:01:32| B*57:01:33| B*57:01:34| B*57:01:35| B*57:01:36| B*57:02:01| B*57:02:02| B*57:03:01:01| B*57:03:01:02| B*57:03:01:03| B*57:03:02| B*57:03:03| B*57:03:04| B*57:04:01| B*57:04:02| B*57:04:03| B*57:05| B*57:06| B*57:07| B*57:08| B*57:09| B*57:10| B*57:11| B*57:12| B*57:13| B*57:14:01| B*57:14:02| B*57:15| B*57:16| B*57:17| B*57:18| B*57:19| B*57:20| B*57:21| B*57:22| B*57:23| B*57:24| B*57:25| B*57:26| B*57:27| B*57:29| B*57:30| B*57:31| B*57:32| B*57:33| B*57:34| B*57:35| B*57:36| B*57:37| B*57:38| B*57:39| B*57:40| B*57:41| B*57:42| B*57:43| B*57:44| B*57:45| B*57:46| B*57:47| B*57:48| B*57:49| B*57:50| B*57:51| B*57:52| B*57:53| B*57:54| B*57:55| B*57:56| B*57:57| B*57:58| B*57:59| B*57:60| B*57:61| B*57:62| B*57:63| B*57:64| B*57:65| B*57:66| B*57:67:01| B*57:67:02| B*57:68| B*57:69| B*57:70| B*57:71| B*57:72| B*57:73| B*57:74| B*57:75| B*57:76| B*57:77| B*57:78| B*57:80| B*57:81| B*57:82| B*57:83| B*57:84| B*57:85| B*57:86| B*57:87| B*57:88| B*57:89| B*57:90| B*57:91| B*57:92| B*57:93| B*57:94| B*57:95| B*57:96| B*57:97| B*57:98Q| B*57:99| B*57:100| B*57:101| B*57:102| B*57:103| B*57:104| B*57:105| B*57:106| B*57:107| B*57:108| B*57:109| B*57:110| B*57:111| B*57:112| B*57:113| B*57:114</t>
+  </si>
+  <si>
+    <t>B*58:01:01:01| B*58:01:01:02| B*58:01:01:03| B*58:01:01:04| B*58:01:01:05| B*58:01:02| B*58:01:03| B*58:01:04| B*58:01:05| B*58:01:06| B*58:01:07| B*58:01:08| B*58:01:09| B*58:01:10| B*58:01:11| B*58:01:12| B*58:01:13| B*58:01:14| B*58:01:15| B*58:01:16| B*58:01:17| B*58:01:18| B*58:01:19| B*58:01:20| B*58:01:21| B*58:01:22| B*58:01:23| B*58:01:24| B*58:01:25| B*58:01:26| B*58:01:27| B*58:01:28| B*58:01:29| B*58:01:30| B*58:01:31| B*58:02:01| B*58:02:02| B*58:04| B*58:05| B*58:06| B*58:07| B*58:11| B*58:12| B*58:13| B*58:14| B*58:15| B*58:16:01| B*58:16:02| B*58:18| B*58:19| B*58:20| B*58:21| B*58:22| B*58:23| B*58:24| B*58:25| B*58:26| B*58:27| B*58:28:01| B*58:28:02| B*58:29| B*58:32| B*58:33| B*58:34| B*58:35| B*58:36| B*58:37| B*58:38| B*58:40| B*58:41| B*58:42| B*58:43| B*58:44| B*58:45:01| B*58:45:02| B*58:46| B*58:47| B*58:48| B*58:49| B*58:50| B*58:51| B*58:52| B*58:53| B*58:54| B*58:55| B*58:56| B*58:57| B*58:58| B*58:59:01| B*58:59:02| B*58:60| B*58:61| B*58:62| B*58:63| B*58:64| B*58:65| B*58:66| B*58:67| B*58:68| B*58:69| B*58:70| B*58:71| B*58:73| B*58:74| B*58:75| B*58:76| B*58:77| B*58:78| B*58:79| B*58:80| B*58:81| B*58:82| B*58:83| B*58:84| B*58:85| B*58:86| B*58:87| B*58:88| B*58:89| B*58:90| B*58:91| B*58:92| B*58:95| B*58:96| B*58:97| B*58:98| B*58:99| B*58:100</t>
+  </si>
+  <si>
+    <t>B*59:01:01:01| B*59:01:01:02| B*59:02| B*59:03| B*59:04| B*59:05| B*59:06| B*59:07| B*59:08| B*59:09</t>
+  </si>
+  <si>
+    <t>B*40:01:01| B*40:01:02:01| B*40:01:02:02| B*40:01:02:03| B*40:01:02:04| B*40:01:02:05| B*40:01:02:06| B*40:01:02:07| B*40:01:02:08| B*40:01:02:09| B*40:01:03| B*40:01:04| B*40:01:05| B*40:01:06| B*40:01:07| B*40:01:08| B*40:01:09| B*40:01:10| B*40:01:11| B*40:01:12| B*40:01:13| B*40:01:14| B*40:01:15| B*40:01:16| B*40:01:17| B*40:01:18| B*40:01:19| B*40:01:20| B*40:01:21| B*40:01:22| B*40:01:23| B*40:01:24| B*40:01:25| B*40:01:26| B*40:01:27| B*40:01:28| B*40:01:29| B*40:01:30| B*40:01:31| B*40:01:32| B*40:01:33| B*40:01:34| B*40:01:35| B*40:01:36| B*40:01:37| B*40:01:38| B*40:01:39| B*40:01:40| B*40:01:41| B*40:01:42| B*40:01:43| B*40:01:44| B*40:01:45| B*40:01:46| B*40:01:47| B*40:01:48| B*40:01:49| B*40:01:50| B*40:01:51| B*40:01:52| B*40:01:53| B*40:01:54| B*40:01:55| B*40:01:56| B*40:01:57| B*40:01:58| B*40:01:59| B*40:01:60| B*40:07| B*40:10:01:01| B*40:10:01:02| B*40:10:02| B*40:14:01| B*40:14:02| B*40:14:03| B*40:30| B*40:31| B*40:33| B*40:34| B*40:36| B*40:38| B*40:42| B*40:43| B*40:45| B*40:46| B*40:48| B*40:49| B*40:52| B*40:54| B*40:55| B*40:61| B*40:62| B*40:63| B*40:65| B*40:66| B*40:67| B*40:69| B*40:72:01| B*40:72:02| B*40:73| B*40:74| B*40:76| B*40:77| B*47:02</t>
+  </si>
+  <si>
+    <t>B*40:02:01:01| B*40:02:01:02| B*40:02:01:03| B*40:02:01:04| B*40:02:01:05| B*40:02:01:06| B*40:02:01:07| B*40:02:01:08| B*40:02:02| B*40:02:03| B*40:02:04| B*40:02:05| B*40:02:06| B*40:02:07| B*40:02:08| B*40:02:09| B*40:02:10| B*40:02:11| B*40:02:12| B*40:02:13| B*40:02:14| B*40:02:15| B*40:02:16| B*40:02:17| B*40:02:18| B*40:02:19| B*40:02:20| B*40:02:21| B*40:02:22| B*40:02:23| B*40:02:24| B*40:02:25| B*40:02:26| B*40:03:01:01| B*40:03:01:02| B*40:04:01| B*40:04:02| B*40:06:01:01| B*40:06:01:02| B*40:06:02| B*40:06:03| B*40:06:04:01| B*40:06:04:02| B*40:06:05| B*40:06:06| B*40:06:07| B*40:06:08| B*40:06:09| B*40:06:10| B*40:06:11| B*40:06:12| B*40:06:13| B*40:06:14| B*40:06:15| B*40:06:16| B*40:06:17| B*40:06:18| B*40:08| B*40:09| B*40:11:01| B*40:11:02| B*40:16| B*40:18| B*40:20:01:01| B*40:20:01:02| B*40:24| B*40:27:01| B*40:27:02| B*40:29| B*40:35:01| B*40:35:02| B*40:37| B*40:40| B*40:44| B*40:50| B*40:53| B*40:56| B*40:57| B*40:70:01| B*40:70:02| B*40:71| B*40:75</t>
+  </si>
+  <si>
+    <t>B*15:01:01:01| B*15:01:01:03| B*15:01:01:04| B*15:01:01:05| B*15:01:01:06| B*15:01:01:07| B*15:01:01:08| B*15:01:01:09| B*15:01:01:10| B*15:01:01:11| B*15:01:01:12| B*15:01:01:13| B*15:01:01:14| B*15:01:01:15| B*15:01:01:16| B*15:01:01:17| B*15:01:01:18| B*15:01:01:19| B*15:01:01:20| B*15:01:02| B*15:01:03| B*15:01:04| B*15:01:06| B*15:01:07| B*15:01:08| B*15:01:09| B*15:01:10| B*15:01:11| B*15:01:12| B*15:01:13| B*15:01:14| B*15:01:15| B*15:01:16| B*15:01:17| B*15:01:18| B*15:01:19| B*15:01:20| B*15:01:21| B*15:01:22| B*15:01:23| B*15:01:24| B*15:01:25| B*15:01:26| B*15:01:27| B*15:01:28| B*15:01:29| B*15:01:30| B*15:01:31| B*15:01:32| B*15:01:33| B*15:01:34| B*15:01:35| B*15:01:36| B*15:01:37| B*15:01:38| B*15:01:39| B*15:01:40| B*15:01:41| B*15:01:42| B*15:01:43| B*15:01:44| B*15:01:45| B*15:01:46| B*15:01:47| B*15:01:48| B*15:01:49| B*15:01:50| B*15:01:51| B*15:01:52| B*15:01:53| B*15:01:54| B*15:01:55| B*15:04:01:01| B*15:04:01:02| B*15:04:02| B*15:04:03| B*15:04:04| B*15:05:01| B*15:05:02| B*15:05:03| B*15:06| B*15:07:01:01| B*15:07:01:02| B*15:07:02| B*15:07:03| B*15:15| B*15:20| B*15:24:01| B*15:24:02| B*15:25:01| B*15:25:02| B*15:25:03| B*15:25:04| B*15:27:01| B*15:27:02| B*15:27:03| B*15:27:04| B*15:28| B*15:30:01:01| B*15:30:01:02| B*15:32:01| B*15:32:02| B*15:34| B*15:35| B*15:38:01| B*15:38:02| B*15:39:01| B*15:39:02| B*15:40:01| B*15:40:02| B*15:45| B*15:48| B*15:50| B*15:56| B*15:57| B*15:58| B*15:60| B*15:63| B*15:65| B*15:66| B*15:70| B*15:71| B*15:73| B*15:75| B*15:77| B*15:81| B*15:82| B*15:83| B*15:84| B*15:85| B*15:92| B*15:96| B*15:97| B*15:102| B*15:107| B*15:146</t>
+  </si>
+  <si>
+    <t>B*15:16:01:01| B*15:16:01:02| B*15:16:01:03| B*15:16:02| B*15:16:03| B*15:17:01:01| B*15:17:01:02| B*15:17:02| B*15:17:03| B*15:17:04| B*15:17:05| B*15:17:06| B*15:17:07| B*15:67| B*15:95</t>
+  </si>
+  <si>
+    <t>B*14:01:01:01| B*14:01:01:02| B*14:01:01:03| B*14:01:02| B*14:01:03| B*14:01:04| B*14:01:05| B*14:01:06| B*14:01:07| B*14:01:08| B*14:01:09</t>
+  </si>
+  <si>
+    <t>B*14:02:01:01| B*14:02:01:02| B*14:02:01:03| B*14:02:01:04| B*14:02:01:05| B*14:02:01:06| B*14:02:02| B*14:02:03| B*14:02:04| B*14:02:05| B*14:02:06| B*14:02:07| B*14:02:08| B*14:02:09| B*14:02:10| B*14:02:11| B*14:02:12| B*14:02:13| B*14:02:14| B*14:02:15| B*14:02:16| B*14:02:17| B*14:02:18| B*14:02:19| B*14:02:20| B*14:02:21</t>
+  </si>
+  <si>
+    <t>B*67:01:01| B*67:01:02| B*67:01:03| B*67:02| B*67:03| B*67:04| B*67:05| B*67:06| B*67:07</t>
+  </si>
+  <si>
+    <t>B*07:02:01:01| B*07:02:01:02| B*07:02:01:03| B*07:02:01:04| B*07:02:01:05| B*07:02:01:06| B*07:02:01:07| B*07:02:01:08| B*07:02:01:09| B*07:02:01:10| B*07:02:01:11| B*07:02:01:12| B*07:02:01:13| B*07:02:01:14| B*07:02:02| B*07:02:03| B*07:02:04| B*07:02:05| B*07:02:06| B*07:02:07| B*07:02:08| B*07:02:09| B*07:02:10| B*07:02:11| B*07:02:12| B*07:02:13| B*07:02:14| B*07:02:15| B*07:02:16| B*07:02:17| B*07:02:18| B*07:02:19| B*07:02:20| B*07:02:21| B*07:02:22| B*07:02:23| B*07:02:24| B*07:02:25| B*07:02:26| B*07:02:27| B*07:02:28| B*07:02:29| B*07:02:30| B*07:02:31| B*07:02:32| B*07:02:33| B*07:02:34| B*07:02:35| B*07:02:36| B*07:02:37| B*07:02:38| B*07:02:39| B*07:02:40| B*07:02:41| B*07:02:42| B*07:02:43| B*07:02:44| B*07:02:45| B*07:02:46| B*07:02:47| B*07:02:48| B*07:02:49| B*07:02:50| B*07:02:51| B*07:02:52| B*07:02:53| B*07:02:54| B*07:02:55| B*07:02:56| B*07:02:57| B*07:02:58| B*07:02:59| B*07:02:60| B*07:02:61| B*07:02:62| B*07:02:63| B*07:02:64| B*07:02:65| B*07:02:66| B*07:02:67| B*07:02:68| B*07:02:69| B*07:02:70| B*07:02:71| B*07:02:72| B*07:02:73| B*07:03| B*07:04:01| B*07:04:02| B*07:05:01:01| B*07:05:01:02| B*07:05:01:03| B*07:05:01:04| B*07:05:02| B*07:05:03| B*07:05:04| B*07:05:05| B*07:05:06| B*07:05:07| B*07:05:08| B*07:05:09| B*07:06:01| B*07:06:02| B*07:06:03| B*07:07:01| B*07:07:02| B*07:08:01| B*07:08:02| B*07:09:01| B*07:09:02| B*07:10| B*07:11| B*07:12| B*07:13| B*07:14| B*07:15| B*07:16| B*07:17| B*07:18:01| B*07:18:02| B*07:19| B*07:20| B*07:21| B*07:22:01| B*07:22:02| B*07:23| B*07:24| B*07:25| B*07:26| B*07:27| B*07:28| B*07:29| B*07:30| B*07:31| B*07:32| B*07:33:01| B*07:33:02| B*07:33:03| B*07:34| B*07:35| B*07:36| B*07:37:01| B*07:37:02| B*07:38| B*07:39| B*07:40| B*07:41| B*07:42| B*07:43| B*07:45| B*07:46| B*07:47| B*07:48| B*07:50| B*07:51| B*07:52| B*07:53| B*07:54| B*07:55| B*07:56:01| B*07:56:02| B*07:57| B*07:58| B*07:59| B*07:60| B*07:61| B*07:62| B*07:63| B*07:64| B*07:65| B*07:66| B*07:68:01| B*07:68:02| B*07:68:03| B*07:69| B*07:70| B*07:71| B*07:72| B*07:73| B*07:74| B*07:75:01:01| B*07:75:01:02| B*07:76| B*07:77| B*07:78| B*07:79| B*07:80| B*07:81| B*07:82| B*07:83| B*07:84| B*07:85:01| B*07:85:02| B*07:86| B*07:87| B*07:88| B*07:89| B*07:90| B*07:91| B*07:92| B*07:93| B*07:94| B*07:95| B*07:96:01| B*07:96:02| B*07:97| B*07:98| B*07:99| B*07:100| B*07:101| B*07:102| B*07:103| B*07:104| B*07:105| B*07:106| B*07:107| B*07:108| B*07:109| B*07:110| B*07:112| B*07:113| B*07:114| B*07:115| B*07:116| B*07:117| B*07:118| B*07:119| B*07:120| B*07:121| B*07:122| B*07:123| B*07:124| B*07:125| B*07:126| B*07:127| B*07:128| B*07:129| B*07:130| B*07:131| B*07:132| B*07:133| B*07:134| B*07:136:01| B*07:136:02| B*07:137| B*07:138| B*07:139:01| B*07:139:02| B*07:140| B*07:141| B*07:142| B*07:143| B*07:144| B*07:145| B*07:146| B*07:147| B*07:148| B*07:149| B*07:150| B*07:151:01| B*07:151:02| B*07:152| B*07:153| B*07:154| B*07:155| B*07:156| B*07:157| B*07:158| B*07:159| B*07:160| B*07:162| B*07:163| B*07:164| B*07:165| B*07:166| B*07:168| B*07:169| B*07:170| B*07:171| B*07:172| B*07:173| B*07:174| B*07:175| B*07:176| B*07:177| B*07:178| B*07:179| B*07:180| B*07:183| B*07:184| B*07:185| B*07:186| B*07:187| B*07:188| B*07:189| B*07:190| B*07:191| B*07:192| B*07:193| B*07:194| B*07:195| B*07:196| B*07:197| B*07:198| B*07:199| B*07:200| B*07:202| B*07:203| B*07:204| B*07:205| B*07:206| B*07:207| B*07:208| B*07:209| B*07:210| B*07:211| B*07:212| B*07:213| B*07:214| B*07:215| B*07:216| B*07:217| B*07:218| B*07:219| B*07:220| B*07:221| B*07:222| B*07:223| B*07:224| B*07:225| B*07:226| B*07:227| B*07:228:01| B*07:228:02| B*07:229| B*07:230| B*07:232| B*07:233| B*07:234| B*07:235| B*07:236| B*07:237| B*07:238| B*07:239| B*07:240| B*07:241| B*07:242| B*07:243| B*07:244| B*07:245| B*07:246| B*07:247| B*07:248| B*07:249| B*07:250| B*07:252| B*07:253| B*07:254| B*07:255| B*07:256| B*07:257| B*07:258| B*07:259| B*07:260| B*07:261| B*07:262| B*07:263| B*07:264| B*07:265| B*07:266| B*07:267| B*07:268| B*07:269| B*07:270| B*07:271| B*07:273| B*07:274| B*07:275| B*07:276:01| B*07:276:02| B*07:277| B*07:278| B*07:279| B*07:280| B*07:281| B*07:282| B*07:283| B*07:284| B*07:286| B*07:287| B*07:288| B*07:289| B*07:290| B*07:291| B*07:292| B*07:293| B*07:294| B*07:295| B*07:296| B*07:297| B*07:298| B*07:299| B*07:300| B*07:301| B*07:302| B*07:303:01| B*07:303:02| B*07:304| B*07:305| B*07:306| B*07:307| B*07:308| B*07:309| B*07:310| B*07:311| B*07:312| B*07:313| B*07:314| B*07:317| B*07:319| B*07:320| B*07:321| B*07:322| B*07:323| B*07:324| B*07:326| B*07:327| B*07:328| B*07:329| B*07:331| B*07:332| B*07:333| B*07:334| B*07:335| B*07:336| B*07:337| B*07:338| B*07:339| B*07:340| B*07:341| B*07:342| B*07:344| B*07:345| B*07:346| B*07:347| B*07:348| B*07:349| B*07:350| B*07:352| B*07:353| B*07:354| B*07:355| B*07:356| B*07:357| B*07:358| B*56:05:01| B*56:05:02</t>
+  </si>
+  <si>
+    <t>B*15:09:01| B*15:09:02| B*15:29| B*15:37| B*15:47:01| B*15:47:02| B*15:51| B*15:80| B*15:103| B*15:114| B*15:220:01:01| B*15:220:01:02| B*15:10:01| B*15:10:02| B*15:10:03| B*15:10:04| B*15:18:01:01| B*15:18:01:02| B*15:18:01:03| B*15:18:01:04| B*15:18:01:05| B*15:18:02| B*15:18:03| B*15:18:04| B*15:18:05| B*15:18:06| B*15:18:07| B*15:64:01| B*15:64:02| B*15:72| B*15:90| B*15:93| B*15:99| B*15:108| B*15:03:01:01| B*15:03:01:02| B*15:03:01:03| B*15:03:02| B*15:03:03| B*15:03:04| B*15:03:05| B*15:03:06| B*15:03:07| B*15:03:08| B*15:49| B*15:54| B*15:61| B*15:69| B*15:74| B*15:98</t>
+  </si>
+  <si>
+    <t>B*15:10:01| B*15:10:02| B*15:10:03| B*15:10:04| B*15:18:01:01| B*15:18:01:02| B*15:18:01:03| B*15:18:01:04| B*15:18:01:05| B*15:18:02| B*15:18:03| B*15:18:04| B*15:18:05| B*15:18:06| B*15:18:07| B*15:64:01| B*15:64:02| B*15:72| B*15:90| B*15:93| B*15:99| B*15:108</t>
+  </si>
+  <si>
+    <t>B*15:03:01:01| B*15:03:01:02| B*15:03:01:03| B*15:03:02| B*15:03:03| B*15:03:04| B*15:03:05| B*15:03:06| B*15:03:07| B*15:03:08| B*15:49| B*15:54| B*15:61| B*15:69| B*15:74| B*15:98</t>
   </si>
   <si>
     <t>B*73:01| B*73:02</t>
   </si>
   <si>
-    <t>B*81:01| B*81:02| B*81:03| B*81:05| B*81:06| B*81:07| B*81:08</t>
-  </si>
-  <si>
-    <t>B*82:01| B*82:02| B*82:03</t>
-  </si>
-  <si>
-    <t>B*82:02| B*82:03| B*82:01</t>
+    <t>B*15:02:01:01| B*15:02:01:02| B*15:02:01:03| B*15:02:02| B*15:02:03| B*15:02:04| B*15:02:05| B*15:02:06| B*15:02:07| B*15:02:08| B*15:02:09| B*15:02:10| B*15:02:11| B*15:02:12| B*15:08:01| B*15:08:02| B*15:11:01| B*15:11:02| B*15:11:03| B*15:11:04| B*15:11:05| B*15:11:06| B*15:11:07| B*15:21:01:01| B*15:21:01:02| B*15:31| B*15:44| B*15:88</t>
+  </si>
+  <si>
+    <t>B*15:12:01| B*15:12:02| B*15:12:03| B*15:14| B*15:19</t>
+  </si>
+  <si>
+    <t>B*15:13:01| B*15:13:02| B*15:89</t>
+  </si>
+  <si>
+    <t>B*56:06| B*78:01:01:01| B*78:01:01:02| B*78:01:02| B*78:02:01| B*78:02:02| B*78:03| B*78:05| B*78:06| B*78:07| B*78:08| B*78:09| B*78:10</t>
+  </si>
+  <si>
+    <t>B*08:01:01:01| B*08:01:01:02| B*08:01:01:03| B*08:01:01:04| B*08:01:01:05| B*08:01:01:06| B*08:01:01:07| B*08:01:01:08| B*08:01:01:09| B*08:01:01:10| B*08:01:01:11| B*08:01:01:12| B*08:01:01:13| B*08:01:01:14| B*08:01:02| B*08:01:03| B*08:01:04| B*08:01:05| B*08:01:06| B*08:01:07| B*08:01:08| B*08:01:09| B*08:01:10| B*08:01:11| B*08:01:12| B*08:01:13| B*08:01:14| B*08:01:15| B*08:01:16| B*08:01:17| B*08:01:18| B*08:01:19| B*08:01:20| B*08:01:21| B*08:01:22| B*08:01:23| B*08:01:24| B*08:01:25| B*08:01:26| B*08:01:27| B*08:01:28| B*08:01:29| B*08:01:30| B*08:01:31| B*08:01:32| B*08:01:33| B*08:01:34| B*08:01:35| B*08:01:36| B*08:01:37| B*08:01:38| B*08:01:39| B*08:01:40| B*08:01:41| B*08:01:42| B*08:01:43| B*08:01:44| B*08:01:45| B*08:01:46| B*08:01:47| B*08:01:48| B*08:02| B*08:03| B*08:05| B*08:07| B*08:09| B*08:10| B*08:11| B*08:12:01| B*08:12:02| B*08:12:03| B*08:13| B*08:14| B*08:15| B*08:16| B*08:17| B*08:18| B*08:20:01| B*08:20:02| B*08:21| B*08:22| B*08:23| B*08:24| B*08:25| B*08:26:01| B*08:26:02| B*08:26:03| B*08:27| B*08:28| B*08:29| B*08:31| B*08:32| B*08:33| B*08:34| B*08:35| B*08:36| B*08:37| B*08:38:01| B*08:38:02| B*08:39| B*08:40| B*08:41| B*08:42| B*08:43| B*08:44| B*08:45| B*08:46| B*08:47| B*08:48| B*08:49| B*08:50| B*08:51| B*08:52| B*08:53:01| B*08:53:02| B*08:54:01| B*08:54:02| B*08:55| B*08:56:01| B*08:56:02| B*08:57| B*08:58| B*08:59:01| B*08:59:02| B*08:60| B*08:61| B*08:62| B*08:63| B*08:64| B*08:65| B*08:66| B*08:68| B*08:69| B*08:70| B*08:71| B*08:73| B*08:74| B*08:75| B*08:76| B*08:77| B*08:78| B*08:79| B*08:80| B*08:81| B*08:83| B*08:84| B*08:85| B*08:87| B*08:88| B*08:89| B*08:90| B*08:91| B*08:92| B*08:93| B*08:94| B*08:95| B*08:96| B*08:97| B*08:98| B*08:99| B*08:100| B*08:101| B*08:102| B*08:103| B*08:104| B*08:105| B*08:106| B*08:107| B*08:108| B*08:109| B*08:110| B*08:111| B*08:112| B*08:113| B*08:114| B*08:115| B*08:116| B*08:117| B*08:118| B*08:119| B*08:120| B*08:121| B*08:122| B*08:123| B*08:124| B*08:125| B*08:126| B*08:127| B*08:128| B*08:129| B*08:130| B*08:131| B*08:132| B*08:133| B*08:134| B*08:135| B*08:136| B*08:137| B*08:138| B*08:139| B*08:140| B*08:141| B*08:142| B*08:143| B*08:144| B*08:145| B*08:146| B*08:147| B*08:149| B*08:150| B*08:151| B*08:152| B*08:153| B*08:154| B*08:155| B*08:156| B*08:157| B*08:158| B*08:159| B*08:160| B*08:161| B*08:162| B*08:163| B*08:164| B*08:165| B*08:166| B*08:167| B*08:168| B*08:169| B*08:170| B*08:171| B*08:172| B*08:173| B*08:174| B*08:175| B*08:176| B*08:177| B*08:178| B*08:179| B*08:180| B*08:181| B*08:182| B*08:183| B*08:184| B*08:185| B*08:186| B*08:187| B*08:188| B*08:189| B*08:190| B*08:191| B*08:192| B*08:193| B*08:194| B*08:195| B*08:196| B*08:197| B*08:198| B*08:199| B*08:200| B*08:201| B*08:202| B*08:203| B*08:204| B*08:205| B*08:206| B*08:207| B*08:208| B*08:209| B*08:210| B*08:211| B*08:212| B*08:213| B*08:216| B*08:217| B*08:218| B*08:219| B*08:221| B*08:222| B*08:223| B*08:224</t>
+  </si>
+  <si>
+    <t>B*81:01:01| B*81:01:02| B*81:01:03| B*81:02| B*81:03| B*81:05| B*81:06| B*81:07| B*81:08</t>
+  </si>
+  <si>
+    <t>B*82:02:01:01| B*82:02:01:02| B*82:02:02| B*82:03| B*82:01:01:01| B*82:01:01:02| B*82:01:02</t>
   </si>
   <si>
     <t>B*83:01</t>
   </si>
   <si>
+    <t>C0</t>
+  </si>
+  <si>
     <t>C01</t>
   </si>
   <si>
-    <t>C0</t>
-  </si>
-  <si>
     <t>C02</t>
   </si>
   <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
     <t>C10</t>
   </si>
   <si>
-    <t>C09</t>
-  </si>
-  <si>
-    <t>C03</t>
-  </si>
-  <si>
-    <t>C04</t>
-  </si>
-  <si>
-    <t>C05</t>
-  </si>
-  <si>
-    <t>C06</t>
-  </si>
-  <si>
-    <t>C07</t>
-  </si>
-  <si>
-    <t>C08</t>
-  </si>
-  <si>
     <t>C12</t>
   </si>
   <si>
@@ -643,64 +643,91 @@
     <t>C18</t>
   </si>
   <si>
-    <t>C*01:02| C*01:03| C*01:04| C*01:05| C*01:06| C*01:07| C*01:08| C*01:09| C*01:10| C*01:11| C*01:12| C*01:13| C*01:14| C*01:15| C*01:16| C*01:17| C*01:18| C*01:19| C*01:20| C*01:21| C*01:22| C*01:23| C*01:24| C*01:25| C*01:26| C*01:27| C*01:28| C*01:29| C*01:30| C*01:31| C*01:32| C*01:33| C*01:34| C*01:35| C*01:36| C*01:38| C*01:39| C*01:40| C*01:41| C*01:42| C*01:43| C*01:44| C*01:45| C*01:46| C*01:47| C*01:48| C*01:49| C*01:50| C*01:51| C*01:52| C*01:53| C*01:54| C*01:55| C*01:57| C*01:58| C*01:59| C*01:60| C*01:61| C*01:62| C*01:63| C*01:64| C*01:65| C*01:66| C*01:67| C*01:68| C*01:70| C*01:71| C*01:72| C*01:73| C*01:74| C*01:75| C*01:76| C*01:77| C*01:78| C*01:79| C*01:80| C*01:81| C*01:82| C*01:83| C*01:84| C*01:85| C*01:87| C*01:88| C*01:90| C*01:91| C*01:92| C*01:93| C*01:94| C*01:95| C*01:96| C*01:97| C*01:99| C*01:100| C*01:101| C*01:102| C*01:103| C*01:104| C*01:105| C*01:106| C*01:107| C*01:108| C*01:110| C*01:112| C*01:113| C*01:114| C*01:115| C*01:116| C*01:118| C*01:119| C*01:120| C*01:121Q| C*01:122| C*01:123| C*01:124| C*01:125| C*01:126| C*01:127| C*01:128| C*01:129| C*01:130| C*01:131| C*01:132| C*01:133| C*01:134| C*01:135| C*01:136| C*01:138| C*01:139| C*01:140| C*01:141| C*01:142| C*01:144| C*01:146| C*01:147| C*01:148| C*14:02| C*14:03| C*14:05| C*14:08</t>
-  </si>
-  <si>
-    <t>C*01:37N| C*01:56N| C*01:69N| C*01:86N| C*01:89N| C*01:98N| C*01:109N| C*01:111N| C*01:117N| C*01:137N| C*01:143N| C*01:145N| C*02:38N| C*02:52N| C*02:92N| C*02:105N| C*02:121N| C*03:20N| C*03:121N| C*03:189N| C*03:201N| C*03:208N| C*03:224N| C*03:229N| C*03:265N| C*03:277N| C*03:316N| C*03:318N| C*03:323N| C*03:363N| C*03:366N| C*04:09N| C*04:88N| C*04:93N| C*04:95N| C*04:105N| C*04:115N| C*04:123N| C*04:170N| C*04:173N| C*04:191N| C*04:203N| C*04:205N| C*04:215N| C*04:217N| C*04:225N| C*04:233N| C*04:234N| C*04:236N| C*04:253N| C*04:255N| C*04:279N| C*05:07N| C*05:48N| C*05:91N| C*05:92N| C*05:99N| C*05:113N| C*05:128N| C*05:153N| C*05:154N| C*06:16N| C*06:46N| C*06:49N| C*06:79N| C*06:116N| C*06:128N| C*06:134N| C*06:152N| C*06:171N| C*06:175N| C*06:208N| C*06:211N| C*07:02N| C*07:32N| C*07:33N| C*07:55N| C*07:61N| C*07:98N| C*07:104N| C*07:152N| C*07:164N| C*07:191N| C*07:198N| C*07:227N| C*07:264N| C*07:329N| C*07:347N| C*07:350N| C*07:393N| C*07:437N| C*07:451N| C*07:452N| C*07:476N| C*07:483N| C*07:484N| C*07:491N| C*07:507N| C*07:551N| C*07:593N| C*07:600N| C*07:603N| C*08:26N| C*08:36N| C*08:52N| C*08:55N| C*08:88N| C*08:89N| C*08:121N| C*08:127N| C*08:129N| C*08:130N| C*12:39N| C*12:46N| C*12:80N| C*12:84N| C*12:104N| C*12:105N| C*12:148N| C*12:219N| C*14:07N| C*14:21N| C*14:35N| C*14:47N| C*15:02N| C*15:92N| C*15:95N| C*15:115N| C*15:122N| C*15:145N| C*16:30N| C*16:77N| C*16:89N| C*17:27N| C*18:07N</t>
-  </si>
-  <si>
-    <t>C*02:02| C*02:03| C*02:04| C*02:05| C*02:06| C*02:07| C*02:08| C*02:09| C*02:10| C*02:11| C*02:12| C*02:13| C*02:14| C*02:15| C*02:16| C*02:17| C*02:18| C*02:19| C*02:20| C*02:21| C*02:22| C*02:23| C*02:24| C*02:25Q| C*02:26| C*02:27| C*02:28| C*02:29| C*02:30| C*02:31| C*02:32| C*02:33| C*02:34| C*02:35| C*02:36| C*02:37| C*02:39| C*02:40| C*02:42| C*02:43| C*02:44| C*02:45| C*02:46| C*02:47| C*02:48| C*02:49| C*02:50| C*02:51| C*02:53| C*02:54| C*02:55| C*02:56| C*02:57| C*02:58| C*02:59| C*02:60| C*02:61| C*02:62| C*02:63| C*02:64| C*02:65| C*02:66| C*02:67Q| C*02:68| C*02:69| C*02:70| C*02:71| C*02:72| C*02:73| C*02:74| C*02:75| C*02:76| C*02:77| C*02:78| C*02:79| C*02:80| C*02:81| C*02:82| C*02:83| C*02:84| C*02:85| C*02:86| C*02:87| C*02:88| C*02:89| C*02:90| C*02:91| C*02:93| C*02:94| C*02:95| C*02:96| C*02:97| C*02:98| C*02:99| C*02:100| C*02:101| C*02:102| C*02:103| C*02:104| C*02:106| C*02:107| C*02:108| C*02:109| C*02:110| C*02:111| C*02:112| C*02:113| C*02:114| C*02:115| C*02:116| C*02:117| C*02:118| C*02:119| C*02:120| C*02:122| C*02:123| C*02:124| C*02:125| C*02:126| C*02:127| C*02:128| C*02:129| C*02:130| C*02:131| C*02:132| C*02:133| C*02:134</t>
-  </si>
-  <si>
-    <t>C*03:02| C*03:04| C*03:06| C*03:08| C*03:14| C*03:17| C*03:23| C*03:25| C*03:26| C*03:27| C*03:28| C*03:29| C*03:32| C*03:33| C*03:34| C*03:35| C*03:36| C*03:37| C*03:38| C*03:41| C*03:46</t>
-  </si>
-  <si>
-    <t>C*03:03| C*03:13| C*03:18| C*03:21| C*03:30| C*03:31</t>
-  </si>
-  <si>
-    <t>C*03:05| C*03:07| C*03:09| C*03:10| C*03:11| C*03:15| C*03:16| C*03:19| C*03:22Q| C*03:24| C*03:39| C*03:40| C*03:42| C*03:43| C*03:44| C*03:45| C*03:47| C*03:48| C*03:49| C*03:50| C*03:51| C*03:52| C*03:53| C*03:54| C*03:55| C*03:56| C*03:57| C*03:58| C*03:59| C*03:60| C*03:61| C*03:62| C*03:63| C*03:64| C*03:65| C*03:66| C*03:67| C*03:68| C*03:69| C*03:70| C*03:71| C*03:72| C*03:73| C*03:74| C*03:75| C*03:76| C*03:77| C*03:78| C*03:79| C*03:80| C*03:81| C*03:82| C*03:83| C*03:84| C*03:85| C*03:86| C*03:87| C*03:88| C*03:89| C*03:90| C*03:91| C*03:92| C*03:93| C*03:94| C*03:95| C*03:96| C*03:97| C*03:98| C*03:99| C*03:100| C*03:101| C*03:102| C*03:103| C*03:104| C*03:105| C*03:106| C*03:107| C*03:108| C*03:109| C*03:110| C*03:111| C*03:112| C*03:113| C*03:114| C*03:115| C*03:116| C*03:117| C*03:118| C*03:119| C*03:120| C*03:122| C*03:123| C*03:124| C*03:125| C*03:126| C*03:127| C*03:128| C*03:129| C*03:130| C*03:131| C*03:132| C*03:133| C*03:134| C*03:135| C*03:136| C*03:137| C*03:138| C*03:139| C*03:140| C*03:141| C*03:142| C*03:143| C*03:144| C*03:145| C*03:146| C*03:147| C*03:148| C*03:149| C*03:150| C*03:151| C*03:152| C*03:153| C*03:154| C*03:155| C*03:156| C*03:157| C*03:158| C*03:159| C*03:160| C*03:161| C*03:162| C*03:163| C*03:164| C*03:165| C*03:166| C*03:167| C*03:168| C*03:169Q| C*03:170| C*03:171| C*03:172| C*03:173| C*03:174| C*03:175| C*03:176| C*03:177| C*03:178| C*03:179| C*03:180| C*03:181| C*03:182| C*03:183| C*03:184| C*03:185| C*03:186| C*03:187| C*03:188| C*03:190| C*03:191| C*03:192| C*03:193| C*03:194| C*03:195| C*03:196| C*03:197| C*03:198| C*03:199| C*03:200| C*03:202| C*03:203| C*03:204| C*03:205| C*03:206| C*03:207| C*03:209| C*03:210| C*03:211| C*03:212| C*03:213| C*03:214| C*03:215| C*03:216| C*03:217| C*03:218| C*03:219| C*03:220| C*03:221| C*03:222| C*03:223| C*03:225| C*03:226| C*03:227| C*03:228| C*03:230| C*03:231| C*03:232| C*03:233| C*03:234| C*03:235| C*03:236| C*03:237| C*03:238| C*03:239| C*03:240| C*03:241| C*03:242| C*03:243| C*03:244Q| C*03:245| C*03:246| C*03:247| C*03:248| C*03:249| C*03:250| C*03:251| C*03:252| C*03:253| C*03:254| C*03:255| C*03:256| C*03:257| C*03:258| C*03:259| C*03:260| C*03:261| C*03:262| C*03:263| C*03:264| C*03:266| C*03:267| C*03:268| C*03:269| C*03:270| C*03:271| C*03:272| C*03:273| C*03:274| C*03:275| C*03:276| C*03:278| C*03:279| C*03:280| C*03:281| C*03:282| C*03:283| C*03:284| C*03:285| C*03:286| C*03:287| C*03:288| C*03:289| C*03:290| C*03:291| C*03:292| C*03:293| C*03:294| C*03:295| C*03:296| C*03:297| C*03:298| C*03:299| C*03:300| C*03:301| C*03:302| C*03:303| C*03:304| C*03:305| C*03:306| C*03:307| C*03:308| C*03:309| C*03:310| C*03:311| C*03:312| C*03:313| C*03:314| C*03:315| C*03:317| C*03:319| C*03:320| C*03:321| C*03:322| C*03:324| C*03:325| C*03:326| C*03:327| C*03:328| C*03:329| C*03:330| C*03:331| C*03:332| C*03:333| C*03:334| C*03:335| C*03:336| C*03:337| C*03:338| C*03:339| C*03:340| C*03:341| C*03:342| C*03:343| C*03:344| C*03:345| C*03:346| C*03:347| C*03:348| C*03:349| C*03:350| C*03:351| C*03:352| C*03:353| C*03:354| C*03:355| C*03:356| C*03:357| C*03:358| C*03:359| C*03:360| C*03:361| C*03:362| C*03:364| C*03:365| C*03:367| C*03:368| C*03:369| C*03:370| C*03:371| C*15:07| C*15:21| C*03:03| C*03:13| C*03:18| C*03:21| C*03:30| C*03:31| C*03:02| C*03:04| C*03:06| C*03:08| C*03:14| C*03:17| C*03:23| C*03:25| C*03:26| C*03:27| C*03:28| C*03:29| C*03:32| C*03:33| C*03:34| C*03:35| C*03:36| C*03:37| C*03:38| C*03:41| C*03:46</t>
-  </si>
-  <si>
-    <t>C*04:01| C*04:03| C*04:04| C*04:05| C*04:06| C*04:07| C*04:08| C*04:10| C*04:11| C*04:12| C*04:13| C*04:14| C*04:15| C*04:16| C*04:17| C*04:18| C*04:19| C*04:20| C*04:23| C*04:24| C*04:25| C*04:26| C*04:27| C*04:28| C*04:29| C*04:30| C*04:31| C*04:32| C*04:33| C*04:34| C*04:35| C*04:36| C*04:37| C*04:38| C*04:39| C*04:40| C*04:41| C*04:42| C*04:43| C*04:44| C*04:45| C*04:46| C*04:47| C*04:48| C*04:49| C*04:50| C*04:51| C*04:52| C*04:53| C*04:54| C*04:55| C*04:56| C*04:57| C*04:58| C*04:59Q| C*04:60| C*04:61| C*04:62| C*04:63| C*04:64| C*04:65| C*04:66| C*04:67| C*04:68| C*04:69| C*04:70| C*04:71| C*04:72| C*04:73| C*04:74| C*04:75| C*04:76| C*04:77| C*04:78| C*04:79| C*04:80| C*04:81| C*04:82| C*04:83| C*04:84| C*04:85| C*04:86| C*04:87| C*04:89| C*04:90| C*04:91| C*04:92| C*04:94| C*04:96| C*04:97| C*04:98| C*04:99| C*04:100| C*04:101| C*04:102| C*04:103| C*04:104| C*04:106| C*04:107| C*04:108| C*04:109| C*04:110| C*04:111| C*04:112| C*04:113| C*04:114| C*04:116| C*04:117| C*04:118| C*04:119| C*04:120| C*04:121| C*04:122| C*04:124| C*04:125| C*04:126| C*04:127| C*04:128| C*04:129| C*04:130| C*04:131| C*04:132| C*04:133| C*04:134| C*04:135| C*04:136| C*04:137| C*04:138| C*04:139| C*04:140| C*04:141| C*04:142| C*04:143| C*04:144| C*04:145| C*04:146| C*04:147| C*04:148| C*04:149| C*04:150| C*04:151| C*04:152| C*04:153| C*04:154| C*04:155| C*04:156| C*04:157| C*04:158| C*04:159| C*04:160| C*04:161| C*04:162| C*04:163| C*04:164| C*04:165| C*04:166| C*04:167| C*04:168| C*04:169| C*04:171| C*04:172| C*04:174| C*04:175| C*04:176| C*04:177| C*04:178| C*04:179| C*04:180| C*04:181| C*04:182| C*04:183| C*04:184| C*04:185| C*04:186| C*04:187| C*04:188| C*04:189| C*04:190| C*04:192| C*04:193| C*04:194| C*04:195| C*04:196| C*04:197| C*04:198| C*04:199| C*04:200| C*04:201| C*04:202| C*04:204| C*04:206| C*04:207| C*04:208| C*04:209| C*04:210| C*04:211| C*04:212| C*04:213| C*04:214| C*04:216| C*04:218| C*04:219| C*04:220| C*04:221| C*04:222| C*04:223| C*04:224| C*04:226| C*04:227| C*04:228| C*04:229| C*04:230| C*04:231| C*04:232| C*04:235| C*04:237| C*04:238| C*04:239| C*04:240| C*04:241| C*04:242| C*04:243| C*04:244| C*04:245| C*04:246| C*04:247| C*04:248| C*04:249| C*04:250| C*04:251| C*04:252| C*04:254| C*04:256| C*04:257| C*04:258| C*04:259| C*04:260| C*04:261| C*04:262| C*04:263| C*04:264| C*04:265| C*04:266| C*04:267| C*04:268| C*04:269| C*04:270| C*04:271| C*04:272| C*04:273| C*04:274| C*04:275| C*04:276| C*04:277| C*04:278| C*04:280| C*04:281| C*04:282| C*04:283| C*04:284| C*04:285| C*04:286</t>
-  </si>
-  <si>
-    <t>C*05:01| C*05:03| C*05:04| C*05:05| C*05:06| C*05:08| C*05:09| C*05:10| C*05:11| C*05:12| C*05:13| C*05:14| C*05:15| C*05:16| C*05:17| C*05:18| C*05:19| C*05:20| C*05:21| C*05:22| C*05:23| C*05:24| C*05:25| C*05:26| C*05:27| C*05:28| C*05:29| C*05:30| C*05:31| C*05:32| C*05:33| C*05:34| C*05:35| C*05:36| C*05:37| C*05:38| C*05:39| C*05:40| C*05:41| C*05:42| C*05:43| C*05:44| C*05:45| C*05:46| C*05:47| C*05:49| C*05:50| C*05:51Q| C*05:52| C*05:53| C*05:54| C*05:55| C*05:56| C*05:57| C*05:58| C*05:59| C*05:60| C*05:61| C*05:62| C*05:63| C*05:64| C*05:65| C*05:66| C*05:67| C*05:68| C*05:69| C*05:70| C*05:71| C*05:72| C*05:73| C*05:74| C*05:75| C*05:76| C*05:77| C*05:78| C*05:79| C*05:80| C*05:81| C*05:82| C*05:83| C*05:84| C*05:85| C*05:86| C*05:87| C*05:88| C*05:89| C*05:90| C*05:93| C*05:94| C*05:95| C*05:96| C*05:97| C*05:98| C*05:100| C*05:101| C*05:102| C*05:103| C*05:104| C*05:105| C*05:106| C*05:107| C*05:108| C*05:109| C*05:110| C*05:111| C*05:112| C*05:114| C*05:115| C*05:116| C*05:117| C*05:118| C*05:119| C*05:120| C*05:121| C*05:122| C*05:123| C*05:124| C*05:125| C*05:126| C*05:127| C*05:129| C*05:130| C*05:131| C*05:132| C*05:133| C*05:134| C*05:135| C*05:136| C*05:137| C*05:138| C*05:139| C*05:140| C*05:141| C*05:142| C*05:143| C*05:144| C*05:145| C*05:146| C*05:147| C*05:148| C*05:149| C*05:150| C*05:151| C*05:152| C*05:155| C*05:156| C*05:157</t>
-  </si>
-  <si>
-    <t>C*06:02| C*06:03| C*06:04| C*06:05| C*06:06| C*06:07| C*06:08| C*06:09| C*06:10| C*06:11| C*06:12| C*06:13| C*06:14| C*06:15| C*06:17| C*06:18| C*06:19| C*06:20| C*06:21| C*06:22| C*06:23| C*06:24| C*06:25| C*06:26| C*06:27| C*06:28| C*06:29| C*06:30| C*06:31| C*06:32| C*06:33| C*06:34| C*06:35| C*06:36| C*06:37| C*06:38| C*06:39| C*06:40| C*06:41| C*06:42| C*06:43| C*06:44| C*06:45| C*06:47| C*06:48| C*06:50| C*06:51| C*06:52| C*06:53| C*06:54| C*06:55| C*06:56| C*06:57| C*06:58| C*06:59| C*06:60| C*06:61| C*06:62| C*06:63| C*06:64| C*06:65| C*06:66| C*06:67| C*06:68| C*06:69| C*06:70| C*06:71| C*06:72| C*06:73| C*06:74Q| C*06:75| C*06:76| C*06:77| C*06:78| C*06:80| C*06:81| C*06:82| C*06:83| C*06:84| C*06:85| C*06:86| C*06:87| C*06:88| C*06:89| C*06:90| C*06:91| C*06:92| C*06:93| C*06:94| C*06:95| C*06:96| C*06:97| C*06:98| C*06:99| C*06:100| C*06:101| C*06:102| C*06:103| C*06:104| C*06:105| C*06:106| C*06:107| C*06:108| C*06:109| C*06:110| C*06:111| C*06:112| C*06:113| C*06:114| C*06:115| C*06:117| C*06:118| C*06:119| C*06:120| C*06:121| C*06:122| C*06:123| C*06:124| C*06:125| C*06:126| C*06:127| C*06:129| C*06:130| C*06:131| C*06:132| C*06:133| C*06:135| C*06:136| C*06:137| C*06:138| C*06:139| C*06:140| C*06:141| C*06:142| C*06:143| C*06:144| C*06:145| C*06:146| C*06:147| C*06:148| C*06:149| C*06:150| C*06:151| C*06:153| C*06:154| C*06:155| C*06:156| C*06:157| C*06:158| C*06:159| C*06:160| C*06:161| C*06:162| C*06:163| C*06:164| C*06:165| C*06:166| C*06:167| C*06:168| C*06:169| C*06:170| C*06:172| C*06:173| C*06:174| C*06:176| C*06:177| C*06:178| C*06:179| C*06:180| C*06:181| C*06:182| C*06:183| C*06:184| C*06:185| C*06:186| C*06:187| C*06:188| C*06:189| C*06:190| C*06:191| C*06:192| C*06:193| C*06:194| C*06:195| C*06:196| C*06:197| C*06:198| C*06:199| C*06:200Q| C*06:201| C*06:202| C*06:203| C*06:204| C*06:205| C*06:206| C*06:207| C*06:209| C*06:210| C*06:212| C*18:01| C*18:02</t>
-  </si>
-  <si>
-    <t>C*07:01| C*07:01Q| C*07:02| C*07:03| C*07:04| C*07:05| C*07:06| C*07:07| C*07:08| C*07:09| C*07:10| C*07:11| C*07:12| C*07:13| C*07:14| C*07:15| C*07:16| C*07:17| C*07:18| C*07:19| C*07:20| C*07:21| C*07:22| C*07:23| C*07:24| C*07:25| C*07:26| C*07:27| C*07:28| C*07:29| C*07:30| C*07:31| C*07:35| C*07:36| C*07:37| C*07:38| C*07:39| C*07:40| C*07:41| C*07:42| C*07:43| C*07:44| C*07:45| C*07:46| C*07:47| C*07:48| C*07:49| C*07:50| C*07:51| C*07:52| C*07:53| C*07:54| C*07:56| C*07:57| C*07:58| C*07:59| C*07:60| C*07:62| C*07:63| C*07:64| C*07:65| C*07:66| C*07:67| C*07:68| C*07:69| C*07:70| C*07:71| C*07:72| C*07:73| C*07:74| C*07:75| C*07:76| C*07:77| C*07:78| C*07:79| C*07:80| C*07:81| C*07:82| C*07:83| C*07:84| C*07:85| C*07:86| C*07:87| C*07:88| C*07:89| C*07:90| C*07:91| C*07:92| C*07:93| C*07:94| C*07:95| C*07:96| C*07:97| C*07:99| C*07:100| C*07:101| C*07:102| C*07:103| C*07:105| C*07:106| C*07:107| C*07:108| C*07:109| C*07:110| C*07:111| C*07:112| C*07:113| C*07:114| C*07:115| C*07:116| C*07:117| C*07:118| C*07:119| C*07:120| C*07:121Q| C*07:122| C*07:123| C*07:124| C*07:125| C*07:126| C*07:127| C*07:128| C*07:129| C*07:130| C*07:131| C*07:132| C*07:133| C*07:134| C*07:135| C*07:136| C*07:137| C*07:138| C*07:139| C*07:140| C*07:141| C*07:142| C*07:143| C*07:144| C*07:145| C*07:146| C*07:147| C*07:148| C*07:149| C*07:150Q| C*07:151| C*07:153| C*07:154| C*07:155| C*07:156| C*07:157| C*07:158| C*07:159| C*07:160| C*07:161| C*07:162| C*07:163| C*07:165| C*07:166| C*07:167| C*07:168| C*07:169| C*07:170| C*07:171| C*07:172| C*07:173| C*07:174| C*07:175| C*07:176| C*07:177| C*07:178| C*07:179| C*07:180| C*07:181| C*07:182| C*07:183| C*07:184| C*07:185| C*07:186| C*07:187| C*07:188| C*07:189| C*07:190| C*07:192| C*07:193| C*07:194| C*07:195| C*07:196| C*07:197| C*07:199| C*07:200| C*07:201| C*07:202| C*07:203| C*07:204| C*07:205| C*07:206| C*07:207| C*07:208| C*07:209| C*07:210| C*07:211| C*07:212| C*07:213| C*07:214| C*07:215| C*07:216| C*07:217| C*07:218| C*07:219| C*07:220| C*07:221| C*07:222| C*07:223| C*07:224| C*07:225| C*07:226| C*07:228| C*07:229| C*07:230| C*07:231| C*07:232| C*07:233| C*07:234| C*07:235Q| C*07:236| C*07:237| C*07:238| C*07:239| C*07:240| C*07:241| C*07:242| C*07:243| C*07:244| C*07:245| C*07:246| C*07:247| C*07:248| C*07:249| C*07:250| C*07:251| C*07:252| C*07:253| C*07:254| C*07:255| C*07:256| C*07:257| C*07:258| C*07:259| C*07:260| C*07:261| C*07:262| C*07:263| C*07:265| C*07:266| C*07:267| C*07:268| C*07:269| C*07:270| C*07:271| C*07:272| C*07:273| C*07:274| C*07:275| C*07:276| C*07:277| C*07:278| C*07:279| C*07:280| C*07:281| C*07:282| C*07:283| C*07:284| C*07:285| C*07:286| C*07:287| C*07:288| C*07:289| C*07:290| C*07:291| C*07:292| C*07:293| C*07:294| C*07:296| C*07:297| C*07:298| C*07:299| C*07:300| C*07:301| C*07:302| C*07:303| C*07:304| C*07:305| C*07:306| C*07:307| C*07:308| C*07:309| C*07:310| C*07:311| C*07:312| C*07:313| C*07:314| C*07:315| C*07:316| C*07:317| C*07:318| C*07:319| C*07:320| C*07:321| C*07:322| C*07:323| C*07:324| C*07:325| C*07:326| C*07:327| C*07:328| C*07:330| C*07:331| C*07:332| C*07:333| C*07:334| C*07:335| C*07:336| C*07:337| C*07:338| C*07:339| C*07:340| C*07:341| C*07:342| C*07:343| C*07:344| C*07:345| C*07:346| C*07:348| C*07:349| C*07:351| C*07:352| C*07:353| C*07:354| C*07:355| C*07:356| C*07:357| C*07:358| C*07:359| C*07:360| C*07:361| C*07:362| C*07:363| C*07:364| C*07:365| C*07:366| C*07:367| C*07:368| C*07:369| C*07:370| C*07:371| C*07:372| C*07:373| C*07:374| C*07:375| C*07:376| C*07:377| C*07:378| C*07:379| C*07:380| C*07:381| C*07:382| C*07:383| C*07:384| C*07:385| C*07:386| C*07:387| C*07:388| C*07:389| C*07:390| C*07:391| C*07:392| C*07:394| C*07:395| C*07:396| C*07:397| C*07:398| C*07:399| C*07:400| C*07:401| C*07:402| C*07:403| C*07:404| C*07:405| C*07:406| C*07:407| C*07:408| C*07:409| C*07:410| C*07:411| C*07:412| C*07:413| C*07:414| C*07:415| C*07:416| C*07:417| C*07:418| C*07:419| C*07:420| C*07:421| C*07:422| C*07:423| C*07:424| C*07:425| C*07:426| C*07:427| C*07:428| C*07:429| C*07:430| C*07:431| C*07:432| C*07:433| C*07:434| C*07:435| C*07:436| C*07:438| C*07:439| C*07:440| C*07:441| C*07:442| C*07:443| C*07:444| C*07:445| C*07:446| C*07:447| C*07:448| C*07:449| C*07:450| C*07:453| C*07:454| C*07:455| C*07:456| C*07:457| C*07:458| C*07:459| C*07:460| C*07:461| C*07:462| C*07:463| C*07:464| C*07:465| C*07:466| C*07:467| C*07:468| C*07:469| C*07:470| C*07:471| C*07:472| C*07:473| C*07:474| C*07:475| C*07:477| C*07:478| C*07:479| C*07:480| C*07:481| C*07:482| C*07:485| C*07:486| C*07:487| C*07:488| C*07:489| C*07:490| C*07:492| C*07:493| C*07:494Q| C*07:495| C*07:496| C*07:497| C*07:498| C*07:499| C*07:500| C*07:501| C*07:502| C*07:503| C*07:504| C*07:505| C*07:506| C*07:508| C*07:509| C*07:510| C*07:511| C*07:512| C*07:513Q| C*07:514| C*07:515| C*07:516| C*07:517| C*07:518| C*07:519| C*07:520| C*07:521| C*07:522| C*07:523| C*07:524| C*07:525| C*07:526| C*07:527| C*07:528| C*07:529| C*07:530| C*07:531| C*07:532| C*07:533| C*07:534| C*07:535| C*07:536| C*07:537| C*07:538| C*07:539| C*07:540| C*07:541| C*07:542| C*07:543| C*07:544| C*07:545| C*07:546| C*07:547| C*07:548| C*07:549| C*07:550| C*07:552| C*07:553| C*07:554| C*07:555| C*07:556| C*07:557| C*07:558| C*07:559| C*07:560| C*07:561| C*07:562| C*07:563| C*07:564| C*07:565| C*07:566| C*07:567| C*07:568| C*07:569| C*07:570| C*07:571| C*07:572| C*07:573| C*07:574| C*07:575| C*07:576| C*07:577| C*07:578| C*07:579| C*07:580| C*07:581| C*07:582Q| C*07:583| C*07:584| C*07:585| C*07:586| C*07:587| C*07:588| C*07:589| C*07:590| C*07:591| C*07:592| C*07:594| C*07:595| C*07:596| C*07:597| C*07:598| C*07:599| C*07:601| C*07:602| C*07:604| C*07:605| C*07:606| C*07:607| C*07:608| C*07:609| C*07:610| C*12:14| C*17:01| C*17:03</t>
-  </si>
-  <si>
-    <t>C*08:01| C*08:02| C*08:03| C*08:04| C*08:05| C*08:06| C*08:07| C*08:08| C*08:09| C*08:10| C*08:11| C*08:12| C*08:13| C*08:14| C*08:15| C*08:16| C*08:17| C*08:18| C*08:19| C*08:20| C*08:21| C*08:22| C*08:23| C*08:24| C*08:25| C*08:27| C*08:28| C*08:29| C*08:30| C*08:31| C*08:32| C*08:33| C*08:34| C*08:35| C*08:37| C*08:38| C*08:39| C*08:40| C*08:41| C*08:42| C*08:43| C*08:44| C*08:45| C*08:46| C*08:47| C*08:48| C*08:49| C*08:50| C*08:51| C*08:53| C*08:54| C*08:56| C*08:57| C*08:58| C*08:59| C*08:60| C*08:61| C*08:62| C*08:63| C*08:65| C*08:66| C*08:67| C*08:68| C*08:69| C*08:70Q| C*08:71| C*08:72| C*08:73| C*08:74| C*08:75| C*08:76| C*08:77| C*08:78| C*08:79| C*08:80| C*08:81| C*08:82| C*08:83| C*08:84| C*08:85| C*08:86| C*08:87| C*08:90| C*08:91| C*08:92| C*08:93| C*08:94| C*08:95| C*08:96| C*08:97| C*08:98| C*08:99| C*08:100| C*08:101| C*08:102| C*08:103| C*08:104| C*08:105| C*08:106| C*08:107| C*08:108| C*08:109| C*08:110| C*08:111| C*08:112| C*08:113| C*08:114| C*08:115| C*08:116| C*08:117| C*08:118| C*08:119| C*08:120| C*08:122| C*08:123| C*08:124| C*08:125| C*08:126| C*08:128| C*08:131| C*08:132| C*08:133| C*08:134| C*08:135| C*08:136| C*08:137| C*08:138| C*08:139| C*08:140| C*08:141Q| C*08:142| C*08:143| C*08:144| C*08:145| C*08:146| C*08:147| C*08:148| C*08:149| C*08:150| C*08:151| C*08:152| C*08:153| C*08:154| C*08:155| C*08:156| C*08:157| C*08:158| C*08:159</t>
-  </si>
-  <si>
-    <t>C*12:02| C*12:03| C*12:04| C*12:05| C*12:06| C*12:07| C*12:08| C*12:09| C*12:10| C*12:11| C*12:12| C*12:13| C*12:15| C*12:16| C*12:17| C*12:18| C*12:19| C*12:20| C*12:21| C*12:22| C*12:23| C*12:24| C*12:25| C*12:26| C*12:27| C*12:28| C*12:29| C*12:30| C*12:31| C*12:32| C*12:33| C*12:34| C*12:35| C*12:36| C*12:37| C*12:38| C*12:40| C*12:41| C*12:42Q| C*12:43| C*12:44| C*12:45| C*12:47| C*12:48| C*12:49| C*12:50| C*12:51| C*12:52| C*12:53| C*12:54| C*12:55| C*12:56| C*12:57| C*12:58| C*12:59| C*12:60| C*12:61| C*12:62| C*12:63| C*12:64| C*12:65| C*12:66| C*12:67| C*12:68| C*12:69| C*12:70| C*12:71| C*12:72| C*12:73| C*12:74| C*12:75| C*12:76| C*12:77| C*12:78| C*12:79| C*12:81| C*12:82| C*12:83| C*12:85| C*12:86| C*12:87| C*12:88| C*12:89| C*12:90| C*12:91| C*12:92| C*12:93| C*12:94| C*12:95| C*12:96| C*12:97| C*12:98| C*12:99| C*12:100| C*12:101| C*12:102| C*12:103| C*12:106| C*12:107| C*12:108| C*12:109| C*12:110| C*12:111| C*12:112| C*12:113| C*12:114| C*12:115| C*12:116| C*12:117| C*12:118| C*12:119| C*12:120| C*12:121| C*12:122| C*12:123| C*12:124| C*12:125| C*12:126| C*12:127| C*12:128| C*12:129| C*12:130| C*12:131| C*12:132| C*12:133| C*12:134| C*12:135| C*12:136| C*12:137| C*12:138| C*12:139| C*12:140| C*12:141| C*12:142| C*12:143| C*12:144| C*12:145| C*12:146| C*12:147| C*12:149| C*12:150| C*12:151| C*12:152| C*12:153| C*12:154| C*12:155Q| C*12:156| C*12:157| C*12:158| C*12:159| C*12:160| C*12:161| C*12:162| C*12:163| C*12:164| C*12:165| C*12:166| C*12:167| C*12:168| C*12:169| C*12:170| C*12:171| C*12:172| C*12:173| C*12:174| C*12:175| C*12:176| C*12:177| C*12:178| C*12:179| C*12:180| C*12:181| C*12:182| C*12:183| C*12:184| C*12:185| C*12:186| C*12:187| C*12:188| C*12:189| C*12:190| C*12:191| C*12:192| C*12:193| C*12:194| C*12:195| C*12:196| C*12:197| C*12:198| C*12:199| C*12:200| C*12:201| C*12:202| C*12:203| C*12:204| C*12:205| C*12:206| C*12:207| C*12:208| C*12:209| C*12:210| C*12:211| C*12:212| C*12:213| C*12:214| C*12:215| C*12:216| C*12:217| C*12:218| C*12:220| C*12:221</t>
-  </si>
-  <si>
-    <t>C*14:04| C*14:06| C*14:09| C*14:10| C*14:11| C*14:12| C*14:13| C*14:14| C*14:15| C*14:16| C*14:17| C*14:18| C*14:19| C*14:20| C*14:22| C*14:23| C*14:24| C*14:25| C*14:26| C*14:27| C*14:28| C*14:29| C*14:30| C*14:31| C*14:32| C*14:33| C*14:34| C*14:36| C*14:37| C*14:38| C*14:39| C*14:40| C*14:41| C*14:42| C*14:43| C*14:44| C*14:45| C*14:46| C*14:48| C*14:49| C*14:50| C*14:51| C*14:52| C*14:53| C*14:54| C*14:55| C*14:56| C*14:57| C*14:58| C*14:59| C*14:60| C*14:61| C*14:62| C*14:63| C*14:64| C*14:65| C*14:66| C*14:67| C*14:68| C*14:69| C*14:70| C*14:71| C*14:72| C*14:73| C*14:74| C*14:75| C*14:76| C*14:77| C*14:78| C*14:79| C*14:80| C*14:81| C*14:82| C*14:83| C*14:84| C*14:85| C*14:86| C*14:87| C*14:88| C*14:89| C*14:90</t>
-  </si>
-  <si>
-    <t>C*15:02| C*15:03| C*15:04| C*15:05| C*15:06| C*15:08| C*15:09| C*15:10| C*15:11| C*15:12| C*15:13| C*15:15| C*15:16| C*15:17| C*15:18| C*15:19| C*15:22| C*15:23| C*15:24| C*15:25| C*15:26| C*15:27| C*15:28| C*15:29| C*15:30| C*15:31| C*15:32Q| C*15:33| C*15:34| C*15:35| C*15:36| C*15:37| C*15:38| C*15:39| C*15:40| C*15:41| C*15:42| C*15:43| C*15:44| C*15:45| C*15:46| C*15:47| C*15:48| C*15:49| C*15:50| C*15:51| C*15:52| C*15:53| C*15:54| C*15:55| C*15:56| C*15:57| C*15:58| C*15:59| C*15:60| C*15:61| C*15:62| C*15:63| C*15:64| C*15:65| C*15:66| C*15:67| C*15:68| C*15:69| C*15:70| C*15:71| C*15:72| C*15:73| C*15:74| C*15:75| C*15:76| C*15:77| C*15:78| C*15:79| C*15:80| C*15:81| C*15:82| C*15:83| C*15:84Q| C*15:85| C*15:86| C*15:87| C*15:88| C*15:89| C*15:90| C*15:91| C*15:93| C*15:94| C*15:96Q| C*15:97| C*15:98| C*15:99| C*15:100| C*15:101| C*15:102| C*15:103| C*15:104| C*15:105Q| C*15:106| C*15:107| C*15:108| C*15:109| C*15:110| C*15:111| C*15:112| C*15:113| C*15:114| C*15:116| C*15:117| C*15:118| C*15:119| C*15:120| C*15:121| C*15:123| C*15:124| C*15:125| C*15:126| C*15:127| C*15:128| C*15:129| C*15:130| C*15:131| C*15:132| C*15:133| C*15:134| C*15:135| C*15:136| C*15:137| C*15:138| C*15:139| C*15:140| C*15:141| C*15:142| C*15:143| C*15:144| C*15:146| C*15:147| C*15:148| C*15:149| C*15:150| C*15:151</t>
-  </si>
-  <si>
-    <t>C*16:01| C*16:02| C*16:04| C*16:06| C*16:07| C*16:08| C*16:09| C*16:10| C*16:11| C*16:12| C*16:13| C*16:14| C*16:15| C*16:16Q| C*16:17| C*16:18| C*16:19| C*16:20| C*16:21| C*16:22| C*16:23| C*16:24| C*16:25| C*16:26| C*16:27| C*16:28| C*16:29| C*16:31| C*16:32| C*16:33| C*16:34| C*16:35| C*16:36| C*16:37| C*16:38| C*16:39| C*16:40| C*16:41| C*16:42| C*16:43| C*16:44| C*16:45| C*16:46| C*16:47| C*16:48| C*16:49| C*16:50| C*16:51| C*16:52| C*16:53| C*16:54| C*16:55| C*16:56| C*16:57| C*16:58| C*16:59| C*16:60| C*16:61| C*16:62| C*16:63| C*16:64| C*16:65| C*16:66| C*16:67| C*16:68| C*16:69| C*16:70| C*16:71| C*16:72| C*16:73| C*16:74| C*16:75| C*16:76| C*16:78| C*16:79| C*16:80| C*16:81| C*16:82| C*16:83| C*16:84| C*16:85| C*16:86| C*16:87| C*16:88| C*16:90| C*16:91| C*16:92| C*16:93| C*16:94| C*16:95| C*16:96| C*16:97| C*16:98| C*16:99| C*16:100| C*16:101| C*16:102| C*16:103| C*16:104| C*16:105| C*16:106| C*16:107| C*16:108| C*16:109| C*16:110| C*16:111| C*16:112| C*16:113| C*16:114| C*16:115| C*16:116</t>
-  </si>
-  <si>
-    <t>C*17:02| C*17:04| C*17:05| C*17:06| C*17:07| C*17:08| C*17:09| C*17:10| C*17:11| C*17:12| C*17:13| C*17:14| C*17:15| C*17:16| C*17:17| C*17:18| C*17:19| C*17:20| C*17:21| C*17:22| C*17:23| C*17:24| C*17:25| C*17:26| C*17:28| C*17:29| C*17:30| C*17:31| C*17:32| C*17:33| C*17:34| C*17:35| C*17:36| C*17:37| C*17:38</t>
-  </si>
-  <si>
-    <t>C*18:03| C*18:04| C*18:05| C*18:06| C*18:08| C*18:09| C*18:10</t>
+    <t>C*01:37N| C*01:56N| C*01:69N| C*01:86N| C*01:89N| C*01:98N| C*01:109N| C*01:111N| C*01:117N| C*01:137N| C*01:143N| C*01:145N| C*01:171N| C*02:38:01N| C*02:38:02N| C*02:52N| C*02:92N| C*02:105N| C*02:121N| C*02:135N| C*02:150N| C*02:165N| C*03:20N| C*03:121N| C*03:189N| C*03:201N| C*03:208N| C*03:224N| C*03:229N| C*03:265N| C*03:277N| C*03:316N| C*03:318N| C*03:323N| C*03:363N| C*03:366N| C*03:377N| C*03:380N| C*03:391N| C*03:392N| C*03:396N| C*03:421N| C*03:424N| C*03:432N| C*03:444N| C*03:445N| C*03:446N| C*03:447N| C*03:449N| C*04:09N| C*04:88N| C*04:93N| C*04:95N| C*04:105N| C*04:115N| C*04:123N| C*04:170N| C*04:173N| C*04:191N| C*04:203N| C*04:205N| C*04:215N| C*04:217N| C*04:225N| C*04:233N| C*04:234N| C*04:236N| C*04:253N| C*04:255N| C*04:279N| C*04:300N| C*04:305N| C*04:309N| C*04:349N| C*04:350N| C*05:07N| C*05:48N| C*05:91N| C*05:92N| C*05:99N| C*05:113N| C*05:128N| C*05:153N| C*05:154N| C*05:169N| C*05:175N| C*05:180N| C*06:16N| C*06:46N| C*06:49N| C*06:79N| C*06:116N| C*06:128N| C*06:134N| C*06:152N| C*06:171:01:01N| C*06:171:01:02N| C*06:175N| C*06:208N| C*06:211N| C*06:215N| C*06:220N| C*07:02:01:17N| C*07:32N| C*07:33N| C*07:55N| C*07:61N| C*07:98N| C*07:104N| C*07:152N| C*07:164N| C*07:191N| C*07:198N| C*07:227N| C*07:264N| C*07:329N| C*07:347N| C*07:350N| C*07:393N| C*07:437N| C*07:451N| C*07:452N| C*07:476N| C*07:483N| C*07:484N| C*07:491:01N| C*07:491:02N| C*07:507N| C*07:551N| C*07:593N| C*07:600:01N| C*07:600:02N| C*07:603N| C*07:633N| C*07:672N| C*07:675N| C*07:686N| C*07:690N| C*07:702N| C*08:26N| C*08:36N| C*08:52N| C*08:55N| C*08:88N| C*08:89N| C*08:121N| C*08:127N| C*08:129N| C*08:130N| C*08:161N| C*08:173N| C*12:39N| C*12:46N| C*12:80N| C*12:84N| C*12:104N| C*12:105N| C*12:148N| C*12:219N| C*12:232N| C*12:236N| C*14:07N| C*14:21N| C*14:35N| C*14:47N| C*14:93N| C*14:97N| C*14:99N| C*15:02:01:08N| C*15:92N| C*15:95N| C*15:115N| C*15:122N| C*15:145N| C*15:156N| C*15:160N| C*15:164N| C*15:177N| C*16:30N| C*16:77N| C*16:89N| C*16:123N| C*16:132N| C*17:27N| C*18:07N</t>
+  </si>
+  <si>
+    <t>C*01:02:01:01| C*01:02:01:02| C*01:02:01:03| C*01:02:01:04| C*01:02:01:05| C*01:02:01:06| C*01:02:01:07| C*01:02:01:08| C*01:02:01:09| C*01:02:01:10| C*01:02:01:11| C*01:02:02| C*01:02:03| C*01:02:04| C*01:02:05| C*01:02:06| C*01:02:07| C*01:02:08| C*01:02:09| C*01:02:10| C*01:02:11| C*01:02:12| C*01:02:13| C*01:02:14| C*01:02:15| C*01:02:16| C*01:02:17| C*01:02:18| C*01:02:19| C*01:02:20| C*01:02:21| C*01:02:22| C*01:02:23| C*01:02:24| C*01:02:25| C*01:02:26| C*01:02:27| C*01:02:28| C*01:02:29| C*01:02:30:01| C*01:02:30:02| C*01:02:31| C*01:02:32| C*01:02:33| C*01:02:34| C*01:02:35| C*01:02:36| C*01:02:37| C*01:02:38| C*01:02:39| C*01:02:40| C*01:02:41| C*01:02:42| C*01:02:43| C*01:02:44| C*01:02:45| C*01:02:46| C*01:02:47| C*01:02:48| C*01:02:49| C*01:02:50| C*01:02:51| C*01:02:52| C*01:02:53| C*01:02:54| C*01:02:55| C*01:03| C*01:04| C*01:05| C*01:06| C*01:07:01| C*01:07:02| C*01:08| C*01:09| C*01:10| C*01:11| C*01:12:01| C*01:12:02| C*01:13| C*01:14| C*01:15:01| C*01:15:02| C*01:16| C*01:17| C*01:18| C*01:19| C*01:20| C*01:21| C*01:22| C*01:23| C*01:24| C*01:25| C*01:26| C*01:27| C*01:28| C*01:29| C*01:30| C*01:31| C*01:32:01| C*01:32:02| C*01:33| C*01:34| C*01:35| C*01:36| C*01:38| C*01:39| C*01:40| C*01:41| C*01:42| C*01:43| C*01:44| C*01:45| C*01:46| C*01:47| C*01:48| C*01:49:01| C*01:49:02| C*01:50| C*01:51| C*01:52| C*01:53| C*01:54| C*01:55| C*01:57| C*01:58| C*01:59| C*01:60| C*01:61| C*01:62| C*01:63:02| C*01:64| C*01:65| C*01:66| C*01:67| C*01:68| C*01:70| C*01:71| C*01:72| C*01:73| C*01:74| C*01:75| C*01:76| C*01:77| C*01:78| C*01:79:01| C*01:79:02| C*01:80| C*01:81| C*01:82| C*01:83| C*01:84| C*01:85| C*01:87| C*01:88| C*01:90| C*01:91| C*01:92| C*01:93| C*01:94| C*01:95| C*01:96| C*01:97| C*01:99| C*01:100| C*01:101| C*01:102| C*01:103| C*01:104| C*01:105| C*01:106| C*01:107| C*01:108| C*01:110| C*01:112| C*01:113| C*01:114:01| C*01:114:02| C*01:115| C*01:116| C*01:118| C*01:119| C*01:120| C*01:121Q| C*01:122| C*01:123| C*01:124| C*01:125| C*01:126| C*01:127| C*01:128| C*01:129| C*01:130| C*01:131| C*01:132| C*01:133| C*01:134| C*01:135| C*01:136| C*01:138| C*01:139| C*01:140| C*01:141| C*01:142| C*01:144| C*01:146:01| C*01:146:02| C*01:147| C*01:148| C*01:149| C*01:150| C*01:151| C*01:152| C*01:153| C*01:154| C*01:155| C*01:156| C*01:157| C*01:158| C*01:159| C*01:160| C*01:161| C*01:162| C*01:163| C*01:164| C*01:165| C*01:166| C*01:167| C*01:168| C*01:169:01| C*01:169:02| C*01:170| C*01:172| C*01:173| C*01:174| C*01:175| C*01:176| C*14:02:01:01| C*14:02:01:02| C*14:02:01:03| C*14:02:01:04| C*14:02:01:05| C*14:02:01:06| C*14:02:01:07| C*14:02:01:08| C*14:02:01:09| C*14:02:02| C*14:02:03| C*14:02:04| C*14:02:05| C*14:02:06| C*14:02:07| C*14:02:08| C*14:02:09| C*14:02:10| C*14:02:11| C*14:02:12| C*14:02:13| C*14:02:14| C*14:02:15| C*14:02:16| C*14:02:17| C*14:02:18| C*14:02:19| C*14:02:20| C*14:02:21| C*14:02:22| C*14:02:23| C*14:02:24| C*14:02:25| C*14:02:26| C*14:02:27| C*14:02:28| C*14:02:29| C*14:02:30| C*14:02:31| C*14:03| C*14:05| C*14:08</t>
+  </si>
+  <si>
+    <t>C*02:02:01| C*02:02:02:01| C*02:02:02:02| C*02:02:02:03| C*02:02:02:04| C*02:02:02:05| C*02:02:02:06| C*02:02:02:07| C*02:02:02:08| C*02:02:02:09| C*02:02:02:10| C*02:02:02:11| C*02:02:02:12| C*02:02:02:13| C*02:02:02:14| C*02:02:02:15| C*02:02:02:16| C*02:02:02:17| C*02:02:02:18| C*02:02:02:19| C*02:02:02:20| C*02:02:03| C*02:02:05| C*02:02:06| C*02:02:07| C*02:02:08| C*02:02:09| C*02:02:10| C*02:02:11| C*02:02:12| C*02:02:13| C*02:02:14| C*02:02:15| C*02:02:16| C*02:02:17| C*02:02:18| C*02:02:19| C*02:02:20| C*02:02:21| C*02:02:22| C*02:02:23| C*02:02:24| C*02:02:25| C*02:02:26| C*02:02:27| C*02:02:28| C*02:02:29| C*02:02:30| C*02:02:31| C*02:02:32| C*02:02:33| C*02:02:34| C*02:02:35| C*02:02:36| C*02:02:37| C*02:02:38| C*02:02:39| C*02:02:40| C*02:02:41| C*02:02:42| C*02:02:43| C*02:02:44| C*02:02:45| C*02:02:46| C*02:02:47| C*02:02:48| C*02:02:49| C*02:02:50| C*02:02:51| C*02:02:52| C*02:03| C*02:04| C*02:05:01| C*02:05:02| C*02:05:03| C*02:06:01| C*02:06:02| C*02:07| C*02:08| C*02:09| C*02:10:01:01| C*02:10:01:02| C*02:10:01:03| C*02:10:01:04| C*02:10:01:05| C*02:10:01:06| C*02:10:01:07| C*02:10:02| C*02:10:03| C*02:10:04| C*02:10:05| C*02:11| C*02:12| C*02:13| C*02:14:01| C*02:14:02| C*02:15| C*02:16:02| C*02:17| C*02:18| C*02:19| C*02:20| C*02:21| C*02:22| C*02:23| C*02:24| C*02:25Q| C*02:26:01| C*02:26:02| C*02:26:03| C*02:27:01| C*02:27:02| C*02:28| C*02:29| C*02:30| C*02:31| C*02:32| C*02:33| C*02:34| C*02:35| C*02:36:01| C*02:36:02| C*02:37| C*02:39| C*02:40:01| C*02:40:02| C*02:42| C*02:43:01| C*02:43:02| C*02:44| C*02:45| C*02:46| C*02:47| C*02:48| C*02:49| C*02:50| C*02:51| C*02:53:01| C*02:53:02| C*02:54| C*02:55:01| C*02:55:02| C*02:56| C*02:57| C*02:58| C*02:59| C*02:60| C*02:61| C*02:62| C*02:63| C*02:64| C*02:65| C*02:66| C*02:67Q| C*02:68| C*02:69| C*02:70| C*02:71| C*02:72| C*02:73| C*02:74| C*02:75| C*02:76| C*02:77| C*02:78| C*02:79| C*02:80| C*02:81| C*02:82| C*02:83| C*02:84| C*02:85| C*02:86| C*02:87| C*02:88| C*02:89| C*02:90| C*02:91| C*02:93| C*02:94| C*02:95| C*02:96| C*02:97| C*02:98| C*02:99| C*02:100| C*02:101| C*02:102| C*02:103| C*02:104| C*02:106| C*02:107| C*02:108| C*02:109| C*02:110| C*02:111| C*02:112| C*02:113| C*02:114| C*02:115| C*02:116| C*02:117| C*02:118| C*02:119| C*02:120| C*02:122| C*02:123| C*02:124| C*02:125| C*02:126| C*02:127| C*02:128| C*02:129| C*02:130| C*02:131| C*02:132| C*02:133| C*02:134| C*02:136| C*02:137| C*02:138| C*02:139| C*02:140| C*02:141| C*02:142| C*02:143| C*02:144| C*02:145| C*02:146| C*02:147| C*02:148| C*02:149| C*02:151| C*02:152| C*02:153| C*02:154| C*02:155| C*02:156| C*02:157| C*02:158| C*02:159| C*02:160| C*02:161| C*02:162| C*02:163| C*02:164| C*02:166</t>
+  </si>
+  <si>
+    <t>C*03:05| C*03:07:01:01| C*03:07:01:02| C*03:07:02| C*03:09| C*03:10| C*03:11:01| C*03:11:02| C*03:15| C*03:16| C*03:19| C*03:22Q| C*03:24| C*03:39| C*03:40:01| C*03:40:02| C*03:40:03| C*03:40:04| C*03:42| C*03:43:01| C*03:43:02| C*03:44| C*03:45| C*03:47| C*03:48| C*03:49| C*03:50| C*03:51| C*03:52| C*03:53| C*03:54| C*03:55| C*03:56| C*03:57:01| C*03:57:02| C*03:58| C*03:59| C*03:60| C*03:61| C*03:62| C*03:63| C*03:64:01| C*03:64:02| C*03:65| C*03:66| C*03:67| C*03:68| C*03:69| C*03:70| C*03:71| C*03:72| C*03:73| C*03:74| C*03:75| C*03:76| C*03:77| C*03:78| C*03:79| C*03:80:01| C*03:80:02| C*03:81| C*03:82| C*03:83| C*03:84| C*03:85| C*03:86| C*03:87:01| C*03:87:02| C*03:88| C*03:89| C*03:90| C*03:91:01| C*03:91:02| C*03:92| C*03:93| C*03:94| C*03:95| C*03:96| C*03:97| C*03:98| C*03:100| C*03:101| C*03:102| C*03:103| C*03:104| C*03:105| C*03:106| C*03:107| C*03:108| C*03:109| C*03:110| C*03:111| C*03:112| C*03:113:01| C*03:113:02| C*03:114| C*03:115:01| C*03:115:02| C*03:116:01| C*03:116:02| C*03:117| C*03:118| C*03:119:01| C*03:119:02| C*03:120| C*03:122| C*03:123| C*03:124| C*03:125| C*03:126| C*03:127| C*03:128| C*03:129| C*03:130| C*03:131| C*03:132| C*03:133| C*03:134| C*03:135| C*03:136| C*03:137| C*03:138| C*03:139| C*03:140| C*03:141| C*03:142| C*03:143| C*03:144| C*03:145| C*03:146| C*03:147| C*03:148| C*03:149| C*03:150| C*03:151| C*03:152| C*03:153| C*03:154| C*03:155| C*03:156| C*03:157| C*03:158| C*03:159| C*03:160| C*03:161| C*03:162| C*03:163| C*03:164| C*03:165:01| C*03:165:02| C*03:166| C*03:167| C*03:168| C*03:169Q| C*03:170| C*03:171| C*03:172| C*03:173| C*03:174| C*03:175| C*03:176| C*03:177| C*03:178| C*03:179| C*03:180| C*03:181| C*03:182| C*03:183| C*03:184:01| C*03:184:02| C*03:185| C*03:186:01| C*03:186:02| C*03:187| C*03:188| C*03:190| C*03:191| C*03:192| C*03:193| C*03:194| C*03:195| C*03:196| C*03:197| C*03:198| C*03:199| C*03:200| C*03:202| C*03:203| C*03:204| C*03:205| C*03:206| C*03:207| C*03:209| C*03:210| C*03:211:01| C*03:211:02| C*03:212| C*03:213| C*03:214| C*03:215| C*03:216| C*03:217| C*03:218| C*03:219| C*03:220| C*03:221| C*03:222| C*03:223| C*03:225| C*03:226| C*03:227| C*03:228| C*03:230| C*03:231| C*03:232| C*03:233| C*03:234| C*03:235| C*03:236| C*03:237| C*03:238| C*03:239| C*03:240| C*03:241| C*03:242| C*03:243| C*03:244Q| C*03:245| C*03:246| C*03:247| C*03:248| C*03:249| C*03:250| C*03:251| C*03:252| C*03:253| C*03:254| C*03:255| C*03:256| C*03:257| C*03:258| C*03:259| C*03:260| C*03:261| C*03:262| C*03:263:01| C*03:263:02| C*03:263:03| C*03:264| C*03:266| C*03:267| C*03:268| C*03:269| C*03:270| C*03:271| C*03:272| C*03:273| C*03:274| C*03:275| C*03:276| C*03:278| C*03:279| C*03:280| C*03:281| C*03:282| C*03:283| C*03:284| C*03:285| C*03:286| C*03:287:01| C*03:287:02| C*03:288| C*03:289| C*03:290| C*03:291| C*03:292| C*03:293| C*03:294| C*03:295| C*03:296:01| C*03:296:02| C*03:297| C*03:298| C*03:299| C*03:300| C*03:301| C*03:302| C*03:303| C*03:304| C*03:305| C*03:306| C*03:307| C*03:308| C*03:309| C*03:310| C*03:311| C*03:312| C*03:313| C*03:314| C*03:315| C*03:317| C*03:319| C*03:320| C*03:321| C*03:322| C*03:324| C*03:325| C*03:326| C*03:327| C*03:328| C*03:329| C*03:330| C*03:331| C*03:332| C*03:333| C*03:334| C*03:335| C*03:336| C*03:337| C*03:338| C*03:339| C*03:340| C*03:341| C*03:342| C*03:343| C*03:344:01:01| C*03:344:01:02| C*03:345| C*03:346| C*03:347| C*03:348| C*03:349| C*03:350| C*03:351| C*03:352| C*03:353| C*03:354| C*03:355| C*03:356| C*03:357| C*03:358| C*03:359| C*03:360| C*03:361| C*03:362| C*03:364| C*03:365| C*03:367| C*03:368| C*03:369| C*03:370| C*03:371| C*03:372| C*03:373| C*03:374| C*03:375| C*03:376| C*03:378| C*03:379| C*03:381| C*03:382| C*03:383| C*03:384| C*03:385| C*03:386| C*03:387| C*03:388| C*03:389| C*03:390| C*03:393| C*03:394| C*03:395| C*03:397| C*03:398| C*03:399| C*03:400| C*03:401| C*03:402| C*03:403| C*03:404| C*03:405| C*03:406| C*03:407| C*03:408| C*03:409| C*03:410| C*03:411| C*03:412| C*03:413| C*03:414| C*03:415| C*03:416| C*03:417| C*03:418| C*03:419| C*03:420| C*03:422| C*03:423| C*03:425| C*03:426| C*03:427| C*03:428| C*03:429| C*03:430| C*03:431| C*03:433| C*03:434| C*03:435| C*03:436| C*03:437| C*03:438| C*03:439| C*03:440| C*03:441| C*03:442Q| C*03:443| C*03:448Q| C*03:450| C*03:451| C*03:452| C*03:453| C*03:454| C*03:455| C*03:456| C*03:457| C*03:458| C*03:459| C*03:460| C*15:07| C*15:21| C*03:03:01:01| C*03:03:01:02| C*03:03:01:03| C*03:03:01:04| C*03:03:01:05| C*03:03:01:06| C*03:03:01:07| C*03:03:01:08| C*03:03:01:09| C*03:03:01:10| C*03:03:01:11| C*03:03:01:12| C*03:03:01:13| C*03:03:01:14| C*03:03:02| C*03:03:03| C*03:03:04| C*03:03:05| C*03:03:06| C*03:03:07| C*03:03:08| C*03:03:09| C*03:03:10| C*03:03:11| C*03:03:12| C*03:03:13| C*03:03:14| C*03:03:15| C*03:03:16| C*03:03:17| C*03:03:18| C*03:03:19| C*03:03:20| C*03:03:21| C*03:03:22| C*03:03:23| C*03:03:24| C*03:03:25| C*03:03:26| C*03:03:27| C*03:03:28| C*03:03:29| C*03:03:30| C*03:03:31| C*03:03:32| C*03:03:33| C*03:03:34| C*03:03:35| C*03:03:36| C*03:03:37| C*03:03:38| C*03:03:39| C*03:03:40| C*03:03:41| C*03:03:42| C*03:03:43| C*03:03:44| C*03:03:45| C*03:03:46| C*03:03:47| C*03:03:48| C*03:03:49| C*03:03:50| C*03:03:51| C*03:03:52| C*03:03:53| C*03:13:01:01| C*03:13:01:02| C*03:13:02| C*03:18:01| C*03:18:02| C*03:18:03| C*03:21| C*03:30| C*03:31| C*03:02:01| C*03:02:02:01| C*03:02:02:02| C*03:02:02:03| C*03:02:02:04| C*03:02:02:05| C*03:02:03| C*03:02:04| C*03:02:05| C*03:02:06| C*03:02:07| C*03:02:08| C*03:02:09| C*03:02:10| C*03:02:11| C*03:02:12| C*03:02:13| C*03:02:14| C*03:02:15| C*03:02:16| C*03:02:17| C*03:02:18| C*03:02:19| C*03:02:20| C*03:02:21| C*03:02:22| C*03:04:01:01| C*03:04:01:02| C*03:04:01:03| C*03:04:01:04| C*03:04:01:05| C*03:04:01:06| C*03:04:01:07| C*03:04:01:08| C*03:04:01:09| C*03:04:01:10| C*03:04:01:11| C*03:04:01:12| C*03:04:01:13| C*03:04:02| C*03:04:03| C*03:04:04| C*03:04:05| C*03:04:06| C*03:04:07| C*03:04:08| C*03:04:09| C*03:04:10| C*03:04:11| C*03:04:12| C*03:04:13| C*03:04:14| C*03:04:15| C*03:04:16| C*03:04:17| C*03:04:18| C*03:04:19| C*03:04:20| C*03:04:21| C*03:04:22| C*03:04:23| C*03:04:24| C*03:04:25| C*03:04:26| C*03:04:27| C*03:04:28| C*03:04:29| C*03:04:30| C*03:04:31| C*03:04:32| C*03:04:33| C*03:04:34| C*03:04:35| C*03:04:36| C*03:04:37| C*03:04:38| C*03:04:39| C*03:04:40| C*03:04:41| C*03:04:42| C*03:04:43| C*03:04:44| C*03:04:45| C*03:04:46| C*03:04:47| C*03:04:48| C*03:04:49| C*03:04:50| C*03:04:51| C*03:04:52| C*03:04:53| C*03:04:54| C*03:04:55| C*03:04:56| C*03:04:57| C*03:04:58| C*03:04:59| C*03:04:60| C*03:04:61| C*03:04:62| C*03:04:63| C*03:04:64| C*03:04:65| C*03:04:66| C*03:04:67| C*03:04:68| C*03:04:69| C*03:04:70| C*03:04:71| C*03:04:72| C*03:04:73| C*03:06:01| C*03:06:02| C*03:08| C*03:14| C*03:17:01| C*03:17:02| C*03:23| C*03:25| C*03:26:01| C*03:26:02| C*03:27| C*03:28| C*03:29| C*03:32| C*03:33| C*03:34| C*03:35:01| C*03:35:02:01| C*03:35:02:02| C*03:36| C*03:37:01| C*03:37:02| C*03:38:01| C*03:38:02| C*03:41:01| C*03:41:02| C*03:46</t>
+  </si>
+  <si>
+    <t>C*04:01:01:01| C*04:01:01:02| C*04:01:01:03| C*04:01:01:04| C*04:01:01:05| C*04:01:01:06| C*04:01:01:07| C*04:01:01:08| C*04:01:01:09| C*04:01:01:10| C*04:01:01:11| C*04:01:01:12| C*04:01:01:13| C*04:01:01:14| C*04:01:01:15| C*04:01:01:16| C*04:01:01:17| C*04:01:01:18| C*04:01:01:19| C*04:01:01:20| C*04:01:01:21| C*04:01:01:22| C*04:01:01:23| C*04:01:01:24| C*04:01:01:25| C*04:01:01:26| C*04:01:01:27| C*04:01:01:28| C*04:01:01:29| C*04:01:01:31| C*04:01:01:32| C*04:01:01:33| C*04:01:02| C*04:01:03| C*04:01:04| C*04:01:05| C*04:01:06| C*04:01:07| C*04:01:08| C*04:01:09| C*04:01:10| C*04:01:11| C*04:01:12| C*04:01:13| C*04:01:14| C*04:01:15| C*04:01:16| C*04:01:17| C*04:01:18| C*04:01:19| C*04:01:20| C*04:01:21| C*04:01:22| C*04:01:23| C*04:01:24| C*04:01:25| C*04:01:26| C*04:01:27| C*04:01:28| C*04:01:29| C*04:01:30| C*04:01:31| C*04:01:32| C*04:01:33| C*04:01:34| C*04:01:35| C*04:01:36| C*04:01:37| C*04:01:38| C*04:01:39| C*04:01:40| C*04:01:41| C*04:01:42| C*04:01:43| C*04:01:44| C*04:01:45| C*04:01:46| C*04:01:47| C*04:01:48| C*04:01:49| C*04:01:50| C*04:01:51| C*04:01:52| C*04:01:53| C*04:01:54| C*04:01:55| C*04:01:56| C*04:01:57| C*04:01:58| C*04:01:59| C*04:01:60| C*04:01:61| C*04:01:62| C*04:01:63| C*04:01:64| C*04:01:65| C*04:01:66| C*04:01:67| C*04:01:68| C*04:01:69| C*04:01:70| C*04:01:71| C*04:01:72| C*04:01:73| C*04:01:74| C*04:01:75| C*04:01:76| C*04:01:77| C*04:01:78| C*04:01:79| C*04:01:80| C*04:01:81| C*04:01:82| C*04:01:83| C*04:01:84| C*04:01:85| C*04:01:86| C*04:01:87| C*04:01:88| C*04:01:89| C*04:01:90| C*04:01:91| C*04:01:92| C*04:01:93| C*04:01:94| C*04:01:95| C*04:01:96| C*04:01:97| C*04:01:98| C*04:01:99| C*04:01:100| C*04:01:101| C*04:01:102| C*04:01:103| C*04:01:104| C*04:01:105| C*04:01:106| C*04:01:107| C*04:01:108| C*04:01:109| C*04:01:110| C*04:01:111| C*04:01:112| C*04:01:113| C*04:03:01:01| C*04:03:01:02| C*04:03:02| C*04:03:03| C*04:03:04| C*04:03:05| C*04:04:01:01| C*04:04:01:02| C*04:04:02| C*04:05| C*04:06:01| C*04:06:02| C*04:07:01| C*04:07:02| C*04:08| C*04:10| C*04:11| C*04:12| C*04:13:01:01| C*04:13:01:02| C*04:14| C*04:15:01| C*04:15:02| C*04:15:03| C*04:16| C*04:17| C*04:18| C*04:19| C*04:20| C*04:23| C*04:24| C*04:25| C*04:26| C*04:27| C*04:28| C*04:29| C*04:30| C*04:31| C*04:32| C*04:33| C*04:34| C*04:35| C*04:36| C*04:37| C*04:38| C*04:39| C*04:40| C*04:41| C*04:42:01| C*04:42:02| C*04:43| C*04:44| C*04:45| C*04:46| C*04:47| C*04:48| C*04:49| C*04:50| C*04:51| C*04:52| C*04:53| C*04:54:01| C*04:54:02| C*04:55| C*04:56| C*04:57| C*04:58| C*04:59Q| C*04:60| C*04:61| C*04:62| C*04:63| C*04:64:01| C*04:64:02| C*04:65| C*04:66| C*04:67| C*04:68| C*04:69| C*04:70| C*04:71| C*04:72| C*04:73| C*04:74| C*04:75| C*04:76| C*04:77| C*04:78| C*04:79| C*04:80| C*04:81| C*04:82| C*04:83| C*04:84| C*04:85| C*04:86| C*04:87| C*04:89| C*04:90| C*04:91| C*04:92| C*04:94:01| C*04:94:02| C*04:96| C*04:97| C*04:98:01| C*04:98:02| C*04:99| C*04:100| C*04:101| C*04:102| C*04:103| C*04:104| C*04:106| C*04:107| C*04:108| C*04:109| C*04:110| C*04:111| C*04:112| C*04:113| C*04:114| C*04:116| C*04:117| C*04:118| C*04:119| C*04:120| C*04:121| C*04:122| C*04:124| C*04:125| C*04:126| C*04:127| C*04:128| C*04:129| C*04:130| C*04:131| C*04:132| C*04:133| C*04:134| C*04:135| C*04:136| C*04:137| C*04:138| C*04:139| C*04:140| C*04:141| C*04:142| C*04:143| C*04:144| C*04:145| C*04:146| C*04:147| C*04:148| C*04:149| C*04:150| C*04:151| C*04:152| C*04:153| C*04:154| C*04:155| C*04:156| C*04:157| C*04:158| C*04:159| C*04:160| C*04:161| C*04:162| C*04:163| C*04:164:01| C*04:164:02| C*04:165| C*04:166:01| C*04:166:02| C*04:167| C*04:168| C*04:169| C*04:171| C*04:172| C*04:174| C*04:175| C*04:176| C*04:177| C*04:178| C*04:179| C*04:180:01| C*04:180:02| C*04:181| C*04:182| C*04:183| C*04:184| C*04:185| C*04:186| C*04:187| C*04:188| C*04:189| C*04:190| C*04:192| C*04:193| C*04:194| C*04:195| C*04:196| C*04:197| C*04:198| C*04:199| C*04:200| C*04:201:01| C*04:201:02| C*04:202| C*04:204| C*04:206| C*04:207| C*04:208| C*04:209| C*04:210| C*04:211| C*04:212| C*04:213| C*04:214| C*04:216| C*04:218| C*04:219| C*04:220| C*04:221| C*04:222| C*04:223:01| C*04:223:02| C*04:224| C*04:226| C*04:227| C*04:228| C*04:229| C*04:230| C*04:231| C*04:232| C*04:235| C*04:237| C*04:238| C*04:239| C*04:240| C*04:241| C*04:242| C*04:243| C*04:244| C*04:245| C*04:246| C*04:247| C*04:248| C*04:249| C*04:250| C*04:251| C*04:252| C*04:254| C*04:256| C*04:257| C*04:258| C*04:259| C*04:260| C*04:261| C*04:262| C*04:263| C*04:264| C*04:265| C*04:266| C*04:267| C*04:268| C*04:269| C*04:270| C*04:271| C*04:272| C*04:273| C*04:274| C*04:275| C*04:276| C*04:277| C*04:278| C*04:280| C*04:281| C*04:282| C*04:283| C*04:284| C*04:285| C*04:286| C*04:287| C*04:288| C*04:289| C*04:290| C*04:291| C*04:292| C*04:293| C*04:294| C*04:295| C*04:296| C*04:297| C*04:298| C*04:299| C*04:301| C*04:302| C*04:303| C*04:304| C*04:306| C*04:307| C*04:308| C*04:310| C*04:311| C*04:312| C*04:313:01:01| C*04:313:01:02| C*04:314| C*04:315| C*04:316| C*04:317| C*04:318| C*04:319| C*04:320| C*04:321| C*04:322| C*04:323| C*04:324| C*04:325| C*04:326| C*04:327| C*04:328| C*04:329| C*04:330| C*04:331| C*04:332| C*04:333| C*04:334| C*04:335| C*04:336| C*04:337| C*04:338| C*04:339:01| C*04:339:02| C*04:340| C*04:341| C*04:342| C*04:343| C*04:344| C*04:345| C*04:346| C*04:347| C*04:348| C*04:351| C*04:352| C*04:353| C*04:354| C*04:355| C*04:356| C*04:357| C*04:358| C*04:359</t>
+  </si>
+  <si>
+    <t>C*05:01:01:01| C*05:01:01:02| C*05:01:01:03| C*05:01:01:04| C*05:01:01:05| C*05:01:01:06| C*05:01:01:07| C*05:01:01:08| C*05:01:01:09| C*05:01:01:10| C*05:01:01:11| C*05:01:01:12| C*05:01:01:13| C*05:01:01:14| C*05:01:01:15| C*05:01:01:16| C*05:01:02| C*05:01:03| C*05:01:04| C*05:01:05| C*05:01:06| C*05:01:07| C*05:01:08| C*05:01:09| C*05:01:10| C*05:01:11| C*05:01:12| C*05:01:13| C*05:01:14| C*05:01:15| C*05:01:16| C*05:01:17| C*05:01:18| C*05:01:19| C*05:01:20| C*05:01:21| C*05:01:22| C*05:01:23| C*05:01:24| C*05:01:25| C*05:01:26| C*05:01:27| C*05:01:28| C*05:01:29| C*05:01:30| C*05:01:31| C*05:01:32| C*05:01:33| C*05:01:34| C*05:01:35| C*05:01:36| C*05:01:37| C*05:01:38| C*05:01:39| C*05:01:40| C*05:01:41| C*05:01:42| C*05:01:43| C*05:01:44| C*05:01:45| C*05:03| C*05:04:01| C*05:04:02| C*05:05:01| C*05:05:02| C*05:06| C*05:08| C*05:09:01| C*05:09:02| C*05:09:03| C*05:10| C*05:11| C*05:12| C*05:13| C*05:14| C*05:15| C*05:16| C*05:17| C*05:18:01| C*05:18:02| C*05:18:03| C*05:18:04| C*05:18:05| C*05:19| C*05:20| C*05:21| C*05:22:01| C*05:22:02| C*05:23| C*05:24| C*05:25| C*05:26| C*05:27| C*05:28| C*05:29:01| C*05:29:02| C*05:30| C*05:31| C*05:32| C*05:33| C*05:34| C*05:35| C*05:36| C*05:37| C*05:38| C*05:39| C*05:40| C*05:41| C*05:42| C*05:43| C*05:44:01| C*05:44:02| C*05:45| C*05:46| C*05:47| C*05:49| C*05:50| C*05:51Q| C*05:52| C*05:53| C*05:54| C*05:55| C*05:56| C*05:57| C*05:58:01| C*05:58:02| C*05:58:03| C*05:58:04| C*05:59| C*05:60| C*05:61| C*05:62| C*05:63| C*05:64:01| C*05:64:02| C*05:65| C*05:66| C*05:67| C*05:68| C*05:69| C*05:70| C*05:71| C*05:72| C*05:73| C*05:74| C*05:75| C*05:76| C*05:77| C*05:78:01| C*05:78:02| C*05:79| C*05:80| C*05:81| C*05:82| C*05:83| C*05:84| C*05:85| C*05:86| C*05:87| C*05:88| C*05:89| C*05:90| C*05:93| C*05:94| C*05:95| C*05:96| C*05:97| C*05:98| C*05:100| C*05:101| C*05:102| C*05:103:01| C*05:103:02| C*05:104| C*05:105| C*05:106:01| C*05:106:02| C*05:107| C*05:108| C*05:109| C*05:110| C*05:111| C*05:112| C*05:114| C*05:115| C*05:116| C*05:117| C*05:118| C*05:119| C*05:120| C*05:121| C*05:122| C*05:123| C*05:124| C*05:125| C*05:126| C*05:127| C*05:129| C*05:130| C*05:131| C*05:132| C*05:133| C*05:134| C*05:135| C*05:136| C*05:137| C*05:138| C*05:139| C*05:140| C*05:141| C*05:142| C*05:143| C*05:144| C*05:145| C*05:146| C*05:147| C*05:148| C*05:149| C*05:150| C*05:151| C*05:152| C*05:155| C*05:156| C*05:157| C*05:158| C*05:159| C*05:160| C*05:161| C*05:162| C*05:163| C*05:164| C*05:165| C*05:166| C*05:167| C*05:168| C*05:170| C*05:171:01:01| C*05:171:01:02| C*05:172| C*05:173| C*05:174| C*05:176| C*05:177| C*05:178| C*05:179| C*05:181| C*05:182| C*05:183| C*05:184| C*05:185| C*05:186| C*05:187| C*05:188| C*05:189| C*05:190| C*05:191| C*05:192| C*05:193| C*05:194| C*05:195| C*05:196| C*05:197| C*05:198| C*05:199| C*05:200| C*05:201| C*05:202Q| C*05:203</t>
+  </si>
+  <si>
+    <t>C*06:02:01:01| C*06:02:01:02| C*06:02:01:03| C*06:02:01:04| C*06:02:01:05| C*06:02:01:06| C*06:02:01:07| C*06:02:01:08| C*06:02:01:09| C*06:02:01:10| C*06:02:01:11| C*06:02:01:12| C*06:02:01:13| C*06:02:01:14| C*06:02:01:15| C*06:02:01:16| C*06:02:01:17| C*06:02:03| C*06:02:04| C*06:02:05| C*06:02:06| C*06:02:07| C*06:02:08| C*06:02:09| C*06:02:10| C*06:02:11| C*06:02:12| C*06:02:13| C*06:02:14| C*06:02:15| C*06:02:16| C*06:02:17| C*06:02:18| C*06:02:19| C*06:02:20| C*06:02:21| C*06:02:22| C*06:02:23| C*06:02:24| C*06:02:25| C*06:02:26| C*06:02:27| C*06:02:28| C*06:02:29| C*06:02:30| C*06:02:31| C*06:02:32| C*06:02:33| C*06:02:34| C*06:02:35| C*06:02:36| C*06:02:37| C*06:02:38| C*06:02:39| C*06:02:40| C*06:02:41| C*06:02:42| C*06:02:43| C*06:02:44| C*06:02:45| C*06:02:46| C*06:02:47| C*06:02:48| C*06:02:49| C*06:02:50:01| C*06:02:50:02| C*06:02:51| C*06:02:52| C*06:02:53| C*06:02:54| C*06:02:55| C*06:02:56| C*06:02:57| C*06:02:58| C*06:02:59| C*06:02:60| C*06:02:61| C*06:02:62| C*06:02:63| C*06:02:64| C*06:02:65| C*06:02:66| C*06:02:67| C*06:02:68| C*06:02:69| C*06:02:70| C*06:02:71| C*06:03:01| C*06:03:02| C*06:04:01| C*06:04:02| C*06:05| C*06:06| C*06:07| C*06:08| C*06:09:01| C*06:09:02| C*06:10| C*06:11| C*06:12| C*06:13| C*06:14| C*06:15| C*06:17| C*06:18| C*06:19| C*06:20| C*06:21| C*06:22| C*06:23| C*06:24| C*06:25| C*06:26| C*06:27| C*06:28| C*06:29| C*06:30| C*06:31| C*06:32| C*06:33| C*06:34:01| C*06:34:02| C*06:35| C*06:36| C*06:37| C*06:38| C*06:39| C*06:40| C*06:41| C*06:42:01| C*06:42:02| C*06:43:01| C*06:43:02| C*06:44| C*06:45| C*06:47| C*06:48| C*06:50| C*06:51| C*06:52| C*06:53:01| C*06:53:02| C*06:54| C*06:55| C*06:56| C*06:57| C*06:58| C*06:59| C*06:60| C*06:61| C*06:62| C*06:63| C*06:64| C*06:65| C*06:66| C*06:67| C*06:68| C*06:69| C*06:70:01| C*06:70:02| C*06:71| C*06:72| C*06:73| C*06:74Q| C*06:75| C*06:76:01| C*06:76:02| C*06:77| C*06:78| C*06:80| C*06:81| C*06:82| C*06:83| C*06:84| C*06:85| C*06:86| C*06:87| C*06:88| C*06:89| C*06:90| C*06:91| C*06:92| C*06:93| C*06:94| C*06:95| C*06:96| C*06:97| C*06:98| C*06:99| C*06:100| C*06:101| C*06:102:01| C*06:102:02| C*06:103| C*06:104| C*06:105| C*06:106:01| C*06:106:02| C*06:107| C*06:108| C*06:109| C*06:110| C*06:111| C*06:112| C*06:113| C*06:114| C*06:115| C*06:117| C*06:118| C*06:119| C*06:120| C*06:121| C*06:122| C*06:123| C*06:124| C*06:125| C*06:126| C*06:127:01:01| C*06:127:01:02| C*06:127:02| C*06:129| C*06:130| C*06:131| C*06:132:01| C*06:132:02| C*06:133| C*06:135| C*06:136| C*06:137| C*06:138| C*06:139| C*06:140| C*06:141| C*06:142| C*06:143| C*06:144| C*06:145| C*06:146| C*06:147| C*06:148| C*06:149| C*06:150| C*06:151| C*06:153| C*06:154| C*06:155:01:01| C*06:155:01:02| C*06:156| C*06:157| C*06:158| C*06:159| C*06:160| C*06:161| C*06:162| C*06:163| C*06:164| C*06:165| C*06:166| C*06:167| C*06:168| C*06:169| C*06:170| C*06:172| C*06:173| C*06:174| C*06:176| C*06:177| C*06:178| C*06:179| C*06:180| C*06:181| C*06:182| C*06:183| C*06:184| C*06:185| C*06:186| C*06:187| C*06:188| C*06:189| C*06:190| C*06:191| C*06:192| C*06:193| C*06:194| C*06:195| C*06:196| C*06:197| C*06:198| C*06:199| C*06:200Q| C*06:201| C*06:202| C*06:203| C*06:204| C*06:205| C*06:206| C*06:207| C*06:209| C*06:210| C*06:212| C*06:213| C*06:214| C*06:216| C*06:217| C*06:218| C*06:219| C*06:221| C*06:222| C*06:223| C*06:224| C*06:225| C*06:226| C*06:227| C*06:228| C*06:229| C*06:230| C*06:231| C*06:232| C*06:233| C*06:234| C*06:235| C*06:236| C*06:237| C*06:238| C*06:239| C*06:240| C*06:241| C*06:242| C*06:243| C*06:244| C*06:245| C*06:246| C*06:247| C*06:248| C*06:249| C*06:250| C*06:251| C*18:01| C*18:02:01| C*18:02:02| C*18:02:03</t>
+  </si>
+  <si>
+    <t>C*07:01:01:01| C*07:01:01:02| C*07:01:01:03| C*07:01:01:04| C*07:01:01:05| C*07:01:01:06| C*07:01:01:07| C*07:01:01:08| C*07:01:01:09| C*07:01:01:10| C*07:01:01:11| C*07:01:01:12| C*07:01:01:13| C*07:01:01:14Q| C*07:01:01:15| C*07:01:01:16| C*07:01:01:17| C*07:01:01:18| C*07:01:01:19| C*07:01:01:20| C*07:01:01:21| C*07:01:01:22| C*07:01:01:23| C*07:01:01:24| C*07:01:01:25| C*07:01:01:26| C*07:01:01:27| C*07:01:01:28| C*07:01:02| C*07:01:03| C*07:01:04| C*07:01:05| C*07:01:06| C*07:01:07| C*07:01:08| C*07:01:09| C*07:01:10| C*07:01:11| C*07:01:12| C*07:01:13| C*07:01:14| C*07:01:15| C*07:01:16| C*07:01:17| C*07:01:18| C*07:01:19| C*07:01:20| C*07:01:21| C*07:01:22| C*07:01:23| C*07:01:24| C*07:01:25| C*07:01:26| C*07:01:27| C*07:01:28| C*07:01:29| C*07:01:30| C*07:01:31| C*07:01:32| C*07:01:33| C*07:01:34| C*07:01:35| C*07:01:36| C*07:01:37| C*07:01:38| C*07:01:39| C*07:01:40| C*07:01:41| C*07:01:42| C*07:01:43| C*07:01:44| C*07:01:45| C*07:01:46| C*07:01:47| C*07:01:48| C*07:01:49| C*07:01:50| C*07:01:51| C*07:01:52| C*07:01:53| C*07:01:54| C*07:01:55| C*07:01:56| C*07:01:57| C*07:01:58| C*07:01:59| C*07:01:60| C*07:01:61| C*07:01:62| C*07:01:63| C*07:01:64| C*07:01:65| C*07:01:66| C*07:01:67| C*07:01:68| C*07:01:69| C*07:01:70| C*07:01:71| C*07:01:72| C*07:01:73| C*07:01:74| C*07:01:75| C*07:01:76| C*07:01:77| C*07:02:01:01| C*07:02:01:02| C*07:02:01:03| C*07:02:01:04| C*07:02:01:05| C*07:02:01:06| C*07:02:01:07| C*07:02:01:08| C*07:02:01:09| C*07:02:01:10| C*07:02:01:11| C*07:02:01:12| C*07:02:01:13| C*07:02:01:14| C*07:02:01:15| C*07:02:01:16| C*07:02:01:18| C*07:02:01:19| C*07:02:01:20| C*07:02:01:21| C*07:02:01:22| C*07:02:01:23| C*07:02:01:24| C*07:02:01:25| C*07:02:01:26| C*07:02:01:27| C*07:02:01:28| C*07:02:01:29| C*07:02:01:30| C*07:02:01:31| C*07:02:01:32| C*07:02:01:33| C*07:02:01:34| C*07:02:01:35| C*07:02:01:36| C*07:02:02| C*07:02:03| C*07:02:04| C*07:02:05| C*07:02:06| C*07:02:07| C*07:02:08| C*07:02:09| C*07:02:10| C*07:02:11| C*07:02:12| C*07:02:13| C*07:02:14| C*07:02:15| C*07:02:16| C*07:02:17| C*07:02:18| C*07:02:19| C*07:02:20| C*07:02:21| C*07:02:22| C*07:02:23| C*07:02:24| C*07:02:25| C*07:02:26| C*07:02:27| C*07:02:28| C*07:02:29| C*07:02:30| C*07:02:31| C*07:02:32| C*07:02:33| C*07:02:34| C*07:02:35| C*07:02:36| C*07:02:37| C*07:02:38| C*07:02:39| C*07:02:40| C*07:02:41| C*07:02:42| C*07:02:43| C*07:02:44| C*07:02:45| C*07:02:46| C*07:02:47| C*07:02:48| C*07:02:49| C*07:02:50| C*07:02:51| C*07:02:52| C*07:02:53| C*07:02:54| C*07:02:55| C*07:02:56| C*07:02:57| C*07:02:58| C*07:02:59| C*07:02:60| C*07:02:61| C*07:02:62| C*07:02:63| C*07:02:64| C*07:02:65| C*07:02:66| C*07:02:67| C*07:02:68| C*07:02:69| C*07:02:70| C*07:02:71| C*07:02:72| C*07:02:73| C*07:02:74| C*07:02:75| C*07:02:76| C*07:02:77| C*07:02:78| C*07:02:79| C*07:02:80| C*07:02:81| C*07:02:82| C*07:02:83| C*07:02:84| C*07:02:85| C*07:02:86| C*07:02:87| C*07:02:88| C*07:02:89| C*07:02:90| C*07:02:91| C*07:02:92| C*07:02:93| C*07:02:94| C*07:02:95| C*07:02:96| C*07:02:97| C*07:02:98| C*07:02:99| C*07:02:100| C*07:02:101| C*07:02:102| C*07:02:103| C*07:02:104:01| C*07:02:104:02| C*07:03| C*07:04:01:01| C*07:04:01:02| C*07:04:01:03| C*07:04:01:04| C*07:04:02:01| C*07:04:02:02| C*07:04:03| C*07:04:04| C*07:04:05| C*07:04:06| C*07:04:07| C*07:04:08| C*07:04:09| C*07:04:10| C*07:04:11| C*07:04:12| C*07:04:13| C*07:04:14| C*07:04:15| C*07:04:16| C*07:04:17| C*07:04:18| C*07:05| C*07:06:01:01| C*07:06:01:02| C*07:06:02| C*07:07| C*07:08| C*07:09| C*07:10| C*07:11| C*07:12| C*07:13| C*07:14| C*07:15| C*07:16| C*07:17:01| C*07:17:02| C*07:17:03| C*07:17:04| C*07:18:01:01| C*07:18:01:02| C*07:18:01:03| C*07:18:02| C*07:18:03| C*07:19| C*07:20| C*07:21| C*07:22| C*07:23| C*07:24| C*07:25| C*07:26:01| C*07:26:02| C*07:26:03| C*07:27:01| C*07:27:02| C*07:28| C*07:29:01| C*07:29:02| C*07:30| C*07:31:01| C*07:31:02| C*07:35| C*07:36| C*07:37| C*07:38:01| C*07:38:02| C*07:39| C*07:40| C*07:41| C*07:42| C*07:43:01| C*07:43:02| C*07:44| C*07:45| C*07:46| C*07:47| C*07:48| C*07:49| C*07:50| C*07:51| C*07:52| C*07:53| C*07:54| C*07:56:01| C*07:56:02| C*07:57| C*07:58| C*07:59| C*07:60| C*07:62| C*07:63| C*07:64| C*07:65| C*07:66| C*07:67| C*07:68| C*07:69| C*07:70| C*07:71| C*07:72| C*07:73:01| C*07:73:02| C*07:74| C*07:75| C*07:76:01| C*07:76:02| C*07:77| C*07:78:01| C*07:78:02| C*07:79| C*07:80| C*07:81| C*07:82| C*07:83| C*07:84| C*07:85| C*07:86| C*07:87| C*07:88| C*07:89| C*07:90| C*07:91| C*07:92| C*07:93| C*07:94| C*07:95| C*07:96:01| C*07:96:02| C*07:97| C*07:99| C*07:100| C*07:101| C*07:102| C*07:103| C*07:105| C*07:106| C*07:107| C*07:108:01| C*07:108:02| C*07:109:01| C*07:109:02| C*07:110| C*07:111| C*07:112| C*07:113| C*07:114| C*07:115| C*07:116| C*07:117| C*07:118| C*07:119| C*07:120| C*07:121Q| C*07:122| C*07:123| C*07:124| C*07:125| C*07:126| C*07:127:01| C*07:127:02| C*07:128| C*07:129| C*07:130| C*07:131:01| C*07:131:02| C*07:132| C*07:133:01| C*07:133:02| C*07:134| C*07:135| C*07:136| C*07:137:01| C*07:137:02| C*07:138| C*07:139| C*07:140| C*07:141:01| C*07:141:02| C*07:142| C*07:143| C*07:144| C*07:145| C*07:146| C*07:147| C*07:148| C*07:149| C*07:150Q| C*07:151| C*07:153| C*07:154| C*07:155| C*07:156| C*07:157| C*07:158| C*07:159| C*07:160| C*07:161| C*07:162| C*07:163| C*07:165| C*07:166| C*07:167| C*07:168| C*07:169| C*07:170| C*07:171| C*07:172:01| C*07:172:02| C*07:173| C*07:174| C*07:175| C*07:176| C*07:177| C*07:178| C*07:179| C*07:180| C*07:181| C*07:182| C*07:183| C*07:184| C*07:185| C*07:186| C*07:187| C*07:188| C*07:189| C*07:190| C*07:192| C*07:193| C*07:194| C*07:195| C*07:196| C*07:197| C*07:199:01| C*07:199:02| C*07:200| C*07:201| C*07:202| C*07:203| C*07:204:01| C*07:204:02| C*07:205| C*07:206| C*07:207| C*07:208| C*07:209| C*07:210| C*07:211| C*07:212| C*07:213| C*07:214| C*07:215| C*07:216| C*07:217| C*07:218| C*07:219| C*07:220| C*07:221| C*07:222| C*07:223| C*07:224| C*07:225| C*07:226| C*07:228| C*07:229| C*07:230| C*07:231| C*07:232| C*07:233| C*07:234| C*07:235Q| C*07:236| C*07:237| C*07:238| C*07:239| C*07:240| C*07:241| C*07:242| C*07:243| C*07:244| C*07:245| C*07:246:01| C*07:246:02| C*07:247| C*07:248| C*07:249| C*07:250| C*07:251| C*07:252| C*07:253| C*07:254| C*07:255| C*07:256| C*07:257:01| C*07:257:02| C*07:257:03| C*07:257:04| C*07:258| C*07:259| C*07:260:01| C*07:260:02| C*07:261| C*07:262| C*07:263| C*07:265| C*07:266| C*07:267| C*07:268| C*07:269| C*07:270| C*07:271| C*07:272| C*07:273| C*07:274| C*07:275| C*07:276| C*07:277| C*07:278| C*07:279| C*07:280| C*07:281| C*07:282| C*07:283| C*07:284| C*07:285| C*07:286| C*07:287| C*07:288| C*07:289| C*07:290| C*07:291| C*07:292| C*07:293| C*07:294| C*07:296| C*07:297| C*07:298| C*07:299| C*07:300| C*07:301| C*07:302| C*07:303| C*07:304| C*07:305| C*07:306| C*07:307| C*07:308| C*07:309| C*07:310| C*07:311| C*07:312| C*07:313| C*07:314:01| C*07:314:02| C*07:314:03| C*07:315| C*07:316| C*07:317| C*07:318| C*07:319| C*07:320| C*07:321| C*07:322| C*07:323| C*07:324| C*07:325| C*07:326| C*07:327| C*07:328| C*07:330:01| C*07:330:02| C*07:331| C*07:332| C*07:333| C*07:334| C*07:335| C*07:336| C*07:337| C*07:338| C*07:339| C*07:340| C*07:341:01| C*07:341:02| C*07:342| C*07:343:01:01| C*07:343:01:02| C*07:344| C*07:345| C*07:346| C*07:348| C*07:349| C*07:351| C*07:352| C*07:353| C*07:354| C*07:355| C*07:356| C*07:357| C*07:358| C*07:359| C*07:360| C*07:361| C*07:362| C*07:363| C*07:364| C*07:365| C*07:366| C*07:367| C*07:368:01| C*07:368:02| C*07:369| C*07:370| C*07:371| C*07:372| C*07:373| C*07:374| C*07:375| C*07:376| C*07:377| C*07:378| C*07:379| C*07:380| C*07:381| C*07:382| C*07:383| C*07:384| C*07:385| C*07:386| C*07:387| C*07:388| C*07:389| C*07:390| C*07:391| C*07:392| C*07:394| C*07:395| C*07:396| C*07:397| C*07:398| C*07:399| C*07:400| C*07:401| C*07:402| C*07:403| C*07:404| C*07:405| C*07:406| C*07:407| C*07:408| C*07:409| C*07:410| C*07:411| C*07:412| C*07:413| C*07:414| C*07:415| C*07:416| C*07:417| C*07:418| C*07:419| C*07:420| C*07:421| C*07:422| C*07:423| C*07:424| C*07:425| C*07:426| C*07:427| C*07:428| C*07:429| C*07:430| C*07:431| C*07:432| C*07:433| C*07:434| C*07:435| C*07:436| C*07:438| C*07:439| C*07:440| C*07:441:01| C*07:441:02| C*07:442| C*07:443| C*07:444| C*07:445| C*07:446| C*07:447| C*07:448| C*07:449| C*07:450| C*07:453| C*07:454:01| C*07:454:02| C*07:455| C*07:456| C*07:457| C*07:458| C*07:459| C*07:460| C*07:461| C*07:462| C*07:463| C*07:464| C*07:465| C*07:466| C*07:467| C*07:468| C*07:469| C*07:470| C*07:471| C*07:472| C*07:473| C*07:474| C*07:475| C*07:477| C*07:478| C*07:479| C*07:480| C*07:481| C*07:482| C*07:485| C*07:486| C*07:487| C*07:488| C*07:489| C*07:490| C*07:492| C*07:493| C*07:494Q| C*07:495| C*07:496| C*07:497| C*07:498| C*07:499| C*07:500| C*07:501| C*07:502| C*07:503| C*07:504| C*07:505| C*07:506| C*07:508| C*07:509| C*07:510| C*07:511| C*07:512| C*07:513Q| C*07:514| C*07:515| C*07:516| C*07:517| C*07:518| C*07:519| C*07:520| C*07:521:01| C*07:521:02| C*07:522| C*07:523| C*07:524| C*07:525| C*07:526:01| C*07:526:02| C*07:527| C*07:528| C*07:529| C*07:530| C*07:531| C*07:532| C*07:533| C*07:534| C*07:535| C*07:536| C*07:537| C*07:538| C*07:539| C*07:540| C*07:541| C*07:542| C*07:543| C*07:544| C*07:545| C*07:546| C*07:547| C*07:548| C*07:549| C*07:550| C*07:552| C*07:553| C*07:554| C*07:555| C*07:556| C*07:557| C*07:558:01:01| C*07:558:01:02| C*07:559| C*07:560| C*07:561| C*07:562| C*07:563| C*07:564| C*07:565| C*07:566| C*07:567| C*07:568| C*07:569| C*07:570| C*07:571| C*07:572| C*07:573| C*07:574| C*07:575| C*07:576| C*07:577| C*07:578| C*07:579| C*07:580| C*07:581| C*07:582Q| C*07:583| C*07:584| C*07:585| C*07:586| C*07:587| C*07:588| C*07:589| C*07:590| C*07:591| C*07:592| C*07:594| C*07:595| C*07:596| C*07:597| C*07:598| C*07:599| C*07:601| C*07:602| C*07:604| C*07:605| C*07:606| C*07:607| C*07:608| C*07:609| C*07:610| C*07:611| C*07:612| C*07:613| C*07:614| C*07:615| C*07:616| C*07:617| C*07:618| C*07:619| C*07:620| C*07:621| C*07:622| C*07:623| C*07:624| C*07:625| C*07:626| C*07:627| C*07:628| C*07:629| C*07:630| C*07:631| C*07:632Q| C*07:634| C*07:635| C*07:636| C*07:637| C*07:638| C*07:639| C*07:640| C*07:641| C*07:642| C*07:643| C*07:644| C*07:645| C*07:646| C*07:647| C*07:648| C*07:649| C*07:650:01| C*07:650:02| C*07:651| C*07:652| C*07:653| C*07:654| C*07:655| C*07:656| C*07:657| C*07:658| C*07:659| C*07:660| C*07:661| C*07:662| C*07:663Q| C*07:664| C*07:665| C*07:666| C*07:667| C*07:668| C*07:669| C*07:670| C*07:671| C*07:673| C*07:674| C*07:676| C*07:677| C*07:678| C*07:679| C*07:680| C*07:681| C*07:682:01:01| C*07:682:01:02| C*07:682:02| C*07:683| C*07:684| C*07:685| C*07:687| C*07:688| C*07:689| C*07:691| C*07:692| C*07:693| C*07:694| C*07:695:01:01| C*07:695:01:02| C*07:696| C*07:697Q| C*07:698| C*07:699| C*07:700| C*07:701| C*07:703| C*07:704| C*07:705| C*07:706| C*07:707| C*07:708| C*07:709| C*07:710| C*07:711| C*07:712| C*07:713| C*07:714| C*07:715| C*07:716| C*07:717| C*07:718| C*07:719| C*07:720| C*07:721| C*07:722| C*07:723| C*07:724| C*12:14:01| C*12:14:02| C*17:01:01:02| C*17:01:01:03| C*17:01:01:04| C*17:01:01:05| C*17:01:02| C*17:01:03| C*17:01:04| C*17:01:05| C*17:01:06| C*17:01:07| C*17:01:08| C*17:01:09| C*17:01:10| C*17:01:11| C*17:01:12| C*17:01:13| C*17:01:14| C*17:03:01:01| C*17:03:01:02| C*17:03:01:03| C*17:03:02</t>
+  </si>
+  <si>
+    <t>C*08:01:01:01| C*08:01:01:02| C*08:01:02| C*08:01:03| C*08:01:04| C*08:01:05| C*08:01:06| C*08:01:07| C*08:01:08| C*08:01:09| C*08:01:10| C*08:01:11| C*08:01:12| C*08:01:13| C*08:01:14| C*08:01:15| C*08:01:16| C*08:01:17| C*08:01:18| C*08:01:19| C*08:01:20| C*08:01:21| C*08:01:22| C*08:01:23| C*08:01:24| C*08:01:25| C*08:01:26| C*08:02:01:01| C*08:02:01:02| C*08:02:01:03| C*08:02:01:04| C*08:02:02| C*08:02:03| C*08:02:04| C*08:02:05| C*08:02:06| C*08:02:07| C*08:02:08| C*08:02:09| C*08:02:10| C*08:02:11| C*08:02:12| C*08:02:13| C*08:02:14| C*08:02:15| C*08:02:16| C*08:02:17| C*08:02:18| C*08:02:19| C*08:02:20| C*08:02:21| C*08:02:22| C*08:02:23| C*08:03:01| C*08:03:02| C*08:03:03| C*08:03:04| C*08:04:01| C*08:04:02| C*08:04:03| C*08:05| C*08:06| C*08:07| C*08:08:01| C*08:08:02| C*08:09| C*08:10| C*08:11| C*08:12| C*08:13| C*08:14| C*08:15:01| C*08:15:02| C*08:16:01| C*08:16:02| C*08:17| C*08:18| C*08:19:01| C*08:19:02| C*08:20| C*08:21| C*08:22| C*08:23| C*08:24| C*08:25| C*08:27| C*08:28| C*08:29| C*08:30| C*08:31| C*08:32| C*08:33:01| C*08:33:02| C*08:33:03| C*08:34| C*08:35| C*08:37| C*08:38| C*08:39| C*08:40| C*08:41| C*08:42| C*08:43| C*08:44| C*08:45| C*08:46| C*08:47| C*08:48| C*08:49| C*08:50| C*08:51| C*08:53| C*08:54| C*08:56| C*08:57| C*08:58| C*08:59| C*08:60| C*08:61| C*08:62:01| C*08:62:02| C*08:63| C*08:65| C*08:66| C*08:67| C*08:68| C*08:69| C*08:70Q| C*08:71| C*08:72:01| C*08:72:02| C*08:73| C*08:74| C*08:75| C*08:76| C*08:77| C*08:78| C*08:79| C*08:80| C*08:81| C*08:82| C*08:83| C*08:84| C*08:85| C*08:86| C*08:87| C*08:90| C*08:91| C*08:92| C*08:93| C*08:94| C*08:95| C*08:96| C*08:97| C*08:98| C*08:99| C*08:100| C*08:101| C*08:102| C*08:103| C*08:104| C*08:105| C*08:106| C*08:107| C*08:108| C*08:109| C*08:110| C*08:111| C*08:112| C*08:113| C*08:114| C*08:115| C*08:116| C*08:117| C*08:118| C*08:119| C*08:120| C*08:122| C*08:123| C*08:124| C*08:125| C*08:126| C*08:128| C*08:131| C*08:132| C*08:133| C*08:134| C*08:135| C*08:136| C*08:137| C*08:138| C*08:139| C*08:140| C*08:141Q| C*08:142| C*08:143| C*08:144:01| C*08:144:02| C*08:145| C*08:146| C*08:147| C*08:148| C*08:149| C*08:150| C*08:151| C*08:152| C*08:153| C*08:154| C*08:155| C*08:156| C*08:157| C*08:158| C*08:159| C*08:160| C*08:162| C*08:163| C*08:164| C*08:165| C*08:166| C*08:167| C*08:168| C*08:169| C*08:170| C*08:171| C*08:172| C*08:174| C*08:175| C*08:176| C*08:177| C*08:178</t>
+  </si>
+  <si>
+    <t>C*03:03:01:01| C*03:03:01:02| C*03:03:01:03| C*03:03:01:04| C*03:03:01:05| C*03:03:01:06| C*03:03:01:07| C*03:03:01:08| C*03:03:01:09| C*03:03:01:10| C*03:03:01:11| C*03:03:01:12| C*03:03:01:13| C*03:03:01:14| C*03:03:02| C*03:03:03| C*03:03:04| C*03:03:05| C*03:03:06| C*03:03:07| C*03:03:08| C*03:03:09| C*03:03:10| C*03:03:11| C*03:03:12| C*03:03:13| C*03:03:14| C*03:03:15| C*03:03:16| C*03:03:17| C*03:03:18| C*03:03:19| C*03:03:20| C*03:03:21| C*03:03:22| C*03:03:23| C*03:03:24| C*03:03:25| C*03:03:26| C*03:03:27| C*03:03:28| C*03:03:29| C*03:03:30| C*03:03:31| C*03:03:32| C*03:03:33| C*03:03:34| C*03:03:35| C*03:03:36| C*03:03:37| C*03:03:38| C*03:03:39| C*03:03:40| C*03:03:41| C*03:03:42| C*03:03:43| C*03:03:44| C*03:03:45| C*03:03:46| C*03:03:47| C*03:03:48| C*03:03:49| C*03:03:50| C*03:03:51| C*03:03:52| C*03:03:53| C*03:13:01:01| C*03:13:01:02| C*03:13:02| C*03:18:01| C*03:18:02| C*03:18:03| C*03:21| C*03:30| C*03:31</t>
+  </si>
+  <si>
+    <t>C*03:02:01| C*03:02:02:01| C*03:02:02:02| C*03:02:02:03| C*03:02:02:04| C*03:02:02:05| C*03:02:03| C*03:02:04| C*03:02:05| C*03:02:06| C*03:02:07| C*03:02:08| C*03:02:09| C*03:02:10| C*03:02:11| C*03:02:12| C*03:02:13| C*03:02:14| C*03:02:15| C*03:02:16| C*03:02:17| C*03:02:18| C*03:02:19| C*03:02:20| C*03:02:21| C*03:02:22| C*03:04:01:01| C*03:04:01:02| C*03:04:01:03| C*03:04:01:04| C*03:04:01:05| C*03:04:01:06| C*03:04:01:07| C*03:04:01:08| C*03:04:01:09| C*03:04:01:10| C*03:04:01:11| C*03:04:01:12| C*03:04:01:13| C*03:04:02| C*03:04:03| C*03:04:04| C*03:04:05| C*03:04:06| C*03:04:07| C*03:04:08| C*03:04:09| C*03:04:10| C*03:04:11| C*03:04:12| C*03:04:13| C*03:04:14| C*03:04:15| C*03:04:16| C*03:04:17| C*03:04:18| C*03:04:19| C*03:04:20| C*03:04:21| C*03:04:22| C*03:04:23| C*03:04:24| C*03:04:25| C*03:04:26| C*03:04:27| C*03:04:28| C*03:04:29| C*03:04:30| C*03:04:31| C*03:04:32| C*03:04:33| C*03:04:34| C*03:04:35| C*03:04:36| C*03:04:37| C*03:04:38| C*03:04:39| C*03:04:40| C*03:04:41| C*03:04:42| C*03:04:43| C*03:04:44| C*03:04:45| C*03:04:46| C*03:04:47| C*03:04:48| C*03:04:49| C*03:04:50| C*03:04:51| C*03:04:52| C*03:04:53| C*03:04:54| C*03:04:55| C*03:04:56| C*03:04:57| C*03:04:58| C*03:04:59| C*03:04:60| C*03:04:61| C*03:04:62| C*03:04:63| C*03:04:64| C*03:04:65| C*03:04:66| C*03:04:67| C*03:04:68| C*03:04:69| C*03:04:70| C*03:04:71| C*03:04:72| C*03:04:73| C*03:06:01| C*03:06:02| C*03:08| C*03:14| C*03:17:01| C*03:17:02| C*03:23| C*03:25| C*03:26:01| C*03:26:02| C*03:27| C*03:28| C*03:29| C*03:32| C*03:33| C*03:34| C*03:35:01| C*03:35:02:01| C*03:35:02:02| C*03:36| C*03:37:01| C*03:37:02| C*03:38:01| C*03:38:02| C*03:41:01| C*03:41:02| C*03:46</t>
+  </si>
+  <si>
+    <t>C*12:02:01| C*12:02:02:01| C*12:02:02:02| C*12:02:02:03| C*12:02:03| C*12:02:04| C*12:02:05| C*12:02:06| C*12:02:07| C*12:02:08| C*12:02:09| C*12:02:10| C*12:02:11| C*12:02:12| C*12:02:13| C*12:02:14| C*12:02:15| C*12:02:16| C*12:02:17| C*12:02:18| C*12:02:19| C*12:02:20| C*12:02:21| C*12:02:22| C*12:02:23| C*12:02:24| C*12:02:25| C*12:03:01:01| C*12:03:01:02| C*12:03:01:03| C*12:03:01:04| C*12:03:01:05| C*12:03:01:06| C*12:03:01:07| C*12:03:01:08| C*12:03:01:09| C*12:03:01:10| C*12:03:01:11| C*12:03:01:12| C*12:03:01:13| C*12:03:02| C*12:03:03| C*12:03:04| C*12:03:05| C*12:03:06| C*12:03:07| C*12:03:08| C*12:03:09| C*12:03:10| C*12:03:11| C*12:03:12| C*12:03:13| C*12:03:14| C*12:03:15| C*12:03:16| C*12:03:17| C*12:03:18| C*12:03:19| C*12:03:20| C*12:03:21| C*12:03:22| C*12:03:23| C*12:03:24| C*12:03:25| C*12:03:26| C*12:03:27| C*12:03:28| C*12:03:29| C*12:03:30| C*12:03:31| C*12:03:32| C*12:03:33| C*12:03:34:01| C*12:03:34:02| C*12:03:35| C*12:03:36| C*12:03:37| C*12:03:38| C*12:03:39| C*12:03:40| C*12:03:41| C*12:03:42| C*12:03:43| C*12:03:44| C*12:03:45| C*12:03:46| C*12:03:47| C*12:03:48| C*12:03:49| C*12:03:50| C*12:03:51| C*12:03:52| C*12:03:53| C*12:03:54| C*12:03:55| C*12:04:01| C*12:04:02| C*12:05| C*12:06| C*12:07| C*12:08| C*12:09| C*12:10:01| C*12:10:02| C*12:11| C*12:12| C*12:13:01:01| C*12:13:01:02| C*12:15| C*12:16| C*12:17| C*12:18:01| C*12:18:02| C*12:19| C*12:20| C*12:21| C*12:22| C*12:23| C*12:24| C*12:25| C*12:26| C*12:27| C*12:28| C*12:29| C*12:30| C*12:31| C*12:32| C*12:33| C*12:34| C*12:35| C*12:36| C*12:37| C*12:38| C*12:40| C*12:41| C*12:42Q| C*12:43| C*12:44| C*12:45| C*12:47| C*12:48| C*12:49| C*12:50| C*12:51| C*12:52| C*12:53| C*12:54| C*12:55| C*12:56| C*12:57:01| C*12:57:02| C*12:58| C*12:59| C*12:60| C*12:61| C*12:62| C*12:63| C*12:64| C*12:65| C*12:66| C*12:67| C*12:68| C*12:69| C*12:70| C*12:71| C*12:72| C*12:73| C*12:74| C*12:75| C*12:76| C*12:77| C*12:78| C*12:79| C*12:81| C*12:82| C*12:83| C*12:85| C*12:86| C*12:87| C*12:88| C*12:89| C*12:90| C*12:91| C*12:92| C*12:93| C*12:94| C*12:95| C*12:96| C*12:97| C*12:98| C*12:99:01| C*12:99:02| C*12:100| C*12:101| C*12:102| C*12:103| C*12:106| C*12:107| C*12:108| C*12:109| C*12:110| C*12:111| C*12:112| C*12:113| C*12:114| C*12:115| C*12:116| C*12:117| C*12:118| C*12:119| C*12:120| C*12:121| C*12:122| C*12:123| C*12:124| C*12:125| C*12:126| C*12:127| C*12:128| C*12:129| C*12:130| C*12:131| C*12:132| C*12:133| C*12:134| C*12:135| C*12:136| C*12:137| C*12:138| C*12:139| C*12:140:01| C*12:140:02| C*12:141| C*12:142| C*12:143| C*12:144| C*12:145| C*12:146| C*12:147| C*12:149| C*12:150| C*12:151| C*12:152| C*12:153| C*12:154| C*12:155Q| C*12:156| C*12:157| C*12:158| C*12:159| C*12:160| C*12:161| C*12:162| C*12:163| C*12:164| C*12:165| C*12:166| C*12:167| C*12:168| C*12:169| C*12:170| C*12:171| C*12:172| C*12:173| C*12:174| C*12:175| C*12:176| C*12:177| C*12:178| C*12:179| C*12:180| C*12:181| C*12:182| C*12:183| C*12:184| C*12:185| C*12:186| C*12:187| C*12:188| C*12:189| C*12:190| C*12:191| C*12:192| C*12:193| C*12:194| C*12:195:01| C*12:195:02| C*12:195:03| C*12:196| C*12:197| C*12:198| C*12:199| C*12:200| C*12:201| C*12:202| C*12:203| C*12:204| C*12:205| C*12:206| C*12:207| C*12:208| C*12:209| C*12:210| C*12:211| C*12:212| C*12:213| C*12:214| C*12:215| C*12:216| C*12:217| C*12:218| C*12:220| C*12:221| C*12:222| C*12:223| C*12:224| C*12:225| C*12:226| C*12:227| C*12:228| C*12:229| C*12:230| C*12:231| C*12:233| C*12:234| C*12:235| C*12:237| C*12:238| C*12:239| C*12:240| C*12:241| C*12:242| C*12:243| C*12:244| C*12:245| C*12:246| C*12:247| C*12:248| C*12:249| C*12:250| C*12:251| C*12:252| C*12:253| C*12:254| C*12:255| C*12:256| C*12:257| C*12:258| C*12:259| C*12:260| C*12:261| C*12:262| C*12:263| C*12:264| C*12:265| C*12:266| C*12:267</t>
+  </si>
+  <si>
+    <t>C*14:04| C*14:06| C*14:09| C*14:10| C*14:11| C*14:12| C*14:13| C*14:14| C*14:15| C*14:16| C*14:17| C*14:18| C*14:19| C*14:20| C*14:22| C*14:23| C*14:24:01| C*14:24:02| C*14:25| C*14:26| C*14:27| C*14:28:01| C*14:28:02| C*14:29| C*14:30| C*14:31| C*14:32| C*14:33| C*14:34| C*14:36| C*14:37| C*14:38| C*14:39| C*14:40| C*14:41| C*14:42| C*14:43| C*14:44| C*14:45| C*14:46:01| C*14:46:02| C*14:48| C*14:49| C*14:50| C*14:51| C*14:52| C*14:53| C*14:54| C*14:55| C*14:56| C*14:57| C*14:58| C*14:59| C*14:60| C*14:61| C*14:62| C*14:63| C*14:64| C*14:65| C*14:66| C*14:67| C*14:68| C*14:69| C*14:70| C*14:71| C*14:72| C*14:73| C*14:74| C*14:75| C*14:76| C*14:77| C*14:78| C*14:79| C*14:80| C*14:81| C*14:82| C*14:83| C*14:84| C*14:85| C*14:86| C*14:87| C*14:88| C*14:89| C*14:90| C*14:91| C*14:92| C*14:94| C*14:95| C*14:96| C*14:98| C*14:100| C*14:101| C*14:102| C*14:103| C*14:104</t>
+  </si>
+  <si>
+    <t>C*15:02:01:01| C*15:02:01:02| C*15:02:01:03| C*15:02:01:04| C*15:02:01:05| C*15:02:01:06| C*15:02:01:07| C*15:02:02:01| C*15:02:02:02| C*15:02:03| C*15:02:04| C*15:02:05| C*15:02:06| C*15:02:07| C*15:02:08| C*15:02:09| C*15:02:10| C*15:02:11| C*15:02:12| C*15:02:13| C*15:02:14| C*15:02:15| C*15:02:16| C*15:02:17| C*15:02:18| C*15:02:19| C*15:02:20| C*15:02:21| C*15:02:22| C*15:02:23| C*15:02:24| C*15:02:25| C*15:02:26| C*15:02:27| C*15:02:28| C*15:02:29| C*15:02:30| C*15:02:31| C*15:02:32| C*15:02:33| C*15:02:34| C*15:02:35| C*15:02:36| C*15:02:37| C*15:02:38| C*15:02:39| C*15:02:40| C*15:03| C*15:04:01| C*15:04:02| C*15:04:03| C*15:05:01:01| C*15:05:01:02| C*15:05:02:01| C*15:05:02:02| C*15:05:03| C*15:05:04| C*15:05:05| C*15:05:06| C*15:05:07| C*15:05:08| C*15:05:09| C*15:05:10| C*15:05:11| C*15:05:12| C*15:05:13| C*15:05:14| C*15:05:15| C*15:06:01| C*15:06:02| C*15:06:03| C*15:08:01| C*15:08:02| C*15:09| C*15:10:01| C*15:10:02| C*15:10:03| C*15:10:04| C*15:11| C*15:12| C*15:13:01:01| C*15:13:01:02| C*15:15| C*15:16| C*15:17| C*15:18| C*15:19| C*15:22| C*15:23:01| C*15:23:02| C*15:24| C*15:25| C*15:26| C*15:27| C*15:28| C*15:29| C*15:30| C*15:31| C*15:32Q| C*15:33| C*15:34| C*15:35| C*15:36| C*15:37| C*15:38| C*15:39| C*15:40| C*15:41| C*15:42| C*15:43| C*15:44:01| C*15:44:02| C*15:45| C*15:46| C*15:47| C*15:48| C*15:49| C*15:50| C*15:51| C*15:52| C*15:53| C*15:54| C*15:55| C*15:56| C*15:57| C*15:58| C*15:59| C*15:60| C*15:61| C*15:62| C*15:63| C*15:64| C*15:65| C*15:66| C*15:67| C*15:68| C*15:69| C*15:70| C*15:71| C*15:72| C*15:73| C*15:74| C*15:75| C*15:76| C*15:77| C*15:78:01| C*15:78:02| C*15:79| C*15:80| C*15:81| C*15:82| C*15:83| C*15:84Q| C*15:85| C*15:86| C*15:87| C*15:88| C*15:89| C*15:90| C*15:91| C*15:93| C*15:94| C*15:96Q| C*15:97| C*15:98| C*15:99| C*15:100| C*15:101| C*15:102| C*15:103| C*15:104| C*15:105Q| C*15:106| C*15:107| C*15:108| C*15:109| C*15:110| C*15:111| C*15:112| C*15:113| C*15:114| C*15:116| C*15:117| C*15:118| C*15:119| C*15:120| C*15:121| C*15:123| C*15:124| C*15:125| C*15:126| C*15:127| C*15:128| C*15:129| C*15:130| C*15:131| C*15:132| C*15:133| C*15:134| C*15:135| C*15:136| C*15:137| C*15:138| C*15:139| C*15:140| C*15:141| C*15:142| C*15:143| C*15:144| C*15:146| C*15:147| C*15:148| C*15:149| C*15:150| C*15:151| C*15:152:01| C*15:152:02| C*15:153| C*15:154| C*15:155| C*15:157| C*15:158| C*15:159| C*15:161| C*15:162| C*15:163| C*15:165| C*15:166| C*15:167| C*15:168| C*15:169| C*15:170| C*15:171| C*15:172| C*15:173| C*15:174| C*15:175| C*15:176| C*15:178| C*15:179| C*15:180| C*15:181| C*15:182| C*15:183</t>
+  </si>
+  <si>
+    <t>C*16:01:01:01| C*16:01:01:02| C*16:01:01:03| C*16:01:01:04| C*16:01:01:05| C*16:01:01:06| C*16:01:02| C*16:01:03| C*16:01:04| C*16:01:05| C*16:01:06| C*16:01:07| C*16:01:08| C*16:01:09| C*16:01:10| C*16:01:11| C*16:01:12| C*16:01:13| C*16:01:14| C*16:01:15| C*16:01:16| C*16:01:17| C*16:01:18| C*16:01:19| C*16:01:20| C*16:01:21| C*16:01:22| C*16:01:23| C*16:01:24| C*16:01:25| C*16:01:26| C*16:01:27| C*16:01:28| C*16:01:29| C*16:01:30| C*16:01:31| C*16:01:32| C*16:02:01| C*16:02:02| C*16:02:03| C*16:02:04| C*16:02:05| C*16:02:06| C*16:02:07| C*16:02:08| C*16:02:09| C*16:02:10| C*16:02:11| C*16:02:12| C*16:02:13| C*16:02:14| C*16:02:15| C*16:02:16| C*16:04:01:01| C*16:04:01:02| C*16:04:03| C*16:04:04| C*16:04:05| C*16:06| C*16:07:01| C*16:07:02| C*16:08| C*16:09| C*16:10| C*16:11| C*16:12| C*16:13| C*16:14| C*16:15:01| C*16:15:02| C*16:16Q| C*16:17| C*16:18| C*16:19| C*16:20| C*16:21| C*16:22| C*16:23| C*16:24| C*16:25| C*16:26| C*16:27| C*16:28| C*16:29| C*16:31| C*16:32| C*16:33| C*16:34| C*16:35| C*16:36| C*16:37| C*16:38| C*16:39:01| C*16:39:02| C*16:40| C*16:41| C*16:42| C*16:43| C*16:44| C*16:45| C*16:46| C*16:47| C*16:48| C*16:49| C*16:50| C*16:51| C*16:52| C*16:53| C*16:54| C*16:55| C*16:56| C*16:57| C*16:58| C*16:59| C*16:60| C*16:61| C*16:62| C*16:63| C*16:64| C*16:65| C*16:66| C*16:67| C*16:68| C*16:69| C*16:70| C*16:71| C*16:72| C*16:73| C*16:74| C*16:75| C*16:76| C*16:78| C*16:79| C*16:80| C*16:81| C*16:82| C*16:83| C*16:84| C*16:85| C*16:86| C*16:87| C*16:88| C*16:90| C*16:91| C*16:92| C*16:93| C*16:94| C*16:95| C*16:96| C*16:97| C*16:98| C*16:99| C*16:100| C*16:101| C*16:102| C*16:103| C*16:104| C*16:105| C*16:106| C*16:107| C*16:108| C*16:109| C*16:110| C*16:111| C*16:112| C*16:113| C*16:114| C*16:115| C*16:116| C*16:117| C*16:118| C*16:119| C*16:120| C*16:121| C*16:122| C*16:124| C*16:125| C*16:126| C*16:127| C*16:128| C*16:129| C*16:130| C*16:131| C*16:133| C*16:134| C*16:135| C*16:136| C*16:137| C*16:138| C*16:139| C*16:140| C*16:141| C*16:142| C*16:143| C*16:144| C*16:145| C*16:146</t>
+  </si>
+  <si>
+    <t>C*17:02| C*17:04| C*17:05| C*17:06| C*17:07| C*17:08| C*17:09| C*17:10| C*17:11| C*17:12| C*17:13| C*17:14| C*17:15| C*17:16:01| C*17:16:02| C*17:17| C*17:18| C*17:19| C*17:20| C*17:21| C*17:22| C*17:23| C*17:24| C*17:25| C*17:26| C*17:28| C*17:29| C*17:30| C*17:31| C*17:32| C*17:33| C*17:34| C*17:35| C*17:36| C*17:37| C*17:38| C*17:39| C*17:40| C*17:41</t>
+  </si>
+  <si>
+    <t>C*18:03| C*18:04| C*18:05| C*18:06| C*18:08| C*18:09| C*18:10| C*18:11| C*18:12</t>
+  </si>
+  <si>
+    <t>DR0</t>
   </si>
   <si>
     <t>DR1</t>
   </si>
   <si>
+    <t>DR10</t>
+  </si>
+  <si>
     <t>DR103</t>
   </si>
   <si>
-    <t>DR0</t>
+    <t>DR11</t>
+  </si>
+  <si>
+    <t>DR12</t>
+  </si>
+  <si>
+    <t>DR13</t>
+  </si>
+  <si>
+    <t>DR14</t>
+  </si>
+  <si>
+    <t>DR1403</t>
+  </si>
+  <si>
+    <t>DR1404</t>
+  </si>
+  <si>
+    <t>DR15</t>
+  </si>
+  <si>
+    <t>DR16</t>
   </si>
   <si>
     <t>DR17</t>
@@ -709,115 +736,91 @@
     <t>DR18</t>
   </si>
   <si>
+    <t>DR2</t>
+  </si>
+  <si>
     <t>DR3</t>
   </si>
   <si>
     <t>DR4</t>
   </si>
   <si>
+    <t>DR6</t>
+  </si>
+  <si>
     <t>DR7</t>
   </si>
   <si>
     <t>DR8</t>
   </si>
   <si>
-    <t>DR11</t>
-  </si>
-  <si>
     <t>DR9</t>
   </si>
   <si>
-    <t>DR10</t>
-  </si>
-  <si>
-    <t>DR14</t>
-  </si>
-  <si>
-    <t>DR12</t>
-  </si>
-  <si>
-    <t>DR13</t>
-  </si>
-  <si>
-    <t>DR6</t>
-  </si>
-  <si>
-    <t>DR1403</t>
-  </si>
-  <si>
-    <t>DR1404</t>
-  </si>
-  <si>
-    <t>DR15</t>
-  </si>
-  <si>
-    <t>DR2</t>
-  </si>
-  <si>
-    <t>DR16</t>
-  </si>
-  <si>
-    <t>DRB1*01:01| DRB1*01:02| DRB1*01:04| DRB1*01:05| DRB1*01:06| DRB1*01:07| DRB1*01:08| DRB1*01:09| DRB1*01:10| DRB1*01:11| DRB1*01:12| DRB1*01:13| DRB1*01:14| DRB1*01:15| DRB1*01:16| DRB1*01:17| DRB1*01:18| DRB1*01:19| DRB1*01:20| DRB1*01:21| DRB1*01:22| DRB1*01:23| DRB1*01:24| DRB1*01:25| DRB1*01:26| DRB1*01:27| DRB1*01:28| DRB1*01:29| DRB1*01:30| DRB1*01:31| DRB1*01:32| DRB1*01:34| DRB1*01:35| DRB1*01:36| DRB1*01:37| DRB1*01:38| DRB1*01:41| DRB1*01:42| DRB1*01:43| DRB1*01:44| DRB1*01:45| DRB1*01:46| DRB1*01:47| DRB1*01:48| DRB1*01:49| DRB1*01:50| DRB1*01:51| DRB1*01:53| DRB1*01:54| DRB1*01:55| DRB1*01:56| DRB1*01:57| DRB1*01:58| DRB1*01:59| DRB1*01:60| DRB1*01:61| DRB1*01:63| DRB1*01:64| DRB1*01:65| DRB1*01:66| DRB1*01:67| DRB1*01:69| DRB1*01:70| DRB1*01:71| DRB1*01:72| DRB1*01:73| DRB1*01:74| DRB1*01:75| DRB1*01:76| DRB1*01:77| DRB1*01:78| DRB1*01:79| DRB1*01:80| DRB1*01:81| DRB1*01:82| DRB1*01:83| DRB1*01:84</t>
-  </si>
-  <si>
-    <t>DRB1*01:03</t>
-  </si>
-  <si>
-    <t>DRB1*01:33N| DRB1*01:39N| DRB1*01:40N| DRB1*01:52N| DRB1*01:62N| DRB1*01:68N| DRB1*03:67N| DRB1*03:68N| DRB1*04:81N| DRB1*04:94N| DRB1*04:119N| DRB1*04:120N| DRB1*04:142N| DRB1*04:157N| DRB1*04:158N| DRB1*04:178N| DRB1*04:186N| DRB1*04:212N| DRB1*04:214N| DRB1*07:10N| DRB1*07:26N| DRB1*07:58N| DRB1*07:68N| DRB1*08:60N| DRB1*08:78N| DRB1*11:169N| DRB1*11:217N| DRB1*12:24N| DRB1*12:31N| DRB1*12:60N| DRB1*13:113N| DRB1*13:137N| DRB1*13:142N| DRB1*13:185N| DRB1*13:200N| DRB1*14:92N| DRB1*14:137N| DRB1*14:152N| DRB1*14:166N| DRB1*14:188N| DRB1*15:17N| DRB1*15:50N| DRB1*15:80N| DRB1*15:113N| DRB1*15:115N| DRB1*15:129N| DRB1*15:134N| DRB1*15:137N| DRB1*15:138N| DRB1*16:13N| DRB1*16:21N| DRB1*16:41N| DRB3*01:26N| DRB3*01:40N| DRB3*02:29N| DRB3*02:55N| DRB3*02:67N| DRB4*01:03N| DRB4*01:16N| DRB4*01:38N| DRB4*01:54N| DRB4*01:56N| DRB4*01:57N| DRB4*01:61N| DRB4*02:01N| DRB4*03:01N| DRB5*01:08N| DRB5*01:10N| DRB5*01:27N</t>
-  </si>
-  <si>
-    <t>DRB1*03:01| DRB1*03:04| DRB1*03:10| DRB1*03:11| DRB1*03:43</t>
-  </si>
-  <si>
-    <t>DRB1*03:02| DRB1*03:03</t>
-  </si>
-  <si>
-    <t>DRB1*03:05| DRB1*03:06| DRB1*03:07| DRB1*03:08| DRB1*03:09| DRB1*03:12| DRB1*03:13| DRB1*03:14| DRB1*03:15| DRB1*03:16| DRB1*03:17| DRB1*03:18| DRB1*03:19| DRB1*03:20| DRB1*03:21| DRB1*03:22| DRB1*03:23| DRB1*03:24| DRB1*03:25| DRB1*03:26| DRB1*03:27| DRB1*03:28| DRB1*03:29| DRB1*03:30| DRB1*03:31| DRB1*03:32| DRB1*03:33| DRB1*03:34| DRB1*03:35| DRB1*03:36| DRB1*03:37| DRB1*03:38| DRB1*03:39| DRB1*03:40| DRB1*03:41| DRB1*03:42| DRB1*03:44| DRB1*03:45| DRB1*03:46| DRB1*03:47| DRB1*03:48| DRB1*03:49| DRB1*03:50| DRB1*03:51| DRB1*03:52| DRB1*03:53| DRB1*03:54| DRB1*03:55| DRB1*03:56| DRB1*03:57| DRB1*03:58| DRB1*03:59| DRB1*03:60| DRB1*03:61| DRB1*03:62| DRB1*03:63| DRB1*03:64| DRB1*03:65| DRB1*03:66| DRB1*03:69| DRB1*03:70| DRB1*03:71| DRB1*03:72| DRB1*03:73| DRB1*03:74| DRB1*03:75| DRB1*03:76| DRB1*03:77| DRB1*03:78| DRB1*03:79| DRB1*03:80| DRB1*03:81| DRB1*03:82| DRB1*03:83| DRB1*03:84| DRB1*03:85| DRB1*03:86| DRB1*03:87| DRB1*03:88| DRB1*03:89| DRB1*03:90| DRB1*03:91| DRB1*03:92| DRB1*03:93| DRB1*03:94| DRB1*03:95| DRB1*03:96| DRB1*03:97| DRB1*03:98| DRB1*03:99| DRB1*03:100| DRB1*03:101| DRB1*03:102| DRB1*03:103| DRB1*03:104| DRB1*03:105| DRB1*03:106| DRB1*03:107| DRB1*03:108| DRB1*03:109| DRB1*03:110| DRB1*03:111| DRB1*03:112| DRB1*03:113| DRB1*03:114| DRB1*03:115| DRB1*03:116| DRB1*03:117| DRB1*03:118| DRB1*03:119| DRB1*03:120| DRB1*03:121| DRB1*03:122| DRB1*03:123| DRB1*03:124| DRB1*03:125| DRB1*03:126| DRB1*03:127| DRB1*03:128| DRB1*03:129| DRB1*03:130| DRB1*03:131| DRB1*03:132| DRB1*03:133| DRB1*03:134| DRB1*03:135| DRB1*03:136| DRB1*03:137| DRB1*03:138| DRB1*03:139| DRB1*03:140| DRB1*03:141| DRB1*03:142| DRB1*03:01| DRB1*03:04| DRB1*03:10| DRB1*03:11| DRB1*03:43| DRB1*03:02| DRB1*03:03</t>
-  </si>
-  <si>
-    <t>DRB1*04:01| DRB1*04:02| DRB1*04:03| DRB1*04:04| DRB1*04:05| DRB1*04:06| DRB1*04:07| DRB1*04:08| DRB1*04:09| DRB1*04:10| DRB1*04:11| DRB1*04:12| DRB1*04:13| DRB1*04:14| DRB1*04:15| DRB1*04:16| DRB1*04:17| DRB1*04:18| DRB1*04:19| DRB1*04:20| DRB1*04:21| DRB1*04:22| DRB1*04:23| DRB1*04:24| DRB1*04:25| DRB1*04:26| DRB1*04:27| DRB1*04:28| DRB1*04:29| DRB1*04:30| DRB1*04:31| DRB1*04:32| DRB1*04:33| DRB1*04:34| DRB1*04:35| DRB1*04:36| DRB1*04:37| DRB1*04:38| DRB1*04:39| DRB1*04:40| DRB1*04:41| DRB1*04:42| DRB1*04:43| DRB1*04:44| DRB1*04:45| DRB1*04:46| DRB1*04:47| DRB1*04:48| DRB1*04:49| DRB1*04:50| DRB1*04:51| DRB1*04:52| DRB1*04:53| DRB1*04:54| DRB1*04:55| DRB1*04:56| DRB1*04:57| DRB1*04:58| DRB1*04:59| DRB1*04:60| DRB1*04:61| DRB1*04:62| DRB1*04:63| DRB1*04:64| DRB1*04:65| DRB1*04:66| DRB1*04:67| DRB1*04:68| DRB1*04:69| DRB1*04:70| DRB1*04:71| DRB1*04:72| DRB1*04:73| DRB1*04:74| DRB1*04:75| DRB1*04:76| DRB1*04:77| DRB1*04:78| DRB1*04:79| DRB1*04:80| DRB1*04:82| DRB1*04:83| DRB1*04:84| DRB1*04:85| DRB1*04:86| DRB1*04:87| DRB1*04:88| DRB1*04:89| DRB1*04:90| DRB1*04:91| DRB1*04:92| DRB1*04:93| DRB1*04:95| DRB1*04:96| DRB1*04:97| DRB1*04:98| DRB1*04:99| DRB1*04:100| DRB1*04:101| DRB1*04:102| DRB1*04:103| DRB1*04:104| DRB1*04:105| DRB1*04:106| DRB1*04:107| DRB1*04:108| DRB1*04:109| DRB1*04:110| DRB1*04:111| DRB1*04:112| DRB1*04:113| DRB1*04:114| DRB1*04:115| DRB1*04:116| DRB1*04:117| DRB1*04:118| DRB1*04:121| DRB1*04:122| DRB1*04:123| DRB1*04:124| DRB1*04:125| DRB1*04:126| DRB1*04:127| DRB1*04:128| DRB1*04:129| DRB1*04:130| DRB1*04:131| DRB1*04:132| DRB1*04:133| DRB1*04:134| DRB1*04:135| DRB1*04:136| DRB1*04:137| DRB1*04:138| DRB1*04:139| DRB1*04:140| DRB1*04:141| DRB1*04:143| DRB1*04:144| DRB1*04:145| DRB1*04:146| DRB1*04:147| DRB1*04:148| DRB1*04:149| DRB1*04:150| DRB1*04:151| DRB1*04:152| DRB1*04:153| DRB1*04:154| DRB1*04:155| DRB1*04:156| DRB1*04:159| DRB1*04:160| DRB1*04:161| DRB1*04:162| DRB1*04:163| DRB1*04:164| DRB1*04:165| DRB1*04:166| DRB1*04:167| DRB1*04:168| DRB1*04:169| DRB1*04:170| DRB1*04:171| DRB1*04:172| DRB1*04:173| DRB1*04:174| DRB1*04:175| DRB1*04:176| DRB1*04:177| DRB1*04:179| DRB1*04:180| DRB1*04:181| DRB1*04:182| DRB1*04:183| DRB1*04:184| DRB1*04:185| DRB1*04:187| DRB1*04:188| DRB1*04:189| DRB1*04:190| DRB1*04:191| DRB1*04:192| DRB1*04:193| DRB1*04:194| DRB1*04:195| DRB1*04:196| DRB1*04:197| DRB1*04:198| DRB1*04:199| DRB1*04:200| DRB1*04:201| DRB1*04:202| DRB1*04:203| DRB1*04:204| DRB1*04:205| DRB1*04:206| DRB1*04:207| DRB1*04:208| DRB1*04:209| DRB1*04:210| DRB1*04:211| DRB1*04:213| DRB1*04:215| DRB1*04:216| DRB1*04:217| DRB1*04:218| DRB1*04:219| DRB1*04:220| DRB1*04:221| DRB1*04:222| DRB1*04:223| DRB1*04:224| DRB1*04:225| DRB1*04:226| DRB1*04:227| DRB1*04:228| DRB1*04:229| DRB1*04:230| DRB1*04:231| DRB1*04:232| DRB1*04:233| DRB1*04:234| DRB1*04:235| DRB1*04:236| DRB1*04:237</t>
-  </si>
-  <si>
-    <t>DRB1*07:01| DRB1*07:03| DRB1*07:04| DRB1*07:05| DRB1*07:06| DRB1*07:07| DRB1*07:08| DRB1*07:09| DRB1*07:11| DRB1*07:12| DRB1*07:13| DRB1*07:14| DRB1*07:15| DRB1*07:16| DRB1*07:17| DRB1*07:18| DRB1*07:19| DRB1*07:20| DRB1*07:21| DRB1*07:22| DRB1*07:23| DRB1*07:24| DRB1*07:25| DRB1*07:27| DRB1*07:28| DRB1*07:29| DRB1*07:30| DRB1*07:31| DRB1*07:32| DRB1*07:33| DRB1*07:34| DRB1*07:35| DRB1*07:36| DRB1*07:37| DRB1*07:38| DRB1*07:39| DRB1*07:40| DRB1*07:41| DRB1*07:42| DRB1*07:43| DRB1*07:44| DRB1*07:45| DRB1*07:46| DRB1*07:47| DRB1*07:48| DRB1*07:49| DRB1*07:50| DRB1*07:51| DRB1*07:52| DRB1*07:53| DRB1*07:54| DRB1*07:55| DRB1*07:56| DRB1*07:57| DRB1*07:59| DRB1*07:60| DRB1*07:61| DRB1*07:62| DRB1*07:63| DRB1*07:64| DRB1*07:65| DRB1*07:66| DRB1*07:67| DRB1*07:69| DRB1*07:70| DRB1*07:71| DRB1*07:72| DRB1*07:73| DRB1*07:74| DRB1*07:75| DRB1*07:76| DRB1*07:77| DRB1*07:78| DRB1*07:79| DRB1*07:80| DRB1*07:81| DRB1*07:82| DRB1*07:83| DRB1*07:84</t>
-  </si>
-  <si>
-    <t>DRB1*08:01| DRB1*08:02| DRB1*08:03| DRB1*08:04| DRB1*08:05| DRB1*08:06| DRB1*08:07| DRB1*08:08| DRB1*08:09| DRB1*08:10| DRB1*08:11| DRB1*08:12| DRB1*08:13| DRB1*08:14| DRB1*08:15| DRB1*08:16| DRB1*08:17| DRB1*08:18| DRB1*08:19| DRB1*08:20| DRB1*08:21| DRB1*08:22| DRB1*08:23| DRB1*08:24| DRB1*08:25| DRB1*08:26| DRB1*08:27| DRB1*08:28| DRB1*08:29| DRB1*08:30| DRB1*08:32| DRB1*08:33| DRB1*08:34| DRB1*08:35| DRB1*08:36| DRB1*08:37| DRB1*08:38| DRB1*08:39| DRB1*08:40| DRB1*08:41| DRB1*08:42| DRB1*08:43| DRB1*08:44| DRB1*08:45| DRB1*08:46| DRB1*08:47| DRB1*08:48| DRB1*08:49| DRB1*08:50| DRB1*08:51| DRB1*08:52| DRB1*08:53| DRB1*08:54| DRB1*08:55| DRB1*08:56| DRB1*08:57| DRB1*08:58| DRB1*08:59| DRB1*08:61| DRB1*08:62| DRB1*08:63| DRB1*08:64| DRB1*08:65| DRB1*08:66| DRB1*08:67| DRB1*08:68| DRB1*08:69| DRB1*08:70| DRB1*08:71| DRB1*08:72| DRB1*08:73| DRB1*08:74| DRB1*08:75| DRB1*08:76| DRB1*08:77| DRB1*08:79| DRB1*08:80| DRB1*08:81| DRB1*08:82| DRB1*14:15</t>
-  </si>
-  <si>
-    <t>DRB1*08:31| DRB1*11:01| DRB1*11:02| DRB1*11:03| DRB1*11:04| DRB1*11:05| DRB1*11:06| DRB1*11:07| DRB1*11:08| DRB1*11:09| DRB1*11:10| DRB1*11:11| DRB1*11:12| DRB1*11:13| DRB1*11:14| DRB1*11:15| DRB1*11:16| DRB1*11:18| DRB1*11:19| DRB1*11:20| DRB1*11:21| DRB1*11:22| DRB1*11:23| DRB1*11:24| DRB1*11:25| DRB1*11:26| DRB1*11:27| DRB1*11:28| DRB1*11:29| DRB1*11:30| DRB1*11:31| DRB1*11:32| DRB1*11:33| DRB1*11:34| DRB1*11:35| DRB1*11:36| DRB1*11:37| DRB1*11:38| DRB1*11:39| DRB1*11:40| DRB1*11:41| DRB1*11:42| DRB1*11:43| DRB1*11:44| DRB1*11:45| DRB1*11:46| DRB1*11:47| DRB1*11:48| DRB1*11:49| DRB1*11:50| DRB1*11:51| DRB1*11:52| DRB1*11:53| DRB1*11:54| DRB1*11:55| DRB1*11:56| DRB1*11:57| DRB1*11:58| DRB1*11:59| DRB1*11:60| DRB1*11:61| DRB1*11:62| DRB1*11:63| DRB1*11:64| DRB1*11:65| DRB1*11:66| DRB1*11:67| DRB1*11:68| DRB1*11:69| DRB1*11:70| DRB1*11:72| DRB1*11:73| DRB1*11:74| DRB1*11:75| DRB1*11:76| DRB1*11:77| DRB1*11:78| DRB1*11:79| DRB1*11:80| DRB1*11:81| DRB1*11:82| DRB1*11:83| DRB1*11:84| DRB1*11:85| DRB1*11:86| DRB1*11:87| DRB1*11:88| DRB1*11:89| DRB1*11:90| DRB1*11:91| DRB1*11:92| DRB1*11:93| DRB1*11:94| DRB1*11:95| DRB1*11:96| DRB1*11:97| DRB1*11:98| DRB1*11:99| DRB1*11:100| DRB1*11:101| DRB1*11:102| DRB1*11:103| DRB1*11:104| DRB1*11:105| DRB1*11:106| DRB1*11:107| DRB1*11:108| DRB1*11:109| DRB1*11:110| DRB1*11:111| DRB1*11:112| DRB1*11:113| DRB1*11:114| DRB1*11:115| DRB1*11:116| DRB1*11:117| DRB1*11:118| DRB1*11:119| DRB1*11:120| DRB1*11:121| DRB1*11:122| DRB1*11:123| DRB1*11:124| DRB1*11:125| DRB1*11:126| DRB1*11:127| DRB1*11:128| DRB1*11:129| DRB1*11:130| DRB1*11:131| DRB1*11:132| DRB1*11:133| DRB1*11:134| DRB1*11:135| DRB1*11:136| DRB1*11:137| DRB1*11:138| DRB1*11:139| DRB1*11:140| DRB1*11:141| DRB1*11:142| DRB1*11:143| DRB1*11:144| DRB1*11:145| DRB1*11:146| DRB1*11:147| DRB1*11:148| DRB1*11:149| DRB1*11:150| DRB1*11:151| DRB1*11:152| DRB1*11:153| DRB1*11:154| DRB1*11:155| DRB1*11:156| DRB1*11:157| DRB1*11:158| DRB1*11:159| DRB1*11:160| DRB1*11:161| DRB1*11:162| DRB1*11:163| DRB1*11:164| DRB1*11:165| DRB1*11:166| DRB1*11:167| DRB1*11:168| DRB1*11:170| DRB1*11:171| DRB1*11:172| DRB1*11:173| DRB1*11:174| DRB1*11:175| DRB1*11:176| DRB1*11:177| DRB1*11:178| DRB1*11:179| DRB1*11:180| DRB1*11:181| DRB1*11:182| DRB1*11:183| DRB1*11:184| DRB1*11:185| DRB1*11:186| DRB1*11:187| DRB1*11:188| DRB1*11:189| DRB1*11:190| DRB1*11:191| DRB1*11:192| DRB1*11:193| DRB1*11:194| DRB1*11:195| DRB1*11:196| DRB1*11:197| DRB1*11:198| DRB1*11:199| DRB1*11:200| DRB1*11:201| DRB1*11:202| DRB1*11:203| DRB1*11:204| DRB1*11:205| DRB1*11:206| DRB1*11:207| DRB1*11:208| DRB1*11:209| DRB1*11:210| DRB1*11:211| DRB1*11:212| DRB1*11:213| DRB1*11:214| DRB1*11:215| DRB1*11:216| DRB1*11:218| DRB1*11:219| DRB1*11:220| DRB1*13:24| DRB1*13:25| DRB1*13:46| DRB1*13:50| DRB1*13:62</t>
-  </si>
-  <si>
-    <t>DRB1*09:01| DRB1*09:02| DRB1*09:03| DRB1*09:04| DRB1*09:05| DRB1*09:06| DRB1*09:07| DRB1*09:08| DRB1*09:09| DRB1*09:10| DRB1*09:11| DRB1*09:12| DRB1*09:13| DRB1*09:14| DRB1*09:15| DRB1*09:16| DRB1*09:17| DRB1*09:18| DRB1*09:19| DRB1*09:20| DRB1*09:21| DRB1*09:22| DRB1*09:23| DRB1*09:24| DRB1*09:25| DRB1*09:26| DRB1*09:27| DRB1*09:28| DRB1*09:29| DRB1*09:30| DRB1*09:31| DRB1*09:32</t>
-  </si>
-  <si>
-    <t>DRB1*10:01| DRB1*10:02| DRB1*10:03| DRB1*10:04| DRB1*10:05| DRB1*10:06| DRB1*10:07| DRB1*10:08| DRB1*10:09| DRB1*10:10| DRB1*10:11| DRB1*10:12| DRB1*10:13| DRB1*10:14| DRB1*10:15| DRB1*10:16| DRB1*10:17| DRB1*10:18| DRB1*10:19| DRB1*10:20| DRB1*10:21| DRB1*10:22| DRB1*10:23| DRB1*10:24</t>
-  </si>
-  <si>
-    <t>DRB1*11:17| DRB1*13:26| DRB1*13:54| DRB1*14:01| DRB1*14:02| DRB1*14:05| DRB1*14:06| DRB1*14:07| DRB1*14:08| DRB1*14:09| DRB1*14:10| DRB1*14:11| DRB1*14:12| DRB1*14:13| DRB1*14:14| DRB1*14:19| DRB1*14:20| DRB1*14:21| DRB1*14:22| DRB1*14:23| DRB1*14:24| DRB1*14:26| DRB1*14:27| DRB1*14:28| DRB1*14:29| DRB1*14:31| DRB1*14:32| DRB1*14:34| DRB1*14:35| DRB1*14:36| DRB1*14:37| DRB1*14:38| DRB1*14:39| DRB1*14:40| DRB1*14:41| DRB1*14:42| DRB1*14:43| DRB1*14:44| DRB1*14:45| DRB1*14:46| DRB1*14:47| DRB1*14:48| DRB1*14:49| DRB1*14:50| DRB1*14:51| DRB1*14:52| DRB1*14:54| DRB1*14:55| DRB1*14:56| DRB1*14:57| DRB1*14:58| DRB1*14:59| DRB1*14:60| DRB1*14:61| DRB1*14:62| DRB1*14:64| DRB1*14:68| DRB1*14:69| DRB1*14:70| DRB1*14:71| DRB1*14:72| DRB1*14:73| DRB1*14:74| DRB1*14:75| DRB1*14:76| DRB1*14:77| DRB1*14:78| DRB1*14:79| DRB1*14:80| DRB1*14:81| DRB1*14:82| DRB1*14:83| DRB1*14:84| DRB1*14:85| DRB1*14:86| DRB1*14:87| DRB1*14:88| DRB1*14:89| DRB1*14:90| DRB1*14:91| DRB1*14:93| DRB1*14:94| DRB1*14:95| DRB1*14:96| DRB1*14:97| DRB1*14:98| DRB1*14:99| DRB1*14:100| DRB1*14:101| DRB1*14:102| DRB1*14:103| DRB1*14:104| DRB1*14:105| DRB1*14:106| DRB1*14:107| DRB1*14:108| DRB1*14:109| DRB1*14:110| DRB1*14:111| DRB1*14:112| DRB1*14:113| DRB1*14:114| DRB1*14:115| DRB1*14:116| DRB1*14:117| DRB1*14:118| DRB1*14:119| DRB1*14:120| DRB1*14:121| DRB1*14:122| DRB1*14:123| DRB1*14:124| DRB1*14:125| DRB1*14:126| DRB1*14:127| DRB1*14:128| DRB1*14:129| DRB1*14:130| DRB1*14:131| DRB1*14:132| DRB1*14:133| DRB1*14:134| DRB1*14:135| DRB1*14:136| DRB1*14:138| DRB1*14:139| DRB1*14:140| DRB1*14:141| DRB1*14:142| DRB1*14:143| DRB1*14:144| DRB1*14:145| DRB1*14:146| DRB1*14:147| DRB1*14:148| DRB1*14:149| DRB1*14:150| DRB1*14:151| DRB1*14:153| DRB1*14:154| DRB1*14:155| DRB1*14:156| DRB1*14:157| DRB1*14:158| DRB1*14:159| DRB1*14:160| DRB1*14:161| DRB1*14:162| DRB1*14:163| DRB1*14:164| DRB1*14:165| DRB1*14:167| DRB1*14:168| DRB1*14:169| DRB1*14:170| DRB1*14:171| DRB1*14:172| DRB1*14:173| DRB1*14:174| DRB1*14:175| DRB1*14:176| DRB1*14:177| DRB1*14:178| DRB1*14:179| DRB1*14:180| DRB1*14:181| DRB1*14:182| DRB1*14:183| DRB1*14:184| DRB1*14:185| DRB1*14:187| DRB1*14:189| DRB1*14:190| DRB1*14:03| DRB1*14:04</t>
-  </si>
-  <si>
-    <t>DRB1*12:01| DRB1*12:02| DRB1*12:03| DRB1*12:04| DRB1*12:05| DRB1*12:06| DRB1*12:07| DRB1*12:08| DRB1*12:09| DRB1*12:10| DRB1*12:11| DRB1*12:12| DRB1*12:13| DRB1*12:14| DRB1*12:15| DRB1*12:16| DRB1*12:17| DRB1*12:18| DRB1*12:19| DRB1*12:20| DRB1*12:21| DRB1*12:22| DRB1*12:23| DRB1*12:25| DRB1*12:26| DRB1*12:27| DRB1*12:28| DRB1*12:29| DRB1*12:30| DRB1*12:32| DRB1*12:33| DRB1*12:34| DRB1*12:35| DRB1*12:36| DRB1*12:37| DRB1*12:38| DRB1*12:39| DRB1*12:40| DRB1*12:41| DRB1*12:42| DRB1*12:43| DRB1*12:44| DRB1*12:45| DRB1*12:46| DRB1*12:47| DRB1*12:48| DRB1*12:49| DRB1*12:50| DRB1*12:51| DRB1*12:52| DRB1*12:53| DRB1*12:54| DRB1*12:55| DRB1*12:56| DRB1*12:57| DRB1*12:58| DRB1*12:59| DRB1*12:61| DRB1*12:62| DRB1*12:63| DRB1*12:64| DRB1*12:65| DRB1*12:66| DRB1*12:67| DRB1*12:68</t>
-  </si>
-  <si>
-    <t>DRB1*13:01| DRB1*13:02| DRB1*13:03| DRB1*13:04| DRB1*13:05| DRB1*13:06| DRB1*13:07| DRB1*13:08| DRB1*13:09| DRB1*13:10| DRB1*13:11| DRB1*13:12| DRB1*13:13| DRB1*13:14| DRB1*13:15| DRB1*13:16| DRB1*13:17| DRB1*13:18| DRB1*13:19| DRB1*13:20| DRB1*13:21| DRB1*13:22| DRB1*13:23| DRB1*13:27| DRB1*13:28| DRB1*13:29| DRB1*13:30| DRB1*13:31| DRB1*13:32| DRB1*13:33| DRB1*13:34| DRB1*13:35| DRB1*13:36| DRB1*13:37| DRB1*13:38| DRB1*13:39| DRB1*13:40| DRB1*13:41| DRB1*13:42| DRB1*13:43| DRB1*13:44| DRB1*13:45| DRB1*13:47| DRB1*13:48| DRB1*13:51| DRB1*13:52| DRB1*13:53| DRB1*13:55| DRB1*13:57| DRB1*13:58| DRB1*13:59| DRB1*13:61| DRB1*13:63| DRB1*13:64| DRB1*13:65| DRB1*13:66| DRB1*13:67| DRB1*13:68| DRB1*13:69| DRB1*13:70| DRB1*13:71| DRB1*13:72| DRB1*13:73| DRB1*13:74| DRB1*13:75| DRB1*13:76| DRB1*13:77| DRB1*13:78| DRB1*13:79| DRB1*13:80| DRB1*13:81| DRB1*13:82| DRB1*13:83| DRB1*13:84| DRB1*13:85| DRB1*13:86| DRB1*13:87| DRB1*13:88| DRB1*13:89| DRB1*13:90| DRB1*13:91| DRB1*13:92| DRB1*13:93| DRB1*13:94| DRB1*13:95| DRB1*13:96| DRB1*13:97| DRB1*13:98| DRB1*13:99| DRB1*13:100| DRB1*13:101| DRB1*13:102| DRB1*13:103| DRB1*13:104| DRB1*13:105| DRB1*13:106| DRB1*13:107| DRB1*13:108| DRB1*13:109| DRB1*13:110| DRB1*13:111| DRB1*13:112| DRB1*13:114| DRB1*13:115| DRB1*13:116| DRB1*13:117| DRB1*13:118| DRB1*13:119| DRB1*13:120| DRB1*13:121| DRB1*13:122| DRB1*13:123| DRB1*13:124| DRB1*13:125| DRB1*13:126| DRB1*13:127| DRB1*13:128| DRB1*13:129| DRB1*13:130| DRB1*13:131| DRB1*13:132| DRB1*13:133| DRB1*13:134| DRB1*13:135| DRB1*13:136| DRB1*13:138| DRB1*13:139| DRB1*13:140| DRB1*13:141| DRB1*13:143| DRB1*13:144| DRB1*13:145| DRB1*13:146| DRB1*13:147| DRB1*13:148| DRB1*13:149| DRB1*13:150| DRB1*13:151| DRB1*13:152| DRB1*13:153| DRB1*13:154| DRB1*13:155| DRB1*13:156| DRB1*13:157| DRB1*13:158| DRB1*13:159| DRB1*13:160| DRB1*13:161| DRB1*13:162| DRB1*13:163| DRB1*13:164| DRB1*13:165| DRB1*13:166| DRB1*13:167| DRB1*13:168| DRB1*13:169| DRB1*13:170| DRB1*13:171| DRB1*13:172| DRB1*13:173| DRB1*13:174| DRB1*13:175| DRB1*13:176| DRB1*13:177| DRB1*13:178| DRB1*13:179| DRB1*13:180| DRB1*13:181| DRB1*13:182| DRB1*13:183| DRB1*13:184| DRB1*13:186| DRB1*13:187| DRB1*13:188| DRB1*13:189| DRB1*13:190| DRB1*13:191| DRB1*13:192| DRB1*13:193| DRB1*13:194| DRB1*13:195| DRB1*13:196| DRB1*13:197| DRB1*13:198| DRB1*13:199| DRB1*13:201| DRB1*13:202| DRB1*13:203| DRB1*13:204| DRB1*13:205| DRB1*13:206| DRB1*13:207| DRB1*13:208| DRB1*13:209| DRB1*13:210| DRB1*13:211| DRB1*13:212| DRB1*13:213| DRB1*13:214| DRB1*13:215| DRB1*13:216| DRB1*13:217| DRB1*13:218| DRB1*13:219| DRB1*13:220| DRB1*13:221| DRB1*13:222| DRB1*13:223| DRB1*13:224| DRB1*13:225| DRB1*13:226| DRB1*13:227| DRB1*13:228| DRB1*13:229| DRB1*13:230| DRB1*13:231| DRB1*13:232| DRB1*13:233| DRB1*13:234| DRB1*13:235| DRB1*13:236| DRB1*13:237| DRB1*13:238| DRB1*13:239| DRB1*13:240| DRB1*13:241| DRB1*13:242| DRB1*13:243| DRB1*13:244| DRB1*13:245| DRB1*13:246| DRB1*13:247| DRB1*14:53</t>
-  </si>
-  <si>
-    <t>DRB1*13:49| DRB1*13:56| DRB1*13:60| DRB1*14:16| DRB1*14:17| DRB1*14:18| DRB1*14:25| DRB1*14:30| DRB1*14:33| DRB1*14:63| DRB1*14:65| DRB1*14:67| DRB1*14:186| DRB1*13:01| DRB1*13:02| DRB1*13:03| DRB1*13:04| DRB1*13:05| DRB1*13:06| DRB1*13:07| DRB1*13:08| DRB1*13:09| DRB1*13:10| DRB1*13:11| DRB1*13:12| DRB1*13:13| DRB1*13:14| DRB1*13:15| DRB1*13:16| DRB1*13:17| DRB1*13:18| DRB1*13:19| DRB1*13:20| DRB1*13:21| DRB1*13:22| DRB1*13:23| DRB1*13:27| DRB1*13:28| DRB1*13:29| DRB1*13:30| DRB1*13:31| DRB1*13:32| DRB1*13:33| DRB1*13:34| DRB1*13:35| DRB1*13:36| DRB1*13:37| DRB1*13:38| DRB1*13:39| DRB1*13:40| DRB1*13:41| DRB1*13:42| DRB1*13:43| DRB1*13:44| DRB1*13:45| DRB1*13:47| DRB1*13:48| DRB1*13:51| DRB1*13:52| DRB1*13:53| DRB1*13:55| DRB1*13:57| DRB1*13:58| DRB1*13:59| DRB1*13:61| DRB1*13:63| DRB1*13:64| DRB1*13:65| DRB1*13:66| DRB1*13:67| DRB1*13:68| DRB1*13:69| DRB1*13:70| DRB1*13:71| DRB1*13:72| DRB1*13:73| DRB1*13:74| DRB1*13:75| DRB1*13:76| DRB1*13:77| DRB1*13:78| DRB1*13:79| DRB1*13:80| DRB1*13:81| DRB1*13:82| DRB1*13:83| DRB1*13:84| DRB1*13:85| DRB1*13:86| DRB1*13:87| DRB1*13:88| DRB1*13:89| DRB1*13:90| DRB1*13:91| DRB1*13:92| DRB1*13:93| DRB1*13:94| DRB1*13:95| DRB1*13:96| DRB1*13:97| DRB1*13:98| DRB1*13:99| DRB1*13:100| DRB1*13:101| DRB1*13:102| DRB1*13:103| DRB1*13:104| DRB1*13:105| DRB1*13:106| DRB1*13:107| DRB1*13:108| DRB1*13:109| DRB1*13:110| DRB1*13:111| DRB1*13:112| DRB1*13:114| DRB1*13:115| DRB1*13:116| DRB1*13:117| DRB1*13:118| DRB1*13:119| DRB1*13:120| DRB1*13:121| DRB1*13:122| DRB1*13:123| DRB1*13:124| DRB1*13:125| DRB1*13:126| DRB1*13:127| DRB1*13:128| DRB1*13:129| DRB1*13:130| DRB1*13:131| DRB1*13:132| DRB1*13:133| DRB1*13:134| DRB1*13:135| DRB1*13:136| DRB1*13:138| DRB1*13:139| DRB1*13:140| DRB1*13:141| DRB1*13:143| DRB1*13:144| DRB1*13:145| DRB1*13:146| DRB1*13:147| DRB1*13:148| DRB1*13:149| DRB1*13:150| DRB1*13:151| DRB1*13:152| DRB1*13:153| DRB1*13:154| DRB1*13:155| DRB1*13:156| DRB1*13:157| DRB1*13:158| DRB1*13:159| DRB1*13:160| DRB1*13:161| DRB1*13:162| DRB1*13:163| DRB1*13:164| DRB1*13:165| DRB1*13:166| DRB1*13:167| DRB1*13:168| DRB1*13:169| DRB1*13:170| DRB1*13:171| DRB1*13:172| DRB1*13:173| DRB1*13:174| DRB1*13:175| DRB1*13:176| DRB1*13:177| DRB1*13:178| DRB1*13:179| DRB1*13:180| DRB1*13:181| DRB1*13:182| DRB1*13:183| DRB1*13:184| DRB1*13:186| DRB1*13:187| DRB1*13:188| DRB1*13:189| DRB1*13:190| DRB1*13:191| DRB1*13:192| DRB1*13:193| DRB1*13:194| DRB1*13:195| DRB1*13:196| DRB1*13:197| DRB1*13:198| DRB1*13:199| DRB1*13:201| DRB1*13:202| DRB1*13:203| DRB1*13:204| DRB1*13:205| DRB1*13:206| DRB1*13:207| DRB1*13:208| DRB1*13:209| DRB1*13:210| DRB1*13:211| DRB1*13:212| DRB1*13:213| DRB1*13:214| DRB1*13:215| DRB1*13:216| DRB1*13:217| DRB1*13:218| DRB1*13:219| DRB1*13:220| DRB1*13:221| DRB1*13:222| DRB1*13:223| DRB1*13:224| DRB1*13:225| DRB1*13:226| DRB1*13:227| DRB1*13:228| DRB1*13:229| DRB1*13:230| DRB1*13:231| DRB1*13:232| DRB1*13:233| DRB1*13:234| DRB1*13:235| DRB1*13:236| DRB1*13:237| DRB1*13:238| DRB1*13:239| DRB1*13:240| DRB1*13:241| DRB1*13:242| DRB1*13:243| DRB1*13:244| DRB1*13:245| DRB1*13:246| DRB1*13:247| DRB1*14:53| DRB1*11:17| DRB1*13:26| DRB1*13:54| DRB1*14:01| DRB1*14:02| DRB1*14:05| DRB1*14:06| DRB1*14:07| DRB1*14:08| DRB1*14:09| DRB1*14:10| DRB1*14:11| DRB1*14:12| DRB1*14:13| DRB1*14:14| DRB1*14:19| DRB1*14:20| DRB1*14:21| DRB1*14:22| DRB1*14:23| DRB1*14:24| DRB1*14:26| DRB1*14:27| DRB1*14:28| DRB1*14:29| DRB1*14:31| DRB1*14:32| DRB1*14:34| DRB1*14:35| DRB1*14:36| DRB1*14:37| DRB1*14:38| DRB1*14:39| DRB1*14:40| DRB1*14:41| DRB1*14:42| DRB1*14:43| DRB1*14:44| DRB1*14:45| DRB1*14:46| DRB1*14:47| DRB1*14:48| DRB1*14:49| DRB1*14:50| DRB1*14:51| DRB1*14:52| DRB1*14:54| DRB1*14:55| DRB1*14:56| DRB1*14:57| DRB1*14:58| DRB1*14:59| DRB1*14:60| DRB1*14:61| DRB1*14:62| DRB1*14:64| DRB1*14:68| DRB1*14:69| DRB1*14:70| DRB1*14:71| DRB1*14:72| DRB1*14:73| DRB1*14:74| DRB1*14:75| DRB1*14:76| DRB1*14:77| DRB1*14:78| DRB1*14:79| DRB1*14:80| DRB1*14:81| DRB1*14:82| DRB1*14:83| DRB1*14:84| DRB1*14:85| DRB1*14:86| DRB1*14:87| DRB1*14:88| DRB1*14:89| DRB1*14:90| DRB1*14:91| DRB1*14:93| DRB1*14:94| DRB1*14:95| DRB1*14:96| DRB1*14:97| DRB1*14:98| DRB1*14:99| DRB1*14:100| DRB1*14:101| DRB1*14:102| DRB1*14:103| DRB1*14:104| DRB1*14:105| DRB1*14:106| DRB1*14:107| DRB1*14:108| DRB1*14:109| DRB1*14:110| DRB1*14:111| DRB1*14:112| DRB1*14:113| DRB1*14:114| DRB1*14:115| DRB1*14:116| DRB1*14:117| DRB1*14:118| DRB1*14:119| DRB1*14:120| DRB1*14:121| DRB1*14:122| DRB1*14:123| DRB1*14:124| DRB1*14:125| DRB1*14:126| DRB1*14:127| DRB1*14:128| DRB1*14:129| DRB1*14:130| DRB1*14:131| DRB1*14:132| DRB1*14:133| DRB1*14:134| DRB1*14:135| DRB1*14:136| DRB1*14:138| DRB1*14:139| DRB1*14:140| DRB1*14:141| DRB1*14:142| DRB1*14:143| DRB1*14:144| DRB1*14:145| DRB1*14:146| DRB1*14:147| DRB1*14:148| DRB1*14:149| DRB1*14:150| DRB1*14:151| DRB1*14:153| DRB1*14:154| DRB1*14:155| DRB1*14:156| DRB1*14:157| DRB1*14:158| DRB1*14:159| DRB1*14:160| DRB1*14:161| DRB1*14:162| DRB1*14:163| DRB1*14:164| DRB1*14:165| DRB1*14:167| DRB1*14:168| DRB1*14:169| DRB1*14:170| DRB1*14:171| DRB1*14:172| DRB1*14:173| DRB1*14:174| DRB1*14:175| DRB1*14:176| DRB1*14:177| DRB1*14:178| DRB1*14:179| DRB1*14:180| DRB1*14:181| DRB1*14:182| DRB1*14:183| DRB1*14:184| DRB1*14:185| DRB1*14:187| DRB1*14:189| DRB1*14:190| DRB1*14:03| DRB1*14:04</t>
-  </si>
-  <si>
-    <t>DRB1*14:03</t>
-  </si>
-  <si>
-    <t>DRB1*14:04</t>
-  </si>
-  <si>
-    <t>DRB1*15:01| DRB1*15:02| DRB1*15:03| DRB1*15:04| DRB1*15:05| DRB1*15:06| DRB1*15:07| DRB1*15:09| DRB1*15:11| DRB1*15:12| DRB1*15:14| DRB1*15:15| DRB1*15:16| DRB1*15:18| DRB1*15:19| DRB1*15:20| DRB1*15:22| DRB1*15:23| DRB1*15:24| DRB1*15:25| DRB1*15:26| DRB1*15:27| DRB1*15:28| DRB1*15:29| DRB1*15:30| DRB1*15:31| DRB1*15:32| DRB1*15:33| DRB1*15:34| DRB1*15:35| DRB1*15:36| DRB1*15:37| DRB1*15:38| DRB1*15:39| DRB1*15:40| DRB1*15:41| DRB1*15:42| DRB1*15:43| DRB1*15:44| DRB1*15:45| DRB1*15:46| DRB1*15:47| DRB1*15:48| DRB1*15:49| DRB1*15:51| DRB1*15:52| DRB1*15:53| DRB1*15:54| DRB1*15:55| DRB1*15:56| DRB1*15:57| DRB1*15:58| DRB1*15:59| DRB1*15:60| DRB1*15:61| DRB1*15:62| DRB1*15:63| DRB1*15:64| DRB1*15:65| DRB1*15:66| DRB1*15:67| DRB1*15:68| DRB1*15:69| DRB1*15:70| DRB1*15:71| DRB1*15:72| DRB1*15:73| DRB1*15:74| DRB1*15:75| DRB1*15:76| DRB1*15:77| DRB1*15:78| DRB1*15:79| DRB1*15:81| DRB1*15:82| DRB1*15:83| DRB1*15:84| DRB1*15:85| DRB1*15:86| DRB1*15:87| DRB1*15:88| DRB1*15:89| DRB1*15:90| DRB1*15:91| DRB1*15:92| DRB1*15:93| DRB1*15:94| DRB1*15:95| DRB1*15:96| DRB1*15:97| DRB1*15:98| DRB1*15:99| DRB1*15:100| DRB1*15:101| DRB1*15:102| DRB1*15:103| DRB1*15:104| DRB1*15:105| DRB1*15:106| DRB1*15:107| DRB1*15:108| DRB1*15:109| DRB1*15:110| DRB1*15:111| DRB1*15:112| DRB1*15:114| DRB1*15:116| DRB1*15:117| DRB1*15:118| DRB1*15:119| DRB1*15:120| DRB1*15:121| DRB1*15:122| DRB1*15:123| DRB1*15:124| DRB1*15:125| DRB1*15:126| DRB1*15:127| DRB1*15:128| DRB1*15:130| DRB1*15:131| DRB1*15:132| DRB1*15:133| DRB1*15:135| DRB1*15:136| DRB1*15:139| DRB1*15:140| DRB1*15:141| DRB1*15:142| DRB1*15:143| DRB1*15:144| DRB1*15:145| DRB1*15:146| DRB1*15:147</t>
-  </si>
-  <si>
-    <t>DRB1*15:08| DRB1*15:10| DRB1*15:13| DRB1*15:21| DRB1*16:03| DRB3*02:61Q| DRB1*15:01| DRB1*15:02| DRB1*15:03| DRB1*15:04| DRB1*15:05| DRB1*15:06| DRB1*15:07| DRB1*15:09| DRB1*15:11| DRB1*15:12| DRB1*15:14| DRB1*15:15| DRB1*15:16| DRB1*15:18| DRB1*15:19| DRB1*15:20| DRB1*15:22| DRB1*15:23| DRB1*15:24| DRB1*15:25| DRB1*15:26| DRB1*15:27| DRB1*15:28| DRB1*15:29| DRB1*15:30| DRB1*15:31| DRB1*15:32| DRB1*15:33| DRB1*15:34| DRB1*15:35| DRB1*15:36| DRB1*15:37| DRB1*15:38| DRB1*15:39| DRB1*15:40| DRB1*15:41| DRB1*15:42| DRB1*15:43| DRB1*15:44| DRB1*15:45| DRB1*15:46| DRB1*15:47| DRB1*15:48| DRB1*15:49| DRB1*15:51| DRB1*15:52| DRB1*15:53| DRB1*15:54| DRB1*15:55| DRB1*15:56| DRB1*15:57| DRB1*15:58| DRB1*15:59| DRB1*15:60| DRB1*15:61| DRB1*15:62| DRB1*15:63| DRB1*15:64| DRB1*15:65| DRB1*15:66| DRB1*15:67| DRB1*15:68| DRB1*15:69| DRB1*15:70| DRB1*15:71| DRB1*15:72| DRB1*15:73| DRB1*15:74| DRB1*15:75| DRB1*15:76| DRB1*15:77| DRB1*15:78| DRB1*15:79| DRB1*15:81| DRB1*15:82| DRB1*15:83| DRB1*15:84| DRB1*15:85| DRB1*15:86| DRB1*15:87| DRB1*15:88| DRB1*15:89| DRB1*15:90| DRB1*15:91| DRB1*15:92| DRB1*15:93| DRB1*15:94| DRB1*15:95| DRB1*15:96| DRB1*15:97| DRB1*15:98| DRB1*15:99| DRB1*15:100| DRB1*15:101| DRB1*15:102| DRB1*15:103| DRB1*15:104| DRB1*15:105| DRB1*15:106| DRB1*15:107| DRB1*15:108| DRB1*15:109| DRB1*15:110| DRB1*15:111| DRB1*15:112| DRB1*15:114| DRB1*15:116| DRB1*15:117| DRB1*15:118| DRB1*15:119| DRB1*15:120| DRB1*15:121| DRB1*15:122| DRB1*15:123| DRB1*15:124| DRB1*15:125| DRB1*15:126| DRB1*15:127| DRB1*15:128| DRB1*15:130| DRB1*15:131| DRB1*15:132| DRB1*15:133| DRB1*15:135| DRB1*15:136| DRB1*15:139| DRB1*15:140| DRB1*15:141| DRB1*15:142| DRB1*15:143| DRB1*15:144| DRB1*15:145| DRB1*15:146| DRB1*15:147| DRB1*16:01| DRB1*16:02| DRB1*16:04| DRB1*16:05| DRB1*16:07| DRB1*16:08| DRB1*16:09| DRB1*16:10| DRB1*16:11| DRB1*16:12| DRB1*16:14| DRB1*16:15| DRB1*16:16| DRB1*16:17| DRB1*16:18| DRB1*16:19| DRB1*16:20| DRB1*16:22| DRB1*16:23| DRB1*16:24| DRB1*16:25| DRB1*16:26| DRB1*16:27| DRB1*16:28| DRB1*16:29| DRB1*16:30| DRB1*16:31| DRB1*16:32| DRB1*16:33| DRB1*16:34| DRB1*16:35| DRB1*16:36| DRB1*16:37| DRB1*16:38| DRB1*16:39| DRB1*16:40| DRB1*16:42| DRB1*16:43| DRB1*16:44| DRB1*16:45| DRB1*16:46| DRB1*16:47</t>
-  </si>
-  <si>
-    <t>DRB1*16:01| DRB1*16:02| DRB1*16:04| DRB1*16:05| DRB1*16:07| DRB1*16:08| DRB1*16:09| DRB1*16:10| DRB1*16:11| DRB1*16:12| DRB1*16:14| DRB1*16:15| DRB1*16:16| DRB1*16:17| DRB1*16:18| DRB1*16:19| DRB1*16:20| DRB1*16:22| DRB1*16:23| DRB1*16:24| DRB1*16:25| DRB1*16:26| DRB1*16:27| DRB1*16:28| DRB1*16:29| DRB1*16:30| DRB1*16:31| DRB1*16:32| DRB1*16:33| DRB1*16:34| DRB1*16:35| DRB1*16:36| DRB1*16:37| DRB1*16:38| DRB1*16:39| DRB1*16:40| DRB1*16:42| DRB1*16:43| DRB1*16:44| DRB1*16:45| DRB1*16:46| DRB1*16:47</t>
+    <t>DRB1*01:33N| DRB1*01:39N| DRB1*01:40N| DRB1*01:52N| DRB1*01:62N| DRB1*01:68N| DRB1*03:67N| DRB1*03:68N| DRB1*03:156N| DRB1*04:81N| DRB1*04:94:01N| DRB1*04:119N| DRB1*04:120N| DRB1*04:142N| DRB1*04:157N| DRB1*04:158N| DRB1*04:178N| DRB1*04:186N| DRB1*04:212N| DRB1*04:214N| DRB1*04:247N| DRB1*04:264N| DRB1*04:266N| DRB1*04:267N| DRB1*07:10N| DRB1*07:26N| DRB1*07:58N| DRB1*07:68N| DRB1*07:87N| DRB1*08:60N| DRB1*08:78N| DRB1*08:89N| DRB1*09:37N| DRB1*11:169N| DRB1*11:217N| DRB1*11:246N| DRB1*11:250N| DRB1*12:24N| DRB1*12:31N| DRB1*12:60N| DRB1*12:72N| DRB1*12:74N| DRB1*13:113N| DRB1*13:137N| DRB1*13:142N| DRB1*13:185N| DRB1*13:200N| DRB1*13:249N| DRB1*13:252N| DRB1*13:255N| DRB1*13:268N| DRB1*14:92N| DRB1*14:137N| DRB1*14:152N| DRB1*14:166N| DRB1*14:188N| DRB1*14:195N| DRB1*14:197N| DRB1*15:17N| DRB1*15:50N| DRB1*15:80N| DRB1*15:113N| DRB1*15:115N| DRB1*15:129N| DRB1*15:134N| DRB1*15:137N| DRB1*15:138N| DRB1*15:148N| DRB1*15:154N| DRB1*15:159N| DRB1*16:13N| DRB1*16:21N| DRB1*16:41N| DRB3*01:26N| DRB3*01:40:01N| DRB3*01:40:02N| DRB3*02:29N| DRB3*02:55N| DRB3*02:67N| DRB3*02:80N| DRB4*01:03:01:02N| DRB4*01:16N| DRB4*01:38N| DRB4*01:54N| DRB4*01:56N| DRB4*01:57N| DRB4*01:61N| DRB4*01:65N| DRB4*01:71N| DRB4*01:80N| DRB4*01:84N| DRB4*02:01N| DRB4*03:01N| DRB5*01:08N| DRB5*01:10N| DRB5*01:27N| DRB5*01:48N| DRB5*01:49N| DRB5*02:19N</t>
+  </si>
+  <si>
+    <t>DRB1*01:01:01| DRB1*01:01:02| DRB1*01:01:03| DRB1*01:01:04| DRB1*01:01:05| DRB1*01:01:06| DRB1*01:01:07| DRB1*01:01:08| DRB1*01:01:09| DRB1*01:01:10| DRB1*01:01:11| DRB1*01:01:12| DRB1*01:01:13| DRB1*01:01:14| DRB1*01:01:15| DRB1*01:01:16| DRB1*01:01:17| DRB1*01:01:18| DRB1*01:01:19| DRB1*01:01:20| DRB1*01:01:21| DRB1*01:01:22| DRB1*01:01:23| DRB1*01:01:24| DRB1*01:01:25| DRB1*01:01:26| DRB1*01:01:27| DRB1*01:01:28| DRB1*01:01:29| DRB1*01:01:30| DRB1*01:01:31| DRB1*01:01:32| DRB1*01:01:33| DRB1*01:02:01:01| DRB1*01:02:01:02| DRB1*01:02:02| DRB1*01:02:03| DRB1*01:02:04| DRB1*01:02:05| DRB1*01:02:06| DRB1*01:02:07| DRB1*01:02:08| DRB1*01:02:09| DRB1*01:02:10| DRB1*01:02:11| DRB1*01:02:12| DRB1*01:02:13| DRB1*01:04| DRB1*01:05| DRB1*01:06| DRB1*01:07| DRB1*01:08| DRB1*01:09| DRB1*01:10| DRB1*01:11:01| DRB1*01:11:02| DRB1*01:12| DRB1*01:13| DRB1*01:14| DRB1*01:15| DRB1*01:16| DRB1*01:17| DRB1*01:18:01| DRB1*01:18:02| DRB1*01:19| DRB1*01:20:01| DRB1*01:20:02| DRB1*01:21| DRB1*01:22| DRB1*01:23| DRB1*01:24:01| DRB1*01:24:02| DRB1*01:25| DRB1*01:26| DRB1*01:27| DRB1*01:28| DRB1*01:29:01| DRB1*01:29:02| DRB1*01:30| DRB1*01:31| DRB1*01:32| DRB1*01:34| DRB1*01:35| DRB1*01:36| DRB1*01:37| DRB1*01:38| DRB1*01:41| DRB1*01:42| DRB1*01:43| DRB1*01:44:01| DRB1*01:44:02| DRB1*01:45| DRB1*01:46| DRB1*01:47| DRB1*01:48| DRB1*01:49| DRB1*01:50| DRB1*01:51| DRB1*01:53| DRB1*01:54| DRB1*01:55| DRB1*01:56| DRB1*01:57| DRB1*01:58| DRB1*01:59| DRB1*01:60| DRB1*01:61| DRB1*01:63| DRB1*01:64| DRB1*01:65:01| DRB1*01:65:02| DRB1*01:66| DRB1*01:67| DRB1*01:69| DRB1*01:70| DRB1*01:71| DRB1*01:72| DRB1*01:73| DRB1*01:74| DRB1*01:75| DRB1*01:76| DRB1*01:77| DRB1*01:78| DRB1*01:79| DRB1*01:80| DRB1*01:81| DRB1*01:82| DRB1*01:83| DRB1*01:84| DRB1*01:85| DRB1*01:86| DRB1*01:87| DRB1*01:88| DRB1*01:89| DRB1*01:90| DRB1*01:91Q| DRB1*01:92| DRB1*01:93| DRB1*01:94| DRB1*01:95| DRB1*01:96| DRB1*01:97| DRB1*01:98| DRB1*01:99</t>
+  </si>
+  <si>
+    <t>DRB1*10:01:01:01| DRB1*10:01:01:02| DRB1*10:01:01:03| DRB1*10:01:02| DRB1*10:01:03| DRB1*10:01:04| DRB1*10:01:05| DRB1*10:01:06| DRB1*10:01:07| DRB1*10:01:08| DRB1*10:01:09| DRB1*10:01:10| DRB1*10:01:11| DRB1*10:01:12| DRB1*10:02| DRB1*10:03| DRB1*10:04| DRB1*10:05| DRB1*10:06| DRB1*10:07| DRB1*10:08| DRB1*10:09| DRB1*10:10| DRB1*10:11| DRB1*10:12| DRB1*10:13| DRB1*10:14| DRB1*10:15| DRB1*10:16| DRB1*10:17| DRB1*10:18| DRB1*10:19| DRB1*10:20| DRB1*10:21| DRB1*10:22| DRB1*10:23| DRB1*10:24| DRB1*10:25| DRB1*10:26| DRB1*10:27| DRB1*10:28| DRB1*10:29| DRB1*10:30| DRB1*10:31| DRB1*10:32| DRB1*10:33</t>
+  </si>
+  <si>
+    <t>DRB1*01:03:01| DRB1*01:03:02| DRB1*01:03:03| DRB1*01:03:04</t>
+  </si>
+  <si>
+    <t>DRB1*08:31| DRB1*11:01:01:01| DRB1*11:01:01:02| DRB1*11:01:01:03| DRB1*11:01:01:04| DRB1*11:01:02| DRB1*11:01:03| DRB1*11:01:04| DRB1*11:01:05| DRB1*11:01:06| DRB1*11:01:07| DRB1*11:01:08| DRB1*11:01:09| DRB1*11:01:10| DRB1*11:01:11| DRB1*11:01:12| DRB1*11:01:13| DRB1*11:01:14| DRB1*11:01:15| DRB1*11:01:16| DRB1*11:01:17| DRB1*11:01:18| DRB1*11:01:19| DRB1*11:01:20| DRB1*11:01:21| DRB1*11:01:22| DRB1*11:01:23| DRB1*11:01:24| DRB1*11:01:25| DRB1*11:01:26| DRB1*11:01:27| DRB1*11:01:28| DRB1*11:01:29| DRB1*11:01:30| DRB1*11:01:31| DRB1*11:01:32| DRB1*11:01:33| DRB1*11:02:01| DRB1*11:02:02| DRB1*11:02:03| DRB1*11:02:04| DRB1*11:02:05| DRB1*11:03:01| DRB1*11:03:02| DRB1*11:03:03| DRB1*11:03:04| DRB1*11:04:01| DRB1*11:04:02| DRB1*11:04:03| DRB1*11:04:04| DRB1*11:04:05| DRB1*11:04:06| DRB1*11:04:07| DRB1*11:04:08| DRB1*11:04:09| DRB1*11:04:10| DRB1*11:04:11| DRB1*11:04:12| DRB1*11:04:13| DRB1*11:04:14| DRB1*11:04:15| DRB1*11:04:16| DRB1*11:04:17| DRB1*11:04:18| DRB1*11:05| DRB1*11:06:01| DRB1*11:06:02| DRB1*11:06:03| DRB1*11:07:01| DRB1*11:07:02| DRB1*11:08:01| DRB1*11:08:02| DRB1*11:08:03| DRB1*11:09| DRB1*11:10:01| DRB1*11:10:02| DRB1*11:11:01| DRB1*11:11:03| DRB1*11:12:01| DRB1*11:12:02| DRB1*11:12:03| DRB1*11:13:01| DRB1*11:13:02| DRB1*11:14:01| DRB1*11:14:02| DRB1*11:15| DRB1*11:16| DRB1*11:18| DRB1*11:19:01| DRB1*11:19:02| DRB1*11:19:03| DRB1*11:20| DRB1*11:21| DRB1*11:22| DRB1*11:23:01| DRB1*11:23:02| DRB1*11:24:01| DRB1*11:24:02| DRB1*11:25| DRB1*11:26| DRB1*11:27:01| DRB1*11:27:02| DRB1*11:27:03| DRB1*11:28:01| DRB1*11:28:02| DRB1*11:29:01| DRB1*11:29:02| DRB1*11:30| DRB1*11:31| DRB1*11:32| DRB1*11:33| DRB1*11:34| DRB1*11:35| DRB1*11:36| DRB1*11:37:01| DRB1*11:37:02| DRB1*11:38| DRB1*11:39| DRB1*11:40| DRB1*11:41| DRB1*11:42:01| DRB1*11:42:02| DRB1*11:43| DRB1*11:44| DRB1*11:45| DRB1*11:46:01| DRB1*11:46:02| DRB1*11:47| DRB1*11:48| DRB1*11:49:01| DRB1*11:49:02| DRB1*11:50| DRB1*11:51| DRB1*11:52| DRB1*11:53| DRB1*11:54:01| DRB1*11:54:02| DRB1*11:55| DRB1*11:56| DRB1*11:57| DRB1*11:58:01| DRB1*11:58:02| DRB1*11:59| DRB1*11:60| DRB1*11:61| DRB1*11:62:01| DRB1*11:62:02| DRB1*11:63:01| DRB1*11:63:02| DRB1*11:64| DRB1*11:65:01| DRB1*11:65:02| DRB1*11:66:01| DRB1*11:66:02| DRB1*11:67| DRB1*11:68| DRB1*11:69| DRB1*11:70| DRB1*11:72| DRB1*11:73| DRB1*11:74:01| DRB1*11:74:02| DRB1*11:75| DRB1*11:76| DRB1*11:77| DRB1*11:78| DRB1*11:79| DRB1*11:80| DRB1*11:81| DRB1*11:82| DRB1*11:83| DRB1*11:84:01| DRB1*11:84:02| DRB1*11:84:03| DRB1*11:85| DRB1*11:86| DRB1*11:87| DRB1*11:88| DRB1*11:89| DRB1*11:90| DRB1*11:91| DRB1*11:92| DRB1*11:93| DRB1*11:94| DRB1*11:95| DRB1*11:96| DRB1*11:97| DRB1*11:98| DRB1*11:99| DRB1*11:100| DRB1*11:101:01| DRB1*11:101:02| DRB1*11:102:01| DRB1*11:102:02| DRB1*11:103:01| DRB1*11:103:02| DRB1*11:104| DRB1*11:105| DRB1*11:106| DRB1*11:107| DRB1*11:108| DRB1*11:109| DRB1*11:110| DRB1*11:111| DRB1*11:112| DRB1*11:113| DRB1*11:114| DRB1*11:115| DRB1*11:116| DRB1*11:117:01| DRB1*11:117:02| DRB1*11:118| DRB1*11:119| DRB1*11:120| DRB1*11:121| DRB1*11:122| DRB1*11:123| DRB1*11:124:01| DRB1*11:124:02| DRB1*11:125| DRB1*11:126| DRB1*11:127| DRB1*11:128| DRB1*11:129| DRB1*11:130| DRB1*11:131| DRB1*11:132| DRB1*11:133| DRB1*11:134| DRB1*11:135| DRB1*11:136| DRB1*11:137| DRB1*11:138| DRB1*11:139| DRB1*11:140| DRB1*11:141| DRB1*11:142| DRB1*11:143| DRB1*11:144| DRB1*11:145| DRB1*11:146| DRB1*11:147:01| DRB1*11:147:02| DRB1*11:148| DRB1*11:149| DRB1*11:150| DRB1*11:151| DRB1*11:152| DRB1*11:153| DRB1*11:154| DRB1*11:155| DRB1*11:156| DRB1*11:157| DRB1*11:158| DRB1*11:159| DRB1*11:160| DRB1*11:161| DRB1*11:162| DRB1*11:163| DRB1*11:164| DRB1*11:165:01| DRB1*11:165:02| DRB1*11:166| DRB1*11:167| DRB1*11:168| DRB1*11:170| DRB1*11:171| DRB1*11:172| DRB1*11:173| DRB1*11:174| DRB1*11:175| DRB1*11:176| DRB1*11:177| DRB1*11:178| DRB1*11:179| DRB1*11:180| DRB1*11:181| DRB1*11:182| DRB1*11:183| DRB1*11:184| DRB1*11:185| DRB1*11:186| DRB1*11:187| DRB1*11:188| DRB1*11:189| DRB1*11:190| DRB1*11:191| DRB1*11:192| DRB1*11:193:01| DRB1*11:193:02| DRB1*11:194| DRB1*11:195| DRB1*11:196| DRB1*11:197| DRB1*11:198| DRB1*11:199| DRB1*11:200| DRB1*11:201| DRB1*11:202| DRB1*11:203| DRB1*11:204| DRB1*11:205| DRB1*11:206| DRB1*11:207| DRB1*11:208| DRB1*11:209| DRB1*11:210| DRB1*11:211| DRB1*11:212| DRB1*11:213| DRB1*11:214| DRB1*11:215| DRB1*11:216| DRB1*11:218| DRB1*11:219| DRB1*11:220| DRB1*11:221| DRB1*11:222| DRB1*11:223| DRB1*11:224| DRB1*11:225| DRB1*11:226| DRB1*11:227| DRB1*11:228| DRB1*11:229| DRB1*11:230| DRB1*11:231| DRB1*11:232| DRB1*11:233| DRB1*11:234| DRB1*11:235| DRB1*11:236| DRB1*11:237| DRB1*11:238| DRB1*11:239| DRB1*11:240| DRB1*11:241| DRB1*11:242| DRB1*11:243| DRB1*11:244| DRB1*11:245| DRB1*11:247| DRB1*11:248Q| DRB1*11:249| DRB1*11:251| DRB1*11:252| DRB1*11:253| DRB1*11:254| DRB1*13:24| DRB1*13:25| DRB1*13:46| DRB1*13:50:01| DRB1*13:50:02| DRB1*13:50:03| DRB1*13:62</t>
+  </si>
+  <si>
+    <t>DRB1*12:01:01:01| DRB1*12:01:01:02| DRB1*12:01:01:03| DRB1*12:01:01:04| DRB1*12:01:01:05| DRB1*12:01:01:06| DRB1*12:01:02| DRB1*12:01:03| DRB1*12:01:04| DRB1*12:01:05| DRB1*12:01:06| DRB1*12:01:07| DRB1*12:01:08| DRB1*12:01:09| DRB1*12:02:01:01| DRB1*12:02:01:02| DRB1*12:02:01:03| DRB1*12:02:01:04| DRB1*12:02:02| DRB1*12:02:03| DRB1*12:02:04| DRB1*12:02:05| DRB1*12:02:06| DRB1*12:02:07| DRB1*12:02:08| DRB1*12:03:02| DRB1*12:03:03| DRB1*12:04| DRB1*12:05| DRB1*12:06| DRB1*12:07| DRB1*12:08| DRB1*12:09| DRB1*12:10| DRB1*12:11| DRB1*12:12| DRB1*12:13| DRB1*12:14| DRB1*12:15| DRB1*12:16:01| DRB1*12:16:02| DRB1*12:16:03| DRB1*12:17| DRB1*12:18| DRB1*12:19| DRB1*12:20| DRB1*12:21| DRB1*12:22| DRB1*12:23| DRB1*12:25| DRB1*12:26| DRB1*12:27| DRB1*12:28| DRB1*12:29| DRB1*12:30| DRB1*12:32| DRB1*12:33| DRB1*12:34| DRB1*12:35| DRB1*12:36| DRB1*12:37| DRB1*12:38| DRB1*12:39| DRB1*12:40| DRB1*12:41| DRB1*12:42| DRB1*12:43| DRB1*12:44| DRB1*12:45| DRB1*12:46| DRB1*12:47| DRB1*12:48| DRB1*12:49| DRB1*12:50| DRB1*12:51| DRB1*12:52| DRB1*12:53| DRB1*12:54| DRB1*12:55| DRB1*12:56| DRB1*12:57| DRB1*12:58| DRB1*12:59| DRB1*12:61| DRB1*12:62| DRB1*12:63| DRB1*12:64| DRB1*12:65| DRB1*12:66| DRB1*12:67| DRB1*12:68| DRB1*12:69| DRB1*12:70| DRB1*12:71| DRB1*12:73| DRB1*12:75</t>
+  </si>
+  <si>
+    <t>DRB1*13:01:01:01| DRB1*13:01:01:02| DRB1*13:01:02| DRB1*13:01:03| DRB1*13:01:04| DRB1*13:01:05| DRB1*13:01:06| DRB1*13:01:07| DRB1*13:01:08| DRB1*13:01:09| DRB1*13:01:10| DRB1*13:01:11| DRB1*13:01:12| DRB1*13:01:13| DRB1*13:01:14| DRB1*13:01:15| DRB1*13:01:16| DRB1*13:01:17| DRB1*13:01:18| DRB1*13:01:19| DRB1*13:01:20| DRB1*13:01:21| DRB1*13:01:22| DRB1*13:01:23| DRB1*13:01:24| DRB1*13:01:25| DRB1*13:01:26| DRB1*13:02:01:01| DRB1*13:02:01:02| DRB1*13:02:01:03| DRB1*13:02:02| DRB1*13:02:03| DRB1*13:02:04| DRB1*13:02:05| DRB1*13:02:06| DRB1*13:02:07| DRB1*13:02:08| DRB1*13:02:09| DRB1*13:02:10| DRB1*13:02:11| DRB1*13:02:12| DRB1*13:02:13| DRB1*13:02:14| DRB1*13:02:15| DRB1*13:02:16| DRB1*13:02:17| DRB1*13:03:01| DRB1*13:03:02| DRB1*13:03:03| DRB1*13:03:04| DRB1*13:03:05| DRB1*13:03:06| DRB1*13:03:07| DRB1*13:03:08| DRB1*13:03:09| DRB1*13:04| DRB1*13:05:01| DRB1*13:05:02| DRB1*13:05:03| DRB1*13:06| DRB1*13:07:01| DRB1*13:07:02| DRB1*13:08| DRB1*13:09| DRB1*13:10| DRB1*13:11:01| DRB1*13:11:02| DRB1*13:12:01| DRB1*13:12:02| DRB1*13:12:03| DRB1*13:12:04| DRB1*13:13| DRB1*13:14:01| DRB1*13:14:02| DRB1*13:14:03| DRB1*13:15| DRB1*13:16| DRB1*13:17| DRB1*13:18| DRB1*13:19| DRB1*13:20| DRB1*13:21:01| DRB1*13:21:02| DRB1*13:22:01| DRB1*13:22:02| DRB1*13:23:01| DRB1*13:23:02| DRB1*13:27| DRB1*13:28| DRB1*13:29| DRB1*13:30| DRB1*13:31| DRB1*13:32| DRB1*13:33:01| DRB1*13:33:02| DRB1*13:33:03| DRB1*13:34| DRB1*13:35| DRB1*13:36| DRB1*13:37| DRB1*13:38| DRB1*13:39| DRB1*13:40| DRB1*13:41| DRB1*13:42| DRB1*13:43| DRB1*13:44| DRB1*13:45| DRB1*13:47| DRB1*13:48| DRB1*13:51| DRB1*13:52| DRB1*13:53| DRB1*13:55| DRB1*13:57| DRB1*13:58| DRB1*13:59| DRB1*13:61:01| DRB1*13:61:02| DRB1*13:63| DRB1*13:64| DRB1*13:65| DRB1*13:66:01| DRB1*13:66:02| DRB1*13:67| DRB1*13:68| DRB1*13:69| DRB1*13:70| DRB1*13:71| DRB1*13:72| DRB1*13:73| DRB1*13:74| DRB1*13:75| DRB1*13:76| DRB1*13:77| DRB1*13:78| DRB1*13:79| DRB1*13:80| DRB1*13:81| DRB1*13:82| DRB1*13:83| DRB1*13:84| DRB1*13:85| DRB1*13:86| DRB1*13:87| DRB1*13:88| DRB1*13:89:01| DRB1*13:89:02| DRB1*13:90| DRB1*13:91| DRB1*13:92| DRB1*13:93| DRB1*13:94:01| DRB1*13:94:02| DRB1*13:95| DRB1*13:96:01| DRB1*13:96:02| DRB1*13:97:01| DRB1*13:97:02| DRB1*13:98| DRB1*13:99| DRB1*13:100| DRB1*13:101| DRB1*13:102| DRB1*13:103| DRB1*13:104| DRB1*13:105| DRB1*13:106| DRB1*13:107| DRB1*13:108| DRB1*13:109| DRB1*13:110| DRB1*13:111| DRB1*13:112| DRB1*13:114| DRB1*13:115| DRB1*13:116| DRB1*13:117| DRB1*13:118| DRB1*13:119| DRB1*13:120| DRB1*13:121| DRB1*13:122| DRB1*13:123| DRB1*13:124| DRB1*13:125| DRB1*13:126| DRB1*13:127| DRB1*13:128| DRB1*13:129| DRB1*13:130| DRB1*13:131| DRB1*13:132| DRB1*13:133| DRB1*13:134| DRB1*13:135| DRB1*13:136| DRB1*13:138| DRB1*13:139| DRB1*13:140| DRB1*13:141| DRB1*13:143| DRB1*13:144| DRB1*13:145| DRB1*13:146| DRB1*13:147| DRB1*13:148| DRB1*13:149| DRB1*13:150| DRB1*13:151| DRB1*13:152| DRB1*13:153| DRB1*13:154| DRB1*13:155| DRB1*13:156| DRB1*13:157| DRB1*13:158| DRB1*13:159| DRB1*13:160| DRB1*13:161| DRB1*13:162| DRB1*13:163| DRB1*13:164| DRB1*13:165| DRB1*13:166| DRB1*13:167| DRB1*13:168| DRB1*13:169| DRB1*13:170| DRB1*13:171:01| DRB1*13:171:02| DRB1*13:172| DRB1*13:173| DRB1*13:174| DRB1*13:175| DRB1*13:176| DRB1*13:177| DRB1*13:178| DRB1*13:179| DRB1*13:180| DRB1*13:181| DRB1*13:182| DRB1*13:183| DRB1*13:184| DRB1*13:186| DRB1*13:187| DRB1*13:188| DRB1*13:189| DRB1*13:190| DRB1*13:191| DRB1*13:192| DRB1*13:193| DRB1*13:194| DRB1*13:195| DRB1*13:196| DRB1*13:197| DRB1*13:198| DRB1*13:199| DRB1*13:201| DRB1*13:202| DRB1*13:203| DRB1*13:204| DRB1*13:205| DRB1*13:206| DRB1*13:207| DRB1*13:208| DRB1*13:209| DRB1*13:210| DRB1*13:211| DRB1*13:212| DRB1*13:213| DRB1*13:214| DRB1*13:215| DRB1*13:216| DRB1*13:217| DRB1*13:218| DRB1*13:219| DRB1*13:220| DRB1*13:221| DRB1*13:222| DRB1*13:223| DRB1*13:224| DRB1*13:225| DRB1*13:226| DRB1*13:227| DRB1*13:228| DRB1*13:229| DRB1*13:230| DRB1*13:231| DRB1*13:232| DRB1*13:233| DRB1*13:234| DRB1*13:235| DRB1*13:236| DRB1*13:237| DRB1*13:238| DRB1*13:239| DRB1*13:240| DRB1*13:241| DRB1*13:242:01| DRB1*13:242:02| DRB1*13:243| DRB1*13:244| DRB1*13:245| DRB1*13:246| DRB1*13:247| DRB1*13:248| DRB1*13:250| DRB1*13:251| DRB1*13:253| DRB1*13:254| DRB1*13:256| DRB1*13:257| DRB1*13:258| DRB1*13:259| DRB1*13:260| DRB1*13:261| DRB1*13:262| DRB1*13:263| DRB1*13:264| DRB1*13:265| DRB1*13:266| DRB1*13:267| DRB1*13:269| DRB1*13:270| DRB1*13:271| DRB1*13:272| DRB1*13:273| DRB1*13:274| DRB1*13:275| DRB1*13:276| DRB1*14:53</t>
+  </si>
+  <si>
+    <t>DRB1*11:17| DRB1*13:26:01| DRB1*13:26:02| DRB1*13:54| DRB1*14:01:01| DRB1*14:01:02| DRB1*14:01:03| DRB1*14:01:04| DRB1*14:02:01:01| DRB1*14:02:01:02| DRB1*14:02:02| DRB1*14:02:03| DRB1*14:02:04| DRB1*14:02:05| DRB1*14:02:06| DRB1*14:02:07| DRB1*14:05:01:01| DRB1*14:05:01:02| DRB1*14:05:02| DRB1*14:05:03| DRB1*14:05:04| DRB1*14:06:01| DRB1*14:06:02| DRB1*14:06:03| DRB1*14:06:04| DRB1*14:07:01| DRB1*14:07:02| DRB1*14:08| DRB1*14:09| DRB1*14:10| DRB1*14:11| DRB1*14:12:01| DRB1*14:12:02| DRB1*14:13| DRB1*14:14| DRB1*14:19| DRB1*14:20| DRB1*14:21| DRB1*14:22| DRB1*14:23:01| DRB1*14:23:02| DRB1*14:23:03| DRB1*14:23:04| DRB1*14:24| DRB1*14:26| DRB1*14:27:01| DRB1*14:27:02| DRB1*14:28| DRB1*14:29| DRB1*14:31| DRB1*14:32:01| DRB1*14:32:02| DRB1*14:32:03| DRB1*14:34| DRB1*14:35| DRB1*14:36| DRB1*14:37| DRB1*14:38:01| DRB1*14:38:02| DRB1*14:39| DRB1*14:40| DRB1*14:41| DRB1*14:42| DRB1*14:43| DRB1*14:44:01| DRB1*14:44:02| DRB1*14:44:03| DRB1*14:45| DRB1*14:46| DRB1*14:47| DRB1*14:48| DRB1*14:49| DRB1*14:50| DRB1*14:51| DRB1*14:52| DRB1*14:54:01:01| DRB1*14:54:01:02| DRB1*14:54:01:03| DRB1*14:54:01:04| DRB1*14:54:02| DRB1*14:54:03| DRB1*14:54:04| DRB1*14:54:05| DRB1*14:54:06| DRB1*14:54:07| DRB1*14:55| DRB1*14:56| DRB1*14:57| DRB1*14:58| DRB1*14:59| DRB1*14:60| DRB1*14:61| DRB1*14:62| DRB1*14:64| DRB1*14:68:01| DRB1*14:68:02| DRB1*14:69| DRB1*14:70| DRB1*14:71| DRB1*14:72| DRB1*14:73| DRB1*14:74| DRB1*14:75| DRB1*14:76| DRB1*14:77| DRB1*14:78| DRB1*14:79| DRB1*14:80| DRB1*14:81| DRB1*14:82| DRB1*14:83| DRB1*14:84| DRB1*14:85| DRB1*14:86| DRB1*14:87| DRB1*14:88| DRB1*14:89| DRB1*14:90| DRB1*14:91| DRB1*14:93| DRB1*14:94| DRB1*14:95| DRB1*14:96| DRB1*14:97| DRB1*14:98| DRB1*14:99| DRB1*14:100| DRB1*14:101| DRB1*14:102| DRB1*14:103| DRB1*14:104| DRB1*14:105| DRB1*14:106| DRB1*14:107| DRB1*14:108| DRB1*14:109| DRB1*14:110| DRB1*14:111| DRB1*14:112| DRB1*14:113| DRB1*14:114| DRB1*14:115| DRB1*14:116| DRB1*14:117| DRB1*14:118| DRB1*14:119| DRB1*14:120| DRB1*14:121| DRB1*14:122| DRB1*14:123| DRB1*14:124| DRB1*14:125| DRB1*14:126:01| DRB1*14:126:02| DRB1*14:127:01| DRB1*14:127:02| DRB1*14:128| DRB1*14:129| DRB1*14:130| DRB1*14:131| DRB1*14:132| DRB1*14:133| DRB1*14:134| DRB1*14:135| DRB1*14:136| DRB1*14:138| DRB1*14:139| DRB1*14:140| DRB1*14:141| DRB1*14:142| DRB1*14:143| DRB1*14:144| DRB1*14:145| DRB1*14:146| DRB1*14:147| DRB1*14:148| DRB1*14:149| DRB1*14:150| DRB1*14:151| DRB1*14:153| DRB1*14:154| DRB1*14:155| DRB1*14:156| DRB1*14:157| DRB1*14:158| DRB1*14:159| DRB1*14:160| DRB1*14:161| DRB1*14:162| DRB1*14:163| DRB1*14:164| DRB1*14:165| DRB1*14:167| DRB1*14:168| DRB1*14:169| DRB1*14:170| DRB1*14:171| DRB1*14:172| DRB1*14:173| DRB1*14:174| DRB1*14:175| DRB1*14:176| DRB1*14:177| DRB1*14:178| DRB1*14:179| DRB1*14:180| DRB1*14:181| DRB1*14:182| DRB1*14:183| DRB1*14:184| DRB1*14:185| DRB1*14:187| DRB1*14:189| DRB1*14:190| DRB1*14:191| DRB1*14:192| DRB1*14:193| DRB1*14:194| DRB1*14:196| DRB1*14:198| DRB1*14:199| DRB1*14:200| DRB1*14:201| DRB1*14:202| DRB1*14:203| DRB1*14:204| DRB1*14:205| DRB1*14:206| DRB1*14:207| DRB1*14:03:01| DRB1*14:03:02| DRB1*14:04:01| DRB1*14:04:02| DRB1*14:04:03| DRB1*14:04:04| DRB1*14:04:05| DRB1*14:04:06</t>
+  </si>
+  <si>
+    <t>DRB1*14:03:01| DRB1*14:03:02</t>
+  </si>
+  <si>
+    <t>DRB1*14:04:01| DRB1*14:04:02| DRB1*14:04:03| DRB1*14:04:04| DRB1*14:04:05| DRB1*14:04:06</t>
+  </si>
+  <si>
+    <t>DRB1*15:01:01:01| DRB1*15:01:01:02| DRB1*15:01:01:03| DRB1*15:01:01:04| DRB1*15:01:01:05| DRB1*15:01:02| DRB1*15:01:03| DRB1*15:01:04| DRB1*15:01:05| DRB1*15:01:06| DRB1*15:01:07| DRB1*15:01:08| DRB1*15:01:09| DRB1*15:01:10| DRB1*15:01:11| DRB1*15:01:12| DRB1*15:01:13| DRB1*15:01:14| DRB1*15:01:15| DRB1*15:01:16| DRB1*15:01:17| DRB1*15:01:18| DRB1*15:01:19| DRB1*15:01:20| DRB1*15:01:21| DRB1*15:01:22| DRB1*15:01:23| DRB1*15:01:24| DRB1*15:01:25| DRB1*15:01:26| DRB1*15:01:27| DRB1*15:01:28| DRB1*15:01:29| DRB1*15:01:30| DRB1*15:01:31| DRB1*15:01:32| DRB1*15:01:33| DRB1*15:01:34| DRB1*15:01:35| DRB1*15:01:36| DRB1*15:01:37| DRB1*15:01:38| DRB1*15:02:01:01| DRB1*15:02:01:02| DRB1*15:02:01:03| DRB1*15:02:02| DRB1*15:02:03| DRB1*15:02:04| DRB1*15:02:05| DRB1*15:02:06| DRB1*15:02:07| DRB1*15:02:08| DRB1*15:02:09| DRB1*15:02:10| DRB1*15:02:11| DRB1*15:02:12| DRB1*15:02:13| DRB1*15:02:14| DRB1*15:02:15| DRB1*15:02:16| DRB1*15:02:17| DRB1*15:02:18| DRB1*15:02:19| DRB1*15:03:01:01| DRB1*15:03:01:02| DRB1*15:03:02| DRB1*15:03:03| DRB1*15:04| DRB1*15:05| DRB1*15:06:01| DRB1*15:06:02| DRB1*15:06:03| DRB1*15:07:01| DRB1*15:07:02| DRB1*15:07:03| DRB1*15:09| DRB1*15:11| DRB1*15:12| DRB1*15:14| DRB1*15:15:01| DRB1*15:15:02| DRB1*15:15:03| DRB1*15:16| DRB1*15:18| DRB1*15:19| DRB1*15:20| DRB1*15:22| DRB1*15:23| DRB1*15:24| DRB1*15:25| DRB1*15:26| DRB1*15:27| DRB1*15:28| DRB1*15:29| DRB1*15:30| DRB1*15:31| DRB1*15:32| DRB1*15:33| DRB1*15:34| DRB1*15:35| DRB1*15:36| DRB1*15:37:01| DRB1*15:37:02| DRB1*15:38| DRB1*15:39| DRB1*15:40| DRB1*15:41| DRB1*15:42| DRB1*15:43| DRB1*15:44| DRB1*15:45| DRB1*15:46| DRB1*15:47| DRB1*15:48| DRB1*15:49| DRB1*15:51| DRB1*15:52| DRB1*15:53| DRB1*15:54| DRB1*15:55| DRB1*15:56| DRB1*15:57| DRB1*15:58| DRB1*15:59| DRB1*15:60| DRB1*15:61| DRB1*15:62| DRB1*15:63| DRB1*15:64| DRB1*15:65| DRB1*15:66:01| DRB1*15:66:02| DRB1*15:67| DRB1*15:68| DRB1*15:69| DRB1*15:70| DRB1*15:71| DRB1*15:72| DRB1*15:73| DRB1*15:74| DRB1*15:75| DRB1*15:76| DRB1*15:77| DRB1*15:78| DRB1*15:79| DRB1*15:81| DRB1*15:82| DRB1*15:83| DRB1*15:84| DRB1*15:85| DRB1*15:86| DRB1*15:87| DRB1*15:88| DRB1*15:89| DRB1*15:90| DRB1*15:91| DRB1*15:92| DRB1*15:93| DRB1*15:94| DRB1*15:95| DRB1*15:96| DRB1*15:97| DRB1*15:98| DRB1*15:99| DRB1*15:100| DRB1*15:101| DRB1*15:102| DRB1*15:103| DRB1*15:104:01| DRB1*15:104:02| DRB1*15:104:03| DRB1*15:105:01| DRB1*15:105:02| DRB1*15:106| DRB1*15:107| DRB1*15:108| DRB1*15:109| DRB1*15:110| DRB1*15:111| DRB1*15:112| DRB1*15:114| DRB1*15:116| DRB1*15:117| DRB1*15:118| DRB1*15:119| DRB1*15:120| DRB1*15:121| DRB1*15:122| DRB1*15:123| DRB1*15:124| DRB1*15:125| DRB1*15:126| DRB1*15:127| DRB1*15:128| DRB1*15:130| DRB1*15:131| DRB1*15:132| DRB1*15:133| DRB1*15:135| DRB1*15:136| DRB1*15:139| DRB1*15:140| DRB1*15:141| DRB1*15:142| DRB1*15:143| DRB1*15:144| DRB1*15:145| DRB1*15:146| DRB1*15:147| DRB1*15:149| DRB1*15:150| DRB1*15:151| DRB1*15:152| DRB1*15:153| DRB1*15:155| DRB1*15:156| DRB1*15:157| DRB1*15:158| DRB1*15:160| DRB1*15:161| DRB1*15:162</t>
+  </si>
+  <si>
+    <t>DRB1*16:01:01| DRB1*16:01:02| DRB1*16:01:03| DRB1*16:01:04| DRB1*16:01:05| DRB1*16:01:06| DRB1*16:01:07| DRB1*16:01:08| DRB1*16:01:09| DRB1*16:01:10| DRB1*16:01:11| DRB1*16:01:12| DRB1*16:01:13| DRB1*16:01:14| DRB1*16:01:15| DRB1*16:02:01:01| DRB1*16:02:01:02| DRB1*16:02:01:03| DRB1*16:02:02| DRB1*16:02:03| DRB1*16:02:04| DRB1*16:02:05| DRB1*16:02:06| DRB1*16:02:07| DRB1*16:04:01| DRB1*16:04:02| DRB1*16:05:01| DRB1*16:05:02| DRB1*16:07| DRB1*16:08| DRB1*16:09:01| DRB1*16:09:02| DRB1*16:10:01| DRB1*16:10:02| DRB1*16:11| DRB1*16:12| DRB1*16:14| DRB1*16:15| DRB1*16:16| DRB1*16:17| DRB1*16:18| DRB1*16:19| DRB1*16:20| DRB1*16:22| DRB1*16:23| DRB1*16:24| DRB1*16:25| DRB1*16:26| DRB1*16:27| DRB1*16:28| DRB1*16:29| DRB1*16:30| DRB1*16:31| DRB1*16:32| DRB1*16:33| DRB1*16:34| DRB1*16:35| DRB1*16:36| DRB1*16:37| DRB1*16:38:01| DRB1*16:38:02| DRB1*16:39| DRB1*16:40| DRB1*16:42| DRB1*16:43| DRB1*16:44| DRB1*16:45| DRB1*16:46| DRB1*16:47| DRB1*16:48| DRB1*16:49| DRB1*16:50| DRB1*16:51| DRB1*16:52| DRB1*16:53</t>
+  </si>
+  <si>
+    <t>DRB1*03:01:01:01| DRB1*03:01:01:02| DRB1*03:01:01:03| DRB1*03:01:02| DRB1*03:01:03| DRB1*03:01:04| DRB1*03:01:05| DRB1*03:01:06| DRB1*03:01:07| DRB1*03:01:08| DRB1*03:01:09| DRB1*03:01:10| DRB1*03:01:11| DRB1*03:01:12| DRB1*03:01:13| DRB1*03:01:14| DRB1*03:01:15| DRB1*03:01:16| DRB1*03:01:17| DRB1*03:01:18| DRB1*03:01:19| DRB1*03:01:20| DRB1*03:01:21| DRB1*03:01:22| DRB1*03:01:23| DRB1*03:01:24| DRB1*03:01:25| DRB1*03:01:26| DRB1*03:01:27| DRB1*03:01:28| DRB1*03:04:01| DRB1*03:04:02| DRB1*03:10| DRB1*03:11:01| DRB1*03:43</t>
+  </si>
+  <si>
+    <t>DRB1*03:02:01| DRB1*03:02:02| DRB1*03:02:03| DRB1*03:03</t>
+  </si>
+  <si>
+    <t>DRB1*15:08| DRB1*15:10| DRB1*15:13| DRB1*15:21| DRB1*16:03| DRB3*02:61Q| DRB1*15:01:01:01| DRB1*15:01:01:02| DRB1*15:01:01:03| DRB1*15:01:01:04| DRB1*15:01:01:05| DRB1*15:01:02| DRB1*15:01:03| DRB1*15:01:04| DRB1*15:01:05| DRB1*15:01:06| DRB1*15:01:07| DRB1*15:01:08| DRB1*15:01:09| DRB1*15:01:10| DRB1*15:01:11| DRB1*15:01:12| DRB1*15:01:13| DRB1*15:01:14| DRB1*15:01:15| DRB1*15:01:16| DRB1*15:01:17| DRB1*15:01:18| DRB1*15:01:19| DRB1*15:01:20| DRB1*15:01:21| DRB1*15:01:22| DRB1*15:01:23| DRB1*15:01:24| DRB1*15:01:25| DRB1*15:01:26| DRB1*15:01:27| DRB1*15:01:28| DRB1*15:01:29| DRB1*15:01:30| DRB1*15:01:31| DRB1*15:01:32| DRB1*15:01:33| DRB1*15:01:34| DRB1*15:01:35| DRB1*15:01:36| DRB1*15:01:37| DRB1*15:01:38| DRB1*15:02:01:01| DRB1*15:02:01:02| DRB1*15:02:01:03| DRB1*15:02:02| DRB1*15:02:03| DRB1*15:02:04| DRB1*15:02:05| DRB1*15:02:06| DRB1*15:02:07| DRB1*15:02:08| DRB1*15:02:09| DRB1*15:02:10| DRB1*15:02:11| DRB1*15:02:12| DRB1*15:02:13| DRB1*15:02:14| DRB1*15:02:15| DRB1*15:02:16| DRB1*15:02:17| DRB1*15:02:18| DRB1*15:02:19| DRB1*15:03:01:01| DRB1*15:03:01:02| DRB1*15:03:02| DRB1*15:03:03| DRB1*15:04| DRB1*15:05| DRB1*15:06:01| DRB1*15:06:02| DRB1*15:06:03| DRB1*15:07:01| DRB1*15:07:02| DRB1*15:07:03| DRB1*15:09| DRB1*15:11| DRB1*15:12| DRB1*15:14| DRB1*15:15:01| DRB1*15:15:02| DRB1*15:15:03| DRB1*15:16| DRB1*15:18| DRB1*15:19| DRB1*15:20| DRB1*15:22| DRB1*15:23| DRB1*15:24| DRB1*15:25| DRB1*15:26| DRB1*15:27| DRB1*15:28| DRB1*15:29| DRB1*15:30| DRB1*15:31| DRB1*15:32| DRB1*15:33| DRB1*15:34| DRB1*15:35| DRB1*15:36| DRB1*15:37:01| DRB1*15:37:02| DRB1*15:38| DRB1*15:39| DRB1*15:40| DRB1*15:41| DRB1*15:42| DRB1*15:43| DRB1*15:44| DRB1*15:45| DRB1*15:46| DRB1*15:47| DRB1*15:48| DRB1*15:49| DRB1*15:51| DRB1*15:52| DRB1*15:53| DRB1*15:54| DRB1*15:55| DRB1*15:56| DRB1*15:57| DRB1*15:58| DRB1*15:59| DRB1*15:60| DRB1*15:61| DRB1*15:62| DRB1*15:63| DRB1*15:64| DRB1*15:65| DRB1*15:66:01| DRB1*15:66:02| DRB1*15:67| DRB1*15:68| DRB1*15:69| DRB1*15:70| DRB1*15:71| DRB1*15:72| DRB1*15:73| DRB1*15:74| DRB1*15:75| DRB1*15:76| DRB1*15:77| DRB1*15:78| DRB1*15:79| DRB1*15:81| DRB1*15:82| DRB1*15:83| DRB1*15:84| DRB1*15:85| DRB1*15:86| DRB1*15:87| DRB1*15:88| DRB1*15:89| DRB1*15:90| DRB1*15:91| DRB1*15:92| DRB1*15:93| DRB1*15:94| DRB1*15:95| DRB1*15:96| DRB1*15:97| DRB1*15:98| DRB1*15:99| DRB1*15:100| DRB1*15:101| DRB1*15:102| DRB1*15:103| DRB1*15:104:01| DRB1*15:104:02| DRB1*15:104:03| DRB1*15:105:01| DRB1*15:105:02| DRB1*15:106| DRB1*15:107| DRB1*15:108| DRB1*15:109| DRB1*15:110| DRB1*15:111| DRB1*15:112| DRB1*15:114| DRB1*15:116| DRB1*15:117| DRB1*15:118| DRB1*15:119| DRB1*15:120| DRB1*15:121| DRB1*15:122| DRB1*15:123| DRB1*15:124| DRB1*15:125| DRB1*15:126| DRB1*15:127| DRB1*15:128| DRB1*15:130| DRB1*15:131| DRB1*15:132| DRB1*15:133| DRB1*15:135| DRB1*15:136| DRB1*15:139| DRB1*15:140| DRB1*15:141| DRB1*15:142| DRB1*15:143| DRB1*15:144| DRB1*15:145| DRB1*15:146| DRB1*15:147| DRB1*15:149| DRB1*15:150| DRB1*15:151| DRB1*15:152| DRB1*15:153| DRB1*15:155| DRB1*15:156| DRB1*15:157| DRB1*15:158| DRB1*15:160| DRB1*15:161| DRB1*15:162| DRB1*16:01:01| DRB1*16:01:02| DRB1*16:01:03| DRB1*16:01:04| DRB1*16:01:05| DRB1*16:01:06| DRB1*16:01:07| DRB1*16:01:08| DRB1*16:01:09| DRB1*16:01:10| DRB1*16:01:11| DRB1*16:01:12| DRB1*16:01:13| DRB1*16:01:14| DRB1*16:01:15| DRB1*16:02:01:01| DRB1*16:02:01:02| DRB1*16:02:01:03| DRB1*16:02:02| DRB1*16:02:03| DRB1*16:02:04| DRB1*16:02:05| DRB1*16:02:06| DRB1*16:02:07| DRB1*16:04:01| DRB1*16:04:02| DRB1*16:05:01| DRB1*16:05:02| DRB1*16:07| DRB1*16:08| DRB1*16:09:01| DRB1*16:09:02| DRB1*16:10:01| DRB1*16:10:02| DRB1*16:11| DRB1*16:12| DRB1*16:14| DRB1*16:15| DRB1*16:16| DRB1*16:17| DRB1*16:18| DRB1*16:19| DRB1*16:20| DRB1*16:22| DRB1*16:23| DRB1*16:24| DRB1*16:25| DRB1*16:26| DRB1*16:27| DRB1*16:28| DRB1*16:29| DRB1*16:30| DRB1*16:31| DRB1*16:32| DRB1*16:33| DRB1*16:34| DRB1*16:35| DRB1*16:36| DRB1*16:37| DRB1*16:38:01| DRB1*16:38:02| DRB1*16:39| DRB1*16:40| DRB1*16:42| DRB1*16:43| DRB1*16:44| DRB1*16:45| DRB1*16:46| DRB1*16:47| DRB1*16:48| DRB1*16:49| DRB1*16:50| DRB1*16:51| DRB1*16:52| DRB1*16:53</t>
+  </si>
+  <si>
+    <t>DRB1*03:05:01| DRB1*03:05:02| DRB1*03:05:03| DRB1*03:06| DRB1*03:07:01| DRB1*03:07:02| DRB1*03:08| DRB1*03:09| DRB1*03:12| DRB1*03:13:01| DRB1*03:13:02| DRB1*03:14| DRB1*03:15:01| DRB1*03:15:02| DRB1*03:16| DRB1*03:17| DRB1*03:18| DRB1*03:19| DRB1*03:20| DRB1*03:21| DRB1*03:22| DRB1*03:23| DRB1*03:24| DRB1*03:25:01| DRB1*03:25:02| DRB1*03:26| DRB1*03:27| DRB1*03:28| DRB1*03:29| DRB1*03:30| DRB1*03:31| DRB1*03:32| DRB1*03:33| DRB1*03:34| DRB1*03:35| DRB1*03:36| DRB1*03:37| DRB1*03:38| DRB1*03:39| DRB1*03:40| DRB1*03:41:01| DRB1*03:41:02| DRB1*03:42| DRB1*03:44| DRB1*03:45| DRB1*03:46| DRB1*03:47| DRB1*03:48| DRB1*03:49| DRB1*03:50| DRB1*03:51| DRB1*03:52| DRB1*03:53| DRB1*03:54| DRB1*03:55| DRB1*03:56| DRB1*03:57| DRB1*03:58| DRB1*03:59| DRB1*03:60| DRB1*03:61| DRB1*03:62| DRB1*03:63| DRB1*03:64| DRB1*03:65| DRB1*03:66| DRB1*03:69| DRB1*03:70| DRB1*03:71:01| DRB1*03:71:02| DRB1*03:72| DRB1*03:73| DRB1*03:74| DRB1*03:75| DRB1*03:76| DRB1*03:77| DRB1*03:78| DRB1*03:79| DRB1*03:80| DRB1*03:81| DRB1*03:82| DRB1*03:83| DRB1*03:84| DRB1*03:85| DRB1*03:86| DRB1*03:87| DRB1*03:88| DRB1*03:89| DRB1*03:90| DRB1*03:91| DRB1*03:92| DRB1*03:93| DRB1*03:94| DRB1*03:95| DRB1*03:96| DRB1*03:97| DRB1*03:98| DRB1*03:99| DRB1*03:100:01| DRB1*03:100:02| DRB1*03:101| DRB1*03:102| DRB1*03:103| DRB1*03:104| DRB1*03:105| DRB1*03:106| DRB1*03:107| DRB1*03:108| DRB1*03:109| DRB1*03:110| DRB1*03:111| DRB1*03:112| DRB1*03:113| DRB1*03:114| DRB1*03:115| DRB1*03:116| DRB1*03:117| DRB1*03:118| DRB1*03:119| DRB1*03:120| DRB1*03:121| DRB1*03:122| DRB1*03:123| DRB1*03:124| DRB1*03:125| DRB1*03:126| DRB1*03:127| DRB1*03:128| DRB1*03:129| DRB1*03:130| DRB1*03:131| DRB1*03:132| DRB1*03:133| DRB1*03:134| DRB1*03:135| DRB1*03:136| DRB1*03:137| DRB1*03:138| DRB1*03:139| DRB1*03:140| DRB1*03:141| DRB1*03:142| DRB1*03:143| DRB1*03:144| DRB1*03:145| DRB1*03:146| DRB1*03:147| DRB1*03:148| DRB1*03:149| DRB1*03:150| DRB1*03:151| DRB1*03:152| DRB1*03:153| DRB1*03:154| DRB1*03:155| DRB1*03:157| DRB1*03:158| DRB1*03:01:01:01| DRB1*03:01:01:02| DRB1*03:01:01:03| DRB1*03:01:02| DRB1*03:01:03| DRB1*03:01:04| DRB1*03:01:05| DRB1*03:01:06| DRB1*03:01:07| DRB1*03:01:08| DRB1*03:01:09| DRB1*03:01:10| DRB1*03:01:11| DRB1*03:01:12| DRB1*03:01:13| DRB1*03:01:14| DRB1*03:01:15| DRB1*03:01:16| DRB1*03:01:17| DRB1*03:01:18| DRB1*03:01:19| DRB1*03:01:20| DRB1*03:01:21| DRB1*03:01:22| DRB1*03:01:23| DRB1*03:01:24| DRB1*03:01:25| DRB1*03:01:26| DRB1*03:01:27| DRB1*03:01:28| DRB1*03:04:01| DRB1*03:04:02| DRB1*03:10| DRB1*03:11:01| DRB1*03:43| DRB1*03:02:01| DRB1*03:02:02| DRB1*03:02:03| DRB1*03:03</t>
+  </si>
+  <si>
+    <t>DRB1*04:01:01:01| DRB1*04:01:01:02| DRB1*04:01:01:03| DRB1*04:01:02| DRB1*04:01:03| DRB1*04:01:04| DRB1*04:01:05| DRB1*04:01:06| DRB1*04:01:07| DRB1*04:01:08| DRB1*04:01:09| DRB1*04:01:10| DRB1*04:01:11| DRB1*04:01:12| DRB1*04:01:13| DRB1*04:01:14| DRB1*04:01:15| DRB1*04:01:16| DRB1*04:01:17| DRB1*04:01:18| DRB1*04:01:19| DRB1*04:01:20| DRB1*04:01:21| DRB1*04:02:01| DRB1*04:02:02| DRB1*04:02:03| DRB1*04:02:04| DRB1*04:02:05| DRB1*04:02:06| DRB1*04:03:01:01| DRB1*04:03:01:02| DRB1*04:03:02| DRB1*04:03:03| DRB1*04:03:04| DRB1*04:03:05| DRB1*04:03:06| DRB1*04:03:07| DRB1*04:03:08| DRB1*04:03:09| DRB1*04:03:10| DRB1*04:03:11| DRB1*04:03:12| DRB1*04:03:13| DRB1*04:03:14| DRB1*04:03:15| DRB1*04:04:01| DRB1*04:04:02| DRB1*04:04:03| DRB1*04:04:04| DRB1*04:04:05| DRB1*04:04:06| DRB1*04:04:07| DRB1*04:04:08| DRB1*04:04:09| DRB1*04:04:10| DRB1*04:04:11| DRB1*04:04:12| DRB1*04:04:13| DRB1*04:04:14| DRB1*04:04:15| DRB1*04:05:01:01| DRB1*04:05:01:02| DRB1*04:05:01:03| DRB1*04:05:02| DRB1*04:05:03| DRB1*04:05:04| DRB1*04:05:05| DRB1*04:05:06| DRB1*04:05:07| DRB1*04:05:08| DRB1*04:05:09| DRB1*04:05:10| DRB1*04:05:11| DRB1*04:05:13| DRB1*04:05:14| DRB1*04:05:15| DRB1*04:05:16| DRB1*04:05:17| DRB1*04:05:18| DRB1*04:05:19| DRB1*04:05:20| DRB1*04:06:01| DRB1*04:06:02| DRB1*04:06:03| DRB1*04:06:04| DRB1*04:06:05| DRB1*04:06:06| DRB1*04:06:07| DRB1*04:07:01:01| DRB1*04:07:01:02| DRB1*04:07:02| DRB1*04:07:03| DRB1*04:07:04| DRB1*04:07:05| DRB1*04:07:06| DRB1*04:08:01| DRB1*04:08:02| DRB1*04:08:03| DRB1*04:08:04| DRB1*04:09| DRB1*04:10:01| DRB1*04:10:02| DRB1*04:10:03| DRB1*04:11:01| DRB1*04:11:02| DRB1*04:11:03| DRB1*04:11:04| DRB1*04:11:05| DRB1*04:12| DRB1*04:13| DRB1*04:14| DRB1*04:15| DRB1*04:16| DRB1*04:17:01| DRB1*04:17:02| DRB1*04:18| DRB1*04:19| DRB1*04:20| DRB1*04:21| DRB1*04:22| DRB1*04:23| DRB1*04:24| DRB1*04:25| DRB1*04:26| DRB1*04:27| DRB1*04:28| DRB1*04:29| DRB1*04:30| DRB1*04:31| DRB1*04:32| DRB1*04:33| DRB1*04:34| DRB1*04:35| DRB1*04:36| DRB1*04:37| DRB1*04:38| DRB1*04:39| DRB1*04:40| DRB1*04:41| DRB1*04:42| DRB1*04:43| DRB1*04:44:01| DRB1*04:44:02| DRB1*04:45| DRB1*04:46| DRB1*04:47| DRB1*04:48| DRB1*04:49| DRB1*04:50| DRB1*04:51| DRB1*04:52| DRB1*04:53:01| DRB1*04:53:02| DRB1*04:54| DRB1*04:55| DRB1*04:56:01| DRB1*04:56:02| DRB1*04:57| DRB1*04:58| DRB1*04:59| DRB1*04:60| DRB1*04:61| DRB1*04:62| DRB1*04:63| DRB1*04:64| DRB1*04:65| DRB1*04:66| DRB1*04:67| DRB1*04:68| DRB1*04:69| DRB1*04:70| DRB1*04:71| DRB1*04:72:01| DRB1*04:72:02| DRB1*04:73:01| DRB1*04:73:02| DRB1*04:74| DRB1*04:75| DRB1*04:76| DRB1*04:77| DRB1*04:78| DRB1*04:79| DRB1*04:80| DRB1*04:82| DRB1*04:83| DRB1*04:84| DRB1*04:85| DRB1*04:86| DRB1*04:87| DRB1*04:88| DRB1*04:89| DRB1*04:90| DRB1*04:91| DRB1*04:92| DRB1*04:93| DRB1*04:95:01| DRB1*04:95:02| DRB1*04:96| DRB1*04:97| DRB1*04:98:01| DRB1*04:98:02| DRB1*04:99| DRB1*04:100| DRB1*04:101| DRB1*04:102| DRB1*04:103| DRB1*04:104| DRB1*04:105:01| DRB1*04:105:02| DRB1*04:106| DRB1*04:107| DRB1*04:108| DRB1*04:109| DRB1*04:110| DRB1*04:111| DRB1*04:112| DRB1*04:113| DRB1*04:114| DRB1*04:115| DRB1*04:116| DRB1*04:117| DRB1*04:118| DRB1*04:121| DRB1*04:122| DRB1*04:123| DRB1*04:124| DRB1*04:125| DRB1*04:126| DRB1*04:127| DRB1*04:128| DRB1*04:129| DRB1*04:130| DRB1*04:131:01| DRB1*04:131:02| DRB1*04:132| DRB1*04:133| DRB1*04:134| DRB1*04:135| DRB1*04:136| DRB1*04:137| DRB1*04:138| DRB1*04:139| DRB1*04:140| DRB1*04:141| DRB1*04:143| DRB1*04:144| DRB1*04:145| DRB1*04:146| DRB1*04:147| DRB1*04:148| DRB1*04:149| DRB1*04:150| DRB1*04:151| DRB1*04:152| DRB1*04:153| DRB1*04:154| DRB1*04:155| DRB1*04:156| DRB1*04:159| DRB1*04:160| DRB1*04:161| DRB1*04:162| DRB1*04:163| DRB1*04:164| DRB1*04:165| DRB1*04:166| DRB1*04:167| DRB1*04:168| DRB1*04:169| DRB1*04:170| DRB1*04:171| DRB1*04:172| DRB1*04:173| DRB1*04:174| DRB1*04:175| DRB1*04:176| DRB1*04:177| DRB1*04:179| DRB1*04:180| DRB1*04:181| DRB1*04:182| DRB1*04:183| DRB1*04:184| DRB1*04:185| DRB1*04:187| DRB1*04:188| DRB1*04:189| DRB1*04:190| DRB1*04:191| DRB1*04:192| DRB1*04:193| DRB1*04:194| DRB1*04:195| DRB1*04:196| DRB1*04:197| DRB1*04:198| DRB1*04:199| DRB1*04:200| DRB1*04:201| DRB1*04:202| DRB1*04:203| DRB1*04:204| DRB1*04:205| DRB1*04:206| DRB1*04:207| DRB1*04:208| DRB1*04:209| DRB1*04:210| DRB1*04:211| DRB1*04:213| DRB1*04:215| DRB1*04:216| DRB1*04:217| DRB1*04:218| DRB1*04:219| DRB1*04:220| DRB1*04:221| DRB1*04:222| DRB1*04:223| DRB1*04:224| DRB1*04:225| DRB1*04:226:01| DRB1*04:226:02| DRB1*04:227| DRB1*04:228| DRB1*04:229| DRB1*04:230| DRB1*04:231| DRB1*04:232| DRB1*04:233| DRB1*04:234| DRB1*04:235| DRB1*04:236| DRB1*04:237| DRB1*04:238| DRB1*04:239| DRB1*04:240| DRB1*04:241| DRB1*04:242| DRB1*04:243| DRB1*04:244| DRB1*04:245| DRB1*04:246| DRB1*04:248| DRB1*04:249| DRB1*04:250| DRB1*04:251| DRB1*04:252| DRB1*04:253| DRB1*04:254| DRB1*04:255| DRB1*04:256| DRB1*04:257| DRB1*04:258| DRB1*04:259| DRB1*04:260| DRB1*04:261| DRB1*04:262| DRB1*04:263| DRB1*04:265| DRB1*04:268| DRB1*04:269| DRB1*04:270| DRB1*04:271| DRB1*04:272</t>
+  </si>
+  <si>
+    <t>DRB1*13:49| DRB1*13:56| DRB1*13:60| DRB1*14:16| DRB1*14:17| DRB1*14:18| DRB1*14:25| DRB1*14:30| DRB1*14:33| DRB1*14:63| DRB1*14:65| DRB1*14:67| DRB1*14:186| DRB1*13:01:01:01| DRB1*13:01:01:02| DRB1*13:01:02| DRB1*13:01:03| DRB1*13:01:04| DRB1*13:01:05| DRB1*13:01:06| DRB1*13:01:07| DRB1*13:01:08| DRB1*13:01:09| DRB1*13:01:10| DRB1*13:01:11| DRB1*13:01:12| DRB1*13:01:13| DRB1*13:01:14| DRB1*13:01:15| DRB1*13:01:16| DRB1*13:01:17| DRB1*13:01:18| DRB1*13:01:19| DRB1*13:01:20| DRB1*13:01:21| DRB1*13:01:22| DRB1*13:01:23| DRB1*13:01:24| DRB1*13:01:25| DRB1*13:01:26| DRB1*13:02:01:01| DRB1*13:02:01:02| DRB1*13:02:01:03| DRB1*13:02:02| DRB1*13:02:03| DRB1*13:02:04| DRB1*13:02:05| DRB1*13:02:06| DRB1*13:02:07| DRB1*13:02:08| DRB1*13:02:09| DRB1*13:02:10| DRB1*13:02:11| DRB1*13:02:12| DRB1*13:02:13| DRB1*13:02:14| DRB1*13:02:15| DRB1*13:02:16| DRB1*13:02:17| DRB1*13:03:01| DRB1*13:03:02| DRB1*13:03:03| DRB1*13:03:04| DRB1*13:03:05| DRB1*13:03:06| DRB1*13:03:07| DRB1*13:03:08| DRB1*13:03:09| DRB1*13:04| DRB1*13:05:01| DRB1*13:05:02| DRB1*13:05:03| DRB1*13:06| DRB1*13:07:01| DRB1*13:07:02| DRB1*13:08| DRB1*13:09| DRB1*13:10| DRB1*13:11:01| DRB1*13:11:02| DRB1*13:12:01| DRB1*13:12:02| DRB1*13:12:03| DRB1*13:12:04| DRB1*13:13| DRB1*13:14:01| DRB1*13:14:02| DRB1*13:14:03| DRB1*13:15| DRB1*13:16| DRB1*13:17| DRB1*13:18| DRB1*13:19| DRB1*13:20| DRB1*13:21:01| DRB1*13:21:02| DRB1*13:22:01| DRB1*13:22:02| DRB1*13:23:01| DRB1*13:23:02| DRB1*13:27| DRB1*13:28| DRB1*13:29| DRB1*13:30| DRB1*13:31| DRB1*13:32| DRB1*13:33:01| DRB1*13:33:02| DRB1*13:33:03| DRB1*13:34| DRB1*13:35| DRB1*13:36| DRB1*13:37| DRB1*13:38| DRB1*13:39| DRB1*13:40| DRB1*13:41| DRB1*13:42| DRB1*13:43| DRB1*13:44| DRB1*13:45| DRB1*13:47| DRB1*13:48| DRB1*13:51| DRB1*13:52| DRB1*13:53| DRB1*13:55| DRB1*13:57| DRB1*13:58| DRB1*13:59| DRB1*13:61:01| DRB1*13:61:02| DRB1*13:63| DRB1*13:64| DRB1*13:65| DRB1*13:66:01| DRB1*13:66:02| DRB1*13:67| DRB1*13:68| DRB1*13:69| DRB1*13:70| DRB1*13:71| DRB1*13:72| DRB1*13:73| DRB1*13:74| DRB1*13:75| DRB1*13:76| DRB1*13:77| DRB1*13:78| DRB1*13:79| DRB1*13:80| DRB1*13:81| DRB1*13:82| DRB1*13:83| DRB1*13:84| DRB1*13:85| DRB1*13:86| DRB1*13:87| DRB1*13:88| DRB1*13:89:01| DRB1*13:89:02| DRB1*13:90| DRB1*13:91| DRB1*13:92| DRB1*13:93| DRB1*13:94:01| DRB1*13:94:02| DRB1*13:95| DRB1*13:96:01| DRB1*13:96:02| DRB1*13:97:01| DRB1*13:97:02| DRB1*13:98| DRB1*13:99| DRB1*13:100| DRB1*13:101| DRB1*13:102| DRB1*13:103| DRB1*13:104| DRB1*13:105| DRB1*13:106| DRB1*13:107| DRB1*13:108| DRB1*13:109| DRB1*13:110| DRB1*13:111| DRB1*13:112| DRB1*13:114| DRB1*13:115| DRB1*13:116| DRB1*13:117| DRB1*13:118| DRB1*13:119| DRB1*13:120| DRB1*13:121| DRB1*13:122| DRB1*13:123| DRB1*13:124| DRB1*13:125| DRB1*13:126| DRB1*13:127| DRB1*13:128| DRB1*13:129| DRB1*13:130| DRB1*13:131| DRB1*13:132| DRB1*13:133| DRB1*13:134| DRB1*13:135| DRB1*13:136| DRB1*13:138| DRB1*13:139| DRB1*13:140| DRB1*13:141| DRB1*13:143| DRB1*13:144| DRB1*13:145| DRB1*13:146| DRB1*13:147| DRB1*13:148| DRB1*13:149| DRB1*13:150| DRB1*13:151| DRB1*13:152| DRB1*13:153| DRB1*13:154| DRB1*13:155| DRB1*13:156| DRB1*13:157| DRB1*13:158| DRB1*13:159| DRB1*13:160| DRB1*13:161| DRB1*13:162| DRB1*13:163| DRB1*13:164| DRB1*13:165| DRB1*13:166| DRB1*13:167| DRB1*13:168| DRB1*13:169| DRB1*13:170| DRB1*13:171:01| DRB1*13:171:02| DRB1*13:172| DRB1*13:173| DRB1*13:174| DRB1*13:175| DRB1*13:176| DRB1*13:177| DRB1*13:178| DRB1*13:179| DRB1*13:180| DRB1*13:181| DRB1*13:182| DRB1*13:183| DRB1*13:184| DRB1*13:186| DRB1*13:187| DRB1*13:188| DRB1*13:189| DRB1*13:190| DRB1*13:191| DRB1*13:192| DRB1*13:193| DRB1*13:194| DRB1*13:195| DRB1*13:196| DRB1*13:197| DRB1*13:198| DRB1*13:199| DRB1*13:201| DRB1*13:202| DRB1*13:203| DRB1*13:204| DRB1*13:205| DRB1*13:206| DRB1*13:207| DRB1*13:208| DRB1*13:209| DRB1*13:210| DRB1*13:211| DRB1*13:212| DRB1*13:213| DRB1*13:214| DRB1*13:215| DRB1*13:216| DRB1*13:217| DRB1*13:218| DRB1*13:219| DRB1*13:220| DRB1*13:221| DRB1*13:222| DRB1*13:223| DRB1*13:224| DRB1*13:225| DRB1*13:226| DRB1*13:227| DRB1*13:228| DRB1*13:229| DRB1*13:230| DRB1*13:231| DRB1*13:232| DRB1*13:233| DRB1*13:234| DRB1*13:235| DRB1*13:236| DRB1*13:237| DRB1*13:238| DRB1*13:239| DRB1*13:240| DRB1*13:241| DRB1*13:242:01| DRB1*13:242:02| DRB1*13:243| DRB1*13:244| DRB1*13:245| DRB1*13:246| DRB1*13:247| DRB1*13:248| DRB1*13:250| DRB1*13:251| DRB1*13:253| DRB1*13:254| DRB1*13:256| DRB1*13:257| DRB1*13:258| DRB1*13:259| DRB1*13:260| DRB1*13:261| DRB1*13:262| DRB1*13:263| DRB1*13:264| DRB1*13:265| DRB1*13:266| DRB1*13:267| DRB1*13:269| DRB1*13:270| DRB1*13:271| DRB1*13:272| DRB1*13:273| DRB1*13:274| DRB1*13:275| DRB1*13:276| DRB1*14:53| DRB1*11:17| DRB1*13:26:01| DRB1*13:26:02| DRB1*13:54| DRB1*14:01:01| DRB1*14:01:02| DRB1*14:01:03| DRB1*14:01:04| DRB1*14:02:01:01| DRB1*14:02:01:02| DRB1*14:02:02| DRB1*14:02:03| DRB1*14:02:04| DRB1*14:02:05| DRB1*14:02:06| DRB1*14:02:07| DRB1*14:05:01:01| DRB1*14:05:01:02| DRB1*14:05:02| DRB1*14:05:03| DRB1*14:05:04| DRB1*14:06:01| DRB1*14:06:02| DRB1*14:06:03| DRB1*14:06:04| DRB1*14:07:01| DRB1*14:07:02| DRB1*14:08| DRB1*14:09| DRB1*14:10| DRB1*14:11| DRB1*14:12:01| DRB1*14:12:02| DRB1*14:13| DRB1*14:14| DRB1*14:19| DRB1*14:20| DRB1*14:21| DRB1*14:22| DRB1*14:23:01| DRB1*14:23:02| DRB1*14:23:03| DRB1*14:23:04| DRB1*14:24| DRB1*14:26| DRB1*14:27:01| DRB1*14:27:02| DRB1*14:28| DRB1*14:29| DRB1*14:31| DRB1*14:32:01| DRB1*14:32:02| DRB1*14:32:03| DRB1*14:34| DRB1*14:35| DRB1*14:36| DRB1*14:37| DRB1*14:38:01| DRB1*14:38:02| DRB1*14:39| DRB1*14:40| DRB1*14:41| DRB1*14:42| DRB1*14:43| DRB1*14:44:01| DRB1*14:44:02| DRB1*14:44:03| DRB1*14:45| DRB1*14:46| DRB1*14:47| DRB1*14:48| DRB1*14:49| DRB1*14:50| DRB1*14:51| DRB1*14:52| DRB1*14:54:01:01| DRB1*14:54:01:02| DRB1*14:54:01:03| DRB1*14:54:01:04| DRB1*14:54:02| DRB1*14:54:03| DRB1*14:54:04| DRB1*14:54:05| DRB1*14:54:06| DRB1*14:54:07| DRB1*14:55| DRB1*14:56| DRB1*14:57| DRB1*14:58| DRB1*14:59| DRB1*14:60| DRB1*14:61| DRB1*14:62| DRB1*14:64| DRB1*14:68:01| DRB1*14:68:02| DRB1*14:69| DRB1*14:70| DRB1*14:71| DRB1*14:72| DRB1*14:73| DRB1*14:74| DRB1*14:75| DRB1*14:76| DRB1*14:77| DRB1*14:78| DRB1*14:79| DRB1*14:80| DRB1*14:81| DRB1*14:82| DRB1*14:83| DRB1*14:84| DRB1*14:85| DRB1*14:86| DRB1*14:87| DRB1*14:88| DRB1*14:89| DRB1*14:90| DRB1*14:91| DRB1*14:93| DRB1*14:94| DRB1*14:95| DRB1*14:96| DRB1*14:97| DRB1*14:98| DRB1*14:99| DRB1*14:100| DRB1*14:101| DRB1*14:102| DRB1*14:103| DRB1*14:104| DRB1*14:105| DRB1*14:106| DRB1*14:107| DRB1*14:108| DRB1*14:109| DRB1*14:110| DRB1*14:111| DRB1*14:112| DRB1*14:113| DRB1*14:114| DRB1*14:115| DRB1*14:116| DRB1*14:117| DRB1*14:118| DRB1*14:119| DRB1*14:120| DRB1*14:121| DRB1*14:122| DRB1*14:123| DRB1*14:124| DRB1*14:125| DRB1*14:126:01| DRB1*14:126:02| DRB1*14:127:01| DRB1*14:127:02| DRB1*14:128| DRB1*14:129| DRB1*14:130| DRB1*14:131| DRB1*14:132| DRB1*14:133| DRB1*14:134| DRB1*14:135| DRB1*14:136| DRB1*14:138| DRB1*14:139| DRB1*14:140| DRB1*14:141| DRB1*14:142| DRB1*14:143| DRB1*14:144| DRB1*14:145| DRB1*14:146| DRB1*14:147| DRB1*14:148| DRB1*14:149| DRB1*14:150| DRB1*14:151| DRB1*14:153| DRB1*14:154| DRB1*14:155| DRB1*14:156| DRB1*14:157| DRB1*14:158| DRB1*14:159| DRB1*14:160| DRB1*14:161| DRB1*14:162| DRB1*14:163| DRB1*14:164| DRB1*14:165| DRB1*14:167| DRB1*14:168| DRB1*14:169| DRB1*14:170| DRB1*14:171| DRB1*14:172| DRB1*14:173| DRB1*14:174| DRB1*14:175| DRB1*14:176| DRB1*14:177| DRB1*14:178| DRB1*14:179| DRB1*14:180| DRB1*14:181| DRB1*14:182| DRB1*14:183| DRB1*14:184| DRB1*14:185| DRB1*14:187| DRB1*14:189| DRB1*14:190| DRB1*14:191| DRB1*14:192| DRB1*14:193| DRB1*14:194| DRB1*14:196| DRB1*14:198| DRB1*14:199| DRB1*14:200| DRB1*14:201| DRB1*14:202| DRB1*14:203| DRB1*14:204| DRB1*14:205| DRB1*14:206| DRB1*14:207| DRB1*14:03:01| DRB1*14:03:02| DRB1*14:04:01| DRB1*14:04:02| DRB1*14:04:03| DRB1*14:04:04| DRB1*14:04:05| DRB1*14:04:06</t>
+  </si>
+  <si>
+    <t>DRB1*07:01:01:01| DRB1*07:01:01:02| DRB1*07:01:01:03| DRB1*07:01:01:04| DRB1*07:01:02| DRB1*07:01:03| DRB1*07:01:04| DRB1*07:01:05| DRB1*07:01:06| DRB1*07:01:07| DRB1*07:01:08| DRB1*07:01:09| DRB1*07:01:10| DRB1*07:01:11| DRB1*07:01:12| DRB1*07:01:13| DRB1*07:01:14| DRB1*07:01:15| DRB1*07:01:16| DRB1*07:01:17| DRB1*07:01:18| DRB1*07:01:19| DRB1*07:01:20| DRB1*07:01:21| DRB1*07:01:22| DRB1*07:03| DRB1*07:04| DRB1*07:05| DRB1*07:06| DRB1*07:07| DRB1*07:08| DRB1*07:09| DRB1*07:11| DRB1*07:12| DRB1*07:13| DRB1*07:14| DRB1*07:15| DRB1*07:16| DRB1*07:17| DRB1*07:18| DRB1*07:19| DRB1*07:20| DRB1*07:21| DRB1*07:22| DRB1*07:23| DRB1*07:24| DRB1*07:25| DRB1*07:27| DRB1*07:28| DRB1*07:29| DRB1*07:30| DRB1*07:31| DRB1*07:32| DRB1*07:33| DRB1*07:34| DRB1*07:35| DRB1*07:36| DRB1*07:37| DRB1*07:38| DRB1*07:39| DRB1*07:40| DRB1*07:41| DRB1*07:42| DRB1*07:43| DRB1*07:44| DRB1*07:45| DRB1*07:46| DRB1*07:47| DRB1*07:48| DRB1*07:49| DRB1*07:50| DRB1*07:51| DRB1*07:52| DRB1*07:53| DRB1*07:54| DRB1*07:55| DRB1*07:56| DRB1*07:57| DRB1*07:59| DRB1*07:60| DRB1*07:61| DRB1*07:62| DRB1*07:63| DRB1*07:64| DRB1*07:65| DRB1*07:66| DRB1*07:67| DRB1*07:69| DRB1*07:70| DRB1*07:71| DRB1*07:72| DRB1*07:73| DRB1*07:74| DRB1*07:75| DRB1*07:76| DRB1*07:77| DRB1*07:78| DRB1*07:79| DRB1*07:80| DRB1*07:81| DRB1*07:82| DRB1*07:83| DRB1*07:84| DRB1*07:85| DRB1*07:86| DRB1*07:88| DRB1*07:89| DRB1*07:90| DRB1*07:91| DRB1*07:92| DRB1*07:93| DRB1*07:94| DRB1*07:95| DRB1*07:96| DRB1*07:97| DRB1*07:98| DRB1*07:99| DRB1*07:100</t>
+  </si>
+  <si>
+    <t>DRB1*08:01:01| DRB1*08:01:02| DRB1*08:01:04| DRB1*08:01:05| DRB1*08:01:06| DRB1*08:01:07| DRB1*08:02:01:01| DRB1*08:02:01:02| DRB1*08:02:02| DRB1*08:02:03| DRB1*08:02:04| DRB1*08:03:02:01| DRB1*08:03:02:02| DRB1*08:03:03| DRB1*08:03:04| DRB1*08:03:05| DRB1*08:03:06| DRB1*08:03:07| DRB1*08:03:08| DRB1*08:03:09| DRB1*08:04:01| DRB1*08:04:02| DRB1*08:04:03| DRB1*08:04:04| DRB1*08:04:05| DRB1*08:04:06| DRB1*08:04:07| DRB1*08:05| DRB1*08:06| DRB1*08:07| DRB1*08:08| DRB1*08:09| DRB1*08:10| DRB1*08:11| DRB1*08:12| DRB1*08:13| DRB1*08:14| DRB1*08:15| DRB1*08:16| DRB1*08:17| DRB1*08:18| DRB1*08:19| DRB1*08:20| DRB1*08:21| DRB1*08:22| DRB1*08:23| DRB1*08:24:01| DRB1*08:24:02| DRB1*08:25| DRB1*08:26| DRB1*08:27| DRB1*08:28| DRB1*08:29| DRB1*08:30:01| DRB1*08:30:02| DRB1*08:30:03| DRB1*08:32| DRB1*08:33| DRB1*08:34| DRB1*08:35| DRB1*08:36:01| DRB1*08:36:02| DRB1*08:37| DRB1*08:38| DRB1*08:39| DRB1*08:40| DRB1*08:41| DRB1*08:42| DRB1*08:43| DRB1*08:44| DRB1*08:45:01| DRB1*08:45:02| DRB1*08:46| DRB1*08:47| DRB1*08:48| DRB1*08:49| DRB1*08:50| DRB1*08:51| DRB1*08:52| DRB1*08:53| DRB1*08:54| DRB1*08:55| DRB1*08:56| DRB1*08:57| DRB1*08:58| DRB1*08:59| DRB1*08:61| DRB1*08:62| DRB1*08:63| DRB1*08:64| DRB1*08:65| DRB1*08:66| DRB1*08:67| DRB1*08:68:01| DRB1*08:68:02| DRB1*08:69| DRB1*08:70| DRB1*08:71| DRB1*08:72| DRB1*08:73| DRB1*08:74| DRB1*08:75| DRB1*08:76| DRB1*08:77| DRB1*08:79| DRB1*08:80| DRB1*08:81| DRB1*08:82| DRB1*08:83| DRB1*08:84| DRB1*08:85| DRB1*08:86| DRB1*08:87| DRB1*08:88| DRB1*14:15</t>
+  </si>
+  <si>
+    <t>DRB1*09:01:02:01| DRB1*09:01:02:02| DRB1*09:01:03| DRB1*09:01:04| DRB1*09:01:05| DRB1*09:01:06| DRB1*09:01:07| DRB1*09:01:08| DRB1*09:01:09| DRB1*09:01:10| DRB1*09:01:11| DRB1*09:02:01| DRB1*09:02:02| DRB1*09:03| DRB1*09:04| DRB1*09:05| DRB1*09:06| DRB1*09:07| DRB1*09:08| DRB1*09:09| DRB1*09:10| DRB1*09:11| DRB1*09:12| DRB1*09:13| DRB1*09:14| DRB1*09:15| DRB1*09:16| DRB1*09:17| DRB1*09:18| DRB1*09:19| DRB1*09:20| DRB1*09:21| DRB1*09:22| DRB1*09:23| DRB1*09:24| DRB1*09:25| DRB1*09:26| DRB1*09:27| DRB1*09:28| DRB1*09:29| DRB1*09:30| DRB1*09:31| DRB1*09:32| DRB1*09:33| DRB1*09:34| DRB1*09:35| DRB1*09:36| DRB1*09:38| DRB1*09:39| DRB1*09:40</t>
+  </si>
+  <si>
+    <t>DR51</t>
   </si>
   <si>
     <t>DR52</t>
@@ -826,16 +829,16 @@
     <t>DR53</t>
   </si>
   <si>
-    <t>DR51</t>
-  </si>
-  <si>
-    <t>DRB3*01:01| DRB3*01:02| DRB3*01:03| DRB3*01:04| DRB3*01:05| DRB3*01:06| DRB3*01:07| DRB3*01:08| DRB3*01:09| DRB3*01:10| DRB3*01:11| DRB3*01:12| DRB3*01:13| DRB3*01:14| DRB3*01:15| DRB3*01:16| DRB3*01:17| DRB3*01:18| DRB3*01:19| DRB3*01:20| DRB3*01:21| DRB3*01:22| DRB3*01:23| DRB3*01:24| DRB3*01:25| DRB3*01:27| DRB3*01:28| DRB3*01:29| DRB3*01:30| DRB3*01:31| DRB3*01:32| DRB3*01:33| DRB3*01:34| DRB3*01:35| DRB3*01:36| DRB3*01:37| DRB3*01:38| DRB3*01:39| DRB3*01:41| DRB3*01:42| DRB3*01:43| DRB3*01:44| DRB3*01:45| DRB3*01:46| DRB3*01:47| DRB3*02:01| DRB3*02:02| DRB3*02:03| DRB3*02:04| DRB3*02:05| DRB3*02:06| DRB3*02:07| DRB3*02:08| DRB3*02:09| DRB3*02:10| DRB3*02:11| DRB3*02:12| DRB3*02:13| DRB3*02:14| DRB3*02:15| DRB3*02:16| DRB3*02:17| DRB3*02:18| DRB3*02:19| DRB3*02:20| DRB3*02:21| DRB3*02:22| DRB3*02:23| DRB3*02:24| DRB3*02:25| DRB3*02:26| DRB3*02:27| DRB3*02:28| DRB3*02:30| DRB3*02:31| DRB3*02:32| DRB3*02:33| DRB3*02:34| DRB3*02:35| DRB3*02:36| DRB3*02:37| DRB3*02:38| DRB3*02:39| DRB3*02:40| DRB3*02:41| DRB3*02:42| DRB3*02:43| DRB3*02:44| DRB3*02:45| DRB3*02:46| DRB3*02:47| DRB3*02:48| DRB3*02:49| DRB3*02:50| DRB3*02:51| DRB3*02:52| DRB3*02:53| DRB3*02:54| DRB3*02:56| DRB3*02:57| DRB3*02:58| DRB3*02:59| DRB3*02:60| DRB3*02:62| DRB3*02:63| DRB3*02:64| DRB3*02:65| DRB3*02:66| DRB3*02:68| DRB3*03:01| DRB3*03:02| DRB3*03:03| DRB3*03:04| DRB3*03:05| DRB3*03:06| DRB3*03:07| DRB3*03:08| DRB3*03:09| DRB3*03:10| DRB3*03:11| DRB3*03:12| DRB3*03:13| DRB3*03:14| DRB3*03:15</t>
-  </si>
-  <si>
-    <t>DRB4*01:01| DRB4*01:02| DRB4*01:03| DRB4*01:04| DRB4*01:05| DRB4*01:06| DRB4*01:07| DRB4*01:08| DRB4*01:09| DRB4*01:10| DRB4*01:11| DRB4*01:12| DRB4*01:13| DRB4*01:14| DRB4*01:15| DRB4*01:17| DRB4*01:18| DRB4*01:19| DRB4*01:20| DRB4*01:21| DRB4*01:22| DRB4*01:23| DRB4*01:24| DRB4*01:25| DRB4*01:26| DRB4*01:27| DRB4*01:28| DRB4*01:29| DRB4*01:30| DRB4*01:31| DRB4*01:32| DRB4*01:33| DRB4*01:34| DRB4*01:35| DRB4*01:36| DRB4*01:37| DRB4*01:39| DRB4*01:40| DRB4*01:41| DRB4*01:42| DRB4*01:43| DRB4*01:44| DRB4*01:45| DRB4*01:46| DRB4*01:47| DRB4*01:48| DRB4*01:49| DRB4*01:50| DRB4*01:51| DRB4*01:52| DRB4*01:53| DRB4*01:55| DRB4*01:58| DRB4*01:59| DRB4*01:60| DRB4*01:62| DRB4*01:63</t>
-  </si>
-  <si>
-    <t>DRB5*01:01| DRB5*01:02| DRB5*01:03| DRB5*01:04| DRB5*01:05| DRB5*01:06| DRB5*01:07| DRB5*01:09| DRB5*01:11| DRB5*01:12| DRB5*01:13| DRB5*01:14| DRB5*01:15| DRB5*01:16| DRB5*01:17| DRB5*01:18| DRB5*01:19| DRB5*01:20| DRB5*01:21| DRB5*01:22| DRB5*01:23| DRB5*01:24| DRB5*01:25| DRB5*01:26| DRB5*01:28| DRB5*01:29| DRB5*01:30| DRB5*01:31| DRB5*01:32| DRB5*01:33| DRB5*01:34| DRB5*01:35| DRB5*02:02| DRB5*02:03| DRB5*02:04| DRB5*02:05| DRB5*02:06| DRB5*02:07| DRB5*02:08| DRB5*02:09| DRB5*02:10| DRB5*02:11| DRB5*02:12| DRB5*02:13| DRB5*02:14| DRB5*02:15| DRB5*02:16| DRB5*02:17| DRB5*02:18</t>
+    <t>DRB5*01:01:01:01| DRB5*01:01:01:02| DRB5*01:01:02| DRB5*01:01:03| DRB5*01:02| DRB5*01:03| DRB5*01:04| DRB5*01:05| DRB5*01:06| DRB5*01:07| DRB5*01:09| DRB5*01:11| DRB5*01:12| DRB5*01:13| DRB5*01:14| DRB5*01:15| DRB5*01:16| DRB5*01:17| DRB5*01:18| DRB5*01:19| DRB5*01:20| DRB5*01:21| DRB5*01:22| DRB5*01:23| DRB5*01:24| DRB5*01:25| DRB5*01:26| DRB5*01:28| DRB5*01:29| DRB5*01:30| DRB5*01:31| DRB5*01:32| DRB5*01:33| DRB5*01:34| DRB5*01:35| DRB5*01:36| DRB5*01:37| DRB5*01:38| DRB5*01:39| DRB5*01:40| DRB5*01:41| DRB5*01:42| DRB5*01:43| DRB5*01:44| DRB5*01:45| DRB5*01:46| DRB5*01:47| DRB5*01:50| DRB5*01:51| DRB5*02:02:01| DRB5*02:02:02| DRB5*02:02:03| DRB5*02:03| DRB5*02:04| DRB5*02:05| DRB5*02:06| DRB5*02:07| DRB5*02:08| DRB5*02:09| DRB5*02:10| DRB5*02:11| DRB5*02:12| DRB5*02:13| DRB5*02:14| DRB5*02:15| DRB5*02:16| DRB5*02:17| DRB5*02:18| DRB5*02:20| DRB5*02:21| DRB5*02:22| DRB5*02:23| DRB5*02:24</t>
+  </si>
+  <si>
+    <t>DRB3*01:01:02:01| DRB3*01:01:02:02| DRB3*01:01:03| DRB3*01:01:04| DRB3*01:01:05| DRB3*01:01:06| DRB3*01:01:07| DRB3*01:01:08| DRB3*01:02| DRB3*01:03| DRB3*01:04| DRB3*01:05| DRB3*01:06| DRB3*01:07| DRB3*01:08| DRB3*01:09| DRB3*01:10| DRB3*01:11| DRB3*01:12| DRB3*01:13| DRB3*01:14| DRB3*01:15| DRB3*01:16| DRB3*01:17| DRB3*01:18| DRB3*01:19| DRB3*01:20| DRB3*01:21| DRB3*01:22| DRB3*01:23| DRB3*01:24| DRB3*01:25| DRB3*01:27| DRB3*01:28| DRB3*01:29| DRB3*01:30| DRB3*01:31| DRB3*01:32| DRB3*01:33| DRB3*01:34| DRB3*01:35| DRB3*01:36| DRB3*01:37| DRB3*01:38| DRB3*01:39| DRB3*01:41| DRB3*01:42| DRB3*01:43| DRB3*01:44| DRB3*01:45| DRB3*01:46| DRB3*01:47| DRB3*01:48| DRB3*01:49| DRB3*01:50| DRB3*01:51| DRB3*01:52| DRB3*01:53| DRB3*01:54| DRB3*01:55| DRB3*01:56| DRB3*02:01| DRB3*02:02:01:01| DRB3*02:02:01:02| DRB3*02:02:01:03| DRB3*02:02:02| DRB3*02:02:03| DRB3*02:02:04| DRB3*02:02:05| DRB3*02:02:06| DRB3*02:02:07| DRB3*02:02:08| DRB3*02:02:09| DRB3*02:02:10| DRB3*02:02:11| DRB3*02:02:12| DRB3*02:02:13| DRB3*02:02:14| DRB3*02:02:15| DRB3*02:02:16| DRB3*02:03| DRB3*02:04| DRB3*02:05| DRB3*02:06| DRB3*02:07| DRB3*02:08| DRB3*02:09| DRB3*02:10| DRB3*02:11| DRB3*02:12| DRB3*02:13| DRB3*02:14| DRB3*02:15| DRB3*02:16| DRB3*02:17| DRB3*02:18| DRB3*02:19| DRB3*02:20| DRB3*02:21| DRB3*02:22:01| DRB3*02:22:02| DRB3*02:23| DRB3*02:24| DRB3*02:25| DRB3*02:26| DRB3*02:27| DRB3*02:28| DRB3*02:30| DRB3*02:31:01| DRB3*02:31:02| DRB3*02:32| DRB3*02:33| DRB3*02:34| DRB3*02:35| DRB3*02:36| DRB3*02:37| DRB3*02:38| DRB3*02:39| DRB3*02:40| DRB3*02:41| DRB3*02:42| DRB3*02:43| DRB3*02:44| DRB3*02:45| DRB3*02:46| DRB3*02:47| DRB3*02:48| DRB3*02:49| DRB3*02:50| DRB3*02:51| DRB3*02:52| DRB3*02:53| DRB3*02:54| DRB3*02:56| DRB3*02:57| DRB3*02:58| DRB3*02:59| DRB3*02:60| DRB3*02:62| DRB3*02:63| DRB3*02:64| DRB3*02:65| DRB3*02:66| DRB3*02:68| DRB3*02:69| DRB3*02:70| DRB3*02:71| DRB3*02:72| DRB3*02:73| DRB3*02:74| DRB3*02:75| DRB3*02:76| DRB3*02:77| DRB3*02:78| DRB3*02:79| DRB3*02:81| DRB3*02:82| DRB3*02:83| DRB3*02:84| DRB3*02:85| DRB3*02:86| DRB3*02:87| DRB3*03:01:01| DRB3*03:01:02| DRB3*03:01:03| DRB3*03:01:04| DRB3*03:01:05| DRB3*03:01:06| DRB3*03:01:07| DRB3*03:02| DRB3*03:03| DRB3*03:04| DRB3*03:05| DRB3*03:06| DRB3*03:07| DRB3*03:08| DRB3*03:09| DRB3*03:10| DRB3*03:11| DRB3*03:12| DRB3*03:13| DRB3*03:14| DRB3*03:15| DRB3*03:16| DRB3*03:17| DRB3*03:18| DRB3*03:19| DRB3*03:20| DRB3*03:21</t>
+  </si>
+  <si>
+    <t>DRB4*01:01:01:01| DRB4*01:01:02| DRB4*01:02| DRB4*01:03:01:01| DRB4*01:03:01:03| DRB4*01:03:01:04| DRB4*01:03:01:05| DRB4*01:03:01:06| DRB4*01:03:01:07| DRB4*01:03:01:08| DRB4*01:03:02| DRB4*01:03:03| DRB4*01:03:04| DRB4*01:03:05| DRB4*01:03:06| DRB4*01:03:07| DRB4*01:03:08| DRB4*01:03:09| DRB4*01:03:10| DRB4*01:03:11| DRB4*01:04| DRB4*01:05| DRB4*01:06| DRB4*01:07:01| DRB4*01:07:02| DRB4*01:08| DRB4*01:09| DRB4*01:10| DRB4*01:11| DRB4*01:12| DRB4*01:13| DRB4*01:14| DRB4*01:15| DRB4*01:17| DRB4*01:18| DRB4*01:19| DRB4*01:20| DRB4*01:21| DRB4*01:22| DRB4*01:23| DRB4*01:24| DRB4*01:25| DRB4*01:26| DRB4*01:27| DRB4*01:28| DRB4*01:29| DRB4*01:30| DRB4*01:31| DRB4*01:32| DRB4*01:33| DRB4*01:34| DRB4*01:35| DRB4*01:36| DRB4*01:37| DRB4*01:39| DRB4*01:40| DRB4*01:41| DRB4*01:42| DRB4*01:43| DRB4*01:44| DRB4*01:45| DRB4*01:46| DRB4*01:47| DRB4*01:48| DRB4*01:49| DRB4*01:50| DRB4*01:51| DRB4*01:52| DRB4*01:53| DRB4*01:55| DRB4*01:58| DRB4*01:59| DRB4*01:60| DRB4*01:62| DRB4*01:63| DRB4*01:64| DRB4*01:66| DRB4*01:67| DRB4*01:68| DRB4*01:69| DRB4*01:70| DRB4*01:72| DRB4*01:73| DRB4*01:74| DRB4*01:75| DRB4*01:76| DRB4*01:77| DRB4*01:78| DRB4*01:79| DRB4*01:81| DRB4*01:82| DRB4*01:83| DRB4*01:85| DRB4*01:86</t>
+  </si>
+  <si>
+    <t>DQA0</t>
   </si>
   <si>
     <t>DQA01:01</t>
@@ -880,12 +883,27 @@
     <t>DQA01:14</t>
   </si>
   <si>
-    <t>DQA0</t>
+    <t>DQA01:17</t>
+  </si>
+  <si>
+    <t>DQA01:18</t>
+  </si>
+  <si>
+    <t>DQA01:19</t>
+  </si>
+  <si>
+    <t>DQA01:20</t>
+  </si>
+  <si>
+    <t>DQA01:21</t>
   </si>
   <si>
     <t>DQA02:01</t>
   </si>
   <si>
+    <t>DQA02:03</t>
+  </si>
+  <si>
     <t>DQA03:01</t>
   </si>
   <si>
@@ -898,6 +916,9 @@
     <t>DQA03:04</t>
   </si>
   <si>
+    <t>DQA03:05</t>
+  </si>
+  <si>
     <t>DQA04:01</t>
   </si>
   <si>
@@ -907,6 +928,9 @@
     <t>DQA04:04</t>
   </si>
   <si>
+    <t>DQA04:05</t>
+  </si>
+  <si>
     <t>DQA05:01</t>
   </si>
   <si>
@@ -940,25 +964,37 @@
     <t>DQA05:11</t>
   </si>
   <si>
+    <t>DQA05:12</t>
+  </si>
+  <si>
+    <t>DQA05:13</t>
+  </si>
+  <si>
+    <t>DQA05:14</t>
+  </si>
+  <si>
     <t>DQA06:01</t>
   </si>
   <si>
     <t>DQA06:02</t>
   </si>
   <si>
-    <t>DQA1*01:01</t>
-  </si>
-  <si>
-    <t>DQA1*01:02</t>
-  </si>
-  <si>
-    <t>DQA1*01:03</t>
-  </si>
-  <si>
-    <t>DQA1*01:04</t>
-  </si>
-  <si>
-    <t>DQA1*01:05</t>
+    <t>DQA1*01:15N| DQA1*01:16N| DQA1*02:02N| DQA1*04:03N</t>
+  </si>
+  <si>
+    <t>DQA1*01:01:01:01| DQA1*01:01:01:02| DQA1*01:01:01:03| DQA1*01:01:01:05| DQA1*01:01:02| DQA1*01:01:03</t>
+  </si>
+  <si>
+    <t>DQA1*01:02:01:01| DQA1*01:02:01:02| DQA1*01:02:01:03| DQA1*01:02:01:04| DQA1*01:02:01:05| DQA1*01:02:01:06| DQA1*01:02:01:07| DQA1*01:02:01:08| DQA1*01:02:01:09| DQA1*01:02:01:10| DQA1*01:02:02:01| DQA1*01:02:02:02| DQA1*01:02:03| DQA1*01:02:04</t>
+  </si>
+  <si>
+    <t>DQA1*01:03:01:01| DQA1*01:03:01:02| DQA1*01:03:01:03| DQA1*01:03:01:04| DQA1*01:03:01:05| DQA1*01:03:01:06| DQA1*01:03:01:07| DQA1*01:03:01:08</t>
+  </si>
+  <si>
+    <t>DQA1*01:04:01:01| DQA1*01:04:01:02| DQA1*01:04:01:03| DQA1*01:04:01:04| DQA1*01:04:02</t>
+  </si>
+  <si>
+    <t>DQA1*01:05:01| DQA1*01:05:02</t>
   </si>
   <si>
     <t>DQA1*01:06</t>
@@ -988,25 +1024,43 @@
     <t>DQA1*01:14</t>
   </si>
   <si>
-    <t>DQA1*01:15N| DQA1*01:16N| DQA1*04:03N</t>
-  </si>
-  <si>
-    <t>DQA1*02:01</t>
-  </si>
-  <si>
-    <t>DQA1*03:01</t>
-  </si>
-  <si>
-    <t>DQA1*03:02</t>
-  </si>
-  <si>
-    <t>DQA1*03:03</t>
+    <t>DQA1*01:17</t>
+  </si>
+  <si>
+    <t>DQA1*01:18</t>
+  </si>
+  <si>
+    <t>DQA1*01:19</t>
+  </si>
+  <si>
+    <t>DQA1*01:20</t>
+  </si>
+  <si>
+    <t>DQA1*01:21</t>
+  </si>
+  <si>
+    <t>DQA1*02:01:01:01| DQA1*02:01:01:02| DQA1*02:01:02</t>
+  </si>
+  <si>
+    <t>DQA1*02:03</t>
+  </si>
+  <si>
+    <t>DQA1*03:01:01| DQA1*03:01:03</t>
+  </si>
+  <si>
+    <t>DQA1*03:02:01:01| DQA1*03:02:01:02</t>
+  </si>
+  <si>
+    <t>DQA1*03:03:01:01| DQA1*03:03:01:02| DQA1*03:03:01:03| DQA1*03:03:01:04| DQA1*03:03:01:05| DQA1*03:03:02</t>
   </si>
   <si>
     <t>DQA1*03:04</t>
   </si>
   <si>
-    <t>DQA1*04:01</t>
+    <t>DQA1*03:05</t>
+  </si>
+  <si>
+    <t>DQA1*04:01:01:01| DQA1*04:01:01:02| DQA1*04:01:01:03| DQA1*04:01:01:04| DQA1*04:01:02:01| DQA1*04:01:02:02</t>
   </si>
   <si>
     <t>DQA1*04:02</t>
@@ -1015,22 +1069,25 @@
     <t>DQA1*04:04</t>
   </si>
   <si>
-    <t>DQA1*05:01</t>
+    <t>DQA1*04:05</t>
+  </si>
+  <si>
+    <t>DQA1*05:01:01:01| DQA1*05:01:01:02| DQA1*05:01:01:03| DQA1*05:01:02| DQA1*05:01:04</t>
   </si>
   <si>
     <t>DQA1*05:02</t>
   </si>
   <si>
-    <t>DQA1*05:03</t>
+    <t>DQA1*05:03:01:01| DQA1*05:03:01:02</t>
   </si>
   <si>
     <t>DQA1*05:04</t>
   </si>
   <si>
-    <t>DQA1*05:05</t>
-  </si>
-  <si>
-    <t>DQA1*05:06</t>
+    <t>DQA1*05:05:01:01| DQA1*05:05:01:02| DQA1*05:05:01:03| DQA1*05:05:01:04| DQA1*05:05:01:05| DQA1*05:05:01:06| DQA1*05:05:01:07| DQA1*05:05:01:08| DQA1*05:05:01:09| DQA1*05:05:01:10| DQA1*05:05:01:11| DQA1*05:05:01:12| DQA1*05:05:01:13</t>
+  </si>
+  <si>
+    <t>DQA1*05:06:01:01| DQA1*05:06:01:02</t>
   </si>
   <si>
     <t>DQA1*05:07</t>
@@ -1048,16 +1105,40 @@
     <t>DQA1*05:11</t>
   </si>
   <si>
-    <t>DQA1*06:01</t>
+    <t>DQA1*05:12</t>
+  </si>
+  <si>
+    <t>DQA1*05:13</t>
+  </si>
+  <si>
+    <t>DQA1*05:14</t>
+  </si>
+  <si>
+    <t>DQA1*06:01:01:01| DQA1*06:01:01:02| DQA1*06:01:02</t>
   </si>
   <si>
     <t>DQA1*06:02</t>
   </si>
   <si>
+    <t>DQ0</t>
+  </si>
+  <si>
+    <t>DQ1</t>
+  </si>
+  <si>
     <t>DQ2</t>
   </si>
   <si>
-    <t>DQ0</t>
+    <t>DQ3</t>
+  </si>
+  <si>
+    <t>DQ4</t>
+  </si>
+  <si>
+    <t>DQ5</t>
+  </si>
+  <si>
+    <t>DQ6</t>
   </si>
   <si>
     <t>DQ7</t>
@@ -1069,49 +1150,34 @@
     <t>DQ9</t>
   </si>
   <si>
-    <t>DQ3</t>
-  </si>
-  <si>
-    <t>DQ4</t>
-  </si>
-  <si>
-    <t>DQ5</t>
-  </si>
-  <si>
-    <t>DQ6</t>
-  </si>
-  <si>
-    <t>DQ1</t>
-  </si>
-  <si>
-    <t>DQB1*02:01| DQB1*02:02| DQB1*02:03| DQB1*02:04| DQB1*02:05| DQB1*02:06| DQB1*02:07| DQB1*02:08| DQB1*02:09| DQB1*02:10| DQB1*02:11| DQB1*02:12| DQB1*02:13| DQB1*02:14| DQB1*02:15| DQB1*02:16| DQB1*02:17| DQB1*02:19| DQB1*02:21| DQB1*02:22| DQB1*02:23| DQB1*02:24| DQB1*02:25| DQB1*02:26| DQB1*02:27| DQB1*02:28| DQB1*02:29| DQB1*02:30| DQB1*02:31| DQB1*02:32| DQB1*02:33| DQB1*02:34| DQB1*02:35| DQB1*02:36| DQB1*02:37| DQB1*02:38| DQB1*02:39| DQB1*02:40| DQB1*02:41| DQB1*02:42| DQB1*02:43| DQB1*02:44| DQB1*02:45| DQB1*02:46| DQB1*02:47| DQB1*02:48| DQB1*02:49| DQB1*02:50| DQB1*02:51| DQB1*02:52| DQB1*02:53Q| DQB1*02:54| DQB1*02:55| DQB1*02:56| DQB1*02:57| DQB1*02:59| DQB1*02:60| DQB1*02:61| DQB1*02:62| DQB1*02:63| DQB1*02:64| DQB1*02:65| DQB1*02:66| DQB1*02:68| DQB1*02:69| DQB1*02:70| DQB1*02:71| DQB1*02:72| DQB1*02:73| DQB1*02:74| DQB1*02:75| DQB1*02:76| DQB1*02:77| DQB1*02:78| DQB1*02:79| DQB1*02:80| DQB1*02:81| DQB1*02:82| DQB1*02:83| DQB1*02:84| DQB1*02:85| DQB1*02:86| DQB1*02:87| DQB1*02:88| DQB1*02:89| DQB1*02:90| DQB1*02:91| DQB1*02:92| DQB1*02:93| DQB1*02:94| DQB1*02:95| DQB1*02:97| DQB1*02:98| DQB1*02:99| DQB1*02:100| DQB1*02:101| DQB1*02:102| DQB1*02:103| DQB1*02:104</t>
-  </si>
-  <si>
-    <t>DQB1*02:18N| DQB1*02:20N| DQB1*02:58N| DQB1*02:67N| DQB1*02:96N| DQB1*03:66N| DQB1*03:84N| DQB1*03:90N| DQB1*03:95N| DQB1*03:118N| DQB1*03:213N| DQB1*03:237N| DQB1*03:269N| DQB1*04:25N| DQB1*04:36N| DQB1*04:41N| DQB1*05:41N| DQB1*05:90N| DQB1*05:110N| DQB1*05:128N| DQB1*06:26N| DQB1*06:54N| DQB1*06:75N| DQB1*06:77N| DQB1*06:102N| DQB1*06:112N| DQB1*06:144N| DQB1*06:158N| DQB1*06:179N| DQB1*06:193N| DQB1*06:216N</t>
-  </si>
-  <si>
-    <t>DQB1*03:01| DQB1*03:04| DQB1*03:09| DQB1*03:13| DQB1*03:16| DQB1*03:19| DQB1*03:06| DQB1*03:14| DQB1*03:21| DQB1*03:22| DQB1*03:23| DQB1*03:24| DQB1*03:25| DQB1*03:26| DQB1*03:27| DQB1*03:28| DQB1*03:29| DQB1*03:30| DQB1*03:31| DQB1*03:32| DQB1*03:33| DQB1*03:34| DQB1*03:35| DQB1*03:36| DQB1*03:37| DQB1*03:38| DQB1*03:39| DQB1*03:40| DQB1*03:41| DQB1*03:42| DQB1*03:43| DQB1*03:44| DQB1*03:45| DQB1*03:46| DQB1*03:47| DQB1*03:48| DQB1*03:49| DQB1*03:50| DQB1*03:51| DQB1*03:52| DQB1*03:53| DQB1*03:54| DQB1*03:55| DQB1*03:56| DQB1*03:57| DQB1*03:58| DQB1*03:59| DQB1*03:60| DQB1*03:61| DQB1*03:62| DQB1*03:63| DQB1*03:64| DQB1*03:65| DQB1*03:67| DQB1*03:68| DQB1*03:69| DQB1*03:70| DQB1*03:71| DQB1*03:72| DQB1*03:73| DQB1*03:74| DQB1*03:75| DQB1*03:76| DQB1*03:77| DQB1*03:78| DQB1*03:79| DQB1*03:80| DQB1*03:81| DQB1*03:82| DQB1*03:83| DQB1*03:85| DQB1*03:86| DQB1*03:87| DQB1*03:88| DQB1*03:89| DQB1*03:91Q| DQB1*03:92| DQB1*03:93| DQB1*03:94| DQB1*03:96| DQB1*03:97| DQB1*03:98| DQB1*03:99Q| DQB1*03:100| DQB1*03:101| DQB1*03:102| DQB1*03:103| DQB1*03:104| DQB1*03:105| DQB1*03:106| DQB1*03:107| DQB1*03:108| DQB1*03:109| DQB1*03:110| DQB1*03:111| DQB1*03:112| DQB1*03:113| DQB1*03:114| DQB1*03:115| DQB1*03:116| DQB1*03:117| DQB1*03:119| DQB1*03:120| DQB1*03:121| DQB1*03:122| DQB1*03:123| DQB1*03:124| DQB1*03:125| DQB1*03:126| DQB1*03:127| DQB1*03:128| DQB1*03:129| DQB1*03:130| DQB1*03:131| DQB1*03:132| DQB1*03:133| DQB1*03:134| DQB1*03:135| DQB1*03:136| DQB1*03:137| DQB1*03:138| DQB1*03:139| DQB1*03:140| DQB1*03:141| DQB1*03:142| DQB1*03:143| DQB1*03:144| DQB1*03:145| DQB1*03:146| DQB1*03:147| DQB1*03:148| DQB1*03:149| DQB1*03:150| DQB1*03:151| DQB1*03:152| DQB1*03:153| DQB1*03:154| DQB1*03:155| DQB1*03:156| DQB1*03:157| DQB1*03:158| DQB1*03:159| DQB1*03:160| DQB1*03:161| DQB1*03:162| DQB1*03:163| DQB1*03:164| DQB1*03:165| DQB1*03:166| DQB1*03:167| DQB1*03:168| DQB1*03:169| DQB1*03:170| DQB1*03:171| DQB1*03:172| DQB1*03:173| DQB1*03:174| DQB1*03:175| DQB1*03:176| DQB1*03:177| DQB1*03:178| DQB1*03:179| DQB1*03:180| DQB1*03:181| DQB1*03:182| DQB1*03:183| DQB1*03:184| DQB1*03:185| DQB1*03:186| DQB1*03:187| DQB1*03:188| DQB1*03:189| DQB1*03:190| DQB1*03:191| DQB1*03:192| DQB1*03:193| DQB1*03:194| DQB1*03:195| DQB1*03:196| DQB1*03:197Q| DQB1*03:198| DQB1*03:199| DQB1*03:200| DQB1*03:201| DQB1*03:202| DQB1*03:203| DQB1*03:204| DQB1*03:205| DQB1*03:206| DQB1*03:207| DQB1*03:208| DQB1*03:209| DQB1*03:210| DQB1*03:211| DQB1*03:212| DQB1*03:214| DQB1*03:215| DQB1*03:216| DQB1*03:217| DQB1*03:218| DQB1*03:219| DQB1*03:220| DQB1*03:221| DQB1*03:222| DQB1*03:223| DQB1*03:224| DQB1*03:225| DQB1*03:226| DQB1*03:227| DQB1*03:228| DQB1*03:229| DQB1*03:230| DQB1*03:231| DQB1*03:232| DQB1*03:233| DQB1*03:234| DQB1*03:235| DQB1*03:236| DQB1*03:238| DQB1*03:239| DQB1*03:240| DQB1*03:241| DQB1*03:242| DQB1*03:243| DQB1*03:244| DQB1*03:245| DQB1*03:246| DQB1*03:247| DQB1*03:248| DQB1*03:249| DQB1*03:250| DQB1*03:251| DQB1*03:252| DQB1*03:253| DQB1*03:254| DQB1*03:255| DQB1*03:256| DQB1*03:257| DQB1*03:258| DQB1*03:259| DQB1*03:260| DQB1*03:261| DQB1*03:262| DQB1*03:263| DQB1*03:264| DQB1*03:265| DQB1*03:266| DQB1*03:267| DQB1*03:268| DQB1*03:270| DQB1*03:271| DQB1*03:272| DQB1*03:273| DQB1*03:274</t>
-  </si>
-  <si>
-    <t>DQB1*03:02| DQB1*03:05| DQB1*03:07| DQB1*03:08| DQB1*03:10| DQB1*03:11| DQB1*03:18| DQB1*03:06| DQB1*03:14| DQB1*03:21| DQB1*03:22| DQB1*03:23| DQB1*03:24| DQB1*03:25| DQB1*03:26| DQB1*03:27| DQB1*03:28| DQB1*03:29| DQB1*03:30| DQB1*03:31| DQB1*03:32| DQB1*03:33| DQB1*03:34| DQB1*03:35| DQB1*03:36| DQB1*03:37| DQB1*03:38| DQB1*03:39| DQB1*03:40| DQB1*03:41| DQB1*03:42| DQB1*03:43| DQB1*03:44| DQB1*03:45| DQB1*03:46| DQB1*03:47| DQB1*03:48| DQB1*03:49| DQB1*03:50| DQB1*03:51| DQB1*03:52| DQB1*03:53| DQB1*03:54| DQB1*03:55| DQB1*03:56| DQB1*03:57| DQB1*03:58| DQB1*03:59| DQB1*03:60| DQB1*03:61| DQB1*03:62| DQB1*03:63| DQB1*03:64| DQB1*03:65| DQB1*03:67| DQB1*03:68| DQB1*03:69| DQB1*03:70| DQB1*03:71| DQB1*03:72| DQB1*03:73| DQB1*03:74| DQB1*03:75| DQB1*03:76| DQB1*03:77| DQB1*03:78| DQB1*03:79| DQB1*03:80| DQB1*03:81| DQB1*03:82| DQB1*03:83| DQB1*03:85| DQB1*03:86| DQB1*03:87| DQB1*03:88| DQB1*03:89| DQB1*03:91Q| DQB1*03:92| DQB1*03:93| DQB1*03:94| DQB1*03:96| DQB1*03:97| DQB1*03:98| DQB1*03:99Q| DQB1*03:100| DQB1*03:101| DQB1*03:102| DQB1*03:103| DQB1*03:104| DQB1*03:105| DQB1*03:106| DQB1*03:107| DQB1*03:108| DQB1*03:109| DQB1*03:110| DQB1*03:111| DQB1*03:112| DQB1*03:113| DQB1*03:114| DQB1*03:115| DQB1*03:116| DQB1*03:117| DQB1*03:119| DQB1*03:120| DQB1*03:121| DQB1*03:122| DQB1*03:123| DQB1*03:124| DQB1*03:125| DQB1*03:126| DQB1*03:127| DQB1*03:128| DQB1*03:129| DQB1*03:130| DQB1*03:131| DQB1*03:132| DQB1*03:133| DQB1*03:134| DQB1*03:135| DQB1*03:136| DQB1*03:137| DQB1*03:138| DQB1*03:139| DQB1*03:140| DQB1*03:141| DQB1*03:142| DQB1*03:143| DQB1*03:144| DQB1*03:145| DQB1*03:146| DQB1*03:147| DQB1*03:148| DQB1*03:149| DQB1*03:150| DQB1*03:151| DQB1*03:152| DQB1*03:153| DQB1*03:154| DQB1*03:155| DQB1*03:156| DQB1*03:157| DQB1*03:158| DQB1*03:159| DQB1*03:160| DQB1*03:161| DQB1*03:162| DQB1*03:163| DQB1*03:164| DQB1*03:165| DQB1*03:166| DQB1*03:167| DQB1*03:168| DQB1*03:169| DQB1*03:170| DQB1*03:171| DQB1*03:172| DQB1*03:173| DQB1*03:174| DQB1*03:175| DQB1*03:176| DQB1*03:177| DQB1*03:178| DQB1*03:179| DQB1*03:180| DQB1*03:181| DQB1*03:182| DQB1*03:183| DQB1*03:184| DQB1*03:185| DQB1*03:186| DQB1*03:187| DQB1*03:188| DQB1*03:189| DQB1*03:190| DQB1*03:191| DQB1*03:192| DQB1*03:193| DQB1*03:194| DQB1*03:195| DQB1*03:196| DQB1*03:197Q| DQB1*03:198| DQB1*03:199| DQB1*03:200| DQB1*03:201| DQB1*03:202| DQB1*03:203| DQB1*03:204| DQB1*03:205| DQB1*03:206| DQB1*03:207| DQB1*03:208| DQB1*03:209| DQB1*03:210| DQB1*03:211| DQB1*03:212| DQB1*03:214| DQB1*03:215| DQB1*03:216| DQB1*03:217| DQB1*03:218| DQB1*03:219| DQB1*03:220| DQB1*03:221| DQB1*03:222| DQB1*03:223| DQB1*03:224| DQB1*03:225| DQB1*03:226| DQB1*03:227| DQB1*03:228| DQB1*03:229| DQB1*03:230| DQB1*03:231| DQB1*03:232| DQB1*03:233| DQB1*03:234| DQB1*03:235| DQB1*03:236| DQB1*03:238| DQB1*03:239| DQB1*03:240| DQB1*03:241| DQB1*03:242| DQB1*03:243| DQB1*03:244| DQB1*03:245| DQB1*03:246| DQB1*03:247| DQB1*03:248| DQB1*03:249| DQB1*03:250| DQB1*03:251| DQB1*03:252| DQB1*03:253| DQB1*03:254| DQB1*03:255| DQB1*03:256| DQB1*03:257| DQB1*03:258| DQB1*03:259| DQB1*03:260| DQB1*03:261| DQB1*03:262| DQB1*03:263| DQB1*03:264| DQB1*03:265| DQB1*03:266| DQB1*03:267| DQB1*03:268| DQB1*03:270| DQB1*03:271| DQB1*03:272| DQB1*03:273| DQB1*03:274</t>
-  </si>
-  <si>
-    <t>DQB1*03:03| DQB1*03:12| DQB1*03:15| DQB1*03:17| DQB1*03:20| DQB1*03:06| DQB1*03:14| DQB1*03:21| DQB1*03:22| DQB1*03:23| DQB1*03:24| DQB1*03:25| DQB1*03:26| DQB1*03:27| DQB1*03:28| DQB1*03:29| DQB1*03:30| DQB1*03:31| DQB1*03:32| DQB1*03:33| DQB1*03:34| DQB1*03:35| DQB1*03:36| DQB1*03:37| DQB1*03:38| DQB1*03:39| DQB1*03:40| DQB1*03:41| DQB1*03:42| DQB1*03:43| DQB1*03:44| DQB1*03:45| DQB1*03:46| DQB1*03:47| DQB1*03:48| DQB1*03:49| DQB1*03:50| DQB1*03:51| DQB1*03:52| DQB1*03:53| DQB1*03:54| DQB1*03:55| DQB1*03:56| DQB1*03:57| DQB1*03:58| DQB1*03:59| DQB1*03:60| DQB1*03:61| DQB1*03:62| DQB1*03:63| DQB1*03:64| DQB1*03:65| DQB1*03:67| DQB1*03:68| DQB1*03:69| DQB1*03:70| DQB1*03:71| DQB1*03:72| DQB1*03:73| DQB1*03:74| DQB1*03:75| DQB1*03:76| DQB1*03:77| DQB1*03:78| DQB1*03:79| DQB1*03:80| DQB1*03:81| DQB1*03:82| DQB1*03:83| DQB1*03:85| DQB1*03:86| DQB1*03:87| DQB1*03:88| DQB1*03:89| DQB1*03:91Q| DQB1*03:92| DQB1*03:93| DQB1*03:94| DQB1*03:96| DQB1*03:97| DQB1*03:98| DQB1*03:99Q| DQB1*03:100| DQB1*03:101| DQB1*03:102| DQB1*03:103| DQB1*03:104| DQB1*03:105| DQB1*03:106| DQB1*03:107| DQB1*03:108| DQB1*03:109| DQB1*03:110| DQB1*03:111| DQB1*03:112| DQB1*03:113| DQB1*03:114| DQB1*03:115| DQB1*03:116| DQB1*03:117| DQB1*03:119| DQB1*03:120| DQB1*03:121| DQB1*03:122| DQB1*03:123| DQB1*03:124| DQB1*03:125| DQB1*03:126| DQB1*03:127| DQB1*03:128| DQB1*03:129| DQB1*03:130| DQB1*03:131| DQB1*03:132| DQB1*03:133| DQB1*03:134| DQB1*03:135| DQB1*03:136| DQB1*03:137| DQB1*03:138| DQB1*03:139| DQB1*03:140| DQB1*03:141| DQB1*03:142| DQB1*03:143| DQB1*03:144| DQB1*03:145| DQB1*03:146| DQB1*03:147| DQB1*03:148| DQB1*03:149| DQB1*03:150| DQB1*03:151| DQB1*03:152| DQB1*03:153| DQB1*03:154| DQB1*03:155| DQB1*03:156| DQB1*03:157| DQB1*03:158| DQB1*03:159| DQB1*03:160| DQB1*03:161| DQB1*03:162| DQB1*03:163| DQB1*03:164| DQB1*03:165| DQB1*03:166| DQB1*03:167| DQB1*03:168| DQB1*03:169| DQB1*03:170| DQB1*03:171| DQB1*03:172| DQB1*03:173| DQB1*03:174| DQB1*03:175| DQB1*03:176| DQB1*03:177| DQB1*03:178| DQB1*03:179| DQB1*03:180| DQB1*03:181| DQB1*03:182| DQB1*03:183| DQB1*03:184| DQB1*03:185| DQB1*03:186| DQB1*03:187| DQB1*03:188| DQB1*03:189| DQB1*03:190| DQB1*03:191| DQB1*03:192| DQB1*03:193| DQB1*03:194| DQB1*03:195| DQB1*03:196| DQB1*03:197Q| DQB1*03:198| DQB1*03:199| DQB1*03:200| DQB1*03:201| DQB1*03:202| DQB1*03:203| DQB1*03:204| DQB1*03:205| DQB1*03:206| DQB1*03:207| DQB1*03:208| DQB1*03:209| DQB1*03:210| DQB1*03:211| DQB1*03:212| DQB1*03:214| DQB1*03:215| DQB1*03:216| DQB1*03:217| DQB1*03:218| DQB1*03:219| DQB1*03:220| DQB1*03:221| DQB1*03:222| DQB1*03:223| DQB1*03:224| DQB1*03:225| DQB1*03:226| DQB1*03:227| DQB1*03:228| DQB1*03:229| DQB1*03:230| DQB1*03:231| DQB1*03:232| DQB1*03:233| DQB1*03:234| DQB1*03:235| DQB1*03:236| DQB1*03:238| DQB1*03:239| DQB1*03:240| DQB1*03:241| DQB1*03:242| DQB1*03:243| DQB1*03:244| DQB1*03:245| DQB1*03:246| DQB1*03:247| DQB1*03:248| DQB1*03:249| DQB1*03:250| DQB1*03:251| DQB1*03:252| DQB1*03:253| DQB1*03:254| DQB1*03:255| DQB1*03:256| DQB1*03:257| DQB1*03:258| DQB1*03:259| DQB1*03:260| DQB1*03:261| DQB1*03:262| DQB1*03:263| DQB1*03:264| DQB1*03:265| DQB1*03:266| DQB1*03:267| DQB1*03:268| DQB1*03:270| DQB1*03:271| DQB1*03:272| DQB1*03:273| DQB1*03:274</t>
-  </si>
-  <si>
-    <t>DQB1*03:06| DQB1*03:14| DQB1*03:21| DQB1*03:22| DQB1*03:23| DQB1*03:24| DQB1*03:25| DQB1*03:26| DQB1*03:27| DQB1*03:28| DQB1*03:29| DQB1*03:30| DQB1*03:31| DQB1*03:32| DQB1*03:33| DQB1*03:34| DQB1*03:35| DQB1*03:36| DQB1*03:37| DQB1*03:38| DQB1*03:39| DQB1*03:40| DQB1*03:41| DQB1*03:42| DQB1*03:43| DQB1*03:44| DQB1*03:45| DQB1*03:46| DQB1*03:47| DQB1*03:48| DQB1*03:49| DQB1*03:50| DQB1*03:51| DQB1*03:52| DQB1*03:53| DQB1*03:54| DQB1*03:55| DQB1*03:56| DQB1*03:57| DQB1*03:58| DQB1*03:59| DQB1*03:60| DQB1*03:61| DQB1*03:62| DQB1*03:63| DQB1*03:64| DQB1*03:65| DQB1*03:67| DQB1*03:68| DQB1*03:69| DQB1*03:70| DQB1*03:71| DQB1*03:72| DQB1*03:73| DQB1*03:74| DQB1*03:75| DQB1*03:76| DQB1*03:77| DQB1*03:78| DQB1*03:79| DQB1*03:80| DQB1*03:81| DQB1*03:82| DQB1*03:83| DQB1*03:85| DQB1*03:86| DQB1*03:87| DQB1*03:88| DQB1*03:89| DQB1*03:91Q| DQB1*03:92| DQB1*03:93| DQB1*03:94| DQB1*03:96| DQB1*03:97| DQB1*03:98| DQB1*03:99Q| DQB1*03:100| DQB1*03:101| DQB1*03:102| DQB1*03:103| DQB1*03:104| DQB1*03:105| DQB1*03:106| DQB1*03:107| DQB1*03:108| DQB1*03:109| DQB1*03:110| DQB1*03:111| DQB1*03:112| DQB1*03:113| DQB1*03:114| DQB1*03:115| DQB1*03:116| DQB1*03:117| DQB1*03:119| DQB1*03:120| DQB1*03:121| DQB1*03:122| DQB1*03:123| DQB1*03:124| DQB1*03:125| DQB1*03:126| DQB1*03:127| DQB1*03:128| DQB1*03:129| DQB1*03:130| DQB1*03:131| DQB1*03:132| DQB1*03:133| DQB1*03:134| DQB1*03:135| DQB1*03:136| DQB1*03:137| DQB1*03:138| DQB1*03:139| DQB1*03:140| DQB1*03:141| DQB1*03:142| DQB1*03:143| DQB1*03:144| DQB1*03:145| DQB1*03:146| DQB1*03:147| DQB1*03:148| DQB1*03:149| DQB1*03:150| DQB1*03:151| DQB1*03:152| DQB1*03:153| DQB1*03:154| DQB1*03:155| DQB1*03:156| DQB1*03:157| DQB1*03:158| DQB1*03:159| DQB1*03:160| DQB1*03:161| DQB1*03:162| DQB1*03:163| DQB1*03:164| DQB1*03:165| DQB1*03:166| DQB1*03:167| DQB1*03:168| DQB1*03:169| DQB1*03:170| DQB1*03:171| DQB1*03:172| DQB1*03:173| DQB1*03:174| DQB1*03:175| DQB1*03:176| DQB1*03:177| DQB1*03:178| DQB1*03:179| DQB1*03:180| DQB1*03:181| DQB1*03:182| DQB1*03:183| DQB1*03:184| DQB1*03:185| DQB1*03:186| DQB1*03:187| DQB1*03:188| DQB1*03:189| DQB1*03:190| DQB1*03:191| DQB1*03:192| DQB1*03:193| DQB1*03:194| DQB1*03:195| DQB1*03:196| DQB1*03:197Q| DQB1*03:198| DQB1*03:199| DQB1*03:200| DQB1*03:201| DQB1*03:202| DQB1*03:203| DQB1*03:204| DQB1*03:205| DQB1*03:206| DQB1*03:207| DQB1*03:208| DQB1*03:209| DQB1*03:210| DQB1*03:211| DQB1*03:212| DQB1*03:214| DQB1*03:215| DQB1*03:216| DQB1*03:217| DQB1*03:218| DQB1*03:219| DQB1*03:220| DQB1*03:221| DQB1*03:222| DQB1*03:223| DQB1*03:224| DQB1*03:225| DQB1*03:226| DQB1*03:227| DQB1*03:228| DQB1*03:229| DQB1*03:230| DQB1*03:231| DQB1*03:232| DQB1*03:233| DQB1*03:234| DQB1*03:235| DQB1*03:236| DQB1*03:238| DQB1*03:239| DQB1*03:240| DQB1*03:241| DQB1*03:242| DQB1*03:243| DQB1*03:244| DQB1*03:245| DQB1*03:246| DQB1*03:247| DQB1*03:248| DQB1*03:249| DQB1*03:250| DQB1*03:251| DQB1*03:252| DQB1*03:253| DQB1*03:254| DQB1*03:255| DQB1*03:256| DQB1*03:257| DQB1*03:258| DQB1*03:259| DQB1*03:260| DQB1*03:261| DQB1*03:262| DQB1*03:263| DQB1*03:264| DQB1*03:265| DQB1*03:266| DQB1*03:267| DQB1*03:268| DQB1*03:270| DQB1*03:271| DQB1*03:272| DQB1*03:273| DQB1*03:274| DQB1*03:01| DQB1*03:04| DQB1*03:09| DQB1*03:13| DQB1*03:16| DQB1*03:19| DQB1*03:02| DQB1*03:05| DQB1*03:07| DQB1*03:08| DQB1*03:10| DQB1*03:11| DQB1*03:18| DQB1*03:03| DQB1*03:12| DQB1*03:15| DQB1*03:17| DQB1*03:20</t>
-  </si>
-  <si>
-    <t>DQB1*04:01| DQB1*04:02| DQB1*04:03| DQB1*04:04| DQB1*04:05| DQB1*04:06| DQB1*04:07| DQB1*04:08| DQB1*04:09| DQB1*04:10| DQB1*04:11| DQB1*04:12| DQB1*04:13| DQB1*04:14| DQB1*04:15| DQB1*04:16| DQB1*04:17| DQB1*04:18| DQB1*04:19| DQB1*04:20| DQB1*04:21| DQB1*04:22| DQB1*04:23| DQB1*04:24| DQB1*04:26| DQB1*04:27| DQB1*04:28| DQB1*04:29| DQB1*04:30| DQB1*04:31| DQB1*04:32| DQB1*04:33| DQB1*04:34| DQB1*04:35| DQB1*04:37| DQB1*04:38| DQB1*04:39| DQB1*04:40| DQB1*04:42</t>
-  </si>
-  <si>
-    <t>DQB1*05:01| DQB1*05:02| DQB1*05:03| DQB1*05:04| DQB1*05:05| DQB1*05:06| DQB1*05:07| DQB1*05:08| DQB1*05:09| DQB1*05:10| DQB1*05:11| DQB1*05:12| DQB1*05:13| DQB1*05:14| DQB1*05:15| DQB1*05:16| DQB1*05:17| DQB1*05:18| DQB1*05:19| DQB1*05:20| DQB1*05:21| DQB1*05:22| DQB1*05:23| DQB1*05:24| DQB1*05:25| DQB1*05:26| DQB1*05:27| DQB1*05:28| DQB1*05:29| DQB1*05:30| DQB1*05:31| DQB1*05:32| DQB1*05:33| DQB1*05:34| DQB1*05:35| DQB1*05:36| DQB1*05:37| DQB1*05:38| DQB1*05:39| DQB1*05:40| DQB1*05:42| DQB1*05:43| DQB1*05:44| DQB1*05:45| DQB1*05:46| DQB1*05:47| DQB1*05:48| DQB1*05:49| DQB1*05:50| DQB1*05:51| DQB1*05:52| DQB1*05:53| DQB1*05:54| DQB1*05:55| DQB1*05:56| DQB1*05:57| DQB1*05:58| DQB1*05:59| DQB1*05:60| DQB1*05:61| DQB1*05:62| DQB1*05:63| DQB1*05:64| DQB1*05:65| DQB1*05:66| DQB1*05:67| DQB1*05:68| DQB1*05:69| DQB1*05:70| DQB1*05:71| DQB1*05:72| DQB1*05:73| DQB1*05:74| DQB1*05:75| DQB1*05:76| DQB1*05:77| DQB1*05:78| DQB1*05:79| DQB1*05:80| DQB1*05:81| DQB1*05:82| DQB1*05:83| DQB1*05:84| DQB1*05:85| DQB1*05:86| DQB1*05:87Q| DQB1*05:88| DQB1*05:89| DQB1*05:91| DQB1*05:92| DQB1*05:93| DQB1*05:94| DQB1*05:95| DQB1*05:96| DQB1*05:97| DQB1*05:98| DQB1*05:99| DQB1*05:100| DQB1*05:101| DQB1*05:102| DQB1*05:103| DQB1*05:104| DQB1*05:105| DQB1*05:106| DQB1*05:107| DQB1*05:108| DQB1*05:109| DQB1*05:111| DQB1*05:112| DQB1*05:113| DQB1*05:114| DQB1*05:115| DQB1*05:116| DQB1*05:117| DQB1*05:118| DQB1*05:119| DQB1*05:120| DQB1*05:121| DQB1*05:122| DQB1*05:123| DQB1*05:124| DQB1*05:125| DQB1*05:126| DQB1*05:127| DQB1*05:129| DQB1*05:130| DQB1*05:131| DQB1*05:132Q| DQB1*05:133| DQB1*05:134| DQB1*05:135| DQB1*05:136| DQB1*05:137| DQB1*05:138| DQB1*05:139| DQB1*05:140| DQB1*05:141| DQB1*05:142| DQB1*05:143| DQB1*05:144| DQB1*05:145| DQB1*05:146| DQB1*05:147| DQB1*05:148| DQB1*05:149| DQB1*05:150| DQB1*05:151| DQB1*05:152| DQB1*05:153| DQB1*05:154| DQB1*05:155| DQB1*05:156| DQB1*05:157| DQB1*05:158| DQB1*06:06| DQB1*06:10| DQB1*06:11| DQB1*06:12</t>
-  </si>
-  <si>
-    <t>DQB1*06:01| DQB1*06:02| DQB1*06:03| DQB1*06:04| DQB1*06:05| DQB1*06:07| DQB1*06:08| DQB1*06:09| DQB1*06:13| DQB1*06:14| DQB1*06:15| DQB1*06:16| DQB1*06:17| DQB1*06:18| DQB1*06:19| DQB1*06:20| DQB1*06:21| DQB1*06:22| DQB1*06:23| DQB1*06:24| DQB1*06:25| DQB1*06:27| DQB1*06:28| DQB1*06:29| DQB1*06:30| DQB1*06:31| DQB1*06:32| DQB1*06:33| DQB1*06:34| DQB1*06:35| DQB1*06:36| DQB1*06:37| DQB1*06:38| DQB1*06:39| DQB1*06:40| DQB1*06:41| DQB1*06:42| DQB1*06:43| DQB1*06:44| DQB1*06:45| DQB1*06:46| DQB1*06:47| DQB1*06:48| DQB1*06:49| DQB1*06:50| DQB1*06:51| DQB1*06:52| DQB1*06:53| DQB1*06:55| DQB1*06:56| DQB1*06:57| DQB1*06:58| DQB1*06:59| DQB1*06:60| DQB1*06:61| DQB1*06:62| DQB1*06:63| DQB1*06:64| DQB1*06:65| DQB1*06:66| DQB1*06:67| DQB1*06:68| DQB1*06:69| DQB1*06:70| DQB1*06:71| DQB1*06:72| DQB1*06:73| DQB1*06:74| DQB1*06:76| DQB1*06:78| DQB1*06:79| DQB1*06:80| DQB1*06:81| DQB1*06:82| DQB1*06:83| DQB1*06:84| DQB1*06:85| DQB1*06:86| DQB1*06:87| DQB1*06:88| DQB1*06:89| DQB1*06:90| DQB1*06:91| DQB1*06:92| DQB1*06:93| DQB1*06:94| DQB1*06:95| DQB1*06:96| DQB1*06:97| DQB1*06:98| DQB1*06:99| DQB1*06:100| DQB1*06:101| DQB1*06:103| DQB1*06:104| DQB1*06:105| DQB1*06:106| DQB1*06:107| DQB1*06:108| DQB1*06:109| DQB1*06:110| DQB1*06:111| DQB1*06:113| DQB1*06:114| DQB1*06:115| DQB1*06:116| DQB1*06:117| DQB1*06:118| DQB1*06:119| DQB1*06:120| DQB1*06:121| DQB1*06:122| DQB1*06:123| DQB1*06:124| DQB1*06:125| DQB1*06:126| DQB1*06:127| DQB1*06:128| DQB1*06:129| DQB1*06:130| DQB1*06:131| DQB1*06:132| DQB1*06:133| DQB1*06:134| DQB1*06:135| DQB1*06:136| DQB1*06:137| DQB1*06:138| DQB1*06:139| DQB1*06:140| DQB1*06:141| DQB1*06:142| DQB1*06:143| DQB1*06:145| DQB1*06:146| DQB1*06:147| DQB1*06:148| DQB1*06:149| DQB1*06:150| DQB1*06:151| DQB1*06:152| DQB1*06:153| DQB1*06:154| DQB1*06:155| DQB1*06:156| DQB1*06:157| DQB1*06:159| DQB1*06:160| DQB1*06:161| DQB1*06:162| DQB1*06:163| DQB1*06:164| DQB1*06:165| DQB1*06:166| DQB1*06:167| DQB1*06:168| DQB1*06:169| DQB1*06:170| DQB1*06:171| DQB1*06:172| DQB1*06:173| DQB1*06:174| DQB1*06:175| DQB1*06:176| DQB1*06:177| DQB1*06:178| DQB1*06:180| DQB1*06:181| DQB1*06:182| DQB1*06:183| DQB1*06:184| DQB1*06:185| DQB1*06:186| DQB1*06:187| DQB1*06:188| DQB1*06:189| DQB1*06:190| DQB1*06:191| DQB1*06:192| DQB1*06:194| DQB1*06:195| DQB1*06:196| DQB1*06:197| DQB1*06:198| DQB1*06:199| DQB1*06:200| DQB1*06:201| DQB1*06:202| DQB1*06:203| DQB1*06:204| DQB1*06:205| DQB1*06:206| DQB1*06:207| DQB1*06:208| DQB1*06:209| DQB1*06:210| DQB1*06:211| DQB1*06:212| DQB1*06:213| DQB1*06:214| DQB1*06:215| DQB1*06:217| DQB1*06:218| DQB1*06:219| DQB1*06:221| DQB1*06:222| DQB1*06:223| DQB1*06:224| DQB1*06:225| DQB1*06:226| DQB1*06:227| DQB1*06:228| DQB1*06:229| DQB1*06:230| DQB1*06:231| DQB1*06:232| DQB1*06:233| DQB1*06:234| DQB1*06:235| DQB1*06:236| DQB1*06:237| DQB1*06:238| DQB1*06:239| DQB1*06:240| DQB1*06:241| DQB1*06:242| DQB1*06:243| DQB1*06:244| DQB1*06:245| DQB1*06:246| DQB1*06:247| DQB1*06:248| DQB1*06:249| DQB1*06:10| DQB1*06:11| DQB1*06:12</t>
-  </si>
-  <si>
-    <t>DQB1*06:10| DQB1*06:11| DQB1*06:12| DQB1*05:01| DQB1*05:02| DQB1*05:03| DQB1*05:04| DQB1*05:05| DQB1*05:06| DQB1*05:07| DQB1*05:08| DQB1*05:09| DQB1*05:10| DQB1*05:11| DQB1*05:12| DQB1*05:13| DQB1*05:14| DQB1*05:15| DQB1*05:16| DQB1*05:17| DQB1*05:18| DQB1*05:19| DQB1*05:20| DQB1*05:21| DQB1*05:22| DQB1*05:23| DQB1*05:24| DQB1*05:25| DQB1*05:26| DQB1*05:27| DQB1*05:28| DQB1*05:29| DQB1*05:30| DQB1*05:31| DQB1*05:32| DQB1*05:33| DQB1*05:34| DQB1*05:35| DQB1*05:36| DQB1*05:37| DQB1*05:38| DQB1*05:39| DQB1*05:40| DQB1*05:42| DQB1*05:43| DQB1*05:44| DQB1*05:45| DQB1*05:46| DQB1*05:47| DQB1*05:48| DQB1*05:49| DQB1*05:50| DQB1*05:51| DQB1*05:52| DQB1*05:53| DQB1*05:54| DQB1*05:55| DQB1*05:56| DQB1*05:57| DQB1*05:58| DQB1*05:59| DQB1*05:60| DQB1*05:61| DQB1*05:62| DQB1*05:63| DQB1*05:64| DQB1*05:65| DQB1*05:66| DQB1*05:67| DQB1*05:68| DQB1*05:69| DQB1*05:70| DQB1*05:71| DQB1*05:72| DQB1*05:73| DQB1*05:74| DQB1*05:75| DQB1*05:76| DQB1*05:77| DQB1*05:78| DQB1*05:79| DQB1*05:80| DQB1*05:81| DQB1*05:82| DQB1*05:83| DQB1*05:84| DQB1*05:85| DQB1*05:86| DQB1*05:87Q| DQB1*05:88| DQB1*05:89| DQB1*05:91| DQB1*05:92| DQB1*05:93| DQB1*05:94| DQB1*05:95| DQB1*05:96| DQB1*05:97| DQB1*05:98| DQB1*05:99| DQB1*05:100| DQB1*05:101| DQB1*05:102| DQB1*05:103| DQB1*05:104| DQB1*05:105| DQB1*05:106| DQB1*05:107| DQB1*05:108| DQB1*05:109| DQB1*05:111| DQB1*05:112| DQB1*05:113| DQB1*05:114| DQB1*05:115| DQB1*05:116| DQB1*05:117| DQB1*05:118| DQB1*05:119| DQB1*05:120| DQB1*05:121| DQB1*05:122| DQB1*05:123| DQB1*05:124| DQB1*05:125| DQB1*05:126| DQB1*05:127| DQB1*05:129| DQB1*05:130| DQB1*05:131| DQB1*05:132Q| DQB1*05:133| DQB1*05:134| DQB1*05:135| DQB1*05:136| DQB1*05:137| DQB1*05:138| DQB1*05:139| DQB1*05:140| DQB1*05:141| DQB1*05:142| DQB1*05:143| DQB1*05:144| DQB1*05:145| DQB1*05:146| DQB1*05:147| DQB1*05:148| DQB1*05:149| DQB1*05:150| DQB1*05:151| DQB1*05:152| DQB1*05:153| DQB1*05:154| DQB1*05:155| DQB1*05:156| DQB1*05:157| DQB1*05:158| DQB1*06:06| DQB1*06:01| DQB1*06:02| DQB1*06:03| DQB1*06:04| DQB1*06:05| DQB1*06:07| DQB1*06:08| DQB1*06:09| DQB1*06:13| DQB1*06:14| DQB1*06:15| DQB1*06:16| DQB1*06:17| DQB1*06:18| DQB1*06:19| DQB1*06:20| DQB1*06:21| DQB1*06:22| DQB1*06:23| DQB1*06:24| DQB1*06:25| DQB1*06:27| DQB1*06:28| DQB1*06:29| DQB1*06:30| DQB1*06:31| DQB1*06:32| DQB1*06:33| DQB1*06:34| DQB1*06:35| DQB1*06:36| DQB1*06:37| DQB1*06:38| DQB1*06:39| DQB1*06:40| DQB1*06:41| DQB1*06:42| DQB1*06:43| DQB1*06:44| DQB1*06:45| DQB1*06:46| DQB1*06:47| DQB1*06:48| DQB1*06:49| DQB1*06:50| DQB1*06:51| DQB1*06:52| DQB1*06:53| DQB1*06:55| DQB1*06:56| DQB1*06:57| DQB1*06:58| DQB1*06:59| DQB1*06:60| DQB1*06:61| DQB1*06:62| DQB1*06:63| DQB1*06:64| DQB1*06:65| DQB1*06:66| DQB1*06:67| DQB1*06:68| DQB1*06:69| DQB1*06:70| DQB1*06:71| DQB1*06:72| DQB1*06:73| DQB1*06:74| DQB1*06:76| DQB1*06:78| DQB1*06:79| DQB1*06:80| DQB1*06:81| DQB1*06:82| DQB1*06:83| DQB1*06:84| DQB1*06:85| DQB1*06:86| DQB1*06:87| DQB1*06:88| DQB1*06:89| DQB1*06:90| DQB1*06:91| DQB1*06:92| DQB1*06:93| DQB1*06:94| DQB1*06:95| DQB1*06:96| DQB1*06:97| DQB1*06:98| DQB1*06:99| DQB1*06:100| DQB1*06:101| DQB1*06:103| DQB1*06:104| DQB1*06:105| DQB1*06:106| DQB1*06:107| DQB1*06:108| DQB1*06:109| DQB1*06:110| DQB1*06:111| DQB1*06:113| DQB1*06:114| DQB1*06:115| DQB1*06:116| DQB1*06:117| DQB1*06:118| DQB1*06:119| DQB1*06:120| DQB1*06:121| DQB1*06:122| DQB1*06:123| DQB1*06:124| DQB1*06:125| DQB1*06:126| DQB1*06:127| DQB1*06:128| DQB1*06:129| DQB1*06:130| DQB1*06:131| DQB1*06:132| DQB1*06:133| DQB1*06:134| DQB1*06:135| DQB1*06:136| DQB1*06:137| DQB1*06:138| DQB1*06:139| DQB1*06:140| DQB1*06:141| DQB1*06:142| DQB1*06:143| DQB1*06:145| DQB1*06:146| DQB1*06:147| DQB1*06:148| DQB1*06:149| DQB1*06:150| DQB1*06:151| DQB1*06:152| DQB1*06:153| DQB1*06:154| DQB1*06:155| DQB1*06:156| DQB1*06:157| DQB1*06:159| DQB1*06:160| DQB1*06:161| DQB1*06:162| DQB1*06:163| DQB1*06:164| DQB1*06:165| DQB1*06:166| DQB1*06:167| DQB1*06:168| DQB1*06:169| DQB1*06:170| DQB1*06:171| DQB1*06:172| DQB1*06:173| DQB1*06:174| DQB1*06:175| DQB1*06:176| DQB1*06:177| DQB1*06:178| DQB1*06:180| DQB1*06:181| DQB1*06:182| DQB1*06:183| DQB1*06:184| DQB1*06:185| DQB1*06:186| DQB1*06:187| DQB1*06:188| DQB1*06:189| DQB1*06:190| DQB1*06:191| DQB1*06:192| DQB1*06:194| DQB1*06:195| DQB1*06:196| DQB1*06:197| DQB1*06:198| DQB1*06:199| DQB1*06:200| DQB1*06:201| DQB1*06:202| DQB1*06:203| DQB1*06:204| DQB1*06:205| DQB1*06:206| DQB1*06:207| DQB1*06:208| DQB1*06:209| DQB1*06:210| DQB1*06:211| DQB1*06:212| DQB1*06:213| DQB1*06:214| DQB1*06:215| DQB1*06:217| DQB1*06:218| DQB1*06:219| DQB1*06:221| DQB1*06:222| DQB1*06:223| DQB1*06:224| DQB1*06:225| DQB1*06:226| DQB1*06:227| DQB1*06:228| DQB1*06:229| DQB1*06:230| DQB1*06:231| DQB1*06:232| DQB1*06:233| DQB1*06:234| DQB1*06:235| DQB1*06:236| DQB1*06:237| DQB1*06:238| DQB1*06:239| DQB1*06:240| DQB1*06:241| DQB1*06:242| DQB1*06:243| DQB1*06:244| DQB1*06:245| DQB1*06:246| DQB1*06:247| DQB1*06:248| DQB1*06:249</t>
+    <t>DQB1*02:18N| DQB1*02:20N| DQB1*02:58N| DQB1*02:67N| DQB1*02:96N| DQB1*02:129N| DQB1*02:132N| DQB1*02:134N| DQB1*03:66N| DQB1*03:84N| DQB1*03:90N| DQB1*03:95N| DQB1*03:118N| DQB1*03:213N| DQB1*03:237N| DQB1*03:269N| DQB1*03:276N| DQB1*03:282N| DQB1*03:303N| DQB1*03:310N| DQB1*03:334N| DQB1*03:338N| DQB1*03:339N| DQB1*03:340N| DQB1*04:25N| DQB1*04:36N| DQB1*04:41N| DQB1*04:46N| DQB1*04:59N| DQB1*05:41N| DQB1*05:90N| DQB1*05:110N| DQB1*05:128N| DQB1*05:185N| DQB1*06:26N| DQB1*06:54N| DQB1*06:75N| DQB1*06:77N| DQB1*06:102N| DQB1*06:112N| DQB1*06:144N| DQB1*06:158N| DQB1*06:179N| DQB1*06:193N| DQB1*06:216N| DQB1*06:252N</t>
+  </si>
+  <si>
+    <t>DQB1*06:10| DQB1*06:11:01| DQB1*06:11:02| DQB1*06:11:03| DQB1*06:11:04| DQB1*06:12| DQB1*05:01:01:01| DQB1*05:01:01:02| DQB1*05:01:01:03| DQB1*05:01:01:04| DQB1*05:01:01:05| DQB1*05:01:02| DQB1*05:01:03| DQB1*05:01:04| DQB1*05:01:05| DQB1*05:01:06| DQB1*05:01:07| DQB1*05:01:08| DQB1*05:01:09| DQB1*05:01:10| DQB1*05:01:11| DQB1*05:01:12| DQB1*05:01:13| DQB1*05:01:14| DQB1*05:01:15| DQB1*05:01:16| DQB1*05:01:17| DQB1*05:01:18| DQB1*05:01:19| DQB1*05:01:20| DQB1*05:01:21| DQB1*05:01:22| DQB1*05:01:23| DQB1*05:01:24:01| DQB1*05:01:24:02| DQB1*05:01:25| DQB1*05:01:26| DQB1*05:01:27| DQB1*05:01:28| DQB1*05:01:29| DQB1*05:01:30| DQB1*05:01:31| DQB1*05:01:32| DQB1*05:02:01:01| DQB1*05:02:01:02| DQB1*05:02:01:03| DQB1*05:02:01:04| DQB1*05:02:02| DQB1*05:02:03| DQB1*05:02:04| DQB1*05:02:05| DQB1*05:02:06| DQB1*05:02:07| DQB1*05:02:08| DQB1*05:02:09| DQB1*05:02:10| DQB1*05:02:11| DQB1*05:02:12| DQB1*05:02:13| DQB1*05:02:14| DQB1*05:02:15| DQB1*05:02:16| DQB1*05:02:17| DQB1*05:02:18| DQB1*05:02:19| DQB1*05:03:01:01| DQB1*05:03:01:02| DQB1*05:03:01:03| DQB1*05:03:02| DQB1*05:03:03| DQB1*05:03:04| DQB1*05:03:05| DQB1*05:03:06| DQB1*05:03:07| DQB1*05:03:08| DQB1*05:03:09| DQB1*05:03:10| DQB1*05:03:11| DQB1*05:03:12| DQB1*05:03:13| DQB1*05:03:14| DQB1*05:03:15| DQB1*05:03:16| DQB1*05:03:17| DQB1*05:03:18| DQB1*05:03:19| DQB1*05:03:20| DQB1*05:04| DQB1*05:05:01| DQB1*05:05:02| DQB1*05:06:01| DQB1*05:06:02| DQB1*05:07| DQB1*05:08| DQB1*05:09| DQB1*05:10| DQB1*05:11:01| DQB1*05:11:02| DQB1*05:12| DQB1*05:13| DQB1*05:14| DQB1*05:15| DQB1*05:16| DQB1*05:17| DQB1*05:18| DQB1*05:19| DQB1*05:20| DQB1*05:21| DQB1*05:22| DQB1*05:23| DQB1*05:24| DQB1*05:25| DQB1*05:26| DQB1*05:27| DQB1*05:28| DQB1*05:29| DQB1*05:30| DQB1*05:31| DQB1*05:32| DQB1*05:33| DQB1*05:34| DQB1*05:35| DQB1*05:36| DQB1*05:37| DQB1*05:38| DQB1*05:39| DQB1*05:40| DQB1*05:42| DQB1*05:43:01| DQB1*05:43:02| DQB1*05:44| DQB1*05:45| DQB1*05:46| DQB1*05:47| DQB1*05:48| DQB1*05:49| DQB1*05:50| DQB1*05:51| DQB1*05:52| DQB1*05:53| DQB1*05:54| DQB1*05:55| DQB1*05:56| DQB1*05:57| DQB1*05:58| DQB1*05:59| DQB1*05:60| DQB1*05:61| DQB1*05:62| DQB1*05:63| DQB1*05:64| DQB1*05:65| DQB1*05:66:01| DQB1*05:66:02| DQB1*05:67| DQB1*05:68| DQB1*05:69| DQB1*05:70| DQB1*05:71| DQB1*05:72| DQB1*05:73| DQB1*05:74| DQB1*05:75| DQB1*05:76| DQB1*05:77| DQB1*05:78| DQB1*05:79| DQB1*05:80| DQB1*05:81| DQB1*05:82| DQB1*05:83| DQB1*05:84| DQB1*05:85| DQB1*05:86| DQB1*05:87Q| DQB1*05:88| DQB1*05:89:01| DQB1*05:89:02| DQB1*05:91| DQB1*05:92| DQB1*05:93| DQB1*05:94| DQB1*05:95| DQB1*05:96| DQB1*05:97| DQB1*05:98| DQB1*05:99| DQB1*05:100| DQB1*05:101| DQB1*05:102| DQB1*05:103| DQB1*05:104| DQB1*05:105| DQB1*05:106| DQB1*05:107| DQB1*05:108| DQB1*05:109| DQB1*05:111| DQB1*05:112| DQB1*05:113| DQB1*05:114| DQB1*05:115| DQB1*05:116| DQB1*05:117| DQB1*05:118| DQB1*05:119| DQB1*05:120| DQB1*05:121| DQB1*05:122| DQB1*05:123| DQB1*05:124| DQB1*05:125| DQB1*05:126| DQB1*05:127| DQB1*05:129| DQB1*05:130| DQB1*05:131| DQB1*05:132Q| DQB1*05:133| DQB1*05:134| DQB1*05:135| DQB1*05:136| DQB1*05:137| DQB1*05:138| DQB1*05:139| DQB1*05:140| DQB1*05:141| DQB1*05:142| DQB1*05:143| DQB1*05:144| DQB1*05:145| DQB1*05:146| DQB1*05:147| DQB1*05:148| DQB1*05:149| DQB1*05:150| DQB1*05:151| DQB1*05:152| DQB1*05:153| DQB1*05:154| DQB1*05:155| DQB1*05:156| DQB1*05:157| DQB1*05:158| DQB1*05:159| DQB1*05:160| DQB1*05:161| DQB1*05:162| DQB1*05:163| DQB1*05:164| DQB1*05:165| DQB1*05:166| DQB1*05:167| DQB1*05:168| DQB1*05:169| DQB1*05:170| DQB1*05:171| DQB1*05:172| DQB1*05:173| DQB1*05:174| DQB1*05:175| DQB1*05:176| DQB1*05:177| DQB1*05:178| DQB1*05:179| DQB1*05:180| DQB1*05:181| DQB1*05:182| DQB1*05:183| DQB1*05:184| DQB1*05:186| DQB1*05:187| DQB1*05:188| DQB1*05:189| DQB1*05:190| DQB1*05:191| DQB1*05:192| DQB1*05:193| DQB1*05:194| DQB1*05:195| DQB1*05:196| DQB1*05:197| DQB1*05:198| DQB1*05:199| DQB1*06:06| DQB1*06:01:01:01| DQB1*06:01:01:02| DQB1*06:01:02| DQB1*06:01:03| DQB1*06:01:04| DQB1*06:01:05| DQB1*06:01:06| DQB1*06:01:07| DQB1*06:01:08| DQB1*06:01:09| DQB1*06:01:10| DQB1*06:01:11| DQB1*06:01:12| DQB1*06:01:13| DQB1*06:01:14| DQB1*06:01:15| DQB1*06:01:16| DQB1*06:01:17| DQB1*06:01:18| DQB1*06:01:19| DQB1*06:02:01:01| DQB1*06:02:01:02| DQB1*06:02:01:03| DQB1*06:02:01:04| DQB1*06:02:02| DQB1*06:02:03| DQB1*06:02:04| DQB1*06:02:05| DQB1*06:02:06| DQB1*06:02:07| DQB1*06:02:08| DQB1*06:02:09| DQB1*06:02:10| DQB1*06:02:11| DQB1*06:02:12| DQB1*06:02:13| DQB1*06:02:14| DQB1*06:02:15| DQB1*06:02:16| DQB1*06:02:17| DQB1*06:02:18| DQB1*06:02:19| DQB1*06:02:20| DQB1*06:02:21| DQB1*06:02:22| DQB1*06:02:23| DQB1*06:02:24| DQB1*06:02:25| DQB1*06:02:26| DQB1*06:02:27| DQB1*06:02:28| DQB1*06:02:29| DQB1*06:02:30| DQB1*06:02:31| DQB1*06:02:32| DQB1*06:02:33| DQB1*06:02:34| DQB1*06:02:35| DQB1*06:02:36| DQB1*06:02:37| DQB1*06:02:38| DQB1*06:03:01:01| DQB1*06:03:01:02| DQB1*06:03:01:03| DQB1*06:03:02| DQB1*06:03:03| DQB1*06:03:04| DQB1*06:03:05| DQB1*06:03:06| DQB1*06:03:07| DQB1*06:03:08| DQB1*06:03:09| DQB1*06:03:10| DQB1*06:03:11| DQB1*06:03:12| DQB1*06:03:13| DQB1*06:03:14| DQB1*06:03:15| DQB1*06:03:16| DQB1*06:03:17| DQB1*06:03:18| DQB1*06:03:19| DQB1*06:03:20| DQB1*06:03:21| DQB1*06:03:22| DQB1*06:03:23| DQB1*06:03:24| DQB1*06:03:25| DQB1*06:03:26| DQB1*06:03:27| DQB1*06:03:28| DQB1*06:03:29| DQB1*06:03:30| DQB1*06:03:31| DQB1*06:03:32| DQB1*06:03:33| DQB1*06:03:34| DQB1*06:03:35| DQB1*06:04:01| DQB1*06:04:02| DQB1*06:04:03| DQB1*06:04:04| DQB1*06:04:05| DQB1*06:04:06| DQB1*06:04:07| DQB1*06:04:08| DQB1*06:04:09| DQB1*06:04:10| DQB1*06:04:11| DQB1*06:04:12| DQB1*06:05:01| DQB1*06:05:02| DQB1*06:07:01| DQB1*06:07:02| DQB1*06:08:01| DQB1*06:08:02| DQB1*06:08:03| DQB1*06:09:01:01| DQB1*06:09:01:02| DQB1*06:09:02| DQB1*06:09:03| DQB1*06:09:04| DQB1*06:09:05| DQB1*06:09:06| DQB1*06:09:07| DQB1*06:09:08| DQB1*06:09:09| DQB1*06:09:10| DQB1*06:13:01| DQB1*06:13:02| DQB1*06:13:03| DQB1*06:14:01| DQB1*06:14:02| DQB1*06:14:03| DQB1*06:15:01| DQB1*06:15:02| DQB1*06:16| DQB1*06:17| DQB1*06:18:01| DQB1*06:18:02| DQB1*06:19:01| DQB1*06:19:02| DQB1*06:20| DQB1*06:21| DQB1*06:22:01| DQB1*06:22:02| DQB1*06:22:03| DQB1*06:23| DQB1*06:24| DQB1*06:25| DQB1*06:27:01| DQB1*06:27:02| DQB1*06:28| DQB1*06:29| DQB1*06:30| DQB1*06:31| DQB1*06:32:01| DQB1*06:32:02| DQB1*06:33| DQB1*06:34| DQB1*06:35| DQB1*06:36| DQB1*06:37| DQB1*06:38| DQB1*06:39| DQB1*06:40| DQB1*06:41| DQB1*06:42| DQB1*06:43| DQB1*06:44| DQB1*06:45| DQB1*06:46| DQB1*06:47| DQB1*06:48:01| DQB1*06:48:02| DQB1*06:49| DQB1*06:50| DQB1*06:51:01| DQB1*06:51:02| DQB1*06:52| DQB1*06:53:01| DQB1*06:53:02| DQB1*06:55| DQB1*06:56| DQB1*06:57| DQB1*06:58| DQB1*06:59| DQB1*06:60| DQB1*06:61| DQB1*06:62| DQB1*06:63| DQB1*06:64| DQB1*06:65| DQB1*06:66| DQB1*06:67| DQB1*06:68| DQB1*06:69:01| DQB1*06:69:02| DQB1*06:70| DQB1*06:71| DQB1*06:72| DQB1*06:73| DQB1*06:74| DQB1*06:76| DQB1*06:78| DQB1*06:79:01| DQB1*06:79:02| DQB1*06:80| DQB1*06:81| DQB1*06:82| DQB1*06:83| DQB1*06:84| DQB1*06:85| DQB1*06:86| DQB1*06:87| DQB1*06:88| DQB1*06:89| DQB1*06:90| DQB1*06:91| DQB1*06:92| DQB1*06:93| DQB1*06:94| DQB1*06:95| DQB1*06:96:01| DQB1*06:96:02| DQB1*06:97| DQB1*06:98| DQB1*06:99:01| DQB1*06:99:02| DQB1*06:100| DQB1*06:101| DQB1*06:103| DQB1*06:104| DQB1*06:105| DQB1*06:106| DQB1*06:107| DQB1*06:108| DQB1*06:109| DQB1*06:110| DQB1*06:111| DQB1*06:113| DQB1*06:114| DQB1*06:115| DQB1*06:116| DQB1*06:117| DQB1*06:118:01| DQB1*06:118:02| DQB1*06:118:03| DQB1*06:119| DQB1*06:120| DQB1*06:121| DQB1*06:122| DQB1*06:123| DQB1*06:124| DQB1*06:125| DQB1*06:126| DQB1*06:127| DQB1*06:128| DQB1*06:129| DQB1*06:130| DQB1*06:131| DQB1*06:132| DQB1*06:133| DQB1*06:134| DQB1*06:135| DQB1*06:136| DQB1*06:137| DQB1*06:138| DQB1*06:139| DQB1*06:140| DQB1*06:141| DQB1*06:142| DQB1*06:143| DQB1*06:145| DQB1*06:146:01| DQB1*06:146:02| DQB1*06:147| DQB1*06:148| DQB1*06:149| DQB1*06:150| DQB1*06:151| DQB1*06:152| DQB1*06:153:01| DQB1*06:153:02| DQB1*06:154| DQB1*06:155| DQB1*06:156| DQB1*06:157| DQB1*06:159| DQB1*06:160| DQB1*06:161| DQB1*06:162| DQB1*06:163| DQB1*06:164| DQB1*06:165| DQB1*06:166| DQB1*06:167| DQB1*06:168| DQB1*06:169| DQB1*06:170| DQB1*06:171| DQB1*06:172| DQB1*06:173| DQB1*06:174| DQB1*06:175| DQB1*06:176| DQB1*06:177| DQB1*06:178| DQB1*06:180| DQB1*06:181| DQB1*06:182| DQB1*06:183| DQB1*06:184| DQB1*06:185| DQB1*06:186| DQB1*06:187| DQB1*06:188| DQB1*06:189| DQB1*06:190:01| DQB1*06:190:02| DQB1*06:191| DQB1*06:192| DQB1*06:194| DQB1*06:195| DQB1*06:196| DQB1*06:197| DQB1*06:198| DQB1*06:199| DQB1*06:200| DQB1*06:201| DQB1*06:202| DQB1*06:203| DQB1*06:204| DQB1*06:205| DQB1*06:206:01| DQB1*06:206:02| DQB1*06:207| DQB1*06:208| DQB1*06:209| DQB1*06:210| DQB1*06:211| DQB1*06:212| DQB1*06:213| DQB1*06:214| DQB1*06:215| DQB1*06:217| DQB1*06:218| DQB1*06:219| DQB1*06:221| DQB1*06:222| DQB1*06:223| DQB1*06:224| DQB1*06:225| DQB1*06:226| DQB1*06:227| DQB1*06:228| DQB1*06:229| DQB1*06:230| DQB1*06:231| DQB1*06:232| DQB1*06:233| DQB1*06:234| DQB1*06:235| DQB1*06:236| DQB1*06:237| DQB1*06:238| DQB1*06:239| DQB1*06:240| DQB1*06:241| DQB1*06:242| DQB1*06:243| DQB1*06:244| DQB1*06:245| DQB1*06:246| DQB1*06:247| DQB1*06:248| DQB1*06:249| DQB1*06:250| DQB1*06:251| DQB1*06:253| DQB1*06:254| DQB1*06:255| DQB1*06:256| DQB1*06:257| DQB1*06:258| DQB1*06:259| DQB1*06:260| DQB1*06:261| DQB1*06:262| DQB1*06:263| DQB1*06:264| DQB1*06:265| DQB1*06:266| DQB1*06:267| DQB1*06:268| DQB1*06:269| DQB1*06:270| DQB1*06:271| DQB1*06:272| DQB1*06:273| DQB1*06:274| DQB1*06:275| DQB1*06:276| DQB1*06:277| DQB1*06:278| DQB1*06:279| DQB1*06:280| DQB1*06:281| DQB1*06:282| DQB1*06:283| DQB1*06:284| DQB1*06:285| DQB1*06:286| DQB1*06:287| DQB1*06:288| DQB1*06:289| DQB1*06:290| DQB1*06:291| DQB1*06:292| DQB1*06:293| DQB1*06:294| DQB1*06:295| DQB1*06:296| DQB1*06:297| DQB1*06:298| DQB1*06:299| DQB1*06:300| DQB1*06:301| DQB1*06:302</t>
+  </si>
+  <si>
+    <t>DQB1*02:01:01| DQB1*02:01:02| DQB1*02:01:03| DQB1*02:01:04| DQB1*02:01:05| DQB1*02:01:06| DQB1*02:01:07| DQB1*02:01:08| DQB1*02:01:09| DQB1*02:01:10| DQB1*02:01:11| DQB1*02:01:12| DQB1*02:01:13| DQB1*02:01:14| DQB1*02:01:15| DQB1*02:01:16| DQB1*02:01:17| DQB1*02:01:18| DQB1*02:01:19| DQB1*02:01:20| DQB1*02:01:21| DQB1*02:01:22| DQB1*02:01:23| DQB1*02:01:24| DQB1*02:01:25| DQB1*02:01:26| DQB1*02:01:27| DQB1*02:01:28| DQB1*02:01:29| DQB1*02:01:30| DQB1*02:01:31| DQB1*02:02:01:01| DQB1*02:02:01:02| DQB1*02:02:01:03| DQB1*02:02:01:04| DQB1*02:02:02| DQB1*02:02:03| DQB1*02:02:04| DQB1*02:02:05| DQB1*02:02:06| DQB1*02:02:07| DQB1*02:02:08| DQB1*02:02:09| DQB1*02:03:01| DQB1*02:03:02| DQB1*02:04| DQB1*02:05| DQB1*02:06| DQB1*02:07:01| DQB1*02:07:02| DQB1*02:08| DQB1*02:09| DQB1*02:10| DQB1*02:11| DQB1*02:12| DQB1*02:13| DQB1*02:14:01| DQB1*02:14:02| DQB1*02:15| DQB1*02:16| DQB1*02:17| DQB1*02:19| DQB1*02:21| DQB1*02:22| DQB1*02:23| DQB1*02:24| DQB1*02:25| DQB1*02:26| DQB1*02:27| DQB1*02:28| DQB1*02:29| DQB1*02:30| DQB1*02:31| DQB1*02:32| DQB1*02:33| DQB1*02:34| DQB1*02:35| DQB1*02:36| DQB1*02:37| DQB1*02:38| DQB1*02:39| DQB1*02:40| DQB1*02:41| DQB1*02:42| DQB1*02:43| DQB1*02:44| DQB1*02:45| DQB1*02:46| DQB1*02:47| DQB1*02:48| DQB1*02:49| DQB1*02:50| DQB1*02:51| DQB1*02:52| DQB1*02:53Q| DQB1*02:54| DQB1*02:55| DQB1*02:56| DQB1*02:57| DQB1*02:59| DQB1*02:60| DQB1*02:61| DQB1*02:62| DQB1*02:63| DQB1*02:64| DQB1*02:65| DQB1*02:66| DQB1*02:68| DQB1*02:69| DQB1*02:70| DQB1*02:71| DQB1*02:72| DQB1*02:73| DQB1*02:74| DQB1*02:75| DQB1*02:76| DQB1*02:77| DQB1*02:78| DQB1*02:79| DQB1*02:80| DQB1*02:81| DQB1*02:82| DQB1*02:83| DQB1*02:84| DQB1*02:85| DQB1*02:86| DQB1*02:87| DQB1*02:88| DQB1*02:89:01| DQB1*02:89:02| DQB1*02:90| DQB1*02:91| DQB1*02:92| DQB1*02:93| DQB1*02:94| DQB1*02:95| DQB1*02:97| DQB1*02:98| DQB1*02:99| DQB1*02:100| DQB1*02:101| DQB1*02:102| DQB1*02:103| DQB1*02:104| DQB1*02:105| DQB1*02:106| DQB1*02:107| DQB1*02:108| DQB1*02:109| DQB1*02:110| DQB1*02:111| DQB1*02:112| DQB1*02:113| DQB1*02:114| DQB1*02:115| DQB1*02:116| DQB1*02:117| DQB1*02:118| DQB1*02:119| DQB1*02:120| DQB1*02:121| DQB1*02:122| DQB1*02:123| DQB1*02:124| DQB1*02:125| DQB1*02:126| DQB1*02:127| DQB1*02:128| DQB1*02:130| DQB1*02:131| DQB1*02:133| DQB1*02:135| DQB1*02:136| DQB1*02:137| DQB1*02:138| DQB1*02:139| DQB1*02:140</t>
+  </si>
+  <si>
+    <t>DQB1*03:06| DQB1*03:14:01| DQB1*03:14:02| DQB1*03:21| DQB1*03:22| DQB1*03:23:01| DQB1*03:23:02| DQB1*03:23:03| DQB1*03:24| DQB1*03:25:01| DQB1*03:25:02| DQB1*03:26| DQB1*03:27| DQB1*03:28| DQB1*03:29| DQB1*03:30| DQB1*03:31| DQB1*03:32| DQB1*03:33| DQB1*03:34| DQB1*03:35| DQB1*03:36| DQB1*03:37| DQB1*03:38| DQB1*03:39| DQB1*03:40| DQB1*03:41| DQB1*03:42| DQB1*03:43| DQB1*03:44| DQB1*03:45| DQB1*03:46| DQB1*03:47| DQB1*03:48| DQB1*03:49| DQB1*03:50| DQB1*03:51| DQB1*03:52| DQB1*03:53| DQB1*03:54| DQB1*03:55| DQB1*03:56| DQB1*03:57| DQB1*03:58| DQB1*03:59| DQB1*03:60| DQB1*03:61| DQB1*03:62| DQB1*03:63| DQB1*03:64| DQB1*03:65| DQB1*03:67| DQB1*03:68| DQB1*03:69| DQB1*03:70| DQB1*03:71| DQB1*03:72| DQB1*03:73| DQB1*03:74| DQB1*03:75| DQB1*03:76| DQB1*03:77| DQB1*03:78| DQB1*03:79| DQB1*03:80| DQB1*03:81| DQB1*03:82| DQB1*03:83| DQB1*03:85| DQB1*03:86| DQB1*03:87| DQB1*03:88| DQB1*03:89| DQB1*03:91Q| DQB1*03:92| DQB1*03:93| DQB1*03:94| DQB1*03:96| DQB1*03:97| DQB1*03:98| DQB1*03:99Q| DQB1*03:100| DQB1*03:101| DQB1*03:102| DQB1*03:103| DQB1*03:104| DQB1*03:105| DQB1*03:106| DQB1*03:107| DQB1*03:108| DQB1*03:109| DQB1*03:110| DQB1*03:111| DQB1*03:112| DQB1*03:113| DQB1*03:114| DQB1*03:115| DQB1*03:116| DQB1*03:117| DQB1*03:119| DQB1*03:120| DQB1*03:121| DQB1*03:122| DQB1*03:123| DQB1*03:124| DQB1*03:125| DQB1*03:126| DQB1*03:127| DQB1*03:128| DQB1*03:129| DQB1*03:130| DQB1*03:131| DQB1*03:132| DQB1*03:133| DQB1*03:134| DQB1*03:135| DQB1*03:136| DQB1*03:137| DQB1*03:138| DQB1*03:139| DQB1*03:140| DQB1*03:141| DQB1*03:142| DQB1*03:143| DQB1*03:144| DQB1*03:145| DQB1*03:146| DQB1*03:147| DQB1*03:148| DQB1*03:149| DQB1*03:150| DQB1*03:151| DQB1*03:152| DQB1*03:153| DQB1*03:154| DQB1*03:155| DQB1*03:156| DQB1*03:157| DQB1*03:158| DQB1*03:159| DQB1*03:160| DQB1*03:161| DQB1*03:162| DQB1*03:163| DQB1*03:164| DQB1*03:165| DQB1*03:166| DQB1*03:167| DQB1*03:168| DQB1*03:169| DQB1*03:170| DQB1*03:171| DQB1*03:172| DQB1*03:173| DQB1*03:174| DQB1*03:175| DQB1*03:176| DQB1*03:177| DQB1*03:178| DQB1*03:179| DQB1*03:180| DQB1*03:181| DQB1*03:182| DQB1*03:183| DQB1*03:184| DQB1*03:185| DQB1*03:186| DQB1*03:187| DQB1*03:188| DQB1*03:189| DQB1*03:190| DQB1*03:191| DQB1*03:192| DQB1*03:193| DQB1*03:194| DQB1*03:195| DQB1*03:196| DQB1*03:197Q| DQB1*03:198:01| DQB1*03:198:02| DQB1*03:199| DQB1*03:200| DQB1*03:201| DQB1*03:202| DQB1*03:203| DQB1*03:204| DQB1*03:205| DQB1*03:206| DQB1*03:207| DQB1*03:208| DQB1*03:209| DQB1*03:210| DQB1*03:211| DQB1*03:212| DQB1*03:214| DQB1*03:215| DQB1*03:216| DQB1*03:217| DQB1*03:218| DQB1*03:219| DQB1*03:220| DQB1*03:221| DQB1*03:222| DQB1*03:223| DQB1*03:224| DQB1*03:225| DQB1*03:226| DQB1*03:227| DQB1*03:228| DQB1*03:229| DQB1*03:230| DQB1*03:231| DQB1*03:232| DQB1*03:233| DQB1*03:234| DQB1*03:235| DQB1*03:236| DQB1*03:238| DQB1*03:239| DQB1*03:240| DQB1*03:241| DQB1*03:242| DQB1*03:243| DQB1*03:244| DQB1*03:245| DQB1*03:246| DQB1*03:247| DQB1*03:248| DQB1*03:249| DQB1*03:250| DQB1*03:251| DQB1*03:252| DQB1*03:253| DQB1*03:254| DQB1*03:255| DQB1*03:256| DQB1*03:257| DQB1*03:258| DQB1*03:259| DQB1*03:260| DQB1*03:261| DQB1*03:262| DQB1*03:263| DQB1*03:264| DQB1*03:265| DQB1*03:266| DQB1*03:267| DQB1*03:268| DQB1*03:270| DQB1*03:271| DQB1*03:272| DQB1*03:273| DQB1*03:274| DQB1*03:275| DQB1*03:277| DQB1*03:278| DQB1*03:279| DQB1*03:280| DQB1*03:281| DQB1*03:283| DQB1*03:284| DQB1*03:285| DQB1*03:286| DQB1*03:287| DQB1*03:288| DQB1*03:289| DQB1*03:290| DQB1*03:291| DQB1*03:292| DQB1*03:293| DQB1*03:294| DQB1*03:295| DQB1*03:296| DQB1*03:297| DQB1*03:298| DQB1*03:299| DQB1*03:300| DQB1*03:301| DQB1*03:302| DQB1*03:304| DQB1*03:305| DQB1*03:306| DQB1*03:307| DQB1*03:308| DQB1*03:309| DQB1*03:311| DQB1*03:312| DQB1*03:313| DQB1*03:314| DQB1*03:315| DQB1*03:316| DQB1*03:317:01| DQB1*03:317:02| DQB1*03:318| DQB1*03:319| DQB1*03:320| DQB1*03:321| DQB1*03:322| DQB1*03:323| DQB1*03:324| DQB1*03:326| DQB1*03:327| DQB1*03:328| DQB1*03:329| DQB1*03:330| DQB1*03:331| DQB1*03:332| DQB1*03:333| DQB1*03:335| DQB1*03:336| DQB1*03:337| DQB1*03:341| DQB1*03:342| DQB1*03:343| DQB1*03:344| DQB1*03:345| DQB1*03:346| DQB1*03:347| DQB1*03:348| DQB1*03:349| DQB1*03:350| DQB1*03:351| DQB1*03:352| DQB1*03:353| DQB1*03:01:01:01| DQB1*03:01:01:02| DQB1*03:01:01:03| DQB1*03:01:01:04| DQB1*03:01:01:05| DQB1*03:01:01:06| DQB1*03:01:01:07| DQB1*03:01:01:08| DQB1*03:01:01:09| DQB1*03:01:01:10| DQB1*03:01:01:11| DQB1*03:01:01:12| DQB1*03:01:01:14| DQB1*03:01:01:15| DQB1*03:01:01:16| DQB1*03:01:01:17| DQB1*03:01:01:18| DQB1*03:01:01:19| DQB1*03:01:01:20| DQB1*03:01:02| DQB1*03:01:03| DQB1*03:01:04| DQB1*03:01:05| DQB1*03:01:06| DQB1*03:01:07| DQB1*03:01:08| DQB1*03:01:09| DQB1*03:01:10| DQB1*03:01:11| DQB1*03:01:12| DQB1*03:01:13| DQB1*03:01:14| DQB1*03:01:15| DQB1*03:01:16| DQB1*03:01:17| DQB1*03:01:18| DQB1*03:01:19| DQB1*03:01:20| DQB1*03:01:21| DQB1*03:01:22| DQB1*03:01:23| DQB1*03:01:24| DQB1*03:01:25| DQB1*03:01:26| DQB1*03:01:27| DQB1*03:01:28| DQB1*03:01:29| DQB1*03:01:30| DQB1*03:01:31| DQB1*03:01:32| DQB1*03:01:33| DQB1*03:01:34| DQB1*03:01:35| DQB1*03:01:36| DQB1*03:01:37| DQB1*03:01:38| DQB1*03:01:39| DQB1*03:01:40| DQB1*03:01:41| DQB1*03:01:42| DQB1*03:01:43| DQB1*03:01:44| DQB1*03:01:45| DQB1*03:01:46| DQB1*03:04:01| DQB1*03:04:02| DQB1*03:04:03| DQB1*03:04:04| DQB1*03:09| DQB1*03:13| DQB1*03:16| DQB1*03:19:01| DQB1*03:19:02| DQB1*03:19:03| DQB1*03:19:04| DQB1*03:02:01:01| DQB1*03:02:01:02| DQB1*03:02:01:03| DQB1*03:02:01:04| DQB1*03:02:01:05| DQB1*03:02:01:06| DQB1*03:02:02| DQB1*03:02:03| DQB1*03:02:04| DQB1*03:02:05| DQB1*03:02:06| DQB1*03:02:07| DQB1*03:02:08| DQB1*03:02:09| DQB1*03:02:10| DQB1*03:02:11| DQB1*03:02:12| DQB1*03:02:13| DQB1*03:02:14| DQB1*03:02:15| DQB1*03:02:16| DQB1*03:02:17| DQB1*03:02:18| DQB1*03:02:19| DQB1*03:02:20| DQB1*03:02:21| DQB1*03:02:22| DQB1*03:02:23| DQB1*03:02:24| DQB1*03:02:25| DQB1*03:02:26| DQB1*03:02:27| DQB1*03:02:28| DQB1*03:02:29| DQB1*03:02:30| DQB1*03:05:01| DQB1*03:05:02| DQB1*03:05:03| DQB1*03:05:04| DQB1*03:07| DQB1*03:08| DQB1*03:10:01| DQB1*03:10:02:01| DQB1*03:10:02:02| DQB1*03:11| DQB1*03:18| DQB1*03:03:02:01| DQB1*03:03:02:02| DQB1*03:03:02:03| DQB1*03:03:02:04| DQB1*03:03:02:05| DQB1*03:03:03| DQB1*03:03:04| DQB1*03:03:05| DQB1*03:03:06| DQB1*03:03:07| DQB1*03:03:08| DQB1*03:03:09| DQB1*03:03:10| DQB1*03:03:11| DQB1*03:03:12| DQB1*03:03:13| DQB1*03:03:14| DQB1*03:03:15| DQB1*03:03:16| DQB1*03:03:17| DQB1*03:03:18| DQB1*03:03:19| DQB1*03:03:20| DQB1*03:03:21| DQB1*03:12| DQB1*03:15| DQB1*03:17:01| DQB1*03:17:02| DQB1*03:20</t>
+  </si>
+  <si>
+    <t>DQB1*04:01:01:01| DQB1*04:01:01:02| DQB1*04:01:02| DQB1*04:01:03| DQB1*04:01:04| DQB1*04:01:05| DQB1*04:02:01:01| DQB1*04:02:01:04| DQB1*04:02:01:05| DQB1*04:02:01:06| DQB1*04:02:01:07| DQB1*04:02:01:08| DQB1*04:02:01:09| DQB1*04:02:01:10| DQB1*04:02:02| DQB1*04:02:03| DQB1*04:02:04| DQB1*04:02:05| DQB1*04:02:06| DQB1*04:02:07| DQB1*04:02:08| DQB1*04:02:09| DQB1*04:02:10| DQB1*04:02:11| DQB1*04:02:12| DQB1*04:02:13| DQB1*04:02:14| DQB1*04:02:15| DQB1*04:02:16| DQB1*04:02:17| DQB1*04:02:18| DQB1*04:03:01| DQB1*04:03:02| DQB1*04:03:03| DQB1*04:04| DQB1*04:05| DQB1*04:06| DQB1*04:07| DQB1*04:08| DQB1*04:09| DQB1*04:10| DQB1*04:11| DQB1*04:12| DQB1*04:13| DQB1*04:14| DQB1*04:15| DQB1*04:16| DQB1*04:17| DQB1*04:18| DQB1*04:19| DQB1*04:20| DQB1*04:21| DQB1*04:22| DQB1*04:23| DQB1*04:24| DQB1*04:26| DQB1*04:27| DQB1*04:28| DQB1*04:29| DQB1*04:30| DQB1*04:31| DQB1*04:32| DQB1*04:33| DQB1*04:34| DQB1*04:35| DQB1*04:37| DQB1*04:38| DQB1*04:39| DQB1*04:40| DQB1*04:42| DQB1*04:43| DQB1*04:44| DQB1*04:45| DQB1*04:47| DQB1*04:48| DQB1*04:49| DQB1*04:50| DQB1*04:51| DQB1*04:52| DQB1*04:53| DQB1*04:54| DQB1*04:55| DQB1*04:56| DQB1*04:57| DQB1*04:58| DQB1*04:60| DQB1*04:61</t>
+  </si>
+  <si>
+    <t>DQB1*05:01:01:01| DQB1*05:01:01:02| DQB1*05:01:01:03| DQB1*05:01:01:04| DQB1*05:01:01:05| DQB1*05:01:02| DQB1*05:01:03| DQB1*05:01:04| DQB1*05:01:05| DQB1*05:01:06| DQB1*05:01:07| DQB1*05:01:08| DQB1*05:01:09| DQB1*05:01:10| DQB1*05:01:11| DQB1*05:01:12| DQB1*05:01:13| DQB1*05:01:14| DQB1*05:01:15| DQB1*05:01:16| DQB1*05:01:17| DQB1*05:01:18| DQB1*05:01:19| DQB1*05:01:20| DQB1*05:01:21| DQB1*05:01:22| DQB1*05:01:23| DQB1*05:01:24:01| DQB1*05:01:24:02| DQB1*05:01:25| DQB1*05:01:26| DQB1*05:01:27| DQB1*05:01:28| DQB1*05:01:29| DQB1*05:01:30| DQB1*05:01:31| DQB1*05:01:32| DQB1*05:02:01:01| DQB1*05:02:01:02| DQB1*05:02:01:03| DQB1*05:02:01:04| DQB1*05:02:02| DQB1*05:02:03| DQB1*05:02:04| DQB1*05:02:05| DQB1*05:02:06| DQB1*05:02:07| DQB1*05:02:08| DQB1*05:02:09| DQB1*05:02:10| DQB1*05:02:11| DQB1*05:02:12| DQB1*05:02:13| DQB1*05:02:14| DQB1*05:02:15| DQB1*05:02:16| DQB1*05:02:17| DQB1*05:02:18| DQB1*05:02:19| DQB1*05:03:01:01| DQB1*05:03:01:02| DQB1*05:03:01:03| DQB1*05:03:02| DQB1*05:03:03| DQB1*05:03:04| DQB1*05:03:05| DQB1*05:03:06| DQB1*05:03:07| DQB1*05:03:08| DQB1*05:03:09| DQB1*05:03:10| DQB1*05:03:11| DQB1*05:03:12| DQB1*05:03:13| DQB1*05:03:14| DQB1*05:03:15| DQB1*05:03:16| DQB1*05:03:17| DQB1*05:03:18| DQB1*05:03:19| DQB1*05:03:20| DQB1*05:04| DQB1*05:05:01| DQB1*05:05:02| DQB1*05:06:01| DQB1*05:06:02| DQB1*05:07| DQB1*05:08| DQB1*05:09| DQB1*05:10| DQB1*05:11:01| DQB1*05:11:02| DQB1*05:12| DQB1*05:13| DQB1*05:14| DQB1*05:15| DQB1*05:16| DQB1*05:17| DQB1*05:18| DQB1*05:19| DQB1*05:20| DQB1*05:21| DQB1*05:22| DQB1*05:23| DQB1*05:24| DQB1*05:25| DQB1*05:26| DQB1*05:27| DQB1*05:28| DQB1*05:29| DQB1*05:30| DQB1*05:31| DQB1*05:32| DQB1*05:33| DQB1*05:34| DQB1*05:35| DQB1*05:36| DQB1*05:37| DQB1*05:38| DQB1*05:39| DQB1*05:40| DQB1*05:42| DQB1*05:43:01| DQB1*05:43:02| DQB1*05:44| DQB1*05:45| DQB1*05:46| DQB1*05:47| DQB1*05:48| DQB1*05:49| DQB1*05:50| DQB1*05:51| DQB1*05:52| DQB1*05:53| DQB1*05:54| DQB1*05:55| DQB1*05:56| DQB1*05:57| DQB1*05:58| DQB1*05:59| DQB1*05:60| DQB1*05:61| DQB1*05:62| DQB1*05:63| DQB1*05:64| DQB1*05:65| DQB1*05:66:01| DQB1*05:66:02| DQB1*05:67| DQB1*05:68| DQB1*05:69| DQB1*05:70| DQB1*05:71| DQB1*05:72| DQB1*05:73| DQB1*05:74| DQB1*05:75| DQB1*05:76| DQB1*05:77| DQB1*05:78| DQB1*05:79| DQB1*05:80| DQB1*05:81| DQB1*05:82| DQB1*05:83| DQB1*05:84| DQB1*05:85| DQB1*05:86| DQB1*05:87Q| DQB1*05:88| DQB1*05:89:01| DQB1*05:89:02| DQB1*05:91| DQB1*05:92| DQB1*05:93| DQB1*05:94| DQB1*05:95| DQB1*05:96| DQB1*05:97| DQB1*05:98| DQB1*05:99| DQB1*05:100| DQB1*05:101| DQB1*05:102| DQB1*05:103| DQB1*05:104| DQB1*05:105| DQB1*05:106| DQB1*05:107| DQB1*05:108| DQB1*05:109| DQB1*05:111| DQB1*05:112| DQB1*05:113| DQB1*05:114| DQB1*05:115| DQB1*05:116| DQB1*05:117| DQB1*05:118| DQB1*05:119| DQB1*05:120| DQB1*05:121| DQB1*05:122| DQB1*05:123| DQB1*05:124| DQB1*05:125| DQB1*05:126| DQB1*05:127| DQB1*05:129| DQB1*05:130| DQB1*05:131| DQB1*05:132Q| DQB1*05:133| DQB1*05:134| DQB1*05:135| DQB1*05:136| DQB1*05:137| DQB1*05:138| DQB1*05:139| DQB1*05:140| DQB1*05:141| DQB1*05:142| DQB1*05:143| DQB1*05:144| DQB1*05:145| DQB1*05:146| DQB1*05:147| DQB1*05:148| DQB1*05:149| DQB1*05:150| DQB1*05:151| DQB1*05:152| DQB1*05:153| DQB1*05:154| DQB1*05:155| DQB1*05:156| DQB1*05:157| DQB1*05:158| DQB1*05:159| DQB1*05:160| DQB1*05:161| DQB1*05:162| DQB1*05:163| DQB1*05:164| DQB1*05:165| DQB1*05:166| DQB1*05:167| DQB1*05:168| DQB1*05:169| DQB1*05:170| DQB1*05:171| DQB1*05:172| DQB1*05:173| DQB1*05:174| DQB1*05:175| DQB1*05:176| DQB1*05:177| DQB1*05:178| DQB1*05:179| DQB1*05:180| DQB1*05:181| DQB1*05:182| DQB1*05:183| DQB1*05:184| DQB1*05:186| DQB1*05:187| DQB1*05:188| DQB1*05:189| DQB1*05:190| DQB1*05:191| DQB1*05:192| DQB1*05:193| DQB1*05:194| DQB1*05:195| DQB1*05:196| DQB1*05:197| DQB1*05:198| DQB1*05:199| DQB1*06:06| DQB1*06:10| DQB1*06:11:01| DQB1*06:11:02| DQB1*06:11:03| DQB1*06:11:04| DQB1*06:12</t>
+  </si>
+  <si>
+    <t>DQB1*06:01:01:01| DQB1*06:01:01:02| DQB1*06:01:02| DQB1*06:01:03| DQB1*06:01:04| DQB1*06:01:05| DQB1*06:01:06| DQB1*06:01:07| DQB1*06:01:08| DQB1*06:01:09| DQB1*06:01:10| DQB1*06:01:11| DQB1*06:01:12| DQB1*06:01:13| DQB1*06:01:14| DQB1*06:01:15| DQB1*06:01:16| DQB1*06:01:17| DQB1*06:01:18| DQB1*06:01:19| DQB1*06:02:01:01| DQB1*06:02:01:02| DQB1*06:02:01:03| DQB1*06:02:01:04| DQB1*06:02:02| DQB1*06:02:03| DQB1*06:02:04| DQB1*06:02:05| DQB1*06:02:06| DQB1*06:02:07| DQB1*06:02:08| DQB1*06:02:09| DQB1*06:02:10| DQB1*06:02:11| DQB1*06:02:12| DQB1*06:02:13| DQB1*06:02:14| DQB1*06:02:15| DQB1*06:02:16| DQB1*06:02:17| DQB1*06:02:18| DQB1*06:02:19| DQB1*06:02:20| DQB1*06:02:21| DQB1*06:02:22| DQB1*06:02:23| DQB1*06:02:24| DQB1*06:02:25| DQB1*06:02:26| DQB1*06:02:27| DQB1*06:02:28| DQB1*06:02:29| DQB1*06:02:30| DQB1*06:02:31| DQB1*06:02:32| DQB1*06:02:33| DQB1*06:02:34| DQB1*06:02:35| DQB1*06:02:36| DQB1*06:02:37| DQB1*06:02:38| DQB1*06:03:01:01| DQB1*06:03:01:02| DQB1*06:03:01:03| DQB1*06:03:02| DQB1*06:03:03| DQB1*06:03:04| DQB1*06:03:05| DQB1*06:03:06| DQB1*06:03:07| DQB1*06:03:08| DQB1*06:03:09| DQB1*06:03:10| DQB1*06:03:11| DQB1*06:03:12| DQB1*06:03:13| DQB1*06:03:14| DQB1*06:03:15| DQB1*06:03:16| DQB1*06:03:17| DQB1*06:03:18| DQB1*06:03:19| DQB1*06:03:20| DQB1*06:03:21| DQB1*06:03:22| DQB1*06:03:23| DQB1*06:03:24| DQB1*06:03:25| DQB1*06:03:26| DQB1*06:03:27| DQB1*06:03:28| DQB1*06:03:29| DQB1*06:03:30| DQB1*06:03:31| DQB1*06:03:32| DQB1*06:03:33| DQB1*06:03:34| DQB1*06:03:35| DQB1*06:04:01| DQB1*06:04:02| DQB1*06:04:03| DQB1*06:04:04| DQB1*06:04:05| DQB1*06:04:06| DQB1*06:04:07| DQB1*06:04:08| DQB1*06:04:09| DQB1*06:04:10| DQB1*06:04:11| DQB1*06:04:12| DQB1*06:05:01| DQB1*06:05:02| DQB1*06:07:01| DQB1*06:07:02| DQB1*06:08:01| DQB1*06:08:02| DQB1*06:08:03| DQB1*06:09:01:01| DQB1*06:09:01:02| DQB1*06:09:02| DQB1*06:09:03| DQB1*06:09:04| DQB1*06:09:05| DQB1*06:09:06| DQB1*06:09:07| DQB1*06:09:08| DQB1*06:09:09| DQB1*06:09:10| DQB1*06:13:01| DQB1*06:13:02| DQB1*06:13:03| DQB1*06:14:01| DQB1*06:14:02| DQB1*06:14:03| DQB1*06:15:01| DQB1*06:15:02| DQB1*06:16| DQB1*06:17| DQB1*06:18:01| DQB1*06:18:02| DQB1*06:19:01| DQB1*06:19:02| DQB1*06:20| DQB1*06:21| DQB1*06:22:01| DQB1*06:22:02| DQB1*06:22:03| DQB1*06:23| DQB1*06:24| DQB1*06:25| DQB1*06:27:01| DQB1*06:27:02| DQB1*06:28| DQB1*06:29| DQB1*06:30| DQB1*06:31| DQB1*06:32:01| DQB1*06:32:02| DQB1*06:33| DQB1*06:34| DQB1*06:35| DQB1*06:36| DQB1*06:37| DQB1*06:38| DQB1*06:39| DQB1*06:40| DQB1*06:41| DQB1*06:42| DQB1*06:43| DQB1*06:44| DQB1*06:45| DQB1*06:46| DQB1*06:47| DQB1*06:48:01| DQB1*06:48:02| DQB1*06:49| DQB1*06:50| DQB1*06:51:01| DQB1*06:51:02| DQB1*06:52| DQB1*06:53:01| DQB1*06:53:02| DQB1*06:55| DQB1*06:56| DQB1*06:57| DQB1*06:58| DQB1*06:59| DQB1*06:60| DQB1*06:61| DQB1*06:62| DQB1*06:63| DQB1*06:64| DQB1*06:65| DQB1*06:66| DQB1*06:67| DQB1*06:68| DQB1*06:69:01| DQB1*06:69:02| DQB1*06:70| DQB1*06:71| DQB1*06:72| DQB1*06:73| DQB1*06:74| DQB1*06:76| DQB1*06:78| DQB1*06:79:01| DQB1*06:79:02| DQB1*06:80| DQB1*06:81| DQB1*06:82| DQB1*06:83| DQB1*06:84| DQB1*06:85| DQB1*06:86| DQB1*06:87| DQB1*06:88| DQB1*06:89| DQB1*06:90| DQB1*06:91| DQB1*06:92| DQB1*06:93| DQB1*06:94| DQB1*06:95| DQB1*06:96:01| DQB1*06:96:02| DQB1*06:97| DQB1*06:98| DQB1*06:99:01| DQB1*06:99:02| DQB1*06:100| DQB1*06:101| DQB1*06:103| DQB1*06:104| DQB1*06:105| DQB1*06:106| DQB1*06:107| DQB1*06:108| DQB1*06:109| DQB1*06:110| DQB1*06:111| DQB1*06:113| DQB1*06:114| DQB1*06:115| DQB1*06:116| DQB1*06:117| DQB1*06:118:01| DQB1*06:118:02| DQB1*06:118:03| DQB1*06:119| DQB1*06:120| DQB1*06:121| DQB1*06:122| DQB1*06:123| DQB1*06:124| DQB1*06:125| DQB1*06:126| DQB1*06:127| DQB1*06:128| DQB1*06:129| DQB1*06:130| DQB1*06:131| DQB1*06:132| DQB1*06:133| DQB1*06:134| DQB1*06:135| DQB1*06:136| DQB1*06:137| DQB1*06:138| DQB1*06:139| DQB1*06:140| DQB1*06:141| DQB1*06:142| DQB1*06:143| DQB1*06:145| DQB1*06:146:01| DQB1*06:146:02| DQB1*06:147| DQB1*06:148| DQB1*06:149| DQB1*06:150| DQB1*06:151| DQB1*06:152| DQB1*06:153:01| DQB1*06:153:02| DQB1*06:154| DQB1*06:155| DQB1*06:156| DQB1*06:157| DQB1*06:159| DQB1*06:160| DQB1*06:161| DQB1*06:162| DQB1*06:163| DQB1*06:164| DQB1*06:165| DQB1*06:166| DQB1*06:167| DQB1*06:168| DQB1*06:169| DQB1*06:170| DQB1*06:171| DQB1*06:172| DQB1*06:173| DQB1*06:174| DQB1*06:175| DQB1*06:176| DQB1*06:177| DQB1*06:178| DQB1*06:180| DQB1*06:181| DQB1*06:182| DQB1*06:183| DQB1*06:184| DQB1*06:185| DQB1*06:186| DQB1*06:187| DQB1*06:188| DQB1*06:189| DQB1*06:190:01| DQB1*06:190:02| DQB1*06:191| DQB1*06:192| DQB1*06:194| DQB1*06:195| DQB1*06:196| DQB1*06:197| DQB1*06:198| DQB1*06:199| DQB1*06:200| DQB1*06:201| DQB1*06:202| DQB1*06:203| DQB1*06:204| DQB1*06:205| DQB1*06:206:01| DQB1*06:206:02| DQB1*06:207| DQB1*06:208| DQB1*06:209| DQB1*06:210| DQB1*06:211| DQB1*06:212| DQB1*06:213| DQB1*06:214| DQB1*06:215| DQB1*06:217| DQB1*06:218| DQB1*06:219| DQB1*06:221| DQB1*06:222| DQB1*06:223| DQB1*06:224| DQB1*06:225| DQB1*06:226| DQB1*06:227| DQB1*06:228| DQB1*06:229| DQB1*06:230| DQB1*06:231| DQB1*06:232| DQB1*06:233| DQB1*06:234| DQB1*06:235| DQB1*06:236| DQB1*06:237| DQB1*06:238| DQB1*06:239| DQB1*06:240| DQB1*06:241| DQB1*06:242| DQB1*06:243| DQB1*06:244| DQB1*06:245| DQB1*06:246| DQB1*06:247| DQB1*06:248| DQB1*06:249| DQB1*06:250| DQB1*06:251| DQB1*06:253| DQB1*06:254| DQB1*06:255| DQB1*06:256| DQB1*06:257| DQB1*06:258| DQB1*06:259| DQB1*06:260| DQB1*06:261| DQB1*06:262| DQB1*06:263| DQB1*06:264| DQB1*06:265| DQB1*06:266| DQB1*06:267| DQB1*06:268| DQB1*06:269| DQB1*06:270| DQB1*06:271| DQB1*06:272| DQB1*06:273| DQB1*06:274| DQB1*06:275| DQB1*06:276| DQB1*06:277| DQB1*06:278| DQB1*06:279| DQB1*06:280| DQB1*06:281| DQB1*06:282| DQB1*06:283| DQB1*06:284| DQB1*06:285| DQB1*06:286| DQB1*06:287| DQB1*06:288| DQB1*06:289| DQB1*06:290| DQB1*06:291| DQB1*06:292| DQB1*06:293| DQB1*06:294| DQB1*06:295| DQB1*06:296| DQB1*06:297| DQB1*06:298| DQB1*06:299| DQB1*06:300| DQB1*06:301| DQB1*06:302| DQB1*06:10| DQB1*06:11:01| DQB1*06:11:02| DQB1*06:11:03| DQB1*06:11:04| DQB1*06:12</t>
+  </si>
+  <si>
+    <t>DQB1*03:01:01:01| DQB1*03:01:01:02| DQB1*03:01:01:03| DQB1*03:01:01:04| DQB1*03:01:01:05| DQB1*03:01:01:06| DQB1*03:01:01:07| DQB1*03:01:01:08| DQB1*03:01:01:09| DQB1*03:01:01:10| DQB1*03:01:01:11| DQB1*03:01:01:12| DQB1*03:01:01:14| DQB1*03:01:01:15| DQB1*03:01:01:16| DQB1*03:01:01:17| DQB1*03:01:01:18| DQB1*03:01:01:19| DQB1*03:01:01:20| DQB1*03:01:02| DQB1*03:01:03| DQB1*03:01:04| DQB1*03:01:05| DQB1*03:01:06| DQB1*03:01:07| DQB1*03:01:08| DQB1*03:01:09| DQB1*03:01:10| DQB1*03:01:11| DQB1*03:01:12| DQB1*03:01:13| DQB1*03:01:14| DQB1*03:01:15| DQB1*03:01:16| DQB1*03:01:17| DQB1*03:01:18| DQB1*03:01:19| DQB1*03:01:20| DQB1*03:01:21| DQB1*03:01:22| DQB1*03:01:23| DQB1*03:01:24| DQB1*03:01:25| DQB1*03:01:26| DQB1*03:01:27| DQB1*03:01:28| DQB1*03:01:29| DQB1*03:01:30| DQB1*03:01:31| DQB1*03:01:32| DQB1*03:01:33| DQB1*03:01:34| DQB1*03:01:35| DQB1*03:01:36| DQB1*03:01:37| DQB1*03:01:38| DQB1*03:01:39| DQB1*03:01:40| DQB1*03:01:41| DQB1*03:01:42| DQB1*03:01:43| DQB1*03:01:44| DQB1*03:01:45| DQB1*03:01:46| DQB1*03:04:01| DQB1*03:04:02| DQB1*03:04:03| DQB1*03:04:04| DQB1*03:09| DQB1*03:13| DQB1*03:16| DQB1*03:19:01| DQB1*03:19:02| DQB1*03:19:03| DQB1*03:19:04| DQB1*03:06| DQB1*03:14:01| DQB1*03:14:02| DQB1*03:21| DQB1*03:22| DQB1*03:23:01| DQB1*03:23:02| DQB1*03:23:03| DQB1*03:24| DQB1*03:25:01| DQB1*03:25:02| DQB1*03:26| DQB1*03:27| DQB1*03:28| DQB1*03:29| DQB1*03:30| DQB1*03:31| DQB1*03:32| DQB1*03:33| DQB1*03:34| DQB1*03:35| DQB1*03:36| DQB1*03:37| DQB1*03:38| DQB1*03:39| DQB1*03:40| DQB1*03:41| DQB1*03:42| DQB1*03:43| DQB1*03:44| DQB1*03:45| DQB1*03:46| DQB1*03:47| DQB1*03:48| DQB1*03:49| DQB1*03:50| DQB1*03:51| DQB1*03:52| DQB1*03:53| DQB1*03:54| DQB1*03:55| DQB1*03:56| DQB1*03:57| DQB1*03:58| DQB1*03:59| DQB1*03:60| DQB1*03:61| DQB1*03:62| DQB1*03:63| DQB1*03:64| DQB1*03:65| DQB1*03:67| DQB1*03:68| DQB1*03:69| DQB1*03:70| DQB1*03:71| DQB1*03:72| DQB1*03:73| DQB1*03:74| DQB1*03:75| DQB1*03:76| DQB1*03:77| DQB1*03:78| DQB1*03:79| DQB1*03:80| DQB1*03:81| DQB1*03:82| DQB1*03:83| DQB1*03:85| DQB1*03:86| DQB1*03:87| DQB1*03:88| DQB1*03:89| DQB1*03:91Q| DQB1*03:92| DQB1*03:93| DQB1*03:94| DQB1*03:96| DQB1*03:97| DQB1*03:98| DQB1*03:99Q| DQB1*03:100| DQB1*03:101| DQB1*03:102| DQB1*03:103| DQB1*03:104| DQB1*03:105| DQB1*03:106| DQB1*03:107| DQB1*03:108| DQB1*03:109| DQB1*03:110| DQB1*03:111| DQB1*03:112| DQB1*03:113| DQB1*03:114| DQB1*03:115| DQB1*03:116| DQB1*03:117| DQB1*03:119| DQB1*03:120| DQB1*03:121| DQB1*03:122| DQB1*03:123| DQB1*03:124| DQB1*03:125| DQB1*03:126| DQB1*03:127| DQB1*03:128| DQB1*03:129| DQB1*03:130| DQB1*03:131| DQB1*03:132| DQB1*03:133| DQB1*03:134| DQB1*03:135| DQB1*03:136| DQB1*03:137| DQB1*03:138| DQB1*03:139| DQB1*03:140| DQB1*03:141| DQB1*03:142| DQB1*03:143| DQB1*03:144| DQB1*03:145| DQB1*03:146| DQB1*03:147| DQB1*03:148| DQB1*03:149| DQB1*03:150| DQB1*03:151| DQB1*03:152| DQB1*03:153| DQB1*03:154| DQB1*03:155| DQB1*03:156| DQB1*03:157| DQB1*03:158| DQB1*03:159| DQB1*03:160| DQB1*03:161| DQB1*03:162| DQB1*03:163| DQB1*03:164| DQB1*03:165| DQB1*03:166| DQB1*03:167| DQB1*03:168| DQB1*03:169| DQB1*03:170| DQB1*03:171| DQB1*03:172| DQB1*03:173| DQB1*03:174| DQB1*03:175| DQB1*03:176| DQB1*03:177| DQB1*03:178| DQB1*03:179| DQB1*03:180| DQB1*03:181| DQB1*03:182| DQB1*03:183| DQB1*03:184| DQB1*03:185| DQB1*03:186| DQB1*03:187| DQB1*03:188| DQB1*03:189| DQB1*03:190| DQB1*03:191| DQB1*03:192| DQB1*03:193| DQB1*03:194| DQB1*03:195| DQB1*03:196| DQB1*03:197Q| DQB1*03:198:01| DQB1*03:198:02| DQB1*03:199| DQB1*03:200| DQB1*03:201| DQB1*03:202| DQB1*03:203| DQB1*03:204| DQB1*03:205| DQB1*03:206| DQB1*03:207| DQB1*03:208| DQB1*03:209| DQB1*03:210| DQB1*03:211| DQB1*03:212| DQB1*03:214| DQB1*03:215| DQB1*03:216| DQB1*03:217| DQB1*03:218| DQB1*03:219| DQB1*03:220| DQB1*03:221| DQB1*03:222| DQB1*03:223| DQB1*03:224| DQB1*03:225| DQB1*03:226| DQB1*03:227| DQB1*03:228| DQB1*03:229| DQB1*03:230| DQB1*03:231| DQB1*03:232| DQB1*03:233| DQB1*03:234| DQB1*03:235| DQB1*03:236| DQB1*03:238| DQB1*03:239| DQB1*03:240| DQB1*03:241| DQB1*03:242| DQB1*03:243| DQB1*03:244| DQB1*03:245| DQB1*03:246| DQB1*03:247| DQB1*03:248| DQB1*03:249| DQB1*03:250| DQB1*03:251| DQB1*03:252| DQB1*03:253| DQB1*03:254| DQB1*03:255| DQB1*03:256| DQB1*03:257| DQB1*03:258| DQB1*03:259| DQB1*03:260| DQB1*03:261| DQB1*03:262| DQB1*03:263| DQB1*03:264| DQB1*03:265| DQB1*03:266| DQB1*03:267| DQB1*03:268| DQB1*03:270| DQB1*03:271| DQB1*03:272| DQB1*03:273| DQB1*03:274| DQB1*03:275| DQB1*03:277| DQB1*03:278| DQB1*03:279| DQB1*03:280| DQB1*03:281| DQB1*03:283| DQB1*03:284| DQB1*03:285| DQB1*03:286| DQB1*03:287| DQB1*03:288| DQB1*03:289| DQB1*03:290| DQB1*03:291| DQB1*03:292| DQB1*03:293| DQB1*03:294| DQB1*03:295| DQB1*03:296| DQB1*03:297| DQB1*03:298| DQB1*03:299| DQB1*03:300| DQB1*03:301| DQB1*03:302| DQB1*03:304| DQB1*03:305| DQB1*03:306| DQB1*03:307| DQB1*03:308| DQB1*03:309| DQB1*03:311| DQB1*03:312| DQB1*03:313| DQB1*03:314| DQB1*03:315| DQB1*03:316| DQB1*03:317:01| DQB1*03:317:02| DQB1*03:318| DQB1*03:319| DQB1*03:320| DQB1*03:321| DQB1*03:322| DQB1*03:323| DQB1*03:324| DQB1*03:326| DQB1*03:327| DQB1*03:328| DQB1*03:329| DQB1*03:330| DQB1*03:331| DQB1*03:332| DQB1*03:333| DQB1*03:335| DQB1*03:336| DQB1*03:337| DQB1*03:341| DQB1*03:342| DQB1*03:343| DQB1*03:344| DQB1*03:345| DQB1*03:346| DQB1*03:347| DQB1*03:348| DQB1*03:349| DQB1*03:350| DQB1*03:351| DQB1*03:352| DQB1*03:353</t>
+  </si>
+  <si>
+    <t>DQB1*03:02:01:01| DQB1*03:02:01:02| DQB1*03:02:01:03| DQB1*03:02:01:04| DQB1*03:02:01:05| DQB1*03:02:01:06| DQB1*03:02:02| DQB1*03:02:03| DQB1*03:02:04| DQB1*03:02:05| DQB1*03:02:06| DQB1*03:02:07| DQB1*03:02:08| DQB1*03:02:09| DQB1*03:02:10| DQB1*03:02:11| DQB1*03:02:12| DQB1*03:02:13| DQB1*03:02:14| DQB1*03:02:15| DQB1*03:02:16| DQB1*03:02:17| DQB1*03:02:18| DQB1*03:02:19| DQB1*03:02:20| DQB1*03:02:21| DQB1*03:02:22| DQB1*03:02:23| DQB1*03:02:24| DQB1*03:02:25| DQB1*03:02:26| DQB1*03:02:27| DQB1*03:02:28| DQB1*03:02:29| DQB1*03:02:30| DQB1*03:05:01| DQB1*03:05:02| DQB1*03:05:03| DQB1*03:05:04| DQB1*03:07| DQB1*03:08| DQB1*03:10:01| DQB1*03:10:02:01| DQB1*03:10:02:02| DQB1*03:11| DQB1*03:18| DQB1*03:06| DQB1*03:14:01| DQB1*03:14:02| DQB1*03:21| DQB1*03:22| DQB1*03:23:01| DQB1*03:23:02| DQB1*03:23:03| DQB1*03:24| DQB1*03:25:01| DQB1*03:25:02| DQB1*03:26| DQB1*03:27| DQB1*03:28| DQB1*03:29| DQB1*03:30| DQB1*03:31| DQB1*03:32| DQB1*03:33| DQB1*03:34| DQB1*03:35| DQB1*03:36| DQB1*03:37| DQB1*03:38| DQB1*03:39| DQB1*03:40| DQB1*03:41| DQB1*03:42| DQB1*03:43| DQB1*03:44| DQB1*03:45| DQB1*03:46| DQB1*03:47| DQB1*03:48| DQB1*03:49| DQB1*03:50| DQB1*03:51| DQB1*03:52| DQB1*03:53| DQB1*03:54| DQB1*03:55| DQB1*03:56| DQB1*03:57| DQB1*03:58| DQB1*03:59| DQB1*03:60| DQB1*03:61| DQB1*03:62| DQB1*03:63| DQB1*03:64| DQB1*03:65| DQB1*03:67| DQB1*03:68| DQB1*03:69| DQB1*03:70| DQB1*03:71| DQB1*03:72| DQB1*03:73| DQB1*03:74| DQB1*03:75| DQB1*03:76| DQB1*03:77| DQB1*03:78| DQB1*03:79| DQB1*03:80| DQB1*03:81| DQB1*03:82| DQB1*03:83| DQB1*03:85| DQB1*03:86| DQB1*03:87| DQB1*03:88| DQB1*03:89| DQB1*03:91Q| DQB1*03:92| DQB1*03:93| DQB1*03:94| DQB1*03:96| DQB1*03:97| DQB1*03:98| DQB1*03:99Q| DQB1*03:100| DQB1*03:101| DQB1*03:102| DQB1*03:103| DQB1*03:104| DQB1*03:105| DQB1*03:106| DQB1*03:107| DQB1*03:108| DQB1*03:109| DQB1*03:110| DQB1*03:111| DQB1*03:112| DQB1*03:113| DQB1*03:114| DQB1*03:115| DQB1*03:116| DQB1*03:117| DQB1*03:119| DQB1*03:120| DQB1*03:121| DQB1*03:122| DQB1*03:123| DQB1*03:124| DQB1*03:125| DQB1*03:126| DQB1*03:127| DQB1*03:128| DQB1*03:129| DQB1*03:130| DQB1*03:131| DQB1*03:132| DQB1*03:133| DQB1*03:134| DQB1*03:135| DQB1*03:136| DQB1*03:137| DQB1*03:138| DQB1*03:139| DQB1*03:140| DQB1*03:141| DQB1*03:142| DQB1*03:143| DQB1*03:144| DQB1*03:145| DQB1*03:146| DQB1*03:147| DQB1*03:148| DQB1*03:149| DQB1*03:150| DQB1*03:151| DQB1*03:152| DQB1*03:153| DQB1*03:154| DQB1*03:155| DQB1*03:156| DQB1*03:157| DQB1*03:158| DQB1*03:159| DQB1*03:160| DQB1*03:161| DQB1*03:162| DQB1*03:163| DQB1*03:164| DQB1*03:165| DQB1*03:166| DQB1*03:167| DQB1*03:168| DQB1*03:169| DQB1*03:170| DQB1*03:171| DQB1*03:172| DQB1*03:173| DQB1*03:174| DQB1*03:175| DQB1*03:176| DQB1*03:177| DQB1*03:178| DQB1*03:179| DQB1*03:180| DQB1*03:181| DQB1*03:182| DQB1*03:183| DQB1*03:184| DQB1*03:185| DQB1*03:186| DQB1*03:187| DQB1*03:188| DQB1*03:189| DQB1*03:190| DQB1*03:191| DQB1*03:192| DQB1*03:193| DQB1*03:194| DQB1*03:195| DQB1*03:196| DQB1*03:197Q| DQB1*03:198:01| DQB1*03:198:02| DQB1*03:199| DQB1*03:200| DQB1*03:201| DQB1*03:202| DQB1*03:203| DQB1*03:204| DQB1*03:205| DQB1*03:206| DQB1*03:207| DQB1*03:208| DQB1*03:209| DQB1*03:210| DQB1*03:211| DQB1*03:212| DQB1*03:214| DQB1*03:215| DQB1*03:216| DQB1*03:217| DQB1*03:218| DQB1*03:219| DQB1*03:220| DQB1*03:221| DQB1*03:222| DQB1*03:223| DQB1*03:224| DQB1*03:225| DQB1*03:226| DQB1*03:227| DQB1*03:228| DQB1*03:229| DQB1*03:230| DQB1*03:231| DQB1*03:232| DQB1*03:233| DQB1*03:234| DQB1*03:235| DQB1*03:236| DQB1*03:238| DQB1*03:239| DQB1*03:240| DQB1*03:241| DQB1*03:242| DQB1*03:243| DQB1*03:244| DQB1*03:245| DQB1*03:246| DQB1*03:247| DQB1*03:248| DQB1*03:249| DQB1*03:250| DQB1*03:251| DQB1*03:252| DQB1*03:253| DQB1*03:254| DQB1*03:255| DQB1*03:256| DQB1*03:257| DQB1*03:258| DQB1*03:259| DQB1*03:260| DQB1*03:261| DQB1*03:262| DQB1*03:263| DQB1*03:264| DQB1*03:265| DQB1*03:266| DQB1*03:267| DQB1*03:268| DQB1*03:270| DQB1*03:271| DQB1*03:272| DQB1*03:273| DQB1*03:274| DQB1*03:275| DQB1*03:277| DQB1*03:278| DQB1*03:279| DQB1*03:280| DQB1*03:281| DQB1*03:283| DQB1*03:284| DQB1*03:285| DQB1*03:286| DQB1*03:287| DQB1*03:288| DQB1*03:289| DQB1*03:290| DQB1*03:291| DQB1*03:292| DQB1*03:293| DQB1*03:294| DQB1*03:295| DQB1*03:296| DQB1*03:297| DQB1*03:298| DQB1*03:299| DQB1*03:300| DQB1*03:301| DQB1*03:302| DQB1*03:304| DQB1*03:305| DQB1*03:306| DQB1*03:307| DQB1*03:308| DQB1*03:309| DQB1*03:311| DQB1*03:312| DQB1*03:313| DQB1*03:314| DQB1*03:315| DQB1*03:316| DQB1*03:317:01| DQB1*03:317:02| DQB1*03:318| DQB1*03:319| DQB1*03:320| DQB1*03:321| DQB1*03:322| DQB1*03:323| DQB1*03:324| DQB1*03:326| DQB1*03:327| DQB1*03:328| DQB1*03:329| DQB1*03:330| DQB1*03:331| DQB1*03:332| DQB1*03:333| DQB1*03:335| DQB1*03:336| DQB1*03:337| DQB1*03:341| DQB1*03:342| DQB1*03:343| DQB1*03:344| DQB1*03:345| DQB1*03:346| DQB1*03:347| DQB1*03:348| DQB1*03:349| DQB1*03:350| DQB1*03:351| DQB1*03:352| DQB1*03:353</t>
+  </si>
+  <si>
+    <t>DQB1*03:03:02:01| DQB1*03:03:02:02| DQB1*03:03:02:03| DQB1*03:03:02:04| DQB1*03:03:02:05| DQB1*03:03:03| DQB1*03:03:04| DQB1*03:03:05| DQB1*03:03:06| DQB1*03:03:07| DQB1*03:03:08| DQB1*03:03:09| DQB1*03:03:10| DQB1*03:03:11| DQB1*03:03:12| DQB1*03:03:13| DQB1*03:03:14| DQB1*03:03:15| DQB1*03:03:16| DQB1*03:03:17| DQB1*03:03:18| DQB1*03:03:19| DQB1*03:03:20| DQB1*03:03:21| DQB1*03:12| DQB1*03:15| DQB1*03:17:01| DQB1*03:17:02| DQB1*03:20| DQB1*03:06| DQB1*03:14:01| DQB1*03:14:02| DQB1*03:21| DQB1*03:22| DQB1*03:23:01| DQB1*03:23:02| DQB1*03:23:03| DQB1*03:24| DQB1*03:25:01| DQB1*03:25:02| DQB1*03:26| DQB1*03:27| DQB1*03:28| DQB1*03:29| DQB1*03:30| DQB1*03:31| DQB1*03:32| DQB1*03:33| DQB1*03:34| DQB1*03:35| DQB1*03:36| DQB1*03:37| DQB1*03:38| DQB1*03:39| DQB1*03:40| DQB1*03:41| DQB1*03:42| DQB1*03:43| DQB1*03:44| DQB1*03:45| DQB1*03:46| DQB1*03:47| DQB1*03:48| DQB1*03:49| DQB1*03:50| DQB1*03:51| DQB1*03:52| DQB1*03:53| DQB1*03:54| DQB1*03:55| DQB1*03:56| DQB1*03:57| DQB1*03:58| DQB1*03:59| DQB1*03:60| DQB1*03:61| DQB1*03:62| DQB1*03:63| DQB1*03:64| DQB1*03:65| DQB1*03:67| DQB1*03:68| DQB1*03:69| DQB1*03:70| DQB1*03:71| DQB1*03:72| DQB1*03:73| DQB1*03:74| DQB1*03:75| DQB1*03:76| DQB1*03:77| DQB1*03:78| DQB1*03:79| DQB1*03:80| DQB1*03:81| DQB1*03:82| DQB1*03:83| DQB1*03:85| DQB1*03:86| DQB1*03:87| DQB1*03:88| DQB1*03:89| DQB1*03:91Q| DQB1*03:92| DQB1*03:93| DQB1*03:94| DQB1*03:96| DQB1*03:97| DQB1*03:98| DQB1*03:99Q| DQB1*03:100| DQB1*03:101| DQB1*03:102| DQB1*03:103| DQB1*03:104| DQB1*03:105| DQB1*03:106| DQB1*03:107| DQB1*03:108| DQB1*03:109| DQB1*03:110| DQB1*03:111| DQB1*03:112| DQB1*03:113| DQB1*03:114| DQB1*03:115| DQB1*03:116| DQB1*03:117| DQB1*03:119| DQB1*03:120| DQB1*03:121| DQB1*03:122| DQB1*03:123| DQB1*03:124| DQB1*03:125| DQB1*03:126| DQB1*03:127| DQB1*03:128| DQB1*03:129| DQB1*03:130| DQB1*03:131| DQB1*03:132| DQB1*03:133| DQB1*03:134| DQB1*03:135| DQB1*03:136| DQB1*03:137| DQB1*03:138| DQB1*03:139| DQB1*03:140| DQB1*03:141| DQB1*03:142| DQB1*03:143| DQB1*03:144| DQB1*03:145| DQB1*03:146| DQB1*03:147| DQB1*03:148| DQB1*03:149| DQB1*03:150| DQB1*03:151| DQB1*03:152| DQB1*03:153| DQB1*03:154| DQB1*03:155| DQB1*03:156| DQB1*03:157| DQB1*03:158| DQB1*03:159| DQB1*03:160| DQB1*03:161| DQB1*03:162| DQB1*03:163| DQB1*03:164| DQB1*03:165| DQB1*03:166| DQB1*03:167| DQB1*03:168| DQB1*03:169| DQB1*03:170| DQB1*03:171| DQB1*03:172| DQB1*03:173| DQB1*03:174| DQB1*03:175| DQB1*03:176| DQB1*03:177| DQB1*03:178| DQB1*03:179| DQB1*03:180| DQB1*03:181| DQB1*03:182| DQB1*03:183| DQB1*03:184| DQB1*03:185| DQB1*03:186| DQB1*03:187| DQB1*03:188| DQB1*03:189| DQB1*03:190| DQB1*03:191| DQB1*03:192| DQB1*03:193| DQB1*03:194| DQB1*03:195| DQB1*03:196| DQB1*03:197Q| DQB1*03:198:01| DQB1*03:198:02| DQB1*03:199| DQB1*03:200| DQB1*03:201| DQB1*03:202| DQB1*03:203| DQB1*03:204| DQB1*03:205| DQB1*03:206| DQB1*03:207| DQB1*03:208| DQB1*03:209| DQB1*03:210| DQB1*03:211| DQB1*03:212| DQB1*03:214| DQB1*03:215| DQB1*03:216| DQB1*03:217| DQB1*03:218| DQB1*03:219| DQB1*03:220| DQB1*03:221| DQB1*03:222| DQB1*03:223| DQB1*03:224| DQB1*03:225| DQB1*03:226| DQB1*03:227| DQB1*03:228| DQB1*03:229| DQB1*03:230| DQB1*03:231| DQB1*03:232| DQB1*03:233| DQB1*03:234| DQB1*03:235| DQB1*03:236| DQB1*03:238| DQB1*03:239| DQB1*03:240| DQB1*03:241| DQB1*03:242| DQB1*03:243| DQB1*03:244| DQB1*03:245| DQB1*03:246| DQB1*03:247| DQB1*03:248| DQB1*03:249| DQB1*03:250| DQB1*03:251| DQB1*03:252| DQB1*03:253| DQB1*03:254| DQB1*03:255| DQB1*03:256| DQB1*03:257| DQB1*03:258| DQB1*03:259| DQB1*03:260| DQB1*03:261| DQB1*03:262| DQB1*03:263| DQB1*03:264| DQB1*03:265| DQB1*03:266| DQB1*03:267| DQB1*03:268| DQB1*03:270| DQB1*03:271| DQB1*03:272| DQB1*03:273| DQB1*03:274| DQB1*03:275| DQB1*03:277| DQB1*03:278| DQB1*03:279| DQB1*03:280| DQB1*03:281| DQB1*03:283| DQB1*03:284| DQB1*03:285| DQB1*03:286| DQB1*03:287| DQB1*03:288| DQB1*03:289| DQB1*03:290| DQB1*03:291| DQB1*03:292| DQB1*03:293| DQB1*03:294| DQB1*03:295| DQB1*03:296| DQB1*03:297| DQB1*03:298| DQB1*03:299| DQB1*03:300| DQB1*03:301| DQB1*03:302| DQB1*03:304| DQB1*03:305| DQB1*03:306| DQB1*03:307| DQB1*03:308| DQB1*03:309| DQB1*03:311| DQB1*03:312| DQB1*03:313| DQB1*03:314| DQB1*03:315| DQB1*03:316| DQB1*03:317:01| DQB1*03:317:02| DQB1*03:318| DQB1*03:319| DQB1*03:320| DQB1*03:321| DQB1*03:322| DQB1*03:323| DQB1*03:324| DQB1*03:326| DQB1*03:327| DQB1*03:328| DQB1*03:329| DQB1*03:330| DQB1*03:331| DQB1*03:332| DQB1*03:333| DQB1*03:335| DQB1*03:336| DQB1*03:337| DQB1*03:341| DQB1*03:342| DQB1*03:343| DQB1*03:344| DQB1*03:345| DQB1*03:346| DQB1*03:347| DQB1*03:348| DQB1*03:349| DQB1*03:350| DQB1*03:351| DQB1*03:352| DQB1*03:353</t>
   </si>
 </sst>
 </file>
@@ -1170,16 +1236,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2680,14 +2743,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="200.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2702,288 +2765,376 @@
       <c r="A2" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>308</v>
+      <c r="B2" s="1" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>309</v>
+      <c r="B3" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>310</v>
+      <c r="B4" s="1" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>311</v>
+      <c r="B5" s="1" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>312</v>
+      <c r="B6" s="1" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>313</v>
+      <c r="B7" s="1" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>314</v>
+      <c r="B8" s="1" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>315</v>
+      <c r="B9" s="1" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>316</v>
+      <c r="B10" s="1" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>317</v>
+      <c r="B11" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>318</v>
+      <c r="B12" s="1" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>319</v>
+      <c r="B13" s="1" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>320</v>
+      <c r="B14" s="1" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>321</v>
+      <c r="B15" s="1" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>322</v>
+      <c r="B16" s="1" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>323</v>
+      <c r="B17" s="1" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>324</v>
+      <c r="B18" s="1" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>325</v>
+      <c r="B19" s="1" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>326</v>
+      <c r="B20" s="1" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>327</v>
+      <c r="B21" s="1" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>328</v>
+      <c r="B22" s="1" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>329</v>
+      <c r="B23" s="1" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>330</v>
+      <c r="B24" s="1" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>331</v>
+      <c r="B25" s="1" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>332</v>
+      <c r="B26" s="1" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>333</v>
+      <c r="B27" s="1" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>334</v>
+      <c r="B28" s="1" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>335</v>
+      <c r="B29" s="1" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>336</v>
+      <c r="B30" s="1" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>337</v>
+      <c r="B31" s="1" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>338</v>
+      <c r="B32" s="1" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>339</v>
+      <c r="B33" s="1" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>340</v>
+      <c r="B34" s="1" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>341</v>
+      <c r="B35" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>342</v>
+      <c r="B36" s="1" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>343</v>
+      <c r="B37" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -3013,82 +3164,82 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>344</v>
+        <v>366</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>354</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>345</v>
+        <v>367</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>355</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>346</v>
+        <v>368</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>356</v>
+        <v>378</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>347</v>
+        <v>369</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>357</v>
+        <v>379</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>348</v>
+        <v>370</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>358</v>
+        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>349</v>
+        <v>371</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>359</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>350</v>
+        <v>372</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>360</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>351</v>
+        <v>373</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>361</v>
+        <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>352</v>
+        <v>374</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>353</v>
+        <v>375</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>363</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>